<commit_message>
milof sauf 2 datasets
</commit_message>
<xml_diff>
--- a/f1score_merlin_abnormal_point_results.xlsx
+++ b/f1score_merlin_abnormal_point_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AO8"/>
+  <dimension ref="A1:AQ8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -581,55 +581,65 @@
       </c>
       <c r="AE1" s="1" t="inlineStr">
         <is>
+          <t>Unnamed: 0.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1</t>
+        </is>
+      </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1</t>
+        </is>
+      </c>
+      <c r="AG1" s="1" t="inlineStr">
+        <is>
           <t>Note</t>
         </is>
       </c>
-      <c r="AF1" s="1" t="inlineStr">
+      <c r="AH1" s="1" t="inlineStr">
         <is>
           <t>Dataset</t>
         </is>
       </c>
-      <c r="AG1" s="1" t="inlineStr">
+      <c r="AI1" s="1" t="inlineStr">
         <is>
           <t>Dataset length</t>
         </is>
       </c>
-      <c r="AH1" s="1" t="inlineStr">
+      <c r="AJ1" s="1" t="inlineStr">
         <is>
           <t>Type</t>
         </is>
       </c>
-      <c r="AI1" s="1" t="inlineStr">
+      <c r="AK1" s="1" t="inlineStr">
         <is>
           <t>#discords</t>
         </is>
       </c>
-      <c r="AJ1" s="1" t="inlineStr">
+      <c r="AL1" s="1" t="inlineStr">
         <is>
           <t>Position discord</t>
         </is>
       </c>
-      <c r="AK1" s="1" t="inlineStr">
+      <c r="AM1" s="1" t="inlineStr">
         <is>
           <t>discord length</t>
         </is>
       </c>
-      <c r="AL1" s="1" t="inlineStr">
+      <c r="AN1" s="1" t="inlineStr">
         <is>
           <t>MILOF_identified</t>
         </is>
       </c>
-      <c r="AM1" s="1" t="inlineStr">
+      <c r="AO1" s="1" t="inlineStr">
         <is>
           <t>MILOF_Overlap_merlin</t>
         </is>
       </c>
-      <c r="AN1" s="1" t="inlineStr">
+      <c r="AP1" s="1" t="inlineStr">
         <is>
           <t>MILOFbest_param</t>
         </is>
       </c>
-      <c r="AO1" s="1" t="inlineStr">
+      <c r="AQ1" s="1" t="inlineStr">
         <is>
           <t>MILOFtime_taken</t>
         </is>
@@ -726,46 +736,52 @@
       <c r="AD2" t="n">
         <v>0</v>
       </c>
-      <c r="AE2" t="inlineStr"/>
-      <c r="AF2" t="inlineStr">
+      <c r="AE2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG2" t="inlineStr"/>
+      <c r="AH2" t="inlineStr">
         <is>
           <t>nab-data/realKnownCause/ambient_temperature_system_failure.csv</t>
         </is>
       </c>
-      <c r="AG2" t="n">
+      <c r="AI2" t="n">
         <v>7267</v>
       </c>
-      <c r="AH2" t="inlineStr">
+      <c r="AJ2" t="inlineStr">
         <is>
           <t>NAB</t>
         </is>
       </c>
-      <c r="AI2" t="n">
-        <v>2</v>
-      </c>
-      <c r="AJ2" t="inlineStr">
+      <c r="AK2" t="n">
+        <v>2</v>
+      </c>
+      <c r="AL2" t="inlineStr">
         <is>
           <t>3540; 5999</t>
         </is>
       </c>
-      <c r="AK2" t="n">
+      <c r="AM2" t="n">
         <v>362</v>
       </c>
-      <c r="AL2" t="inlineStr">
-        <is>
-          <t>[1287, 3876]</t>
-        </is>
-      </c>
-      <c r="AM2" t="n">
-        <v>0</v>
-      </c>
       <c r="AN2" t="inlineStr">
         <is>
-          <t>{'Numk': 14, 'KPar': 11, 'Bucket_index': 500}</t>
+          <t>[3213, 3637, 6012]</t>
         </is>
       </c>
       <c r="AO2" t="n">
-        <v>122.325254590949</v>
+        <v>0</v>
+      </c>
+      <c r="AP2" t="inlineStr">
+        <is>
+          <t>{'Numk': 17, 'KPar': 4, 'Bucket_index': 500}</t>
+        </is>
+      </c>
+      <c r="AQ2" t="n">
+        <v>178.6288073339965</v>
       </c>
     </row>
     <row r="3">
@@ -859,46 +875,52 @@
       <c r="AD3" t="n">
         <v>1</v>
       </c>
-      <c r="AE3" t="inlineStr"/>
-      <c r="AF3" t="inlineStr">
+      <c r="AE3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG3" t="inlineStr"/>
+      <c r="AH3" t="inlineStr">
         <is>
           <t>nab-data/realKnownCause/cpu_utilization_asg_misconfiguration.csv</t>
         </is>
       </c>
-      <c r="AG3" t="n">
+      <c r="AI3" t="n">
         <v>18050</v>
       </c>
-      <c r="AH3" t="inlineStr">
+      <c r="AJ3" t="inlineStr">
         <is>
           <t>NAB</t>
         </is>
       </c>
-      <c r="AI3" t="n">
-        <v>1</v>
-      </c>
-      <c r="AJ3" t="inlineStr">
+      <c r="AK3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL3" t="inlineStr">
         <is>
           <t>16551</t>
         </is>
       </c>
-      <c r="AK3" t="n">
+      <c r="AM3" t="n">
         <v>1498</v>
       </c>
-      <c r="AL3" t="inlineStr">
-        <is>
-          <t>[18010]</t>
-        </is>
-      </c>
-      <c r="AM3" t="n">
-        <v>0</v>
-      </c>
       <c r="AN3" t="inlineStr">
         <is>
-          <t>{'Numk': 5, 'KPar': 8, 'Bucket_index': 500}</t>
+          <t>[16727, 17627, 17951]</t>
         </is>
       </c>
       <c r="AO3" t="n">
-        <v>246.2038500059862</v>
+        <v>0</v>
+      </c>
+      <c r="AP3" t="inlineStr">
+        <is>
+          <t>{'Numk': 23, 'KPar': 14, 'Bucket_index': 500}</t>
+        </is>
+      </c>
+      <c r="AQ3" t="n">
+        <v>430.6199549960438</v>
       </c>
     </row>
     <row r="4">
@@ -992,45 +1014,51 @@
       <c r="AD4" t="n">
         <v>2</v>
       </c>
-      <c r="AE4" t="inlineStr"/>
-      <c r="AF4" t="inlineStr">
+      <c r="AE4" t="n">
+        <v>2</v>
+      </c>
+      <c r="AF4" t="n">
+        <v>2</v>
+      </c>
+      <c r="AG4" t="inlineStr"/>
+      <c r="AH4" t="inlineStr">
         <is>
           <t>nab-data/realKnownCause/ec2_request_latency_system_failure.csv</t>
         </is>
       </c>
-      <c r="AG4" t="n">
+      <c r="AI4" t="n">
         <v>4032</v>
       </c>
-      <c r="AH4" t="inlineStr">
+      <c r="AJ4" t="inlineStr">
         <is>
           <t>NAB</t>
         </is>
       </c>
-      <c r="AI4" t="n">
-        <v>3</v>
-      </c>
-      <c r="AJ4" t="inlineStr">
+      <c r="AK4" t="n">
+        <v>3</v>
+      </c>
+      <c r="AL4" t="inlineStr">
         <is>
           <t>2014; 3328; 3956</t>
         </is>
       </c>
-      <c r="AK4" t="n">
+      <c r="AM4" t="n">
         <v>134</v>
       </c>
-      <c r="AL4" t="inlineStr">
+      <c r="AN4" t="inlineStr">
         <is>
           <t>[2588, 2806, 3362, 3467, 3984]</t>
         </is>
       </c>
-      <c r="AM4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN4" t="inlineStr">
+      <c r="AO4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP4" t="inlineStr">
         <is>
           <t>{'Numk': 34, 'KPar': 5, 'Bucket_index': 500}</t>
         </is>
       </c>
-      <c r="AO4" t="n">
+      <c r="AQ4" t="n">
         <v>51.45069594099186</v>
       </c>
     </row>
@@ -1125,45 +1153,51 @@
       <c r="AD5" t="n">
         <v>3</v>
       </c>
-      <c r="AE5" t="inlineStr"/>
-      <c r="AF5" t="inlineStr">
+      <c r="AE5" t="n">
+        <v>3</v>
+      </c>
+      <c r="AF5" t="n">
+        <v>3</v>
+      </c>
+      <c r="AG5" t="inlineStr"/>
+      <c r="AH5" t="inlineStr">
         <is>
           <t>nab-data/realKnownCause/machine_temperature_system_failure.csv</t>
         </is>
       </c>
-      <c r="AG5" t="n">
+      <c r="AI5" t="n">
         <v>22695</v>
       </c>
-      <c r="AH5" t="inlineStr">
+      <c r="AJ5" t="inlineStr">
         <is>
           <t>NAB</t>
         </is>
       </c>
-      <c r="AI5" t="n">
-        <v>4</v>
-      </c>
-      <c r="AJ5" t="inlineStr">
+      <c r="AK5" t="n">
+        <v>4</v>
+      </c>
+      <c r="AL5" t="inlineStr">
         <is>
           <t>2126; 3703; 16057; 19232</t>
         </is>
       </c>
-      <c r="AK5" t="n">
+      <c r="AM5" t="n">
         <v>566</v>
       </c>
-      <c r="AL5" t="inlineStr">
+      <c r="AN5" t="inlineStr">
         <is>
           <t>no</t>
         </is>
       </c>
-      <c r="AM5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN5" t="inlineStr">
+      <c r="AO5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP5" t="inlineStr">
         <is>
           <t>params</t>
         </is>
       </c>
-      <c r="AO5" t="n">
+      <c r="AQ5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1258,45 +1292,51 @@
       <c r="AD6" t="n">
         <v>4</v>
       </c>
-      <c r="AE6" t="inlineStr"/>
-      <c r="AF6" t="inlineStr">
+      <c r="AE6" t="n">
+        <v>4</v>
+      </c>
+      <c r="AF6" t="n">
+        <v>4</v>
+      </c>
+      <c r="AG6" t="inlineStr"/>
+      <c r="AH6" t="inlineStr">
         <is>
           <t>nab-data/realKnownCause/nyc_taxi.csv</t>
         </is>
       </c>
-      <c r="AG6" t="n">
+      <c r="AI6" t="n">
         <v>10320</v>
       </c>
-      <c r="AH6" t="inlineStr">
+      <c r="AJ6" t="inlineStr">
         <is>
           <t>NAB</t>
         </is>
       </c>
-      <c r="AI6" t="n">
-        <v>5</v>
-      </c>
-      <c r="AJ6" t="inlineStr">
+      <c r="AK6" t="n">
+        <v>5</v>
+      </c>
+      <c r="AL6" t="inlineStr">
         <is>
           <t>5839; 7080; 8423; 8731; 9977</t>
         </is>
       </c>
-      <c r="AK6" t="n">
+      <c r="AM6" t="n">
         <v>206</v>
       </c>
-      <c r="AL6" t="inlineStr">
+      <c r="AN6" t="inlineStr">
         <is>
           <t>[1446, 7008, 9079, 10086, 10088, 10092]</t>
         </is>
       </c>
-      <c r="AM6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN6" t="inlineStr">
+      <c r="AO6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP6" t="inlineStr">
         <is>
           <t>{'Numk': 14, 'KPar': 10, 'Bucket_index': 500}</t>
         </is>
       </c>
-      <c r="AO6" t="n">
+      <c r="AQ6" t="n">
         <v>173.5355705979746</v>
       </c>
     </row>
@@ -1391,45 +1431,51 @@
       <c r="AD7" t="n">
         <v>5</v>
       </c>
-      <c r="AE7" t="inlineStr"/>
-      <c r="AF7" t="inlineStr">
+      <c r="AE7" t="n">
+        <v>5</v>
+      </c>
+      <c r="AF7" t="n">
+        <v>5</v>
+      </c>
+      <c r="AG7" t="inlineStr"/>
+      <c r="AH7" t="inlineStr">
         <is>
           <t>nab-data/realKnownCause/rogue_agent_key_hold.csv</t>
         </is>
       </c>
-      <c r="AG7" t="n">
+      <c r="AI7" t="n">
         <v>1882</v>
       </c>
-      <c r="AH7" t="inlineStr">
+      <c r="AJ7" t="inlineStr">
         <is>
           <t>NAB</t>
         </is>
       </c>
-      <c r="AI7" t="n">
-        <v>2</v>
-      </c>
-      <c r="AJ7" t="inlineStr">
+      <c r="AK7" t="n">
+        <v>2</v>
+      </c>
+      <c r="AL7" t="inlineStr">
         <is>
           <t>669; 1240</t>
         </is>
       </c>
-      <c r="AK7" t="n">
+      <c r="AM7" t="n">
         <v>94</v>
       </c>
-      <c r="AL7" t="inlineStr">
+      <c r="AN7" t="inlineStr">
         <is>
           <t>[6, 9, 10, 11, 14, 20, 21, 23, 40, 41, 42, 88, 94, 115, 116, 121, 137, 139, 140, 156, 158, 163, 164, 170, 171, 187, 193, 201, 208, 209, 214, 218, 219, 221, 222, 246, 251, 252, 270, 284, 291, 295, 296, 299, 300, 303, 304, 305, 306, 307, 308, 309, 310, 311, 312, 313, 314, 315, 316, 317, 318, 319, 320, 321, 322, 323, 324, 325, 326, 327, 328, 330, 331, 332, 333, 334, 335, 336, 337, 338, 339, 340, 341, 342, 343, 344, 345, 346, 347, 348, 349, 350, 351, 352, 353, 354, 355, 356, 357, 358, 359, 360, 361, 362, 363, 364, 365, 366, 367, 368, 369, 370, 371, 372, 373, 374, 375, 376, 377, 378, 379, 380, 381, 382, 383, 384, 385, 386, 387, 388, 389, 390, 391, 392, 393, 394, 395, 396, 397, 398, 399, 400, 401, 402, 403, 404, 405, 406, 407, 408, 409, 410, 411, 412, 413, 414, 415, 416, 417, 418, 419, 431, 436, 454, 455, 478, 482, 499, 524, 534, 535, 541, 547, 548, 549, 550, 551, 552, 553, 554, 555, 556, 557, 558, 559, 560, 561, 562, 563, 565, 566, 567, 568, 570, 571, 573, 574, 575, 576, 577, 578, 580, 581, 582, 583, 584, 585, 586, 587, 588, 589, 590, 591, 592, 593, 594, 595, 596, 597, 598, 599, 600, 601, 602, 603, 604, 605, 606, 607, 608, 609, 610, 611, 612, 613, 614, 617, 618, 619, 621, 622, 623, 624, 625, 626, 627, 628, 629, 630, 631, 632, 633, 634, 635, 636, 637, 638, 639, 640, 641, 642, 643, 644, 645, 646, 647, 648, 649, 650, 651, 652, 653, 654, 655, 656, 657, 658, 659, 660, 661, 662, 663, 664, 665, 666, 667, 668, 669, 670, 671, 672, 673, 674, 675, 676, 677, 678, 679, 680, 681, 682, 683, 684, 685, 686, 687, 688, 689, 690, 691, 692, 693, 694, 695, 696, 697, 698, 699, 700, 701, 702, 703, 704, 705, 706, 707, 708, 709, 710, 711, 712, 713, 714, 715, 716, 717, 718, 719, 720, 721, 722, 723, 724, 725, 726, 727, 728, 729, 730, 731, 732, 733, 747, 750, 754, 764, 765, 770, 771, 772, 773, 778, 779, 780, 801, 802, 803, 804, 805, 806, 807, 808, 813, 814, 817, 818, 837, 838, 839, 841, 842, 843, 844, 845, 846, 847, 848, 849, 850, 851, 852, 853, 854, 855, 856, 857, 858, 859, 860, 861, 862, 863, 864, 865, 866, 867, 868, 869, 870, 871, 872, 873, 874, 875, 876, 877, 878, 879, 881, 882, 883, 884, 885, 886, 887, 888, 889, 890, 891, 892, 893, 894, 895, 896, 897, 898, 899, 900, 901, 902, 903, 904, 905, 906, 907, 908, 909, 910, 911, 912, 913, 914, 915, 916, 917, 918, 919, 920, 921, 922, 923, 924, 925, 926, 927, 928, 929, 930, 931, 932, 933, 934, 935, 936, 937, 938, 939, 940, 941, 942, 943, 944, 945, 946, 947, 948, 949, 950, 951, 952, 953, 954, 955, 956, 957, 958, 959, 960, 961, 962, 963, 964, 965, 966, 967, 968, 969, 970, 971, 972, 973, 974, 975, 976, 977, 978, 979, 980, 981, 982, 983, 984, 985, 986, 987, 988, 989, 990, 991, 992, 993, 994, 995, 996, 997, 998, 999, 1000, 1001, 1002, 1003, 1004, 1005, 1006, 1007, 1008, 1009, 1011, 1012, 1013, 1014, 1015, 1016, 1017, 1018, 1019, 1020, 1021, 1022, 1023, 1024, 1025, 1026, 1027, 1028, 1029, 1030, 1031, 1032, 1033, 1034, 1035, 1036, 1037, 1038, 1039, 1040, 1041, 1042, 1043, 1044, 1045, 1046, 1047, 1048, 1049, 1050, 1051, 1052, 1053, 1054, 1055, 1056, 1057, 1058, 1059, 1060, 1061, 1062, 1063, 1064, 1065, 1066, 1067, 1068, 1069, 1070, 1071, 1072, 1073, 1074, 1075, 1076, 1077, 1078, 1079, 1080, 1081, 1082, 1083, 1084, 1085, 1086, 1087, 1088, 1089, 1090, 1091, 1092, 1093, 1094, 1095, 1096, 1097, 1098, 1099, 1100, 1101, 1102, 1103, 1104, 1105, 1106, 1107, 1108, 1109, 1111, 1114, 1115, 1116, 1117, 1118, 1119, 1120, 1121, 1122, 1123, 1124, 1125, 1126, 1127, 1128, 1129, 1130, 1131, 1132, 1133, 1134, 1135, 1136, 1137, 1138, 1139, 1140, 1141, 1142, 1143, 1144, 1145, 1146, 1147, 1148, 1149, 1150, 1151, 1152, 1153, 1154, 1155, 1156, 1157, 1158, 1159, 1160, 1161, 1162, 1163, 1164, 1165, 1166, 1167, 1168, 1169, 1170, 1171, 1172, 1173, 1174, 1175, 1176, 1177, 1178, 1179, 1180, 1181, 1182, 1183, 1184, 1185, 1186, 1187, 1188, 1189, 1190, 1191, 1192, 1193, 1194, 1195, 1196, 1197, 1198, 1199, 1200, 1201, 1202, 1203, 1204, 1205, 1206, 1207, 1208, 1209, 1210, 1211, 1212, 1213, 1214, 1215, 1216, 1217, 1218, 1219, 1220, 1221, 1222, 1223, 1224, 1225, 1226, 1227, 1228, 1229, 1230, 1231, 1232, 1233, 1234, 1235, 1236, 1237, 1238, 1239, 1240, 1241, 1242, 1243, 1244, 1245, 1246, 1247, 1248, 1249, 1250, 1251, 1252, 1253, 1254, 1255, 1256, 1257, 1258, 1259, 1260, 1261, 1262, 1263, 1264, 1265, 1266, 1267, 1268, 1269, 1270, 1271, 1274, 1275, 1276, 1277, 1278, 1279, 1280, 1281, 1282, 1283, 1284, 1285, 1286, 1287, 1288, 1289, 1290, 1291, 1292, 1293, 1294, 1295, 1296, 1297, 1298, 1299, 1300, 1301, 1302, 1304, 1305, 1306, 1307, 1308, 1309, 1310, 1311, 1312, 1315, 1316, 1331, 1332, 1333, 1334, 1335, 1338, 1339, 1340, 1341, 1342, 1346, 1347, 1348, 1349, 1350, 1351, 1352, 1353, 1354, 1355, 1356, 1357, 1358, 1359, 1360, 1361, 1362, 1363, 1364, 1365, 1366, 1367, 1368, 1369, 1370, 1371, 1372, 1373, 1374, 1375, 1376, 1377, 1378, 1379, 1380, 1381, 1382, 1383, 1384, 1385, 1410, 1431, 1437, 1438, 1439, 1442, 1443, 1445, 1446, 1447, 1448, 1458, 1462, 1479, 1480, 1515, 1516, 1537, 1538, 1539, 1540, 1544, 1545, 1546, 1547, 1548, 1549, 1552, 1571, 1593, 1594, 1595, 1596, 1597, 1598, 1599, 1600, 1601, 1604, 1644, 1659, 1683, 1684, 1692, 1694, 1697, 1699, 1700, 1701, 1704, 1705, 1706, 1707, 1712, 1721, 1722, 1725, 1726, 1727, 1728, 1729, 1730, 1731, 1732, 1733, 1734, 1735, 1736, 1761, 1801, 1812, 1813, 1814, 1815, 1816, 1819, 1820, 1821, 1861, 1862, 1863, 1864, 1865, 1866, 1867, 1868, 1878, 1881]</t>
         </is>
       </c>
-      <c r="AM7" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN7" t="inlineStr">
+      <c r="AO7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP7" t="inlineStr">
         <is>
           <t>{'Numk': 25, 'KPar': 23, 'Bucket_index': 500}</t>
         </is>
       </c>
-      <c r="AO7" t="n">
+      <c r="AQ7" t="n">
         <v>30.80908843316138</v>
       </c>
     </row>
@@ -1524,45 +1570,51 @@
       <c r="AD8" t="n">
         <v>6</v>
       </c>
-      <c r="AE8" t="inlineStr"/>
-      <c r="AF8" t="inlineStr">
+      <c r="AE8" t="n">
+        <v>6</v>
+      </c>
+      <c r="AF8" t="n">
+        <v>6</v>
+      </c>
+      <c r="AG8" t="inlineStr"/>
+      <c r="AH8" t="inlineStr">
         <is>
           <t>nab-data/realKnownCause/rogue_agent_key_updown.csv</t>
         </is>
       </c>
-      <c r="AG8" t="n">
+      <c r="AI8" t="n">
         <v>5315</v>
       </c>
-      <c r="AH8" t="inlineStr">
+      <c r="AJ8" t="inlineStr">
         <is>
           <t>NAB</t>
         </is>
       </c>
-      <c r="AI8" t="n">
-        <v>2</v>
-      </c>
-      <c r="AJ8" t="inlineStr">
+      <c r="AK8" t="n">
+        <v>2</v>
+      </c>
+      <c r="AL8" t="inlineStr">
         <is>
           <t>2243; 2877</t>
         </is>
       </c>
-      <c r="AK8" t="n">
+      <c r="AM8" t="n">
         <v>264</v>
       </c>
-      <c r="AL8" t="inlineStr">
+      <c r="AN8" t="inlineStr">
         <is>
           <t>[309, 2245, 4453]</t>
         </is>
       </c>
-      <c r="AM8" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN8" t="inlineStr">
+      <c r="AO8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP8" t="inlineStr">
         <is>
           <t>{'Numk': 40, 'KPar': 6, 'Bucket_index': 500}</t>
         </is>
       </c>
-      <c r="AO8" t="n">
+      <c r="AQ8" t="n">
         <v>26.32769314292818</v>
       </c>
     </row>

</xml_diff>

<commit_message>
first good results of arimafd
</commit_message>
<xml_diff>
--- a/f1score_merlin_abnormal_point_results.xlsx
+++ b/f1score_merlin_abnormal_point_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BV8"/>
+  <dimension ref="A1:CB8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -686,115 +686,145 @@
       </c>
       <c r="AZ1" s="1" t="inlineStr">
         <is>
+          <t>Unnamed: 0.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1</t>
+        </is>
+      </c>
+      <c r="BA1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1</t>
+        </is>
+      </c>
+      <c r="BB1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1</t>
+        </is>
+      </c>
+      <c r="BC1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1</t>
+        </is>
+      </c>
+      <c r="BD1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1</t>
+        </is>
+      </c>
+      <c r="BE1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1</t>
+        </is>
+      </c>
+      <c r="BF1" s="1" t="inlineStr">
+        <is>
           <t>Note</t>
         </is>
       </c>
-      <c r="BA1" s="1" t="inlineStr">
+      <c r="BG1" s="1" t="inlineStr">
         <is>
           <t>Dataset</t>
         </is>
       </c>
-      <c r="BB1" s="1" t="inlineStr">
+      <c r="BH1" s="1" t="inlineStr">
         <is>
           <t>Dataset length</t>
         </is>
       </c>
-      <c r="BC1" s="1" t="inlineStr">
+      <c r="BI1" s="1" t="inlineStr">
         <is>
           <t>Type</t>
         </is>
       </c>
-      <c r="BD1" s="1" t="inlineStr">
+      <c r="BJ1" s="1" t="inlineStr">
         <is>
           <t>#discords</t>
         </is>
       </c>
-      <c r="BE1" s="1" t="inlineStr">
+      <c r="BK1" s="1" t="inlineStr">
         <is>
           <t>Position discord</t>
         </is>
       </c>
-      <c r="BF1" s="1" t="inlineStr">
+      <c r="BL1" s="1" t="inlineStr">
         <is>
           <t>discord length</t>
         </is>
       </c>
-      <c r="BG1" s="1" t="inlineStr">
+      <c r="BM1" s="1" t="inlineStr">
         <is>
           <t>HS-tree_identified</t>
         </is>
       </c>
-      <c r="BH1" s="1" t="inlineStr">
+      <c r="BN1" s="1" t="inlineStr">
         <is>
           <t>HS-tree_Overlap_merlin</t>
         </is>
       </c>
-      <c r="BI1" s="1" t="inlineStr">
+      <c r="BO1" s="1" t="inlineStr">
         <is>
           <t>HS-treebest_param</t>
         </is>
       </c>
-      <c r="BJ1" s="1" t="inlineStr">
+      <c r="BP1" s="1" t="inlineStr">
         <is>
           <t>HS-treetime_taken</t>
         </is>
       </c>
-      <c r="BK1" s="1" t="inlineStr">
+      <c r="BQ1" s="1" t="inlineStr">
         <is>
           <t>ARIMAFD_identified</t>
         </is>
       </c>
-      <c r="BL1" s="1" t="inlineStr">
+      <c r="BR1" s="1" t="inlineStr">
         <is>
           <t>ARIMAFD_Overlap_merlin</t>
         </is>
       </c>
-      <c r="BM1" s="1" t="inlineStr">
+      <c r="BS1" s="1" t="inlineStr">
         <is>
           <t>ARIMAFDbest_param</t>
         </is>
       </c>
-      <c r="BN1" s="1" t="inlineStr">
+      <c r="BT1" s="1" t="inlineStr">
         <is>
           <t>ARIMAFDtime_taken</t>
         </is>
       </c>
-      <c r="BO1" s="1" t="inlineStr">
+      <c r="BU1" s="1" t="inlineStr">
         <is>
           <t>MILOF_identified</t>
         </is>
       </c>
-      <c r="BP1" s="1" t="inlineStr">
+      <c r="BV1" s="1" t="inlineStr">
         <is>
           <t>MILOF_Overlap_merlin</t>
         </is>
       </c>
-      <c r="BQ1" s="1" t="inlineStr">
+      <c r="BW1" s="1" t="inlineStr">
         <is>
           <t>MILOFbest_param</t>
         </is>
       </c>
-      <c r="BR1" s="1" t="inlineStr">
+      <c r="BX1" s="1" t="inlineStr">
         <is>
           <t>MILOFtime_taken</t>
         </is>
       </c>
-      <c r="BS1" s="1" t="inlineStr">
+      <c r="BY1" s="1" t="inlineStr">
         <is>
           <t>iforestASD_identified</t>
         </is>
       </c>
-      <c r="BT1" s="1" t="inlineStr">
+      <c r="BZ1" s="1" t="inlineStr">
         <is>
           <t>iforestASD_Overlap_merlin</t>
         </is>
       </c>
-      <c r="BU1" s="1" t="inlineStr">
+      <c r="CA1" s="1" t="inlineStr">
         <is>
           <t>iforestASDbest_param</t>
         </is>
       </c>
-      <c r="BV1" s="1" t="inlineStr">
+      <c r="CB1" s="1" t="inlineStr">
         <is>
           <t>iforestASDtime_taken</t>
         </is>
@@ -954,93 +984,111 @@
       <c r="AY2" t="n">
         <v>0</v>
       </c>
-      <c r="AZ2" t="inlineStr"/>
-      <c r="BA2" t="inlineStr">
+      <c r="AZ2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF2" t="inlineStr"/>
+      <c r="BG2" t="inlineStr">
         <is>
           <t>nab-data/realKnownCause/ambient_temperature_system_failure.csv</t>
         </is>
       </c>
-      <c r="BB2" t="n">
+      <c r="BH2" t="n">
         <v>7267</v>
       </c>
-      <c r="BC2" t="inlineStr">
+      <c r="BI2" t="inlineStr">
         <is>
           <t>NAB</t>
         </is>
       </c>
-      <c r="BD2" t="n">
-        <v>2</v>
-      </c>
-      <c r="BE2" t="inlineStr">
+      <c r="BJ2" t="n">
+        <v>2</v>
+      </c>
+      <c r="BK2" t="inlineStr">
         <is>
           <t>3540; 5999</t>
         </is>
       </c>
-      <c r="BF2" t="n">
+      <c r="BL2" t="n">
         <v>362</v>
       </c>
-      <c r="BG2" t="inlineStr">
+      <c r="BM2" t="inlineStr">
         <is>
           <t>[3152, 5046, 5048, 5050, 5052, 5053, 5054, 5055, 5056, 5057, 5058, 5059, 5060, 5061, 5062, 5063, 5064, 5065, 5066, 5067, 5068, 5069, 5070, 5071, 5072, 5073, 5074, 5075, 5076, 5077, 5078, 5079, 5080, 5100, 5101, 5366, 5367, 5368, 5369, 5370, 5371, 5372, 5373, 5374, 5375, 5376, 5377, 5378, 5379, 5380, 5381, 5382, 5383, 5384, 5385, 5386, 5387, 5402, 5403, 5404, 5405, 5406, 5407, 5408, 5454, 5456, 5457, 5458, 5459, 5460, 5461, 5462, 5463, 5465, 5466, 5467, 5468, 5469, 5470, 5471, 5472, 5473, 5474, 5475, 5476, 5477, 5478, 5479, 5480, 5481, 5482, 5483, 5484, 5486, 5487, 5495, 5496, 5497, 5498, 5499, 5500, 5501, 5502, 5503, 5504, 5505, 5506, 5507, 5508, 5509, 5510, 5511, 5512, 5513, 5514, 5515, 5516, 5517, 5518, 5519, 5520, 5521, 5522, 5523, 5524, 5525, 5526, 5527, 5528, 5529, 5530, 5531, 5532, 5533, 5534, 5535, 5536, 5537, 5538, 5539, 5540, 5541, 5542, 5543, 5544, 5545, 5546, 5547, 5548, 5549, 5550, 5551, 5552, 5553, 5554, 5556, 5570, 5571, 5572, 5573, 5574, 5575, 5576, 5577, 5595, 5596, 5597, 5598, 5599, 5622, 5644, 5645, 5646, 5684, 5686, 5689, 5690, 5691, 5692, 5693, 5694, 5695, 5696, 5697, 5698, 5699, 5700, 5701, 5702, 5703, 5704, 5705, 5706, 5707, 5708, 5709, 5710, 5711, 5712, 5713, 5714, 5715, 5716, 5717, 5718, 5719, 5720, 5721, 5722, 5723, 5736, 5737, 5738, 5739, 5740, 5741, 5742, 5763, 5764, 5765, 5766, 5786, 5787, 5788, 5789, 5809, 5811, 5812, 5813, 5814, 5834, 5836, 5837, 5838, 5839, 5840, 5841, 5842, 5843, 5844, 5845, 5846, 5847, 5848, 5849, 5850, 5851, 5852, 5853, 5854, 5855, 5856, 5857, 5858, 5859, 5860, 5861, 5862, 5863, 5864, 5865, 5866, 5867, 5868, 5869, 5870, 5871, 5872, 5873, 5874, 5875, 5876, 5877, 5878, 5879, 5880, 5881, 5882, 5889, 5893, 5894, 5895, 5896, 5897, 5915, 5916, 5917, 5918, 5919, 5942, 5943, 5944, 5962, 5964, 5965, 5966, 5967, 5969, 5992, 5993, 5994, 5995, 5996, 5997, 5998, 5999, 6000, 6001, 6002, 6003, 6004, 6005, 6006, 6007, 6008, 6009, 6010, 6011, 6012, 6013, 6014, 6015, 6016, 6017, 6018, 6019, 6020, 6021, 6022, 6023, 6024, 6025, 6026, 6027, 6028, 6029, 6030, 6031, 6032, 6033, 6034, 6035, 6036, 6037, 6038, 6039, 6040, 6041, 6042, 6044, 6057, 6058, 6059, 6060, 6061, 6062, 6063, 6064, 6065, 6084, 6086, 6087, 6088, 6109, 6111, 6123, 6124, 6125, 6126, 6127, 6128, 6129, 6130, 6131, 6132, 6133, 6134, 6146, 6148, 6149, 6150, 6151, 6152, 6153, 6154, 6155, 6156, 6157, 6158, 6159, 6160, 6161, 6162, 6163, 6164, 6165, 6166, 6167, 6168, 6169, 6170, 6171, 6172, 6173, 6174, 6175, 6176, 6177, 6178, 6179, 6180, 6181, 6182, 6183, 6184, 6185, 6186, 6187, 6188, 6189, 6190, 6191, 6192, 6193, 6194, 6195, 6196, 6197, 6198, 6199, 6200, 6201, 6202, 6203, 6204, 6205, 6206, 6207, 6208, 6209, 6216, 6217, 6218, 6219, 6220, 6221, 6222, 6223, 6224, 6225, 6226, 6227, 6228, 6229, 6243, 6244, 6245, 6246, 6247, 6248, 6249, 6250, 6251, 6252, 6268, 6269, 6270, 6271, 6272, 6273, 6274, 6275, 6276, 6277, 6293, 6294, 6295, 6296, 6297, 6298, 6299, 6300, 6316, 6317, 6318, 6319, 6320, 6321, 6322, 6323, 6324, 6325, 6326, 6327, 6328, 6329, 6330, 6331, 6332, 6333, 6334, 6335, 6336, 6337, 6338, 6339, 6340, 6341, 6342, 6343, 6344, 6345, 6346, 6347, 6348, 6349, 6350, 6351, 6352, 6353, 6354, 6355, 6356, 6357, 6358, 6359, 6360, 6361, 6362, 6363, 6364, 6365, 6366, 6367, 6368, 6369, 6370, 6371, 6372, 6373, 6374, 6375, 6376, 6385, 6386, 6387, 6388, 6389, 6390, 6391, 6392, 6393, 6394, 6395, 6396, 6397, 6413, 6414, 6415, 6416, 6417, 6418, 6419, 6420, 6439, 6440, 6441, 6442, 6443, 6460, 6462, 6463, 6464, 6465, 6466, 6484, 6485, 6486, 6487, 6488, 6489, 6490, 6491, 6492, 6493, 6494, 6495, 6496, 6497, 6498, 6499, 6500, 6501, 6502, 6503, 6504, 6505, 6506, 6507, 6508, 6509, 6510, 6511, 6512, 6513, 6514, 6515, 6516, 6517, 6518, 6519, 6520, 6521, 6522, 6523, 6524, 6525, 6526, 6527, 6528, 6529, 6530, 6531, 6532, 6533, 6534, 6535, 6536, 6537, 6538, 6539, 6540, 6541, 6542, 6549, 6550, 6552, 6553, 6554, 6555, 6556, 6557, 6558, 6559, 6560, 6561, 6562, 6563, 6564, 6565, 6566, 6567, 6568, 6569, 6570, 6571, 6572, 6573, 6574, 6575, 6576, 6577, 6578, 6579, 6580, 6581, 6582, 6583, 6584, 6585, 6586, 6587, 6588, 6589, 6590, 6591, 6592, 6593, 6594, 6597, 6598, 6599, 6600, 6601, 6602, 6603, 6604, 6605, 6606, 6607, 6608, 6609, 6610, 6611, 6612, 6613, 6614, 6620, 6621, 6623, 6624, 6625, 6626, 6627, 6628, 6629, 6630, 6631, 6632, 6633, 6634, 6635, 6636, 6638, 6639, 6640, 6646, 6650, 6651, 6652, 6653, 6654, 6655, 6656, 6657, 6658, 6659, 6660, 6661, 6662, 6663, 6664, 6665, 6666, 6667, 6668, 6669, 6670, 6671, 6672, 6673, 6674, 6675, 6676, 6677, 6678, 6679, 6680, 6681, 6682, 6683, 6684, 6685, 6686, 6687, 6688, 6689, 6690, 6691, 6692, 6693, 6694, 6695, 6696, 6697, 6698, 6699, 6700, 6701, 6702, 6703, 6704, 6705, 6706, 6707, 6708, 6709, 6710, 6711, 6712, 6713, 6714, 6715, 6716, 6717, 6718]</t>
         </is>
       </c>
-      <c r="BH2" t="n">
+      <c r="BN2" t="n">
         <v>0.1511879049676026</v>
       </c>
-      <c r="BI2" t="inlineStr">
+      <c r="BO2" t="inlineStr">
         <is>
           <t>{'initial_window': 203, 'window_size': 1680, 'num_trees': 27, 'max_depth': 12}</t>
         </is>
       </c>
-      <c r="BJ2" t="n">
+      <c r="BP2" t="n">
         <v>5.046027642907575</v>
       </c>
-      <c r="BK2" t="inlineStr">
+      <c r="BQ2" t="inlineStr">
         <is>
           <t>[849, 2047, 2115, 2116, 5952, 6109, 6201, 6208, 6945, 7185]</t>
         </is>
       </c>
-      <c r="BL2" t="n">
+      <c r="BR2" t="n">
         <v>0.3749999999999999</v>
       </c>
-      <c r="BM2" t="inlineStr">
+      <c r="BS2" t="inlineStr">
         <is>
           <t>{'AR_window_size': 69, 'differencing-order': 0}</t>
         </is>
       </c>
-      <c r="BN2" t="n">
+      <c r="BT2" t="n">
         <v>147.1378787180874</v>
       </c>
-      <c r="BO2" t="inlineStr">
+      <c r="BU2" t="inlineStr">
         <is>
           <t xml:space="preserve">[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86, 87, 88, 89, 90, 91, 92, 93, 94, 95, 96, 97, 98, 99, 100, 101, 102, 103, 104, 105, 106, 107, 108, 109, 110, 111, 112, 113, 114, 115, 116, 117, 118, 119, 120, 121, 122, 123, 124, 125, 126, 127, 128, 129, 130, 131, 132, 133, 134, 135, 136, 137, 138, 139, 140, 141, 142, 143, 144, 145, 146, 147, 148, 149, 150, 151, 152, 153, 154, 155, 156, 157, 158, 159, 160, 161, 162, 163, 164, 165, 166, 167, 168, 169, 170, 171, 172, 173, 174, 175, 176, 177, 178, 179, 180, 181, 182, 183, 184, 185, 186, 187, 188, 189, 190, 191, 192, 193, 194, 195, 196, 197, 198, 199, 200, 201, 202, 203, 204, 205, 206, 207, 208, 209, 210, 211, 212, 213, 214, 215, 216, 217, 218, 219, 220, 221, 222, 223, 224, 225, 226, 227, 228, 229, 230, 231, 232, 233, 234, 235, 236, 237, 238, 239, 240, 241, 242, 243, 244, 245, 246, 247, 248, 249, 250, 251, 252, 253, 254, 255, 256, 257, 258, 259, 260, 261, 262, 263, 264, 265, 266, 267, 268, 269, 270, 271, 272, 273, 274, 275, 276, 277, 278, 279, 280, 281, 282, 283, 284, 285, 286, 287, 288, 289, 290, 291, 292, 293, 294, 295, 296, 297, 298, 299, 300, 301, 302, 303, 304, 305, 306, 307, 308, 309, 310, 311, 312, 313, 314, 315, 316, 317, 318, 319, 320, 321, 322, 323, 324, 325, 326, 327, 328, 329, 330, 331, 332, 333, 334, 335, 336, 337, 338, 339, 340, 341, 342, 343, 344, 345, 346, 347, 348, 349, 350, 351, 352, 353, 354, 355, 356, 357, 358, 359, 360, 361, 362, 363, 364, 365, 366, 367, 368, 369, 370, 371, 372, 373, 374, 375, 376, 377, 378, 379, 380, 381, 382, 383, 384, 385, 386, 387, 388, 389, 390, 391, 392, 393, 394, 395, 396, 397, 398, 399, 400, 401, 402, 403, 404, 405, 406, 407, 408, 409, 410, 411, 412, 413, 414, 415, 416, 417, 418, 419, 420, 421, 422, 423, 424, 425, 426, 427, 428, 429, 430, 431, 432, 433, 434, 435, 436, 437, 438, 439, 440, 441, 442, 443, 444, 445, 446, 447, 448, 449, 450, 451, 452, 453, 454, 455, 456, 457, 458, 459, 460, 461, 462, 463, 464, 465, 466, 467, 468, 469, 470, 471, 472, 473, 474, 475, 476, 477, 478, 479, 480, 481, 482, 483, 484, 485, 486, 487, 488, 489, 490, 491, 492, 493, 494, 495, 496, 497, 498, 499, 500, 501, 502, 503, 504, 505, 506, 507, 508, 509, 510, 511, 512, 513, 514, 515, 516, 517, 518, 519, 520, 521, 522, 523, 524, 525, 526, 527, 528, 529, 530, 531, 532, 533, 534, 535, 536, 537, 538, 539, 540, 541, 542, 543, 544, 545, 546, 547, 548, 549, 550, 551, 552, 553, 554, 555, 556, 557, 558, 559, 560, 561, 562, 563, 564, 565, 566, 567, 568, 569, 570, 571, 572, 573, 574, 575, 576, 577, 578, 579, 580, 581, 582, 583, 584, 585, 586, 587, 588, 589, 590, 591, 592, 593, 594, 595, 596, 597, 598, 599, 600, 601, 602, 603, 604, 605, 606, 607, 608, 609, 610, 611, 612, 613, 614, 615, 616, 617, 618, 619, 620, 621, 622, 623, 624, 625, 626, 627, 628, 629, 630, 631, 632, 633, 634, 635, 636, 637, 638, 639, 640, 641, 642, 643, 644, 645, 646, 647, 648, 649, 650, 651, 652, 653, 654, 655, 656, 657, 658, 659, 660, 661, 662, 663, 664, 665, 666, 667, 668, 669, 670, 671, 672, 673, 674, 675, 676, 677, 678, 679, 680, 681, 682, 683, 684, 685, 686, 687, 688, 689, 690, 691, 692, 693, 694, 695, 696, 697, 698, 699, 700, 701, 702, 703, 704, 705, 706, 707, 708, 709, 710, 711, 712, 713, 714, 715, 716, 717, 718, 719, 720, 721, 722, 723, 724, 725, 726, 727, 728, 729, 730, 731, 732, 733, 734, 735, 736, 737, 738, 739, 740, 741, 742, 743, 744, 745, 746, 747, 748, 749, 750, 751, 752, 753, 754, 755, 756, 757, 758, 759, 760, 761, 762, 763, 764, 765, 766, 767, 768, 769, 770, 771, 772, 773, 774, 775, 776, 777, 778, 779, 780, 781, 782, 783, 784, 785, 786, 787, 788, 789, 790, 791, 792, 793, 794, 795, 796, 797, 798, 799, 800, 801, 802, 803, 804, 805, 806, 807, 808, 809, 810, 811, 812, 813, 814, 815, 816, 817, 818, 819, 820, 821, 822, 823, 824, 825, 826, 827, 828, 829, 830, 831, 832, 833, 834, 835, 836, 837, 838, 839, 840, 841, 842, 843, 844, 845, 846, 847, 848, 849, 850, 851, 852, 853, 854, 855, 856, 857, 858, 859, 860, 861, 862, 863, 864, 865, 866, 867, 868, 869, 870, 871, 872, 873, 874, 875, 876, 877, 878, 879, 880, 881, 882, 883, 884, 885, 886, 887, 888, 889, 890, 891, 892, 893, 894, 895, 896, 897, 898, 899, 900, 901, 902, 903, 904, 905, 906, 907, 908, 909, 910, 911, 912, 913, 914, 915, 916, 917, 918, 919, 920, 921, 922, 923, 924, 925, 926, 927, 928, 929, 930, 931, 932, 933, 934, 935, 936, 937, 938, 939, 940, 941, 942, 943, 944, 945, 946, 947, 948, 949, 950, 951, 952, 953, 954, 955, 956, 957, 958, 959, 960, 961, 962, 963, 964, 965, 966, 967, 968, 969, 970, 971, 972, 973, 974, 975, 976, 977, 978, 979, 980, 981, 982, 983, 984, 985, 986, 987, 988, 989, 990, 991, 992, 993, 994, 995, 996, 997, 998, 999, 1000, 1001, 1002, 1003, 1004, 1005, 1006, 1007, 1008, 1009, 1010, 1011, 1012, 1013, 1014, 1015, 1016, 1017, 1018, 1019, 1020, 1021, 1022, 1023, 1024, 1025, 1026, 1027, 1028, 1029, 1030, 1031, 1032, 1033, 1034, 1035, 1036, 1037, 1038, 1039, 1040, 1041, 1042, 1043, 1044, 1045, 1046, 1047, 1048, 1049, 1050, 1051, 1052, 1053, 1054, 1055, 1056, 1057, 1058, 1059, 1060, 1061, 1062, 1063, 1064, 1065, 1066, 1067, 1068, 1069, 1070, 1071, 1072, 1073, 1074, 1075, 1076, 1077, 1078, 1079, 1080, 1081, 1082, 1083, 1084, 1085, 1086, 1087, 1088, 1089, 1090, 1091, 1092, 1093, 1094, 1095, 1096, 1097, 1098, 1099, 1100, 1101, 1102, 1103, 1104, 1105, 1106, 1107, 1108, 1109, 1110, 1111, 1112, 1113, 1114, 1115, 1116, 1117, 1118, 1119, 1120, 1121, 1122, 1123, 1124, 1125, 1126, 1127, 1128, 1129, 1130, 1131, 1132, 1133, 1134, 1135, 1136, 1137, 1138, 1139, 1140, 1141, 1142, 1143, 1144, 1145, 1146, 1147, 1148, 1149, 1150, 1151, 1152, 1153, 1154, 1155, 1156, 1157, 1158, 1159, 1160, 1161, 1162, 1163, 1164, 1165, 1166, 1167, 1168, 1169, 1170, 1171, 1172, 1173, 1174, 1175, 1176, 1177, 1178, 1179, 1180, 1181, 1182, 1183, 1184, 1185, 1186, 1187, 1188, 1189, 1190, 1191, 1192, 1193, 1194, 1195, 1196, 1197, 1198, 1199, 1200, 1201, 1202, 1203, 1204, 1205, 1206, 1207, 1208, 1209, 1210, 1211, 1212, 1213, 1214, 1215, 1216, 1217, 1218, 1219, 1220, 1221, 1222, 1223, 1224, 1225, 1226, 1227, 1228, 1229, 1230, 1231, 1232, 1233, 1234, 1235, 1236, 1237, 1238, 1239, 1240, 1241, 1242, 1243, 1244, 1245, 1246, 1247, 1248, 1249, 1250, 1251, 1252, 1253, 1254, 1255, 1256, 1257, 1258, 1259, 1260, 1261, 1262, 1263, 1264, 1265, 1266, 1267, 1268, 1269, 1270, 1271, 1272, 1273, 1274, 1275, 1276, 1277, 1278, 1279, 1280, 1281, 1282, 1283, 1284, 1285, 1286, 1287, 1288, 1289, 1290, 1291, 1292, 1293, 1294, 1295, 1296, 1297, 1298, 1299, 1300, 1301, 1302, 1303, 1304, 1305, 1306, 1307, 1308, 1309, 1310, 1311, 1312, 1313, 1314, 1315, 1316, 1317, 1318, 1319, 1320, 1321, 1322, 1323, 1324, 1325, 1326, 1327, 1328, 1329, 1330, 1331, 1332, 1333, 1334, 1335, 1336, 1337, 1338, 1339, 1340, 1341, 1342, 1343, 1344, 1345, 1346, 1347, 1348, 1349, 1350, 1351, 1352, 1353, 1354, 1355, 1356, 1357, 1358, 1359, 1360, 1361, 1362, 1363, 1364, 1365, 1366, 1367, 1368, 1369, 1370, 1371, 1372, 1373, 1374, 1375, 1376, 1377, 1378, 1379, 1380, 1381, 1382, 1383, 1384, 1385, 1386, 1387, 1388, 1389, 1390, 1391, 1392, 1393, 1394, 1395, 1396, 1397, 1398, 1399, 1400, 1401, 1402, 1403, 1404, 1405, 1406, 1407, 1408, 1409, 1410, 1411, 1412, 1413, 1414, 1415, 1416, 1417, 1418, 1419, 1420, 1421, 1422, 1423, 1424, 1425, 1426, 1427, 1428, 1429, 1430, 1431, 1432, 1433, 1434, 1435, 1436, 1437, 1438, 1439, 1440, 1441, 1442, 1443, 1444, 1445, 1446, 1447, 1448, 1449, 1450, 1451, 1452, 1453, 1454, 1455, 1456, 1457, 1458, 1459, 1460, 1461, 1462, 1463, 1464, 1465, 1466, 1467, 1468, 1469, 1470, 1471, 1472, 1473, 1474, 1475, 1476, 1477, 1478, 1479, 1480, 1481, 1482, 1483, 1484, 1485, 1486, 1487, 1488, 1489, 1490, 1491, 1492, 1493, 1494, 1495, 1496, 1497, 1498, 1499, 1500, 1501, 1502, 1503, 1504, 1505, 1506, 1507, 1508, 1509, 1510, 1511, 1512, 1513, 1514, 1515, 1516, 1517, 1518, 1519, 1520, 1521, 1522, 1523, 1524, 1525, 1526, 1527, 1528, 1529, 1530, 1531, 1532, 1533, 1534, 1535, 1536, 1537, 1538, 1539, 1540, 1542, 1543, 1544, 1545, 1546, 1547, 1548, 1549, 1550, 1551, 1552, 1553, 1554, 1555, 1556, 1557, 1558, 1559, 1560, 1561, 1562, 1563, 1564, 1565, 1566, 1567, 1568, 1569, 1570, 1571, 1572, 1573, 1574, 1575, 1576, 1577, 1578, 1579, 1580, 1581, 1582, 1583, 1584, 1585, 1586, 1587, 1588, 1589, 1590, 1591, 1592, 1593, 1594, 1595, 1596, 1597, 1598, 1599, 1600, 1601, 1602, 1603, 1604, 1605, 1606, 1607, 1608, 1609, 1610, 1611, 1612, 1613, 1614, 1615, 1616, 1617, 1618, 1619, 1620, 1621, 1622, 1623, 1624, 1625, 1626, 1627, 1628, 1629, 1630, 1631, 1632, 1633, 1634, 1635, 1636, 1637, 1638, 1639, 1640, 1641, 1642, 1643, 1644, 1645, 1646, 1647, 1648, 1649, 1650, 1651, 1652, 1653, 1654, 1655, 1656, 1657, 1658, 1659, 1660, 1661, 1662, 1663, 1664, 1665, 1666, 1667, 1668, 1669, 1670, 1671, 1672, 1673, 1674, 1675, 1676, 1677, 1678, 1679, 1680, 1681, 1682, 1683, 1684, 1685, 1686, 1687, 1688, 1689, 1690, 1691, 1692, 1693, 1694, 1695, 1696, 1697, 1698, 1699, 1700, 1701, 1702, 1703, 1704, 1705, 1706, 1707, 1708, 1709, 1710, 1711, 1712, 1713, 1714, 1715, 1716, 1717, 1718, 1719, 1720, 1721, 1722, 1723, 1724, 1725, 1726, 1727, 1728, 1729, 1730, 1731, 1732, 1733, 1734, 1735, 1736, 1737, 1738, 1739, 1740, 1741, 1742, 1743, 1744, 1745, 1746, 1747, 1748, 1749, 1750, 1751, 1752, 1753, 1754, 1755, 1756, 1757, 1758, 1759, 1760, 1761, 1762, 1763, 1764, 1765, 1766, 1767, 1768, 1769, 1770, 1771, 1772, 1773, 1774, 1775, 1776, 1777, 1778, 1779, 1780, 1781, 1782, 1783, 1784, 1785, 1786, 1787, 1788, 1789, 1790, 1791, 1792, 1793, 1794, 1795, 1796, 1797, 1798, 1799, 1800, 1801, 1802, 1803, 1804, 1805, 1806, 1807, 1808, 1809, 1810, 1811, 1812, 1813, 1814, 1815, 1816, 1817, 1818, 1819, 1820, 1821, 1822, 1823, 1824, 1825, 1826, 1827, 1828, 1829, 1830, 1831, 1832, 1833, 1834, 1835, 1836, 1837, 1838, 1839, 1840, 1841, 1842, 1843, 1844, 1845, 1846, 1847, 1848, 1849, 1850, 1851, 1852, 1853, 1854, 1855, 1856, 1857, 1858, 1859, 1860, 1861, 1862, 1863, 1864, 1865, 1866, 1867, 1868, 1869, 1870, 1871, 1872, 1873, 1874, 1875, 1876, 1877, 1878, 1879, 1880, 1881, 1882, 1883, 1884, 1885, 1886, 1887, 1888, 1889, 1890, 1891, 1892, 1893, 1894, 1895, 1896, 1897, 1898, 1899, 1900, 1901, 1902, 1903, 1904, 1905, 1906, 1907, 1908, 1909, 1910, 1911, 1912, 1913, 1914, 1915, 1916, 1917, 1918, 1919, 1920, 1921, 1922, 1923, 1924, 1925, 1926, 1927, 1928, 1929, 1930, 1931, 1932, 1933, 1934, 1935, 1936, 1937, 1938, 1939, 1940, 1941, 1942, 1943, 1944, 1945, 1946, 1947, 1948, 1949, 1950, 1951, 1952, 1953, 1954, 1955, 1956, 1957, 1958, 1959, 1960, 1961, 1962, 1963, 1964, 1965, 1966, 1967, 1968, 1969, 1970, 1971, 1972, 1973, 1974, 1975, 1976, 1977, 1978, 1979, 1980, 1981, 1982, 1983, 1984, 1985, 1986, 1987, 1988, 1989, 1991, 1992, 1993, 1994, 1995, 1996, 1997, 1998, 1999, 2000, 2001, 2002, 2003, 2004, 2005, 2006, 2007, 2008, 2009, 2010, 2011, 2012, 2013, 2014, 2015, 2016, 2017, 2018, 2019, 2020, 2021, 2022, 2023, 2024, 2025, 2026, 2027, 2028, 2029, 2030, 2031, 2032, 2033, 2034, 2035, 2036, 2037, 2038, 2039, 2040, 2041, 2042, 2043, 2044, 2045, 2046, 2047, 2048, 2049, 2050, 2051, 2052, 2053, 2054, 2055, 2056, 2057, 2058, 2059, 2060, 2061, 2062, 2063, 2064, 2065, 2066, 2067, 2068, 2069, 2070, 2071, 2072, 2073, 2074, 2075, 2076, 2077, 2078, 2079, 2080, 2081, 2082, 2083, 2084, 2085, 2086, 2087, 2088, 2089, 2090, 2091, 2092, 2093, 2094, 2095, 2096, 2097, 2098, 2099, 2100, 2101, 2102, 2103, 2104, 2105, 2106, 2107, 2108, 2109, 2110, 2111, 2112, 2113, 2114, 2115, 2116, 2117, 2118, 2119, 2120, 2121, 2122, 2123, 2124, 2125, 2126, 2127, 2128, 2129, 2130, 2131, 2132, 2133, 2134, 2135, 2136, 2137, 2138, 2139, 2140, 2141, 2142, 2143, 2144, 2145, 2146, 2147, 2148, 2149, 2150, 2151, 2152, 2153, 2154, 2155, 2156, 2157, 2158, 2159, 2160, 2161, 2162, 2163, 2164, 2165, 2166, 2167, 2168, 2169, 2170, 2171, 2172, 2173, 2174, 2175, 2176, 2177, 2178, 2179, 2180, 2181, 2182, 2183, 2184, 2185, 2186, 2187, 2188, 2189, 2190, 2191, 2192, 2193, 2194, 2195, 2196, 2197, 2198, 2199, 2200, 2201, 2202, 2203, 2204, 2205, 2206, 2207, 2208, 2209, 2210, 2211, 2212, 2213, 2214, 2215, 2216, 2217, 2218, 2219, 2220, 2221, 2222, 2223, 2224, 2225, 2226, 2227, 2228, 2229, 2230, 2231, 2232, 2233, 2234, 2235, 2236, 2237, 2238, 2239, 2240, 2241, 2242, 2243, 2244, 2245, 2246, 2247, 2248, 2249, 2250, 2251, 2252, 2253, 2254, 2255, 2256, 2257, 2258, 2259, 2260, 2261, 2262, 2263, 2264, 2265, 2266, 2267, 2268, 2269, 2270, 2271, 2272, 2273, 2274, 2275, 2276, 2277, 2278, 2279, 2280, 2281, 2282, 2283, 2284, 2285, 2286, 2287, 2288, 2289, 2290, 2291, 2292, 2293, 2294, 2295, 2296, 2297, 2298, 2299, 2300, 2301, 2302, 2303, 2304, 2305, 2306, 2307, 2309, 2310, 2311, 2312, 2313, 2314, 2315, 2316, 2317, 2318, 2319, 2320, 2321, 2322, 2323, 2324, 2325, 2326, 2327, 2328, 2329, 2330, 2331, 2332, 2333, 2334, 2335, 2336, 2337, 2338, 2339, 2340, 2341, 2342, 2343, 2344, 2345, 2346, 2347, 2348, 2349, 2350, 2351, 2352, 2353, 2354, 2355, 2356, 2357, 2358, 2359, 2360, 2361, 2362, 2363, 2364, 2365, 2366, 2367, 2368, 2369, 2370, 2371, 2372, 2373, 2374, 2375, 2376, 2377, 2378, 2379, 2380, 2381, 2382, 2383, 2384, 2385, 2386, 2387, 2388, 2389, 2390, 2391, 2392, 2393, 2394, 2395, 2396, 2397, 2398, 2399, 2400, 2401, 2402, 2403, 2404, 2405, 2406, 2407, 2408, 2409, 2410, 2411, 2412, 2413, 2414, 2415, 2416, 2417, 2418, 2419, 2420, 2421, 2422, 2423, 2424, 2425, 2426, 2427, 2428, 2429, 2430, 2431, 2432, 2433, 2434, 2435, 2436, 2437, 2438, 2439, 2440, 2441, 2442, 2443, 2444, 2445, 2446, 2447, 2448, 2449, 2450, 2451, 2452, 2453, 2454, 2455, 2456, 2457, 2458, 2459, 2460, 2461, 2462, 2463, 2464, 2465, 2466, 2467, 2468, 2469, 2470, 2471, 2472, 2473, 2474, 2475, 2476, 2477, 2478, 2479, 2480, 2481, 2482, 2483, 2484, 2485, 2486, 2487, 2488, 2489, 2490, 2491, 2492, 2493, 2494, 2495, 2496, 2497, 2498, 2499, 2500, 2501, 2502, 2503, 2504, 2505, 2506, 2507, 2508, 2509, 2510, 2511, 2512, 2513, 2514, 2515, 2516, 2517, 2518, 2519, 2521, 2522, 2523, 2524, 2525, 2526, 2527, 2528, 2529, 2530, 2531, 2532, 2533, 2534, 2535, 2536, 2537, 2538, 2539, 2540, 2541, 2542, 2543, 2544, 2545, 2546, 2547, 2548, 2549, 2550, 2551, 2552, 2553, 2554, 2555, 2556, 2557, 2558, 2559, 2560, 2561, 2562, 2563, 2564, 2565, 2566, 2567, 2568, 2569, 2570, 2571, 2572, 2573, 2574, 2575, 2576, 2577, 2578, 2580, 2581, 2582, 2583, 2584, 2585, 2587, 2588, 2589, 2590, 2591, 2592, 2593, 2594, 2595, 2596, 2597, 2598, 2599, 2600, 2601, 2602, 2603, 2604, 2605, 2606, 2607, 2608, 2609, 2610, 2611, 2612, 2613, 2614, 2615, 2616, 2617, 2618, 2619, 2620, 2621, 2622, 2623, 2624, 2625, 2626, 2627, 2628, 2629, 2630, 2631, 2632, 2633, 2634, 2635, 2636, 2637, 2638, 2639, 2640, 2641, 2642, 2643, 2644, 2645, 2646, 2647, 2648, 2649, 2650, 2651, 2652, 2653, 2654, 2655, 2656, 2657, 2658, 2659, 2660, 2661, 2662, 2663, 2664, 2665, 2666, 2667, 2668, 2669, 2670, 2671, 2672, 2673, 2674, 2675, 2676, 2677, 2678, 2679, 2680, 2681, 2682, 2683, 2684, 2685, 2686, 2687, 2688, 2689, 2690, 2691, 2692, 2693, 2694, 2695, 2696, 2697, 2698, 2699, 2700, 2701, 2702, 2703, 2704, 2705, 2706, 2707, 2708, 2709, 2710, 2711, 2712, 2713, 2714, 2715, 2716, 2717, 2718, 2719, 2720, 2721, 2722, 2723, 2724, 2725, 2726, 2727, 2728, 2729, 2730, 2731, 2732, 2733, 2734, 2735, 2736, 2737, 2738, 2739, 2740, 2741, 2742, 2743, 2744, 2745, 2746, 2747, 2748, 2749, 2750, 2751, 2752, 2753, 2754, 2755, 2756, 2757, 2758, 2759, 2760, 2761, 2762, 2763, 2764, 2765, 2766, 2767, 2768, 2769, 2770, 2771, 2772, 2773, 2774, 2775, 2776, 2777, 2778, 2779, 2780, 2781, 2782, 2783, 2784, 2785, 2786, 2787, 2788, 2789, 2790, 2791, 2792, 2793, 2794, 2795, 2796, 2797, 2798, 2799, 2800, 2801, 2802, 2803, 2804, 2805, 2806, 2807, 2808, 2809, 2810, 2811, 2812, 2813, 2814, 2815, 2816, 2817, 2818, 2819, 2820, 2821, 2822, 2823, 2824, 2825, 2826, 2827, 2828, 2829, 2830, 2831, 2832, 2833, 2834, 2835, 2836, 2837, 2838, 2839, 2840, 2841, 2842, 2843, 2844, 2845, 2846, 2847, 2848, 2849, 2850, 2851, 2852, 2853, 2854, 2855, 2856, 2857, 2858, 2859, 2860, 2861, 2862, 2863, 2864, 2865, 2866, 2867, 2868, 2869, 2870, 2871, 2872, 2873, 2874, 2875, 2876, 2877, 2878, 2879, 2880, 2881, 2882, 2883, 2884, 2885, 2886, 2887, 2888, 2889, 2890, 2891, 2892, 2893, 2894, 2895, 2896, 2897, 2898, 2899, 2900, 2901, 2902, 2903, 2904, 2905, 2906, 2907, 2908, 2909, 2910, 2911, 2912, 2913, 2914, 2915, 2916, 2917, 2918, 2919, 2920, 2921, 2922, 2923, 2924, 2925, 2926, 2927, 2928, 2929, 2930, 2931, 2932, 2933, 2934, 2935, 2936, 2937, 2938, 2939, 2940, 2941, 2942, 2943, 2944, 2945, 2946, 2947, 2948, 2949, 2950, 2951, 2952, 2953, 2954, 2955, 2956, 2957, 2958, 2959, 2960, 2961, 2962, 2963, 2964, 2965, 2966, 2967, 2968, 2969, 2970, 2971, 2972, 2973, 2974, 2975, 2976, 2977, 2978, 2979, 2980, 2981, 2982, 2983, 2985, 2986, 2987, 2988, 2989, 2990, 2991, 2992, 2993, 2994, 2995, 2996, 2997, 2998, 2999, 3000, 3001, 3002, 3003, 3004, 3005, 3006, 3007, 3008, 3009, 3010, 3011, 3012, 3013, 3014, 3015, 3016, 3017, 3018, 3019, 3020, 3021, 3022, 3023, 3024, 3025, 3026, 3027, 3028, 3029, 3030, 3031, 3032, 3033, 3034, 3035, 3036, 3037, 3038, 3039, 3040, 3041, 3042, 3043, 3044, 3045, 3046, 3047, 3048, 3049, 3050, 3051, 3052, 3053, 3054, 3055, 3056, 3057, 3058, 3059, 3060, 3061, 3062, 3063, 3064, 3065, 3066, 3067, 3068, 3069, 3070, 3071, 3072, 3073, 3074, 3075, 3076, 3077, 3078, 3079, 3080, 3081, 3082, 3083, 3084, 3085, 3086, 3087, 3088, 3089, 3090, 3091, 3092, 3093, 3094, 3095, 3096, 3097, 3098, 3099, 3100, 3101, 3102, 3103, 3104, 3105, 3106, 3107, 3108, 3109, 3110, 3111, 3112, 3113, 3114, 3115, 3116, 3117, 3118, 3119, 3120, 3121, 3122, 3123, 3124, 3125, 3126, 3127, 3128, 3129, 3130, 3131, 3132, 3133, 3134, 3135, 3136, 3137, 3138, 3139, 3140, 3141, 3142, 3143, 3144, 3145, 3146, 3147, 3148, 3149, 3150, 3151, 3152, 3153, 3154, 3155, 3156, 3157, 3158, 3159, 3160, 3161, 3162, 3163, 3164, 3165, 3166, 3167, 3168, 3169, 3170, 3171, 3172, 3173, 3174, 3175, 3176, 3177, 3178, 3179, 3180, 3181, 3182, 3183, 3184, 3185, 3186, 3187, 3188, 3189, 3190, 3191, 3192, 3193, 3194, 3195, 3196, 3197, 3198, 3199, 3200, 3201, 3202, 3203, 3204, 3205, 3206, 3207, 3208, 3209, 3210, 3211, 3212, 3213, 3214, 3215, 3216, 3217, 3218, 3219, 3220, 3221, 3222, 3223, 3224, 3225, 3226, 3227, 3228, 3229, 3230, 3231, 3232, 3233, 3234, 3235, 3236, 3237, 3238, 3239, 3240, 3241, 3242, 3243, 3244, 3245, 3246, 3247, 3248, 3249, 3250, 3251, 3252, 3253, 3254, 3255, 3256, 3257, 3258, 3259, 3260, 3261, 3262, 3263, 3264, 3265, 3266, 3267, 3268, 3269, 3270, 3271, 3272, 3273, 3274, 3275, 3276, 3277, 3278, 3279, 3280, 3281, 3282, 3283, 3284, 3285, 3286, 3287, 3288, 3289, 3290, 3291, 3292, 3293, 3294, 3295, 3296, 3297, 3298, 3299, 3300, 3301, 3302, 3303, 3304, 3305, 3306, 3307, 3308, 3309, 3310, 3311, 3312, 3313, 3314, 3315, 3316, 3317, 3318, 3319, 3320, 3321, 3322, 3323, 3324, 3325, 3326, 3327, 3328, 3329, 3330, 3331, 3332, 3333, 3334, 3335, 3336, 3337, 3338, 3339, 3340, 3341, 3342, 3343, 3344, 3345, 3346, 3347, 3348, 3349, 3350, 3351, 3352, 3353, 3354, 3355, 3356, 3357, 3358, 3359, 3360, 3361, 3362, 3363, 3364, 3365, 3366, 3367, 3368, 3369, 3370, 3371, 3372, 3373, 3374, 3375, 3376, 3377, 3378, 3379, 3380, 3381, 3382, 3383, 3384, 3385, 3386, 3387, 3388, 3389, 3390, 3391, 3392, 3393, 3394, 3395, 3396, 3397, 3398, 3399, 3400, 3401, 3402, 3403, 3404, 3405, 3406, 3407, 3408, 3409, 3410, 3411, 3412, 3413, 3414, 3415, 3416, 3417, 3418, 3419, 3420, 3421, 3422, 3423, 3424, 3425, 3426, 3427, 3428, 3429, 3430, 3431, 3432, 3433, 3434, 3435, 3436, 3437, 3438, 3439, 3440, 3441, 3442, 3443, 3444, 3445, 3446, 3447, 3448, 3449, 3450, 3451, 3452, 3453, 3454, 3455, 3456, 3457, 3458, 3459, 3460, 3461, 3462, 3463, 3464, 3465, 3466, 3467, 3468, 3469, 3470, 3471, 3472, 3473, 3474, 3475, 3476, 3477, 3478, 3479, 3480, 3481, 3482, 3483, 3484, 3485, 3486, 3487, 3488, 3489, 3490, 3491, 3492, 3493, 3494, 3495, 3496, 3497, 3498, 3499, 3500, 3501, 3502, 3503, 3504, 3505, 3506, 3507, 3508, 3509, 3510, 3511, 3512, 3513, 3514, 3515, 3516, 3517, 3518, 3519, 3520, 3521, 3522, 3523, 3524, 3525, 3526, 3527, 3528, 3529, 3530, 3531, 3532, 3533, 3534, 3535, 3536, 3537, 3538, 3539, 3540, 3541, 3542, 3543, 3544, 3545, 3546, 3547, 3548, 3549, 3550, 3551, 3552, 3553, 3554, 3555, 3556, 3557, 3558, 3559, 3560, 3561, 3562, 3563, 3564, 3565, 3566, 3567, 3568, 3569, 3570, 3571, 3572, 3573, 3574, 3575, 3576, 3577, 3578, 3579, 3580, 3581, 3582, 3583, 3584, 3585, 3586, 3587, 3588, 3589, 3590, 3591, 3592, 3593, 3594, 3595, 3596, 3597, 3598, 3599, 3600, 3601, 3602, 3603, 3604, 3605, 3606, 3607, 3608, 3609, 3610, 3611, 3612, 3613, 3614, 3615, 3616, 3617, 3618, 3619, 3620, 3621, 3622, 3623, 3624, 3625, 3626, 3627, 3628, 3629, 3630, 3631, 3632, 3633, 3634, 3635, 3636, 3637, 3638, 3639, 3640, 3641, 3642, 3643, 3644, 3645, 3646, 3647, 3648, 3649, 3650, 3651, 3652, 3653, 3654, 3655, 3656, 3657, 3658, 3659, 3660, 3661, 3662, 3663, 3664, 3665, 3666, 3667, 3668, 3669, 3670, 3671, 3672, 3673, 3674, 3675, 3676, 3677, 3678, 3679, 3680, 3681, 3682, 3683, 3684, 3685, 3686, 3687, 3688, 3689, 3690, 3691, 3692, 3693, 3694, 3695, 3696, 3697, 3698, 3699, 3700, 3701, 3702, 3703, 3704, 3705, 3706, 3707, 3708, 3709, 3710, 3711, 3712, 3713, 3714, 3715, 3716, 3717, 3718, 3719, 3720, 3721, 3722, 3723, 3724, 3725, 3726, 3727, 3728, 3729, 3730, 3731, 3732, 3733, 3734, 3735, 3736, 3737, 3738, 3739, 3740, 3741, 3742, 3743, 3744, 3745, 3746, 3747, 3748, 3749, 3750, 3751, 3752, 3753, 3754, 3755, 3756, 3757, 3758, 3759, 3760, 3761, 3762, 3763, 3764, 3765, 3766, 3767, 3768, 3769, 3770, 3771, 3772, 3773, 3774, 3775, 3776, 3777, 3778, 3779, 3780, 3781, 3782, 3783, 3784, 3785, 3786, 3787, 3788, 3789, 3790, 3791, 3792, 3793, 3794, 3795, 3796, 3797, 3798, 3799, 3800, 3801, 3802, 3803, 3804, 3805, 3806, 3807, 3808, 3809, 3810, 3811, 3812, 3813, 3814, 3815, 3816, 3817, 3818, 3819, 3820, 3821, 3822, 3823, 3824, 3825, 3826, 3827, 3828, 3829, 3830, 3831, 3832, 3833, 3834, 3835, 3836, 3837, 3838, 3839, 3840, 3841, 3842, 3843, 3844, 3845, 3846, 3847, 3848, 3849, 3850, 3851, 3852, 3853, 3854, 3855, 3856, 3857, 3858, 3859, 3860, 3861, 3862, 3863, 3864, 3865, 3866, 3867, 3868, 3869, 3870, 3871, 3872, 3873, 3874, 3875, 3876, 3877, 3878, 3879, 3880, 3881, 3882, 3883, 3884, 3885, 3886, 3887, 3888, 3889, 3890, 3891, 3892, 3893, 3894, 3895, 3896, 3897, 3898, 3899, 3900, 3901, 3902, 3903, 3904, 3905, 3906, 3907, 3908, 3909, 3910, 3911, 3912, 3913, 3914, 3915, 3916, 3917, 3918, 3919, 3920, 3921, 3922, 3923, 3924, 3925, 3926, 3927, 3928, 3929, 3930, 3931, 3932, 3933, 3934, 3935, 3936, 3937, 3938, 3939, 3940, 3941, 3942, 3943, 3944, 3945, 3946, 3947, 3948, 3949, 3950, 3951, 3952, 3953, 3954, 3955, 3956, 3957, 3958, 3959, 3960, 3961, 3962, 3963, 3964, 3965, 3966, 3967, 3968, 3969, 3970, 3971, 3972, 3973, 3974, 3975, 3976, 3977, 3978, 3979, 3980, 3981, 3982, 3983, 3984, 3985, 3986, 3987, 3988, 3989, 3990, 3991, 3992, 3993, 3994, 3995, 3996, 3997, 3998, 3999, 4000, 4001, 4002, 4003, 4004, 4005, 4006, 4007, 4008, 4009, 4010, 4011, 4012, 4013, 4014, 4015, 4016, 4017, 4018, 4019, 4020, 4021, 4022, 4023, 4024, 4025, 4026, 4027, 4028, 4029, 4030, 4031, 4032, 4033, 4034, 4035, 4036, 4037, 4038, 4039, 4040, 4041, 4042, 4043, 4044, 4045, 4046, 4047, 4048, 4049, 4050, 4051, 4052, 4053, 4054, 4055, 4056, 4057, 4059, 4060, 4061, 4062, 4063, 4064, 4065, 4066, 4067, 4068, 4069, 4070, 4071, 4072, 4073, 4075, 4076, 4077, 4078, 4079, 4080, 4081, 4082, 4083, 4084, 4085, 4086, 4087, 4088, 4089, 4090, 4091, 4092, 4093, 4094, 4095, 4096, 4097, 4098, 4099, 4100, 4101, 4102, 4103, 4104, 4105, 4106, 4107, 4108, 4109, 4110, 4111, 4112, 4113, 4114, 4115, 4116, 4117, 4118, 4119, 4120, 4121, 4122, 4123, 4124, 4125, 4126, 4127, 4128, 4129, 4130, 4131, 4132, 4133, 4134, 4135, 4136, 4137, 4138, 4139, 4140, 4141, 4142, 4143, 4144, 4145, 4146, 4147, 4148, 4149, 4150, 4151, 4152, 4153, 4154, 4155, 4156, 4157, 4158, 4159, 4160, 4161, 4162, 4163, 4164, 4165, 4166, 4167, 4168, 4169, 4170, 4172, 4173, 4174, 4175, 4176, 4177, 4178, 4179, 4180, 4181, 4182, 4183, 4184, 4185, 4186, 4187, 4188, 4189, 4190, 4191, 4192, 4193, 4194, 4195, 4196, 4197, 4198, 4199, 4200, 4201, 4202, 4203, 4204, 4205, 4206, 4207, 4208, 4209, 4210, 4211, 4212, 4213, 4214, 4215, 4216, 4218, 4219, 4220, 4221, 4222, 4223, 4224, 4225, 4226, 4227, 4228, 4229, 4230, 4231, 4232, 4233, 4234, 4235, 4236, 4237, 4238, 4239, 4240, 4241, 4242, 4243, 4244, 4245, 4246, 4247, 4248, 4249, 4250, 4251, 4252, 4253, 4254, 4255, 4256, 4257, 4258, 4259, 4260, 4261, 4262, 4263, 4264, 4265, 4266, 4267, 4268, 4269, 4270, 4271, 4272, 4273, 4274, 4275, 4276, 4277, 4278, 4279, 4280, 4281, 4282, 4283, 4284, 4285, 4286, 4287, 4288, 4289, 4290, 4291, 4292, 4293, 4294, 4295, 4296, 4297, 4298, 4299, 4300, 4301, 4302, 4303, 4304, 4305, 4306, 4307, 4308, 4309, 4310, 4311, 4312, 4313, 4314, 4315, 4316, 4317, 4318, 4319, 4320, 4321, 4322, 4323, 4324, 4325, 4326, 4327, 4328, 4329, 4330, 4331, 4332, 4333, 4334, 4335, 4336, 4337, 4338, 4339, 4340, 4341, 4342, 4343, 4344, 4345, 4346, 4347, 4348, 4349, 4350, 4351, 4352, 4353, 4354, 4355, 4356, 4357, 4358, 4359, 4360, 4361, 4362, 4363, 4364, 4365, 4366, 4367, 4368, 4369, 4370, 4371, 4372, 4373, 4374, 4375, 4376, 4377, 4378, 4379, 4380, 4381, 4382, 4383, 4384, 4385, 4386, 4387, 4388, 4389, 4390, 4391, 4392, 4393, 4394, 4395, 4396, 4397, 4398, 4399, 4400, 4401, 4402, 4403, 4404, 4405, 4406, 4407, 4408, 4409, 4410, 4411, 4412, 4413, 4414, 4415, 4416, 4417, 4418, 4419, 4420, 4421, 4422, 4423, 4424, 4425, 4426, 4427, 4428, 4429, 4430, 4431, 4432, 4433, 4434, 4435, 4436, 4437, 4438, 4439, 4440, 4441, 4442, 4443, 4444, 4445, 4446, 4447, 4448, 4449, 4450, 4451, 4452, 4453, 4454, 4455, 4456, 4457, 4458, 4459, 4460, 4461, 4462, 4463, 4464, 4465, 4466, 4467, 4468, 4469, 4470, 4471, 4472, 4473, 4474, 4475, 4476, 4477, 4478, 4479, 4480, 4481, 4482, 4483, 4484, 4486, 4487, 4488, 4489, 4490, 4491, 4492, 4493, 4494, 4495, 4496, 4497, 4498, 4499, 4500, 4501, 4502, 4503, 4504, 4505, 4506, 4507, 4508, 4509, 4510, 4511, 4512, 4513, 4514, 4515, 4516, 4517, 4518, 4519, 4520, 4521, 4522, 4523, 4524, 4525, 4526, 4527, 4528, 4529, 4530, 4531, 4532, 4533, 4534, 4535, 4536, 4537, 4538, 4539, 4540, 4541, 4542, 4543, 4544, 4545, 4546, 4547, 4548, 4549, 4550, 4551, 4552, 4553, 4554, 4555, 4556, 4557, 4558, 4559, 4560, 4561, 4562, 4563, 4564, 4565, 4566, 4567, 4568, 4569, 4570, 4571, 4572, 4573, 4574, 4575, 4576, 4577, 4578, 4579, 4580, 4581, 4582, 4583, 4584, 4585, 4586, 4587, 4588, 4589, 4590, 4591, 4592, 4593, 4594, 4595, 4596, 4597, 4598, 4599, 4600, 4601, 4602, 4603, 4604, 4605, 4606, 4607, 4608, 4609, 4610, 4611, 4612, 4613, 4614, 4615, 4616, 4617, 4618, 4619, 4620, 4621, 4622, 4623, 4624, 4625, 4626, 4627, 4628, 4629, 4630, 4631, 4632, 4633, 4634, 4635, 4636, 4637, 4638, 4639, 4640, 4641, 4642, 4643, 4644, 4645, 4646, 4647, 4648, 4649, 4650, 4651, 4652, 4653, 4654, 4655, 4656, 4657, 4658, 4659, 4660, 4661, 4662, 4663, 4664, 4665, 4666, 4667, 4668, 4669, 4670, 4671, 4672, 4673, 4674, 4675, 4676, 4677, 4678, 4679, 4680, 4681, 4682, 4683, 4684, 4685, 4686, 4687, 4688, 4689, 4690, 4691, 4692, 4693, 4694, 4695, 4696, 4697, 4698, 4699, 4700, 4701, 4702, 4703, 4704, 4705, 4706, 4707, 4708, 4709, 4710, 4711, 4712, 4713, 4714, 4715, 4716, 4717, 4718, 4719, 4720, 4721, 4722, 4723, 4724, 4725, 4726, 4727, 4728, 4729, 4730, 4731, 4732, 4733, 4734, 4735, 4736, 4737, 4738, 4739, 4740, 4741, 4742, 4743, 4744, 4745, 4746, 4747, 4748, 4749, 4750, 4751, 4752, 4753, 4754, 4755, 4756, 4757, 4758, 4759, 4760, 4761, 4762, 4763, 4764, 4765, 4766, 4767, 4768, 4769, 4770, 4771, 4772, 4773, 4774, 4775, 4776, 4777, 4778, 4779, 4780, 4781, 4782, 4783, 4784, 4785, 4786, 4787, 4788, 4789, 4790, 4791, 4792, 4793, 4794, 4795, 4796, 4797, 4798, 4799, 4800, 4801, 4802, 4803, 4804, 4805, 4806, 4807, 4808, 4809, 4810, 4811, 4812, 4813, 4814, 4815, 4816, 4817, 4818, 4819, 4820, 4821, 4822, 4823, 4824, 4825, 4826, 4827, 4828, 4829, 4830, 4831, 4832, 4833, 4834, 4835, 4836, 4837, 4838, 4839, 4840, 4841, 4842, 4843, 4844, 4845, 4846, 4847, 4848, 4849, 4850, 4851, 4852, 4853, 4854, 4855, 4856, 4857, 4858, 4859, 4860, 4861, 4862, 4863, 4864, 4865, 4866, 4867, 4868, 4869, 4870, 4871, 4872, 4873, 4874, 4875, 4876, 4877, 4878, 4879, 4880, 4881, 4882, 4883, 4884, 4885, 4886, 4887, 4888, 4889, 4890, 4891, 4892, 4893, 4894, 4895, 4896, 4897, 4898, 4899, 4900, 4901, 4902, 4903, 4904, 4905, 4906, 4907, 4908, 4909, 4910, 4911, 4912, 4913, 4914, 4915, 4916, 4917, 4918, 4919, 4920, 4921, 4922, 4923, 4924, 4925, 4926, 4927, 4928, 4929, 4930, 4931, 4932, 4933, 4934, 4935, 4936, 4937, 4938, 4939, 4940, 4941, 4942, 4943, 4944, 4945, 4946, 4947, 4948, 4949, 4950, 4951, 4952, 4953, 4954, 4955, 4956, 4957, 4958, 4959, 4960, 4961, 4962, 4963, 4964, 4965, 4966, 4967, 4968, 4969, 4970, 4971, 4972, 4973, 4974, 4975, 4976, 4977, 4978, 4979, 4980, 4981, 4982, 4983, 4984, 4985, 4986, 4987, 4988, 4989, 4990, 4991, 4992, 4993, 4994, 4995, 4996, 4997, 4998, 4999, 5000, 5001, 5002, 5003, 5004, 5005, 5006, 5007, 5008, 5009, 5010, 5011, 5012, 5013, 5014, 5015, 5016, 5017, 5018, 5019, 5020, 5021, 5022, 5023, 5024, 5025, 5026, 5027, 5028, 5029, 5030, 5031, 5032, 5033, 5034, 5035, 5036, 5037, 5038, 5039, 5040, 5041, 5042, 5043, 5044, 5045, 5046, 5047, 5048, 5049, 5050, 5051, 5052, 5053, 5054, 5055, 5056, 5057, 5058, 5059, 5060, 5061, 5062, 5063, 5064, 5065, 5066, 5067, 5068, 5069, 5070, 5071, 5072, 5073, 5074, 5075, 5076, 5077, 5078, 5079, 5080, 5081, 5082, 5083, 5084, 5085, 5086, 5087, 5088, 5089, 5090, 5091, 5092, 5093, 5094, 5095, 5096, 5097, 5098, 5099, 5100, 5101, 5102, 5103, 5104, 5105, 5106, 5107, 5108, 5109, 5110, 5111, 5112, 5113, 5114, 5115, 5116, 5117, 5118, 5119, 5120, 5121, 5122, 5123, 5124, 5125, 5126, 5127, 5128, 5129, 5130, 5131, 5132, 5133, 5134, 5135, 5136, 5137, 5138, 5139, 5140, 5141, 5142, 5143, 5144, 5145, 5146, 5147, 5148, 5149, 5150, 5151, 5152, 5153, 5154, 5155, 5156, 5157, 5158, 5159, 5160, 5161, 5162, 5163, 5164, 5165, 5166, 5167, 5168, 5169, 5170, 5171, 5172, 5173, 5174, 5175, 5176, 5177, 5178, 5179, 5180, 5181, 5182, 5183, 5184, 5185, 5186, 5187, 5188, 5189, 5190, 5191, 5192, 5193, 5194, 5195, 5196, 5197, 5198, 5199, 5200, 5201, 5202, 5203, 5204, 5205, 5206, 5207, 5208, 5209, 5210, 5211, 5212, 5213, 5214, 5215, 5217, 5218, 5219, 5220, 5221, 5222, 5223, 5224, 5225, 5226, 5227, 5228, 5229, 5230, 5231, 5232, 5233, 5234, 5235, 5236, 5237, 5238, 5239, 5240, 5241, 5242, 5243, 5244, 5245, 5246, 5247, 5248, 5249, 5250, 5251, 5252, 5253, 5254, 5255, 5256, 5257, 5258, 5259, 5260, 5261, 5262, 5263, 5264, 5265, 5266, 5267, 5268, 5269, 5270, 5271, 5272, 5273, 5274, 5275, 5276, 5277, 5278, 5279, 5280, 5281, 5282, 5283, 5284, 5285, 5286, 5287, 5288, 5289, 5290, 5291, 5292, 5293, 5294, 5295, 5296, 5297, 5298, 5299, 5300, 5301, 5302, 5303, 5304, 5305, 5306, 5307, 5308, 5309, 5310, 5311, 5312, 5313, 5314, 5315, 5316, 5317, 5318, 5319, 5320, 5321, 5322, 5323, 5324, 5325, 5326, 5328, 5329, 5330, 5331, 5332, 5333, 5334, 5335, 5336, 5337, 5338, 5339, 5340, 5341, 5342, 5343, 5344, 5345, 5346, 5347, 5348, 5349, 5350, 5351, 5352, 5353, 5354, 5355, 5356, 5357, 5358, 5359, 5360, 5361, 5362, 5363, 5364, 5365, 5366, 5367, 5368, 5369, 5370, 5371, 5372, 5373, 5374, 5375, 5376, 5377, 5378, 5379, 5380, 5381, 5382, 5383, 5384, 5385, 5386, 5387, 5388, 5389, 5390, 5391, 5392, 5393, 5394, 5395, 5396, 5397, 5398, 5399, 5400, 5401, 5402, 5403, 5404, 5405, 5406, 5407, 5408, 5409, 5410, 5411, 5412, 5413, 5414, 5415, 5416, 5417, 5418, 5419, 5420, 5421, 5422, 5423, 5424, 5425, 5426, 5427, 5428, 5429, 5430, 5431, 5432, 5433, 5434, 5435, 5436, 5437, 5438, 5439, 5440, 5441, 5442, 5443, 5444, 5445, 5446, 5447, 5448, 5449, 5450, 5451, 5452, 5453, 5454, 5456, 5457, 5458, 5459, 5460, 5461, 5462, 5463, 5464, 5465, 5466, 5467, 5468, 5469, 5470, 5471, 5472, 5473, 5474, 5475, 5476, 5477, 5478, 5479, 5480, 5481, 5482, 5483, 5484, 5485, 5486, 5487, 5488, 5489, 5490, 5491, 5492, 5493, 5494, 5495, 5496, 5497, 5498, 5499, 5500, 5501, 5502, 5503, 5504, 5505, 5506, 5507, 5508, 5509, 5510, 5511, 5512, 5513, 5514, 5515, 5516, 5517, 5518, 5519, 5520, 5521, 5522, 5523, 5524, 5525, 5526, 5527, 5528, 5529, 5530, 5531, 5532, 5533, 5534, 5535, 5536, 5537, 5538, 5539, 5540, 5541, 5542, 5543, 5544, 5545, 5546, 5547, 5548, 5549, 5550, 5551, 5552, 5553, 5554, 5555, 5556, 5557, 5558, 5559, 5560, 5561, 5562, 5563, 5564, 5565, 5566, 5567, 5568, 5569, 5570, 5571, 5572, 5573, 5574, 5575, 5576, 5577, 5578, 5579, 5580, 5581, 5582, 5583, 5584, 5585, 5586, 5587, 5588, 5589, 5590, 5591, 5592, 5593, 5594, 5595, 5596, 5597, 5598, 5599, 5600, 5601, 5602, 5603, 5604, 5605, 5606, 5607, 5608, 5609, 5610, 5611, 5612, 5613, 5614, 5615, 5616, 5617, 5618, 5619, 5620, 5621, 5622, 5623, 5624, 5625, 5626, 5627, 5628, 5629, 5630, 5631, 5632, 5633, 5634, 5635, 5636, 5637, 5638, 5639, 5640, 5641, 5642, 5643, 5644, 5645, 5646, 5647, 5648, 5649, 5650, 5651, 5652, 5653, 5654, 5655, 5656, 5657, 5658, 5660, 5661, </t>
         </is>
       </c>
-      <c r="BP2" t="n">
+      <c r="BV2" t="n">
         <v>0.07643312101910829</v>
       </c>
-      <c r="BQ2" t="inlineStr">
+      <c r="BW2" t="inlineStr">
         <is>
           <t>{'Numk': 31, 'KPar': 8, 'Bucket_index': 1000}</t>
         </is>
       </c>
-      <c r="BR2" t="n">
+      <c r="BX2" t="n">
         <v>193.3085851250216</v>
       </c>
-      <c r="BS2" t="inlineStr">
+      <c r="BY2" t="inlineStr">
         <is>
           <t>no</t>
         </is>
       </c>
-      <c r="BT2" t="n">
-        <v>0</v>
-      </c>
-      <c r="BU2" t="inlineStr">
+      <c r="BZ2" t="n">
+        <v>0</v>
+      </c>
+      <c r="CA2" t="inlineStr">
         <is>
           <t>params</t>
         </is>
       </c>
-      <c r="BV2" t="n">
+      <c r="CB2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1198,93 +1246,111 @@
       <c r="AY3" t="n">
         <v>1</v>
       </c>
-      <c r="AZ3" t="inlineStr"/>
-      <c r="BA3" t="inlineStr">
+      <c r="AZ3" t="n">
+        <v>1</v>
+      </c>
+      <c r="BA3" t="n">
+        <v>1</v>
+      </c>
+      <c r="BB3" t="n">
+        <v>1</v>
+      </c>
+      <c r="BC3" t="n">
+        <v>1</v>
+      </c>
+      <c r="BD3" t="n">
+        <v>1</v>
+      </c>
+      <c r="BE3" t="n">
+        <v>1</v>
+      </c>
+      <c r="BF3" t="inlineStr"/>
+      <c r="BG3" t="inlineStr">
         <is>
           <t>nab-data/realKnownCause/cpu_utilization_asg_misconfiguration.csv</t>
         </is>
       </c>
-      <c r="BB3" t="n">
+      <c r="BH3" t="n">
         <v>18050</v>
       </c>
-      <c r="BC3" t="inlineStr">
+      <c r="BI3" t="inlineStr">
         <is>
           <t>NAB</t>
         </is>
       </c>
-      <c r="BD3" t="n">
-        <v>1</v>
-      </c>
-      <c r="BE3" t="inlineStr">
+      <c r="BJ3" t="n">
+        <v>1</v>
+      </c>
+      <c r="BK3" t="inlineStr">
         <is>
           <t>16551</t>
         </is>
       </c>
-      <c r="BF3" t="n">
+      <c r="BL3" t="n">
         <v>1498</v>
       </c>
-      <c r="BG3" t="inlineStr">
-        <is>
-          <t>[1, 3, 34, 551, 623, 779, 791, 803, 815, 863, 875, 935, 947, 1031, 1151, 1163, 1211, 1247, 1271, 1295, 1307, 1319, 1355, 1379, 1463, 1487, 1619, 1643, 1703, 2412, 2424, 2436, 2459, 2472, 2496, 2532, 2544, 2556, 2568, 2580, 2592, 2604, 2616, 2628, 2640, 2664, 2676, 2700, 2712, 2736, 2748, 2760, 2772, 2784, 2808, 2820, 2833, 2917, 3395, 3407, 3443, 3467, 3479, 3491, 3515, 3527, 3575, 3599, 3611, 3659, 3683, 3695, 3707, 3719, 3731, 3755, 3779, 3803, 3827, 3863, 3875, 3971, 3995, 4019, 4043, 4067, 4091, 4103, 4115, 4127, 4139, 4151, 4163, 4175, 4187, 4199, 4211, 4247, 4271, 4283, 4295, 4307, 4439, 4451, 4511, 4523, 4535, 4547, 4559, 4583, 4593, 4596, 4597, 4607, 4619, 4655, 4679, 4703, 4727, 4739, 4751, 4763, 4775, 4787, 4799, 4823, 4835, 4871, 4907, 4919, 4931, 4943, 4955, 4967, 4979, 4991, 5003, 5015, 5027, 5051, 5063, 5087, 5099, 5111, 5123, 5135, 5159, 5171, 5183, 5195, 5207, 5219, 5243, 5267, 5279, 5303, 5315, 5351, 5363, 5375, 5399, 5435, 5459, 5471, 5519, 5531, 5543, 5555, 5567, 5579, 5591, 5639, 5723, 5735, 5747, 5759, 5771, 5783, 5795, 5819, 5831, 5843, 5855, 5867, 5879, 5939, 5949, 5952, 6359, 6647, 6779, 6803, 6815, 6827, 6839, 6851, 6863, 6875, 6887, 6923, 6935, 6947, 6959, 6983, 7055, 7103, 7127, 7139, 7187, 7211, 7247, 7271, 7295, 7307, 7331, 7367, 7403, 7427, 7451, 7475, 7499, 7511, 7535, 7559, 7571, 7583, 7595, 7619, 7631, 7655, 8007, 8013, 8016, 8227, 8230, 8231, 8243, 8255, 8259, 8260, 8267, 8279, 8291, 8303, 8307, 8308, 8309, 8312, 8327, 8339, 8363, 8379, 8387, 8399, 8411, 8435, 8495, 8531, 8543, 8567, 8615, 8651, 8663, 8675, 8699, 8735, 8747, 8771, 8783, 8795, 8807, 8831, 8843, 8855, 8867, 8879, 8915, 8949, 8951, 8952, 8954, 8958, 8963, 8975, 8987, 8999, 9023, 9047, 9059, 9071, 9083, 9095, 9107, 9119, 9131, 9143, 9154, 9155, 9158, 9161, 9163, 9165, 9635, 9659, 9695, 9707, 9719, 9731, 9743, 9755, 9767, 9779, 9791, 9803, 9815, 9827, 9839, 9863, 9875, 9887, 9899, 9911, 9923, 9935, 9947, 9971, 9983, 9995, 10007, 10019, 10031, 10043, 10079, 10103, 10127, 10163, 10175, 10199, 10211, 10223, 10235, 10247, 10271, 10307, 10319, 10343, 10355, 10367, 10379, 10391, 10463, 10475, 10487, 10499, 10535, 10583, 10595, 10607, 10691, 10715, 10739, 10751, 10763, 10775, 10787, 10799, 10811, 10823, 10835, 10847, 10859, 10871, 10877, 10895, 10907, 10919, 10931, 10955, 10979, 11039, 11063, 11075, 11171, 11231, 11315, 11447, 11531, 11579, 11615, 11712, 11723, 11733, 11736, 11769, 11783, 11807, 11843, 11927, 11975, 12023, 12035, 12047, 12059, 12095, 12119, 12131, 12143, 12191, 12203, 12215, 12239, 12251, 12263, 12275, 12323, 12347, 12359, 12371, 12383, 12395, 12407, 12431, 12443, 12467, 12479, 12503, 12515, 12527, 12539, 12551, 12552, 12563, 12575, 12579, 12587, 12611, 12623, 12635, 12647, 12659, 12671, 12683, 12707, 12719, 12731, 12743, 12755, 12767, 12791, 12803, 12815, 12827, 12851, 12863, 12875, 12887, 12888, 12899, 12911, 12923, 12947, 12971, 13007, 13055, 13067, 13091, 13103, 13127, 13139, 13151, 13163, 13175, 13187, 13199, 13211, 13223, 13247, 13259, 13272, 13284, 13331, 13332, 13343, 13355, 13367, 13379, 13403, 13415, 13439, 13451, 13463, 13475, 13487, 13499, 13500, 13523, 13524, 13535, 13547, 13559, 13571, 13595, 13619, 13655, 13667, 13691, 13715, 13728, 13776, 13932, 14022, 14028, 14112, 14160, 14172, 14196, 14208, 14220, 14232, 14256, 14268, 14292, 14303, 14328, 14364, 14388, 14399, 14424, 14436, 14447, 14459, 14471, 14496, 14508, 14520, 14532, 14544, 14555, 14568, 14580, 14592, 14616, 14628, 14652, 14663, 14676, 14688, 14699, 14711, 14724, 14736, 14748, 14760, 14796, 14820, 14832, 14855, 14868, 14880, 14892, 14904, 14916, 14928, 14940, 14952, 14964, 14987, 15000, 15024, 15048, 15072, 15084, 15096, 15108, 15120, 15132, 15156, 15168, 15180, 15191, 15204, 15215, 15240, 15251, 15264, 15275, 15288, 15324, 15336, 15360, 15372, 15396, 15420, 15431, 15444, 15455, 15468, 15480, 15492, 15503, 15516, 15528, 15563, 15576, 15588, 15612, 15623, 15636, 15660, 15672, 15684, 15696, 15707, 15731, 15744, 15768, 15780, 15828, 15840, 15852, 15876, 15888, 15900, 15912, 15923, 15936, 15948, 15960, 15984, 15996, 16008, 16031, 16044, 16056, 16068, 16079, 16091, 16104, 16116, 16128, 16140, 16152, 16176, 16188, 16212, 16224, 16236, 16248, 16260, 16272, 16331, 16355, 16368, 16380, 16392, 16403, 16416, 16427, 16440, 16451, 16464, 16476, 16487, 16500, 16511, 16524, 16536, 16547, 16560, 16571, 16596, 16608, 16619, 16631, 16644, 16655, 16668, 16680, 16692, 16716, 16727, 16740, 16752, 16872, 16884, 16896, 16908, 16920, 16944, 16956, 16968, 16980, 16992, 16993, 16994, 16997, 16998, 16999, 17000, 17001, 17003, 17004, 17005, 17007, 17008, 17009, 17010, 17011, 17013, 17015, 17016, 17019, 17021, 17022, 17025, 17027, 17031, 17032, 17033, 17035, 17036, 17037, 17038, 17041, 17048, 17049, 17050, 17052, 17055, 17056, 17057, 17061, 17062, 17064, 17065, 17068, 17069, 17070, 17073, 17075, 17076, 17081, 17083, 17084, 17085, 17087, 17089, 17090, 17091, 17093, 17095, 17096, 17100, 17101, 17102, 17103, 17104, 17105, 17109, 17110, 17115, 17120, 17121, 17122, 17125, 17126, 17127, 17128, 17129, 17132, 17133, 17134, 17135, 17136, 17139, 17141, 17143, 17145, 17146, 17147, 17148, 17151, 17153, 17155, 17156, 17157, 17159, 17160, 17161, 17162, 17165, 17167, 17168, 17169, 17170, 17172, 17173, 17175, 17176, 17181, 17182, 17184, 17187, 17190, 17191, 17196, 17197, 17199, 17200, 17201, 17206, 17207, 17208, 17211, 17213, 17214, 17215, 17217, 17219, 17220, 17225, 17226, 17227, 17229, 17231, 17232, 17233, 17235, 17236, 17237, 17238, 17239, 17241, 17242, 17243, 17244, 17247, 17248, 17252, 17253, 17255, 17256, 17259, 17260, 17261, 17262, 17263, 17273, 17275, 17277, 17279, 17280, 17281, 17285, 17286, 17287, 17288, 17289, 17293, 17295, 17297, 17301, 17302, 17303, 17304, 17307, 17312, 17313, 17315, 17316, 17320, 17321, 17322, 17323, 17325, 17327, 17328, 17331, 17337, 17339, 17340, 17343, 17344, 17349, 17350, 17351, 17352, 17355, 17356, 17357, 17359, 17360, 17361, 17362, 17367, 17368, 17369, 17370, 17371, 17381, 17382, 17387, 17388, 17389, 17390, 17393, 17395, 17399, 17401, 17402, 17403, 17404, 17407, 17409, 17410, 17411, 17412, 17415, 17416, 17421, 17423, 17424, 17425, 17427, 17428, 17429, 17430, 17431, 17433, 17435, 17436, 17438, 17439, 17443, 17446, 17448, 17449, 17461, 17462, 17465, 17467, 17468, 17469, 17471, 17472, 17473, 17474, 17479, 17480, 17481, 17484, 17486, 17487, 17488, 17489, 17493, 17494, 17495, 17496, 17499, 17501, 17502, 17503, 17507, 17508, 17509, 17510, 17513, 17515, 17516, 17521, 17522, 17523, 17524, 17525, 17527, 17528, 17530, 17531, 17533, 17534, 17538, 17539, 17540, 17543, 17544, 17545, 17546, 17547, 17549, 17550, 17551, 17552, 17553, 17555, 17556, 17557, 17558, 17559, 17561, 17563, 17564, 17565, 17567, 17569, 17570, 17573, 17575, 17576, 17581, 17582, 17587, 17588, 17593, 17596, 17597, 17599, 17600, 17601, 17602, 17603, 17604, 17607, 17608, 17613, 17616, 17617, 17620, 17621, 17622, 17633, 17635, 17636, 17639, 17640, 17641, 17642, 17643, 17645, 17647, 17648, 17651, 17652, 17653, 17654, 17657, 17658, 17659, 17660, 17664, 17665, 17666, 17667, 17669, 17670, 17675, 17676, 17681, 17682, 17686, 17688, 17693, 17695, 17696, 17699, 17700, 17701, 17702, 17704, 17707, 17708, 17709, 17710, 17712, 17713, 17714, 17719, 17721, 17723, 17725, 17728, 17729, 17730, 17731, 17732, 17733, 17735, 17736, 17738, 17739, 17740, 17741, 17744, 17745, 17746, 17748, 17749, 17750, 17751, 17752, 17753, 17755, 17756, 17759, 17760, 17762, 17770, 17772, 17774, 17775, 17777, 17780, 17781, 17783, 17784, 17785, 17786, 17792, 17801]</t>
-        </is>
-      </c>
-      <c r="BH3" t="n">
-        <v>0.04882301656495205</v>
-      </c>
-      <c r="BI3" t="inlineStr">
-        <is>
-          <t>{'initial_window': 3245, 'window_size': 2395, 'num_trees': 20, 'max_depth': 11}</t>
-        </is>
-      </c>
-      <c r="BJ3" t="n">
-        <v>5.972503450000659</v>
-      </c>
-      <c r="BK3" t="inlineStr">
-        <is>
-          <t>[33, 34, 35, 45, 46, 263, 407, 491, 503, 515, 527, 539, 551, 563, 575, 587, 599, 611, 623, 635, 647, 659, 671, 683, 695, 707, 719, 731, 743, 755, 767, 778, 779, 791, 803, 814, 827, 828, 838, 839, 850, 851, 862, 863, 874, 875, 886, 887, 898, 899, 911, 923, 934, 935, 946, 947, 958, 959, 970, 971, 982, 983, 995, 1006, 1007, 1018, 1019, 1030, 1031, 1042, 1043, 1054, 1055, 1066, 1067, 1078, 1079, 1090, 1091, 1102, 1103, 1114, 1115, 1126, 1127, 1138, 1139, 1150, 1151, 1162, 1163, 1174, 1175, 1186, 1187, 1198, 1199, 1210, 1211, 1222, 1223, 1234, 1235, 1246, 1247, 1258, 1259, 1270, 1271, 1282, 1283, 1294, 1295, 1306, 1307, 1318, 1319, 1330, 1331, 1342, 1343, 1354, 1355, 1366, 1367, 1378, 1379, 1390, 1391, 1402, 1403, 1414, 1415, 1426, 1427, 1438, 1439, 1450, 1451, 1462, 1463, 1474, 1475, 1486, 1487, 1498, 1499, 1510, 1511, 1522, 1523, 1534, 1535, 1546, 1547, 1558, 1559, 1570, 1571, 1582, 1583, 1594, 1595, 1606, 1607, 1618, 1619, 1630, 1631, 1643, 1654, 1655, 1666, 1667, 1678, 1679, 1690, 1691, 1703, 1714, 1715, 1726, 1727, 1738, 1739, 1750, 1751, 1762, 1763, 1774, 1775, 1786, 1787, 1798, 1799, 1810, 1811, 1822, 1823, 1834, 1835, 1846, 1847, 1858, 1859, 1870, 1871, 1882, 1883, 1895, 1906, 1907, 1919, 1931, 1943, 1955, 1966, 1967, 1978, 1979, 1991, 2003, 2015, 2026, 2027, 2039, 2051, 2062, 2063, 2074, 2075, 2086, 2087, 2098, 2099, 2110, 2111, 2123, 2135, 2146, 2147, 2159, 2171, 2183, 2195, 2206, 2207, 2219, 2230, 2231, 2243, 2255, 2267, 2279, 2291, 2303, 2314, 2315, 2327, 2338, 2351, 2363, 2375, 2387, 2410, 2411, 2412, 2424, 2436, 2459, 2470, 2494, 2495, 2508, 2518, 2520, 2532, 2544, 2568, 2580, 2614, 2616, 2662, 2664, 2736, 2748, 2760, 2772, 2796, 2808, 2820, 3395, 3407, 3419, 3443, 3455, 3467, 3479, 3491, 3527, 3539, 3551, 3563, 3575, 3587, 3599, 3611, 3623, 3635, 3647, 3659, 3671, 3683, 3695, 3707, 3719, 3731, 3743, 3754, 3755, 3767, 3779, 3791, 3803, 3815, 3827, 3839, 3850, 3851, 3863, 3875, 3887, 3899, 3911, 3923, 3935, 3947, 3959, 3971, 3983, 3995, 4007, 4019, 4031, 4043, 4055, 4067, 4079, 4091, 4102, 4103, 4115, 4127, 4138, 4139, 4151, 4163, 4175, 4187, 4199, 4211, 4222, 4223, 4235, 4247, 4259, 4271, 4283, 4295, 4307, 4319, 4331, 4343, 4355, 4367, 4379, 4391, 4403, 4415, 4427, 4439, 4451, 4463, 4475, 4487, 4499, 4511, 4523, 4535, 4547, 4558, 4559, 4571, 4583, 4619, 4630, 4631, 4643, 4655, 4667, 4679, 4691, 4703, 4715, 4727, 4739, 4751, 4763, 4775, 4787, 4799, 4811, 4823, 4835, 4847, 4859, 4871, 4883, 4895, 4907, 4919, 4931, 4943, 4955, 4967, 4978, 4979, 4991, 5003, 5015, 5027, 5039, 5051, 5063, 5075, 5087, 5099, 5111, 5122, 5123, 5135, 5147, 5159, 5171, 5183, 5195, 5206, 5207, 5219, 5230, 5231, 5243, 5255, 5267, 5279, 5291, 5314, 5327, 5339, 5351, 5363, 5374, 5375, 5387, 5399, 5411, 5423, 5435, 5447, 5459, 5482, 5495, 5507, 5519, 5531, 5543, 5555, 5567, 5590, 5603, 5614, 5615, 5627, 5651, 5663, 5675, 5687, 5723, 5735, 5747, 5782, 5807, 5830, 5843, 5866, 5878, 5891, 5903, 5915, 5927, 5939, 5951, 6491, 6527, 6551, 6563, 6575, 6587, 6599, 6611, 6623, 6635, 6647, 6659, 6671, 6683, 6695, 6707, 6719, 6731, 6743, 6755, 6767, 6779, 6791, 6803, 6814, 6815, 6827, 6839, 6851, 6863, 6875, 6887, 6899, 6911, 6923, 6935, 6947, 6959, 6971, 6983, 6995, 7007, 7019, 7031, 7043, 7055, 7067, 7079, 7091, 7102, 7103, 7115, 7127, 7139, 7151, 7163, 7175, 7187, 7199, 7211, 7223, 7235, 7247, 7259, 7271, 7282, 7283, 7295, 7307, 7319, 7331, 7343, 7355, 7367, 7379, 7391, 7403, 7415, 7427, 7439, 7451, 7463, 7475, 7487, 7499, 7511, 7523, 7535, 7547, 7559, 7571, 7583, 7595, 7607, 7619, 7631, 7643, 7655, 7667, 7679, 7691, 7703, 7715, 7727, 7739, 7751, 7763, 7775, 7787, 7799, 7811, 7823, 7835, 7847, 7859, 7871, 7883, 7895, 7907, 7919, 7931, 7943, 7955, 7967, 7979, 7991, 8003, 8013, 8026, 8027, 8039, 8051, 8063, 8075, 8087, 8099, 8111, 8123, 8135, 8147, 8159, 8171, 8183, 8195, 8207, 8219, 8229, 8231, 8255, 8314, 8949, 8950, 8952, 8964, 9635, 9659, 9695, 9707, 9719, 9731, 9743, 9755, 9767, 9779, 9791, 9803, 9815, 9827, 9839, 9875, 9887, 9899, 9911, 9923, 9935, 9947, 9971, 9983, 9995, 10007, 10019, 10031, 10042, 10043, 10055, 10066, 10067, 10079, 10091, 10103, 10139, 10162, 10163, 10198, 10199, 10211, 10222, 10223, 10235, 10246, 10247, 10270, 10271, 10294, 10295, 10307, 10318, 10319, 10331, 10343, 10355, 10378, 10379, 10414, 10415, 10426, 10427, 10450, 10451, 10475, 10486, 10487, 10498, 10499, 10511, 10523, 10534, 10535, 10558, 10559, 10571, 10595, 10607, 10618, 10619, 10631, 10643, 10655, 10667, 10679, 10702, 10703, 10726, 10727, 10750, 10751, 10775, 10786, 10787, 10810, 10811, 10823, 10835, 10859, 10870, 10871, 10882, 10883, 10895, 10918, 10919, 10931, 10942, 10943, 10966, 10967, 10979, 10990, 10991, 11003, 11015, 11027, 11050, 11051, 11075, 11086, 11087, 11099, 11111, 11123, 11135, 11147, 11159, 11182, 11183, 11195, 11207, 11219, 11242, 11243, 11255, 11267, 11279, 11291, 11303, 11326, 11327, 11363, 11375, 11387, 11399, 11411, 11423, 11435, 11458, 11471, 11483, 11495, 11507, 11519, 11542, 11543, 11555, 11556, 11567, 11590, 11603, 11626, 11639, 11651, 11663, 11675, 11687, 11699, 11711, 11712, 11819, 12406, 12430, 12466, 12515, 12586, 12610, 12718, 12826, 12850, 12874, 12898, 12946, 12947, 12970, 13006, 13007, 13030, 13031, 13126, 13127, 13246, 13270, 13271, 13282, 13293, 13318, 13331, 13342, 13355, 13365, 13378, 13402, 13415, 13438, 13439, 13462, 13463, 13475, 13487, 13522, 13523, 13535, 13547, 13570, 13594, 13595, 13607, 13619, 13631, 13643, 13654, 13655, 13667, 13678, 13679, 13702, 13703, 13715, 13726, 13727, 13739, 13751, 13763, 13775, 13787, 13799, 13810, 13811, 13823, 13835, 13847, 13883, 13894, 13895, 13907, 13930, 13954, 13967, 13979, 14015, 14026, 14027, 14039, 14051, 14052, 14075, 14087, 14099, 14111, 14112, 14159, 14160, 14172, 14195, 14196, 14208, 14231, 14232, 14254, 14255, 14268, 14280, 14292, 14314, 14328, 14340, 14352, 14364, 14386, 14387, 14410, 14411, 14424, 14436, 14459, 14471, 14482, 14483, 14496, 14520, 14532, 14566, 14568, 14580, 14614, 14616, 14628, 14640, 14652, 14674, 14676, 14688, 14722, 14736, 14748, 14757, 14760, 14772, 14784, 14796, 14818, 14820, 14832, 14844, 14866, 14880, 14904, 14916, 14928, 14940, 14964, 14976, 14998, 15000, 15022, 15024, 15046, 15048, 15060, 15072, 15084, 15093, 15108, 15120, 15132, 15144, 15156, 15168, 15177, 15180, 15202, 15204, 15226, 15228, 15240, 15262, 15264, 15286, 15288, 15300, 15312, 15324, 15336, 15372, 15384, 15396, 15408, 15420, 15429, 15442, 15444, 15466, 15468, 15480, 15492, 15501, 15514, 15516, 15528, 15540, 15552, 15574, 15576, 15588, 15600, 15612, 15634, 15636, 15658, 15660, 15672, 15684, 15696, 15742, 15744, 15766, 15768, 15780, 15792, 15814, 15816, 15825, 15826, 15828, 15840, 15852, 15874, 15876, 15888, 15900, 15912, 15934, 15936, 15948, 15960, 15969, 15972, 15984, 15996, 16008, 16042, 16044, 16056, 16068, 16102, 16104, 16116, 16128, 16137, 16138, 16140, 16152, 16174, 16176, 16188, 16200, 16212, 16224, 16236, 16248, 16260, 16272, 16294, 16296, 16342, 16344, 16366, 16368, 16380, 16389, 16390, 16392, 16414, 16416, 16438, 16440, 16449, 16462, 16464, 16473, 16474, 16476, 16498, 16500, 16522, 16524, 16536, 16558, 16560, 16582, 16584, 16593, 16594, 16596, 16608, 16617, 16642, 16644, 16653, 16666, 16668, 16678, 16680, 16690, 16692, 16704, 16713, 16714, 16716, 16738, 16740, 16752, 16761, 16774, 16776, 16810, 16812, 16822, 16824, 16833, 16834, 16836, 16848, 16858, 16860, 16884, 16894, 16896, 16918, 16920, 16929, 16942, 16944, 16966, 16968, 16980, 16990, 17001, 17006, 17013, 17014, 17017, 17024, 17034, 17052, 17065, 17073, 17074, 17085, 17098, 17123, 17124, 17134, 17135, 17140, 17146, 17150, 17157, 17158, 17187, 17191, 17194, 17197, 17215, 17227, 17228, 17233, 17250, 17254, 17255, 17265, 17275, 17277, 17282, 17284, 17295, 17302, 17303, 17305, 17314, 17317, 17334, 17335, 17346, 17347, 17350, 17351, 17363, 17364, 17365, 17374, 17386, 17397, 17411, 17443, 17444, 17446, 17447, 17457, 17469, 17470, 17503, 17506, 17517, 17536, 17542, 17547, 17553, 17554, 17556, 17565, 17566, 17568, 17572, 17577, 17583, 17603, 17613, 17614, 17624, 17629, 17637, 17638, 17650, 17652, 17655, 17661, 17666, 17667, 17672, 17674, 17677, 17683, 17688, 17746, 17747, 17757, 17758, 17760, 17787, 17792]</t>
-        </is>
-      </c>
-      <c r="BL3" t="n">
-        <v>0.06254767353165522</v>
-      </c>
       <c r="BM3" t="inlineStr">
         <is>
-          <t>{'AR_window_size': 11, 'differencing-order': 1}</t>
+          <t>[1, 3, 34, 240, 551, 587, 623, 659, 779, 803, 815, 839, 851, 863, 875, 887, 899, 935, 947, 959, 1007, 1019, 1031, 1043, 1091, 1103, 1127, 1151, 1163, 1175, 1199, 1211, 1223, 1247, 1259, 1271, 1295, 1307, 1319, 1331, 1355, 1367, 1379, 1403, 1463, 1475, 1487, 1511, 1559, 1571, 1583, 1595, 1607, 1619, 1643, 1655, 1667, 1703, 2412, 2459, 2472, 2532, 2544, 2580, 2616, 2664, 2736, 2748, 2760, 2772, 2808, 2820, 2832, 2833, 2917, 3431, 3479, 3527, 3575, 3599, 3611, 3659, 3683, 3695, 3707, 3719, 3731, 3755, 3779, 3803, 3815, 3827, 3851, 3863, 3875, 3887, 3899, 3911, 3947, 3959, 3971, 3983, 3995, 4019, 4031, 4043, 4054, 4067, 4079, 4091, 4103, 4115, 4127, 4139, 4151, 4163, 4175, 4187, 4199, 4211, 4235, 4247, 4271, 4283, 4295, 4307, 4319, 4367, 4379, 4415, 4427, 4439, 4451, 4463, 4475, 4487, 4499, 4511, 4523, 4535, 4547, 4559, 4571, 4583, 4593, 4596, 4597, 4599, 4607, 4619, 4655, 4667, 4679, 4691, 4703, 4715, 4727, 4739, 4751, 4763, 4775, 4787, 4799, 4811, 4823, 4835, 4847, 4859, 4871, 4883, 4895, 4907, 4919, 4931, 4943, 4955, 4967, 4979, 4991, 4992, 5003, 5015, 5027, 5039, 5051, 5063, 5075, 5087, 5099, 5111, 5123, 5135, 5147, 5159, 5171, 5183, 5195, 5207, 5219, 5230, 5231, 5243, 5267, 5279, 5303, 5315, 5327, 5339, 5351, 5363, 5375, 5387, 5399, 5411, 5422, 5423, 5435, 5459, 5471, 5495, 5519, 5531, 5543, 5555, 5567, 5579, 5591, 5615, 5639, 5651, 5652, 5662, 5663, 5675, 5699, 5700, 5711, 5712, 5723, 5735, 5736, 5747, 5748, 5759, 5760, 5771, 5772, 5783, 5795, 5807, 5819, 5831, 5832, 5843, 5844, 5855, 5867, 5868, 5879, 5880, 5891, 5892, 5903, 5904, 5915, 5916, 5927, 5939, 5940, 5952, 6107, 6234, 6251, 6275, 6299, 6311, 6335, 6359, 6383, 6479, 6503, 6539, 6575, 6599, 6635, 6647, 6731, 6743, 6779, 6791, 6803, 6815, 6827, 6839, 6851, 6863, 6875, 6887, 6899, 6911, 6923, 6935, 6947, 6959, 6971, 6983, 7019, 7031, 7055, 7091, 7103, 7115, 7127, 7139, 7151, 7163, 7187, 7199, 7211, 7223, 7247, 7271, 7283, 7295, 7307, 7331, 7367, 7391, 7403, 7415, 7427, 7439, 7451, 7463, 7475, 7487, 7499, 7511, 7523, 7535, 7559, 7571, 7583, 7595, 7607, 7619, 7631, 7655, 7824, 7908, 7920, 7932, 7944, 7956, 7968, 7980, 8004, 8007, 8013, 8014, 8016, 8208, 8227, 8230, 8231, 8243, 8255, 8256, 8259, 8260, 8261, 8262, 8267, 8279, 8291, 8292, 8303, 8307, 8308, 8309, 8311, 8312, 8327, 8339, 8363, 8379, 8399, 8411, 8435, 8471, 8495, 8507, 8543, 8567, 8568, 8580, 8615, 8628, 8651, 8652, 8663, 8675, 8699, 8711, 8723, 8735, 8736, 8747, 8771, 8783, 8795, 8796, 8807, 8820, 8831, 8832, 8843, 8855, 8867, 8879, 8903, 8915, 8949, 8951, 8952, 8953, 8954, 8958, 8963, 8964, 8975, 8987, 8999, 9011, 9012, 9023, 9035, 9036, 9047, 9048, 9059, 9071, 9083, 9095, 9096, 9107, 9119, 9120, 9131, 9132, 9143, 9144, 9154, 9155, 9157, 9158, 9161, 9163, 9164, 9165, 9635, 9659, 9695, 9707, 9719, 9731, 9743, 9755, 9767, 9779, 9791, 9803, 9815, 9827, 9839, 9863, 9875, 9887, 9899, 9911, 9923, 9935, 9947, 9971, 9983, 9995, 10007, 10019, 10031, 10055, 10067, 10079, 10091, 10103, 10134, 10137, 10139, 10175, 10199, 10211, 10271, 10307, 10367, 10391, 10463, 10475, 10523, 10535, 10583, 10595, 10607, 10691, 10715, 10739, 10763, 10775, 10787, 10799, 10847, 10859, 10877, 10907, 10955, 11039, 11063, 11075, 11171, 11231, 11256, 11315, 11447, 11531, 11544, 11579, 11712, 11733, 11736, 11769, 11770, 11783, 11843, 11867, 11879, 11927, 11975, 12023, 12083, 12095, 12119, 12131, 12143, 12191, 12203, 12239, 12275, 12323, 12347, 12383, 12395, 12407, 12431, 12467, 12479, 12491, 12503, 12515, 12527, 12551, 12563, 12575, 12582, 12587, 12611, 12623, 12635, 12647, 12659, 12671, 12683, 12719, 12731, 12743, 12755, 12767, 12791, 12803, 12815, 12827, 12839, 12851, 12863, 12875, 12887, 12899, 12911, 12923, 12947, 12971, 12983, 13007, 13055, 13067, 13091, 13103, 13127, 13139, 13151, 13163, 13175, 13187, 13199, 13211, 13223, 13247, 13259, 13271, 13272, 13283, 13307, 13319, 13331, 13343, 13355, 13367, 13379, 13403, 13415, 13427, 13439, 13451, 13463, 13475, 13487, 13499, 13511, 13523, 13535, 13547, 13559, 13571, 13572, 13583, 13595, 13607, 13619, 13631, 13643, 13655, 13667, 13691, 13715, 13799, 14022, 14052, 14112, 14123, 14160, 14172, 14196, 14208, 14232, 14243, 14256, 14268, 14280, 14292, 14303, 14316, 14328, 14340, 14352, 14364, 14375, 14388, 14399, 14412, 14424, 14436, 14484, 14496, 14508, 14520, 14532, 14544, 14555, 14568, 14580, 14592, 14603, 14616, 14628, 14652, 14711, 14724, 14736, 14748, 14760, 14796, 14820, 14832, 14868, 14880, 14892, 14904, 14916, 14928, 14940, 14952, 14964, 14976, 14987, 15000, 15024, 15048, 15060, 15072, 15084, 15096, 15108, 15120, 15132, 15156, 15168, 15180, 15204, 15228, 15240, 15251, 15264, 15288, 15300, 15324, 15336, 15360, 15372, 15384, 15396, 15420, 15444, 15455, 15468, 15492, 15516, 15528, 15563, 15576, 15588, 15600, 15612, 15623, 15636, 15660, 15672, 15684, 15696, 15744, 15780, 15840, 15888, 15900, 15912, 15924, 15936, 15948, 15984, 15996, 16031, 16056, 16091, 16104, 16116, 16152, 16156, 16188, 16212, 16236, 16248, 16260, 16272, 16307, 16368, 16392, 16416, 16440, 16476, 16500, 16524, 16584, 16608, 16644, 16655, 16668, 16680, 16734, 16752, 16776, 16824, 16836, 16860, 16872, 16884, 16896, 16907, 16908, 16920, 16926, 16931, 16955, 16956, 16968, 16980, 16992, 16993, 16994, 16995, 16997, 16998, 16999, 17000, 17001, 17003, 17004, 17005, 17006, 17007, 17008, 17009, 17010, 17011, 17013, 17015, 17016, 17017, 17018, 17019, 17020, 17021, 17022, 17023, 17024, 17025, 17026, 17027, 17031, 17032, 17033, 17035, 17036, 17038, 17039, 17041, 17044, 17048, 17049, 17050, 17052, 17055, 17056, 17057, 17058, 17061, 17062, 17063, 17064, 17065, 17068, 17069, 17070, 17071, 17073, 17075, 17076, 17078, 17079, 17081, 17082, 17083, 17084, 17085, 17087, 17089, 17090, 17091, 17093, 17095, 17096, 17097, 17098, 17100, 17101, 17102, 17103, 17104, 17105, 17106, 17109, 17110, 17111, 17115, 17118, 17120, 17121, 17122, 17123, 17125, 17126, 17127, 17128, 17129, 17132, 17133, 17134, 17135, 17136, 17137, 17139, 17141, 17142, 17143, 17145, 17146, 17147, 17148, 17150, 17151, 17153, 17154, 17155, 17156, 17157, 17159, 17160, 17161, 17162, 17165, 17167, 17168, 17169, 17170, 17172, 17173, 17175, 17176, 17178, 17180, 17181, 17184, 17187, 17189, 17190, 17191, 17193, 17195, 17196, 17197, 17199, 17200, 17201, 17206, 17207, 17208, 17211, 17213, 17214, 17215, 17217, 17220, 17222, 17223, 17225, 17226, 17227, 17229, 17230, 17231, 17232, 17233, 17235, 17236, 17237, 17238, 17239, 17240, 17241, 17242, 17243, 17244, 17245, 17247, 17248, 17250, 17252, 17253, 17254, 17255, 17256, 17259, 17260, 17261, 17262, 17263, 17268, 17270, 17273, 17275, 17276, 17277, 17278, 17279, 17280, 17281, 17285, 17286, 17287, 17288, 17289, 17291, 17292, 17293, 17295, 17297, 17301, 17302, 17304, 17305, 17307, 17309, 17312, 17313, 17315, 17316, 17317, 17318, 17320, 17321, 17322, 17323, 17325, 17326, 17328, 17331, 17332, 17335, 17337, 17338, 17339, 17340, 17343, 17344, 17345, 17346, 17349, 17350, 17351, 17352, 17353, 17355, 17356, 17357, 17359, 17360, 17361, 17362, 17363, 17367, 17368, 17369, 17370, 17371, 17373, 17375, 17376, 17378, 17379, 17381, 17382, 17387, 17388, 17389, 17390, 17393, 17395, 17398, 17399, 17401, 17402, 17403, 17404, 17407, 17409, 17410, 17411, 17412, 17415, 17416, 17418, 17421, 17422, 17423, 17424, 17425, 17426, 17427, 17428, 17429, 17430, 17431, 17433, 17434, 17435, 17436, 17438, 17439, 17441, 17442, 17443, 17444, 17445, 17446, 17448, 17449, 17452, 17458, 17459, 17461, 17462, 17465, 17466, 17467, 17468, 17469, 17470, 17471, 17472, 17473, 17474, 17479, 17480, 17481, 17482, 17484, 17485, 17486, 17487, 17488, 17489, 17491, 17493, 17494, 17495, 17496, 17497, 17498, 17499, 17501, 17502, 17503, 17505, 17507, 17508, 17509, 17510, 17511, 17512, 17513, 17514, 17515, 17516, 17521, 17522, 17523, 17524, 17525, 17527, 17528, 17529, 17530, 17531, 17532, 17533, 17534, 17538, 17539, 17540, 17542, 17543, 17544, 17545, 17546, 17547, 17548, 17549, 17550, 17551, 17552, 17553, 17554, 17555, 17556, 17557, 17558, 17559, 17561, 17563, 17564, 17565, 17566, 17567, 17568, 17569, 17570, 17572, 17573, 17575, 17576, 17578, 17579, 17581, 17582, 17584, 17586, 17587, 17588, 17590, 17591, 17592, 17593, 17595, 17596, 17597, 17599, 17600, 17601, 17602, 17603, 17604, 17607, 17608, 17610, 17612, 17613, 17614, 17616, 17617, 17618, 17620, 17621, 17622, 17625, 17631, 17632, 17633, 17634, 17635, 17636, 17640, 17641, 17642, 17643, 17645, 17646, 17647, 17648, 17651, 17652, 17653, 17654, 17655, 17657, 17658, 17659, 17660, 17663, 17664, 17665, 17666, 17667, 17668, 17669, 17670, 17673, 17675, 17676, 17678, 17679, 17681, 17682, 17686, 17687, 17688, 17690, 17693, 17694, 17695, 17696, 17698, 17699, 17700, 17701, 17702, 17703, 17704, 17707, 17708, 17709, 17710, 17711, 17712, 17713, 17714, 17716, 17718, 17719, 17721, 17722, 17723, 17724, 17725, 17726, 17727, 17728, 17729, 17730, 17731, 17732, 17733, 17734, 17735, 17736, 17738, 17739, 17740, 17741, 17744, 17745, 17746, 17748, 17749, 17750, 17751, 17752, 17753, 17754, 17755, 17756, 17758, 17759, 17760, 17761, 17762, 17763, 17764, 17765, 17767, 17768, 17770, 17771, 17772, 17773, 17774, 17775, 17776, 17777, 17778, 17780, 17781, 17783, 17784, 17785, 17786, 17787, 17792, 17793, 17794, 17795, 17796, 17797, 17798, 17799, 17800, 17801, 17802, 17804, 17805, 17807, 17809, 17810, 17811, 17812, 17813, 17814, 17815, 17816, 17817, 17818, 17819, 17820, 17821, 17822, 17823, 17824, 17825, 17826, 17827, 17828, 17829, 17830, 17831, 17832, 17833, 17834, 17835, 17836, 17837, 17838, 17839, 17840, 17841, 17842, 17843, 17844, 17845, 17846, 17847, 17848, 17849, 17850, 17851, 17852, 17853, 17854, 17855, 17856, 17857, 17858, 17859, 17860, 17861, 17862, 17863, 17864, 17865, 17866, 17867, 17868, 17869, 17870, 17871, 17872, 17873, 17874, 17875, 17876, 17877, 17878, 17880, 17881, 17882, 17883, 17884, 17885, 17886, 17887, 17888, 17889, 17890, 17891, 17892, 17893, 17894, 17895, 17896, 17897, 17898, 17899, 17900, 17901, 17902, 17903, 17904, 17905, 17906, 17907, 17908, 17909, 17910, 17911, 17912, 17913, 17914, 17915, 17916, 17917, 17918, 17919, 17920, 17921, 17922, 17923, 17924, 17925, 17926, 17927, 17928, 17929, 17930, 17931, 17932, 17933, 17934, 17935, 17936, 17937, 17938, 17939, 17940, 17941, 17942, 17943, 17944, 17945, 17946, 17947, 17948, 17949, 17950, 17951, 17952, 17953, 17954, 17955, 17956, 17957, 17958, 17959, 17960, 17961, 17962, 17963, 17964, 17965, 17966, 17967, 17968, 17969, 17970, 17971, 17972, 17973, 17974, 17975, 17976, 17977, 17978, 17979, 17980, 17981, 17982, 17983, 17984, 17985, 17986, 17987, 17988, 17989, 17990, 17991, 17992, 17993, 17994, 17995, 17996, 17997, 17998, 17999, 18000, 18001, 18002, 18003, 18004, 18005, 18006, 18007, 18008, 18009, 18010, 18011, 18012, 18013, 18014, 18015, 18016, 18017, 18018, 18019, 18020, 18021, 18022, 18023, 18024, 18025, 18026, 18027, 18028, 18029, 18030, 18031, 18032, 18033, 18034, 18035, 18036, 18037, 18038, 18039, 18040, 18041, 18042, 18043, 18044, 18045, 18046, 18048, 18049]</t>
         </is>
       </c>
       <c r="BN3" t="n">
-        <v>77.45807594503276</v>
+        <v>0.4466762314681971</v>
       </c>
       <c r="BO3" t="inlineStr">
         <is>
+          <t>{'initial_window': 339, 'window_size': 3855, 'num_trees': 19, 'max_depth': 11}</t>
+        </is>
+      </c>
+      <c r="BP3" t="n">
+        <v>10.22733592498116</v>
+      </c>
+      <c r="BQ3" t="inlineStr">
+        <is>
+          <t>[16926, 16998, 17644]</t>
+        </is>
+      </c>
+      <c r="BR3" t="n">
+        <v>1</v>
+      </c>
+      <c r="BS3" t="inlineStr">
+        <is>
+          <t>{'AR_window_size': 29, 'differencing-order': 0}</t>
+        </is>
+      </c>
+      <c r="BT3" t="n">
+        <v>129.9010999479797</v>
+      </c>
+      <c r="BU3" t="inlineStr">
+        <is>
           <t xml:space="preserve">[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86, 87, 88, 89, 90, 91, 92, 93, 94, 95, 96, 97, 98, 99, 100, 101, 102, 103, 104, 105, 106, 107, 108, 109, 110, 111, 112, 113, 114, 115, 116, 117, 118, 119, 120, 121, 122, 123, 124, 125, 126, 127, 128, 129, 130, 131, 132, 133, 134, 135, 136, 137, 138, 139, 140, 141, 142, 143, 144, 145, 146, 147, 148, 149, 150, 151, 152, 153, 154, 155, 156, 157, 158, 159, 160, 161, 162, 163, 164, 165, 166, 167, 168, 169, 170, 171, 172, 173, 174, 175, 176, 177, 178, 179, 180, 181, 182, 183, 184, 185, 186, 187, 188, 189, 190, 191, 192, 193, 194, 195, 196, 197, 198, 199, 200, 201, 202, 203, 204, 205, 206, 207, 208, 209, 210, 211, 212, 213, 214, 215, 216, 217, 218, 219, 220, 221, 222, 223, 224, 225, 226, 227, 228, 229, 230, 231, 232, 233, 234, 235, 236, 237, 238, 239, 240, 241, 242, 243, 244, 245, 246, 247, 248, 249, 250, 251, 252, 253, 254, 255, 256, 257, 258, 259, 260, 261, 262, 263, 264, 265, 266, 267, 268, 269, 270, 271, 272, 273, 274, 275, 276, 277, 278, 279, 280, 281, 282, 283, 284, 285, 286, 287, 288, 289, 290, 291, 292, 293, 294, 295, 296, 297, 298, 299, 300, 301, 302, 303, 304, 305, 306, 307, 308, 309, 310, 311, 312, 313, 314, 315, 316, 317, 318, 319, 320, 321, 322, 323, 324, 325, 326, 327, 328, 329, 330, 331, 332, 333, 334, 335, 336, 337, 338, 339, 340, 341, 342, 343, 344, 345, 346, 347, 348, 349, 350, 351, 352, 353, 354, 355, 356, 357, 358, 359, 360, 361, 362, 363, 364, 365, 366, 367, 368, 369, 370, 371, 372, 373, 374, 375, 376, 377, 378, 379, 380, 381, 382, 383, 384, 385, 386, 387, 388, 389, 390, 391, 392, 393, 394, 395, 396, 397, 398, 399, 400, 401, 402, 403, 404, 405, 406, 407, 408, 409, 410, 411, 412, 413, 414, 415, 416, 417, 418, 419, 420, 421, 422, 423, 424, 425, 426, 427, 428, 429, 430, 431, 432, 433, 434, 435, 436, 437, 438, 439, 440, 441, 442, 443, 444, 445, 446, 447, 448, 449, 450, 451, 452, 453, 454, 455, 456, 457, 458, 459, 460, 461, 462, 463, 464, 465, 466, 467, 468, 469, 470, 471, 472, 473, 474, 475, 476, 477, 478, 479, 480, 481, 482, 483, 484, 485, 486, 487, 488, 489, 490, 491, 492, 493, 494, 495, 496, 497, 498, 499, 500, 501, 502, 503, 504, 505, 506, 507, 508, 509, 510, 511, 512, 513, 514, 515, 516, 517, 518, 519, 520, 521, 522, 523, 524, 525, 526, 527, 528, 529, 530, 531, 532, 533, 534, 535, 536, 537, 538, 539, 540, 541, 542, 543, 544, 545, 546, 547, 548, 549, 550, 551, 552, 553, 554, 555, 556, 557, 558, 559, 560, 561, 562, 563, 564, 565, 566, 567, 568, 569, 570, 571, 572, 573, 574, 575, 576, 577, 578, 579, 580, 581, 582, 583, 584, 585, 586, 587, 588, 589, 590, 591, 592, 593, 594, 595, 596, 597, 598, 599, 600, 601, 602, 603, 604, 605, 606, 607, 608, 609, 610, 611, 612, 613, 614, 615, 616, 617, 618, 619, 620, 621, 622, 623, 624, 625, 626, 627, 628, 629, 630, 631, 632, 633, 634, 635, 636, 637, 638, 639, 640, 641, 642, 643, 644, 645, 646, 647, 648, 649, 650, 651, 652, 653, 654, 655, 656, 657, 658, 659, 660, 661, 662, 663, 664, 665, 666, 667, 668, 669, 670, 671, 672, 673, 674, 675, 676, 677, 678, 679, 680, 681, 682, 683, 684, 685, 686, 687, 688, 689, 690, 691, 692, 693, 694, 695, 696, 697, 698, 699, 700, 701, 702, 703, 704, 705, 706, 707, 708, 709, 710, 711, 712, 713, 714, 715, 716, 717, 718, 719, 720, 721, 722, 723, 724, 725, 726, 727, 728, 729, 730, 731, 732, 733, 734, 735, 736, 737, 738, 739, 740, 741, 742, 743, 744, 745, 746, 747, 748, 749, 750, 751, 752, 753, 754, 755, 756, 757, 758, 759, 760, 761, 762, 763, 764, 765, 766, 767, 768, 769, 770, 771, 772, 773, 774, 775, 776, 777, 778, 779, 780, 781, 782, 783, 784, 785, 786, 787, 788, 789, 790, 791, 792, 793, 794, 795, 796, 797, 798, 799, 800, 801, 802, 803, 804, 805, 806, 807, 808, 809, 810, 811, 812, 813, 814, 815, 816, 817, 818, 819, 820, 821, 822, 823, 824, 825, 826, 827, 828, 829, 830, 831, 832, 833, 834, 835, 836, 837, 838, 839, 840, 841, 842, 843, 844, 845, 846, 847, 848, 849, 850, 851, 852, 853, 854, 855, 856, 857, 858, 859, 860, 861, 862, 863, 864, 865, 866, 867, 868, 869, 870, 871, 872, 873, 874, 875, 876, 877, 878, 879, 880, 881, 882, 883, 884, 885, 886, 887, 888, 889, 890, 891, 892, 893, 894, 895, 896, 897, 898, 899, 900, 901, 902, 903, 904, 905, 906, 907, 908, 909, 910, 911, 912, 913, 914, 915, 916, 917, 918, 919, 920, 921, 922, 923, 924, 925, 926, 927, 928, 929, 930, 931, 932, 933, 934, 935, 936, 937, 938, 939, 940, 941, 942, 943, 944, 945, 946, 947, 948, 949, 950, 951, 952, 953, 954, 955, 956, 957, 958, 959, 960, 961, 962, 963, 964, 965, 966, 967, 968, 969, 970, 971, 972, 973, 974, 975, 976, 977, 978, 979, 980, 981, 982, 983, 984, 985, 986, 987, 988, 989, 990, 991, 992, 993, 994, 995, 996, 997, 998, 999, 1000, 1001, 1002, 1003, 1004, 1005, 1006, 1007, 1008, 1009, 1010, 1011, 1012, 1013, 1014, 1015, 1016, 1017, 1018, 1019, 1020, 1021, 1022, 1023, 1024, 1025, 1026, 1027, 1028, 1029, 1030, 1031, 1032, 1033, 1034, 1035, 1036, 1037, 1038, 1039, 1040, 1041, 1042, 1043, 1044, 1045, 1046, 1047, 1048, 1049, 1050, 1051, 1052, 1053, 1054, 1055, 1056, 1057, 1058, 1059, 1060, 1061, 1062, 1063, 1064, 1065, 1066, 1067, 1068, 1069, 1070, 1071, 1072, 1073, 1074, 1075, 1076, 1077, 1078, 1079, 1080, 1081, 1082, 1083, 1084, 1085, 1086, 1087, 1088, 1089, 1090, 1091, 1092, 1093, 1094, 1095, 1096, 1097, 1098, 1099, 1100, 1101, 1102, 1103, 1104, 1105, 1106, 1107, 1108, 1109, 1110, 1111, 1112, 1113, 1114, 1115, 1116, 1117, 1118, 1119, 1120, 1121, 1122, 1123, 1124, 1125, 1126, 1127, 1128, 1129, 1130, 1131, 1132, 1133, 1134, 1135, 1136, 1137, 1138, 1139, 1140, 1141, 1142, 1143, 1144, 1145, 1146, 1147, 1148, 1149, 1150, 1151, 1152, 1153, 1154, 1155, 1156, 1157, 1158, 1159, 1160, 1161, 1162, 1163, 1164, 1165, 1166, 1167, 1168, 1169, 1170, 1171, 1172, 1173, 1174, 1175, 1176, 1177, 1178, 1179, 1180, 1181, 1182, 1183, 1184, 1185, 1186, 1187, 1188, 1189, 1190, 1191, 1192, 1193, 1194, 1195, 1196, 1197, 1198, 1199, 1200, 1201, 1202, 1203, 1204, 1205, 1206, 1207, 1208, 1209, 1210, 1211, 1212, 1213, 1214, 1215, 1216, 1217, 1218, 1219, 1220, 1221, 1222, 1223, 1224, 1225, 1226, 1227, 1228, 1229, 1230, 1231, 1232, 1233, 1234, 1235, 1236, 1237, 1238, 1239, 1240, 1241, 1242, 1243, 1244, 1245, 1246, 1247, 1248, 1249, 1250, 1251, 1252, 1253, 1254, 1255, 1256, 1257, 1258, 1259, 1260, 1261, 1262, 1263, 1264, 1265, 1266, 1267, 1268, 1269, 1270, 1271, 1272, 1273, 1274, 1275, 1276, 1277, 1278, 1279, 1280, 1281, 1282, 1283, 1284, 1285, 1286, 1287, 1288, 1289, 1290, 1291, 1292, 1293, 1294, 1295, 1296, 1297, 1298, 1299, 1300, 1301, 1302, 1303, 1304, 1305, 1306, 1307, 1308, 1309, 1310, 1311, 1312, 1313, 1314, 1315, 1316, 1317, 1318, 1319, 1320, 1321, 1322, 1323, 1324, 1325, 1326, 1327, 1328, 1329, 1330, 1331, 1332, 1333, 1334, 1335, 1336, 1337, 1338, 1339, 1340, 1341, 1342, 1343, 1344, 1345, 1346, 1347, 1348, 1349, 1350, 1351, 1352, 1353, 1354, 1355, 1356, 1357, 1358, 1359, 1360, 1361, 1362, 1363, 1364, 1365, 1366, 1367, 1368, 1369, 1370, 1371, 1372, 1373, 1374, 1375, 1376, 1377, 1378, 1379, 1380, 1381, 1382, 1383, 1384, 1385, 1386, 1387, 1388, 1389, 1390, 1391, 1392, 1393, 1394, 1395, 1396, 1397, 1398, 1399, 1400, 1401, 1402, 1403, 1404, 1405, 1406, 1407, 1408, 1409, 1410, 1411, 1412, 1413, 1414, 1415, 1416, 1417, 1418, 1419, 1420, 1421, 1422, 1423, 1424, 1425, 1426, 1427, 1428, 1429, 1430, 1431, 1432, 1433, 1434, 1435, 1436, 1437, 1438, 1439, 1440, 1441, 1442, 1443, 1444, 1445, 1446, 1447, 1448, 1449, 1450, 1451, 1452, 1453, 1454, 1455, 1456, 1457, 1458, 1459, 1460, 1461, 1462, 1463, 1464, 1465, 1466, 1467, 1468, 1469, 1470, 1471, 1472, 1473, 1474, 1475, 1476, 1477, 1478, 1479, 1480, 1481, 1482, 1483, 1484, 1485, 1486, 1487, 1488, 1489, 1490, 1491, 1492, 1493, 1494, 1495, 1496, 1497, 1498, 1499, 1500, 1501, 1502, 1503, 1504, 1505, 1506, 1507, 1508, 1509, 1510, 1511, 1512, 1513, 1514, 1515, 1516, 1517, 1518, 1519, 1520, 1521, 1522, 1523, 1524, 1525, 1526, 1527, 1528, 1529, 1530, 1531, 1532, 1533, 1534, 1535, 1536, 1537, 1538, 1539, 1540, 1541, 1542, 1543, 1544, 1545, 1546, 1547, 1548, 1549, 1550, 1551, 1552, 1553, 1554, 1555, 1556, 1557, 1558, 1559, 1560, 1561, 1562, 1563, 1564, 1565, 1566, 1567, 1568, 1569, 1570, 1571, 1572, 1573, 1574, 1575, 1576, 1577, 1578, 1579, 1580, 1581, 1582, 1583, 1584, 1585, 1586, 1587, 1588, 1589, 1590, 1591, 1592, 1593, 1594, 1595, 1596, 1597, 1598, 1599, 1600, 1601, 1602, 1603, 1604, 1605, 1606, 1607, 1608, 1609, 1610, 1611, 1612, 1613, 1614, 1615, 1616, 1617, 1618, 1619, 1620, 1621, 1622, 1623, 1624, 1625, 1626, 1627, 1628, 1629, 1630, 1631, 1632, 1633, 1634, 1635, 1636, 1637, 1638, 1639, 1640, 1641, 1642, 1643, 1644, 1645, 1646, 1647, 1648, 1649, 1650, 1651, 1652, 1653, 1654, 1655, 1656, 1657, 1658, 1659, 1660, 1661, 1662, 1663, 1664, 1665, 1666, 1667, 1668, 1669, 1670, 1671, 1672, 1673, 1674, 1675, 1676, 1677, 1678, 1679, 1680, 1681, 1682, 1683, 1684, 1685, 1686, 1687, 1688, 1689, 1690, 1691, 1692, 1693, 1694, 1695, 1696, 1697, 1698, 1699, 1700, 1701, 1702, 1703, 1704, 1705, 1706, 1707, 1708, 1709, 1710, 1711, 1712, 1713, 1714, 1715, 1716, 1717, 1718, 1719, 1720, 1721, 1722, 1723, 1724, 1725, 1726, 1727, 1728, 1729, 1730, 1731, 1732, 1733, 1734, 1735, 1736, 1737, 1738, 1739, 1740, 1741, 1742, 1743, 1744, 1745, 1746, 1747, 1748, 1749, 1750, 1751, 1752, 1753, 1754, 1755, 1756, 1757, 1758, 1759, 1760, 1761, 1762, 1763, 1764, 1765, 1766, 1767, 1768, 1769, 1770, 1771, 1772, 1773, 1774, 1775, 1776, 1777, 1778, 1779, 1780, 1781, 1782, 1783, 1784, 1785, 1786, 1787, 1788, 1789, 1790, 1791, 1792, 1793, 1794, 1795, 1796, 1797, 1798, 1799, 1800, 1801, 1802, 1803, 1804, 1805, 1806, 1807, 1808, 1809, 1810, 1811, 1812, 1813, 1814, 1815, 1816, 1817, 1818, 1819, 1820, 1821, 1822, 1823, 1824, 1825, 1826, 1827, 1828, 1829, 1830, 1831, 1832, 1833, 1834, 1835, 1836, 1837, 1838, 1839, 1840, 1841, 1842, 1843, 1844, 1845, 1846, 1847, 1848, 1849, 1850, 1851, 1852, 1853, 1854, 1855, 1856, 1857, 1858, 1859, 1860, 1861, 1862, 1863, 1864, 1865, 1866, 1867, 1868, 1869, 1870, 1871, 1872, 1873, 1874, 1875, 1876, 1877, 1878, 1879, 1880, 1881, 1882, 1883, 1884, 1885, 1886, 1887, 1888, 1889, 1890, 1891, 1892, 1893, 1894, 1895, 1896, 1897, 1898, 1899, 1900, 1901, 1902, 1903, 1904, 1905, 1906, 1907, 1908, 1909, 1910, 1911, 1912, 1913, 1914, 1915, 1916, 1917, 1918, 1919, 1920, 1921, 1922, 1923, 1924, 1925, 1926, 1927, 1928, 1929, 1930, 1931, 1932, 1933, 1934, 1935, 1936, 1937, 1938, 1939, 1940, 1941, 1942, 1943, 1944, 1945, 1946, 1947, 1948, 1949, 1950, 1951, 1952, 1953, 1954, 1955, 1956, 1957, 1958, 1959, 1960, 1961, 1962, 1963, 1964, 1965, 1966, 1967, 1968, 1969, 1970, 1971, 1972, 1973, 1974, 1975, 1976, 1977, 1978, 1979, 1980, 1981, 1982, 1983, 1984, 1985, 1986, 1987, 1988, 1989, 1990, 1991, 1992, 1993, 1994, 1995, 1996, 1997, 1998, 1999, 2000, 2001, 2002, 2003, 2004, 2005, 2006, 2007, 2008, 2009, 2010, 2011, 2012, 2013, 2014, 2015, 2016, 2017, 2018, 2019, 2020, 2021, 2022, 2023, 2024, 2025, 2026, 2027, 2028, 2029, 2030, 2031, 2032, 2033, 2034, 2035, 2036, 2037, 2038, 2039, 2040, 2041, 2042, 2043, 2044, 2045, 2046, 2047, 2048, 2049, 2050, 2051, 2052, 2053, 2054, 2055, 2056, 2057, 2058, 2059, 2060, 2061, 2062, 2063, 2064, 2065, 2066, 2067, 2068, 2069, 2070, 2071, 2072, 2073, 2074, 2075, 2076, 2077, 2078, 2079, 2080, 2081, 2082, 2083, 2084, 2085, 2086, 2087, 2088, 2089, 2090, 2091, 2092, 2093, 2094, 2095, 2096, 2097, 2098, 2099, 2100, 2101, 2102, 2103, 2104, 2105, 2106, 2107, 2108, 2109, 2110, 2111, 2112, 2113, 2114, 2115, 2116, 2117, 2118, 2119, 2120, 2121, 2122, 2123, 2124, 2125, 2126, 2127, 2128, 2129, 2130, 2131, 2132, 2133, 2134, 2135, 2136, 2137, 2138, 2139, 2140, 2141, 2142, 2143, 2144, 2145, 2146, 2147, 2148, 2149, 2150, 2151, 2152, 2153, 2154, 2155, 2156, 2157, 2158, 2159, 2160, 2161, 2162, 2163, 2164, 2165, 2166, 2167, 2168, 2169, 2170, 2171, 2172, 2173, 2174, 2175, 2176, 2177, 2178, 2179, 2180, 2181, 2182, 2183, 2184, 2185, 2186, 2187, 2188, 2189, 2190, 2191, 2192, 2193, 2194, 2195, 2196, 2197, 2198, 2199, 2200, 2201, 2202, 2203, 2204, 2205, 2206, 2207, 2208, 2209, 2210, 2211, 2212, 2213, 2214, 2215, 2216, 2217, 2218, 2219, 2220, 2221, 2222, 2223, 2224, 2225, 2226, 2227, 2228, 2229, 2230, 2231, 2232, 2233, 2234, 2235, 2236, 2237, 2238, 2239, 2240, 2241, 2242, 2243, 2244, 2245, 2246, 2247, 2248, 2249, 2250, 2251, 2252, 2253, 2254, 2255, 2256, 2257, 2258, 2259, 2260, 2261, 2262, 2263, 2264, 2265, 2266, 2267, 2268, 2269, 2270, 2271, 2272, 2273, 2274, 2275, 2276, 2277, 2278, 2279, 2280, 2281, 2282, 2283, 2284, 2285, 2286, 2287, 2288, 2289, 2290, 2291, 2292, 2293, 2294, 2295, 2296, 2297, 2298, 2299, 2300, 2301, 2302, 2303, 2304, 2305, 2306, 2307, 2308, 2309, 2310, 2311, 2312, 2313, 2314, 2315, 2316, 2317, 2318, 2319, 2320, 2321, 2322, 2323, 2324, 2325, 2326, 2327, 2328, 2329, 2330, 2331, 2332, 2333, 2334, 2335, 2336, 2337, 2338, 2339, 2340, 2341, 2342, 2343, 2344, 2345, 2346, 2347, 2348, 2349, 2350, 2351, 2352, 2353, 2354, 2355, 2356, 2357, 2358, 2359, 2360, 2361, 2362, 2363, 2364, 2365, 2366, 2367, 2368, 2369, 2370, 2371, 2372, 2373, 2374, 2375, 2376, 2377, 2378, 2379, 2380, 2381, 2382, 2383, 2384, 2385, 2386, 2387, 2388, 2389, 2390, 2391, 2392, 2393, 2394, 2395, 2396, 2397, 2398, 2399, 2400, 2401, 2402, 2403, 2404, 2405, 2406, 2407, 2408, 2409, 2410, 2411, 2412, 2413, 2414, 2415, 2416, 2417, 2418, 2419, 2420, 2421, 2422, 2423, 2424, 2425, 2426, 2427, 2428, 2429, 2430, 2431, 2432, 2433, 2434, 2435, 2436, 2437, 2438, 2439, 2440, 2441, 2442, 2443, 2444, 2445, 2446, 2447, 2448, 2449, 2450, 2451, 2452, 2453, 2454, 2455, 2456, 2457, 2458, 2459, 2460, 2461, 2462, 2463, 2464, 2465, 2466, 2467, 2468, 2469, 2470, 2471, 2472, 2473, 2474, 2475, 2476, 2477, 2478, 2479, 2480, 2481, 2482, 2483, 2484, 2485, 2486, 2487, 2488, 2489, 2490, 2491, 2492, 2493, 2494, 2495, 2496, 2497, 2498, 2499, 2500, 2501, 2502, 2503, 2504, 2505, 2506, 2507, 2508, 2509, 2510, 2511, 2512, 2513, 2514, 2515, 2516, 2517, 2518, 2519, 2520, 2521, 2522, 2523, 2524, 2525, 2526, 2527, 2528, 2529, 2530, 2531, 2532, 2533, 2534, 2535, 2536, 2537, 2538, 2539, 2540, 2541, 2542, 2543, 2544, 2545, 2546, 2547, 2548, 2549, 2550, 2551, 2552, 2553, 2554, 2555, 2556, 2557, 2558, 2559, 2560, 2561, 2562, 2563, 2564, 2565, 2566, 2567, 2568, 2569, 2570, 2571, 2572, 2573, 2574, 2575, 2576, 2577, 2578, 2579, 2580, 2581, 2582, 2583, 2584, 2585, 2586, 2587, 2588, 2589, 2590, 2591, 2592, 2593, 2594, 2595, 2596, 2597, 2598, 2599, 2600, 2601, 2602, 2603, 2604, 2605, 2606, 2607, 2608, 2609, 2610, 2611, 2612, 2613, 2614, 2615, 2616, 2617, 2618, 2619, 2620, 2621, 2622, 2623, 2624, 2625, 2626, 2627, 2628, 2629, 2630, 2631, 2632, 2633, 2634, 2635, 2636, 2637, 2638, 2639, 2640, 2641, 2642, 2643, 2644, 2645, 2646, 2647, 2648, 2649, 2650, 2651, 2652, 2653, 2654, 2655, 2656, 2657, 2658, 2659, 2660, 2661, 2662, 2663, 2664, 2665, 2666, 2667, 2668, 2669, 2670, 2671, 2672, 2673, 2674, 2675, 2676, 2677, 2678, 2679, 2680, 2681, 2682, 2683, 2684, 2685, 2686, 2687, 2688, 2689, 2690, 2691, 2692, 2693, 2694, 2695, 2696, 2697, 2698, 2699, 2700, 2701, 2702, 2703, 2704, 2705, 2706, 2707, 2708, 2709, 2710, 2711, 2712, 2713, 2714, 2715, 2716, 2717, 2718, 2719, 2720, 2721, 2722, 2723, 2724, 2725, 2726, 2727, 2728, 2729, 2730, 2731, 2732, 2733, 2734, 2735, 2736, 2737, 2738, 2739, 2740, 2741, 2742, 2743, 2744, 2745, 2746, 2747, 2748, 2749, 2750, 2751, 2752, 2753, 2754, 2755, 2756, 2757, 2758, 2759, 2760, 2761, 2762, 2763, 2764, 2765, 2766, 2767, 2768, 2769, 2770, 2771, 2772, 2773, 2774, 2775, 2776, 2777, 2778, 2779, 2780, 2781, 2782, 2783, 2784, 2785, 2786, 2787, 2788, 2789, 2790, 2791, 2792, 2793, 2794, 2795, 2796, 2797, 2798, 2799, 2800, 2801, 2802, 2803, 2804, 2805, 2806, 2807, 2808, 2809, 2810, 2811, 2812, 2813, 2814, 2815, 2816, 2817, 2818, 2819, 2820, 2821, 2822, 2823, 2824, 2825, 2826, 2827, 2828, 2829, 2830, 2831, 2832, 2833, 2834, 2835, 2836, 2837, 2838, 2839, 2840, 2841, 2842, 2843, 2844, 2845, 2846, 2847, 2848, 2849, 2850, 2851, 2852, 2853, 2854, 2855, 2856, 2857, 2858, 2859, 2860, 2861, 2862, 2863, 2864, 2865, 2866, 2867, 2868, 2869, 2870, 2871, 2872, 2873, 2874, 2875, 2876, 2877, 2878, 2879, 2880, 2881, 2882, 2883, 2884, 2885, 2886, 2887, 2888, 2889, 2890, 2891, 2892, 2893, 2894, 2895, 2896, 2897, 2898, 2899, 2900, 2901, 2902, 2903, 2904, 2905, 2906, 2907, 2908, 2909, 2910, 2911, 2912, 2913, 2914, 2915, 2916, 2917, 2918, 2919, 2920, 2921, 2922, 2923, 2924, 2925, 2926, 2927, 2928, 2929, 2930, 2931, 2932, 2933, 2934, 2935, 2936, 2937, 2938, 2939, 2940, 2941, 2942, 2943, 2944, 2945, 2946, 2947, 2948, 2949, 2950, 2951, 2952, 2953, 2954, 2955, 2956, 2957, 2958, 2959, 2960, 2961, 2962, 2963, 2964, 2965, 2966, 2967, 2968, 2969, 2970, 2971, 2972, 2973, 2974, 2975, 2976, 2977, 2978, 2979, 2980, 2981, 2982, 2983, 2984, 2985, 2986, 2987, 2988, 2989, 2990, 2991, 2992, 2993, 2994, 2995, 2996, 2997, 2998, 2999, 3000, 3001, 3002, 3003, 3004, 3005, 3006, 3007, 3008, 3009, 3010, 3011, 3012, 3013, 3014, 3015, 3016, 3017, 3018, 3019, 3020, 3021, 3022, 3023, 3024, 3025, 3026, 3027, 3028, 3029, 3030, 3031, 3032, 3033, 3034, 3035, 3036, 3037, 3038, 3039, 3040, 3041, 3042, 3043, 3044, 3045, 3046, 3047, 3048, 3049, 3050, 3051, 3052, 3053, 3054, 3055, 3056, 3057, 3058, 3059, 3060, 3061, 3062, 3063, 3064, 3065, 3066, 3067, 3068, 3069, 3070, 3071, 3072, 3073, 3074, 3075, 3076, 3077, 3078, 3079, 3080, 3081, 3082, 3083, 3084, 3085, 3086, 3087, 3088, 3089, 3090, 3091, 3092, 3093, 3094, 3095, 3096, 3097, 3098, 3099, 3100, 3101, 3102, 3103, 3104, 3105, 3106, 3107, 3108, 3109, 3110, 3111, 3112, 3113, 3114, 3115, 3116, 3117, 3118, 3119, 3120, 3121, 3122, 3123, 3124, 3125, 3126, 3127, 3128, 3129, 3130, 3131, 3132, 3133, 3134, 3135, 3136, 3137, 3138, 3139, 3140, 3141, 3142, 3143, 3144, 3145, 3146, 3147, 3148, 3149, 3150, 3151, 3152, 3153, 3154, 3155, 3156, 3157, 3158, 3159, 3160, 3161, 3162, 3163, 3164, 3165, 3166, 3167, 3168, 3169, 3170, 3171, 3172, 3173, 3174, 3175, 3176, 3177, 3178, 3179, 3180, 3181, 3182, 3183, 3184, 3185, 3186, 3187, 3188, 3189, 3190, 3191, 3192, 3193, 3194, 3195, 3196, 3197, 3198, 3199, 3200, 3201, 3202, 3203, 3204, 3205, 3206, 3207, 3208, 3209, 3210, 3211, 3212, 3213, 3214, 3215, 3216, 3217, 3218, 3219, 3220, 3221, 3222, 3223, 3224, 3225, 3226, 3227, 3228, 3229, 3230, 3231, 3232, 3233, 3234, 3235, 3236, 3237, 3238, 3239, 3240, 3241, 3242, 3243, 3244, 3245, 3246, 3247, 3248, 3249, 3250, 3251, 3252, 3253, 3254, 3255, 3256, 3257, 3258, 3259, 3260, 3261, 3262, 3263, 3264, 3265, 3266, 3267, 3268, 3269, 3270, 3271, 3272, 3273, 3274, 3275, 3276, 3277, 3278, 3279, 3280, 3281, 3282, 3283, 3284, 3285, 3286, 3287, 3288, 3289, 3290, 3291, 3292, 3293, 3294, 3295, 3296, 3297, 3298, 3299, 3300, 3301, 3302, 3303, 3304, 3305, 3306, 3307, 3308, 3309, 3310, 3311, 3312, 3313, 3314, 3315, 3316, 3317, 3318, 3319, 3320, 3321, 3322, 3323, 3324, 3325, 3326, 3327, 3328, 3329, 3330, 3331, 3332, 3333, 3334, 3335, 3336, 3337, 3338, 3339, 3340, 3341, 3342, 3343, 3344, 3345, 3346, 3347, 3348, 3349, 3350, 3351, 3352, 3353, 3354, 3355, 3356, 3357, 3358, 3359, 3360, 3361, 3362, 3363, 3364, 3365, 3366, 3367, 3368, 3369, 3370, 3371, 3372, 3373, 3374, 3375, 3376, 3377, 3378, 3379, 3380, 3381, 3382, 3383, 3384, 3385, 3386, 3387, 3388, 3389, 3390, 3391, 3392, 3393, 3394, 3395, 3396, 3397, 3398, 3399, 3400, 3401, 3402, 3403, 3404, 3405, 3406, 3407, 3408, 3409, 3410, 3411, 3412, 3413, 3414, 3415, 3416, 3417, 3418, 3419, 3420, 3421, 3422, 3423, 3424, 3425, 3426, 3427, 3428, 3429, 3430, 3431, 3432, 3433, 3434, 3435, 3436, 3437, 3438, 3439, 3440, 3441, 3442, 3443, 3444, 3445, 3446, 3447, 3448, 3449, 3450, 3451, 3452, 3453, 3454, 3455, 3456, 3457, 3458, 3459, 3460, 3461, 3462, 3463, 3464, 3465, 3466, 3467, 3468, 3469, 3470, 3471, 3472, 3473, 3474, 3475, 3476, 3477, 3478, 3479, 3480, 3481, 3482, 3483, 3484, 3485, 3486, 3487, 3488, 3489, 3490, 3491, 3492, 3493, 3494, 3495, 3496, 3497, 3498, 3499, 3500, 3501, 3502, 3503, 3504, 3505, 3506, 3507, 3508, 3509, 3510, 3511, 3512, 3513, 3514, 3515, 3516, 3517, 3518, 3519, 3520, 3521, 3522, 3523, 3524, 3525, 3526, 3527, 3528, 3529, 3530, 3531, 3532, 3533, 3534, 3535, 3536, 3537, 3538, 3539, 3540, 3541, 3542, 3543, 3544, 3545, 3546, 3547, 3548, 3549, 3550, 3551, 3552, 3553, 3554, 3555, 3556, 3557, 3558, 3559, 3560, 3561, 3562, 3563, 3564, 3565, 3566, 3567, 3568, 3569, 3570, 3571, 3572, 3573, 3574, 3575, 3576, 3577, 3578, 3579, 3580, 3581, 3582, 3583, 3584, 3585, 3586, 3587, 3588, 3589, 3590, 3591, 3592, 3593, 3594, 3595, 3596, 3597, 3598, 3599, 3600, 3601, 3602, 3603, 3604, 3605, 3606, 3607, 3608, 3609, 3610, 3611, 3612, 3613, 3614, 3615, 3616, 3617, 3618, 3619, 3620, 3621, 3622, 3623, 3624, 3625, 3626, 3627, 3628, 3629, 3630, 3631, 3632, 3633, 3634, 3635, 3636, 3637, 3638, 3639, 3640, 3641, 3642, 3643, 3644, 3645, 3646, 3647, 3648, 3649, 3650, 3651, 3652, 3653, 3654, 3655, 3656, 3657, 3658, 3659, 3660, 3661, 3662, 3663, 3664, 3665, 3666, 3667, 3668, 3669, 3670, 3671, 3672, 3673, 3674, 3675, 3676, 3677, 3678, 3679, 3680, 3681, 3682, 3683, 3684, 3685, 3686, 3687, 3688, 3689, 3690, 3691, 3692, 3693, 3694, 3695, 3696, 3697, 3698, 3699, 3700, 3701, 3702, 3703, 3704, 3705, 3706, 3707, 3708, 3709, 3710, 3711, 3712, 3713, 3714, 3715, 3716, 3717, 3718, 3719, 3720, 3721, 3722, 3723, 3724, 3725, 3726, 3727, 3728, 3729, 3730, 3731, 3732, 3733, 3734, 3735, 3736, 3737, 3738, 3739, 3740, 3741, 3742, 3743, 3744, 3745, 3746, 3747, 3748, 3749, 3750, 3751, 3752, 3753, 3754, 3755, 3756, 3757, 3758, 3759, 3760, 3761, 3762, 3763, 3764, 3765, 3766, 3767, 3768, 3769, 3770, 3771, 3772, 3773, 3774, 3775, 3776, 3777, 3778, 3779, 3780, 3781, 3782, 3783, 3784, 3785, 3786, 3787, 3788, 3789, 3790, 3791, 3792, 3793, 3794, 3795, 3796, 3797, 3798, 3799, 3800, 3801, 3802, 3803, 3804, 3805, 3806, 3807, 3808, 3809, 3810, 3811, 3812, 3813, 3814, 3815, 3816, 3817, 3818, 3819, 3820, 3821, 3822, 3823, 3824, 3825, 3826, 3827, 3828, 3829, 3830, 3831, 3832, 3833, 3834, 3835, 3836, 3837, 3838, 3839, 3840, 3841, 3842, 3843, 3844, 3845, 3846, 3847, 3848, 3849, 3850, 3851, 3852, 3853, 3854, 3855, 3856, 3857, 3858, 3859, 3860, 3861, 3862, 3863, 3864, 3865, 3866, 3867, 3868, 3869, 3870, 3871, 3872, 3873, 3874, 3875, 3876, 3877, 3878, 3879, 3880, 3881, 3882, 3883, 3884, 3885, 3886, 3887, 3888, 3889, 3890, 3891, 3892, 3893, 3894, 3895, 3896, 3897, 3898, 3899, 3900, 3901, 3902, 3903, 3904, 3905, 3906, 3907, 3908, 3909, 3910, 3911, 3912, 3913, 3914, 3915, 3916, 3917, 3918, 3919, 3920, 3921, 3922, 3923, 3924, 3925, 3926, 3927, 3928, 3929, 3930, 3931, 3932, 3933, 3934, 3935, 3936, 3937, 3938, 3939, 3940, 3941, 3942, 3943, 3944, 3945, 3946, 3947, 3948, 3949, 3950, 3951, 3952, 3953, 3954, 3955, 3956, 3957, 3958, 3959, 3960, 3961, 3962, 3963, 3964, 3965, 3966, 3967, 3968, 3969, 3970, 3971, 3972, 3973, 3974, 3975, 3976, 3977, 3978, 3979, 3980, 3981, 3982, 3983, 3984, 3985, 3986, 3987, 3988, 3989, 3990, 3991, 3992, 3993, 3994, 3995, 3996, 3997, 3998, 3999, 4000, 4001, 4002, 4003, 4004, 4005, 4006, 4007, 4008, 4009, 4010, 4011, 4012, 4013, 4014, 4015, 4016, 4017, 4018, 4019, 4020, 4021, 4022, 4023, 4024, 4025, 4026, 4027, 4028, 4029, 4030, 4031, 4032, 4033, 4034, 4035, 4036, 4037, 4038, 4039, 4040, 4041, 4042, 4043, 4044, 4045, 4046, 4047, 4048, 4049, 4050, 4051, 4052, 4053, 4054, 4055, 4056, 4057, 4058, 4059, 4060, 4061, 4062, 4063, 4064, 4065, 4066, 4067, 4068, 4069, 4070, 4071, 4072, 4073, 4074, 4075, 4076, 4077, 4078, 4079, 4080, 4081, 4082, 4083, 4084, 4085, 4086, 4087, 4088, 4089, 4090, 4091, 4092, 4093, 4094, 4095, 4096, 4097, 4098, 4099, 4100, 4101, 4102, 4103, 4104, 4105, 4106, 4107, 4108, 4109, 4110, 4111, 4112, 4113, 4114, 4115, 4116, 4117, 4118, 4119, 4120, 4121, 4122, 4123, 4124, 4125, 4126, 4127, 4128, 4129, 4130, 4131, 4132, 4133, 4134, 4135, 4136, 4137, 4138, 4139, 4140, 4141, 4142, 4143, 4144, 4145, 4146, 4147, 4148, 4149, 4150, 4151, 4152, 4153, 4154, 4155, 4156, 4157, 4158, 4159, 4160, 4161, 4162, 4163, 4164, 4165, 4166, 4167, 4168, 4169, 4170, 4171, 4172, 4173, 4174, 4175, 4176, 4177, 4178, 4179, 4180, 4181, 4182, 4183, 4184, 4185, 4186, 4187, 4188, 4189, 4190, 4191, 4192, 4193, 4194, 4195, 4196, 4197, 4198, 4199, 4200, 4201, 4202, 4203, 4204, 4205, 4206, 4207, 4208, 4209, 4210, 4211, 4212, 4213, 4214, 4215, 4216, 4217, 4218, 4219, 4220, 4221, 4222, 4223, 4224, 4225, 4226, 4227, 4228, 4229, 4230, 4231, 4232, 4233, 4234, 4235, 4236, 4237, 4238, 4239, 4240, 4241, 4242, 4243, 4244, 4245, 4246, 4247, 4248, 4249, 4250, 4251, 4252, 4253, 4254, 4255, 4256, 4257, 4258, 4259, 4260, 4261, 4262, 4263, 4264, 4265, 4266, 4267, 4268, 4269, 4270, 4271, 4272, 4273, 4274, 4275, 4276, 4277, 4278, 4279, 4280, 4281, 4282, 4283, 4284, 4285, 4286, 4287, 4288, 4289, 4290, 4291, 4292, 4293, 4294, 4295, 4296, 4297, 4298, 4299, 4300, 4301, 4302, 4303, 4304, 4305, 4306, 4307, 4308, 4309, 4310, 4311, 4312, 4313, 4314, 4315, 4316, 4317, 4318, 4319, 4320, 4321, 4322, 4323, 4324, 4325, 4326, 4327, 4328, 4329, 4330, 4331, 4332, 4333, 4334, 4335, 4336, 4337, 4338, 4339, 4340, 4341, 4342, 4343, 4344, 4345, 4346, 4347, 4348, 4349, 4350, 4351, 4352, 4353, 4354, 4355, 4356, 4357, 4358, 4359, 4360, 4361, 4362, 4363, 4364, 4365, 4366, 4367, 4368, 4369, 4370, 4371, 4372, 4373, 4374, 4375, 4376, 4377, 4378, 4379, 4380, 4381, 4382, 4383, 4384, 4385, 4386, 4387, 4388, 4389, 4390, 4391, 4392, 4393, 4394, 4395, 4396, 4397, 4398, 4399, 4400, 4401, 4402, 4403, 4404, 4405, 4406, 4407, 4408, 4409, 4410, 4411, 4412, 4413, 4414, 4415, 4416, 4417, 4418, 4419, 4420, 4421, 4422, 4423, 4424, 4425, 4426, 4427, 4428, 4429, 4430, 4431, 4432, 4433, 4434, 4435, 4436, 4437, 4438, 4439, 4440, 4441, 4442, 4443, 4444, 4445, 4446, 4447, 4448, 4449, 4450, 4451, 4452, 4453, 4454, 4455, 4456, 4457, 4458, 4459, 4460, 4461, 4462, 4463, 4464, 4465, 4466, 4467, 4468, 4469, 4470, 4471, 4472, 4473, 4474, 4475, 4476, 4477, 4478, 4479, 4480, 4481, 4482, 4483, 4484, 4485, 4486, 4487, 4488, 4489, 4490, 4491, 4492, 4493, 4494, 4495, 4496, 4497, 4498, 4499, 4500, 4501, 4502, 4503, 4504, 4505, 4506, 4507, 4508, 4509, 4510, 4511, 4512, 4513, 4514, 4515, 4516, 4517, 4518, 4519, 4520, 4521, 4522, 4523, 4524, 4525, 4526, 4527, 4528, 4529, 4530, 4531, 4532, 4533, 4534, 4535, 4536, 4537, 4538, 4539, 4540, 4541, 4542, 4543, 4544, 4545, 4546, 4547, 4548, 4549, 4550, 4551, 4552, 4553, 4554, 4555, 4556, 4557, 4558, 4559, 4560, 4561, 4562, 4563, 4564, 4565, 4566, 4567, 4568, 4569, 4570, 4571, 4572, 4573, 4574, 4575, 4576, 4577, 4578, 4579, 4580, 4581, 4582, 4583, 4584, 4585, 4586, 4587, 4588, 4589, 4590, 4591, 4592, 4593, 4594, 4595, 4596, 4597, 4598, 4599, 4600, 4601, 4602, 4603, 4604, 4605, 4606, 4607, 4608, 4609, 4610, 4611, 4612, 4613, 4614, 4615, 4616, 4617, 4618, 4619, 4620, 4621, 4622, 4623, 4624, 4625, 4626, 4627, 4628, 4629, 4630, 4631, 4632, 4633, 4634, 4635, 4636, 4637, 4638, 4639, 4640, 4641, 4642, 4643, 4644, 4645, 4646, 4647, 4648, 4649, 4650, 4651, 4652, 4653, 4654, 4655, 4656, 4657, 4658, 4659, 4660, 4661, 4662, 4663, 4664, 4665, 4666, 4667, 4668, 4669, 4670, 4671, 4672, 4673, 4674, 4675, 4676, 4677, 4678, 4679, 4680, 4681, 4682, 4683, 4684, 4685, 4686, 4687, 4688, 4689, 4690, 4691, 4692, 4693, 4694, 4695, 4696, 4697, 4698, 4699, 4700, 4701, 4702, 4703, 4704, 4705, 4706, 4707, 4708, 4709, 4710, 4711, 4712, 4713, 4714, 4715, 4716, 4717, 4718, 4719, 4720, 4721, 4722, 4723, 4724, 4725, 4726, 4727, 4728, 4729, 4730, 4731, 4732, 4733, 4734, 4735, 4736, 4737, 4738, 4739, 4740, 4741, 4742, 4743, 4744, 4745, 4746, 4747, 4748, 4749, 4750, 4751, 4752, 4753, 4754, 4755, 4756, 4757, 4758, 4759, 4760, 4761, 4762, 4763, 4764, 4765, 4766, 4767, 4768, 4769, 4770, 4771, 4772, 4773, 4774, 4775, 4776, 4777, 4778, 4779, 4780, 4781, 4782, 4783, 4784, 4785, 4786, 4787, 4788, 4789, 4790, 4791, 4792, 4793, 4794, 4795, 4796, 4797, 4798, 4799, 4800, 4801, 4802, 4803, 4804, 4805, 4806, 4807, 4808, 4809, 4810, 4811, 4812, 4813, 4814, 4815, 4816, 4817, 4818, 4819, 4820, 4821, 4822, 4823, 4824, 4825, 4826, 4827, 4828, 4829, 4830, 4831, 4832, 4833, 4834, 4835, 4836, 4837, 4838, 4839, 4840, 4841, 4842, 4843, 4844, 4845, 4846, 4847, 4848, 4849, 4850, 4851, 4852, 4853, 4854, 4855, 4856, 4857, 4858, 4859, 4860, 4861, 4862, 4863, 4864, 4865, 4866, 4867, 4868, 4869, 4870, 4871, 4872, 4873, 4874, 4875, 4876, 4877, 4878, 4879, 4880, 4881, 4882, 4883, 4884, 4885, 4886, 4887, 4888, 4889, 4890, 4891, 4892, 4893, 4894, 4895, 4896, 4897, 4898, 4899, 4900, 4901, 4902, 4903, 4904, 4905, 4906, 4907, 4908, 4909, 4910, 4911, 4912, 4913, 4914, 4915, 4916, 4917, 4918, 4919, 4920, 4921, 4922, 4923, 4924, 4925, 4926, 4927, 4928, 4929, 4930, 4931, 4932, 4933, 4934, 4935, 4936, 4937, 4938, 4939, 4940, 4941, 4942, 4943, 4944, 4945, 4946, 4947, 4948, 4949, 4950, 4951, 4952, 4953, 4954, 4955, 4956, 4957, 4958, 4959, 4960, 4961, 4962, 4963, 4964, 4965, 4966, 4967, 4968, 4969, 4970, 4971, 4972, 4973, 4974, 4975, 4976, 4977, 4978, 4979, 4980, 4981, 4983, 4984, 4985, 4986, 4987, 4988, 4989, 4990, 4991, 4992, 4993, 4994, 4995, 4996, 4997, 4998, 4999, 5000, 5001, 5002, 5003, 5004, 5005, 5006, 5007, 5008, 5009, 5010, 5011, 5012, 5013, 5014, 5015, 5016, 5017, 5018, 5019, 5020, 5021, 5022, 5023, 5024, 5025, 5026, 5027, 5028, 5029, 5030, 5031, 5032, 5033, 5034, 5035, 5036, 5037, 5038, 5039, 5040, 5041, 5042, 5043, 5044, 5045, 5046, 5047, 5048, 5049, 5050, 5051, 5052, 5053, 5054, 5055, 5056, 5057, 5058, 5059, 5060, 5061, 5062, 5063, 5064, 5065, 5066, 5067, 5068, 5069, 5070, 5071, 5072, 5073, 5074, 5075, 5076, 5077, 5078, 5079, 5080, 5081, 5082, 5083, 5084, 5085, 5086, 5087, 5088, 5089, 5090, 5091, 5092, 5093, 5094, 5095, 5096, 5097, 5098, 5099, 5100, 5101, 5102, 5103, 5104, 5105, 5106, 5107, 5108, 5109, 5110, 5111, 5112, 5113, 5114, 5115, 5116, 5117, 5118, 5119, 5120, 5121, 5122, 5123, 5124, 5125, 5126, 5127, 5128, 5129, 5130, 5131, 5132, 5133, 5134, 5135, 5136, 5137, 5138, 5139, 5140, 5141, 5142, 5143, 5144, 5145, 5146, 5147, 5148, 5149, 5150, 5151, 5152, 5153, 5154, 5155, 5156, 5157, 5158, 5159, 5160, 5161, 5162, 5163, 5164, 5165, 5166, 5167, 5168, 5169, 5170, 5171, 5172, 5173, 5174, 5175, 5176, 5177, 5178, 5179, 5180, 5181, 5182, 5183, 5184, 5185, 5186, 5187, 5188, 5189, 5190, 5191, 5192, 5193, 5194, 5195, 5196, 5197, 5198, 5199, 5200, 5201, 5202, 5203, 5204, 5205, 5206, 5207, 5208, 5209, 5210, 5211, 5212, 5213, 5214, 5215, 5216, 5217, 5218, 5219, 5220, 5221, 5222, 5223, 5224, 5225, 5226, 5227, 5228, 5229, 5230, 5231, 5232, 5233, 5234, 5235, 5236, 5237, 5238, 5239, 5240, 5241, 5242, 5243, 5244, 5245, 5246, 5247, 5248, 5249, 5250, 5251, 5252, 5253, 5254, 5255, 5256, 5257, 5258, 5259, 5260, 5261, 5262, 5263, 5264, 5265, 5266, 5267, 5268, 5269, 5270, 5271, 5272, 5273, 5274, 5275, 5276, 5277, 5278, 5279, 5280, 5281, 5282, 5283, 5284, 5285, 5286, 5287, 5288, 5289, 5290, 5291, 5292, 5293, 5294, 5295, 5296, 5297, 5298, 5299, 5300, 5301, 5302, 5303, 5304, 5305, 5306, 5307, 5308, 5309, 5310, 5311, 5312, 5313, 5314, 5315, 5316, 5317, 5318, 5319, 5320, 5321, 5322, 5323, 5324, 5325, 5326, 5327, 5328, 5329, 5330, 5331, 5332, 5333, 5334, 5335, 5336, 5337, 5338, 5339, 5340, 5341, 5342, 5343, 5344, 5345, 5346, 5347, 5348, 5349, 5350, 5351, 5352, 5353, 5354, 5355, 5356, 5357, 5358, 5359, 5360, 5361, 5362, 5363, 5364, 5365, 5366, 5367, 5368, 5369, 5370, 5371, 5372, 5373, 5374, 5375, 5376, 5377, 5378, 5379, 5380, 5381, 5382, 5383, 5384, 5385, 5386, 5387, 5388, 5389, 5390, 5391, 5392, 5393, 5394, 5395, 5396, 5397, 5398, 5399, 5400, 5401, 5402, 5403, 5404, 5405, 5406, 5407, 5408, 5409, 5410, 5411, 5412, 5413, 5414, 5415, 5416, 5417, 5418, 5419, 5420, 5421, 5422, 5423, 5424, 5425, 5426, 5427, 5428, 5429, 5430, 5431, 5432, 5433, 5434, 5435, 5436, 5437, 5438, 5439, 5440, 5441, 5442, 5443, 5444, 5445, 5446, 5447, 5448, 5449, 5450, 5451, 5452, 5453, 5454, 5455, 5456, 5457, 5458, 5459, 5460, 5461, 5462, 5463, 5464, 5465, 5466, 5467, 5468, 5469, 5470, 5471, 5472, 5473, 5474, 5475, 5476, 5477, 5478, 5479, 5480, 5481, 5482, 5483, 5484, 5485, 5486, 5487, 5488, 5489, 5490, 5491, 5492, 5493, 5494, 5495, 5496, 5497, 5498, 5499, 5500, 5501, 5502, 5503, 5504, 5505, 5506, 5507, 5508, 5509, 5510, 5511, 5512, 5513, 5514, 5515, 5516, 5517, 5518, 5519, 5520, 5521, 5522, 5523, 5524, 5525, 5526, 5527, 5528, 5529, 5530, 5531, 5532, 5533, 5534, 5535, 5536, 5537, 5538, 5539, 5540, 5541, 5542, 5543, 5544, 5545, 5546, 5547, 5548, 5549, 5550, 5551, 5552, 5553, 5554, 5555, 5556, 5557, 5558, 5559, 5560, 5561, 5562, 5563, 5564, 5565, 5566, 5567, 5568, 5569, 5570, 5571, 5572, 5573, 5574, 5575, 5576, 5577, 5578, 5579, 5580, 5581, 5582, 5583, 5584, 5585, 5586, 5587, 5588, 5589, 5590, 5591, 5592, 5593, 5594, 5595, 5596, 5597, 5598, 5599, 5600, 5601, 5602, 5603, 5604, 5605, 5606, 5607, 5608, 5609, 5610, 5611, 5612, 5613, 5614, 5615, 5616, 5617, 5618, 5619, 5620, 5621, 5622, 5623, 5624, 5625, 5626, 5627, 5628, 5629, 5630, 5631, 5632, 5633, 5634, 5635, 5636, 5637, 5638, 5639, 5640, 5641, 5642, 5643, 5644, 5645, 5646, </t>
         </is>
       </c>
-      <c r="BP3" t="n">
+      <c r="BV3" t="n">
         <v>0.07673860911270983</v>
       </c>
-      <c r="BQ3" t="inlineStr">
+      <c r="BW3" t="inlineStr">
         <is>
           <t>{'Numk': 16, 'KPar': 10, 'Bucket_index': 1000}</t>
         </is>
       </c>
-      <c r="BR3" t="n">
+      <c r="BX3" t="n">
         <v>413.5598660029937</v>
       </c>
-      <c r="BS3" t="inlineStr">
+      <c r="BY3" t="inlineStr">
         <is>
           <t>no</t>
         </is>
       </c>
-      <c r="BT3" t="n">
-        <v>0</v>
-      </c>
-      <c r="BU3" t="inlineStr">
+      <c r="BZ3" t="n">
+        <v>0</v>
+      </c>
+      <c r="CA3" t="inlineStr">
         <is>
           <t>params</t>
         </is>
       </c>
-      <c r="BV3" t="n">
+      <c r="CB3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1442,93 +1508,111 @@
       <c r="AY4" t="n">
         <v>2</v>
       </c>
-      <c r="AZ4" t="inlineStr"/>
-      <c r="BA4" t="inlineStr">
+      <c r="AZ4" t="n">
+        <v>2</v>
+      </c>
+      <c r="BA4" t="n">
+        <v>2</v>
+      </c>
+      <c r="BB4" t="n">
+        <v>2</v>
+      </c>
+      <c r="BC4" t="n">
+        <v>2</v>
+      </c>
+      <c r="BD4" t="n">
+        <v>2</v>
+      </c>
+      <c r="BE4" t="n">
+        <v>2</v>
+      </c>
+      <c r="BF4" t="inlineStr"/>
+      <c r="BG4" t="inlineStr">
         <is>
           <t>nab-data/realKnownCause/ec2_request_latency_system_failure.csv</t>
         </is>
       </c>
-      <c r="BB4" t="n">
+      <c r="BH4" t="n">
         <v>4032</v>
       </c>
-      <c r="BC4" t="inlineStr">
+      <c r="BI4" t="inlineStr">
         <is>
           <t>NAB</t>
         </is>
       </c>
-      <c r="BD4" t="n">
-        <v>3</v>
-      </c>
-      <c r="BE4" t="inlineStr">
+      <c r="BJ4" t="n">
+        <v>3</v>
+      </c>
+      <c r="BK4" t="inlineStr">
         <is>
           <t>2014; 3328; 3956</t>
         </is>
       </c>
-      <c r="BF4" t="n">
+      <c r="BL4" t="n">
         <v>134</v>
       </c>
-      <c r="BG4" t="inlineStr">
-        <is>
-          <t>[934, 1296, 1441, 1476, 1500, 1547, 1568, 1665, 1673, 1687, 1690, 1706, 1709, 1712, 1738, 1783, 1787, 1805, 1823, 1862, 1992, 2001, 2011, 2020, 2048, 2081, 2082, 2197, 2232, 2233, 2288, 2458, 2506, 3107, 3193, 3391, 3394, 3395, 3396, 3421, 3577, 3597, 3874, 3980, 4023, 4024, 4025, 4026, 4027, 4028, 4029, 4030, 4031]</t>
-        </is>
-      </c>
-      <c r="BH4" t="n">
-        <v>0.1935483870967742</v>
-      </c>
-      <c r="BI4" t="inlineStr">
-        <is>
-          <t>{'initial_window': 112, 'window_size': 511, 'num_trees': 29, 'max_depth': 17}</t>
-        </is>
-      </c>
-      <c r="BJ4" t="n">
-        <v>83.80600588605739</v>
-      </c>
-      <c r="BK4" t="inlineStr">
+      <c r="BM4" t="inlineStr">
+        <is>
+          <t>[2081, 3394, 3395, 4023, 4025, 4027, 4029, 4030, 4031]</t>
+        </is>
+      </c>
+      <c r="BN4" t="n">
+        <v>1</v>
+      </c>
+      <c r="BO4" t="inlineStr">
+        <is>
+          <t>{'initial_window': 303, 'window_size': 487, 'num_trees': 24, 'max_depth': 13}</t>
+        </is>
+      </c>
+      <c r="BP4" t="n">
+        <v>10.23753639101051</v>
+      </c>
+      <c r="BQ4" t="inlineStr">
         <is>
           <t>[2102, 3413, 3415]</t>
         </is>
       </c>
-      <c r="BL4" t="n">
+      <c r="BR4" t="n">
         <v>0.8</v>
       </c>
-      <c r="BM4" t="inlineStr">
+      <c r="BS4" t="inlineStr">
         <is>
           <t>{'AR_window_size': 20, 'differencing-order': 1}</t>
         </is>
       </c>
-      <c r="BN4" t="n">
+      <c r="BT4" t="n">
         <v>32.07578844204545</v>
       </c>
-      <c r="BO4" t="inlineStr">
+      <c r="BU4" t="inlineStr">
         <is>
           <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86, 87, 88, 89, 90, 91, 92, 93, 94, 95, 96, 97, 98, 99, 100, 101, 102, 103, 104, 105, 106, 107, 108, 109, 110, 111, 112, 113, 114, 115, 116, 117, 118, 119, 120, 121, 122, 123, 124, 125, 126, 127, 128, 129, 130, 131, 132, 133, 134, 135, 136, 137, 138, 139, 140, 141, 142, 143, 144, 145, 146, 147, 148, 149, 150, 151, 152, 153, 154, 155, 156, 157, 158, 159, 160, 161, 162, 163, 164, 165, 166, 167, 168, 169, 170, 171, 172, 173, 174, 175, 176, 177, 178, 179, 180, 181, 182, 183, 184, 185, 186, 187, 188, 189, 190, 191, 192, 193, 194, 195, 196, 197, 198, 199, 200, 201, 202, 203, 204, 205, 206, 207, 208, 209, 210, 211, 212, 213, 214, 215, 216, 217, 218, 219, 220, 221, 222, 223, 224, 225, 226, 227, 228, 229, 230, 231, 232, 233, 234, 235, 236, 237, 238, 239, 240, 241, 242, 243, 244, 245, 246, 247, 248, 249, 250, 251, 252, 253, 254, 255, 256, 257, 258, 259, 260, 261, 262, 263, 264, 265, 266, 267, 268, 269, 270, 271, 272, 273, 274, 275, 276, 277, 278, 279, 280, 281, 282, 283, 284, 285, 286, 287, 288, 289, 290, 291, 292, 293, 294, 295, 296, 297, 298, 299, 300, 301, 302, 303, 304, 305, 306, 307, 308, 309, 310, 311, 312, 313, 314, 315, 316, 317, 318, 319, 320, 321, 322, 323, 324, 325, 326, 327, 328, 329, 330, 331, 332, 333, 334, 335, 336, 337, 338, 339, 340, 341, 342, 343, 344, 345, 346, 347, 348, 349, 350, 351, 352, 353, 354, 355, 356, 357, 358, 359, 360, 361, 362, 363, 364, 365, 366, 367, 368, 369, 370, 371, 372, 373, 374, 375, 376, 377, 378, 379, 380, 381, 382, 383, 384, 385, 386, 387, 388, 389, 390, 391, 392, 393, 394, 395, 396, 397, 398, 399, 400, 401, 402, 403, 404, 405, 406, 407, 408, 409, 410, 411, 412, 413, 414, 415, 416, 417, 418, 419, 420, 421, 422, 423, 424, 425, 426, 427, 428, 429, 430, 431, 432, 433, 434, 435, 436, 437, 438, 439, 440, 441, 442, 443, 444, 445, 446, 447, 448, 449, 450, 451, 452, 453, 454, 455, 456, 457, 458, 459, 460, 461, 462, 463, 464, 465, 466, 467, 468, 469, 470, 471, 472, 473, 474, 475, 476, 477, 478, 479, 480, 481, 482, 483, 484, 485, 486, 487, 488, 489, 490, 491, 492, 493, 494, 495, 496, 497, 498, 499, 500, 501, 502, 503, 504, 505, 506, 507, 508, 509, 510, 511, 512, 513, 514, 515, 516, 517, 518, 519, 520, 521, 522, 523, 524, 525, 526, 527, 528, 529, 530, 531, 532, 533, 534, 535, 536, 537, 538, 539, 540, 541, 542, 543, 544, 545, 546, 547, 548, 549, 550, 551, 552, 553, 554, 555, 556, 557, 558, 559, 560, 561, 562, 563, 564, 565, 566, 567, 568, 569, 570, 571, 572, 573, 574, 575, 576, 577, 578, 579, 580, 581, 582, 583, 584, 585, 586, 587, 588, 589, 590, 591, 592, 593, 594, 595, 596, 597, 598, 599, 600, 601, 602, 603, 604, 605, 606, 607, 608, 609, 610, 611, 612, 613, 614, 615, 616, 617, 618, 619, 620, 621, 622, 623, 624, 625, 626, 627, 628, 629, 630, 631, 632, 633, 634, 635, 636, 637, 638, 639, 640, 641, 642, 643, 644, 645, 646, 647, 648, 649, 650, 651, 652, 653, 654, 655, 656, 657, 658, 659, 660, 661, 662, 663, 664, 665, 666, 667, 668, 669, 670, 671, 672, 673, 674, 675, 676, 677, 678, 679, 680, 681, 682, 683, 684, 685, 686, 687, 688, 689, 690, 691, 692, 693, 694, 695, 696, 697, 698, 699, 700, 701, 702, 703, 704, 705, 706, 707, 708, 709, 710, 711, 712, 713, 714, 715, 716, 717, 718, 719, 720, 721, 722, 723, 724, 725, 726, 727, 728, 729, 730, 731, 732, 733, 734, 735, 736, 737, 738, 739, 740, 741, 742, 743, 744, 745, 746, 747, 748, 749, 750, 751, 752, 753, 754, 755, 756, 757, 758, 759, 760, 761, 762, 763, 764, 765, 766, 767, 768, 769, 770, 771, 772, 773, 774, 775, 776, 777, 778, 779, 780, 781, 782, 783, 784, 785, 786, 787, 788, 789, 790, 791, 792, 793, 794, 795, 796, 797, 798, 799, 800, 801, 802, 803, 804, 805, 806, 807, 808, 809, 810, 811, 812, 813, 814, 815, 816, 817, 818, 819, 820, 821, 822, 823, 824, 825, 826, 827, 828, 829, 830, 831, 832, 833, 834, 835, 836, 837, 838, 839, 840, 841, 842, 843, 844, 845, 846, 847, 848, 849, 850, 851, 852, 853, 854, 855, 856, 857, 858, 859, 860, 861, 862, 863, 864, 865, 866, 867, 868, 869, 870, 871, 872, 873, 874, 875, 876, 877, 878, 879, 880, 881, 882, 883, 884, 885, 886, 887, 888, 889, 890, 891, 892, 893, 894, 895, 896, 897, 898, 899, 900, 901, 902, 903, 904, 905, 906, 907, 908, 909, 910, 911, 912, 913, 914, 915, 916, 917, 918, 919, 920, 921, 922, 923, 924, 925, 926, 927, 928, 929, 930, 931, 932, 933, 934, 935, 936, 937, 938, 939, 940, 941, 942, 943, 944, 945, 946, 947, 948, 949, 950, 951, 952, 953, 954, 955, 956, 957, 958, 959, 960, 961, 962, 963, 964, 965, 966, 967, 968, 969, 970, 971, 972, 973, 974, 975, 976, 977, 978, 979, 980, 981, 982, 983, 984, 985, 986, 987, 988, 989, 990, 991, 992, 993, 994, 995, 996, 997, 998, 999, 1000, 1001, 1002, 1003, 1004, 1005, 1006, 1007, 1008, 1009, 1010, 1011, 1012, 1013, 1014, 1015, 1016, 1017, 1018, 1019, 1020, 1021, 1022, 1023, 1024, 1025, 1026, 1027, 1028, 1029, 1030, 1031, 1032, 1033, 1034, 1035, 1036, 1037, 1038, 1039, 1040, 1041, 1042, 1043, 1044, 1045, 1046, 1047, 1048, 1049, 1050, 1051, 1052, 1053, 1054, 1055, 1056, 1057, 1058, 1059, 1060, 1061, 1062, 1063, 1064, 1065, 1066, 1067, 1068, 1069, 1070, 1071, 1072, 1073, 1074, 1075, 1076, 1077, 1078, 1079, 1080, 1081, 1082, 1083, 1084, 1085, 1086, 1087, 1088, 1089, 1090, 1091, 1092, 1093, 1094, 1095, 1096, 1097, 1098, 1099, 1100, 1101, 1102, 1103, 1104, 1105, 1106, 1107, 1108, 1109, 1110, 1111, 1112, 1113, 1114, 1115, 1116, 1117, 1118, 1119, 1120, 1121, 1122, 1123, 1124, 1125, 1126, 1127, 1128, 1129, 1130, 1131, 1132, 1133, 1134, 1135, 1136, 1137, 1138, 1139, 1140, 1141, 1142, 1143, 1144, 1145, 1146, 1147, 1148, 1149, 1150, 1151, 1152, 1153, 1154, 1155, 1156, 1157, 1158, 1159, 1160, 1161, 1162, 1163, 1164, 1165, 1166, 1167, 1168, 1169, 1170, 1171, 1172, 1173, 1174, 1175, 1176, 1177, 1178, 1179, 1180, 1181, 1182, 1183, 1184, 1185, 1186, 1187, 1188, 1189, 1190, 1191, 1192, 1193, 1194, 1195, 1196, 1197, 1198, 1199, 1200, 1201, 1202, 1203, 1204, 1205, 1206, 1207, 1208, 1209, 1210, 1211, 1212, 1213, 1214, 1215, 1216, 1217, 1218, 1219, 1220, 1221, 1222, 1223, 1224, 1225, 1226, 1227, 1228, 1229, 1230, 1231, 1232, 1233, 1234, 1235, 1236, 1237, 1238, 1239, 1240, 1241, 1242, 1243, 1244, 1245, 1246, 1247, 1248, 1249, 1250, 1251, 1252, 1253, 1254, 1255, 1256, 1257, 1258, 1259, 1260, 1261, 1262, 1263, 1264, 1265, 1266, 1267, 1268, 1269, 1270, 1271, 1272, 1273, 1274, 1275, 1276, 1277, 1278, 1279, 1280, 1281, 1282, 1283, 1284, 1285, 1286, 1287, 1288, 1289, 1290, 1291, 1292, 1293, 1294, 1295, 1296, 1297, 1298, 1299, 1300, 1301, 1302, 1303, 1304, 1305, 1306, 1307, 1308, 1309, 1310, 1311, 1312, 1313, 1314, 1315, 1316, 1317, 1318, 1319, 1320, 1321, 1322, 1323, 1324, 1325, 1326, 1327, 1328, 1329, 1330, 1331, 1332, 1333, 1334, 1335, 1336, 1337, 1338, 1339, 1340, 1341, 1342, 1343, 1344, 1345, 1346, 1347, 1348, 1349, 1350, 1351, 1352, 1353, 1354, 1355, 1356, 1357, 1358, 1359, 1360, 1361, 1362, 1363, 1364, 1365, 1366, 1367, 1368, 1369, 1370, 1371, 1372, 1373, 1374, 1375, 1376, 1377, 1378, 1379, 1380, 1381, 1382, 1383, 1384, 1385, 1386, 1387, 1388, 1389, 1390, 1391, 1392, 1393, 1394, 1395, 1396, 1397, 1398, 1399, 1400, 1401, 1402, 1403, 1404, 1405, 1406, 1407, 1408, 1409, 1410, 1411, 1412, 1413, 1414, 1415, 1416, 1417, 1418, 1419, 1420, 1421, 1422, 1423, 1424, 1425, 1426, 1427, 1428, 1429, 1430, 1431, 1432, 1433, 1434, 1435, 1436, 1437, 1438, 1439, 1440, 1441, 1442, 1443, 1444, 1445, 1446, 1447, 1448, 1449, 1450, 1451, 1452, 1453, 1454, 1455, 1456, 1457, 1458, 1459, 1460, 1461, 1462, 1463, 1464, 1465, 1466, 1467, 1468, 1469, 1470, 1471, 1472, 1473, 1474, 1475, 1476, 1477, 1478, 1479, 1480, 1481, 1482, 1483, 1484, 1485, 1486, 1487, 1488, 1489, 1490, 1491, 1492, 1493, 1494, 1495, 1496, 1497, 1498, 1499, 1500, 1501, 1502, 1503, 1504, 1505, 1506, 1507, 1508, 1509, 1510, 1511, 1512, 1513, 1514, 1515, 1516, 1517, 1518, 1519, 1520, 1521, 1522, 1523, 1524, 1525, 1526, 1527, 1528, 1529, 1530, 1531, 1532, 1533, 1534, 1535, 1536, 1537, 1538, 1539, 1540, 1541, 1542, 1543, 1544, 1545, 1546, 1547, 1548, 1549, 1550, 1551, 1552, 1553, 1554, 1555, 1556, 1557, 1558, 1559, 1560, 1561, 1562, 1563, 1564, 1565, 1566, 1567, 1568, 1569, 1570, 1571, 1572, 1573, 1574, 1575, 1576, 1577, 1578, 1579, 1580, 1581, 1582, 1583, 1584, 1585, 1586, 1587, 1588, 1589, 1590, 1591, 1592, 1593, 1594, 1595, 1596, 1597, 1598, 1599, 1600, 1601, 1602, 1603, 1604, 1605, 1606, 1607, 1608, 1609, 1610, 1611, 1612, 1613, 1614, 1615, 1616, 1617, 1618, 1619, 1620, 1621, 1622, 1623, 1624, 1625, 1626, 1627, 1628, 1629, 1630, 1631, 1632, 1633, 1634, 1635, 1636, 1637, 1638, 1639, 1640, 1641, 1642, 1643, 1644, 1645, 1646, 1647, 1648, 1649, 1650, 1651, 1652, 1653, 1654, 1655, 1656, 1657, 1658, 1659, 1660, 1661, 1662, 1663, 1664, 1665, 1666, 1667, 1668, 1669, 1670, 1671, 1672, 1673, 1674, 1675, 1676, 1677, 1678, 1679, 1680, 1681, 1682, 1683, 1684, 1685, 1686, 1687, 1688, 1689, 1690, 1691, 1692, 1693, 1694, 1695, 1696, 1697, 1698, 1699, 1700, 1701, 1702, 1703, 1704, 1705, 1706, 1707, 1708, 1709, 1710, 1711, 1712, 1713, 1714, 1715, 1716, 1717, 1718, 1719, 1720, 1721, 1722, 1723, 1724, 1725, 1726, 1727, 1728, 1729, 1730, 1731, 1732, 1733, 1734, 1735, 1736, 1737, 1738, 1739, 1740, 1741, 1742, 1743, 1744, 1745, 1746, 1747, 1748, 1749, 1750, 1751, 1752, 1753, 1754, 1755, 1756, 1757, 1758, 1759, 1760, 1761, 1762, 1763, 1764, 1765, 1766, 1767, 1768, 1769, 1770, 1771, 1772, 1773, 1774, 1775, 1776, 1777, 1778, 1779, 1780, 1781, 1782, 1783, 1784, 1785, 1786, 1787, 1788, 1789, 1790, 1791, 1792, 1793, 1794, 1795, 1796, 1797, 1798, 1799, 1800, 1801, 1802, 1803, 1804, 1805, 1806, 1807, 1808, 1809, 1810, 1811, 1812, 1813, 1814, 1815, 1816, 1817, 1818, 1819, 1820, 1821, 1822, 1823, 1824, 1825, 1826, 1827, 1828, 1829, 1830, 1831, 1832, 1833, 1834, 1835, 1836, 1837, 1838, 1839, 1840, 1841, 1842, 1843, 1844, 1845, 1846, 1847, 1848, 1849, 1850, 1851, 1852, 1853, 1854, 1855, 1856, 1857, 1858, 1859, 1860, 1861, 1862, 1863, 1864, 1865, 1866, 1867, 1868, 1869, 1870, 1871, 1872, 1873, 1874, 1875, 1876, 1877, 1878, 1879, 1880, 1881, 1882, 1883, 1884, 1885, 1886, 1887, 1888, 1889, 1890, 1891, 1892, 1893, 1894, 1895, 1896, 1897, 1898, 1899, 1900, 1901, 1902, 1903, 1904, 1905, 1906, 1907, 1908, 1909, 1910, 1911, 1912, 1913, 1914, 1915, 1916, 1917, 1918, 1919, 1920, 1921, 1922, 1923, 1924, 1925, 1926, 1927, 1928, 1929, 1930, 1931, 1932, 1933, 1934, 1935, 1936, 1937, 1938, 1939, 1940, 1941, 1942, 1943, 1944, 1945, 1946, 1947, 1948, 1949, 1950, 1951, 1952, 1953, 1954, 1955, 1956, 1957, 1958, 1959, 1960, 1961, 1962, 1963, 1964, 1965, 1966, 1967, 1968, 1969, 1970, 1971, 1972, 1973, 1974, 1975, 1976, 1977, 1978, 1979, 1980, 1981, 1982, 1983, 1984, 1985, 1986, 1987, 1988, 1989, 1990, 1991, 1992, 1993, 1994, 1995, 1996, 1997, 1998, 1999, 2000, 2001, 2002, 2003, 2004, 2005, 2006, 2007, 2008, 2009, 2010, 2011, 2012, 2013, 2014, 2015, 2016, 2017, 2018, 2019, 2020, 2021, 2022, 2023, 2024, 2025, 2026, 2027, 2028, 2029, 2030, 2031, 2032, 2033, 2034, 2035, 2036, 2037, 2038, 2039, 2040, 2041, 2042, 2043, 2044, 2045, 2046, 2047, 2048, 2049, 2050, 2051, 2052, 2053, 2054, 2055, 2056, 2057, 2058, 2059, 2060, 2061, 2062, 2063, 2064, 2065, 2066, 2067, 2068, 2069, 2070, 2071, 2072, 2073, 2074, 2075, 2076, 2077, 2078, 2079, 2080, 2081, 2082, 2083, 2084, 2085, 2086, 2087, 2088, 2089, 2090, 2091, 2092, 2093, 2094, 2095, 2096, 2097, 2098, 2099, 2100, 2101, 2102, 2103, 2104, 2105, 2106, 2107, 2108, 2109, 2110, 2111, 2112, 2113, 2114, 2115, 2116, 2117, 2118, 2119, 2120, 2121, 2122, 2123, 2124, 2125, 2126, 2127, 2128, 2129, 2130, 2131, 2132, 2133, 2134, 2135, 2136, 2137, 2138, 2139, 2140, 2141, 2142, 2143, 2144, 2145, 2146, 2147, 2148, 2149, 2150, 2151, 2152, 2153, 2154, 2155, 2156, 2157, 2158, 2159, 2160, 2161, 2162, 2163, 2164, 2165, 2166, 2167, 2168, 2169, 2170, 2171, 2172, 2173, 2174, 2175, 2176, 2177, 2178, 2179, 2180, 2181, 2182, 2183, 2184, 2185, 2186, 2187, 2188, 2189, 2190, 2191, 2192, 2193, 2194, 2195, 2196, 2197, 2198, 2199, 2200, 2201, 2202, 2203, 2204, 2205, 2206, 2207, 2208, 2209, 2210, 2211, 2212, 2213, 2214, 2215, 2216, 2217, 2218, 2219, 2220, 2221, 2222, 2223, 2224, 2225, 2226, 2227, 2228, 2229, 2230, 2231, 2232, 2233, 2234, 2235, 2236, 2237, 2238, 2239, 2240, 2241, 2242, 2243, 2244, 2245, 2246, 2247, 2248, 2249, 2250, 2251, 2252, 2253, 2254, 2255, 2256, 2257, 2258, 2259, 2260, 2261, 2262, 2263, 2264, 2265, 2266, 2267, 2268, 2269, 2270, 2271, 2272, 2273, 2274, 2275, 2276, 2277, 2278, 2279, 2280, 2281, 2282, 2283, 2284, 2285, 2286, 2287, 2288, 2289, 2290, 2291, 2292, 2293, 2294, 2295, 2296, 2297, 2298, 2299, 2300, 2301, 2302, 2303, 2304, 2305, 2306, 2307, 2308, 2309, 2310, 2311, 2312, 2313, 2314, 2315, 2316, 2317, 2318, 2319, 2320, 2321, 2322, 2323, 2324, 2325, 2326, 2327, 2328, 2329, 2330, 2331, 2332, 2333, 2334, 2335, 2336, 2337, 2338, 2339, 2340, 2341, 2342, 2343, 2344, 2345, 2346, 2347, 2348, 2349, 2350, 2351, 2352, 2353, 2354, 2355, 2356, 2357, 2358, 2359, 2360, 2361, 2362, 2363, 2364, 2365, 2366, 2367, 2368, 2369, 2370, 2371, 2372, 2373, 2374, 2375, 2376, 2377, 2378, 2379, 2380, 2381, 2382, 2383, 2384, 2385, 2386, 2387, 2388, 2389, 2390, 2391, 2392, 2393, 2394, 2395, 2396, 2397, 2398, 2399, 2400, 2401, 2402, 2403, 2404, 2405, 2406, 2407, 2408, 2409, 2410, 2411, 2412, 2413, 2414, 2415, 2416, 2417, 2418, 2419, 2420, 2421, 2422, 2423, 2424, 2425, 2426, 2427, 2428, 2429, 2430, 2431, 2432, 2433, 2434, 2435, 2436, 2437, 2438, 2439, 2440, 2441, 2442, 2443, 2444, 2445, 2446, 2447, 2448, 2449, 2450, 2451, 2452, 2453, 2454, 2455, 2456, 2457, 2458, 2459, 2460, 2461, 2462, 2463, 2464, 2465, 2466, 2467, 2468, 2469, 2470, 2471, 2472, 2473, 2474, 2475, 2476, 2477, 2478, 2479, 2480, 2481, 2482, 2483, 2484, 2485, 2486, 2487, 2488, 2489, 2490, 2491, 2492, 2493, 2494, 2495, 2496, 2497, 2498, 2499, 2500, 2501, 2502, 2503, 2504, 2505, 2506, 2507, 2508, 2509, 2510, 2511, 2512, 2513, 2514, 2515, 2516, 2517, 2518, 2519, 2520, 2521, 2522, 2523, 2524, 2525, 2526, 2527, 2528, 2529, 2530, 2531, 2532, 2533, 2534, 2535, 2536, 2537, 2538, 2539, 2540, 2541, 2542, 2543, 2544, 2545, 2546, 2547, 2548, 2549, 2550, 2551, 2552, 2553, 2554, 2555, 2556, 2557, 2558, 2559, 2560, 2561, 2562, 2563, 2564, 2565, 2566, 2567, 2568, 2569, 2570, 2571, 2572, 2573, 2574, 2575, 2576, 2577, 2578, 2579, 2580, 2581, 2582, 2583, 2584, 2585, 2586, 2587, 2588, 2589, 2590, 2591, 2592, 2593, 2594, 2595, 2596, 2597, 2598, 2599, 2600, 2601, 2602, 2603, 2604, 2605, 2606, 2607, 2608, 2609, 2610, 2611, 2612, 2613, 2614, 2615, 2616, 2617, 2618, 2619, 2620, 2621, 2622, 2623, 2624, 2625, 2626, 2627, 2628, 2629, 2630, 2631, 2632, 2633, 2634, 2635, 2636, 2637, 2638, 2639, 2640, 2641, 2642, 2643, 2644, 2645, 2646, 2647, 2648, 2649, 2650, 2651, 2652, 2653, 2654, 2655, 2656, 2657, 2658, 2659, 2660, 2661, 2662, 2663, 2664, 2665, 2666, 2667, 2668, 2669, 2670, 2671, 2672, 2673, 2674, 2675, 2676, 2677, 2678, 2679, 2680, 2681, 2682, 2683, 2684, 2685, 2686, 2687, 2688, 2689, 2690, 2691, 2692, 2693, 2694, 2695, 2696, 2697, 2698, 2699, 2700, 2701, 2702, 2703, 2704, 2705, 2706, 2707, 2708, 2709, 2710, 2711, 2712, 2713, 2714, 2715, 2716, 2717, 2718, 2719, 2720, 2721, 2722, 2723, 2724, 2725, 2726, 2727, 2728, 2729, 2730, 2731, 2732, 2733, 2734, 2735, 2736, 2737, 2738, 2739, 2740, 2741, 2742, 2743, 2744, 2745, 2746, 2747, 2748, 2749, 2750, 2751, 2752, 2753, 2754, 2755, 2756, 2757, 2758, 2759, 2760, 2761, 2762, 2763, 2764, 2765, 2766, 2767, 2768, 2769, 2770, 2771, 2772, 2773, 2774, 2775, 2776, 2777, 2778, 2779, 2780, 2781, 2782, 2783, 2784, 2785, 2786, 2787, 2788, 2789, 2790, 2791, 2792, 2793, 2794, 2795, 2796, 2797, 2798, 2799, 2800, 2801, 2802, 2803, 2804, 2805, 2806, 2807, 2808, 2809, 2810, 2811, 2812, 2813, 2814, 2815, 2816, 2817, 2818, 2819, 2820, 2821, 2822, 2823, 2824, 2825, 2826, 2827, 2828, 2829, 2830, 2831, 2832, 2833, 2834, 2835, 2836, 2837, 2838, 2839, 2840, 2841, 2842, 2843, 2844, 2845, 2846, 2847, 2848, 2849, 2850, 2851, 2852, 2853, 2854, 2855, 2856, 2857, 2858, 2859, 2860, 2861, 2862, 2863, 2864, 2865, 2866, 2867, 2868, 2869, 2870, 2871, 2872, 2873, 2874, 2875, 2876, 2877, 2878, 2879, 2880, 2881, 2882, 2883, 2884, 2885, 2886, 2887, 2888, 2889, 2890, 2891, 2892, 2893, 2894, 2895, 2896, 2897, 2898, 2899, 2900, 2901, 2902, 2903, 2904, 2905, 2906, 2907, 2908, 2909, 2910, 2911, 2912, 2913, 2914, 2915, 2916, 2917, 2918, 2919, 2920, 2921, 2922, 2923, 2924, 2925, 2926, 2927, 2928, 2929, 2930, 2931, 2932, 2933, 2934, 2935, 2936, 2937, 2938, 2939, 2940, 2941, 2942, 2943, 2944, 2945, 2946, 2947, 2948, 2949, 2950, 2951, 2952, 2953, 2954, 2955, 2956, 2957, 2958, 2959, 2960, 2961, 2962, 2963, 2964, 2965, 2966, 2967, 2968, 2969, 2970, 2971, 2972, 2973, 2974, 2975, 2976, 2977, 2978, 2979, 2980, 2981, 2982, 2983, 2984, 2985, 2986, 2987, 2988, 2989, 2990, 2991, 2992, 2993, 2994, 2995, 2996, 2997, 2998, 2999, 3000, 3001, 3002, 3003, 3004, 3005, 3006, 3007, 3008, 3009, 3010, 3011, 3012, 3013, 3014, 3015, 3016, 3017, 3018, 3019, 3020, 3021, 3022, 3023, 3024, 3025, 3026, 3027, 3028, 3029, 3030, 3031, 3032, 3033, 3034, 3035, 3036, 3037, 3038, 3039, 3040, 3041, 3042, 3043, 3044, 3045, 3046, 3047, 3048, 3049, 3050, 3051, 3052, 3053, 3054, 3055, 3056, 3057, 3058, 3059, 3060, 3061, 3062, 3063, 3064, 3065, 3066, 3067, 3068, 3069, 3070, 3071, 3072, 3073, 3074, 3075, 3076, 3077, 3078, 3079, 3080, 3081, 3082, 3083, 3084, 3085, 3086, 3087, 3088, 3089, 3090, 3091, 3092, 3093, 3094, 3095, 3096, 3097, 3098, 3099, 3100, 3101, 3102, 3103, 3104, 3105, 3106, 3107, 3108, 3109, 3110, 3111, 3112, 3113, 3114, 3115, 3116, 3117, 3118, 3119, 3120, 3121, 3122, 3123, 3124, 3125, 3126, 3127, 3128, 3129, 3130, 3131, 3132, 3133, 3134, 3135, 3136, 3137, 3138, 3139, 3140, 3141, 3142, 3143, 3144, 3145, 3146, 3147, 3148, 3149, 3150, 3151, 3152, 3153, 3154, 3155, 3156, 3157, 3158, 3159, 3160, 3161, 3162, 3163, 3164, 3165, 3166, 3167, 3168, 3169, 3170, 3171, 3172, 3173, 3174, 3175, 3176, 3177, 3178, 3179, 3180, 3181, 3182, 3183, 3184, 3185, 3186, 3187, 3188, 3189, 3190, 3191, 3192, 3193, 3194, 3195, 3196, 3197, 3198, 3199, 3200, 3201, 3202, 3203, 3204, 3205, 3206, 3207, 3208, 3209, 3210, 3211, 3212, 3213, 3214, 3215, 3216, 3217, 3218, 3219, 3220, 3221, 3222, 3223, 3224, 3225, 3226, 3227, 3228, 3229, 3230, 3231, 3232, 3233, 3234, 3235, 3236, 3237, 3238, 3239, 3240, 3241, 3242, 3243, 3244, 3245, 3246, 3247, 3248, 3249, 3250, 3251, 3252, 3253, 3254, 3255, 3256, 3257, 3258, 3259, 3260, 3261, 3262, 3263, 3264, 3265, 3266, 3267, 3268, 3269, 3270, 3271, 3272, 3273, 3274, 3275, 3276, 3277, 3278, 3279, 3280, 3281, 3282, 3283, 3284, 3285, 3286, 3287, 3288, 3289, 3290, 3291, 3292, 3293, 3294, 3295, 3296, 3297, 3298, 3299, 3300, 3301, 3302, 3303, 3304, 3305, 3306, 3307, 3308, 3309, 3310, 3311, 3312, 3313, 3314, 3315, 3316, 3317, 3318, 3319, 3320, 3321, 3322, 3323, 3324, 3325, 3326, 3327, 3328, 3329, 3330, 3331, 3332, 3333, 3334, 3335, 3336, 3337, 3338, 3339, 3340, 3341, 3342, 3343, 3344, 3345, 3346, 3347, 3348, 3349, 3350, 3351, 3352, 3353, 3354, 3355, 3356, 3357, 3358, 3359, 3360, 3361, 3362, 3363, 3364, 3365, 3366, 3367, 3368, 3369, 3370, 3371, 3372, 3373, 3374, 3375, 3376, 3377, 3378, 3379, 3380, 3381, 3382, 3383, 3384, 3385, 3386, 3387, 3388, 3389, 3390, 3391, 3392, 3393, 3394, 3395, 3396, 3397, 3398, 3399, 3400, 3401, 3402, 3403, 3404, 3405, 3406, 3407, 3408, 3409, 3410, 3411, 3412, 3413, 3414, 3415, 3416, 3417, 3418, 3419, 3420, 3421, 3422, 3423, 3424, 3425, 3426, 3427, 3428, 3429, 3430, 3431, 3432, 3433, 3434, 3435, 3436, 3437, 3438, 3439, 3440, 3441, 3442, 3443, 3444, 3445, 3446, 3447, 3448, 3449, 3450, 3451, 3452, 3453, 3454, 3455, 3456, 3457, 3458, 3459, 3460, 3461, 3462, 3463, 3464, 3465, 3466, 3467, 3468, 3469, 3470, 3471, 3472, 3473, 3474, 3475, 3476, 3477, 3478, 3479, 3480, 3481, 3482, 3483, 3484, 3485, 3486, 3487, 3488, 3489, 3490, 3491, 3492, 3493, 3494, 3495, 3496, 3497, 3498, 3499, 3500, 3501, 3502, 3503, 3504, 3505, 3506, 3507, 3508, 3509, 3510, 3511, 3512, 3513, 3514, 3515, 3516, 3517, 3518, 3519, 3520, 3521, 3522, 3523, 3524, 3525, 3526, 3527, 3528, 3529, 3530, 3531, 3532, 3533, 3534, 3535, 3536, 3537, 3538, 3539, 3540, 3541, 3542, 3543, 3544, 3545, 3546, 3547, 3548, 3549, 3550, 3551, 3552, 3553, 3554, 3555, 3556, 3557, 3558, 3559, 3560, 3561, 3562, 3563, 3564, 3565, 3566, 3567, 3568, 3569, 3570, 3571, 3572, 3573, 3574, 3575, 3576, 3577, 3578, 3579, 3580, 3581, 3582, 3583, 3584, 3585, 3586, 3587, 3588, 3589, 3590, 3591, 3592, 3593, 3594, 3595, 3596, 3597, 3598, 3599, 3600, 3601, 3602, 3603, 3604, 3605, 3606, 3607, 3608, 3609, 3610, 3611, 3612, 3613, 3614, 3615, 3616, 3617, 3618, 3619, 3620, 3621, 3622, 3623, 3624, 3625, 3626, 3627, 3628, 3629, 3630, 3631, 3632, 3633, 3634, 3635, 3636, 3637, 3638, 3639, 3640, 3641, 3642, 3643, 3644, 3645, 3646, 3647, 3648, 3649, 3650, 3651, 3652, 3653, 3654, 3655, 3656, 3657, 3658, 3659, 3660, 3661, 3662, 3663, 3664, 3665, 3666, 3667, 3668, 3669, 3670, 3671, 3672, 3673, 3674, 3675, 3676, 3677, 3678, 3679, 3680, 3681, 3682, 3683, 3684, 3685, 3686, 3687, 3688, 3689, 3690, 3691, 3692, 3693, 3694, 3695, 3696, 3697, 3698, 3699, 3700, 3701, 3702, 3703, 3704, 3705, 3706, 3707, 3708, 3709, 3710, 3711, 3712, 3713, 3714, 3715, 3716, 3717, 3718, 3719, 3720, 3721, 3722, 3723, 3724, 3725, 3726, 3727, 3728, 3729, 3730, 3731, 3732, 3733, 3734, 3735, 3736, 3737, 3738, 3739, 3740, 3741, 3742, 3743, 3744, 3745, 3746, 3747, 3748, 3749, 3750, 3751, 3752, 3753, 3754, 3755, 3756, 3757, 3758, 3759, 3760, 3761, 3762, 3763, 3764, 3765, 3766, 3767, 3768, 3769, 3770, 3771, 3772, 3773, 3774, 3775, 3776, 3777, 3778, 3779, 3780, 3781, 3782, 3783, 3784, 3785, 3786, 3787, 3788, 3789, 3790, 3791, 3792, 3793, 3794, 3795, 3796, 3797, 3798, 3799, 3800, 3801, 3802, 3803, 3804, 3805, 3806, 3807, 3808, 3809, 3810, 3811, 3812, 3813, 3814, 3815, 3816, 3817, 3818, 3819, 3820, 3821, 3822, 3823, 3824, 3825, 3826, 3827, 3828, 3829, 3830, 3831, 3832, 3833, 3834, 3835, 3836, 3837, 3838, 3839, 3840, 3841, 3842, 3843, 3844, 3845, 3846, 3847, 3848, 3849, 3850, 3851, 3852, 3853, 3854, 3855, 3856, 3857, 3858, 3859, 3860, 3861, 3862, 3863, 3864, 3865, 3866, 3867, 3868, 3869, 3870, 3871, 3872, 3873, 3874, 3875, 3876, 3877, 3878, 3879, 3880, 3881, 3882, 3883, 3884, 3885, 3886, 3887, 3888, 3889, 3890, 3891, 3892, 3893, 3894, 3895, 3896, 3897, 3898, 3899, 3900, 3901, 3902, 3903, 3904, 3905, 3906, 3907, 3908, 3909, 3910, 3911, 3912, 3913, 3914, 3915, 3916, 3917, 3918, 3919, 3920, 3921, 3922, 3923, 3924, 3925, 3926, 3927, 3928, 3929, 3930, 3931, 3932, 3933, 3934, 3935, 3936, 3937, 3938, 3939, 3940, 3941, 3942, 3943, 3944, 3945, 3946, 3947, 3948, 3949, 3950, 3951, 3952, 3953, 3954, 3955, 3956, 3957, 3958, 3959, 3960, 3961, 3962, 3963, 3964, 3965, 3966, 3967, 3968, 3969, 3970, 3971, 3972, 3973, 3974, 3975, 3976, 3977, 3978, 3979, 3980, 3981, 3982, 3983, 3984, 3985, 3986, 3987, 3988, 3989, 3990, 3991, 3992, 3993, 3994, 3995, 3996, 3997, 3998, 3999, 4000, 4001, 4002, 4003, 4004, 4005, 4006, 4007, 4008, 4009, 4010, 4011, 4012, 4013, 4014, 4015, 4016, 4017, 4018, 4019, 4020, 4021, 4022, 4023, 4024, 4025, 4026, 4027, 4028, 4029, 4030, 4031]</t>
         </is>
       </c>
-      <c r="BP4" t="n">
+      <c r="BV4" t="n">
         <v>0.0985616599858524</v>
       </c>
-      <c r="BQ4" t="inlineStr">
+      <c r="BW4" t="inlineStr">
         <is>
           <t>{'Numk': 20, 'KPar': 17, 'Bucket_index': 1000}</t>
         </is>
       </c>
-      <c r="BR4" t="n">
+      <c r="BX4" t="n">
         <v>30.30766875389963</v>
       </c>
-      <c r="BS4" t="inlineStr">
+      <c r="BY4" t="inlineStr">
         <is>
           <t>no</t>
         </is>
       </c>
-      <c r="BT4" t="n">
-        <v>0</v>
-      </c>
-      <c r="BU4" t="inlineStr">
+      <c r="BZ4" t="n">
+        <v>0</v>
+      </c>
+      <c r="CA4" t="inlineStr">
         <is>
           <t>params</t>
         </is>
       </c>
-      <c r="BV4" t="n">
+      <c r="CB4" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1686,93 +1770,111 @@
       <c r="AY5" t="n">
         <v>3</v>
       </c>
-      <c r="AZ5" t="inlineStr"/>
-      <c r="BA5" t="inlineStr">
+      <c r="AZ5" t="n">
+        <v>3</v>
+      </c>
+      <c r="BA5" t="n">
+        <v>3</v>
+      </c>
+      <c r="BB5" t="n">
+        <v>3</v>
+      </c>
+      <c r="BC5" t="n">
+        <v>3</v>
+      </c>
+      <c r="BD5" t="n">
+        <v>3</v>
+      </c>
+      <c r="BE5" t="n">
+        <v>3</v>
+      </c>
+      <c r="BF5" t="inlineStr"/>
+      <c r="BG5" t="inlineStr">
         <is>
           <t>nab-data/realKnownCause/machine_temperature_system_failure.csv</t>
         </is>
       </c>
-      <c r="BB5" t="n">
+      <c r="BH5" t="n">
         <v>22695</v>
       </c>
-      <c r="BC5" t="inlineStr">
+      <c r="BI5" t="inlineStr">
         <is>
           <t>NAB</t>
         </is>
       </c>
-      <c r="BD5" t="n">
-        <v>4</v>
-      </c>
-      <c r="BE5" t="inlineStr">
+      <c r="BJ5" t="n">
+        <v>4</v>
+      </c>
+      <c r="BK5" t="inlineStr">
         <is>
           <t>2126; 3703; 16057; 19232</t>
         </is>
       </c>
-      <c r="BF5" t="n">
+      <c r="BL5" t="n">
         <v>566</v>
       </c>
-      <c r="BG5" t="inlineStr">
+      <c r="BM5" t="inlineStr">
         <is>
           <t>[840, 842, 843, 845, 846, 847, 848, 849, 850, 851, 852, 853, 854, 2126, 2127, 2128, 2129, 2130, 2131, 2132, 2133, 2134, 2135, 2136, 2137, 2138, 2139, 2140, 2141, 2142, 2143, 2144, 2145, 2146, 2147, 2148, 2149, 2150, 2151, 2152, 2153, 2154, 2155, 2156, 2157, 2158, 2159, 2160, 2161, 2162, 2163, 2164, 2165, 2166, 2167, 2168, 2169, 2170, 2171, 2172, 2173, 2174, 2175, 2176, 2177, 2178, 2179, 2180, 2181, 2182, 2183, 2184, 2185, 2186, 2187, 2188, 2189, 2190, 2191, 2192, 2193, 2194, 2195, 2196, 2197, 2198, 2199, 2200, 2201, 2202, 2203, 2204, 2205, 2206, 2207, 2208, 2209, 2210, 2211, 2212, 2213, 2214, 2215, 2216, 2217, 2218, 2219, 2220, 2221, 2222, 2223, 2224, 2225, 2226, 2227, 2228, 2229, 2230, 2231, 2232, 2233, 2234, 2235, 2236, 2237, 2238, 2239, 2240, 2241, 2242, 2243, 2244, 2245, 2246, 2247, 2248, 2249, 2250, 2251, 2252, 2253, 2254, 2255, 2256, 2257, 2258, 2259, 2260, 2261, 2262, 2263, 2264, 2265, 2266, 2267, 2269, 2270, 2271, 2272, 2273, 2274, 2276, 2278, 2279, 2280, 2281, 2282, 2283, 2285, 2286, 2287, 2289, 2290, 2291, 2292, 2294, 2298, 2301, 3837, 3839, 3840, 3842, 3844, 3846, 3847, 3848, 3849, 3850, 3851, 3852, 3853, 3854, 3855, 3856, 3857, 3858, 3859, 3860, 3861, 3862, 3863, 3864, 3865, 3866, 3867, 3868, 3869, 3870, 3871, 3872, 3873, 3874, 3875, 3876, 3877, 3878, 3879, 3880, 3881, 3882, 3883, 3884, 3885, 3886, 9721, 9723, 9726, 9727, 9728, 9729, 9730, 9731, 9732, 9733, 9734, 9735, 9736, 9737, 9738, 9739, 9740, 9741, 9742, 9743, 9744, 9745, 9746, 9747, 9748, 15158, 15161, 15162, 15163, 15164, 15165, 15166, 15167, 15168, 15169, 15170, 15171, 15172, 15173, 16332, 16333, 16334, 16335, 16336, 16337, 16338, 16339, 16340, 16341, 16342, 16343, 16344, 16345, 16346, 16347, 16348, 16349, 16350, 16351, 16352, 16353, 16354, 16355, 16356, 16357, 16358, 16359, 16360, 16361, 16362, 16363, 16364, 16365, 16366, 16367, 16368, 16369, 16370, 16371, 16372, 16373, 16374, 16375, 16376, 16377, 16378, 16379, 16380, 16381, 16382, 16384, 16385, 17959, 17963, 17965, 17968, 17969, 17970, 17971, 17972, 17973, 17974, 17975, 17976, 17977, 17978, 17979, 17980, 19245, 19249, 19251, 19254, 19255, 19256, 19257, 19259, 19262, 19263, 19264, 19265, 19266, 19267, 19268, 19269, 19270, 19271, 19272, 19273, 19274, 19275, 19276, 19277, 19278, 19279, 19280, 19281, 19282, 19283, 19284, 19285, 19286, 19287, 19288, 19289, 19290, 19291, 19292, 19293, 19294, 19295, 19296, 19297, 19298, 19299, 19300, 19301, 19302, 19303, 19304, 19305, 19306, 19307, 19308, 19309, 19310, 19311, 19312, 19313, 19314, 19315, 19316, 19317, 19318, 19319, 19320, 19321, 19322, 19323, 19324, 19325, 19326, 19327, 19328, 19329, 19330, 19331, 19332, 19333, 19334, 19335, 19336, 19337, 19338, 19339, 19340, 19341, 19342, 19343, 19344, 19345, 19346, 19347, 19348, 19349, 19350, 19351, 19352, 19353, 19354, 19355, 19356, 19357, 19358, 19359, 19360, 19361, 19362, 19363, 19364, 19365, 19366, 19367, 19368, 19369, 19370, 19371, 19372, 19373, 19374, 19375, 19376, 19377, 19378, 19379, 19380, 19381, 19382, 19383, 19384, 19385, 19386, 19387, 19388, 19389, 19390, 19391, 19392, 19393, 19394, 19395, 19396, 19397, 19398, 19399, 19400, 19401, 19402, 19403, 19404, 19405, 19406, 19407, 19408, 19409, 19410, 19411, 19412, 19413, 19414, 19415, 19416, 19417, 19418, 19419, 19420, 19421, 19422, 19423, 19424, 19425, 19426, 19427, 19428, 19429, 19430, 19431, 19432, 19433, 19434, 19435, 19436, 19437, 19438]</t>
         </is>
       </c>
-      <c r="BH5" t="n">
+      <c r="BN5" t="n">
         <v>0.7578947368421053</v>
       </c>
-      <c r="BI5" t="inlineStr">
+      <c r="BO5" t="inlineStr">
         <is>
           <t>{'initial_window': 892, 'window_size': 486, 'num_trees': 17, 'max_depth': 12}</t>
         </is>
       </c>
-      <c r="BJ5" t="n">
+      <c r="BP5" t="n">
         <v>8.018043743912131</v>
       </c>
-      <c r="BK5" t="inlineStr">
+      <c r="BQ5" t="inlineStr">
         <is>
           <t>no</t>
         </is>
       </c>
-      <c r="BL5" t="n">
-        <v>0</v>
-      </c>
-      <c r="BM5" t="inlineStr">
+      <c r="BR5" t="n">
+        <v>0</v>
+      </c>
+      <c r="BS5" t="inlineStr">
         <is>
           <t>params</t>
         </is>
       </c>
-      <c r="BN5" t="n">
-        <v>0</v>
-      </c>
-      <c r="BO5" t="inlineStr">
+      <c r="BT5" t="n">
+        <v>0</v>
+      </c>
+      <c r="BU5" t="inlineStr">
         <is>
           <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86, 87, 88, 89, 90, 91, 92, 93, 94, 95, 96, 97, 98, 99, 100, 101, 102, 103, 104, 105, 106, 107, 108, 109, 110, 111, 112, 113, 114, 115, 116, 117, 118, 119, 120, 121, 122, 123, 124, 125, 126, 127, 128, 129, 130, 131, 132, 133, 134, 135, 136, 137, 138, 139, 140, 141, 142, 143, 144, 145, 146, 147, 148, 149, 150, 151, 152, 153, 154, 155, 156, 157, 158, 159, 160, 161, 162, 163, 164, 165, 166, 167, 168, 169, 170, 171, 172, 173, 174, 175, 176, 177, 178, 179, 180, 181, 182, 183, 184, 185, 186, 187, 188, 189, 190, 191, 192, 193, 194, 195, 196, 197, 198, 199, 200, 201, 202, 203, 204, 205, 206, 207, 208, 209, 210, 211, 212, 213, 214, 215, 216, 217, 218, 219, 220, 221, 222, 223, 224, 225, 226, 227, 228, 229, 230, 231, 232, 233, 234, 235, 236, 237, 238, 239, 240, 241, 242, 243, 244, 245, 246, 247, 248, 249, 250, 251, 252, 253, 254, 255, 256, 257, 258, 259, 260, 261, 262, 263, 264, 265, 266, 267, 268, 269, 270, 271, 272, 273, 274, 275, 276, 277, 278, 279, 280, 281, 282, 283, 284, 285, 286, 287, 288, 289, 290, 291, 292, 293, 294, 295, 296, 297, 298, 299, 300, 301, 302, 303, 304, 305, 306, 307, 308, 309, 310, 311, 312, 313, 314, 315, 316, 317, 318, 319, 320, 321, 322, 323, 324, 325, 326, 327, 328, 329, 330, 331, 332, 333, 334, 335, 336, 337, 338, 339, 340, 341, 342, 343, 344, 345, 346, 347, 348, 349, 350, 351, 352, 353, 354, 355, 356, 357, 358, 359, 360, 361, 362, 363, 364, 365, 366, 367, 368, 369, 370, 371, 372, 373, 374, 375, 376, 377, 378, 379, 380, 381, 382, 383, 384, 385, 386, 387, 388, 389, 390, 391, 392, 393, 394, 395, 396, 397, 398, 399, 400, 401, 402, 403, 404, 405, 406, 407, 408, 409, 410, 411, 412, 413, 414, 415, 416, 417, 418, 419, 420, 421, 422, 423, 424, 425, 426, 427, 428, 429, 430, 431, 432, 433, 434, 435, 436, 437, 438, 439, 440, 441, 442, 443, 444, 445, 446, 447, 448, 449, 450, 451, 452, 453, 454, 455, 456, 457, 458, 459, 460, 461, 462, 463, 464, 465, 466, 467, 468, 469, 470, 471, 472, 473, 474, 475, 476, 477, 478, 479, 480, 481, 482, 483, 484, 485, 486, 487, 488, 489, 490, 491, 492, 493, 494, 495, 496, 497, 498, 499, 500, 501, 502, 503, 504, 505, 506, 507, 508, 509, 510, 511, 512, 513, 514, 515, 516, 517, 518, 519, 520, 521, 522, 523, 524, 525, 526, 527, 528, 529, 530, 531, 532, 533, 534, 535, 536, 537, 538, 539, 540, 541, 542, 543, 544, 545, 546, 547, 548, 549, 550, 551, 552, 553, 554, 555, 556, 557, 558, 559, 560, 561, 562, 563, 564, 565, 566, 567, 568, 569, 570, 571, 572, 573, 574, 575, 576, 577, 578, 579, 580, 581, 582, 583, 584, 585, 586, 587, 588, 589, 590, 591, 592, 593, 594, 595, 596, 597, 598, 599, 600, 601, 602, 603, 604, 605, 606, 607, 608, 609, 610, 611, 612, 613, 614, 615, 616, 617, 618, 619, 620, 621, 622, 623, 624, 625, 626, 627, 628, 629, 630, 631, 632, 633, 634, 635, 636, 637, 638, 639, 640, 641, 642, 643, 644, 645, 646, 647, 648, 649, 650, 651, 652, 653, 654, 655, 656, 657, 658, 659, 660, 661, 662, 663, 664, 665, 666, 667, 668, 669, 670, 671, 672, 673, 674, 675, 676, 677, 678, 679, 680, 681, 682, 683, 684, 685, 686, 687, 688, 689, 690, 691, 692, 693, 694, 695, 696, 697, 698, 699, 700, 701, 702, 703, 704, 705, 706, 707, 708, 709, 710, 711, 712, 713, 714, 715, 716, 717, 718, 719, 720, 721, 722, 723, 724, 725, 727, 728, 729, 730, 731, 732, 733, 734, 735, 736, 737, 738, 739, 740, 741, 742, 743, 744, 745, 746, 747, 748, 749, 750, 751, 752, 753, 754, 755, 756, 757, 758, 759, 760, 761, 762, 763, 764, 765, 766, 767, 768, 769, 770, 771, 772, 773, 774, 775, 776, 777, 778, 779, 780, 781, 782, 783, 784, 785, 786, 787, 788, 789, 790, 791, 792, 793, 794, 795, 796, 797, 798, 799, 800, 801, 802, 803, 804, 805, 806, 807, 808, 809, 810, 811, 812, 813, 814, 815, 816, 817, 818, 819, 820, 821, 822, 823, 824, 825, 826, 827, 828, 829, 830, 831, 832, 833, 834, 835, 836, 837, 838, 839, 840, 841, 842, 843, 844, 845, 846, 847, 848, 849, 850, 851, 852, 853, 854, 855, 856, 857, 858, 859, 860, 861, 862, 863, 864, 865, 866, 867, 868, 869, 870, 871, 872, 873, 874, 875, 876, 877, 878, 879, 880, 881, 882, 883, 884, 885, 886, 887, 888, 889, 890, 891, 892, 893, 894, 895, 896, 897, 898, 899, 900, 901, 902, 903, 904, 905, 906, 907, 908, 909, 910, 911, 912, 913, 914, 915, 916, 917, 918, 919, 920, 921, 922, 923, 924, 925, 926, 927, 928, 929, 930, 931, 932, 933, 934, 935, 936, 937, 938, 939, 940, 941, 942, 943, 944, 945, 946, 947, 948, 949, 950, 951, 952, 953, 954, 955, 956, 957, 958, 959, 960, 961, 962, 963, 964, 965, 966, 967, 968, 969, 970, 971, 972, 973, 974, 975, 976, 977, 978, 979, 980, 981, 982, 983, 984, 985, 986, 987, 988, 989, 990, 991, 992, 993, 994, 995, 996, 997, 998, 999, 1000, 1001, 1002, 1003, 1004, 1005, 1006, 1007, 1008, 1009, 1010, 1011, 1012, 1013, 1014, 1015, 1016, 1017, 1018, 1019, 1020, 1021, 1022, 1023, 1024, 1025, 1026, 1027, 1028, 1029, 1030, 1031, 1032, 1033, 1034, 1035, 1036, 1037, 1038, 1039, 1040, 1041, 1042, 1043, 1044, 1045, 1046, 1047, 1048, 1049, 1050, 1051, 1052, 1053, 1054, 1055, 1056, 1057, 1058, 1059, 1060, 1061, 1062, 1063, 1064, 1065, 1066, 1067, 1068, 1069, 1070, 1071, 1072, 1073, 1074, 1075, 1076, 1077, 1078, 1079, 1080, 1081, 1082, 1083, 1084, 1085, 1086, 1087, 1088, 1089, 1090, 1091, 1092, 1093, 1094, 1095, 1096, 1097, 1098, 1099, 1100, 1101, 1102, 1103, 1104, 1105, 1106, 1107, 1108, 1109, 1110, 1111, 1112, 1113, 1114, 1115, 1116, 1117, 1118, 1119, 1120, 1121, 1122, 1123, 1124, 1125, 1126, 1127, 1128, 1129, 1130, 1131, 1132, 1133, 1134, 1135, 1136, 1137, 1138, 1139, 1140, 1141, 1142, 1143, 1144, 1145, 1146, 1147, 1148, 1149, 1150, 1151, 1152, 1153, 1154, 1155, 1156, 1157, 1158, 1159, 1160, 1161, 1162, 1163, 1164, 1165, 1166, 1167, 1168, 1169, 1170, 1171, 1172, 1173, 1174, 1175, 1176, 1177, 1178, 1179, 1180, 1181, 1182, 1183, 1184, 1185, 1186, 1187, 1188, 1189, 1190, 1191, 1192, 1193, 1194, 1195, 1196, 1197, 1198, 1199, 1200, 1201, 1202, 1203, 1204, 1205, 1206, 1207, 1208, 1209, 1210, 1211, 1212, 1213, 1214, 1215, 1216, 1217, 1218, 1219, 1220, 1221, 1222, 1223, 1224, 1225, 1226, 1227, 1228, 1229, 1230, 1231, 1232, 1233, 1234, 1235, 1236, 1237, 1238, 1239, 1240, 1241, 1242, 1243, 1244, 1245, 1246, 1247, 1248, 1249, 1250, 1251, 1252, 1253, 1254, 1255, 1256, 1257, 1258, 1259, 1260, 1261, 1262, 1263, 1264, 1265, 1266, 1267, 1268, 1269, 1270, 1271, 1272, 1273, 1274, 1275, 1276, 1277, 1278, 1279, 1280, 1281, 1282, 1283, 1284, 1285, 1286, 1287, 1288, 1289, 1290, 1291, 1292, 1293, 1294, 1295, 1296, 1297, 1298, 1299, 1300, 1301, 1302, 1303, 1304, 1305, 1306, 1307, 1308, 1309, 1310, 1311, 1312, 1313, 1314, 1315, 1316, 1317, 1318, 1319, 1320, 1321, 1322, 1323, 1324, 1325, 1326, 1327, 1328, 1329, 1330, 1331, 1332, 1333, 1334, 1335, 1336, 1337, 1338, 1339, 1340, 1341, 1342, 1343, 1344, 1345, 1346, 1347, 1348, 1349, 1350, 1351, 1352, 1353, 1354, 1355, 1356, 1357, 1358, 1359, 1360, 1361, 1362, 1363, 1364, 1365, 1366, 1367, 1368, 1369, 1370, 1371, 1372, 1373, 1374, 1375, 1376, 1377, 1378, 1379, 1380, 1381, 1382, 1383, 1384, 1385, 1386, 1387, 1388, 1389, 1390, 1391, 1392, 1393, 1394, 1395, 1396, 1397, 1398, 1399, 1400, 1401, 1402, 1403, 1404, 1405, 1406, 1407, 1408, 1409, 1410, 1411, 1412, 1413, 1414, 1415, 1416, 1417, 1418, 1419, 1420, 1421, 1422, 1423, 1424, 1425, 1426, 1427, 1428, 1429, 1430, 1431, 1432, 1433, 1434, 1435, 1436, 1437, 1438, 1439, 1440, 1441, 1442, 1443, 1444, 1445, 1446, 1447, 1448, 1449, 1450, 1451, 1452, 1453, 1454, 1455, 1456, 1457, 1458, 1459, 1460, 1461, 1462, 1463, 1464, 1465, 1466, 1467, 1468, 1469, 1470, 1471, 1472, 1473, 1474, 1475, 1476, 1477, 1478, 1479, 1480, 1481, 1482, 1483, 1484, 1485, 1486, 1487, 1488, 1489, 1490, 1491, 1492, 1493, 1494, 1495, 1496, 1497, 1498, 1499, 1500, 1501, 1502, 1503, 1504, 1505, 1506, 1507, 1508, 1509, 1510, 1511, 1512, 1513, 1514, 1515, 1516, 1517, 1518, 1519, 1520, 1521, 1522, 1523, 1524, 1525, 1526, 1527, 1528, 1529, 1530, 1531, 1532, 1533, 1534, 1535, 1536, 1537, 1538, 1539, 1540, 1541, 1542, 1543, 1544, 1545, 1546, 1547, 1548, 1549, 1550, 1551, 1552, 1553, 1554, 1555, 1556, 1557, 1558, 1559, 1560, 1561, 1562, 1563, 1564, 1565, 1566, 1567, 1568, 1569, 1570, 1571, 1572, 1573, 1574, 1575, 1576, 1577, 1578, 1579, 1580, 1581, 1582, 1583, 1584, 1585, 1586, 1587, 1588, 1589, 1590, 1591, 1592, 1593, 1594, 1595, 1596, 1597, 1598, 1599, 1600, 1601, 1602, 1603, 1604, 1605, 1606, 1607, 1608, 1609, 1610, 1612, 1613, 1614, 1615, 1616, 1617, 1618, 1619, 1620, 1621, 1622, 1623, 1624, 1625, 1626, 1627, 1628, 1629, 1630, 1631, 1632, 1633, 1634, 1635, 1636, 1637, 1638, 1639, 1640, 1641, 1642, 1643, 1644, 1645, 1646, 1647, 1648, 1649, 1650, 1651, 1652, 1653, 1654, 1655, 1656, 1657, 1658, 1659, 1660, 1661, 1662, 1663, 1664, 1665, 1666, 1667, 1668, 1669, 1670, 1671, 1672, 1674, 1675, 1676, 1677, 1678, 1679, 1680, 1681, 1682, 1683, 1684, 1685, 1686, 1687, 1688, 1689, 1690, 1691, 1692, 1693, 1694, 1695, 1696, 1697, 1698, 1699, 1700, 1701, 1702, 1703, 1704, 1705, 1706, 1707, 1708, 1709, 1710, 1711, 1712, 1713, 1714, 1715, 1716, 1717, 1718, 1719, 1720, 1721, 1722, 1723, 1724, 1725, 1726, 1727, 1728, 1729, 1730, 1731, 1732, 1733, 1734, 1735, 1736, 1737, 1738, 1739, 1740, 1741, 1742, 1743, 1744, 1745, 1746, 1747, 1748, 1749, 1750, 1751, 1752, 1753, 1754, 1755, 1756, 1757, 1758, 1759, 1760, 1761, 1762, 1763, 1764, 1765, 1766, 1767, 1768, 1769, 1770, 1771, 1772, 1773, 1774, 1775, 1776, 1777, 1778, 1779, 1780, 1781, 1782, 1783, 1784, 1785, 1786, 1787, 1788, 1789, 1790, 1791, 1792, 1793, 1794, 1795, 1796, 1797, 1798, 1799, 1800, 1801, 1802, 1803, 1804, 1805, 1806, 1807, 1808, 1809, 1810, 1811, 1812, 1813, 1814, 1815, 1816, 1817, 1818, 1819, 1820, 1821, 1822, 1823, 1824, 1825, 1826, 1827, 1828, 1829, 1830, 1831, 1832, 1833, 1834, 1835, 1836, 1837, 1838, 1839, 1840, 1841, 1842, 1843, 1844, 1845, 1846, 1847, 1848, 1849, 1850, 1851, 1852, 1853, 1854, 1855, 1856, 1857, 1858, 1859, 1860, 1861, 1862, 1863, 1864, 1865, 1866, 1867, 1868, 1869, 1870, 1871, 1872, 1874, 1875, 1876, 1877, 1878, 1879, 1880, 1881, 1882, 1883, 1884, 1885, 1886, 1887, 1888, 1889, 1890, 1891, 1892, 1893, 1894, 1895, 1896, 1897, 1898, 1899, 1900, 1901, 1902, 1903, 1904, 1905, 1906, 1907, 1908, 1909, 1910, 1911, 1912, 1913, 1914, 1915, 1916, 1917, 1918, 1919, 1920, 1921, 1922, 1923, 1924, 1925, 1926, 1927, 1928, 1929, 1930, 1931, 1932, 1933, 1934, 1935, 1936, 1937, 1938, 1939, 1940, 1941, 1942, 1943, 1944, 1945, 1946, 1947, 1948, 1949, 1950, 1951, 1952, 1953, 1954, 1955, 1956, 1957, 1958, 1959, 1960, 1961, 1962, 1963, 1964, 1965, 1966, 1967, 1968, 1969, 1970, 1971, 1972, 1973, 1974, 1975, 1976, 1977, 1978, 1979, 1980, 1981, 1982, 1983, 1984, 1985, 1986, 1987, 1988, 1989, 1990, 1991, 1992, 1993, 1994, 1995, 1996, 1997, 1998, 1999, 2000, 2001, 2002, 2003, 2004, 2005, 2006, 2007, 2008, 2009, 2010, 2011, 2012, 2013, 2014, 2015, 2016, 2017, 2018, 2019, 2020, 2021, 2022, 2023, 2024, 2025, 2026, 2027, 2028, 2029, 2030, 2031, 2032, 2033, 2034, 2035, 2036, 2037, 2038, 2039, 2040, 2041, 2042, 2043, 2044, 2045, 2046, 2047, 2048, 2049, 2050, 2051, 2052, 2053, 2054, 2055, 2056, 2057, 2058, 2059, 2060, 2061, 2062, 2063, 2064, 2065, 2066, 2067, 2068, 2069, 2070, 2071, 2072, 2073, 2074, 2075, 2076, 2077, 2078, 2079, 2080, 2081, 2082, 2083, 2084, 2085, 2086, 2087, 2088, 2089, 2090, 2091, 2092, 2093, 2094, 2095, 2096, 2097, 2098, 2099, 2100, 2101, 2102, 2103, 2104, 2105, 2106, 2107, 2108, 2109, 2110, 2111, 2112, 2113, 2114, 2115, 2116, 2117, 2118, 2119, 2120, 2121, 2122, 2123, 2124, 2125, 2126, 2127, 2128, 2129, 2130, 2131, 2132, 2133, 2134, 2135, 2136, 2137, 2138, 2139, 2140, 2141, 2142, 2143, 2144, 2145, 2146, 2147, 2148, 2149, 2150, 2151, 2152, 2153, 2154, 2155, 2156, 2157, 2158, 2159, 2160, 2161, 2162, 2163, 2164, 2165, 2166, 2167, 2168, 2169, 2170, 2171, 2172, 2173, 2174, 2175, 2176, 2177, 2178, 2179, 2180, 2181, 2182, 2183, 2184, 2185, 2186, 2187, 2188, 2189, 2190, 2191, 2192, 2193, 2194, 2195, 2196, 2197, 2198, 2199, 2200, 2201, 2202, 2203, 2204, 2205, 2206, 2207, 2208, 2209, 2210, 2211, 2212, 2213, 2214, 2215, 2216, 2217, 2218, 2219, 2220, 2221, 2222, 2223, 2224, 2225, 2226, 2227, 2228, 2229, 2230, 2231, 2232, 2233, 2234, 2235, 2236, 2237, 2238, 2239, 2240, 2241, 2242, 2243, 2244, 2245, 2246, 2247, 2248, 2249, 2250, 2251, 2252, 2253, 2254, 2255, 2256, 2257, 2258, 2259, 2260, 2261, 2262, 2263, 2264, 2265, 2266, 2267, 2268, 2269, 2270, 2271, 2272, 2273, 2274, 2275, 2276, 2277, 2278, 2279, 2280, 2281, 2282, 2283, 2284, 2285, 2286, 2287, 2288, 2289, 2290, 2291, 2292, 2293, 2294, 2295, 2296, 2297, 2298, 2299, 2300, 2301, 2302, 2303, 2304, 2305, 2306, 2307, 2308, 2309, 2310, 2311, 2312, 2313, 2314, 2315, 2316, 2317, 2318, 2319, 2320, 2321, 2322, 2323, 2324, 2325, 2326, 2327, 2328, 2329, 2330, 2331, 2332, 2333, 2334, 2335, 2336, 2337, 2338, 2339, 2340, 2341, 2342, 2343, 2344, 2345, 2346, 2347, 2348, 2349, 2350, 2351, 2352, 2353, 2354, 2355, 2356, 2357, 2358, 2359, 2360, 2361, 2362, 2363, 2364, 2365, 2366, 2367, 2368, 2369, 2370, 2371, 2372, 2373, 2374, 2375, 2376, 2377, 2378, 2379, 2380, 2381, 2382, 2383, 2384, 2385, 2386, 2387, 2388, 2389, 2390, 2391, 2392, 2393, 2394, 2395, 2396, 2397, 2398, 2399, 2400, 2401, 2402, 2403, 2404, 2405, 2406, 2407, 2408, 2409, 2410, 2411, 2412, 2413, 2414, 2415, 2416, 2417, 2418, 2419, 2420, 2421, 2422, 2423, 2424, 2425, 2426, 2427, 2428, 2429, 2430, 2431, 2432, 2433, 2434, 2435, 2436, 2437, 2438, 2439, 2440, 2441, 2442, 2443, 2444, 2445, 2446, 2447, 2448, 2449, 2450, 2451, 2452, 2453, 2454, 2455, 2456, 2457, 2458, 2459, 2460, 2461, 2462, 2463, 2464, 2465, 2466, 2467, 2468, 2469, 2470, 2471, 2472, 2473, 2474, 2475, 2476, 2477, 2478, 2479, 2480, 2481, 2482, 2483, 2484, 2485, 2486, 2487, 2488, 2489, 2490, 2491, 2492, 2493, 2494, 2495, 2496, 2497, 2498, 2499, 2500, 2501, 2502, 2503, 2504, 2505, 2506, 2507, 2508, 2509, 2510, 2511, 2512, 2513, 2514, 2515, 2516, 2517, 2518, 2519, 2520, 2521, 2522, 2523, 2524, 2525, 2526, 2527, 2528, 2529, 2530, 2531, 2532, 2533, 2534, 2535, 2536, 2537, 2538, 2539, 2540, 2541, 2542, 2543, 2544, 2545, 2546, 2547, 2548, 2549, 2550, 2551, 2552, 2553, 2554, 2555, 2556, 2557, 2558, 2559, 2560, 2561, 2562, 2563, 2564, 2565, 2566, 2567, 2568, 2569, 2570, 2571, 2572, 2573, 2574, 2575, 2576, 2577, 2578, 2579, 2580, 2581, 2582, 2583, 2584, 2585, 2586, 2587, 2588, 2589, 2590, 2591, 2592, 2593, 2594, 2595, 2596, 2597, 2598, 2599, 2600, 2601, 2602, 2603, 2604, 2605, 2606, 2607, 2608, 2609, 2610, 2611, 2612, 2613, 2614, 2615, 2616, 2617, 2618, 2619, 2620, 2621, 2622, 2623, 2624, 2625, 2626, 2627, 2628, 2629, 2630, 2631, 2632, 2633, 2634, 2635, 2636, 2637, 2638, 2639, 2640, 2641, 2642, 2643, 2644, 2645, 2646, 2647, 2648, 2649, 2650, 2651, 2652, 2653, 2654, 2655, 2656, 2657, 2658, 2659, 2660, 2661, 2662, 2663, 2664, 2665, 2666, 2667, 2668, 2669, 2670, 2671, 2672, 2673, 2674, 2675, 2676, 2677, 2678, 2679, 2680, 2681, 2682, 2683, 2684, 2685, 2686, 2687, 2688, 2689, 2690, 2691, 2692, 2693, 2694, 2695, 2696, 2697, 2698, 2699, 2700, 2701, 2702, 2703, 2704, 2705, 2706, 2707, 2708, 2709, 2710, 2711, 2712, 2713, 2714, 2715, 2716, 2717, 2718, 2719, 2720, 2721, 2722, 2723, 2724, 2725, 2726, 2727, 2728, 2729, 2730, 2731, 2732, 2733, 2734, 2735, 2736, 2737, 2738, 2739, 2740, 2741, 2742, 2743, 2744, 2745, 2746, 2747, 2748, 2749, 2750, 2751, 2752, 2753, 2754, 2755, 2756, 2757, 2758, 2759, 2760, 2761, 2762, 2763, 2764, 2765, 2766, 2767, 2768, 2769, 2770, 2771, 2772, 2773, 2774, 2775, 2776, 2777, 2778, 2779, 2780, 2781, 2782, 2783, 2784, 2785, 2786, 2787, 2788, 2789, 2790, 2791, 2792, 2793, 2794, 2795, 2796, 2797, 2798, 2799, 2800, 2801, 2802, 2803, 2804, 2805, 2806, 2807, 2808, 2809, 2810, 2811, 2812, 2813, 2814, 2815, 2816, 2817, 2818, 2819, 2820, 2821, 2822, 2823, 2824, 2825, 2826, 2827, 2828, 2829, 2830, 2831, 2832, 2833, 2834, 2835, 2836, 2837, 2838, 2839, 2840, 2841, 2842, 2843, 2844, 2845, 2846, 2847, 2848, 2849, 2850, 2851, 2852, 2853, 2854, 2855, 2856, 2857, 2858, 2859, 2860, 2861, 2862, 2863, 2864, 2865, 2866, 2867, 2868, 2869, 2870, 2871, 2872, 2873, 2874, 2875, 2876, 2877, 2878, 2879, 2880, 2881, 2882, 2883, 2884, 2885, 2886, 2887, 2888, 2889, 2890, 2891, 2892, 2893, 2894, 2895, 2896, 2897, 2898, 2899, 2900, 2901, 2902, 2903, 2904, 2905, 2906, 2907, 2908, 2909, 2910, 2911, 2912, 2913, 2914, 2915, 2916, 2917, 2918, 2919, 2920, 2921, 2922, 2923, 2924, 2925, 2926, 2927, 2928, 2929, 2930, 2931, 2932, 2933, 2934, 2935, 2936, 2937, 2938, 2939, 2940, 2941, 2942, 2943, 2944, 2945, 2946, 2947, 2948, 2949, 2950, 2951, 2952, 2953, 2954, 2955, 2956, 2957, 2958, 2959, 2960, 2961, 2962, 2963, 2964, 2965, 2967, 2968, 2969, 2970, 2971, 2972, 2973, 2974, 2975, 2976, 2977, 2978, 2979, 2980, 2981, 2982, 2983, 2984, 2985, 2986, 2987, 2988, 2989, 2990, 2991, 2992, 2993, 2994, 2995, 2996, 2997, 2998, 2999, 3000, 3001, 3002, 3003, 3004, 3005, 3006, 3007, 3008, 3009, 3010, 3011, 3012, 3013, 3014, 3015, 3016, 3017, 3018, 3019, 3020, 3021, 3022, 3023, 3024, 3025, 3026, 3027, 3028, 3029, 3030, 3031, 3032, 3033, 3034, 3035, 3036, 3037, 3038, 3039, 3040, 3041, 3042, 3043, 3044, 3045, 3046, 3047, 3048, 3049, 3050, 3051, 3052, 3053, 3054, 3055, 3056, 3057, 3058, 3059, 3060, 3061, 3062, 3063, 3064, 3065, 3066, 3067, 3068, 3069, 3070, 3071, 3072, 3073, 3074, 3075, 3076, 3077, 3078, 3079, 3080, 3081, 3082, 3083, 3084, 3085, 3086, 3087, 3088, 3089, 3090, 3091, 3092, 3093, 3094, 3095, 3096, 3097, 3098, 3099, 3100, 3101, 3102, 3103, 3104, 3105, 3106, 3107, 3108, 3109, 3110, 3111, 3112, 3113, 3114, 3115, 3116, 3117, 3118, 3119, 3120, 3121, 3122, 3123, 3124, 3125, 3126, 3127, 3128, 3129, 3130, 3131, 3132, 3133, 3134, 3135, 3136, 3137, 3138, 3139, 3140, 3141, 3142, 3143, 3144, 3145, 3146, 3147, 3148, 3149, 3150, 3151, 3152, 3153, 3154, 3155, 3156, 3157, 3158, 3159, 3160, 3161, 3162, 3163, 3164, 3165, 3166, 3167, 3168, 3169, 3170, 3171, 3172, 3173, 3174, 3175, 3176, 3177, 3178, 3179, 3180, 3181, 3182, 3183, 3184, 3185, 3186, 3187, 3188, 3189, 3190, 3191, 3192, 3193, 3194, 3195, 3196, 3197, 3198, 3199, 3200, 3201, 3202, 3203, 3204, 3205, 3206, 3207, 3208, 3209, 3210, 3211, 3212, 3213, 3214, 3215, 3216, 3217, 3218, 3219, 3220, 3221, 3222, 3223, 3224, 3225, 3226, 3227, 3228, 3229, 3230, 3231, 3232, 3233, 3234, 3235, 3236, 3237, 3238, 3239, 3240, 3241, 3242, 3243, 3244, 3245, 3246, 3247, 3248, 3249, 3250, 3251, 3252, 3253, 3254, 3255, 3256, 3257, 3258, 3259, 3260, 3261, 3262, 3263, 3264, 3265, 3266, 3267, 3268, 3269, 3270, 3271, 3272, 3273, 3274, 3275, 3276, 3277, 3278, 3279, 3280, 3281, 3282, 3283, 3284, 3285, 3286, 3287, 3288, 3289, 3290, 3291, 3292, 3293, 3294, 3295, 3296, 3297, 3298, 3299, 3300, 3301, 3302, 3303, 3304, 3305, 3306, 3307, 3308, 3309, 3310, 3311, 3312, 3313, 3314, 3315, 3316, 3317, 3318, 3319, 3320, 3321, 3322, 3323, 3324, 3325, 3326, 3327, 3328, 3329, 3330, 3331, 3332, 3333, 3334, 3335, 3336, 3337, 3338, 3339, 3340, 3341, 3342, 3343, 3344, 3345, 3346, 3347, 3348, 3349, 3350, 3351, 3352, 3353, 3354, 3355, 3356, 3357, 3358, 3359, 3360, 3361, 3362, 3363, 3364, 3365, 3366, 3367, 3368, 3369, 3370, 3371, 3372, 3373, 3374, 3375, 3376, 3377, 3378, 3379, 3380, 3381, 3382, 3383, 3384, 3385, 3386, 3387, 3388, 3389, 3390, 3391, 3392, 3393, 3394, 3395, 3396, 3397, 3398, 3399, 3400, 3401, 3402, 3403, 3404, 3405, 3406, 3407, 3408, 3409, 3410, 3411, 3412, 3413, 3414, 3415, 3416, 3417, 3418, 3419, 3420, 3421, 3422, 3423, 3424, 3425, 3426, 3427, 3428, 3429, 3430, 3431, 3432, 3433, 3434, 3435, 3436, 3437, 3438, 3439, 3440, 3441, 3442, 3443, 3444, 3445, 3446, 3447, 3448, 3449, 3450, 3451, 3452, 3453, 3454, 3455, 3456, 3457, 3458, 3459, 3460, 3461, 3462, 3463, 3464, 3465, 3466, 3467, 3468, 3469, 3470, 3471, 3472, 3473, 3474, 3475, 3476, 3477, 3478, 3479, 3480, 3481, 3482, 3483, 3484, 3485, 3486, 3487, 3488, 3489, 3490, 3491, 3492, 3493, 3494, 3495, 3496, 3497, 3498, 3499, 3500, 3501, 3502, 3503, 3504, 3505, 3506, 3507, 3508, 3509, 3510, 3511, 3512, 3513, 3514, 3515, 3516, 3517, 3518, 3519, 3520, 3521, 3522, 3523, 3524, 3525, 3526, 3527, 3528, 3529, 3530, 3531, 3532, 3533, 3534, 3535, 3536, 3537, 3538, 3539, 3540, 3541, 3542, 3543, 3544, 3545, 3546, 3547, 3548, 3549, 3550, 3551, 3552, 3553, 3554, 3555, 3556, 3557, 3558, 3559, 3560, 3561, 3562, 3563, 3564, 3565, 3566, 3567, 3568, 3569, 3570, 3571, 3572, 3573, 3574, 3575, 3576, 3577, 3578, 3579, 3580, 3581, 3582, 3583, 3584, 3585, 3586, 3587, 3588, 3589, 3590, 3591, 3592, 3593, 3594, 3595, 3596, 3597, 3598, 3599, 3600, 3601, 3602, 3603, 3604, 3605, 3606, 3607, 3608, 3609, 3610, 3611, 3612, 3613, 3614, 3615, 3616, 3617, 3618, 3619, 3620, 3621, 3622, 3623, 3624, 3625, 3626, 3627, 3628, 3629, 3630, 3631, 3632, 3633, 3634, 3635, 3636, 3637, 3638, 3639, 3640, 3641, 3642, 3643, 3644, 3645, 3646, 3647, 3648, 3649, 3650, 3651, 3652, 3653, 3654, 3655, 3656, 3657, 3658, 3659, 3660, 3661, 3662, 3663, 3664, 3665, 3666, 3667, 3668, 3669, 3670, 3671, 3672, 3673, 3674, 3675, 3676, 3677, 3678, 3679, 3680, 3681, 3682, 3683, 3684, 3685, 3686, 3687, 3688, 3689, 3690, 3691, 3692, 3693, 3694, 3695, 3696, 3697, 3698, 3699, 3700, 3701, 3702, 3703, 3704, 3705, 3706, 3707, 3708, 3709, 3710, 3711, 3712, 3713, 3714, 3715, 3716, 3717, 3718, 3719, 3720, 3721, 3722, 3723, 3724, 3725, 3726, 3727, 3728, 3729, 3730, 3731, 3732, 3733, 3734, 3735, 3736, 3737, 3738, 3739, 3740, 3741, 3742, 3743, 3744, 3745, 3746, 3747, 3748, 3749, 3750, 3751, 3752, 3753, 3754, 3755, 3756, 3757, 3758, 3759, 3760, 3761, 3762, 3763, 3764, 3765, 3766, 3767, 3768, 3769, 3770, 3771, 3772, 3773, 3774, 3775, 3776, 3777, 3778, 3779, 3780, 3781, 3782, 3783, 3784, 3785, 3786, 3787, 3788, 3789, 3790, 3791, 3792, 3793, 3794, 3795, 3796, 3797, 3798, 3799, 3800, 3801, 3802, 3803, 3804, 3805, 3806, 3807, 3808, 3809, 3810, 3811, 3812, 3813, 3814, 3815, 3816, 3817, 3818, 3819, 3820, 3821, 3822, 3823, 3824, 3825, 3826, 3827, 3828, 3829, 3830, 3831, 3832, 3833, 3834, 3835, 3836, 3837, 3838, 3839, 3840, 3841, 3842, 3843, 3844, 3845, 3846, 3847, 3848, 3849, 3850, 3851, 3852, 3853, 3854, 3855, 3856, 3857, 3858, 3859, 3860, 3861, 3862, 3863, 3864, 3865, 3866, 3867, 3868, 3869, 3870, 3871, 3872, 3873, 3874, 3875, 3876, 3877, 3878, 3879, 3880, 3881, 3882, 3883, 3884, 3885, 3886, 3887, 3888, 3889, 3890, 3891, 3892, 3893, 3894, 3895, 3896, 3897, 3898, 3899, 3900, 3901, 3902, 3903, 3904, 3905, 3906, 3907, 3908, 3909, 3910, 3911, 3912, 3913, 3914, 3915, 3916, 3917, 3918, 3919, 3920, 3921, 3922, 3923, 3924, 3925, 3926, 3927, 3928, 3929, 3930, 3931, 3932, 3933, 3934, 3935, 3936, 3937, 3938, 3939, 3940, 3941, 3942, 3943, 3944, 3945, 3946, 3947, 3948, 3949, 3950, 3951, 3952, 3953, 3954, 3955, 3956, 3957, 3958, 3959, 3960, 3961, 3962, 3963, 3964, 3965, 3966, 3967, 3968, 3969, 3970, 3971, 3972, 3973, 3974, 3975, 3976, 3977, 3978, 3979, 3980, 3981, 3982, 3983, 3984, 3985, 3986, 3987, 3988, 3989, 3990, 3991, 3992, 3993, 3994, 3995, 3996, 3997, 3998, 3999, 4000, 4001, 4002, 4003, 4004, 4005, 4006, 4007, 4008, 4009, 4010, 4011, 4012, 4013, 4014, 4015, 4016, 4017, 4018, 4019, 4020, 4021, 4022, 4023, 4024, 4025, 4026, 4027, 4028, 4029, 4030, 4031, 4032, 4033, 4034, 4035, 4036, 4037, 4038, 4039, 4040, 4041, 4042, 4043, 4044, 4045, 4046, 4047, 4048, 4049, 4050, 4051, 4052, 4053, 4054, 4055, 4056, 4057, 4058, 4059, 4060, 4061, 4062, 4063, 4064, 4065, 4066, 4067, 4068, 4069, 4070, 4071, 4072, 4073, 4074, 4075, 4076, 4077, 4078, 4079, 4080, 4081, 4082, 4083, 4084, 4085, 4086, 4087, 4088, 4089, 4090, 4091, 4092, 4093, 4094, 4095, 4096, 4097, 4098, 4099, 4100, 4101, 4102, 4103, 4104, 4105, 4106, 4107, 4108, 4109, 4110, 4111, 4112, 4113, 4114, 4115, 4116, 4117, 4118, 4119, 4120, 4121, 4122, 4123, 4124, 4125, 4126, 4127, 4128, 4129, 4130, 4131, 4132, 4133, 4134, 4135, 4136, 4137, 4138, 4139, 4140, 4141, 4142, 4143, 4144, 4145, 4146, 4147, 4148, 4149, 4150, 4151, 4152, 4153, 4154, 4155, 4156, 4157, 4158, 4159, 4160, 4161, 4162, 4163, 4164, 4165, 4166, 4167, 4168, 4169, 4170, 4171, 4172, 4173, 4174, 4175, 4176, 4177, 4178, 4179, 4180, 4181, 4182, 4183, 4184, 4185, 4186, 4187, 4188, 4189, 4190, 4191, 4192, 4193, 4194, 4195, 4196, 4197, 4198, 4199, 4200, 4201, 4202, 4203, 4204, 4205, 4206, 4207, 4208, 4209, 4210, 4211, 4212, 4213, 4214, 4215, 4216, 4217, 4218, 4219, 4220, 4221, 4222, 4223, 4224, 4225, 4226, 4227, 4228, 4229, 4230, 4231, 4232, 4233, 4234, 4235, 4236, 4237, 4238, 4239, 4240, 4241, 4242, 4243, 4244, 4245, 4246, 4247, 4248, 4249, 4250, 4251, 4252, 4253, 4254, 4255, 4256, 4257, 4258, 4259, 4260, 4261, 4262, 4263, 4264, 4265, 4266, 4267, 4268, 4269, 4270, 4271, 4272, 4273, 4274, 4275, 4276, 4277, 4278, 4279, 4280, 4281, 4282, 4283, 4284, 4285, 4286, 4287, 4288, 4289, 4290, 4291, 4292, 4293, 4294, 4295, 4296, 4297, 4298, 4299, 4300, 4301, 4302, 4303, 4304, 4305, 4306, 4307, 4308, 4309, 4310, 4311, 4312, 4313, 4314, 4315, 4316, 4317, 4318, 4319, 4320, 4321, 4322, 4323, 4324, 4325, 4326, 4327, 4328, 4329, 4330, 4331, 4332, 4333, 4334, 4335, 4336, 4337, 4338, 4339, 4340, 4341, 4342, 4343, 4344, 4345, 4346, 4347, 4348, 4349, 4350, 4351, 4352, 4353, 4354, 4355, 4356, 4357, 4358, 4359, 4360, 4361, 4362, 4363, 4364, 4365, 4366, 4367, 4368, 4369, 4370, 4371, 4372, 4373, 4374, 4375, 4376, 4377, 4378, 4379, 4380, 4381, 4382, 4383, 4384, 4385, 4386, 4387, 4388, 4389, 4390, 4391, 4392, 4393, 4394, 4395, 4396, 4397, 4398, 4399, 4400, 4401, 4402, 4403, 4404, 4405, 4406, 4407, 4408, 4409, 4410, 4411, 4412, 4413, 4414, 4415, 4416, 4417, 4418, 4419, 4420, 4421, 4422, 4423, 4424, 4425, 4426, 4427, 4428, 4429, 4430, 4431, 4432, 4433, 4434, 4435, 4436, 4437, 4438, 4439, 4440, 4441, 4442, 4443, 4444, 4445, 4446, 4447, 4448, 4449, 4450, 4451, 4452, 4453, 4454, 4455, 4456, 4457, 4458, 4459, 4460, 4461, 4462, 4463, 4464, 4465, 4466, 4467, 4468, 4469, 4470, 4471, 4472, 4473, 4474, 4475, 4476, 4477, 4478, 4479, 4480, 4481, 4482, 4483, 4484, 4485, 4486, 4487, 4488, 4489, 4490, 4491, 4492, 4493, 4494, 4495, 4496, 4497, 4498, 4499, 4500, 4501, 4502, 4503, 4504, 4505, 4506, 4507, 4508, 4509, 4510, 4511, 4512, 4513, 4514, 4515, 4516, 4517, 4518, 4519, 4520, 4521, 4522, 4523, 4524, 4525, 4526, 4527, 4528, 4529, 4530, 4531, 4532, 4533, 4534, 4535, 4536, 4537, 4538, 4539, 4540, 4541, 4542, 4543, 4544, 4545, 4546, 4547, 4548, 4549, 4550, 4551, 4552, 4553, 4554, 4555, 4556, 4557, 4558, 4559, 4560, 4561, 4562, 4563, 4564, 4565, 4566, 4567, 4568, 4569, 4570, 4571, 4572, 4573, 4574, 4575, 4576, 4577, 4578, 4579, 4580, 4581, 4582, 4583, 4584, 4585, 4586, 4587, 4588, 4589, 4590, 4591, 4592, 4593, 4594, 4595, 4596, 4597, 4598, 4599, 4600, 4601, 4602, 4603, 4604, 4605, 4606, 4607, 4608, 4609, 4610, 4611, 4612, 4613, 4614, 4615, 4616, 4617, 4618, 4619, 4620, 4621, 4622, 4623, 4624, 4625, 4626, 4627, 4628, 4629, 4630, 4631, 4632, 4633, 4634, 4635, 4636, 4637, 4638, 4639, 4640, 4641, 4642, 4643, 4644, 4645, 4646, 4647, 4648, 4649, 4650, 4651, 4652, 4653, 4654, 4655, 4656, 4657, 4658, 4659, 4660, 4661, 4662, 4663, 4664, 4665, 4666, 4667, 4668, 4669, 4670, 4671, 4672, 4673, 4674, 4675, 4676, 4677, 4678, 4679, 4680, 4681, 4682, 4683, 4684, 4685, 4686, 4687, 4688, 4689, 4690, 4691, 4692, 4693, 4694, 4695, 4696, 4697, 4698, 4699, 4700, 4701, 4702, 4703, 4704, 4705, 4706, 4707, 4708, 4709, 4710, 4711, 4712, 4713, 4714, 4715, 4716, 4717, 4718, 4719, 4720, 4721, 4722, 4723, 4724, 4725, 4726, 4727, 4728, 4729, 4730, 4731, 4732, 4733, 4734, 4735, 4736, 4737, 4738, 4739, 4740, 4741, 4742, 4743, 4744, 4745, 4746, 4747, 4748, 4749, 4750, 4751, 4752, 4753, 4754, 4755, 4756, 4757, 4758, 4759, 4760, 4761, 4762, 4763, 4764, 4765, 4766, 4767, 4768, 4769, 4770, 4771, 4772, 4773, 4774, 4775, 4776, 4777, 4778, 4779, 4780, 4781, 4782, 4783, 4784, 4785, 4786, 4787, 4788, 4789, 4790, 4791, 4792, 4793, 4794, 4795, 4796, 4797, 4798, 4799, 4800, 4801, 4802, 4803, 4804, 4805, 4806, 4807, 4808, 4809, 4810, 4811, 4812, 4813, 4814, 4815, 4816, 4817, 4818, 4819, 4820, 4821, 4822, 4823, 4824, 4825, 4826, 4827, 4828, 4829, 4830, 4831, 4832, 4833, 4834, 4835, 4836, 4837, 4838, 4839, 4840, 4841, 4842, 4843, 4844, 4845, 4846, 4847, 4848, 4849, 4850, 4851, 4852, 4853, 4854, 4855, 4856, 4857, 4858, 4859, 4860, 4861, 4862, 4863, 4864, 4865, 4866, 4867, 4868, 4869, 4870, 4871, 4872, 4873, 4874, 4875, 4876, 4877, 4878, 4879, 4880, 4881, 4882, 4883, 4884, 4885, 4886, 4887, 4888, 4889, 4890, 4891, 4892, 4893, 4894, 4895, 4896, 4897, 4898, 4899, 4900, 4901, 4902, 4903, 4904, 4905, 4906, 4907, 4908, 4909, 4910, 4911, 4912, 4913, 4914, 4915, 4916, 4917, 4918, 4919, 4920, 4921, 4922, 4923, 4924, 4925, 4926, 4927, 4928, 4929, 4930, 4931, 4932, 4933, 4934, 4935, 4936, 4937, 4938, 4939, 4940, 4941, 4942, 4943, 4944, 4945, 4946, 4947, 4948, 4949, 4950, 4951, 4952, 4953, 4954, 4955, 4956, 4957, 4958, 4959, 4960, 4961, 4962, 4963, 4964, 4965, 4966, 4967, 4968, 4969, 4970, 4971, 4972, 4973, 4974, 4975, 4976, 4977, 4978, 4979, 4980, 4981, 4982, 4983, 4984, 4985, 4986, 4987, 4988, 4989, 4990, 4991, 4992, 4993, 4994, 4995, 4996, 4997, 4998, 4999, 5000, 5001, 5002, 5003, 5004, 5005, 5006, 5007, 5008, 5009, 5010, 5011, 5012, 5013, 5014, 5015, 5016, 5017, 5018, 5019, 5020, 5021, 5022, 5023, 5024, 5025, 5026, 5027, 5028, 5029, 5030, 5031, 5032, 5033, 5034, 5035, 5036, 5037, 5038, 5039, 5040, 5041, 5042, 5043, 5044, 5045, 5046, 5047, 5048, 5049, 5050, 5051, 5052, 5053, 5054, 5055, 5056, 5057, 5058, 5059, 5060, 5061, 5062, 5063, 5064, 5065, 5066, 5067, 5068, 5069, 5070, 5071, 5072, 5073, 5074, 5075, 5076, 5077, 5078, 5079, 5080, 5081, 5082, 5083, 5084, 5085, 5086, 5087, 5088, 5089, 5090, 5091, 5092, 5093, 5094, 5095, 5096, 5097, 5098, 5099, 5100, 5101, 5102, 5103, 5104, 5105, 5106, 5107, 5108, 5109, 5110, 5111, 5112, 5113, 5114, 5115, 5116, 5117, 5118, 5119, 5120, 5121, 5122, 5123, 5124, 5125, 5126, 5127, 5128, 5129, 5130, 5131, 5132, 5133, 5134, 5135, 5136, 5137, 5138, 5139, 5140, 5141, 5142, 5143, 5144, 5145, 5146, 5147, 5148, 5149, 5150, 5151, 5152, 5153, 5154, 5155, 5156, 5157, 5158, 5159, 5160, 5161, 5162, 5163, 5164, 5165, 5166, 5167, 5168, 5169, 5170, 5171, 5172, 5173, 5174, 5175, 5176, 5177, 5178, 5179, 5180, 5181, 5182, 5183, 5184, 5185, 5186, 5187, 5188, 5189, 5190, 5191, 5192, 5193, 5194, 5195, 5196, 5197, 5198, 5199, 5200, 5201, 5202, 5203, 5204, 5205, 5206, 5207, 5208, 5209, 5210, 5211, 5212, 5213, 5214, 5215, 5216, 5217, 5218, 5219, 5220, 5221, 5222, 5223, 5224, 5225, 5226, 5227, 5228, 5229, 5230, 5231, 5232, 5233, 5234, 5235, 5236, 5237, 5238, 5239, 5240, 5241, 5242, 5243, 5244, 5245, 5246, 5247, 5248, 5249, 5250, 5251, 5252, 5253, 5254, 5255, 5256, 5257, 5258, 5259, 5260, 5261, 5262, 5263, 5264, 5265, 5266, 5267, 5268, 5269, 5270, 5271, 5272, 5273, 5274, 5275, 5276, 5277, 5278, 5279, 5280, 5281, 5282, 5283, 5284, 5285, 5286, 5287, 5288, 5289, 5290, 5291, 5292, 5293, 5294, 5295, 5296, 5297, 5298, 5299, 5300, 5301, 5302, 5303, 5304, 5305, 5306, 5307, 5308, 5309, 5310, 5311, 5312, 5313, 5314, 5315, 5316, 5317, 5318, 5319, 5320, 5321, 5322, 5323, 5324, 5325, 5326, 5327, 5328, 5329, 5330, 5331, 5332, 5333, 5334, 5335, 5336, 5337, 5338, 5339, 5340, 5341, 5342, 5343, 5344, 5345, 5346, 5347, 5348, 5349, 5350, 5351, 5352, 5353, 5354, 5355, 5356, 5357, 5358, 5359, 5360, 5361, 5362, 5363, 5364, 5365, 5366, 5367, 5368, 5369, 5370, 5371, 5372, 5373, 5374, 5375, 5376, 5377, 5378, 5379, 5380, 5381, 5382, 5383, 5384, 5385, 5386, 5387, 5388, 5389, 5390, 5391, 5392, 5393, 5394, 5395, 5396, 5397, 5398, 5399, 5400, 5401, 5402, 5403, 5404, 5405, 5406, 5407, 5408, 5409, 5410, 5411, 5412, 5413, 5414, 5415, 5416, 5417, 5418, 5419, 5420, 5421, 5422, 5423, 5424, 5425, 5426, 5427, 5428, 5429, 5430, 5431, 5432, 5433, 5434, 5435, 5436, 5437, 5438, 5439, 5440, 5441, 5442, 5443, 5444, 5445, 5446, 5447, 5448, 5449, 5450, 5451, 5452, 5453, 5454, 5455, 5456, 5457, 5458, 5459, 5460, 5461, 5462, 5463, 5464, 5465, 5466, 5467, 5468, 5469, 5470, 5471, 5472, 5473, 5474, 5475, 5476, 5477, 5478, 5479, 5480, 5481, 5482, 5483, 5484, 5485, 5486, 5487, 5488, 5489, 5490, 5491, 5492, 5493, 5494, 5495, 5496, 5497, 5498, 5499, 5500, 5501, 5502, 5503, 5504, 5505, 5506, 5507, 5508, 5509, 5510, 5511, 5512, 5513, 5514, 5515, 5516, 5517, 5518, 5519, 5520, 5521, 5522, 5523, 5524, 5525, 5526, 5527, 5528, 5529, 5530, 5531, 5532, 5533, 5534, 5535, 5536, 5537, 5538, 5539, 5540, 5541, 5542, 5543, 5544, 5545, 5546, 5547, 5548, 5549, 5550, 5551, 5552, 5553, 5554, 5555, 5556, 5557, 5558, 5559, 5560, 5561, 5562, 5563, 5564, 5565, 5566, 5567, 5568, 5569, 5570, 5571, 5572, 5573, 5574, 5575, 5576, 5577, 5578, 5579, 5580, 5581, 5582, 5583, 5584, 5585, 5586, 5587, 5588, 5589, 5590, 5591, 5592, 5593, 5594, 5595, 5596, 5597, 5598, 5599, 5600, 5601, 5602, 5603, 5604, 5605, 5606, 5607, 5608, 5609, 5610, 5611, 5612, 5613, 5614, 5615, 5616, 5617, 5618, 5619, 5620, 5621, 5622, 5623, 5624, 5625, 5626, 5627, 5628, 5629, 5630, 5631, 5632, 5633, 5634, 5635, 5636, 5637, 5638, 5639, 5640, 5641, 5642, 5643, 5644, 5645, 5646, 5647, 5648, 5649, 5650,</t>
         </is>
       </c>
-      <c r="BP5" t="n">
+      <c r="BV5" t="n">
         <v>0.1476882862277406</v>
       </c>
-      <c r="BQ5" t="inlineStr">
+      <c r="BW5" t="inlineStr">
         <is>
           <t>{'Numk': 15, 'KPar': 5, 'Bucket_index': 1000}</t>
         </is>
       </c>
-      <c r="BR5" t="n">
+      <c r="BX5" t="n">
         <v>1603.097915115068</v>
       </c>
-      <c r="BS5" t="inlineStr">
+      <c r="BY5" t="inlineStr">
         <is>
           <t>[519, 521, 840, 842, 843, 845, 846, 847, 848, 849, 850, 851, 852, 853, 854, 2126, 2127, 2128, 2131, 2132, 2133, 2134, 2136, 2137, 2138, 2139, 2140, 2141, 2142, 2143, 2144, 2145, 2146, 2147, 2148, 2149, 2150, 2151, 2152, 2153, 2154, 2155, 2156, 2157, 2158, 2159, 2160, 2161, 2162, 2163, 2164, 2165, 2166, 2167, 2168, 2169, 2170, 2171, 2172, 2173, 2174, 2175, 2176, 2177, 2178, 2179, 2180, 2181, 2182, 2183, 2184, 2185, 2186, 2187, 2188, 2189, 2190, 2191, 2192, 2193, 2194, 2195, 2196, 2197, 2198, 2199, 2200, 2201, 2202, 2203, 2204, 2205, 2206, 2207, 2208, 2209, 2210, 2211, 2212, 2213, 2214, 2215, 2216, 2217, 2218, 2219, 2220, 2221, 2222, 2223, 2224, 2225, 2226, 2227, 2228, 2229, 2230, 2231, 2232, 2233, 2234, 2235, 2236, 2237, 2238, 2239, 2240, 2241, 2242, 2243, 2244, 2245, 2246, 2247, 2248, 2249, 2250, 2251, 2252, 2253, 2254, 2256, 2257, 2258, 2259, 2260, 2261, 2263, 2265, 2267, 2269, 2270, 2273, 2276, 2280, 2287, 2289, 2290, 2292, 3846, 3847, 3848, 3849, 3853, 3854, 3855, 3856, 3857, 3858, 3859, 3860, 3861, 3862, 3863, 3864, 3865, 3866, 3867, 3868, 3869, 3870, 3871, 3872, 3873, 3874, 3875, 3876, 3877, 3878, 3879, 3880, 3881, 3882, 3883, 3884, 3885, 3886, 3887, 3888, 3889, 3890, 3891, 3892, 3893, 3894, 3895, 3896, 3897, 3898, 3899, 3900, 3901, 3902, 3903, 3904, 3905, 3906, 3907, 3908, 3909, 3910, 3911, 3912, 3913, 9694, 9696, 9697, 9698, 9699, 9700, 9701, 9702, 9703, 9704, 9705, 9706, 9707, 9708, 9709, 9710, 9711, 9712, 9713, 9714, 9715, 9716, 9717, 9718, 9719, 9720, 9721, 9722, 9723, 9724, 9725, 9726, 9727, 9728, 9729, 9730, 9731, 9732, 9733, 9734, 9735, 9736, 9737, 9738, 9739, 9740, 9741, 9742, 9743, 9744, 9745, 9746, 9747, 9748, 9749, 16153, 16154, 16156, 16158, 16178, 16179, 16184, 16185, 16186, 16187, 16188, 16189, 16190, 16191, 16192, 16193, 16194, 16195, 16196, 16197, 16198, 16199, 16200, 16201, 16202, 16241, 16242, 16243, 16244, 16245, 16246, 16247, 16248, 16249, 16250, 16251, 16252, 16253, 16254, 16255, 16256, 16257, 16258, 16259, 16260, 16261, 16262, 16263, 16264, 16265, 16266, 16267, 16268, 16269, 16270, 16271, 16272, 16273, 16275, 16277, 16278, 16279, 16280, 16281, 16282, 16284, 16285, 16286, 16288, 16304, 16305, 16307, 16308, 16309, 16310, 16311, 16312, 16313, 16314, 16316, 16319, 16320, 16321, 16322, 16323, 16324, 16325, 16326, 16327, 16328, 16329, 16330, 16331, 16332, 16333, 16334, 16335, 16336, 16337, 16338, 16339, 16340, 16341, 16342, 16343, 16344, 16345, 16346, 16347, 16348, 16349, 16350, 16351, 16352, 16353, 16354, 16355, 16356, 16357, 16358, 16359, 16360, 16361, 16362, 16363, 16364, 16365, 16366, 16367, 16368, 16369, 16370, 16371, 16372, 16373, 16374, 16375, 16376, 16377, 16378, 16379, 16380, 16381, 16382, 16383, 16384, 16385, 16386, 16387, 16388, 16389, 16390, 16391, 16392, 16393, 16394, 16395, 16396, 16397, 16398, 16399, 16400, 16401, 16402, 16403, 16404, 16405, 16419, 16420, 16421, 16422, 16423, 16424, 16425, 16426, 16427, 16428, 16429, 16430, 16431, 16432, 16433, 16434, 16435, 16608, 16609, 16610, 16611, 16612, 16613, 16614, 16615, 16616, 16617, 16618, 16619, 16620, 16621, 16622, 16623, 16624, 16625, 16626, 16627, 16628, 16629, 16630, 16631, 16632, 16633, 16634, 16635, 16636, 16637, 16638, 16639, 16640, 16641, 16642, 16643, 16644, 16645, 16646, 16647, 16648, 16649, 16650, 16651, 16652, 16653, 16654, 16655, 16656, 16657, 16658, 16659, 16660, 16661, 16662, 16663, 16664, 16665, 16666, 16667, 16668, 16669, 16670, 16671, 16672, 16673, 16674, 16675, 16676, 16677, 16678, 16679, 16680, 16681, 16682, 16917, 16918, 16919, 16920, 16921, 16922, 16923, 16924, 16925, 16926, 16927, 16928, 16929, 16930, 16931, 16932, 16933, 16934, 16935, 16936, 16937, 16938, 16939, 16940, 16941, 16942, 16943, 16944, 16945, 16946, 16947, 16948, 16949, 16950, 16951, 16952, 16953, 16954, 16955, 16956, 16957, 16958, 16959, 16960, 16961, 16962, 16963, 16964, 16965, 16966, 16967, 16968, 16969, 16970, 16971, 16972, 16973, 16974, 16975, 16976, 16977, 16978, 16979, 16980, 16981, 16982, 16983, 16984, 16985, 16986, 16987, 16988, 16989, 16990, 16991, 16992, 16993, 16994, 16995, 16996, 16997, 16998, 16999, 17000, 17001, 17002, 17003, 17004, 17005, 17006, 17007, 17008, 17009, 17010, 17011, 17012, 17013, 17014, 17015, 17016, 17017, 17018, 17019, 17020, 17021, 17022, 17023, 17024, 17025, 17026, 17027, 17028, 17029, 17030, 17031, 17174, 17175, 17176, 17177, 17178, 17179, 17180, 17181, 17182, 17183, 17184, 17185, 17186, 17187, 17188, 17189, 17190, 17191, 17192, 18022, 18023, 18024, 18026, 18028, 18029, 18030, 18031, 18032, 18033, 18034, 18035, 18036, 18037, 18038, 18039, 18040, 18041, 18042, 19317, 19320, 19321, 19323, 19325, 19326, 19328, 19329, 19330, 19331, 19332, 19333, 19334, 19335, 19336, 19337, 19338, 19339, 19340, 19341, 19342, 19343, 19344, 19345, 19346, 19347, 19348, 19349, 19350, 19351, 19352, 19353, 19354, 19355, 19356, 19357, 19358, 19359, 19360, 19361, 19362, 19363, 19364, 19365, 19366, 19367, 19368, 19369, 19370, 19371, 19372, 19373, 19374, 19375, 19376, 19377, 19378, 19379, 19380, 19381, 19382, 19383, 19384, 19385, 19386, 19387, 19388, 19389, 19390, 19391, 19392, 19393, 19394, 19395, 19396, 19397, 19398, 19399, 19400, 19401, 19402, 19403, 19404, 19405, 19406, 19407, 19408, 19409, 19410, 19411, 19412, 19413, 19414, 19415, 19416, 19417, 19418, 19419, 19420, 19421, 19422, 19423, 19424, 19425, 19426, 19427, 19428, 19429, 19430, 19431, 19432, 19433, 19434, 19435, 19436, 19437, 19438, 19439, 19440, 19441, 19442, 19443, 19444, 19445, 19446, 19447, 19448, 19449, 19450, 19451, 19452, 19453, 19454, 19455, 19456, 19457, 19458, 19459, 19460, 19461, 19462, 19463, 19464, 19465, 19466, 19467, 19468, 19469, 19470, 19471, 19472, 19473, 19474, 19475, 19476, 19477, 19478, 19479, 19480, 19481, 19482, 19483, 19484, 19485, 19486, 19487, 19488, 19489, 19490, 19491, 19492, 19493, 19494, 19495, 19496, 19497, 19498, 19499, 19500, 19501, 19502, 19503, 19504, 19505, 19506, 19507, 19508, 19509, 19510, 19511, 19512, 19513, 19514, 19515, 19516, 19517, 19518, 19519, 19520, 19521, 19522, 19523, 19524, 19525, 19526, 19527, 19528, 19529, 19530, 19531, 19532, 19533, 19534, 19535, 19536, 19537, 19538, 19539, 19540, 19541, 19542, 19543, 19544, 19545, 19546, 19547, 19548, 19549, 19550, 19551, 19552, 19553, 19554, 19555, 19556, 19557, 19558, 19559, 19560, 19561, 19562, 19563, 19564, 19565, 19566, 19567, 19568, 19569]</t>
         </is>
       </c>
-      <c r="BT5" t="n">
+      <c r="BZ5" t="n">
         <v>0.6078576723498887</v>
       </c>
-      <c r="BU5" t="inlineStr">
+      <c r="CA5" t="inlineStr">
         <is>
           <t>{'max_features': 1, 'window_size': 1957, 'n_estimator': 23}</t>
         </is>
       </c>
-      <c r="BV5" t="n">
+      <c r="CB5" t="n">
         <v>580.5829102229327</v>
       </c>
     </row>
@@ -1930,93 +2032,111 @@
       <c r="AY6" t="n">
         <v>4</v>
       </c>
-      <c r="AZ6" t="inlineStr"/>
-      <c r="BA6" t="inlineStr">
+      <c r="AZ6" t="n">
+        <v>4</v>
+      </c>
+      <c r="BA6" t="n">
+        <v>4</v>
+      </c>
+      <c r="BB6" t="n">
+        <v>4</v>
+      </c>
+      <c r="BC6" t="n">
+        <v>4</v>
+      </c>
+      <c r="BD6" t="n">
+        <v>4</v>
+      </c>
+      <c r="BE6" t="n">
+        <v>4</v>
+      </c>
+      <c r="BF6" t="inlineStr"/>
+      <c r="BG6" t="inlineStr">
         <is>
           <t>nab-data/realKnownCause/nyc_taxi.csv</t>
         </is>
       </c>
-      <c r="BB6" t="n">
+      <c r="BH6" t="n">
         <v>10320</v>
       </c>
-      <c r="BC6" t="inlineStr">
+      <c r="BI6" t="inlineStr">
         <is>
           <t>NAB</t>
         </is>
       </c>
-      <c r="BD6" t="n">
-        <v>5</v>
-      </c>
-      <c r="BE6" t="inlineStr">
+      <c r="BJ6" t="n">
+        <v>5</v>
+      </c>
+      <c r="BK6" t="inlineStr">
         <is>
           <t>5839; 7080; 8423; 8731; 9977</t>
         </is>
       </c>
-      <c r="BF6" t="n">
+      <c r="BL6" t="n">
         <v>206</v>
       </c>
-      <c r="BG6" t="inlineStr">
-        <is>
-          <t>[8773, 8774, 8822, 8823, 8824, 8825, 8826, 8827, 8828, 8829, 8832, 8833, 8834, 8835, 8836, 8837, 8838]</t>
-        </is>
-      </c>
-      <c r="BH6" t="n">
-        <v>0.3116883116883117</v>
-      </c>
-      <c r="BI6" t="inlineStr">
-        <is>
-          <t>{'initial_window': 548, 'window_size': 248, 'num_trees': 16, 'max_depth': 13}</t>
-        </is>
-      </c>
-      <c r="BJ6" t="n">
-        <v>27.77252390398644</v>
-      </c>
-      <c r="BK6" t="inlineStr">
-        <is>
-          <t>[197, 536, 537, 584, 660, 661, 673, 816, 864, 872, 873, 1200, 1920, 2124, 3324, 3643, 3840, 4416, 4608, 4926, 5196, 5246, 5856, 6000, 6016, 6864, 7003, 7152, 8256, 8448, 8896, 9600, 9680, 9936]</t>
-        </is>
-      </c>
-      <c r="BL6" t="n">
-        <v>0.2484472049689441</v>
-      </c>
       <c r="BM6" t="inlineStr">
         <is>
-          <t>{'AR_window_size': 63, 'differencing-order': 1}</t>
+          <t>[3261, 3262, 5954, 5955, 8833, 8834]</t>
         </is>
       </c>
       <c r="BN6" t="n">
-        <v>129.5341490968131</v>
+        <v>0.5</v>
       </c>
       <c r="BO6" t="inlineStr">
         <is>
+          <t>{'initial_window': 1121, 'window_size': 1899, 'num_trees': 17, 'max_depth': 19}</t>
+        </is>
+      </c>
+      <c r="BP6" t="n">
+        <v>383.268750739051</v>
+      </c>
+      <c r="BQ6" t="inlineStr">
+        <is>
+          <t>[170, 753, 1274, 3660, 6042, 6043, 6045, 6348, 7130, 8282, 8474, 8922, 9393, 10044]</t>
+        </is>
+      </c>
+      <c r="BR6" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="BS6" t="inlineStr">
+        <is>
+          <t>{'AR_window_size': 89, 'differencing-order': 1}</t>
+        </is>
+      </c>
+      <c r="BT6" t="n">
+        <v>390.7265384758357</v>
+      </c>
+      <c r="BU6" t="inlineStr">
+        <is>
           <t xml:space="preserve">[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86, 87, 88, 89, 90, 91, 92, 93, 94, 95, 96, 97, 98, 99, 100, 101, 102, 103, 104, 105, 106, 107, 108, 109, 110, 111, 112, 113, 114, 115, 116, 117, 118, 119, 120, 121, 122, 123, 124, 125, 126, 127, 128, 129, 130, 131, 132, 133, 134, 135, 136, 137, 138, 139, 140, 141, 142, 143, 144, 145, 146, 147, 148, 149, 150, 151, 152, 153, 154, 155, 156, 157, 158, 159, 160, 161, 162, 163, 164, 165, 166, 167, 168, 169, 170, 171, 172, 173, 174, 175, 176, 177, 178, 179, 180, 181, 182, 183, 184, 185, 186, 187, 188, 189, 190, 191, 192, 193, 194, 195, 196, 197, 198, 199, 200, 201, 202, 203, 204, 205, 206, 207, 208, 209, 210, 211, 212, 213, 214, 215, 216, 217, 218, 219, 220, 221, 222, 223, 224, 225, 226, 227, 228, 229, 230, 231, 232, 233, 234, 235, 236, 237, 238, 239, 240, 241, 242, 243, 244, 245, 246, 247, 248, 249, 250, 251, 252, 253, 254, 255, 256, 257, 258, 259, 260, 261, 262, 263, 264, 265, 266, 267, 268, 269, 270, 271, 272, 273, 274, 275, 276, 277, 278, 279, 280, 281, 282, 283, 284, 285, 286, 287, 288, 289, 290, 291, 292, 293, 294, 295, 296, 297, 298, 299, 300, 301, 302, 303, 304, 305, 306, 307, 308, 309, 310, 311, 312, 313, 314, 315, 316, 317, 318, 319, 320, 321, 322, 323, 324, 325, 326, 327, 328, 329, 330, 331, 332, 333, 334, 335, 336, 337, 338, 339, 340, 341, 342, 343, 344, 345, 346, 347, 348, 349, 350, 351, 352, 353, 354, 355, 356, 357, 358, 359, 360, 361, 362, 363, 364, 365, 366, 367, 368, 369, 370, 371, 372, 373, 374, 375, 376, 377, 378, 379, 380, 381, 382, 383, 384, 385, 386, 387, 388, 389, 390, 391, 392, 393, 394, 395, 396, 397, 398, 399, 400, 401, 402, 403, 404, 405, 406, 407, 408, 409, 410, 411, 412, 413, 414, 415, 416, 417, 418, 419, 420, 421, 422, 423, 424, 425, 426, 427, 428, 429, 430, 431, 432, 433, 434, 435, 436, 437, 438, 439, 440, 441, 442, 443, 444, 445, 446, 447, 448, 449, 450, 451, 452, 453, 454, 455, 456, 457, 458, 459, 460, 461, 462, 463, 464, 465, 466, 467, 468, 469, 470, 471, 472, 473, 474, 475, 476, 477, 478, 479, 480, 481, 482, 483, 484, 485, 486, 487, 488, 489, 490, 491, 492, 493, 494, 495, 496, 497, 498, 499, 500, 501, 502, 503, 504, 505, 506, 507, 508, 509, 510, 511, 512, 513, 514, 515, 516, 517, 518, 519, 520, 521, 522, 523, 524, 525, 526, 527, 528, 529, 530, 531, 532, 533, 534, 535, 536, 537, 538, 539, 540, 541, 542, 543, 544, 545, 546, 547, 548, 549, 550, 551, 552, 553, 554, 555, 556, 557, 558, 559, 560, 561, 562, 563, 564, 565, 566, 567, 568, 569, 570, 571, 572, 573, 574, 575, 576, 577, 578, 579, 580, 581, 582, 583, 584, 585, 586, 587, 588, 589, 590, 591, 592, 593, 594, 595, 596, 597, 598, 599, 600, 601, 602, 603, 604, 605, 606, 607, 608, 609, 610, 611, 612, 613, 614, 615, 616, 617, 618, 619, 620, 621, 622, 623, 624, 625, 626, 627, 628, 629, 630, 631, 632, 633, 634, 635, 636, 637, 638, 639, 640, 641, 642, 643, 644, 645, 646, 647, 648, 649, 650, 651, 652, 653, 654, 655, 656, 657, 658, 659, 660, 661, 662, 663, 664, 665, 666, 667, 668, 669, 670, 671, 672, 673, 674, 675, 676, 677, 678, 679, 680, 681, 682, 683, 684, 685, 686, 687, 688, 689, 690, 691, 692, 693, 694, 695, 696, 697, 698, 699, 700, 701, 702, 703, 704, 705, 706, 707, 708, 709, 710, 711, 712, 713, 714, 715, 716, 717, 718, 719, 720, 721, 722, 723, 724, 725, 726, 727, 728, 729, 730, 731, 732, 733, 734, 735, 736, 737, 738, 739, 740, 741, 742, 743, 744, 745, 746, 747, 748, 749, 750, 751, 752, 753, 754, 755, 756, 757, 758, 759, 760, 761, 762, 763, 764, 765, 766, 767, 768, 769, 770, 771, 772, 773, 774, 775, 776, 777, 778, 779, 780, 781, 782, 783, 784, 785, 786, 787, 788, 789, 790, 791, 792, 793, 794, 795, 796, 797, 798, 799, 800, 801, 802, 803, 804, 805, 806, 807, 808, 809, 810, 811, 812, 813, 814, 815, 816, 817, 818, 819, 820, 821, 822, 823, 824, 825, 826, 827, 828, 829, 830, 831, 832, 833, 834, 835, 836, 837, 838, 839, 840, 841, 842, 843, 844, 845, 846, 847, 848, 849, 850, 851, 852, 853, 854, 855, 856, 857, 858, 859, 860, 861, 862, 863, 864, 865, 866, 867, 868, 869, 870, 871, 872, 873, 874, 875, 876, 877, 878, 879, 880, 881, 882, 883, 884, 885, 886, 887, 888, 889, 890, 891, 892, 893, 894, 895, 896, 897, 898, 899, 900, 901, 902, 903, 904, 905, 906, 907, 908, 909, 910, 911, 912, 913, 914, 915, 916, 917, 918, 919, 920, 921, 922, 923, 924, 925, 926, 927, 928, 929, 930, 931, 932, 933, 934, 935, 936, 937, 938, 939, 940, 941, 942, 943, 944, 945, 946, 947, 948, 949, 950, 951, 952, 953, 954, 955, 956, 957, 958, 959, 960, 961, 962, 963, 964, 965, 966, 967, 968, 969, 970, 971, 972, 973, 974, 975, 976, 977, 978, 979, 980, 981, 982, 983, 984, 985, 986, 987, 988, 989, 990, 991, 992, 993, 994, 995, 996, 997, 998, 999, 1000, 1001, 1002, 1003, 1004, 1005, 1006, 1007, 1008, 1009, 1010, 1011, 1012, 1013, 1014, 1015, 1016, 1017, 1018, 1019, 1020, 1021, 1022, 1023, 1024, 1025, 1026, 1027, 1028, 1029, 1030, 1031, 1032, 1033, 1034, 1035, 1036, 1037, 1038, 1039, 1040, 1041, 1042, 1043, 1044, 1045, 1046, 1047, 1048, 1049, 1050, 1051, 1052, 1053, 1054, 1055, 1056, 1057, 1058, 1059, 1060, 1061, 1062, 1063, 1064, 1065, 1066, 1067, 1068, 1069, 1070, 1071, 1072, 1073, 1074, 1075, 1076, 1077, 1078, 1079, 1080, 1081, 1082, 1083, 1084, 1085, 1086, 1087, 1088, 1089, 1090, 1091, 1092, 1093, 1094, 1095, 1096, 1097, 1098, 1099, 1100, 1101, 1102, 1103, 1104, 1105, 1106, 1107, 1108, 1109, 1110, 1111, 1112, 1113, 1114, 1115, 1116, 1117, 1118, 1119, 1120, 1121, 1122, 1123, 1124, 1125, 1126, 1127, 1128, 1129, 1130, 1131, 1132, 1133, 1134, 1135, 1136, 1137, 1138, 1139, 1140, 1141, 1142, 1143, 1144, 1145, 1146, 1147, 1148, 1149, 1150, 1151, 1152, 1153, 1154, 1155, 1156, 1157, 1158, 1159, 1160, 1161, 1162, 1163, 1164, 1165, 1166, 1167, 1168, 1169, 1170, 1171, 1172, 1173, 1174, 1175, 1176, 1177, 1178, 1179, 1180, 1181, 1182, 1183, 1184, 1185, 1186, 1187, 1188, 1189, 1190, 1191, 1192, 1193, 1194, 1195, 1196, 1197, 1198, 1199, 1200, 1201, 1202, 1203, 1204, 1205, 1206, 1207, 1208, 1209, 1210, 1211, 1212, 1213, 1214, 1215, 1216, 1217, 1218, 1219, 1220, 1221, 1222, 1223, 1224, 1225, 1226, 1227, 1228, 1229, 1230, 1231, 1232, 1233, 1234, 1235, 1236, 1237, 1238, 1239, 1240, 1241, 1242, 1243, 1244, 1245, 1246, 1247, 1248, 1249, 1250, 1251, 1252, 1253, 1254, 1255, 1256, 1257, 1258, 1259, 1260, 1261, 1262, 1263, 1264, 1265, 1266, 1267, 1268, 1269, 1270, 1271, 1272, 1273, 1274, 1275, 1276, 1277, 1278, 1279, 1280, 1281, 1282, 1283, 1284, 1285, 1286, 1287, 1288, 1289, 1290, 1291, 1292, 1293, 1294, 1295, 1296, 1297, 1298, 1299, 1300, 1301, 1302, 1303, 1304, 1305, 1306, 1307, 1308, 1309, 1310, 1311, 1312, 1313, 1314, 1315, 1316, 1317, 1318, 1319, 1320, 1321, 1322, 1323, 1324, 1325, 1326, 1327, 1328, 1329, 1330, 1331, 1332, 1333, 1334, 1335, 1336, 1337, 1338, 1339, 1340, 1341, 1342, 1343, 1344, 1345, 1346, 1347, 1348, 1349, 1350, 1351, 1352, 1353, 1354, 1355, 1356, 1357, 1358, 1359, 1360, 1361, 1362, 1363, 1364, 1365, 1366, 1367, 1368, 1369, 1370, 1371, 1372, 1373, 1374, 1375, 1376, 1377, 1378, 1379, 1380, 1381, 1382, 1383, 1384, 1385, 1386, 1387, 1388, 1389, 1390, 1391, 1392, 1393, 1394, 1395, 1396, 1397, 1398, 1399, 1400, 1401, 1402, 1403, 1404, 1405, 1406, 1407, 1408, 1409, 1410, 1411, 1412, 1413, 1414, 1415, 1416, 1417, 1418, 1419, 1420, 1421, 1422, 1423, 1424, 1425, 1426, 1427, 1428, 1429, 1430, 1431, 1432, 1433, 1434, 1435, 1436, 1437, 1438, 1439, 1440, 1441, 1442, 1443, 1444, 1445, 1446, 1447, 1448, 1449, 1450, 1451, 1452, 1453, 1454, 1455, 1456, 1457, 1458, 1459, 1460, 1461, 1462, 1463, 1464, 1465, 1466, 1467, 1468, 1469, 1470, 1471, 1472, 1473, 1474, 1475, 1476, 1477, 1478, 1479, 1480, 1481, 1482, 1483, 1484, 1485, 1486, 1487, 1488, 1489, 1490, 1491, 1492, 1493, 1494, 1495, 1496, 1497, 1498, 1499, 1500, 1501, 1502, 1503, 1504, 1505, 1506, 1507, 1508, 1509, 1510, 1511, 1512, 1513, 1514, 1515, 1516, 1517, 1518, 1519, 1520, 1521, 1522, 1523, 1524, 1525, 1526, 1527, 1528, 1529, 1530, 1531, 1532, 1533, 1534, 1535, 1536, 1537, 1538, 1539, 1540, 1541, 1542, 1543, 1544, 1545, 1546, 1547, 1548, 1549, 1550, 1551, 1552, 1553, 1554, 1555, 1556, 1557, 1558, 1559, 1560, 1561, 1562, 1563, 1564, 1565, 1566, 1567, 1568, 1569, 1570, 1571, 1572, 1573, 1574, 1575, 1576, 1577, 1578, 1579, 1580, 1581, 1582, 1583, 1584, 1585, 1586, 1587, 1588, 1589, 1590, 1591, 1592, 1593, 1594, 1595, 1596, 1597, 1598, 1599, 1600, 1601, 1602, 1603, 1604, 1605, 1606, 1607, 1608, 1609, 1610, 1611, 1612, 1613, 1614, 1615, 1616, 1617, 1618, 1619, 1620, 1621, 1622, 1623, 1624, 1625, 1626, 1627, 1628, 1629, 1630, 1631, 1632, 1633, 1634, 1635, 1636, 1637, 1638, 1639, 1640, 1641, 1642, 1643, 1644, 1645, 1646, 1647, 1648, 1649, 1650, 1651, 1652, 1653, 1654, 1655, 1656, 1657, 1658, 1659, 1660, 1661, 1662, 1663, 1664, 1665, 1666, 1667, 1668, 1669, 1670, 1671, 1672, 1673, 1674, 1675, 1676, 1677, 1678, 1679, 1680, 1681, 1682, 1683, 1684, 1685, 1686, 1687, 1688, 1689, 1690, 1691, 1692, 1693, 1694, 1695, 1696, 1697, 1698, 1699, 1700, 1701, 1702, 1703, 1704, 1705, 1706, 1707, 1708, 1709, 1710, 1711, 1712, 1713, 1714, 1715, 1716, 1717, 1718, 1719, 1720, 1721, 1722, 1723, 1724, 1725, 1726, 1727, 1728, 1729, 1730, 1731, 1732, 1733, 1734, 1735, 1736, 1737, 1738, 1739, 1740, 1741, 1742, 1743, 1744, 1745, 1746, 1747, 1748, 1749, 1750, 1751, 1752, 1753, 1754, 1755, 1756, 1757, 1758, 1759, 1760, 1761, 1762, 1763, 1764, 1765, 1766, 1767, 1768, 1769, 1770, 1771, 1772, 1773, 1774, 1775, 1776, 1777, 1778, 1779, 1780, 1781, 1782, 1783, 1784, 1785, 1786, 1787, 1788, 1789, 1790, 1791, 1792, 1793, 1794, 1795, 1796, 1797, 1798, 1799, 1800, 1801, 1802, 1803, 1804, 1805, 1806, 1807, 1808, 1809, 1810, 1811, 1812, 1813, 1814, 1815, 1816, 1817, 1818, 1819, 1820, 1821, 1822, 1823, 1824, 1825, 1826, 1827, 1828, 1829, 1830, 1831, 1832, 1833, 1834, 1835, 1836, 1837, 1838, 1839, 1840, 1841, 1842, 1843, 1844, 1845, 1846, 1847, 1848, 1849, 1850, 1851, 1852, 1853, 1854, 1855, 1856, 1857, 1858, 1859, 1860, 1861, 1862, 1863, 1864, 1865, 1866, 1867, 1868, 1869, 1870, 1871, 1872, 1873, 1874, 1875, 1876, 1877, 1878, 1879, 1880, 1881, 1882, 1883, 1884, 1885, 1886, 1887, 1888, 1889, 1890, 1891, 1892, 1893, 1894, 1895, 1896, 1897, 1898, 1899, 1900, 1901, 1902, 1903, 1904, 1905, 1906, 1907, 1908, 1909, 1910, 1911, 1912, 1913, 1914, 1915, 1916, 1917, 1918, 1919, 1920, 1921, 1922, 1923, 1924, 1925, 1926, 1927, 1928, 1929, 1930, 1931, 1932, 1933, 1934, 1935, 1936, 1937, 1938, 1939, 1940, 1941, 1942, 1943, 1944, 1945, 1946, 1947, 1948, 1949, 1950, 1951, 1952, 1953, 1954, 1955, 1956, 1957, 1958, 1959, 1960, 1961, 1962, 1963, 1964, 1965, 1966, 1967, 1968, 1969, 1970, 1971, 1972, 1973, 1974, 1975, 1976, 1977, 1978, 1979, 1980, 1981, 1982, 1983, 1984, 1985, 1986, 1987, 1988, 1989, 1990, 1991, 1992, 1993, 1994, 1995, 1996, 1997, 1998, 1999, 2000, 2001, 2002, 2003, 2004, 2005, 2006, 2007, 2008, 2009, 2010, 2011, 2012, 2013, 2014, 2015, 2016, 2017, 2018, 2019, 2020, 2021, 2022, 2023, 2024, 2025, 2026, 2027, 2028, 2029, 2030, 2031, 2032, 2033, 2034, 2035, 2036, 2037, 2038, 2039, 2040, 2041, 2042, 2043, 2044, 2045, 2046, 2047, 2048, 2049, 2050, 2051, 2052, 2053, 2054, 2055, 2056, 2057, 2058, 2059, 2060, 2061, 2062, 2063, 2064, 2065, 2066, 2067, 2068, 2069, 2070, 2071, 2072, 2073, 2074, 2075, 2076, 2077, 2078, 2079, 2080, 2081, 2082, 2083, 2084, 2085, 2086, 2087, 2088, 2089, 2090, 2091, 2092, 2093, 2094, 2095, 2096, 2097, 2098, 2099, 2100, 2101, 2102, 2103, 2104, 2105, 2106, 2107, 2108, 2109, 2110, 2111, 2112, 2113, 2114, 2115, 2116, 2117, 2118, 2119, 2120, 2121, 2122, 2123, 2124, 2125, 2126, 2127, 2128, 2129, 2130, 2131, 2132, 2133, 2134, 2135, 2136, 2137, 2138, 2139, 2140, 2141, 2142, 2143, 2144, 2145, 2146, 2147, 2148, 2149, 2150, 2151, 2152, 2153, 2154, 2155, 2156, 2157, 2158, 2159, 2160, 2161, 2162, 2163, 2164, 2165, 2166, 2167, 2168, 2169, 2170, 2171, 2172, 2173, 2174, 2175, 2176, 2177, 2178, 2179, 2180, 2181, 2182, 2183, 2184, 2185, 2186, 2187, 2188, 2189, 2190, 2191, 2192, 2193, 2194, 2195, 2196, 2197, 2198, 2199, 2200, 2201, 2202, 2203, 2204, 2205, 2206, 2207, 2208, 2209, 2210, 2211, 2212, 2213, 2214, 2215, 2216, 2217, 2218, 2219, 2220, 2221, 2222, 2223, 2224, 2225, 2226, 2227, 2228, 2229, 2230, 2231, 2232, 2233, 2234, 2235, 2236, 2237, 2238, 2239, 2240, 2241, 2242, 2243, 2244, 2245, 2246, 2247, 2248, 2249, 2250, 2251, 2252, 2253, 2254, 2255, 2256, 2257, 2258, 2259, 2260, 2261, 2262, 2263, 2264, 2265, 2266, 2267, 2268, 2269, 2270, 2271, 2272, 2273, 2274, 2275, 2276, 2277, 2278, 2279, 2280, 2281, 2282, 2283, 2284, 2285, 2286, 2287, 2288, 2289, 2290, 2291, 2292, 2293, 2294, 2295, 2296, 2297, 2298, 2299, 2300, 2301, 2302, 2303, 2304, 2305, 2306, 2307, 2308, 2309, 2310, 2311, 2312, 2313, 2314, 2315, 2316, 2317, 2318, 2319, 2320, 2321, 2322, 2323, 2324, 2325, 2326, 2327, 2328, 2329, 2330, 2331, 2332, 2333, 2334, 2335, 2336, 2337, 2338, 2339, 2340, 2341, 2342, 2343, 2344, 2345, 2346, 2347, 2348, 2349, 2350, 2351, 2352, 2353, 2354, 2355, 2356, 2357, 2358, 2359, 2360, 2361, 2362, 2363, 2364, 2365, 2366, 2367, 2368, 2369, 2370, 2371, 2372, 2373, 2374, 2375, 2376, 2377, 2378, 2379, 2380, 2381, 2382, 2383, 2384, 2385, 2386, 2387, 2388, 2389, 2390, 2391, 2392, 2393, 2394, 2395, 2396, 2397, 2398, 2399, 2400, 2401, 2402, 2403, 2404, 2405, 2406, 2407, 2408, 2409, 2410, 2411, 2412, 2413, 2414, 2415, 2416, 2417, 2418, 2419, 2420, 2421, 2422, 2423, 2424, 2425, 2426, 2427, 2428, 2429, 2430, 2431, 2432, 2433, 2434, 2435, 2436, 2437, 2438, 2439, 2440, 2441, 2442, 2443, 2444, 2445, 2446, 2447, 2448, 2449, 2450, 2451, 2452, 2453, 2454, 2455, 2456, 2457, 2458, 2459, 2460, 2461, 2462, 2463, 2464, 2465, 2466, 2467, 2468, 2469, 2470, 2471, 2472, 2473, 2474, 2475, 2476, 2477, 2478, 2479, 2480, 2481, 2482, 2483, 2484, 2485, 2486, 2487, 2488, 2489, 2490, 2491, 2492, 2493, 2494, 2495, 2496, 2497, 2498, 2499, 2500, 2501, 2502, 2503, 2504, 2505, 2506, 2507, 2508, 2509, 2510, 2511, 2512, 2513, 2514, 2515, 2516, 2517, 2518, 2519, 2520, 2521, 2522, 2523, 2524, 2525, 2526, 2527, 2528, 2529, 2530, 2531, 2532, 2533, 2534, 2535, 2536, 2537, 2538, 2539, 2540, 2541, 2542, 2543, 2544, 2545, 2546, 2547, 2548, 2549, 2550, 2551, 2552, 2553, 2554, 2555, 2556, 2557, 2558, 2559, 2560, 2561, 2562, 2563, 2564, 2565, 2566, 2567, 2568, 2569, 2570, 2571, 2572, 2573, 2574, 2575, 2576, 2577, 2578, 2579, 2580, 2581, 2582, 2583, 2584, 2585, 2586, 2587, 2588, 2589, 2590, 2591, 2592, 2593, 2594, 2595, 2596, 2597, 2598, 2599, 2600, 2601, 2602, 2603, 2604, 2605, 2606, 2607, 2608, 2609, 2610, 2611, 2612, 2613, 2614, 2615, 2616, 2617, 2618, 2619, 2620, 2621, 2622, 2623, 2624, 2625, 2626, 2627, 2628, 2629, 2630, 2631, 2632, 2633, 2634, 2635, 2636, 2637, 2638, 2639, 2640, 2641, 2642, 2643, 2644, 2645, 2646, 2647, 2648, 2649, 2650, 2651, 2652, 2653, 2654, 2655, 2656, 2657, 2658, 2659, 2660, 2661, 2662, 2663, 2664, 2665, 2666, 2667, 2668, 2669, 2670, 2671, 2672, 2673, 2674, 2675, 2676, 2677, 2678, 2679, 2680, 2681, 2682, 2683, 2684, 2685, 2686, 2687, 2688, 2689, 2690, 2691, 2692, 2693, 2694, 2695, 2696, 2697, 2698, 2699, 2700, 2701, 2702, 2703, 2704, 2705, 2706, 2707, 2708, 2709, 2710, 2711, 2712, 2713, 2714, 2715, 2716, 2717, 2718, 2719, 2720, 2721, 2722, 2723, 2724, 2725, 2726, 2727, 2728, 2729, 2730, 2731, 2732, 2733, 2734, 2735, 2736, 2737, 2738, 2739, 2740, 2741, 2742, 2743, 2744, 2745, 2746, 2747, 2748, 2749, 2750, 2751, 2752, 2753, 2754, 2755, 2756, 2757, 2758, 2759, 2760, 2761, 2762, 2763, 2764, 2765, 2766, 2767, 2768, 2769, 2770, 2771, 2772, 2773, 2774, 2775, 2776, 2777, 2778, 2779, 2780, 2781, 2782, 2783, 2784, 2785, 2786, 2787, 2788, 2789, 2790, 2791, 2792, 2793, 2794, 2795, 2796, 2797, 2798, 2799, 2800, 2801, 2802, 2803, 2804, 2805, 2806, 2807, 2808, 2809, 2810, 2811, 2812, 2813, 2814, 2815, 2816, 2817, 2818, 2819, 2820, 2821, 2822, 2823, 2824, 2825, 2826, 2827, 2828, 2829, 2830, 2831, 2832, 2833, 2834, 2835, 2836, 2837, 2838, 2839, 2840, 2841, 2842, 2843, 2844, 2845, 2846, 2847, 2848, 2849, 2850, 2851, 2852, 2853, 2854, 2855, 2856, 2857, 2858, 2859, 2860, 2861, 2862, 2863, 2864, 2865, 2866, 2867, 2868, 2869, 2870, 2871, 2872, 2873, 2874, 2875, 2876, 2877, 2878, 2879, 2880, 2881, 2882, 2883, 2884, 2885, 2886, 2887, 2888, 2889, 2890, 2891, 2892, 2893, 2894, 2895, 2896, 2897, 2898, 2899, 2900, 2901, 2902, 2903, 2904, 2905, 2906, 2907, 2908, 2909, 2910, 2911, 2912, 2913, 2914, 2915, 2916, 2917, 2918, 2919, 2920, 2921, 2922, 2923, 2924, 2925, 2926, 2927, 2928, 2929, 2930, 2931, 2932, 2933, 2934, 2935, 2936, 2937, 2938, 2939, 2940, 2941, 2942, 2943, 2944, 2945, 2946, 2947, 2948, 2949, 2950, 2951, 2952, 2953, 2954, 2955, 2956, 2957, 2958, 2959, 2960, 2961, 2962, 2963, 2964, 2965, 2966, 2967, 2968, 2969, 2970, 2971, 2972, 2973, 2974, 2975, 2976, 2977, 2978, 2979, 2980, 2981, 2982, 2983, 2984, 2985, 2986, 2987, 2988, 2989, 2990, 2991, 2992, 2993, 2994, 2995, 2996, 2997, 2998, 2999, 3000, 3001, 3002, 3003, 3004, 3005, 3006, 3007, 3008, 3009, 3010, 3011, 3012, 3013, 3014, 3015, 3016, 3017, 3018, 3019, 3020, 3021, 3022, 3023, 3024, 3025, 3026, 3027, 3028, 3029, 3030, 3031, 3032, 3033, 3034, 3035, 3036, 3037, 3038, 3039, 3040, 3041, 3042, 3043, 3044, 3045, 3046, 3047, 3048, 3049, 3050, 3051, 3052, 3053, 3054, 3055, 3056, 3057, 3058, 3059, 3060, 3061, 3062, 3063, 3064, 3065, 3066, 3067, 3068, 3069, 3070, 3071, 3072, 3073, 3074, 3075, 3076, 3077, 3078, 3079, 3080, 3081, 3082, 3083, 3084, 3085, 3086, 3087, 3088, 3089, 3090, 3091, 3092, 3093, 3094, 3095, 3096, 3097, 3098, 3099, 3100, 3101, 3102, 3103, 3104, 3105, 3106, 3107, 3108, 3109, 3110, 3111, 3112, 3113, 3114, 3115, 3116, 3117, 3118, 3119, 3120, 3121, 3122, 3123, 3124, 3125, 3126, 3127, 3128, 3129, 3130, 3131, 3132, 3133, 3134, 3135, 3136, 3137, 3138, 3139, 3140, 3141, 3142, 3143, 3144, 3145, 3146, 3147, 3148, 3149, 3150, 3151, 3152, 3153, 3154, 3155, 3156, 3157, 3158, 3159, 3160, 3161, 3162, 3163, 3164, 3165, 3166, 3167, 3168, 3169, 3170, 3171, 3172, 3173, 3174, 3175, 3176, 3177, 3178, 3179, 3180, 3181, 3182, 3183, 3184, 3185, 3186, 3187, 3188, 3189, 3190, 3191, 3192, 3193, 3194, 3195, 3196, 3197, 3198, 3199, 3200, 3201, 3202, 3203, 3204, 3205, 3206, 3207, 3208, 3209, 3210, 3211, 3212, 3213, 3214, 3215, 3216, 3217, 3218, 3219, 3220, 3221, 3222, 3223, 3224, 3225, 3226, 3227, 3228, 3229, 3230, 3231, 3232, 3233, 3234, 3235, 3236, 3237, 3238, 3239, 3240, 3241, 3242, 3243, 3244, 3245, 3246, 3247, 3248, 3249, 3250, 3251, 3252, 3253, 3254, 3255, 3256, 3257, 3258, 3259, 3260, 3261, 3262, 3263, 3264, 3265, 3266, 3267, 3268, 3269, 3270, 3271, 3272, 3273, 3274, 3275, 3276, 3277, 3278, 3279, 3280, 3281, 3282, 3283, 3284, 3285, 3286, 3287, 3288, 3289, 3290, 3291, 3292, 3293, 3294, 3295, 3296, 3297, 3298, 3299, 3300, 3301, 3302, 3303, 3304, 3305, 3306, 3307, 3308, 3309, 3310, 3311, 3312, 3313, 3314, 3315, 3316, 3317, 3318, 3319, 3320, 3321, 3322, 3323, 3324, 3325, 3326, 3327, 3328, 3329, 3330, 3331, 3332, 3333, 3334, 3335, 3336, 3337, 3338, 3339, 3340, 3341, 3342, 3343, 3344, 3345, 3346, 3347, 3348, 3349, 3350, 3351, 3352, 3353, 3354, 3355, 3356, 3357, 3358, 3359, 3360, 3361, 3362, 3363, 3364, 3365, 3366, 3367, 3368, 3369, 3370, 3371, 3372, 3373, 3374, 3375, 3376, 3377, 3378, 3379, 3380, 3381, 3382, 3383, 3384, 3385, 3386, 3387, 3388, 3389, 3390, 3391, 3392, 3393, 3394, 3395, 3396, 3397, 3398, 3399, 3400, 3401, 3402, 3403, 3404, 3405, 3406, 3407, 3408, 3409, 3410, 3411, 3412, 3413, 3414, 3415, 3416, 3417, 3418, 3419, 3420, 3421, 3422, 3423, 3424, 3425, 3426, 3427, 3428, 3429, 3430, 3431, 3432, 3433, 3434, 3435, 3436, 3437, 3438, 3439, 3440, 3441, 3442, 3443, 3444, 3445, 3446, 3447, 3448, 3449, 3450, 3451, 3452, 3453, 3454, 3455, 3456, 3457, 3458, 3459, 3460, 3461, 3462, 3463, 3464, 3465, 3466, 3467, 3468, 3469, 3470, 3471, 3472, 3473, 3474, 3475, 3476, 3477, 3478, 3479, 3480, 3481, 3482, 3483, 3484, 3485, 3486, 3487, 3488, 3489, 3490, 3491, 3492, 3493, 3494, 3495, 3496, 3497, 3498, 3499, 3500, 3501, 3502, 3503, 3504, 3505, 3506, 3507, 3508, 3509, 3510, 3511, 3512, 3513, 3514, 3515, 3516, 3517, 3518, 3519, 3520, 3521, 3522, 3523, 3524, 3525, 3526, 3527, 3528, 3529, 3530, 3531, 3532, 3533, 3534, 3535, 3536, 3537, 3538, 3539, 3540, 3541, 3542, 3543, 3544, 3545, 3546, 3547, 3548, 3549, 3550, 3551, 3552, 3553, 3554, 3555, 3556, 3557, 3558, 3559, 3560, 3561, 3562, 3563, 3564, 3565, 3566, 3567, 3568, 3569, 3570, 3571, 3572, 3573, 3574, 3575, 3576, 3577, 3578, 3579, 3580, 3581, 3582, 3583, 3584, 3585, 3586, 3587, 3588, 3589, 3590, 3591, 3592, 3593, 3594, 3595, 3596, 3597, 3598, 3599, 3600, 3601, 3602, 3603, 3604, 3605, 3606, 3607, 3608, 3609, 3610, 3611, 3612, 3613, 3614, 3615, 3616, 3617, 3618, 3619, 3620, 3621, 3622, 3623, 3624, 3625, 3626, 3627, 3628, 3629, 3630, 3631, 3632, 3633, 3634, 3635, 3636, 3637, 3638, 3639, 3640, 3641, 3642, 3643, 3644, 3645, 3646, 3647, 3648, 3649, 3650, 3651, 3652, 3653, 3654, 3655, 3656, 3657, 3658, 3659, 3660, 3661, 3662, 3663, 3664, 3665, 3666, 3667, 3668, 3669, 3670, 3671, 3672, 3673, 3674, 3675, 3676, 3677, 3678, 3679, 3680, 3681, 3682, 3683, 3684, 3685, 3686, 3687, 3688, 3689, 3690, 3691, 3692, 3693, 3694, 3695, 3696, 3697, 3698, 3699, 3700, 3701, 3702, 3703, 3704, 3705, 3706, 3707, 3708, 3709, 3710, 3711, 3712, 3713, 3714, 3715, 3716, 3717, 3718, 3719, 3720, 3721, 3722, 3723, 3724, 3725, 3726, 3727, 3728, 3729, 3730, 3731, 3732, 3733, 3734, 3735, 3736, 3737, 3738, 3739, 3740, 3741, 3742, 3743, 3744, 3745, 3746, 3747, 3748, 3749, 3750, 3751, 3752, 3753, 3754, 3755, 3756, 3757, 3758, 3759, 3760, 3761, 3762, 3763, 3764, 3765, 3766, 3767, 3768, 3769, 3770, 3771, 3772, 3773, 3774, 3775, 3776, 3777, 3778, 3779, 3780, 3781, 3782, 3783, 3784, 3785, 3786, 3787, 3788, 3789, 3790, 3791, 3792, 3793, 3794, 3795, 3796, 3797, 3798, 3799, 3800, 3801, 3802, 3803, 3804, 3805, 3806, 3807, 3808, 3809, 3810, 3811, 3812, 3813, 3814, 3815, 3816, 3817, 3818, 3819, 3820, 3821, 3822, 3823, 3824, 3825, 3826, 3827, 3828, 3829, 3830, 3831, 3832, 3833, 3834, 3835, 3836, 3837, 3838, 3839, 3840, 3841, 3842, 3843, 3844, 3845, 3846, 3847, 3848, 3849, 3850, 3851, 3852, 3853, 3854, 3855, 3856, 3857, 3858, 3859, 3860, 3861, 3862, 3863, 3864, 3865, 3866, 3867, 3868, 3869, 3870, 3871, 3872, 3873, 3874, 3875, 3876, 3877, 3878, 3879, 3880, 3881, 3882, 3883, 3884, 3885, 3886, 3887, 3888, 3889, 3890, 3891, 3892, 3893, 3894, 3895, 3896, 3897, 3898, 3899, 3900, 3901, 3902, 3903, 3904, 3905, 3906, 3907, 3908, 3909, 3910, 3911, 3912, 3913, 3914, 3915, 3916, 3917, 3918, 3919, 3920, 3921, 3922, 3923, 3924, 3925, 3926, 3927, 3928, 3929, 3930, 3931, 3932, 3933, 3934, 3935, 3936, 3937, 3938, 3939, 3940, 3941, 3942, 3943, 3944, 3945, 3946, 3947, 3948, 3949, 3950, 3951, 3952, 3953, 3954, 3955, 3956, 3957, 3958, 3959, 3960, 3961, 3962, 3963, 3964, 3965, 3966, 3967, 3968, 3969, 3970, 3971, 3972, 3973, 3974, 3975, 3976, 3977, 3978, 3979, 3980, 3981, 3982, 3983, 3984, 3985, 3986, 3987, 3988, 3989, 3990, 3991, 3992, 3993, 3994, 3995, 3996, 3997, 3998, 3999, 4000, 4001, 4002, 4003, 4004, 4005, 4006, 4007, 4008, 4009, 4010, 4011, 4012, 4013, 4014, 4015, 4016, 4017, 4018, 4019, 4020, 4021, 4022, 4023, 4024, 4025, 4026, 4027, 4028, 4029, 4030, 4031, 4032, 4033, 4034, 4035, 4036, 4037, 4038, 4039, 4040, 4041, 4042, 4043, 4044, 4045, 4046, 4047, 4048, 4049, 4050, 4051, 4052, 4053, 4054, 4055, 4056, 4057, 4058, 4059, 4060, 4061, 4062, 4063, 4064, 4065, 4066, 4067, 4068, 4069, 4070, 4071, 4072, 4073, 4074, 4075, 4076, 4077, 4078, 4079, 4080, 4081, 4082, 4083, 4084, 4085, 4086, 4087, 4088, 4089, 4090, 4091, 4092, 4093, 4094, 4095, 4096, 4097, 4098, 4099, 4100, 4101, 4102, 4103, 4104, 4105, 4106, 4107, 4108, 4109, 4110, 4111, 4112, 4113, 4114, 4115, 4116, 4117, 4118, 4119, 4120, 4121, 4122, 4123, 4124, 4125, 4126, 4127, 4128, 4129, 4130, 4131, 4132, 4133, 4134, 4135, 4136, 4137, 4138, 4139, 4140, 4141, 4142, 4143, 4144, 4145, 4146, 4147, 4148, 4149, 4150, 4151, 4152, 4153, 4154, 4155, 4156, 4157, 4158, 4159, 4160, 4161, 4162, 4163, 4164, 4165, 4166, 4167, 4168, 4169, 4170, 4171, 4172, 4173, 4174, 4175, 4176, 4177, 4178, 4179, 4180, 4181, 4182, 4183, 4184, 4185, 4186, 4187, 4188, 4189, 4190, 4191, 4192, 4193, 4194, 4195, 4196, 4197, 4198, 4199, 4200, 4201, 4202, 4203, 4204, 4205, 4206, 4207, 4208, 4209, 4210, 4211, 4212, 4213, 4214, 4215, 4216, 4217, 4218, 4219, 4220, 4221, 4222, 4223, 4224, 4225, 4226, 4227, 4228, 4229, 4230, 4231, 4232, 4233, 4234, 4235, 4236, 4237, 4238, 4239, 4240, 4241, 4242, 4243, 4244, 4245, 4246, 4247, 4248, 4249, 4250, 4251, 4252, 4253, 4254, 4255, 4256, 4257, 4258, 4259, 4260, 4261, 4262, 4263, 4264, 4265, 4266, 4267, 4268, 4269, 4270, 4271, 4272, 4273, 4274, 4275, 4276, 4277, 4278, 4279, 4280, 4281, 4282, 4283, 4284, 4285, 4286, 4287, 4288, 4289, 4290, 4291, 4292, 4293, 4294, 4295, 4296, 4297, 4298, 4299, 4300, 4301, 4302, 4303, 4304, 4305, 4306, 4307, 4308, 4309, 4310, 4311, 4312, 4313, 4314, 4315, 4316, 4317, 4318, 4319, 4320, 4321, 4322, 4323, 4324, 4325, 4326, 4327, 4328, 4329, 4330, 4331, 4332, 4333, 4334, 4335, 4336, 4337, 4338, 4339, 4340, 4341, 4342, 4343, 4344, 4345, 4346, 4347, 4348, 4349, 4350, 4351, 4352, 4353, 4354, 4355, 4356, 4357, 4358, 4359, 4360, 4361, 4362, 4363, 4364, 4365, 4366, 4367, 4368, 4369, 4370, 4371, 4372, 4373, 4374, 4375, 4376, 4377, 4378, 4379, 4380, 4381, 4382, 4383, 4384, 4385, 4386, 4387, 4388, 4389, 4390, 4391, 4392, 4393, 4394, 4395, 4396, 4397, 4398, 4399, 4400, 4401, 4402, 4403, 4404, 4405, 4406, 4407, 4408, 4409, 4410, 4411, 4412, 4413, 4414, 4415, 4416, 4417, 4418, 4419, 4420, 4421, 4422, 4423, 4424, 4425, 4426, 4427, 4428, 4429, 4430, 4431, 4432, 4433, 4434, 4435, 4436, 4437, 4438, 4439, 4440, 4441, 4442, 4443, 4444, 4445, 4446, 4447, 4448, 4449, 4450, 4451, 4452, 4453, 4454, 4455, 4456, 4457, 4458, 4459, 4460, 4461, 4462, 4463, 4464, 4465, 4466, 4467, 4468, 4469, 4470, 4471, 4472, 4473, 4474, 4475, 4476, 4477, 4478, 4479, 4480, 4481, 4482, 4483, 4484, 4485, 4486, 4487, 4488, 4489, 4490, 4491, 4492, 4493, 4494, 4495, 4496, 4497, 4498, 4499, 4500, 4501, 4502, 4503, 4504, 4505, 4506, 4507, 4508, 4509, 4510, 4511, 4512, 4513, 4514, 4515, 4516, 4517, 4518, 4519, 4520, 4521, 4522, 4523, 4524, 4525, 4526, 4527, 4528, 4529, 4530, 4531, 4532, 4533, 4534, 4535, 4536, 4537, 4538, 4539, 4540, 4541, 4542, 4543, 4544, 4545, 4546, 4547, 4548, 4549, 4550, 4551, 4552, 4553, 4554, 4555, 4556, 4557, 4558, 4559, 4560, 4561, 4562, 4563, 4564, 4565, 4566, 4567, 4568, 4569, 4570, 4571, 4572, 4573, 4574, 4575, 4576, 4577, 4578, 4579, 4580, 4581, 4582, 4583, 4584, 4585, 4586, 4587, 4588, 4589, 4590, 4591, 4592, 4593, 4594, 4595, 4596, 4597, 4598, 4599, 4600, 4601, 4602, 4603, 4604, 4605, 4606, 4607, 4608, 4609, 4610, 4611, 4612, 4613, 4614, 4615, 4616, 4617, 4618, 4619, 4620, 4621, 4622, 4623, 4624, 4625, 4626, 4627, 4628, 4629, 4630, 4631, 4632, 4633, 4634, 4635, 4636, 4637, 4638, 4639, 4640, 4641, 4642, 4643, 4644, 4645, 4646, 4647, 4648, 4649, 4650, 4651, 4652, 4653, 4654, 4655, 4656, 4657, 4658, 4659, 4660, 4661, 4662, 4663, 4664, 4665, 4666, 4667, 4668, 4669, 4670, 4671, 4672, 4673, 4674, 4675, 4676, 4677, 4678, 4679, 4680, 4681, 4682, 4683, 4684, 4685, 4686, 4687, 4688, 4689, 4690, 4691, 4692, 4693, 4694, 4695, 4696, 4697, 4698, 4699, 4700, 4701, 4702, 4703, 4704, 4705, 4706, 4707, 4708, 4709, 4710, 4711, 4712, 4713, 4714, 4715, 4716, 4717, 4718, 4719, 4720, 4721, 4722, 4723, 4724, 4725, 4726, 4727, 4728, 4729, 4730, 4731, 4732, 4733, 4734, 4735, 4736, 4737, 4738, 4739, 4740, 4741, 4742, 4743, 4744, 4745, 4746, 4747, 4748, 4749, 4750, 4751, 4752, 4753, 4754, 4755, 4756, 4757, 4758, 4759, 4760, 4761, 4762, 4763, 4764, 4765, 4766, 4767, 4768, 4769, 4770, 4771, 4772, 4773, 4774, 4775, 4776, 4777, 4778, 4779, 4780, 4781, 4782, 4783, 4784, 4785, 4786, 4787, 4788, 4789, 4790, 4791, 4792, 4793, 4794, 4795, 4796, 4797, 4798, 4799, 4800, 4801, 4802, 4803, 4804, 4805, 4806, 4807, 4808, 4809, 4810, 4811, 4812, 4813, 4814, 4815, 4816, 4817, 4818, 4819, 4820, 4821, 4822, 4823, 4824, 4825, 4826, 4827, 4828, 4829, 4830, 4831, 4832, 4833, 4834, 4835, 4836, 4837, 4838, 4839, 4840, 4841, 4842, 4843, 4844, 4845, 4846, 4847, 4848, 4849, 4850, 4851, 4852, 4853, 4854, 4855, 4856, 4857, 4858, 4859, 4860, 4861, 4862, 4863, 4864, 4865, 4866, 4867, 4868, 4869, 4870, 4871, 4872, 4873, 4874, 4875, 4876, 4877, 4878, 4879, 4880, 4881, 4882, 4883, 4884, 4885, 4886, 4887, 4888, 4889, 4890, 4891, 4892, 4893, 4894, 4895, 4896, 4897, 4898, 4899, 4900, 4901, 4902, 4903, 4904, 4905, 4906, 4907, 4908, 4909, 4910, 4911, 4912, 4913, 4914, 4915, 4916, 4917, 4918, 4919, 4920, 4921, 4922, 4923, 4924, 4925, 4926, 4927, 4928, 4929, 4930, 4931, 4932, 4933, 4934, 4935, 4936, 4937, 4938, 4939, 4940, 4941, 4942, 4943, 4944, 4945, 4946, 4947, 4948, 4949, 4950, 4951, 4952, 4953, 4954, 4955, 4956, 4957, 4958, 4959, 4960, 4961, 4962, 4963, 4964, 4965, 4966, 4967, 4968, 4969, 4970, 4971, 4972, 4973, 4974, 4975, 4976, 4977, 4978, 4979, 4980, 4981, 4982, 4983, 4984, 4985, 4986, 4987, 4988, 4989, 4990, 4991, 4992, 4993, 4994, 4995, 4996, 4997, 4998, 4999, 5000, 5001, 5002, 5003, 5004, 5005, 5006, 5007, 5008, 5009, 5010, 5011, 5012, 5013, 5014, 5015, 5016, 5017, 5018, 5019, 5020, 5021, 5022, 5023, 5024, 5025, 5026, 5027, 5028, 5029, 5030, 5031, 5032, 5033, 5034, 5035, 5036, 5037, 5038, 5039, 5040, 5041, 5042, 5043, 5044, 5045, 5046, 5047, 5048, 5049, 5050, 5051, 5052, 5053, 5054, 5055, 5056, 5057, 5058, 5059, 5060, 5061, 5062, 5063, 5064, 5065, 5066, 5067, 5068, 5069, 5070, 5071, 5072, 5073, 5074, 5075, 5076, 5077, 5078, 5079, 5080, 5081, 5082, 5083, 5084, 5085, 5086, 5087, 5088, 5089, 5090, 5091, 5092, 5093, 5094, 5095, 5096, 5097, 5098, 5099, 5100, 5101, 5102, 5103, 5104, 5105, 5106, 5107, 5108, 5109, 5110, 5111, 5112, 5113, 5114, 5115, 5116, 5117, 5118, 5119, 5120, 5121, 5122, 5123, 5124, 5125, 5126, 5127, 5128, 5129, 5130, 5131, 5132, 5133, 5134, 5135, 5136, 5137, 5138, 5139, 5140, 5141, 5142, 5143, 5144, 5145, 5146, 5147, 5148, 5149, 5150, 5151, 5152, 5153, 5154, 5155, 5156, 5157, 5158, 5159, 5160, 5161, 5162, 5163, 5164, 5165, 5166, 5167, 5168, 5169, 5170, 5171, 5172, 5173, 5174, 5175, 5176, 5177, 5178, 5179, 5180, 5181, 5182, 5183, 5184, 5185, 5186, 5187, 5188, 5189, 5190, 5191, 5192, 5193, 5194, 5195, 5196, 5197, 5198, 5199, 5200, 5201, 5202, 5203, 5204, 5205, 5206, 5207, 5208, 5209, 5210, 5211, 5212, 5213, 5214, 5215, 5216, 5217, 5218, 5219, 5220, 5221, 5222, 5223, 5224, 5225, 5226, 5227, 5228, 5229, 5230, 5231, 5232, 5233, 5234, 5235, 5236, 5237, 5238, 5239, 5240, 5241, 5242, 5243, 5244, 5245, 5246, 5247, 5248, 5249, 5250, 5251, 5252, 5253, 5254, 5255, 5256, 5257, 5258, 5259, 5260, 5261, 5262, 5263, 5264, 5265, 5266, 5267, 5268, 5269, 5270, 5271, 5272, 5273, 5274, 5275, 5276, 5277, 5278, 5279, 5280, 5281, 5282, 5283, 5284, 5285, 5286, 5287, 5288, 5289, 5290, 5291, 5292, 5293, 5294, 5295, 5296, 5297, 5298, 5299, 5300, 5301, 5302, 5303, 5304, 5305, 5306, 5307, 5308, 5309, 5310, 5311, 5312, 5313, 5314, 5315, 5316, 5317, 5318, 5319, 5320, 5321, 5322, 5323, 5324, 5325, 5326, 5327, 5328, 5329, 5330, 5331, 5332, 5333, 5334, 5335, 5336, 5337, 5338, 5339, 5340, 5341, 5342, 5343, 5344, 5345, 5346, 5347, 5348, 5349, 5350, 5351, 5352, 5353, 5354, 5355, 5356, 5357, 5358, 5359, 5360, 5361, 5362, 5363, 5364, 5365, 5366, 5367, 5368, 5369, 5370, 5371, 5372, 5373, 5374, 5375, 5376, 5377, 5378, 5379, 5380, 5381, 5382, 5383, 5384, 5385, 5386, 5387, 5388, 5389, 5390, 5391, 5392, 5393, 5394, 5395, 5396, 5397, 5398, 5399, 5400, 5401, 5402, 5403, 5404, 5405, 5406, 5407, 5408, 5409, 5410, 5411, 5412, 5413, 5414, 5415, 5416, 5417, 5418, 5419, 5420, 5421, 5422, 5423, 5424, 5425, 5426, 5427, 5428, 5429, 5430, 5431, 5432, 5433, 5434, 5435, 5436, 5437, 5438, 5439, 5440, 5441, 5442, 5443, 5444, 5445, 5446, 5447, 5448, 5449, 5450, 5451, 5452, 5453, 5454, 5455, 5456, 5457, 5458, 5459, 5460, 5461, 5462, 5463, 5464, 5465, 5466, 5467, 5468, 5469, 5470, 5471, 5472, 5473, 5474, 5475, 5476, 5477, 5478, 5479, 5480, 5481, 5482, 5483, 5484, 5485, 5486, 5487, 5488, 5489, 5490, 5491, 5492, 5493, 5494, 5495, 5496, 5497, 5498, 5499, 5500, 5501, 5502, 5503, 5504, 5505, 5506, 5507, 5508, 5509, 5510, 5511, 5512, 5513, 5514, 5515, 5516, 5517, 5518, 5519, 5520, 5521, 5522, 5523, 5524, 5525, 5526, 5527, 5528, 5529, 5530, 5531, 5532, 5533, 5534, 5535, 5536, 5537, 5538, 5539, 5540, 5541, 5542, 5543, 5544, 5545, 5546, 5547, 5548, 5549, 5550, 5551, 5552, 5553, 5554, 5555, 5556, 5557, 5558, 5559, 5560, 5561, 5562, 5563, 5564, 5565, 5566, 5567, 5568, 5569, 5570, 5571, 5572, 5573, 5574, 5575, 5576, 5577, 5578, 5579, 5580, 5581, 5582, 5583, 5584, 5585, 5586, 5587, 5588, 5589, 5590, 5591, 5592, 5593, 5594, 5595, 5596, 5597, 5598, 5599, 5600, 5601, 5602, 5603, 5604, 5605, 5606, 5607, 5608, 5609, 5610, 5611, 5612, 5613, 5614, 5615, 5616, 5617, 5618, 5619, 5620, 5621, 5622, 5623, 5624, 5625, 5626, 5627, 5628, 5629, 5630, 5631, 5632, 5633, 5634, 5635, 5636, 5637, 5638, 5639, 5640, 5641, 5642, 5643, 5644, 5645, </t>
         </is>
       </c>
-      <c r="BP6" t="n">
+      <c r="BV6" t="n">
         <v>0.1814977973568282</v>
       </c>
-      <c r="BQ6" t="inlineStr">
+      <c r="BW6" t="inlineStr">
         <is>
           <t>{'Numk': 35, 'KPar': 28, 'Bucket_index': 1000}</t>
         </is>
       </c>
-      <c r="BR6" t="n">
+      <c r="BX6" t="n">
         <v>376.6167106030043</v>
       </c>
-      <c r="BS6" t="inlineStr">
+      <c r="BY6" t="inlineStr">
         <is>
           <t>no</t>
         </is>
       </c>
-      <c r="BT6" t="n">
-        <v>0</v>
-      </c>
-      <c r="BU6" t="inlineStr">
+      <c r="BZ6" t="n">
+        <v>0</v>
+      </c>
+      <c r="CA6" t="inlineStr">
         <is>
           <t>params</t>
         </is>
       </c>
-      <c r="BV6" t="n">
+      <c r="CB6" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2174,93 +2294,111 @@
       <c r="AY7" t="n">
         <v>5</v>
       </c>
-      <c r="AZ7" t="inlineStr"/>
-      <c r="BA7" t="inlineStr">
+      <c r="AZ7" t="n">
+        <v>5</v>
+      </c>
+      <c r="BA7" t="n">
+        <v>5</v>
+      </c>
+      <c r="BB7" t="n">
+        <v>5</v>
+      </c>
+      <c r="BC7" t="n">
+        <v>5</v>
+      </c>
+      <c r="BD7" t="n">
+        <v>5</v>
+      </c>
+      <c r="BE7" t="n">
+        <v>5</v>
+      </c>
+      <c r="BF7" t="inlineStr"/>
+      <c r="BG7" t="inlineStr">
         <is>
           <t>nab-data/realKnownCause/rogue_agent_key_hold.csv</t>
         </is>
       </c>
-      <c r="BB7" t="n">
+      <c r="BH7" t="n">
         <v>1882</v>
       </c>
-      <c r="BC7" t="inlineStr">
+      <c r="BI7" t="inlineStr">
         <is>
           <t>NAB</t>
         </is>
       </c>
-      <c r="BD7" t="n">
-        <v>2</v>
-      </c>
-      <c r="BE7" t="inlineStr">
+      <c r="BJ7" t="n">
+        <v>2</v>
+      </c>
+      <c r="BK7" t="inlineStr">
         <is>
           <t>669; 1240</t>
         </is>
       </c>
-      <c r="BF7" t="n">
+      <c r="BL7" t="n">
         <v>94</v>
       </c>
-      <c r="BG7" t="inlineStr">
-        <is>
-          <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86, 87, 88, 89, 90, 91, 92, 93, 94, 95, 96, 97, 98, 99, 100, 101, 102, 103, 104, 105, 106, 107, 108, 109, 110, 111, 112, 113, 114, 115, 116, 117, 118, 119, 120, 121, 122, 123, 124, 125, 126, 127, 128, 129, 130, 131, 132, 133, 134, 135, 136, 137, 138, 139, 140, 141, 142, 143, 144, 145, 146, 147, 148, 149, 150, 151, 152, 153, 154, 155, 156, 157, 158, 159, 160, 161, 162, 163, 164, 165, 166, 167, 168, 169, 170, 171, 172, 173, 174, 175, 176, 177, 178, 179, 180, 181, 182, 183, 184, 185, 186, 187, 188, 189, 190, 191, 192, 193, 194, 195, 196, 197, 198, 199, 200, 201, 202, 203, 204, 205, 206, 207, 208, 209, 210, 211, 212, 213, 214, 215, 216, 217, 218, 219, 220, 221, 222, 223, 224, 225, 226, 227, 228, 229, 230, 231, 232, 233, 234, 235, 236, 237, 238, 239, 240, 241, 242, 243, 244, 245, 246, 247, 248, 249, 250, 251, 252, 253, 254, 255, 256, 257, 258, 259, 260, 261, 262, 263, 264, 265, 266, 267, 268, 269, 270, 271, 272, 273, 274, 275, 276, 277, 278, 279, 280, 281, 282, 283, 284, 285, 286, 287, 288, 289, 290, 291, 292, 293, 294, 295, 296, 297, 298, 299, 300, 301, 302, 303, 304, 305, 306, 307, 308, 309, 310, 311, 312, 313, 314, 315, 316, 317, 318, 319, 320, 321, 322, 323, 324, 325, 326, 327, 328, 329, 330, 331, 332, 333, 334, 335, 336, 337, 338, 339, 340, 341, 342, 343, 344, 345, 346, 347, 348, 349, 350, 351, 352, 353, 354, 355, 356, 357, 358, 359, 360, 361, 362, 363, 364, 365, 366, 367, 368, 369, 370, 371, 372, 373, 374, 375, 376, 377, 378, 379, 380, 381, 382, 383, 384, 385, 386, 387, 388, 389, 390, 391, 392, 393, 394, 395, 396, 397, 398, 399, 400, 401, 402, 403, 404, 405, 406, 407, 408, 409, 410, 411, 412, 413, 414, 415, 416, 417, 418, 419, 420, 421, 422, 423, 424, 425, 426, 427, 428, 429, 430, 431, 432, 433, 434, 435, 436, 437, 438, 439, 440, 441, 442, 443, 444, 445, 446, 447, 448, 449, 450, 451, 452, 453, 454, 455, 456, 457, 458, 459, 460, 461, 462, 463, 464, 465, 466, 467, 468, 469, 470, 471, 472, 473, 474, 475, 476, 477, 478, 479, 480, 481, 482, 483, 484, 485, 486, 487, 488, 489, 490, 491, 492, 493, 494, 495, 496, 497, 498, 499, 500, 501, 502, 503, 504, 505, 506, 507, 508, 509, 510, 511, 512, 513, 514, 515, 516, 517, 518, 519, 520, 521, 522, 523, 524, 525, 526, 527, 528, 529, 530, 531, 532, 533, 534, 535, 536, 537, 538, 539, 540, 541, 542, 543, 544, 545, 546, 547, 548, 549, 550, 551, 552, 553, 554, 555, 556, 557, 558, 559, 560, 561, 562, 563, 564, 565, 566, 567, 568, 569, 570, 571, 572, 573, 574, 575, 576, 577, 578, 579, 580, 581, 582, 583, 584, 585, 586, 587, 588, 589, 590, 591, 592, 593, 594, 595, 596, 597, 598, 599, 600, 601, 602, 603, 604, 605, 606, 607, 608, 609, 610, 611, 612, 613, 614, 615, 616, 617, 618, 619, 620, 621, 622, 623, 624, 625, 626, 627, 628, 629, 630, 631, 632, 633, 634, 635, 636, 637, 638, 639, 640, 641, 642, 643, 644, 645, 646, 647, 648, 649, 650, 651, 652, 653, 654, 655, 656, 657, 658, 659, 660, 661, 662, 663, 664, 665, 666, 667, 668, 669, 670, 671, 672, 673, 674, 675, 676, 677, 678, 679, 680, 681, 682, 683, 684, 685, 686, 687, 688, 689, 690, 691, 692, 693, 694, 695, 696, 697, 698, 699, 700, 701, 702, 703, 704, 705, 706, 707, 708, 709, 710, 711, 712, 713, 714, 715, 716, 717, 718, 719, 720, 721, 722, 723, 724, 725, 726, 727, 728, 729, 730, 731, 732, 733, 734, 735, 736, 737, 738, 739, 740, 741, 742, 743, 744, 745, 746, 747, 748, 749, 750, 751, 752, 753, 754, 755, 756, 757, 758, 759, 760, 761, 762, 763, 764, 765, 766, 767, 768, 769, 770, 771, 772, 773, 774, 775, 776, 777, 778, 779, 780, 781, 782, 783, 784, 785, 786, 787, 788, 789, 790, 791, 792, 793, 794, 795, 796, 797, 798, 799, 800, 801, 802, 803, 804, 805, 806, 807, 808, 809, 810, 811, 812, 813, 814, 815, 816, 817, 818, 819, 820, 821, 822, 823, 824, 825, 826, 827, 828, 829, 830, 831, 832, 833, 834, 835, 836, 837, 838, 839, 840, 841, 842, 843, 844, 845, 846, 847, 848, 849, 850, 851, 852, 853, 854, 855, 856, 857, 858, 859, 860, 861, 862, 863, 864, 865, 866, 867, 868, 869, 870, 871, 872, 873, 874, 875, 876, 877, 878, 879, 880, 881, 882, 883, 884, 885, 886, 887, 888, 889, 890, 891, 892, 893, 894, 895, 896, 897, 898, 899, 900, 901, 902, 903, 904, 905, 906, 907, 908, 909, 910, 911, 912, 913, 914, 915, 916, 917, 918, 919, 920, 921, 922, 923, 924, 925, 926, 927, 928, 929, 930, 931, 932, 933, 934, 935, 936, 937, 938, 939, 940, 941, 942, 943, 944, 945, 946, 947, 948, 949, 950, 951, 952, 953, 954, 955, 956, 957, 958, 959, 960, 961, 962, 963, 964, 965, 966, 967, 968, 969, 970, 971, 972, 973, 974, 975, 976, 977, 978, 979, 980, 981, 982, 983, 984, 985, 986, 987, 988, 989, 990, 991, 992, 993, 994, 995, 996, 997, 998, 999, 1000, 1001, 1002, 1003, 1004, 1005, 1006, 1007, 1008, 1009, 1010, 1011, 1012, 1013, 1014, 1015, 1016, 1017, 1018, 1019, 1020, 1021, 1022, 1023, 1024, 1025, 1026, 1027, 1028, 1029, 1030, 1031, 1032, 1033, 1034, 1035, 1036, 1037, 1038, 1039, 1040, 1041, 1042, 1043, 1044, 1045, 1046, 1047, 1048, 1049, 1050, 1051, 1052, 1053, 1054, 1055, 1056, 1057, 1058, 1059, 1060, 1061, 1062, 1063, 1064, 1065, 1066, 1067, 1068, 1069, 1070, 1071, 1072, 1073, 1074, 1075, 1076, 1077, 1078, 1079, 1080, 1081, 1082, 1083, 1084, 1085, 1086, 1087, 1088, 1089, 1090, 1091, 1092, 1093, 1094, 1095, 1096, 1097, 1098, 1099, 1100, 1101, 1102, 1103, 1104, 1105, 1106, 1107, 1108, 1109, 1110, 1111, 1112, 1113, 1114, 1115, 1116, 1117, 1118, 1119, 1120, 1121, 1122, 1123, 1124, 1125, 1126, 1127, 1128, 1129, 1130, 1131, 1132, 1133, 1134, 1135, 1136, 1137, 1138, 1139, 1140, 1141, 1142, 1143, 1144, 1145, 1146, 1147, 1148, 1149, 1150, 1151, 1152, 1153, 1154, 1155, 1156, 1157, 1158, 1159, 1160, 1161, 1162, 1163, 1164, 1165, 1166, 1167, 1168, 1169, 1170, 1171, 1172, 1173, 1174, 1175, 1176, 1177, 1178, 1179, 1180, 1181, 1182, 1183, 1184, 1185, 1186, 1187, 1188, 1189, 1190, 1191, 1192, 1193, 1194, 1195, 1196, 1197, 1198, 1199, 1200, 1201, 1202, 1203, 1204, 1205, 1206, 1207, 1208, 1209, 1210, 1211, 1212, 1213, 1214, 1215, 1216, 1217, 1218, 1219, 1220, 1221, 1222, 1223, 1224, 1225, 1226, 1227, 1228, 1229, 1230, 1231, 1232, 1233, 1234, 1235, 1236, 1237, 1238, 1239, 1240, 1241, 1242, 1243, 1244, 1245, 1246, 1247, 1248, 1249, 1250, 1251, 1252, 1253, 1254, 1255, 1256, 1257, 1258, 1272, 1273, 1303, 1313, 1314, 1317, 1318, 1319, 1320, 1321, 1322, 1323, 1324, 1325, 1326, 1327, 1328, 1329, 1330, 1336, 1337, 1343, 1344, 1345, 1386, 1387, 1388, 1389, 1390, 1391, 1392, 1393, 1394, 1395, 1396, 1397, 1398, 1399, 1400, 1401, 1402, 1403, 1404, 1405, 1406, 1407, 1408, 1409, 1410, 1411, 1412, 1413, 1414, 1415, 1416, 1417, 1418, 1419, 1420, 1421, 1422, 1423, 1424, 1425, 1426, 1427, 1428, 1429, 1430, 1432, 1433, 1434, 1435, 1436, 1440, 1441, 1444, 1449, 1450, 1451, 1452, 1453, 1454, 1455, 1456, 1457, 1459, 1460, 1461, 1463, 1464, 1465, 1466, 1467, 1468, 1469, 1470, 1471, 1472, 1473, 1474, 1475, 1476, 1477, 1478, 1481, 1482, 1483, 1484, 1485, 1486, 1487, 1488, 1489, 1490, 1491, 1492, 1493, 1494, 1495, 1496, 1497, 1498, 1499, 1500, 1501, 1502, 1503, 1504, 1505, 1506, 1507, 1508, 1509, 1510, 1511, 1512, 1513, 1514, 1517, 1518, 1519, 1520, 1521, 1522, 1523, 1524, 1525, 1526, 1527, 1528, 1529, 1530, 1531, 1532, 1533, 1534, 1535, 1536, 1541, 1542, 1543, 1550, 1551, 1553, 1554, 1555, 1556, 1557, 1558, 1559, 1560, 1561, 1562, 1563, 1564, 1565, 1566, 1567, 1568, 1569, 1570, 1572, 1573, 1574, 1575, 1576, 1577, 1578, 1579, 1580, 1581, 1582, 1583, 1584, 1585, 1586, 1587, 1588, 1589, 1590, 1591, 1592, 1602, 1603, 1605, 1606, 1607, 1608, 1609, 1610, 1611, 1612, 1613, 1614, 1615, 1616, 1617, 1618, 1619, 1620, 1621, 1622, 1623, 1624, 1625, 1626, 1627, 1628, 1629, 1630, 1631, 1632, 1633, 1634, 1635, 1636, 1637, 1638, 1639, 1640, 1641, 1642, 1643, 1645, 1646, 1647, 1648, 1649, 1650, 1651, 1652, 1653, 1654, 1655, 1656, 1657, 1658, 1660, 1661, 1662, 1663, 1664, 1665, 1666, 1667, 1668, 1669, 1670, 1671, 1672, 1673, 1674, 1675, 1676, 1677, 1678, 1679, 1680, 1681, 1682, 1683, 1684, 1685, 1686, 1687, 1688, 1689, 1690, 1691, 1692, 1693, 1694, 1695, 1696, 1697, 1698, 1699, 1700, 1701, 1702, 1703, 1704, 1705, 1706, 1707, 1708, 1709, 1710, 1711, 1712, 1713, 1714, 1715, 1716, 1717, 1718, 1719, 1720, 1721, 1722, 1723, 1724, 1725, 1726, 1727, 1728, 1729, 1730, 1731, 1732, 1733, 1734, 1735, 1736, 1737, 1738, 1739, 1740, 1741, 1742, 1743, 1744, 1745, 1746, 1747, 1748, 1749, 1750, 1751, 1752, 1753, 1754, 1755, 1756, 1757, 1758, 1759, 1760, 1761, 1762, 1763, 1764, 1765, 1766, 1767, 1768, 1769, 1770, 1771, 1772, 1773, 1774, 1775, 1776, 1777, 1778, 1779, 1780, 1781, 1782, 1783, 1784, 1785, 1786, 1787, 1788, 1789, 1790, 1791, 1792, 1793, 1794, 1795, 1796, 1797, 1798, 1799, 1800, 1801, 1802, 1803, 1804, 1805, 1806, 1807, 1808, 1809, 1810, 1811, 1812, 1813, 1814, 1815, 1816, 1817, 1818, 1819, 1820, 1821, 1822, 1823, 1824, 1825, 1826, 1827, 1828, 1829, 1830, 1831, 1832, 1833, 1834, 1835, 1836, 1837, 1838, 1839, 1840, 1841, 1842, 1843, 1844, 1845, 1846, 1847, 1848, 1849, 1850, 1851, 1852, 1853, 1854, 1855, 1856, 1857, 1858, 1859, 1860, 1861, 1862, 1863, 1864, 1865, 1866, 1867, 1868, 1869, 1870, 1871, 1872, 1873, 1874, 1875, 1876, 1877, 1878, 1879, 1880, 1881]</t>
-        </is>
-      </c>
-      <c r="BH7" t="n">
-        <v>0.07951408061844284</v>
-      </c>
-      <c r="BI7" t="inlineStr">
-        <is>
-          <t>{'initial_window': 367, 'window_size': 420, 'num_trees': 23, 'max_depth': 10}</t>
-        </is>
-      </c>
-      <c r="BJ7" t="n">
-        <v>1.699256216874346</v>
-      </c>
-      <c r="BK7" t="inlineStr">
+      <c r="BM7" t="inlineStr">
+        <is>
+          <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86, 87, 88, 89, 90, 91, 92, 93, 94, 95, 96, 97, 98, 99, 100, 101, 102, 103, 104, 105, 106, 107, 108, 109, 110, 111, 112, 113, 114, 115, 116, 117, 118, 119, 120, 121, 122, 123, 124, 125, 126, 127, 128, 129, 130, 131, 132, 133, 134, 135, 136, 137, 138, 139, 140, 141, 142, 143, 144, 145, 146, 147, 148, 149, 150, 151, 152, 153, 154, 155, 156, 157, 158, 159, 160, 161, 162, 163, 164, 165, 166, 167, 168, 169, 170, 171, 172, 173, 174, 175, 176, 177, 178, 179, 180, 181, 182, 183, 184, 185, 186, 187, 188, 189, 190, 191, 192, 193, 194, 195, 196, 197, 198, 199, 200, 201, 202, 203, 204, 205, 206, 207, 208, 209, 210, 211, 212, 213, 214, 215, 216, 217, 218, 219, 220, 221, 222, 223, 224, 225, 226, 227, 228, 229, 230, 231, 232, 233, 234, 235, 236, 237, 238, 239, 240, 241, 242, 243, 244, 245, 246, 247, 248, 249, 250, 251, 252, 253, 254, 255, 256, 257, 258, 259, 260, 261, 262, 263, 264, 265, 266, 267, 268, 269, 270, 271, 272, 273, 274, 275, 276, 277, 278, 279, 280, 281, 282, 283, 284, 285, 286, 287, 288, 289, 290, 291, 292, 293, 294, 295, 296, 297, 298, 299, 300, 301, 302, 303, 304, 305, 306, 307, 308, 309, 310, 311, 312, 313, 314, 315, 316, 317, 318, 319, 320, 321, 322, 323, 324, 325, 326, 327, 328, 329, 330, 331, 332, 333, 334, 335, 336, 337, 338, 339, 340, 341, 342, 343, 344, 345, 346, 347, 348, 349, 350, 351, 352, 353, 354, 355, 356, 357, 358, 359, 360, 361, 362, 363, 364, 365, 366, 367, 368, 369, 370, 371, 372, 373, 374, 375, 376, 377, 378, 379, 380, 381, 382, 383, 384, 385, 386, 387, 388, 389, 390, 391, 392, 393, 394, 395, 396, 397, 398, 399, 400, 401, 402, 403, 404, 405, 406, 407, 408, 409, 410, 411, 412, 413, 414, 415, 416, 417, 418, 419, 420, 421, 422, 423, 424, 425, 426, 427, 428, 429, 430, 431, 432, 433, 434, 435, 436, 437, 438, 439, 440, 441, 442, 443, 444, 445, 446, 447, 448, 449, 450, 451, 452, 453, 454, 455, 456, 457, 458, 459, 460, 461, 462, 463, 464, 465, 466, 467, 468, 469, 470, 471, 472, 473, 474, 475, 476, 477, 478, 479, 480, 481, 482, 483, 484, 485, 486, 487, 488, 489, 490, 491, 492, 493, 494, 495, 496, 497, 498, 499, 500, 501, 502, 503, 504, 505, 506, 507, 508, 509, 510, 511, 512, 513, 514, 515, 516, 517, 518, 519, 520, 521, 522, 523, 524, 525, 526, 527, 528, 529, 530, 531, 532, 533, 534, 535, 536, 537, 538, 539, 540, 541, 542, 543, 544, 545, 546, 547, 548, 549, 550, 551, 552, 553, 554, 555, 556, 557, 558, 559, 560, 561, 562, 563, 564, 565, 566, 567, 568, 569, 570, 571, 572, 573, 574, 575, 576, 577, 578, 579, 580, 581, 582, 583, 584, 585, 586, 587, 588, 589, 590, 591, 592, 593, 594, 595, 596, 597, 598, 599, 600, 601, 602, 603, 604, 605, 606, 607, 608, 609, 610, 611, 612, 613, 614, 615, 616, 617, 618, 619, 620, 621, 622, 623, 624, 625, 626, 627, 628, 629, 630, 631, 632, 633, 634, 635, 636, 637, 638, 639, 640, 641, 642, 643, 644, 645, 646, 647, 648, 649, 650, 651, 652, 653, 654, 655, 656, 657, 658, 659, 660, 661, 662, 663, 664, 665, 666, 667, 668, 669, 670, 671, 672, 673, 674, 675, 676, 677, 678, 679, 680, 681, 682, 683, 684, 685, 686, 687, 688, 689, 690, 691, 692, 693, 694, 695, 696, 697, 698, 699, 700, 701, 702, 703, 704, 705, 706, 707, 708, 709, 710, 711, 712, 713, 714, 715, 716, 717, 718, 719, 720, 721, 722, 723, 724, 725, 726, 727, 728, 729, 730, 731, 732, 733, 734, 735, 736, 737, 738, 739, 740, 741, 742, 743, 744, 745, 746, 747, 748, 749, 750, 751, 752, 753, 754, 755, 756, 757, 758, 759, 760, 761, 762, 763, 764, 765, 766, 767, 768, 769, 770, 771, 772, 773, 774, 775, 776, 777, 778, 779, 780, 781, 782, 783, 784, 785, 786, 787, 788, 789, 790, 791, 792, 793, 794, 795, 796, 797, 798, 799, 800, 801, 802, 803, 804, 805, 806, 807, 808, 809, 810, 811, 812, 813, 814, 815, 816, 817, 818, 819, 820, 821, 822, 823, 824, 825, 826, 827, 828, 829, 830, 831, 832, 833, 834, 835, 836, 837, 838, 839, 840, 841, 842, 843, 844, 845, 846, 847, 848, 849, 850, 851, 852, 853, 854, 855, 856, 857, 858, 859, 860, 861, 862, 863, 864, 865, 866, 867, 868, 869, 870, 871, 872, 873, 874, 875, 876, 877, 878, 879, 880, 881, 882, 883, 884, 885, 886, 887, 888, 889, 890, 891, 892, 893, 894, 895, 896, 897, 898, 899, 900, 901, 902, 903, 904, 905, 906, 907, 908, 909, 910, 911, 912, 913, 914, 915, 916, 917, 918, 919, 920, 921, 922, 923, 924, 925, 926, 927, 928, 929, 930, 931, 932, 933, 934, 935, 936, 937, 938, 939, 940, 941, 942, 943, 944, 945, 946, 947, 948, 949, 950, 951, 952, 953, 954, 955, 956, 957, 958, 959, 960, 961, 962, 963, 964, 965, 966, 967, 968, 969, 970, 971, 972, 973, 974, 975, 976, 977, 978, 979, 980, 981, 982, 983, 984, 985, 986, 987, 988, 989, 990, 991, 992, 993, 994, 995, 996, 997, 998, 999, 1000, 1001, 1002, 1003, 1004, 1005, 1006, 1007, 1008, 1009, 1010, 1011, 1012, 1013, 1014, 1015, 1016, 1017, 1018, 1019, 1020, 1021, 1022, 1023, 1024, 1025, 1026, 1027, 1028, 1029, 1030, 1031, 1032, 1033, 1034, 1035, 1036, 1037, 1038, 1039, 1040, 1041, 1042, 1043, 1044, 1045, 1046, 1047, 1048, 1049, 1050, 1051, 1052, 1053, 1054, 1055, 1056, 1057, 1058, 1059, 1060, 1061, 1062, 1063, 1064, 1065, 1066, 1067, 1068, 1069, 1070, 1071, 1072, 1073, 1074, 1075, 1076, 1077, 1078, 1079, 1080, 1081, 1082, 1083, 1084, 1085, 1086, 1087, 1088, 1089, 1090, 1091, 1092, 1093, 1094, 1095, 1096, 1097, 1098, 1099, 1100, 1101, 1102, 1103, 1104, 1105, 1106, 1107, 1108, 1109, 1110, 1111, 1112, 1113, 1114, 1115, 1116, 1117, 1118, 1119, 1120, 1121, 1122, 1123, 1124, 1125, 1126, 1127, 1128, 1129, 1130, 1131, 1132, 1133, 1134, 1135, 1136, 1137, 1138, 1139, 1140, 1141, 1142, 1143, 1144, 1145, 1146, 1147, 1148, 1149, 1150, 1151, 1152, 1153, 1154, 1155, 1156, 1157, 1158, 1159, 1160, 1161, 1162, 1163, 1164, 1165, 1166, 1167, 1168, 1169, 1170, 1171, 1172, 1173, 1174, 1175, 1176, 1177, 1178, 1179, 1180, 1181, 1182, 1183, 1184, 1185, 1186, 1187, 1188, 1189, 1190, 1191, 1192, 1193, 1194, 1195, 1196, 1197, 1198, 1199, 1200, 1201, 1202, 1203, 1204, 1205, 1206, 1207, 1208, 1209, 1210, 1211, 1212, 1213, 1214, 1215, 1216, 1217, 1218, 1219, 1220, 1221, 1222, 1223, 1224, 1225, 1226, 1227, 1228, 1229, 1230, 1231, 1232, 1233, 1234, 1235, 1236, 1237, 1238, 1239, 1240, 1241, 1242, 1243, 1244, 1245, 1246, 1247, 1248, 1249, 1250, 1251, 1252, 1253, 1254, 1255, 1256, 1257, 1258, 1259, 1260, 1261, 1262, 1263, 1264, 1265, 1266, 1267, 1268, 1269, 1270, 1271, 1272, 1273, 1274, 1275, 1276, 1277, 1278, 1279, 1280, 1281, 1282, 1283, 1284, 1285, 1286, 1287, 1288, 1289, 1290, 1291, 1292, 1293, 1294, 1295, 1296, 1297, 1298, 1299, 1300, 1303, 1313, 1314, 1317, 1318, 1319, 1320, 1321, 1322, 1323, 1324, 1325, 1326, 1327, 1328, 1329, 1330, 1336, 1337, 1343, 1344, 1345, 1386, 1387, 1388, 1389, 1390, 1391, 1392, 1393, 1394, 1395, 1396, 1397, 1398, 1399, 1400, 1401, 1402, 1403, 1404, 1405, 1406, 1407, 1408, 1409, 1410, 1411, 1412, 1413, 1414, 1415, 1416, 1417, 1418, 1419, 1420, 1421, 1422, 1423, 1424, 1425, 1426, 1427, 1428, 1429, 1430, 1432, 1433, 1434, 1435, 1436, 1440, 1441, 1444, 1449, 1450, 1451, 1452, 1453, 1454, 1455, 1456, 1457, 1459, 1460, 1461, 1463, 1464, 1465, 1466, 1467, 1468, 1469, 1470, 1471, 1472, 1473, 1474, 1475, 1476, 1477, 1478, 1481, 1482, 1483, 1484, 1485, 1486, 1487, 1488, 1489, 1490, 1491, 1492, 1493, 1494, 1495, 1496, 1497, 1498, 1499, 1500, 1501, 1502, 1503, 1504, 1505, 1506, 1507, 1508, 1509, 1510, 1511, 1512, 1513, 1514, 1517, 1518, 1519, 1520, 1521, 1522, 1523, 1524, 1525, 1526, 1527, 1528, 1529, 1530, 1531, 1532, 1533, 1534, 1535, 1536, 1541, 1542, 1543, 1550, 1551, 1553, 1554, 1555, 1556, 1557, 1558, 1559, 1560, 1561, 1562, 1563, 1564, 1565, 1566, 1567, 1568, 1569, 1570, 1572, 1573, 1574, 1575, 1576, 1577, 1578, 1579, 1580, 1581, 1582, 1583, 1584, 1585, 1586, 1587, 1588, 1589, 1590, 1591, 1592, 1602, 1603, 1605, 1606, 1607, 1608, 1609, 1610, 1611, 1612, 1613, 1614, 1615, 1616, 1617, 1618, 1619, 1620, 1621, 1622, 1623, 1624, 1625, 1626, 1627, 1628, 1629, 1630, 1631, 1632, 1633, 1634, 1635, 1636, 1637, 1638, 1639, 1640, 1641, 1642, 1643, 1645, 1646, 1647, 1648, 1649, 1650, 1651, 1652, 1653, 1654, 1655, 1656, 1657, 1658, 1660, 1661, 1662, 1663, 1664, 1665, 1666, 1667, 1668, 1669, 1670, 1671, 1672, 1673, 1674, 1675, 1676, 1677, 1678, 1679, 1680, 1681, 1682, 1685, 1686, 1687, 1688, 1689, 1690, 1691, 1693, 1695, 1696, 1698, 1702, 1703, 1708, 1709, 1710, 1711, 1713, 1714, 1715, 1716, 1717, 1718, 1719, 1720, 1723, 1724, 1735, 1736, 1737, 1738, 1739, 1740, 1741, 1742, 1743, 1744, 1745, 1746, 1747, 1748, 1749, 1750, 1751, 1752, 1753, 1754, 1755, 1756, 1757, 1758, 1759, 1760, 1761, 1762, 1763, 1764, 1765, 1766, 1767, 1768, 1769, 1770, 1771, 1772, 1773, 1774, 1775, 1776, 1777, 1778, 1779, 1780, 1781, 1782, 1783, 1784, 1785, 1786, 1787, 1788, 1789, 1790, 1791, 1792, 1793, 1794, 1795, 1796, 1797, 1798, 1799, 1800, 1801, 1802, 1803, 1804, 1805, 1806, 1807, 1808, 1809, 1810, 1811, 1812, 1813, 1814, 1815, 1816, 1817, 1818, 1819, 1820, 1821, 1822, 1823, 1824, 1825, 1826, 1827, 1828, 1829, 1830, 1831, 1832, 1833, 1834, 1835, 1836, 1837, 1838, 1839, 1840, 1841, 1842, 1843, 1844, 1845, 1846, 1847, 1848, 1849, 1850, 1851, 1852, 1853, 1854, 1855, 1856, 1857, 1858, 1859, 1860, 1861, 1862, 1863, 1864, 1865, 1866, 1867, 1868, 1869, 1870, 1871, 1872, 1873, 1874, 1875, 1876, 1877, 1878, 1879, 1880, 1881]</t>
+        </is>
+      </c>
+      <c r="BN7" t="n">
+        <v>0.07569939659901262</v>
+      </c>
+      <c r="BO7" t="inlineStr">
+        <is>
+          <t>{'initial_window': 276, 'window_size': 434, 'num_trees': 19, 'max_depth': 14}</t>
+        </is>
+      </c>
+      <c r="BP7" t="n">
+        <v>10.44551553297788</v>
+      </c>
+      <c r="BQ7" t="inlineStr">
         <is>
           <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 60, 61, 64, 65, 66, 67, 68, 69, 70, 71, 79, 80, 84, 85, 86, 89, 90, 91, 92, 93, 94, 97, 98, 99, 100, 101, 102, 108, 112, 113, 114, 115, 116, 123, 124, 125, 126, 130, 133, 138, 139, 140, 141, 142, 149, 150, 151, 152, 154, 155, 157, 158, 159, 162, 163, 167, 168, 170, 171, 174, 175, 185, 186, 187, 189, 190, 191, 195, 196, 199, 200, 201, 202, 203, 206, 210, 211, 212, 215, 216, 220, 221, 222, 223, 224, 226, 227, 228, 229, 232, 233, 234, 235, 247, 248, 249, 252, 253, 254, 255, 256, 257, 259, 262, 266, 267, 268, 269, 282, 283, 284, 285, 287, 288, 294, 295, 296, 298, 299, 304, 312, 314, 319, 325, 329, 330, 332, 333, 334, 341, 342, 347, 348, 353, 354, 355, 357, 358, 359, 360, 361, 362, 363, 364, 365, 366, 367, 368, 369, 370, 371, 372, 373, 374, 375, 376, 377, 382, 384, 385, 386, 387, 388, 389, 390, 391, 392, 393, 394, 395, 396, 397, 398, 399, 400, 401, 402, 403, 404, 405, 406, 407, 408, 409, 410, 411, 412, 413, 414, 415, 416, 417, 418, 419, 420, 421, 422, 423, 424, 425, 426, 427, 428, 429, 430, 431, 432, 433, 434, 435, 436, 437, 438, 439, 440, 441, 442, 443, 444, 445, 446, 447, 448, 449, 450, 451, 452, 453, 454, 455, 456, 457, 458, 459, 460, 461, 462, 463, 464, 465, 466, 467, 468, 469, 470, 471, 472, 479, 482, 487, 488, 489, 490, 492, 496, 502, 503, 504, 505, 507, 508, 509, 510, 511, 512, 513, 514, 515, 516, 520, 521, 527, 528, 529, 530, 531, 532, 536, 537, 538, 539, 542, 543, 544, 545, 547, 548, 551, 553, 554, 555, 560, 561, 562, 563, 564, 569, 570, 571, 573, 574, 575, 576, 577, 578, 579, 580, 581, 582, 587, 588, 589, 593, 594, 597, 601, 602, 603, 604, 605, 606, 607, 608, 609, 610, 611, 612, 614, 615, 616, 617, 623, 627, 628, 629, 633, 634, 635, 636, 637, 638, 639, 640, 641, 642, 643, 644, 645, 646, 647, 648, 649, 650, 651, 652, 653, 654, 655, 656, 657, 658, 659, 660, 661, 662, 663, 667, 668, 669, 670, 673, 675, 676, 677, 678, 679, 680, 681, 682, 683, 684, 685, 686, 687, 688, 689, 690, 691, 692, 693, 694, 695, 696, 697, 698, 699, 700, 701, 702, 703, 704, 705, 706, 707, 708, 709, 710, 711, 712, 713, 714, 715, 716, 717, 718, 719, 720, 721, 722, 723, 724, 725, 726, 727, 728, 729, 730, 731, 732, 733, 734, 735, 736, 737, 738, 739, 740, 741, 742, 743, 744, 745, 746, 747, 748, 749, 750, 751, 752, 753, 754, 755, 756, 757, 758, 759, 760, 761, 762, 763, 764, 765, 766, 767, 768, 769, 770, 771, 772, 773, 774, 775, 776, 777, 778, 779, 780, 781, 782, 790, 791, 792, 793, 796, 797, 798, 799, 801, 802, 806, 807, 808, 809, 810, 811, 813, 814, 816, 819, 822, 828, 829, 830, 835, 836, 837, 840, 842, 843, 844, 845, 849, 850, 851, 852, 853, 854, 855, 856, 857, 861, 865, 866, 867, 868, 871, 872, 875, 879, 880, 881, 884, 885, 886, 887, 888, 889, 892, 893, 894, 895, 896, 897, 898, 899, 900, 901, 902, 903, 904, 905, 906, 907, 908, 909, 910, 911, 912, 913, 914, 915, 916, 917, 918, 919, 920, 921, 922, 923, 924, 925, 926, 927, 928, 929, 930, 935, 936, 937, 938, 939, 940, 941, 942, 943, 944, 945, 946, 947, 948, 949, 950, 951, 952, 953, 954, 955, 956, 957, 958, 959, 960, 961, 962, 963, 964, 965, 966, 967, 968, 969, 970, 971, 972, 973, 974, 975, 976, 977, 978, 979, 980, 981, 982, 983, 984, 985, 986, 987, 988, 989, 990, 991, 992, 993, 994, 995, 996, 997, 998, 999, 1000, 1001, 1002, 1003, 1004, 1005, 1006, 1007, 1008, 1009, 1010, 1011, 1012, 1013, 1014, 1015, 1016, 1017, 1018, 1019, 1020, 1021, 1022, 1023, 1024, 1025, 1026, 1027, 1028, 1029, 1030, 1031, 1032, 1033, 1034, 1035, 1036, 1037, 1038, 1039, 1040, 1041, 1042, 1043, 1044, 1045, 1046, 1047, 1048, 1049, 1050, 1051, 1052, 1053, 1054, 1055, 1056, 1057, 1058, 1059, 1060, 1065, 1066, 1067, 1068, 1069, 1070, 1071, 1072, 1073, 1074, 1075, 1076, 1077, 1078, 1079, 1080, 1081, 1082, 1083, 1084, 1085, 1086, 1087, 1088, 1089, 1090, 1091, 1092, 1093, 1094, 1095, 1096, 1097, 1098, 1099, 1100, 1101, 1102, 1103, 1104, 1105, 1106, 1107, 1108, 1109, 1110, 1111, 1112, 1113, 1114, 1115, 1116, 1117, 1118, 1119, 1120, 1121, 1122, 1123, 1124, 1125, 1126, 1127, 1128, 1129, 1130, 1131, 1132, 1133, 1134, 1135, 1136, 1137, 1138, 1139, 1140, 1141, 1142, 1143, 1144, 1145, 1146, 1147, 1148, 1149, 1150, 1151, 1152, 1153, 1154, 1155, 1156, 1157, 1158, 1159, 1160, 1168, 1169, 1170, 1171, 1172, 1173, 1174, 1175, 1176, 1177, 1178, 1179, 1180, 1181, 1182, 1183, 1184, 1185, 1186, 1187, 1188, 1189, 1190, 1191, 1192, 1193, 1194, 1195, 1196, 1197, 1198, 1199, 1200, 1201, 1202, 1203, 1204, 1205, 1206, 1207, 1208, 1209, 1210, 1211, 1212, 1213, 1214, 1215, 1216, 1217, 1218, 1219, 1220, 1221, 1222, 1223, 1224, 1225, 1226, 1227, 1228, 1229, 1230, 1231, 1232, 1233, 1234, 1235, 1236, 1237, 1238, 1239, 1240, 1241, 1242, 1243, 1244, 1245, 1246, 1247, 1248, 1249, 1250, 1251, 1252, 1253, 1254, 1255, 1256, 1257, 1258, 1259, 1260, 1261, 1262, 1263, 1264, 1265, 1266, 1267, 1268, 1269, 1270, 1271, 1272, 1273, 1274, 1275, 1276, 1277, 1278, 1279, 1280, 1281, 1282, 1283, 1284, 1285, 1286, 1287, 1288, 1289, 1290, 1291, 1292, 1293, 1294, 1295, 1296, 1297, 1298, 1299, 1300, 1301, 1302, 1303, 1304, 1305, 1306, 1307, 1308, 1309, 1310, 1311, 1312, 1313, 1314, 1315, 1316, 1317, 1318, 1319, 1320, 1321, 1322, 1323, 1324, 1325, 1326, 1328, 1329, 1330, 1331, 1332, 1333, 1334, 1335, 1336, 1337, 1338, 1339, 1340, 1341, 1342, 1343, 1344, 1345, 1346, 1347, 1348, 1349, 1350, 1351, 1355, 1356, 1357, 1358, 1359, 1360, 1361, 1362, 1363, 1364, 1367, 1370, 1376, 1380, 1382, 1383, 1384, 1385, 1392, 1393, 1394, 1400, 1401, 1402, 1403, 1404, 1405, 1406, 1407, 1408, 1409, 1410, 1411, 1412, 1413, 1414, 1415, 1416, 1417, 1418, 1419, 1420, 1421, 1422, 1423, 1424, 1425, 1426, 1427, 1428, 1429, 1430, 1431, 1432, 1433, 1434, 1435, 1436, 1437, 1438, 1440, 1441, 1442, 1443, 1444, 1445, 1446, 1447, 1458, 1461, 1467, 1468, 1469, 1470, 1471, 1472, 1476, 1477, 1478, 1479, 1480, 1485, 1488, 1489, 1492, 1493, 1494, 1502, 1503, 1504, 1505, 1506, 1507, 1508, 1509, 1510, 1514, 1515, 1516, 1518, 1519, 1520, 1521, 1527, 1528, 1537, 1538, 1539, 1540, 1541, 1543, 1549, 1550, 1552, 1553, 1554, 1556, 1557, 1561, 1568, 1572, 1573, 1581, 1584, 1585, 1589, 1593, 1597, 1598, 1599, 1600, 1602, 1603, 1607, 1608, 1612, 1613, 1614, 1622, 1624, 1625, 1626, 1627, 1628, 1629, 1630, 1631, 1632, 1634, 1635, 1639, 1640, 1647, 1648, 1649, 1650, 1651, 1652, 1654, 1655, 1656, 1658, 1661, 1662, 1663, 1664, 1665, 1668, 1671, 1672, 1673, 1677, 1678, 1679, 1680, 1684, 1685, 1687, 1688, 1689, 1690, 1691, 1701, 1704, 1706, 1707, 1708, 1709, 1710, 1712, 1714, 1715, 1716, 1717, 1718, 1719, 1721, 1724, 1725, 1726, 1727, 1731, 1732, 1738, 1739, 1740, 1741, 1742, 1743, 1752, 1753, 1758, 1759, 1760, 1761, 1766, 1767, 1773, 1775, 1779, 1780, 1781, 1782, 1783, 1784, 1785, 1786, 1787, 1790, 1791, 1800, 1801, 1802, 1803, 1807, 1808, 1812, 1813, 1815, 1816, 1817, 1820, 1822, 1824, 1825, 1826, 1827, 1828, 1832, 1833, 1834, 1835, 1836, 1837, 1840, 1841, 1842, 1843, 1846, 1850, 1851, 1852, 1854, 1855, 1862, 1864, 1865, 1866, 1867, 1869, 1870, 1876, 1877, 1878, 1879, 1880, 1881]</t>
         </is>
       </c>
-      <c r="BL7" t="n">
+      <c r="BR7" t="n">
         <v>0.1036717062634989</v>
       </c>
-      <c r="BM7" t="inlineStr">
+      <c r="BS7" t="inlineStr">
         <is>
           <t>{'AR_window_size': 53, 'differencing-order': 4}</t>
         </is>
       </c>
-      <c r="BN7" t="n">
+      <c r="BT7" t="n">
         <v>36.00591896218248</v>
       </c>
-      <c r="BO7" t="inlineStr">
+      <c r="BU7" t="inlineStr">
         <is>
           <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86, 87, 88, 89, 90, 91, 92, 93, 94, 95, 96, 97, 98, 99, 100, 101, 102, 103, 104, 105, 106, 107, 108, 109, 110, 111, 112, 113, 114, 115, 116, 117, 118, 119, 120, 121, 122, 123, 124, 125, 126, 127, 128, 129, 130, 131, 132, 133, 134, 135, 136, 137, 138, 139, 140, 141, 142, 143, 144, 145, 146, 147, 148, 149, 150, 151, 153, 154, 155, 156, 157, 158, 159, 160, 161, 162, 163, 164, 165, 166, 167, 168, 169, 170, 171, 172, 173, 174, 175, 176, 177, 178, 179, 180, 181, 182, 183, 184, 185, 186, 187, 188, 189, 190, 191, 192, 193, 194, 195, 196, 197, 198, 199, 200, 201, 202, 203, 204, 205, 206, 207, 208, 209, 210, 211, 212, 213, 214, 215, 216, 217, 218, 219, 220, 221, 222, 223, 224, 225, 226, 227, 228, 229, 230, 231, 232, 233, 234, 235, 236, 237, 238, 239, 240, 241, 242, 243, 244, 246, 247, 248, 249, 250, 251, 252, 253, 254, 255, 256, 257, 258, 259, 260, 261, 262, 263, 264, 265, 267, 268, 269, 270, 271, 272, 273, 274, 275, 276, 277, 278, 279, 280, 281, 282, 283, 284, 285, 286, 287, 288, 289, 290, 291, 292, 293, 294, 295, 296, 297, 298, 299, 300, 301, 302, 303, 304, 305, 306, 307, 308, 309, 310, 311, 312, 313, 314, 315, 316, 317, 318, 319, 320, 321, 322, 323, 324, 325, 326, 327, 328, 329, 330, 331, 332, 333, 334, 335, 336, 337, 338, 339, 340, 341, 342, 343, 344, 345, 346, 347, 348, 349, 350, 351, 352, 353, 354, 355, 356, 357, 358, 359, 360, 361, 362, 363, 364, 365, 366, 367, 368, 369, 370, 371, 372, 373, 374, 375, 376, 377, 378, 379, 380, 381, 382, 383, 384, 385, 386, 387, 388, 389, 390, 391, 392, 393, 394, 395, 396, 397, 398, 399, 400, 401, 402, 403, 404, 405, 406, 407, 408, 409, 410, 411, 412, 413, 414, 415, 416, 417, 418, 419, 420, 421, 422, 423, 424, 425, 426, 427, 428, 429, 430, 431, 433, 434, 435, 436, 437, 438, 439, 440, 441, 442, 443, 444, 445, 446, 447, 448, 449, 450, 451, 452, 453, 454, 455, 456, 457, 458, 459, 460, 461, 462, 463, 464, 465, 466, 467, 468, 469, 470, 471, 472, 473, 474, 475, 476, 477, 478, 479, 480, 481, 482, 483, 484, 485, 486, 487, 488, 489, 490, 491, 492, 493, 494, 495, 496, 497, 498, 499, 500, 501, 502, 503, 504, 505, 506, 507, 508, 509, 510, 511, 512, 513, 514, 515, 516, 517, 518, 519, 520, 521, 522, 523, 524, 525, 526, 527, 528, 529, 530, 531, 532, 533, 534, 535, 536, 537, 538, 539, 540, 541, 542, 543, 544, 545, 546, 547, 548, 549, 550, 551, 552, 553, 554, 555, 556, 557, 558, 559, 560, 561, 562, 563, 564, 565, 566, 567, 568, 569, 570, 571, 572, 573, 574, 575, 576, 577, 578, 579, 580, 581, 582, 583, 584, 585, 586, 587, 588, 589, 590, 591, 592, 593, 594, 595, 596, 597, 598, 599, 600, 601, 602, 603, 604, 605, 606, 607, 608, 609, 610, 611, 612, 613, 614, 615, 616, 617, 618, 619, 620, 621, 622, 623, 624, 625, 626, 627, 628, 629, 630, 631, 632, 633, 634, 635, 636, 637, 638, 639, 640, 641, 642, 643, 644, 645, 646, 647, 648, 649, 650, 651, 652, 653, 654, 655, 656, 657, 658, 659, 660, 661, 662, 663, 664, 665, 666, 667, 668, 669, 670, 671, 672, 673, 674, 675, 676, 677, 678, 679, 680, 681, 682, 683, 684, 685, 686, 687, 688, 689, 690, 691, 692, 693, 694, 695, 696, 697, 698, 699, 700, 701, 702, 703, 704, 705, 706, 707, 708, 709, 710, 711, 712, 713, 714, 715, 716, 717, 718, 719, 720, 721, 722, 723, 724, 725, 726, 727, 728, 729, 730, 731, 732, 733, 734, 735, 736, 737, 738, 739, 740, 741, 742, 743, 744, 745, 746, 747, 748, 749, 750, 751, 752, 753, 754, 755, 756, 757, 758, 759, 760, 761, 762, 763, 764, 765, 766, 767, 768, 769, 770, 771, 772, 773, 774, 775, 776, 777, 778, 779, 780, 781, 782, 783, 784, 785, 786, 787, 788, 789, 790, 791, 792, 793, 794, 795, 796, 797, 798, 799, 800, 801, 802, 803, 804, 805, 806, 807, 808, 809, 810, 811, 812, 813, 814, 815, 816, 817, 818, 819, 820, 821, 822, 823, 824, 825, 826, 827, 828, 829, 830, 831, 832, 833, 834, 835, 836, 837, 838, 839, 840, 841, 842, 843, 844, 845, 846, 847, 848, 849, 850, 851, 852, 853, 854, 855, 856, 857, 858, 859, 860, 861, 862, 863, 864, 865, 866, 867, 868, 869, 870, 871, 872, 873, 874, 875, 876, 877, 878, 879, 880, 881, 882, 883, 884, 885, 886, 887, 888, 889, 890, 891, 892, 893, 894, 895, 896, 897, 898, 899, 900, 901, 902, 903, 904, 905, 906, 907, 908, 909, 910, 911, 912, 913, 914, 915, 916, 917, 918, 919, 920, 921, 922, 923, 924, 925, 926, 927, 928, 929, 930, 931, 932, 933, 934, 935, 936, 937, 938, 939, 940, 941, 942, 943, 944, 945, 946, 947, 948, 949, 950, 951, 952, 953, 954, 955, 956, 957, 958, 959, 960, 961, 962, 963, 964, 965, 966, 967, 968, 969, 970, 971, 972, 973, 974, 975, 976, 977, 978, 979, 980, 981, 982, 983, 984, 985, 986, 987, 988, 989, 990, 991, 992, 993, 994, 995, 996, 997, 998, 999, 1000, 1001, 1002, 1003, 1004, 1005, 1006, 1007, 1008, 1009, 1010, 1011, 1012, 1013, 1014, 1015, 1016, 1017, 1018, 1019, 1020, 1021, 1022, 1023, 1024, 1025, 1026, 1027, 1028, 1029, 1030, 1031, 1032, 1033, 1034, 1035, 1036, 1037, 1038, 1039, 1040, 1041, 1042, 1043, 1044, 1045, 1046, 1047, 1048, 1049, 1050, 1051, 1052, 1053, 1054, 1055, 1056, 1057, 1058, 1059, 1060, 1061, 1062, 1063, 1064, 1065, 1066, 1067, 1068, 1069, 1070, 1071, 1072, 1073, 1074, 1075, 1076, 1077, 1078, 1079, 1080, 1081, 1082, 1083, 1084, 1085, 1086, 1087, 1088, 1089, 1090, 1091, 1092, 1093, 1094, 1095, 1096, 1097, 1098, 1099, 1100, 1101, 1102, 1103, 1104, 1105, 1106, 1107, 1108, 1109, 1110, 1111, 1112, 1113, 1114, 1115, 1116, 1117, 1118, 1119, 1120, 1121, 1122, 1123, 1124, 1125, 1126, 1127, 1128, 1129, 1130, 1131, 1132, 1133, 1134, 1135, 1136, 1137, 1138, 1139, 1140, 1141, 1142, 1143, 1144, 1145, 1146, 1147, 1148, 1149, 1150, 1151, 1152, 1153, 1154, 1155, 1156, 1157, 1158, 1159, 1160, 1161, 1162, 1163, 1164, 1165, 1166, 1167, 1168, 1169, 1170, 1171, 1172, 1173, 1174, 1175, 1176, 1177, 1178, 1179, 1180, 1181, 1182, 1183, 1184, 1185, 1186, 1187, 1188, 1189, 1190, 1191, 1192, 1193, 1194, 1195, 1196, 1197, 1198, 1199, 1200, 1201, 1202, 1203, 1204, 1205, 1206, 1207, 1208, 1209, 1210, 1211, 1212, 1213, 1214, 1215, 1216, 1217, 1218, 1219, 1220, 1221, 1222, 1223, 1224, 1225, 1226, 1227, 1228, 1229, 1230, 1231, 1232, 1233, 1234, 1235, 1236, 1237, 1238, 1239, 1240, 1241, 1242, 1243, 1244, 1245, 1246, 1247, 1248, 1249, 1250, 1251, 1252, 1253, 1254, 1255, 1256, 1257, 1258, 1259, 1260, 1261, 1262, 1263, 1264, 1265, 1266, 1267, 1268, 1269, 1270, 1271, 1272, 1273, 1274, 1275, 1276, 1277, 1278, 1279, 1280, 1281, 1282, 1283, 1284, 1285, 1286, 1287, 1288, 1289, 1290, 1291, 1292, 1293, 1294, 1295, 1296, 1297, 1298, 1299, 1300, 1301, 1302, 1303, 1304, 1305, 1306, 1307, 1308, 1309, 1310, 1311, 1312, 1313, 1314, 1315, 1316, 1317, 1318, 1319, 1321, 1322, 1323, 1331, 1332, 1333, 1334, 1335, 1336, 1337, 1338, 1339, 1340, 1341, 1342, 1343, 1344, 1345, 1346, 1347, 1348, 1349, 1350, 1351, 1352, 1353, 1354, 1355, 1356, 1357, 1358, 1359, 1360, 1361, 1362, 1363, 1364, 1365, 1366, 1367, 1368, 1369, 1370, 1371, 1372, 1373, 1374, 1375, 1376, 1377, 1378, 1379, 1380, 1381, 1382, 1383, 1384, 1385, 1386, 1387, 1388, 1389, 1390, 1391, 1392, 1393, 1394, 1395, 1396, 1397, 1398, 1399, 1400, 1401, 1402, 1403, 1404, 1405, 1406, 1407, 1408, 1409, 1410, 1411, 1412, 1413, 1414, 1415, 1416, 1417, 1418, 1419, 1420, 1421, 1422, 1423, 1424, 1425, 1426, 1427, 1428, 1429, 1430, 1431, 1432, 1433, 1434, 1435, 1436, 1437, 1438, 1439, 1440, 1441, 1442, 1443, 1444, 1445, 1446, 1447, 1448, 1449, 1450, 1451, 1452, 1453, 1454, 1455, 1456, 1457, 1458, 1459, 1460, 1461, 1462, 1463, 1464, 1465, 1466, 1467, 1468, 1469, 1470, 1471, 1472, 1473, 1474, 1475, 1476, 1477, 1478, 1479, 1480, 1481, 1482, 1483, 1484, 1485, 1486, 1487, 1488, 1489, 1490, 1491, 1492, 1493, 1494, 1495, 1496, 1497, 1498, 1499, 1500, 1501, 1502, 1503, 1504, 1505, 1506, 1507, 1508, 1509, 1510, 1511, 1512, 1513, 1514, 1515, 1516, 1517, 1518, 1519, 1520, 1521, 1522, 1523, 1524, 1525, 1526, 1527, 1528, 1529, 1530, 1531, 1532, 1533, 1534, 1535, 1536, 1537, 1538, 1539, 1540, 1541, 1542, 1543, 1544, 1545, 1546, 1547, 1548, 1549, 1550, 1551, 1552, 1553, 1554, 1555, 1556, 1557, 1558, 1559, 1560, 1561, 1562, 1563, 1564, 1565, 1566, 1567, 1568, 1570, 1571, 1572, 1573, 1574, 1575, 1576, 1577, 1578, 1579, 1580, 1581, 1582, 1583, 1584, 1585, 1586, 1587, 1588, 1589, 1590, 1591, 1592, 1593, 1594, 1595, 1596, 1597, 1598, 1599, 1600, 1601, 1602, 1603, 1604, 1605, 1606, 1607, 1608, 1609, 1610, 1611, 1612, 1613, 1614, 1615, 1616, 1617, 1618, 1619, 1620, 1621, 1623, 1624, 1625, 1626, 1627, 1628, 1629, 1630, 1631, 1632, 1633, 1634, 1635, 1636, 1637, 1638, 1639, 1640, 1641, 1642, 1643, 1644, 1645, 1646, 1648, 1649, 1650, 1651, 1652, 1653, 1654, 1655, 1656, 1658, 1659, 1660, 1661, 1662, 1663, 1664, 1665, 1666, 1667, 1668, 1669, 1670, 1671, 1672, 1673, 1674, 1675, 1676, 1677, 1678, 1679, 1680, 1681, 1682, 1683, 1684, 1685, 1686, 1687, 1688, 1689, 1690, 1691, 1692, 1693, 1694, 1695, 1696, 1697, 1698, 1699, 1700, 1701, 1702, 1703, 1704, 1705, 1706, 1707, 1708, 1709, 1710, 1711, 1712, 1713, 1714, 1715, 1716, 1717, 1718, 1719, 1720, 1721, 1722, 1723, 1724, 1725, 1726, 1727, 1728, 1729, 1730, 1731, 1732, 1733, 1734, 1735, 1736, 1737, 1738, 1739, 1740, 1741, 1742, 1743, 1744, 1745, 1746, 1747, 1748, 1749, 1750, 1751, 1752, 1753, 1754, 1755, 1756, 1757, 1758, 1759, 1760, 1761, 1762, 1763, 1764, 1765, 1766, 1767, 1768, 1769, 1770, 1771, 1772, 1773, 1774, 1775, 1776, 1777, 1778, 1779, 1780, 1782, 1783, 1784, 1785, 1786, 1787, 1788, 1789, 1790, 1791, 1792, 1793, 1794, 1795, 1796, 1797, 1798, 1799, 1800, 1801, 1802, 1803, 1804, 1805, 1806, 1807, 1808, 1809, 1810, 1811, 1812, 1813, 1814, 1815, 1816, 1817, 1818, 1819, 1820, 1821, 1822, 1823, 1824, 1825, 1826, 1827, 1828, 1829, 1830, 1831, 1832, 1833, 1834, 1835, 1836, 1837, 1838, 1839, 1840, 1841, 1842, 1843, 1844, 1845, 1846, 1847, 1848, 1849, 1850, 1851, 1852, 1853, 1855, 1856, 1857, 1858, 1859, 1860, 1861, 1862, 1863, 1864, 1865, 1866, 1867, 1868, 1869, 1870, 1871, 1872, 1873, 1874, 1875, 1876, 1877, 1878, 1879, 1880, 1881]</t>
         </is>
       </c>
-      <c r="BP7" t="n">
+      <c r="BV7" t="n">
         <v>0.07441860465116279</v>
       </c>
-      <c r="BQ7" t="inlineStr">
+      <c r="BW7" t="inlineStr">
         <is>
           <t>{'Numk': 31, 'KPar': 27, 'Bucket_index': 906}</t>
         </is>
       </c>
-      <c r="BR7" t="n">
+      <c r="BX7" t="n">
         <v>28.91637435695156</v>
       </c>
-      <c r="BS7" t="inlineStr">
+      <c r="BY7" t="inlineStr">
         <is>
           <t>no</t>
         </is>
       </c>
-      <c r="BT7" t="n">
-        <v>0</v>
-      </c>
-      <c r="BU7" t="inlineStr">
+      <c r="BZ7" t="n">
+        <v>0</v>
+      </c>
+      <c r="CA7" t="inlineStr">
         <is>
           <t>params</t>
         </is>
       </c>
-      <c r="BV7" t="n">
+      <c r="CB7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2418,93 +2556,111 @@
       <c r="AY8" t="n">
         <v>6</v>
       </c>
-      <c r="AZ8" t="inlineStr"/>
-      <c r="BA8" t="inlineStr">
+      <c r="AZ8" t="n">
+        <v>6</v>
+      </c>
+      <c r="BA8" t="n">
+        <v>6</v>
+      </c>
+      <c r="BB8" t="n">
+        <v>6</v>
+      </c>
+      <c r="BC8" t="n">
+        <v>6</v>
+      </c>
+      <c r="BD8" t="n">
+        <v>6</v>
+      </c>
+      <c r="BE8" t="n">
+        <v>6</v>
+      </c>
+      <c r="BF8" t="inlineStr"/>
+      <c r="BG8" t="inlineStr">
         <is>
           <t>nab-data/realKnownCause/rogue_agent_key_updown.csv</t>
         </is>
       </c>
-      <c r="BB8" t="n">
+      <c r="BH8" t="n">
         <v>5315</v>
       </c>
-      <c r="BC8" t="inlineStr">
+      <c r="BI8" t="inlineStr">
         <is>
           <t>NAB</t>
         </is>
       </c>
-      <c r="BD8" t="n">
-        <v>2</v>
-      </c>
-      <c r="BE8" t="inlineStr">
+      <c r="BJ8" t="n">
+        <v>2</v>
+      </c>
+      <c r="BK8" t="inlineStr">
         <is>
           <t>2243; 2877</t>
         </is>
       </c>
-      <c r="BF8" t="n">
+      <c r="BL8" t="n">
         <v>264</v>
       </c>
-      <c r="BG8" t="inlineStr">
+      <c r="BM8" t="inlineStr">
         <is>
           <t>[0, 1, 2, 3, 8, 240, 244, 245, 246, 247, 248, 254, 258, 259, 262, 263, 264, 265, 266, 267, 268, 270, 271, 272, 288, 289, 292, 293, 294, 295, 296, 297, 298, 299, 300, 301, 302, 303, 304, 305, 306, 307, 309, 310, 311, 312, 315, 317, 319, 320, 321, 322, 323, 324, 325, 326, 331, 332, 334, 335, 337, 338, 342, 343, 344, 345, 347, 348, 349, 350, 351, 352, 528, 529, 530, 532, 533, 540, 542, 546, 547, 548, 549, 550, 551, 552, 553, 554, 556, 559, 561, 566, 567, 568, 569, 570, 571, 575, 582, 584, 585, 593, 596, 597, 599, 603, 605, 610, 612, 615, 813, 814, 815, 817, 819, 820, 824, 827, 828, 830, 834, 835, 837, 838, 840, 841, 842, 843, 852, 853, 856, 857, 862, 866, 868, 869, 875, 876, 877, 885, 886, 1142, 1143, 1145, 1146, 1148, 1149, 1153, 1154, 1157, 1159, 1160, 1162, 1164, 1166, 1169, 1170, 1172, 1174, 1175, 1176, 1178, 1180, 1181, 1182, 1184, 1185, 1186, 1187, 1194, 1373, 1378, 1379, 1380, 1384, 1393, 1394, 1399, 1401, 1402, 1404, 1406, 1409, 1419, 1421, 1422, 1424, 1426, 1428, 1429, 1430, 1431, 1432, 1433, 1434, 1435, 1436, 1438, 1439, 1440, 1443, 1444, 1447, 1449, 1457, 1458, 1459, 1460, 1461, 1464, 1465, 1466, 1467, 1468, 1470, 1471, 1472, 1473, 1474, 1477, 1478, 1479, 1480, 1481, 1553, 1554, 1555, 1556, 1557, 1558, 1559, 1560, 1561, 1562, 1563, 1564, 1565, 1566, 1567, 1568, 1569, 1570, 1571, 1572, 1573, 1574, 1575, 1576, 1577, 1578, 1579, 1580, 1581, 1582, 1583, 1584, 1585, 1586, 1587, 1588, 1589, 1590, 1591, 1592, 1593, 1594, 1595, 1596, 1597, 1598, 1599, 1600, 1601, 1602, 1603, 1604, 1605, 1606, 1607, 1608, 1609, 1610, 1611, 1612, 1613, 1614, 1615, 1616, 1617, 1618, 1619, 1620, 1621, 1622, 1623, 1624, 1625, 1626, 1627, 1628, 1629, 1630, 1631, 1632, 1633, 1634, 1635, 1636, 1637, 1638, 1639, 1640, 1641, 1642, 1643, 1644, 1645, 1646, 1647, 1648, 1649, 1650, 1651, 1652, 1653, 1654, 1655, 1656, 1657, 1658, 1659, 1660, 1661, 1662, 1663, 1664, 1665, 1666, 1667, 1668, 1669, 1670, 1671, 1672, 1673, 1674, 1675, 1676, 1677, 1678, 1679, 1680, 1681, 1682, 1683, 1684, 1685, 1686, 1687, 1688, 1689, 1690, 1691, 1692, 1693, 1694, 1695, 1696, 1697, 1698, 1699, 1700, 1701, 1702, 1703, 1704, 1705, 1706, 1707, 1708, 1709, 1710, 1711, 1712, 1713, 1714, 1715, 1716, 1717, 1718, 1719, 1720, 1721, 1722, 1723, 1724, 1725, 1726, 1727, 1728, 1729, 1730, 1731, 1732, 1733, 1734, 1735, 1736, 1737, 1738, 1739, 1740, 1741, 1742, 1743, 1744, 1745, 1746, 1747, 1748, 1749, 1750, 1751, 1752, 1753, 1754, 1755, 1756, 1757, 1758, 1759, 1760, 1761, 1762, 1763, 1764, 1765, 1766, 1767, 1768, 1769, 1770, 1771, 1772, 1773, 1774, 1775, 1776, 1777, 1778, 1779, 1780, 1781, 1782, 1783, 1784, 1785, 1786, 1787, 1788, 1789, 1790, 1791, 1792, 1793, 1794, 1795, 1796, 1797, 1798, 1799, 1800, 1801, 1802, 1803, 1804, 1805, 1806, 1807, 1808, 1809, 1810, 1811, 1812, 1813, 1814, 1815, 1816, 1817, 1818, 1819, 1820, 1821, 1822, 1823, 1824, 1825, 1826, 1827, 1828, 1829, 1830, 1831, 1832, 1833, 1834, 1835, 1836, 1837, 1838, 1839, 1840, 1841, 1842, 1843, 1844, 1845, 1846, 1847, 1848, 1849, 1850, 1851, 1852, 1853, 1854, 1855, 1856, 1857, 1858, 1859, 1860, 1861, 1862, 1863, 1864, 1865, 1866, 1867, 1868, 1869, 1870, 1871, 1872, 1873, 1874, 1875, 1876, 1877, 1878, 1879, 1880, 1881, 1882, 1883, 1884, 1885, 1886, 1887, 1888, 1889, 1890, 1891, 1892, 1893, 1894, 1895, 1896, 1897, 1898, 1899, 1900, 1901, 1902, 1903, 1904, 1905, 1906, 1907, 1908, 1909, 1910, 1911, 1912, 1913, 1914, 1915, 1916, 1917, 1918, 1919, 1920, 1921, 1922, 1923, 1924, 1925, 1926, 1927, 1928, 1929, 1930, 1931, 1932, 1933, 1934, 1935, 1936, 1937, 1938, 1939, 1940, 1941, 1942, 1943, 1944, 1945, 1946, 1947, 1948, 1949, 1950, 1951, 1952, 1953, 1954, 1955, 1956, 1957, 1958, 1959, 1960, 1961, 1962, 1963, 1964, 1965, 1966, 1967, 1968, 1969, 1970, 1971, 1972, 1973, 1974, 1975, 1976, 1977, 1978, 1979, 1980, 1981, 1982, 1983, 1984, 1985, 1986, 1987, 1988, 1989, 1990, 1991, 1992, 1993, 1994, 1995, 1996, 1997, 1998, 1999, 2000, 2001, 2002, 2003, 2004, 2005, 2006, 2007, 2008, 2009, 2010, 2011, 2012, 2013, 2014, 2015, 2016, 2017, 2018, 2019, 2020, 2021, 2022, 2023, 2024, 2025, 2026, 2027, 2028, 2029, 2030, 2031, 2032, 2033, 2034, 2035, 2036, 2037, 2038, 2039, 2040, 2041, 2042, 2043, 2044, 2045, 2046, 2047, 2048, 2049, 2050, 2051, 2052, 2053, 2054, 2055, 2056, 2057, 2058, 2059, 2060, 2061, 2062, 2063, 2064, 2065, 2066, 2067, 2068, 2069, 2070, 2071, 2072, 2073, 2074, 2075, 2076, 2077, 2078, 2079, 2080, 2081, 2082, 2083, 2084, 2085, 2086, 2087, 2088, 2089, 2090, 2091, 2092, 2093, 2094, 2095, 2096, 2097, 2098, 2099, 2100, 2101, 2102, 2103, 2104, 2105, 2106, 2107, 2108, 2109, 2110, 2111, 2112, 2113, 2114, 2115, 2116, 2117, 2118, 2119, 2120, 2121, 2122, 2123, 2124, 2125, 2126, 2127, 2128, 2129, 2130, 2131, 2132, 2133, 2134, 2135, 2136, 2137, 2138, 2139, 2140, 2141, 2142, 2143, 2144, 2145, 2146, 2147, 2148, 2149, 2150, 2151, 2152, 2153, 2154, 2155, 2156, 2157, 2158, 2159, 2160, 2161, 2162, 2163, 2164, 2165, 2166, 2167, 2168, 2169, 2170, 2171, 2172, 2173, 2174, 2175, 2176, 2177, 2178, 2179, 2180, 2181, 2182, 2183, 2184, 2185, 2186, 2187, 2188, 2189, 2190, 2191, 2192, 2193, 2194, 2195, 2196, 2197, 2198, 2199, 2200, 2201, 2202, 2203, 2204, 2205, 2206, 2207, 2208, 2209, 2210, 2211, 2212, 2213, 2214, 2215, 2216, 2217, 2218, 2219, 2220, 2221, 2222, 2223, 2224, 2225, 2226, 2227, 2228, 2229, 2230, 2231, 2232, 2233, 2234, 2235, 2236, 2237, 2238, 2239, 2240, 2241, 2242, 2243, 2244, 2245, 2246, 2247, 2248, 2249, 2250, 2251, 2252, 2253, 2254, 2255, 2256, 2257, 2258, 2259, 2260, 2261, 2262, 2263, 2264, 2265, 2266, 2267, 2268, 2269, 2270, 2271, 2272, 2273, 2274, 2275, 2276, 2277, 2278, 2279, 2280, 2281, 2282, 2283, 2284, 2285, 2286, 2287, 2288, 2289, 2290, 2291, 2292, 2293, 2294, 2295, 2296, 2297, 2298, 2299, 2300, 2301, 2302, 2303, 2304, 2305, 2306, 2307, 2308, 2309, 2310, 2311, 2312, 2313, 2314, 2315, 2316, 2317, 2318, 2319, 2320, 2321, 2322, 2323, 2324, 2325, 2326, 2327, 2328, 2329, 2448, 2455, 2456, 2457, 2458, 2463, 2464, 2465, 2466, 2470, 2471, 2476, 2481, 2484, 2487, 2491, 2493, 2500, 2503, 2508, 2509, 2510, 2511, 2512, 2513, 2514, 2515, 2516, 2517, 2518, 2519, 2520, 2521, 2522, 2523, 2524, 2525, 2526, 2539, 2546, 2548, 2550, 2551, 2552, 2553, 2555, 2556, 2557, 2558, 2559, 2560, 2568, 2842, 2844, 3053, 3054, 3057, 3101, 3274, 3294, 3295, 3834, 3835, 3836, 3837, 3838, 3839, 3841, 3842, 3843, 3846, 3847, 3848, 3851, 3852, 3853, 3854, 3855, 3856, 3857, 3858, 3859, 3860, 3861, 3862, 3863, 3866, 3870, 4191, 4195, 4196, 4197, 4198, 4215, 4367, 4368, 4370, 4372, 4373, 4374, 4381, 4383, 4384, 4386, 4387, 4388, 4389, 4390, 4391, 4398, 4399, 4400, 4401, 4407, 4410, 4411, 4414, 4415, 4416, 4417, 4420, 4421, 4422, 4423, 4425, 4428, 4429, 4431, 4432, 4433, 4434, 4435, 4436, 4437, 4442, 4444, 4446, 4447, 4448, 4449, 4450, 4453, 4458, 4461, 4467, 4479, 4480, 4481, 4482, 4483, 4486, 4487, 4488, 4489, 4491, 4492, 4493, 4719, 4722, 4723, 4724, 4726, 4727, 4729, 4730, 4731, 4732, 4733, 4734, 4735, 4736, 4737, 4740, 4741, 4753, 4754, 4758, 4760, 4761, 4762, 4764, 4767, 4768, 4769, 4770, 4771, 4772, 4773, 4775, 4777, 4779, 4780, 4781, 4782, 4783, 4784, 4786, 4787, 4788, 4791, 4792, 4797, 4799, 4800, 4801, 4802, 4803, 4804, 4805, 4806, 4807, 4809, 4811, 4812, 4813, 4814, 4815, 4816, 4818, 4833, 4834, 4835, 4836, 4837, 4838, 4839, 4844, 4845, 4846, 4850, 4853, 4990, 4991, 4992, 4993, 4996, 4997, 4998, 4999, 5000, 5002, 5037, 5038, 5039, 5040, 5041, 5043, 5044, 5045, 5048, 5051, 5053, 5054, 5055, 5056, 5057, 5062, 5063, 5064, 5067, 5068, 5069, 5070, 5071, 5072, 5074, 5076, 5077, 5079, 5080, 5081, 5083, 5084, 5085, 5086, 5088, 5089, 5090, 5092, 5094, 5097, 5098, 5099, 5101, 5104, 5105, 5109, 5146, 5147, 5152, 5153, 5154, 5155, 5260, 5262, 5263, 5264, 5265, 5266, 5267, 5268, 5269, 5271, 5272, 5273, 5274, 5276, 5277, 5278, 5279, 5280, 5281, 5283, 5284, 5286, 5287, 5288, 5289, 5290, 5292, 5304, 5305, 5306, 5307, 5308, 5309, 5310, 5312, 5313]</t>
         </is>
       </c>
-      <c r="BH8" t="n">
+      <c r="BN8" t="n">
         <v>0.1502086230876217</v>
       </c>
-      <c r="BI8" t="inlineStr">
+      <c r="BO8" t="inlineStr">
         <is>
           <t>{'initial_window': 279, 'window_size': 777, 'num_trees': 29, 'max_depth': 15}</t>
         </is>
       </c>
-      <c r="BJ8" t="n">
+      <c r="BP8" t="n">
         <v>21.3299277019687</v>
       </c>
-      <c r="BK8" t="inlineStr">
+      <c r="BQ8" t="inlineStr">
         <is>
           <t>[333, 334, 342, 348, 351, 382, 621, 633, 643, 647, 648, 652, 653, 659, 675, 676, 677, 687, 690, 1235, 1236, 1238, 1241, 1243, 1248, 1253, 1254, 1256, 1258, 1260, 1264, 1266, 1272, 1275, 1276, 1281, 1288, 1467, 1487, 1493, 1500, 1516, 1518, 1520, 1522, 1529, 1532, 1534, 1538, 1541, 1553, 1558, 1562, 1567, 1568, 1571, 1575, 1776, 2328, 2329, 2332, 2333, 2339, 2341, 2343, 2344, 2379, 2552, 2563, 2565, 2587, 2593, 2594, 2596, 2597, 2601, 2602, 2604, 2605, 2606, 2608, 2609, 2612, 2620, 2633, 2640, 2662, 2938, 3146, 3147, 3151, 3194, 3195, 3367, 3368, 3929, 3931, 3935, 3947, 4290, 4292, 4309, 4460, 4461, 4466, 4475, 4480, 4482, 4492, 4500, 4501, 4514, 4515, 4516, 4518, 4519, 4531, 4552, 4554, 4555, 4579, 4580, 4586, 4587, 4818, 4819, 4823, 4826, 4829, 4830, 4835, 4851, 4854, 4867, 4868, 4880, 4881, 4892, 4900, 4901, 4906, 4931, 4939, 4940, 4946, 4947, 5085, 5090, 5093, 5094, 5095, 5148, 5149, 5155, 5156, 5166, 5169, 5170, 5174, 5175, 5176, 5180, 5182, 5184, 5185, 5186, 5188, 5191, 5192, 5194, 5195, 5198, 5239, 5240, 5241]</t>
         </is>
       </c>
-      <c r="BL8" t="n">
+      <c r="BR8" t="n">
         <v>0.09326424870466322</v>
       </c>
-      <c r="BM8" t="inlineStr">
+      <c r="BS8" t="inlineStr">
         <is>
           <t>{'AR_window_size': 93, 'differencing-order': 0}</t>
         </is>
       </c>
-      <c r="BN8" t="n">
+      <c r="BT8" t="n">
         <v>231.0503054440487</v>
       </c>
-      <c r="BO8" t="inlineStr">
+      <c r="BU8" t="inlineStr">
         <is>
           <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86, 87, 88, 89, 90, 91, 92, 93, 94, 95, 96, 97, 98, 99, 100, 101, 102, 103, 104, 105, 106, 107, 108, 109, 110, 111, 112, 113, 114, 115, 116, 117, 118, 119, 120, 121, 122, 123, 124, 125, 126, 127, 128, 129, 130, 131, 132, 133, 134, 135, 136, 137, 138, 139, 140, 141, 142, 143, 144, 145, 146, 147, 148, 149, 150, 151, 152, 153, 154, 155, 156, 157, 158, 159, 160, 161, 162, 163, 164, 165, 166, 167, 168, 169, 170, 171, 172, 173, 174, 175, 176, 177, 178, 179, 180, 181, 182, 183, 184, 185, 186, 187, 188, 189, 190, 191, 192, 193, 194, 195, 196, 197, 198, 199, 200, 201, 202, 203, 204, 205, 206, 207, 208, 209, 210, 211, 212, 213, 214, 215, 216, 217, 218, 219, 220, 221, 222, 223, 224, 225, 226, 227, 228, 229, 230, 231, 232, 233, 234, 235, 236, 237, 238, 239, 240, 241, 242, 243, 244, 245, 246, 247, 248, 249, 250, 251, 252, 253, 254, 255, 256, 257, 258, 259, 260, 261, 262, 263, 264, 265, 266, 267, 268, 269, 270, 271, 272, 273, 274, 275, 276, 277, 278, 279, 280, 281, 282, 283, 284, 285, 286, 287, 288, 289, 290, 291, 292, 293, 294, 295, 296, 297, 298, 299, 300, 301, 302, 303, 304, 305, 306, 307, 308, 309, 310, 311, 312, 313, 314, 315, 316, 317, 318, 319, 320, 321, 322, 323, 324, 325, 326, 327, 328, 329, 330, 331, 332, 333, 334, 335, 336, 337, 338, 339, 340, 341, 342, 343, 344, 345, 346, 347, 348, 349, 350, 351, 352, 353, 354, 355, 356, 357, 358, 359, 360, 361, 362, 363, 364, 365, 366, 367, 368, 369, 370, 371, 372, 373, 374, 375, 376, 377, 378, 379, 380, 381, 382, 383, 384, 385, 386, 387, 388, 389, 390, 391, 392, 393, 394, 395, 396, 397, 398, 399, 400, 401, 402, 403, 404, 405, 406, 407, 408, 409, 410, 411, 412, 413, 414, 415, 416, 417, 418, 419, 420, 421, 422, 423, 424, 425, 426, 427, 428, 429, 430, 431, 432, 433, 434, 435, 436, 437, 438, 439, 440, 441, 442, 443, 444, 445, 446, 447, 448, 449, 450, 451, 452, 453, 454, 455, 456, 457, 458, 459, 460, 461, 462, 463, 464, 465, 466, 467, 468, 469, 470, 471, 472, 473, 474, 475, 476, 477, 478, 479, 480, 481, 482, 483, 484, 485, 486, 487, 488, 489, 490, 491, 492, 493, 494, 495, 496, 497, 498, 499, 500, 501, 502, 503, 504, 505, 506, 507, 508, 509, 510, 511, 512, 513, 514, 515, 516, 517, 518, 519, 520, 521, 522, 523, 524, 525, 526, 527, 528, 529, 530, 531, 532, 533, 534, 535, 536, 537, 538, 539, 540, 541, 542, 543, 544, 545, 546, 547, 548, 549, 550, 551, 552, 553, 554, 555, 556, 557, 558, 559, 560, 561, 562, 563, 564, 565, 566, 567, 568, 569, 570, 571, 572, 573, 574, 576, 577, 578, 579, 580, 581, 582, 583, 584, 585, 586, 587, 588, 589, 590, 591, 592, 594, 595, 596, 597, 598, 599, 600, 601, 602, 603, 604, 605, 606, 607, 608, 609, 610, 611, 612, 613, 614, 615, 616, 617, 618, 619, 620, 621, 622, 623, 624, 625, 626, 627, 628, 629, 630, 631, 632, 633, 634, 635, 636, 637, 638, 639, 640, 641, 642, 643, 644, 645, 646, 647, 648, 649, 650, 651, 652, 653, 654, 655, 656, 657, 658, 659, 660, 661, 662, 663, 664, 665, 666, 667, 668, 669, 670, 671, 672, 673, 674, 675, 676, 677, 678, 679, 680, 681, 682, 683, 684, 685, 686, 687, 688, 689, 690, 691, 692, 693, 694, 695, 696, 697, 698, 699, 700, 701, 702, 703, 704, 705, 706, 707, 708, 709, 710, 711, 712, 713, 714, 715, 716, 717, 718, 719, 720, 721, 722, 723, 724, 725, 726, 727, 728, 729, 730, 731, 732, 733, 734, 735, 736, 737, 738, 739, 740, 741, 742, 743, 744, 745, 746, 747, 748, 749, 750, 751, 752, 753, 754, 755, 756, 757, 758, 759, 760, 761, 762, 763, 764, 765, 766, 767, 768, 769, 770, 771, 772, 773, 774, 775, 776, 777, 778, 779, 780, 781, 782, 783, 784, 785, 786, 787, 788, 789, 790, 791, 792, 793, 794, 795, 796, 797, 798, 799, 800, 801, 802, 803, 804, 805, 806, 807, 808, 809, 810, 811, 812, 813, 814, 815, 816, 817, 818, 819, 820, 821, 822, 823, 824, 825, 826, 827, 828, 829, 830, 831, 832, 833, 834, 835, 836, 837, 838, 839, 840, 841, 842, 843, 844, 845, 846, 847, 848, 849, 850, 851, 852, 853, 854, 855, 856, 857, 858, 859, 860, 861, 862, 863, 864, 865, 866, 867, 868, 869, 870, 871, 872, 873, 874, 875, 876, 877, 878, 879, 880, 881, 882, 883, 884, 885, 886, 887, 888, 889, 890, 891, 892, 893, 894, 895, 896, 897, 898, 899, 900, 901, 902, 903, 904, 905, 906, 907, 908, 909, 910, 911, 912, 913, 914, 915, 916, 917, 918, 919, 920, 921, 922, 923, 924, 925, 926, 927, 928, 929, 930, 931, 932, 933, 934, 935, 936, 937, 938, 939, 940, 941, 942, 943, 944, 945, 946, 947, 948, 949, 950, 951, 952, 953, 954, 955, 956, 957, 958, 959, 960, 961, 962, 963, 964, 965, 966, 967, 968, 969, 970, 971, 972, 973, 974, 975, 976, 977, 978, 979, 980, 981, 982, 983, 984, 985, 986, 987, 988, 989, 990, 991, 992, 993, 994, 995, 996, 997, 998, 999, 1000, 1001, 1002, 1003, 1004, 1005, 1006, 1007, 1008, 1009, 1010, 1011, 1012, 1013, 1014, 1015, 1016, 1017, 1018, 1019, 1020, 1021, 1022, 1023, 1024, 1025, 1026, 1027, 1028, 1029, 1030, 1031, 1032, 1033, 1034, 1035, 1036, 1037, 1038, 1039, 1040, 1041, 1042, 1043, 1044, 1045, 1046, 1047, 1048, 1049, 1050, 1051, 1052, 1053, 1054, 1055, 1056, 1057, 1058, 1059, 1060, 1061, 1062, 1063, 1064, 1065, 1066, 1067, 1068, 1069, 1070, 1071, 1072, 1073, 1074, 1075, 1076, 1077, 1078, 1079, 1080, 1081, 1082, 1083, 1084, 1085, 1086, 1087, 1088, 1089, 1090, 1091, 1092, 1093, 1094, 1095, 1096, 1097, 1098, 1099, 1100, 1101, 1102, 1103, 1104, 1105, 1106, 1107, 1108, 1109, 1110, 1111, 1112, 1113, 1114, 1115, 1116, 1117, 1118, 1119, 1120, 1121, 1122, 1123, 1124, 1125, 1126, 1127, 1128, 1129, 1130, 1131, 1132, 1133, 1134, 1135, 1136, 1137, 1138, 1139, 1140, 1141, 1142, 1143, 1144, 1145, 1146, 1147, 1149, 1150, 1151, 1152, 1153, 1154, 1155, 1156, 1157, 1158, 1159, 1160, 1161, 1162, 1163, 1164, 1165, 1166, 1167, 1168, 1169, 1171, 1173, 1174, 1175, 1176, 1177, 1178, 1179, 1180, 1181, 1182, 1183, 1184, 1185, 1186, 1187, 1188, 1189, 1190, 1191, 1192, 1193, 1194, 1195, 1196, 1197, 1198, 1199, 1200, 1201, 1202, 1203, 1204, 1205, 1206, 1207, 1208, 1209, 1210, 1211, 1212, 1213, 1214, 1215, 1216, 1217, 1218, 1219, 1220, 1221, 1222, 1223, 1224, 1225, 1226, 1227, 1228, 1229, 1230, 1231, 1232, 1233, 1234, 1235, 1236, 1237, 1238, 1239, 1240, 1241, 1242, 1243, 1244, 1245, 1246, 1247, 1248, 1249, 1250, 1251, 1252, 1253, 1254, 1255, 1256, 1257, 1258, 1259, 1260, 1261, 1262, 1263, 1264, 1265, 1266, 1267, 1268, 1269, 1270, 1271, 1272, 1273, 1274, 1275, 1276, 1277, 1278, 1279, 1280, 1281, 1282, 1283, 1284, 1285, 1286, 1287, 1288, 1289, 1290, 1291, 1292, 1293, 1294, 1295, 1296, 1297, 1298, 1299, 1300, 1301, 1302, 1303, 1304, 1305, 1306, 1307, 1308, 1309, 1310, 1311, 1312, 1313, 1314, 1315, 1316, 1317, 1318, 1319, 1320, 1321, 1322, 1323, 1324, 1325, 1326, 1327, 1328, 1329, 1330, 1331, 1332, 1333, 1334, 1335, 1336, 1337, 1338, 1339, 1340, 1341, 1342, 1343, 1344, 1345, 1346, 1347, 1348, 1349, 1350, 1351, 1352, 1353, 1354, 1355, 1356, 1357, 1358, 1359, 1360, 1361, 1362, 1363, 1364, 1365, 1366, 1367, 1368, 1369, 1370, 1371, 1372, 1373, 1374, 1375, 1376, 1377, 1378, 1379, 1381, 1382, 1383, 1384, 1385, 1386, 1387, 1388, 1389, 1390, 1391, 1392, 1393, 1394, 1395, 1396, 1397, 1398, 1399, 1400, 1401, 1402, 1403, 1404, 1405, 1406, 1407, 1408, 1409, 1410, 1411, 1412, 1413, 1414, 1415, 1416, 1417, 1418, 1419, 1420, 1421, 1422, 1423, 1424, 1425, 1426, 1427, 1428, 1429, 1430, 1431, 1432, 1433, 1434, 1435, 1436, 1437, 1438, 1439, 1440, 1441, 1442, 1443, 1444, 1445, 1446, 1447, 1448, 1449, 1450, 1451, 1452, 1453, 1454, 1455, 1456, 1457, 1458, 1459, 1460, 1461, 1462, 1463, 1464, 1465, 1466, 1467, 1468, 1469, 1470, 1471, 1472, 1473, 1474, 1475, 1476, 1477, 1478, 1479, 1480, 1481, 1482, 1483, 1484, 1485, 1486, 1487, 1488, 1489, 1490, 1491, 1492, 1493, 1494, 1495, 1496, 1497, 1498, 1499, 1500, 1501, 1502, 1503, 1504, 1505, 1506, 1507, 1508, 1509, 1510, 1511, 1512, 1513, 1514, 1515, 1516, 1517, 1518, 1519, 1520, 1521, 1522, 1523, 1524, 1525, 1526, 1527, 1528, 1529, 1530, 1531, 1532, 1533, 1534, 1535, 1536, 1537, 1538, 1539, 1540, 1541, 1542, 1543, 1544, 1545, 1546, 1547, 1548, 1549, 1550, 1551, 1552, 1553, 1554, 1555, 1556, 1557, 1558, 1559, 1560, 1561, 1562, 1563, 1564, 1565, 1566, 1567, 1568, 1569, 1570, 1571, 1572, 1573, 1574, 1575, 1576, 1577, 1578, 1579, 1580, 1581, 1582, 1583, 1584, 1585, 1586, 1587, 1588, 1589, 1590, 1591, 1592, 1593, 1594, 1595, 1596, 1597, 1598, 1599, 1600, 1601, 1602, 1603, 1604, 1605, 1606, 1607, 1608, 1609, 1610, 1611, 1612, 1613, 1614, 1615, 1616, 1617, 1618, 1619, 1620, 1621, 1622, 1623, 1624, 1625, 1626, 1627, 1628, 1629, 1630, 1631, 1632, 1633, 1634, 1635, 1636, 1637, 1638, 1639, 1640, 1641, 1642, 1643, 1644, 1645, 1646, 1647, 1648, 1649, 1650, 1651, 1652, 1653, 1654, 1655, 1656, 1657, 1658, 1659, 1660, 1661, 1662, 1663, 1664, 1665, 1666, 1667, 1668, 1669, 1670, 1671, 1672, 1673, 1674, 1675, 1676, 1677, 1678, 1679, 1680, 1681, 1682, 1683, 1684, 1685, 1686, 1687, 1688, 1689, 1690, 1691, 1692, 1693, 1694, 1695, 1696, 1697, 1698, 1699, 1700, 1701, 1702, 1703, 1704, 1705, 1706, 1707, 1708, 1709, 1710, 1711, 1712, 1713, 1714, 1715, 1716, 1717, 1718, 1719, 1720, 1721, 1722, 1723, 1724, 1725, 1726, 1727, 1728, 1729, 1730, 1731, 1732, 1733, 1734, 1735, 1736, 1737, 1738, 1739, 1740, 1741, 1742, 1743, 1744, 1745, 1746, 1747, 1748, 1749, 1750, 1751, 1752, 1753, 1754, 1755, 1756, 1757, 1758, 1759, 1760, 1761, 1762, 1763, 1764, 1765, 1766, 1767, 1768, 1769, 1770, 1771, 1772, 1773, 1774, 1775, 1776, 1777, 1778, 1779, 1780, 1781, 1782, 1783, 1784, 1785, 1786, 1787, 1788, 1789, 1790, 1791, 1792, 1793, 1794, 1795, 1796, 1797, 1798, 1799, 1800, 1801, 1802, 1803, 1804, 1805, 1806, 1807, 1808, 1809, 1810, 1811, 1812, 1813, 1814, 1815, 1816, 1817, 1818, 1819, 1820, 1821, 1822, 1823, 1824, 1825, 1826, 1827, 1828, 1829, 1830, 1831, 1832, 1833, 1834, 1835, 1836, 1837, 1838, 1839, 1840, 1841, 1842, 1843, 1844, 1845, 1846, 1847, 1848, 1849, 1850, 1851, 1852, 1853, 1854, 1855, 1856, 1857, 1858, 1859, 1860, 1861, 1862, 1863, 1864, 1865, 1866, 1867, 1868, 1869, 1870, 1871, 1872, 1873, 1874, 1875, 1876, 1877, 1878, 1879, 1880, 1881, 1882, 1883, 1884, 1885, 1886, 1887, 1888, 1889, 1890, 1891, 1892, 1893, 1894, 1895, 1896, 1897, 1898, 1899, 1900, 1901, 1902, 1903, 1904, 1905, 1906, 1907, 1908, 1909, 1910, 1911, 1912, 1913, 1914, 1915, 1916, 1917, 1918, 1919, 1920, 1921, 1922, 1923, 1924, 1925, 1926, 1927, 1928, 1929, 1930, 1931, 1932, 1933, 1934, 1935, 1936, 1937, 1938, 1939, 1940, 1941, 1942, 1943, 1944, 1945, 1946, 1947, 1948, 1949, 1950, 1951, 1952, 1953, 1954, 1955, 1956, 1957, 1958, 1959, 1960, 1961, 1962, 1963, 1964, 1965, 1966, 1967, 1968, 1969, 1970, 1971, 1972, 1973, 1974, 1975, 1976, 1977, 1978, 1979, 1980, 1981, 1982, 1983, 1984, 1985, 1986, 1987, 1988, 1989, 1990, 1991, 1992, 1993, 1994, 1995, 1996, 1997, 1998, 1999, 2000, 2001, 2002, 2003, 2004, 2005, 2006, 2007, 2008, 2009, 2010, 2011, 2012, 2013, 2014, 2015, 2016, 2017, 2018, 2019, 2020, 2021, 2022, 2023, 2024, 2025, 2026, 2027, 2028, 2029, 2030, 2031, 2032, 2033, 2034, 2035, 2036, 2037, 2038, 2039, 2040, 2041, 2042, 2043, 2044, 2045, 2046, 2047, 2048, 2049, 2050, 2051, 2052, 2053, 2054, 2055, 2056, 2057, 2058, 2059, 2060, 2061, 2062, 2063, 2064, 2065, 2066, 2067, 2068, 2069, 2070, 2071, 2072, 2073, 2074, 2075, 2076, 2077, 2078, 2079, 2080, 2081, 2082, 2083, 2084, 2085, 2086, 2087, 2088, 2089, 2090, 2091, 2092, 2093, 2094, 2095, 2096, 2097, 2098, 2099, 2100, 2101, 2102, 2103, 2104, 2105, 2106, 2107, 2108, 2109, 2110, 2111, 2112, 2113, 2114, 2115, 2116, 2117, 2118, 2119, 2120, 2121, 2122, 2123, 2124, 2125, 2126, 2127, 2128, 2129, 2130, 2131, 2132, 2133, 2134, 2135, 2136, 2137, 2138, 2139, 2140, 2141, 2142, 2143, 2144, 2145, 2146, 2147, 2148, 2149, 2150, 2151, 2152, 2153, 2154, 2155, 2156, 2157, 2158, 2159, 2160, 2161, 2162, 2163, 2164, 2165, 2166, 2167, 2168, 2169, 2170, 2171, 2172, 2173, 2174, 2175, 2176, 2177, 2178, 2179, 2180, 2181, 2182, 2183, 2184, 2185, 2186, 2187, 2188, 2189, 2190, 2191, 2192, 2193, 2194, 2195, 2196, 2197, 2198, 2199, 2200, 2201, 2202, 2203, 2204, 2205, 2206, 2207, 2208, 2209, 2210, 2211, 2212, 2213, 2214, 2215, 2216, 2217, 2218, 2219, 2220, 2221, 2222, 2223, 2224, 2225, 2226, 2227, 2228, 2229, 2230, 2231, 2232, 2233, 2234, 2235, 2236, 2237, 2238, 2239, 2240, 2241, 2242, 2243, 2244, 2245, 2246, 2247, 2248, 2249, 2250, 2251, 2252, 2253, 2254, 2255, 2256, 2257, 2258, 2259, 2260, 2261, 2262, 2263, 2264, 2265, 2266, 2267, 2268, 2269, 2270, 2271, 2272, 2273, 2274, 2275, 2276, 2277, 2278, 2279, 2280, 2281, 2282, 2283, 2284, 2285, 2286, 2287, 2288, 2289, 2290, 2291, 2292, 2293, 2294, 2295, 2296, 2297, 2298, 2299, 2300, 2301, 2302, 2303, 2304, 2305, 2306, 2307, 2308, 2309, 2310, 2311, 2312, 2313, 2314, 2315, 2316, 2317, 2318, 2319, 2320, 2321, 2322, 2323, 2324, 2325, 2326, 2327, 2328, 2329, 2330, 2331, 2332, 2333, 2334, 2335, 2336, 2337, 2338, 2339, 2340, 2341, 2342, 2343, 2344, 2345, 2346, 2347, 2348, 2349, 2350, 2351, 2352, 2353, 2354, 2355, 2356, 2357, 2358, 2359, 2360, 2361, 2362, 2363, 2364, 2365, 2366, 2367, 2368, 2369, 2370, 2371, 2372, 2373, 2374, 2375, 2376, 2377, 2378, 2379, 2380, 2381, 2382, 2383, 2384, 2385, 2386, 2387, 2388, 2389, 2390, 2391, 2392, 2393, 2394, 2395, 2396, 2397, 2398, 2399, 2400, 2401, 2402, 2403, 2404, 2405, 2406, 2407, 2408, 2409, 2410, 2411, 2412, 2413, 2414, 2415, 2416, 2417, 2418, 2419, 2420, 2421, 2422, 2423, 2424, 2425, 2426, 2427, 2428, 2429, 2430, 2431, 2432, 2433, 2434, 2435, 2436, 2437, 2438, 2439, 2440, 2441, 2442, 2443, 2444, 2445, 2446, 2447, 2448, 2449, 2450, 2451, 2452, 2453, 2454, 2455, 2456, 2457, 2458, 2459, 2460, 2461, 2462, 2463, 2464, 2465, 2467, 2468, 2469, 2470, 2471, 2472, 2473, 2474, 2475, 2476, 2477, 2478, 2479, 2480, 2481, 2482, 2483, 2484, 2485, 2486, 2487, 2488, 2489, 2490, 2491, 2492, 2493, 2494, 2495, 2496, 2497, 2498, 2499, 2500, 2501, 2502, 2503, 2504, 2505, 2506, 2507, 2509, 2510, 2511, 2512, 2513, 2514, 2516, 2517, 2518, 2519, 2520, 2521, 2522, 2523, 2524, 2525, 2526, 2527, 2528, 2529, 2530, 2531, 2532, 2533, 2534, 2535, 2536, 2537, 2538, 2539, 2540, 2541, 2542, 2543, 2544, 2545, 2546, 2547, 2548, 2549, 2550, 2551, 2552, 2553, 2554, 2555, 2556, 2557, 2558, 2559, 2560, 2561, 2562, 2563, 2564, 2565, 2566, 2567, 2568, 2569, 2570, 2571, 2572, 2573, 2574, 2575, 2576, 2577, 2578, 2579, 2580, 2581, 2582, 2583, 2584, 2585, 2586, 2587, 2588, 2589, 2590, 2591, 2592, 2593, 2594, 2595, 2596, 2597, 2598, 2599, 2600, 2601, 2602, 2603, 2604, 2605, 2606, 2607, 2608, 2609, 2610, 2611, 2612, 2613, 2614, 2615, 2616, 2617, 2618, 2619, 2620, 2621, 2622, 2623, 2624, 2625, 2626, 2627, 2628, 2629, 2630, 2631, 2632, 2633, 2634, 2635, 2636, 2637, 2638, 2639, 2640, 2641, 2642, 2643, 2644, 2645, 2646, 2647, 2648, 2649, 2650, 2651, 2652, 2653, 2654, 2655, 2656, 2657, 2658, 2659, 2660, 2661, 2662, 2663, 2664, 2665, 2666, 2667, 2668, 2669, 2670, 2671, 2672, 2673, 2674, 2675, 2676, 2677, 2678, 2679, 2680, 2681, 2682, 2683, 2684, 2685, 2686, 2687, 2688, 2689, 2690, 2691, 2692, 2693, 2694, 2695, 2696, 2697, 2698, 2699, 2700, 2701, 2702, 2703, 2704, 2705, 2706, 2707, 2708, 2709, 2710, 2711, 2712, 2713, 2714, 2715, 2716, 2717, 2718, 2719, 2720, 2721, 2722, 2723, 2724, 2725, 2726, 2727, 2728, 2729, 2730, 2731, 2732, 2733, 2734, 2735, 2736, 2737, 2738, 2739, 2740, 2741, 2742, 2743, 2744, 2745, 2746, 2747, 2748, 2749, 2750, 2751, 2752, 2753, 2754, 2755, 2756, 2757, 2758, 2759, 2760, 2761, 2762, 2763, 2764, 2765, 2766, 2767, 2768, 2769, 2770, 2771, 2772, 2773, 2774, 2775, 2776, 2777, 2778, 2779, 2780, 2781, 2782, 2783, 2784, 2785, 2786, 2787, 2788, 2789, 2790, 2791, 2792, 2793, 2794, 2795, 2796, 2797, 2798, 2799, 2800, 2801, 2802, 2803, 2804, 2805, 2806, 2807, 2808, 2809, 2810, 2811, 2812, 2813, 2814, 2815, 2816, 2817, 2818, 2819, 2820, 2821, 2822, 2823, 2824, 2825, 2826, 2827, 2828, 2829, 2830, 2831, 2832, 2833, 2834, 2835, 2836, 2837, 2838, 2839, 2840, 2841, 2842, 2843, 2844, 2845, 2846, 2847, 2848, 2849, 2850, 2851, 2852, 2853, 2854, 2855, 2856, 2857, 2858, 2859, 2860, 2861, 2862, 2863, 2864, 2865, 2866, 2867, 2868, 2869, 2870, 2871, 2872, 2873, 2874, 2875, 2876, 2877, 2878, 2879, 2880, 2881, 2882, 2883, 2884, 2885, 2886, 2887, 2888, 2889, 2890, 2891, 2892, 2893, 2894, 2895, 2896, 2897, 2898, 2899, 2900, 2901, 2902, 2903, 2904, 2905, 2906, 2907, 2908, 2909, 2910, 2911, 2912, 2913, 2914, 2915, 2916, 2917, 2918, 2919, 2920, 2921, 2922, 2923, 2924, 2925, 2926, 2927, 2928, 2929, 2930, 2931, 2932, 2933, 2934, 2935, 2936, 2937, 2938, 2939, 2940, 2941, 2942, 2943, 2944, 2945, 2946, 2947, 2948, 2949, 2950, 2951, 2952, 2953, 2954, 2955, 2956, 2957, 2958, 2959, 2960, 2961, 2962, 2963, 2964, 2965, 2966, 2967, 2968, 2969, 2970, 2971, 2972, 2973, 2974, 2975, 2976, 2977, 2978, 2979, 2980, 2981, 2982, 2983, 2984, 2985, 2986, 2987, 2988, 2989, 2990, 2991, 2992, 2993, 2994, 2995, 2996, 2997, 2998, 2999, 3000, 3001, 3002, 3003, 3004, 3005, 3006, 3007, 3008, 3009, 3010, 3011, 3012, 3013, 3014, 3015, 3016, 3017, 3018, 3019, 3020, 3021, 3022, 3023, 3024, 3025, 3026, 3027, 3028, 3029, 3030, 3031, 3032, 3033, 3034, 3035, 3036, 3037, 3038, 3039, 3040, 3041, 3042, 3043, 3044, 3045, 3046, 3047, 3048, 3049, 3050, 3051, 3052, 3053, 3054, 3055, 3056, 3057, 3058, 3059, 3060, 3061, 3062, 3063, 3064, 3065, 3066, 3067, 3068, 3069, 3070, 3071, 3072, 3073, 3074, 3075, 3076, 3077, 3078, 3079, 3080, 3081, 3082, 3083, 3084, 3085, 3086, 3087, 3088, 3089, 3090, 3091, 3092, 3093, 3094, 3095, 3096, 3097, 3098, 3099, 3100, 3102, 3103, 3104, 3105, 3106, 3107, 3108, 3109, 3110, 3111, 3112, 3113, 3114, 3115, 3116, 3117, 3118, 3119, 3120, 3121, 3122, 3123, 3124, 3125, 3126, 3127, 3128, 3129, 3130, 3131, 3132, 3133, 3134, 3135, 3136, 3137, 3138, 3139, 3140, 3141, 3142, 3143, 3144, 3145, 3146, 3147, 3148, 3149, 3150, 3151, 3152, 3153, 3154, 3155, 3156, 3157, 3158, 3159, 3160, 3161, 3162, 3163, 3164, 3165, 3166, 3167, 3168, 3169, 3170, 3171, 3172, 3173, 3174, 3175, 3176, 3177, 3178, 3179, 3180, 3181, 3182, 3183, 3184, 3185, 3186, 3187, 3188, 3189, 3190, 3191, 3192, 3193, 3194, 3195, 3196, 3197, 3198, 3199, 3200, 3201, 3202, 3203, 3204, 3205, 3206, 3207, 3208, 3209, 3210, 3211, 3212, 3213, 3214, 3215, 3216, 3217, 3218, 3219, 3220, 3221, 3222, 3223, 3224, 3225, 3226, 3227, 3228, 3229, 3230, 3231, 3232, 3233, 3234, 3235, 3236, 3237, 3238, 3239, 3240, 3241, 3242, 3243, 3244, 3245, 3246, 3247, 3248, 3249, 3250, 3251, 3252, 3253, 3254, 3255, 3256, 3257, 3258, 3259, 3260, 3261, 3262, 3263, 3264, 3265, 3266, 3267, 3268, 3269, 3270, 3271, 3272, 3273, 3275, 3276, 3277, 3278, 3279, 3280, 3281, 3282, 3283, 3284, 3285, 3286, 3287, 3288, 3289, 3290, 3291, 3292, 3293, 3294, 3295, 3296, 3297, 3298, 3299, 3300, 3301, 3302, 3303, 3304, 3305, 3306, 3307, 3308, 3309, 3310, 3311, 3312, 3313, 3314, 3315, 3316, 3317, 3318, 3319, 3320, 3321, 3322, 3323, 3324, 3325, 3326, 3327, 3328, 3329, 3330, 3331, 3332, 3333, 3334, 3335, 3336, 3337, 3338, 3339, 3340, 3341, 3342, 3343, 3344, 3345, 3346, 3347, 3348, 3349, 3350, 3351, 3352, 3353, 3354, 3355, 3356, 3357, 3358, 3359, 3360, 3361, 3362, 3363, 3364, 3365, 3366, 3367, 3368, 3369, 3370, 3371, 3372, 3373, 3374, 3375, 3376, 3377, 3378, 3379, 3380, 3381, 3382, 3383, 3384, 3385, 3386, 3387, 3388, 3389, 3390, 3391, 3392, 3393, 3394, 3395, 3396, 3397, 3398, 3399, 3400, 3401, 3402, 3403, 3404, 3405, 3406, 3407, 3408, 3409, 3410, 3411, 3412, 3413, 3414, 3415, 3416, 3417, 3418, 3419, 3420, 3421, 3422, 3423, 3424, 3425, 3426, 3427, 3428, 3429, 3430, 3431, 3432, 3433, 3434, 3435, 3436, 3437, 3438, 3439, 3440, 3441, 3442, 3443, 3444, 3445, 3446, 3447, 3448, 3449, 3450, 3451, 3452, 3453, 3454, 3455, 3456, 3457, 3458, 3459, 3460, 3461, 3462, 3463, 3464, 3465, 3466, 3467, 3468, 3469, 3470, 3471, 3472, 3473, 3474, 3475, 3476, 3477, 3478, 3479, 3480, 3481, 3482, 3483, 3484, 3485, 3486, 3487, 3488, 3489, 3490, 3491, 3492, 3493, 3494, 3495, 3496, 3497, 3498, 3499, 3500, 3501, 3502, 3503, 3504, 3505, 3506, 3507, 3508, 3509, 3510, 3511, 3512, 3513, 3514, 3515, 3516, 3517, 3518, 3519, 3520, 3521, 3522, 3523, 3524, 3525, 3526, 3527, 3528, 3529, 3530, 3531, 3532, 3533, 3534, 3535, 3536, 3537, 3538, 3539, 3540, 3541, 3542, 3543, 3544, 3545, 3546, 3547, 3548, 3549, 3550, 3551, 3552, 3553, 3554, 3555, 3556, 3557, 3558, 3559, 3560, 3561, 3562, 3563, 3564, 3565, 3566, 3567, 3568, 3569, 3570, 3571, 3572, 3573, 3574, 3575, 3576, 3577, 3578, 3579, 3580, 3581, 3582, 3583, 3584, 3585, 3586, 3587, 3588, 3589, 3590, 3591, 3592, 3593, 3594, 3595, 3596, 3597, 3598, 3599, 3600, 3601, 3602, 3603, 3604, 3605, 3606, 3607, 3608, 3609, 3610, 3611, 3612, 3613, 3614, 3615, 3616, 3617, 3618, 3619, 3620, 3621, 3622, 3623, 3624, 3625, 3626, 3627, 3628, 3629, 3630, 3631, 3632, 3633, 3634, 3635, 3636, 3637, 3638, 3639, 3640, 3641, 3642, 3643, 3644, 3645, 3646, 3647, 3648, 3649, 3650, 3651, 3652, 3653, 3654, 3655, 3656, 3657, 3658, 3659, 3660, 3661, 3662, 3663, 3664, 3665, 3666, 3667, 3668, 3669, 3670, 3671, 3672, 3673, 3674, 3675, 3676, 3677, 3678, 3679, 3680, 3681, 3682, 3683, 3684, 3685, 3686, 3687, 3688, 3689, 3690, 3691, 3692, 3693, 3694, 3695, 3696, 3697, 3698, 3699, 3700, 3701, 3702, 3703, 3704, 3705, 3706, 3707, 3708, 3709, 3710, 3711, 3712, 3713, 3714, 3715, 3716, 3717, 3718, 3719, 3720, 3721, 3722, 3723, 3724, 3725, 3726, 3727, 3728, 3729, 3730, 3731, 3732, 3733, 3734, 3735, 3736, 3737, 3738, 3739, 3740, 3741, 3742, 3743, 3744, 3745, 3746, 3747, 3748, 3749, 3750, 3751, 3752, 3753, 3754, 3755, 3756, 3757, 3758, 3759, 3760, 3761, 3762, 3763, 3764, 3765, 3766, 3767, 3768, 3769, 3770, 3771, 3772, 3773, 3774, 3775, 3776, 3777, 3778, 3779, 3780, 3781, 3782, 3783, 3784, 3785, 3786, 3787, 3788, 3789, 3790, 3791, 3792, 3793, 3794, 3795, 3796, 3797, 3798, 3799, 3800, 3801, 3802, 3803, 3804, 3805, 3806, 3807, 3808, 3809, 3810, 3811, 3812, 3813, 3814, 3815, 3816, 3817, 3818, 3819, 3820, 3821, 3822, 3823, 3824, 3825, 3826, 3827, 3828, 3829, 3830, 3831, 3832, 3833, 3834, 3835, 3836, 3837, 3838, 3839, 3840, 3841, 3842, 3843, 3844, 3845, 3846, 3847, 3848, 3849, 3850, 3851, 3852, 3853, 3854, 3855, 3856, 3857, 3858, 3859, 3860, 3861, 3862, 3863, 3864, 3865, 3866, 3867, 3868, 3869, 3870, 3871, 3872, 3873, 3874, 3875, 3876, 3877, 3878, 3879, 3880, 3881, 3882, 3883, 3884, 3885, 3886, 3887, 3888, 3889, 3890, 3891, 3892, 3893, 3894, 3895, 3896, 3897, 3898, 3899, 3900, 3901, 3902, 3903, 3904, 3905, 3906, 3907, 3908, 3909, 3910, 3911, 3912, 3913, 3914, 3915, 3916, 3917, 3918, 3919, 3920, 3921, 3922, 3923, 3924, 3925, 3926, 3927, 3928, 3929, 3930, 3931, 3932, 3933, 3934, 3935, 3936, 3937, 3938, 3939, 3940, 3941, 3942, 3943, 3944, 3945, 3946, 3947, 3948, 3949, 3950, 3951, 3952, 3953, 3954, 3955, 3956, 3957, 3958, 3959, 3960, 3961, 3962, 3963, 3964, 3965, 3966, 3967, 3968, 3969, 3970, 3971, 3972, 3973, 3974, 3975, 3976, 3977, 3978, 3979, 3980, 3981, 3982, 3983, 3984, 3985, 3986, 3987, 3988, 3989, 3990, 3991, 3992, 3993, 3994, 3995, 3996, 3997, 3998, 3999, 4000, 4001, 4002, 4003, 4004, 4005, 4006, 4007, 4008, 4009, 4010, 4011, 4012, 4013, 4014, 4015, 4016, 4017, 4018, 4019, 4020, 4021, 4022, 4023, 4024, 4025, 4026, 4027, 4028, 4029, 4030, 4031, 4032, 4033, 4034, 4035, 4036, 4037, 4038, 4039, 4040, 4041, 4042, 4043, 4044, 4045, 4046, 4047, 4048, 4049, 4050, 4051, 4052, 4053, 4054, 4055, 4056, 4057, 4058, 4059, 4060, 4061, 4062, 4063, 4064, 4065, 4066, 4067, 4068, 4069, 4070, 4071, 4072, 4073, 4074, 4075, 4076, 4077, 4078, 4079, 4080, 4081, 4082, 4083, 4084, 4085, 4086, 4087, 4088, 4089, 4090, 4091, 4092, 4093, 4094, 4095, 4096, 4097, 4098, 4099, 4100, 4101, 4102, 4103, 4104, 4105, 4106, 4107, 4108, 4109, 4110, 4111, 4112, 4113, 4114, 4115, 4116, 4117, 4118, 4119, 4120, 4121, 4122, 4123, 4124, 4125, 4126, 4127, 4128, 4129, 4130, 4131, 4132, 4133, 4134, 4135, 4136, 4137, 4138, 4139, 4140, 4141, 4142, 4143, 4144, 4145, 4146, 4147, 4148, 4149, 4150, 4151, 4152, 4153, 4154, 4155, 4156, 4157, 4158, 4159, 4160, 4161, 4162, 4163, 4164, 4165, 4166, 4167, 4168, 4169, 4170, 4171, 4172, 4173, 4174, 4175, 4176, 4177, 4178, 4179, 4180, 4181, 4182, 4183, 4184, 4185, 4186, 4187, 4188, 4189, 4190, 4191, 4192, 4193, 4194, 4195, 4196, 4198, 4199, 4200, 4201, 4202, 4203, 4204, 4205, 4206, 4207, 4208, 4209, 4210, 4211, 4212, 4213, 4214, 4215, 4216, 4217, 4218, 4219, 4220, 4221, 4222, 4223, 4224, 4225, 4226, 4227, 4228, 4229, 4230, 4231, 4232, 4233, 4234, 4235, 4236, 4237, 4238, 4239, 4240, 4241, 4242, 4243, 4244, 4245, 4246, 4247, 4248, 4249, 4250, 4251, 4252, 4253, 4254, 4255, 4256, 4257, 4258, 4259, 4260, 4261, 4262, 4263, 4264, 4265, 4266, 4267, 4268, 4269, 4270, 4271, 4272, 4273, 4274, 4275, 4276, 4277, 4278, 4279, 4280, 4281, 4282, 4283, 4284, 4285, 4286, 4287, 4288, 4289, 4290, 4291, 4292, 4293, 4294, 4295, 4296, 4297, 4298, 4299, 4300, 4301, 4302, 4303, 4304, 4305, 4306, 4307, 4308, 4309, 4310, 4311, 4312, 4313, 4314, 4315, 4316, 4317, 4318, 4319, 4320, 4321, 4322, 4323, 4324, 4325, 4326, 4327, 4328, 4329, 4330, 4331, 4332, 4333, 4334, 4335, 4336, 4337, 4338, 4339, 4340, 4341, 4342, 4343, 4344, 4345, 4346, 4347, 4348, 4349, 4350, 4351, 4352, 4353, 4354, 4355, 4356, 4357, 4358, 4359, 4360, 4361, 4362, 4363, 4364, 4365, 4366, 4367, 4368, 4369, 4370, 4371, 4372, 4373, 4374, 4375, 4376, 4377, 4378, 4379, 4380, 4381, 4382, 4383, 4384, 4385, 4386, 4387, 4389, 4390, 4391, 4392, 4393, 4394, 4395, 4396, 4397, 4398, 4399, 4402, 4403, 4404, 4405, 4406, 4407, 4408, 4409, 4410, 4411, 4412, 4413, 4414, 4415, 4416, 4417, 4418, 4419, 4420, 4421, 4422, 4423, 4424, 4426, 4427, 4428, 4429, 4430, 4431, 4432, 4433, 4434, 4435, 4436, 4437, 4438, 4439, 4440, 4441, 4442, 4443, 4444, 4445, 4446, 4447, 4448, 4449, 4450, 4451, 4452, 4453, 4454, 4455, 4456, 4457, 4458, 4459, 4460, 4461, 4462, 4463, 4464, 4465, 4466, 4467, 4468, 4469, 4470, 4471, 4472, 4473, 4474, 4475, 4476, 4477, 4478, 4479, 4480, 4481, 4482, 4483, 4484, 4485, 4486, 4487, 4488, 4489, 4490, 4491, 4492, 4493, 4494, 4495, 4496, 4497, 4498, 4499, 4500, 4501, 4502, 4503, 4504, 4505, 4506, 4507, 4508, 4509, 4510, 4511, 4512, 4513, 4514, 4515, 4516, 4517, 4518, 4519, 4520, 4521, 4522, 4523, 4524, 4525, 4526, 4527, 4528, 4529, 4530, 4531, 4532, 4533, 4534, 4535, 4536, 4537, 4538, 4539, 4540, 4541, 4542, 4543, 4544, 4545, 4546, 4547, 4548, 4549, 4550, 4551, 4552, 4553, 4554, 4555, 4556, 4557, 4558, 4559, 4560, 4561, 4562, 4563, 4564, 4565, 4566, 4567, 4568, 4569, 4570, 4571, 4572, 4573, 4574, 4575, 4576, 4577, 4578, 4579, 4580, 4581, 4582, 4583, 4584, 4585, 4586, 4587, 4588, 4589, 4590, 4591, 4592, 4593, 4594, 4595, 4596, 4597, 4598, 4599, 4600, 4601, 4602, 4603, 4604, 4605, 4606, 4607, 4608, 4609, 4610, 4611, 4612, 4613, 4614, 4615, 4616, 4617, 4618, 4619, 4620, 4621, 4622, 4623, 4624, 4625, 4626, 4627, 4628, 4629, 4630, 4631, 4632, 4633, 4634, 4635, 4636, 4637, 4638, 4639, 4640, 4641, 4642, 4643, 4644, 4645, 4646, 4647, 4648, 4649, 4650, 4651, 4652, 4653, 4654, 4655, 4656, 4657, 4658, 4659, 4660, 4661, 4662, 4663, 4664, 4665, 4666, 4667, 4668, 4669, 4670, 4671, 4672, 4673, 4674, 4675, 4676, 4677, 4678, 4679, 4680, 4681, 4682, 4683, 4684, 4685, 4686, 4687, 4688, 4689, 4690, 4691, 4692, 4693, 4694, 4695, 4696, 4697, 4698, 4699, 4700, 4701, 4702, 4703, 4704, 4705, 4706, 4707, 4708, 4709, 4710, 4711, 4712, 4713, 4714, 4715, 4716, 4717, 4718, 4719, 4720, 4721, 4722, 4723, 4724, 4725, 4726, 4727, 4728, 4729, 4730, 4731, 4732, 4733, 4734, 4735, 4736, 4737, 4738, 4739, 4740, 4741, 4742, 4743, 4744, 4745, 4746, 4747, 4748, 4749, 4750, 4751, 4752, 4753, 4754, 4755, 4756, 4757, 4758, 4759, 4760, 4761, 4762, 4763, 4764, 4765, 4766, 4767, 4768, 4769, 4770, 4771, 4772, 4773, 4774, 4775, 4776, 4777, 4778, 4779, 4780, 4781, 4782, 4783, 4784, 4785, 4786, 4787, 4788, 4789, 4790, 4791, 4792, 4793, 4794, 4795, 4796, 4797, 4798, 4799, 4800, 4801, 4802, 4803, 4804, 4805, 4806, 4808, 4809, 4810, 4811, 4812, 4813, 4814, 4815, 4816, 4817, 4818, 4819, 4820, 4821, 4822, 4823, 4824, 4825, 4826, 4827, 4828, 4829, 4830, 4831, 4832, 4833, 4834, 4835, 4836, 4837, 4838, 4839, 4840, 4841, 4842, 4843, 4844, 4845, 4846, 4847, 4848, 4849, 4850, 4851, 4852, 4853, 4854, 4855, 4856, 4857, 4858, 4859, 4860, 4861, 4862, 4863, 4864, 4865, 4866, 4867, 4868, 4869, 4870, 4871, 4872, 4873, 4874, 4875, 4876, 4877, 4878, 4879, 4880, 4881, 4882, 4883, 4884, 4885, 4886, 4887, 4888, 4889, 4890, 4891, 4892, 4893, 4894, 4895, 4896, 4897, 4898, 4899, 4900, 4901, 4902, 4903, 4904, 4905, 4906, 4907, 4908, 4909, 4910, 4911, 4912, 4913, 4914, 4915, 4916, 4917, 4918, 4919, 4920, 4921, 4922, 4923, 4924, 4925, 4926, 4927, 4928, 4929, 4930, 4931, 4932, 4933, 4934, 4935, 4936, 4937, 4938, 4939, 4940, 4941, 4942, 4943, 4944, 4945, 4946, 4947, 4948, 4949, 4950, 4951, 4952, 4953, 4954, 4955, 4956, 4957, 4958, 4959, 4960, 4961, 4962, 4963, 4964, 4965, 4966, 4967, 4968, 4969, 4970, 4971, 4972, 4973, 4974, 4975, 4976, 4977, 4978, 4979, 4980, 4981, 4982, 4983, 4984, 4985, 4986, 4987, 4988, 4989, 4990, 4991, 4992, 4993, 4994, 4995, 4996, 4997, 4998, 4999, 5000, 5001, 5002, 5003, 5004, 5005, 5006, 5007, 5008, 5009, 5010, 5011, 5012, 5013, 5014, 5015, 5016, 5017, 5018, 5019, 5020, 5021, 5022, 5023, 5024, 5025, 5026, 5027, 5028, 5029, 5030, 5031, 5032, 5033, 5034, 5035, 5036, 5037, 5038, 5039, 5040, 5041, 5042, 5043, 5044, 5045, 5046, 5047, 5048, 5049, 5050, 5051, 5052, 5053, 5054, 5055, 5056, 5057, 5058, 5059, 5060, 5061, 5062, 5063, 5064, 5065, 5066, 5067, 5068, 5069, 5070, 5071, 5072, 5073, 5074, 5075, 5076, 5077, 5078, 5079, 5080, 5081, 5082, 5083, 5084, 5085, 5086, 5087, 5088, 5090, 5091, 5092, 5093, 5094, 5095, 5096, 5097, 5098, 5099, 5100, 5101, 5102, 5103, 5104, 5105, 5106, 5107, 5108, 5109, 5110, 5111, 5112, 5113, 5114, 5115, 5116, 5117, 5118, 5119, 5120, 5121, 5122, 5123, 5124, 5125, 5126, 5127, 5128, 5129, 5130, 5131, 5132, 5133, 5134, 5135, 5136, 5137, 5138, 5139, 5140, 5141, 5142, 5143, 5144, 5145, 5147, 5148, 5149, 5150, 5151, 5152, 5153, 5154, 5155, 5156, 5157, 5158, 5159, 5160, 5161, 5162, 5163, 5164, 5165, 5166, 5167, 5168, 5169, 5170, 5171, 5172, 5173, 5174, 5175, 5176, 5177, 5178, 5179, 5180, 5181, 5182, 5183, 5184, 5185, 5186, 5187, 5188, 5189, 5190, 5191, 5192, 5193, 5194, 5195, 5196, 5197, 5198, 5199, 5200, 5201, 5202, 5203, 5204, 5205, 5206, 5207, 5208, 5209, 5210, 5211, 5212, 5213, 5214, 5215, 5216, 5217, 5218, 5219, 5220, 5221, 5222, 5223, 5224, 5225, 5226, 5227, 5228, 5229, 5230, 5231, 5232, 5233, 5234, 5235, 5236, 5237, 5238, 5239, 5240, 5241, 5242, 5243, 5244, 5245, 5246, 5247, 5248, 5249, 5250, 5251, 5252, 5253, 5254, 5255, 5256, 5257, 5258, 5259, 5260, 5261, 5262, 5263, 5264, 5265, 5266, 5267, 5268, 5269, 5270, 5271, 5272, 5273, 5274, 5275, 5276, 5277, 5278, 5279, 5280, 5281, 5282, 5283, 5284, 5285, 5286, 5287, 5288, 5289, 5290, 5291, 5292, 5293, 5294, 5295, 5296, 5297, 5298, 5299, 5300, 5301, 5302, 5303, 5304, 5305, 5306, 5307, 5308, 5309, 5310, 5311, 5312, 5313, 5314]</t>
         </is>
       </c>
-      <c r="BP8" t="n">
+      <c r="BV8" t="n">
         <v>0.07697893972403776</v>
       </c>
-      <c r="BQ8" t="inlineStr">
+      <c r="BW8" t="inlineStr">
         <is>
           <t>{'Numk': 48, 'KPar': 20, 'Bucket_index': 569}</t>
         </is>
       </c>
-      <c r="BR8" t="n">
+      <c r="BX8" t="n">
         <v>12.06913982983679</v>
       </c>
-      <c r="BS8" t="inlineStr">
+      <c r="BY8" t="inlineStr">
         <is>
           <t>no</t>
         </is>
       </c>
-      <c r="BT8" t="n">
-        <v>0</v>
-      </c>
-      <c r="BU8" t="inlineStr">
+      <c r="BZ8" t="n">
+        <v>0</v>
+      </c>
+      <c r="CA8" t="inlineStr">
         <is>
           <t>params</t>
         </is>
       </c>
-      <c r="BV8" t="n">
+      <c r="CB8" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
part of results of HS-tree and full results of lamp
</commit_message>
<xml_diff>
--- a/f1score_merlin_abnormal_point_results.xlsx
+++ b/f1score_merlin_abnormal_point_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:CB8"/>
+  <dimension ref="A1:CJ8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -716,115 +716,155 @@
       </c>
       <c r="BF1" s="1" t="inlineStr">
         <is>
+          <t>Unnamed: 0.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1</t>
+        </is>
+      </c>
+      <c r="BG1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1</t>
+        </is>
+      </c>
+      <c r="BH1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1</t>
+        </is>
+      </c>
+      <c r="BI1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1</t>
+        </is>
+      </c>
+      <c r="BJ1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1</t>
+        </is>
+      </c>
+      <c r="BK1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1</t>
+        </is>
+      </c>
+      <c r="BL1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1</t>
+        </is>
+      </c>
+      <c r="BM1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1.1</t>
+        </is>
+      </c>
+      <c r="BN1" s="1" t="inlineStr">
+        <is>
           <t>Note</t>
         </is>
       </c>
-      <c r="BG1" s="1" t="inlineStr">
+      <c r="BO1" s="1" t="inlineStr">
         <is>
           <t>Dataset</t>
         </is>
       </c>
-      <c r="BH1" s="1" t="inlineStr">
+      <c r="BP1" s="1" t="inlineStr">
         <is>
           <t>Dataset length</t>
         </is>
       </c>
-      <c r="BI1" s="1" t="inlineStr">
+      <c r="BQ1" s="1" t="inlineStr">
         <is>
           <t>Type</t>
         </is>
       </c>
-      <c r="BJ1" s="1" t="inlineStr">
+      <c r="BR1" s="1" t="inlineStr">
         <is>
           <t>#discords</t>
         </is>
       </c>
-      <c r="BK1" s="1" t="inlineStr">
+      <c r="BS1" s="1" t="inlineStr">
         <is>
           <t>Position discord</t>
         </is>
       </c>
-      <c r="BL1" s="1" t="inlineStr">
+      <c r="BT1" s="1" t="inlineStr">
         <is>
           <t>discord length</t>
         </is>
       </c>
-      <c r="BM1" s="1" t="inlineStr">
+      <c r="BU1" s="1" t="inlineStr">
         <is>
           <t>HS-tree_identified</t>
         </is>
       </c>
-      <c r="BN1" s="1" t="inlineStr">
+      <c r="BV1" s="1" t="inlineStr">
         <is>
           <t>HS-tree_Overlap_merlin</t>
         </is>
       </c>
-      <c r="BO1" s="1" t="inlineStr">
+      <c r="BW1" s="1" t="inlineStr">
         <is>
           <t>HS-treebest_param</t>
         </is>
       </c>
-      <c r="BP1" s="1" t="inlineStr">
+      <c r="BX1" s="1" t="inlineStr">
         <is>
           <t>HS-treetime_taken</t>
         </is>
       </c>
-      <c r="BQ1" s="1" t="inlineStr">
+      <c r="BY1" s="1" t="inlineStr">
         <is>
           <t>ARIMAFD_identified</t>
         </is>
       </c>
-      <c r="BR1" s="1" t="inlineStr">
+      <c r="BZ1" s="1" t="inlineStr">
         <is>
           <t>ARIMAFD_Overlap_merlin</t>
         </is>
       </c>
-      <c r="BS1" s="1" t="inlineStr">
+      <c r="CA1" s="1" t="inlineStr">
         <is>
           <t>ARIMAFDbest_param</t>
         </is>
       </c>
-      <c r="BT1" s="1" t="inlineStr">
+      <c r="CB1" s="1" t="inlineStr">
         <is>
           <t>ARIMAFDtime_taken</t>
         </is>
       </c>
-      <c r="BU1" s="1" t="inlineStr">
+      <c r="CC1" s="1" t="inlineStr">
         <is>
           <t>MILOF_identified</t>
         </is>
       </c>
-      <c r="BV1" s="1" t="inlineStr">
+      <c r="CD1" s="1" t="inlineStr">
         <is>
           <t>MILOF_Overlap_merlin</t>
         </is>
       </c>
-      <c r="BW1" s="1" t="inlineStr">
+      <c r="CE1" s="1" t="inlineStr">
         <is>
           <t>MILOFbest_param</t>
         </is>
       </c>
-      <c r="BX1" s="1" t="inlineStr">
+      <c r="CF1" s="1" t="inlineStr">
         <is>
           <t>MILOFtime_taken</t>
         </is>
       </c>
-      <c r="BY1" s="1" t="inlineStr">
+      <c r="CG1" s="1" t="inlineStr">
         <is>
           <t>iforestASD_identified</t>
         </is>
       </c>
-      <c r="BZ1" s="1" t="inlineStr">
+      <c r="CH1" s="1" t="inlineStr">
         <is>
           <t>iforestASD_Overlap_merlin</t>
         </is>
       </c>
-      <c r="CA1" s="1" t="inlineStr">
+      <c r="CI1" s="1" t="inlineStr">
         <is>
           <t>iforestASDbest_param</t>
         </is>
       </c>
-      <c r="CB1" s="1" t="inlineStr">
+      <c r="CJ1" s="1" t="inlineStr">
         <is>
           <t>iforestASDtime_taken</t>
         </is>
@@ -1002,93 +1042,117 @@
       <c r="BE2" t="n">
         <v>0</v>
       </c>
-      <c r="BF2" t="inlineStr"/>
-      <c r="BG2" t="inlineStr">
+      <c r="BF2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BH2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BI2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BJ2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN2" t="inlineStr"/>
+      <c r="BO2" t="inlineStr">
         <is>
           <t>nab-data/realKnownCause/ambient_temperature_system_failure.csv</t>
         </is>
       </c>
-      <c r="BH2" t="n">
+      <c r="BP2" t="n">
         <v>7267</v>
       </c>
-      <c r="BI2" t="inlineStr">
+      <c r="BQ2" t="inlineStr">
         <is>
           <t>NAB</t>
         </is>
       </c>
-      <c r="BJ2" t="n">
-        <v>2</v>
-      </c>
-      <c r="BK2" t="inlineStr">
+      <c r="BR2" t="n">
+        <v>2</v>
+      </c>
+      <c r="BS2" t="inlineStr">
         <is>
           <t>3540; 5999</t>
         </is>
       </c>
-      <c r="BL2" t="n">
+      <c r="BT2" t="n">
         <v>362</v>
       </c>
-      <c r="BM2" t="inlineStr">
-        <is>
-          <t>[3152, 5046, 5048, 5050, 5052, 5053, 5054, 5055, 5056, 5057, 5058, 5059, 5060, 5061, 5062, 5063, 5064, 5065, 5066, 5067, 5068, 5069, 5070, 5071, 5072, 5073, 5074, 5075, 5076, 5077, 5078, 5079, 5080, 5100, 5101, 5366, 5367, 5368, 5369, 5370, 5371, 5372, 5373, 5374, 5375, 5376, 5377, 5378, 5379, 5380, 5381, 5382, 5383, 5384, 5385, 5386, 5387, 5402, 5403, 5404, 5405, 5406, 5407, 5408, 5454, 5456, 5457, 5458, 5459, 5460, 5461, 5462, 5463, 5465, 5466, 5467, 5468, 5469, 5470, 5471, 5472, 5473, 5474, 5475, 5476, 5477, 5478, 5479, 5480, 5481, 5482, 5483, 5484, 5486, 5487, 5495, 5496, 5497, 5498, 5499, 5500, 5501, 5502, 5503, 5504, 5505, 5506, 5507, 5508, 5509, 5510, 5511, 5512, 5513, 5514, 5515, 5516, 5517, 5518, 5519, 5520, 5521, 5522, 5523, 5524, 5525, 5526, 5527, 5528, 5529, 5530, 5531, 5532, 5533, 5534, 5535, 5536, 5537, 5538, 5539, 5540, 5541, 5542, 5543, 5544, 5545, 5546, 5547, 5548, 5549, 5550, 5551, 5552, 5553, 5554, 5556, 5570, 5571, 5572, 5573, 5574, 5575, 5576, 5577, 5595, 5596, 5597, 5598, 5599, 5622, 5644, 5645, 5646, 5684, 5686, 5689, 5690, 5691, 5692, 5693, 5694, 5695, 5696, 5697, 5698, 5699, 5700, 5701, 5702, 5703, 5704, 5705, 5706, 5707, 5708, 5709, 5710, 5711, 5712, 5713, 5714, 5715, 5716, 5717, 5718, 5719, 5720, 5721, 5722, 5723, 5736, 5737, 5738, 5739, 5740, 5741, 5742, 5763, 5764, 5765, 5766, 5786, 5787, 5788, 5789, 5809, 5811, 5812, 5813, 5814, 5834, 5836, 5837, 5838, 5839, 5840, 5841, 5842, 5843, 5844, 5845, 5846, 5847, 5848, 5849, 5850, 5851, 5852, 5853, 5854, 5855, 5856, 5857, 5858, 5859, 5860, 5861, 5862, 5863, 5864, 5865, 5866, 5867, 5868, 5869, 5870, 5871, 5872, 5873, 5874, 5875, 5876, 5877, 5878, 5879, 5880, 5881, 5882, 5889, 5893, 5894, 5895, 5896, 5897, 5915, 5916, 5917, 5918, 5919, 5942, 5943, 5944, 5962, 5964, 5965, 5966, 5967, 5969, 5992, 5993, 5994, 5995, 5996, 5997, 5998, 5999, 6000, 6001, 6002, 6003, 6004, 6005, 6006, 6007, 6008, 6009, 6010, 6011, 6012, 6013, 6014, 6015, 6016, 6017, 6018, 6019, 6020, 6021, 6022, 6023, 6024, 6025, 6026, 6027, 6028, 6029, 6030, 6031, 6032, 6033, 6034, 6035, 6036, 6037, 6038, 6039, 6040, 6041, 6042, 6044, 6057, 6058, 6059, 6060, 6061, 6062, 6063, 6064, 6065, 6084, 6086, 6087, 6088, 6109, 6111, 6123, 6124, 6125, 6126, 6127, 6128, 6129, 6130, 6131, 6132, 6133, 6134, 6146, 6148, 6149, 6150, 6151, 6152, 6153, 6154, 6155, 6156, 6157, 6158, 6159, 6160, 6161, 6162, 6163, 6164, 6165, 6166, 6167, 6168, 6169, 6170, 6171, 6172, 6173, 6174, 6175, 6176, 6177, 6178, 6179, 6180, 6181, 6182, 6183, 6184, 6185, 6186, 6187, 6188, 6189, 6190, 6191, 6192, 6193, 6194, 6195, 6196, 6197, 6198, 6199, 6200, 6201, 6202, 6203, 6204, 6205, 6206, 6207, 6208, 6209, 6216, 6217, 6218, 6219, 6220, 6221, 6222, 6223, 6224, 6225, 6226, 6227, 6228, 6229, 6243, 6244, 6245, 6246, 6247, 6248, 6249, 6250, 6251, 6252, 6268, 6269, 6270, 6271, 6272, 6273, 6274, 6275, 6276, 6277, 6293, 6294, 6295, 6296, 6297, 6298, 6299, 6300, 6316, 6317, 6318, 6319, 6320, 6321, 6322, 6323, 6324, 6325, 6326, 6327, 6328, 6329, 6330, 6331, 6332, 6333, 6334, 6335, 6336, 6337, 6338, 6339, 6340, 6341, 6342, 6343, 6344, 6345, 6346, 6347, 6348, 6349, 6350, 6351, 6352, 6353, 6354, 6355, 6356, 6357, 6358, 6359, 6360, 6361, 6362, 6363, 6364, 6365, 6366, 6367, 6368, 6369, 6370, 6371, 6372, 6373, 6374, 6375, 6376, 6385, 6386, 6387, 6388, 6389, 6390, 6391, 6392, 6393, 6394, 6395, 6396, 6397, 6413, 6414, 6415, 6416, 6417, 6418, 6419, 6420, 6439, 6440, 6441, 6442, 6443, 6460, 6462, 6463, 6464, 6465, 6466, 6484, 6485, 6486, 6487, 6488, 6489, 6490, 6491, 6492, 6493, 6494, 6495, 6496, 6497, 6498, 6499, 6500, 6501, 6502, 6503, 6504, 6505, 6506, 6507, 6508, 6509, 6510, 6511, 6512, 6513, 6514, 6515, 6516, 6517, 6518, 6519, 6520, 6521, 6522, 6523, 6524, 6525, 6526, 6527, 6528, 6529, 6530, 6531, 6532, 6533, 6534, 6535, 6536, 6537, 6538, 6539, 6540, 6541, 6542, 6549, 6550, 6552, 6553, 6554, 6555, 6556, 6557, 6558, 6559, 6560, 6561, 6562, 6563, 6564, 6565, 6566, 6567, 6568, 6569, 6570, 6571, 6572, 6573, 6574, 6575, 6576, 6577, 6578, 6579, 6580, 6581, 6582, 6583, 6584, 6585, 6586, 6587, 6588, 6589, 6590, 6591, 6592, 6593, 6594, 6597, 6598, 6599, 6600, 6601, 6602, 6603, 6604, 6605, 6606, 6607, 6608, 6609, 6610, 6611, 6612, 6613, 6614, 6620, 6621, 6623, 6624, 6625, 6626, 6627, 6628, 6629, 6630, 6631, 6632, 6633, 6634, 6635, 6636, 6638, 6639, 6640, 6646, 6650, 6651, 6652, 6653, 6654, 6655, 6656, 6657, 6658, 6659, 6660, 6661, 6662, 6663, 6664, 6665, 6666, 6667, 6668, 6669, 6670, 6671, 6672, 6673, 6674, 6675, 6676, 6677, 6678, 6679, 6680, 6681, 6682, 6683, 6684, 6685, 6686, 6687, 6688, 6689, 6690, 6691, 6692, 6693, 6694, 6695, 6696, 6697, 6698, 6699, 6700, 6701, 6702, 6703, 6704, 6705, 6706, 6707, 6708, 6709, 6710, 6711, 6712, 6713, 6714, 6715, 6716, 6717, 6718]</t>
-        </is>
-      </c>
-      <c r="BN2" t="n">
-        <v>0.1511879049676026</v>
-      </c>
-      <c r="BO2" t="inlineStr">
-        <is>
-          <t>{'initial_window': 203, 'window_size': 1680, 'num_trees': 27, 'max_depth': 12}</t>
-        </is>
-      </c>
-      <c r="BP2" t="n">
-        <v>5.046027642907575</v>
-      </c>
-      <c r="BQ2" t="inlineStr">
+      <c r="BU2" t="inlineStr">
+        <is>
+          <t>[208, 211, 282, 303, 304, 305, 306, 307, 308, 328, 329, 330, 331, 350, 351, 352, 353, 354, 355, 356, 357, 358, 359, 363, 364, 372, 374, 375, 376, 377, 378, 379, 380, 381, 382, 383, 386, 430, 435, 438, 610, 615, 636, 638, 639, 660, 663, 681, 683, 684, 903, 907, 911, 912, 913, 1079, 1080, 1248, 1407, 1426, 1427, 1428, 1430, 1432, 1445, 1446, 1447, 1448, 1449, 1450, 1451, 1452, 1453, 1454, 1455, 1456, 1457, 1458, 1459, 1460, 1461, 1464, 1465, 1468, 1469, 1470, 1471, 1472, 1473, 1474, 1475, 1476, 1477, 1478, 1479, 1480, 1481, 1482, 1483, 1484, 1485, 1486, 1494, 1500, 1502, 1503, 1549, 1550, 1551, 1552, 1553, 1554, 1555, 1556, 1557, 1558, 1559, 1560, 1561, 1562, 1563, 1564, 1565, 1566, 1567, 1571, 1573, 1574, 1575, 1576, 1577, 1578, 1579, 1580, 1581, 1582, 1583, 1584, 1585, 1586, 1587, 1589, 1772, 1775, 1776, 1777, 1779, 1794, 1796, 1797, 1798, 1800, 1820, 1821, 1822, 1824, 1825, 1826, 1827, 1828, 1829, 1830, 1835, 1844, 1846, 1850, 1852, 1920, 1922, 1925, 1928, 1929, 1931, 1933, 1934, 2076, 2077, 2078, 2082, 2097, 2099, 2100, 2115, 2123, 2124, 2125, 2126, 2127, 2128, 2149, 2170, 2173, 2176, 2177, 2178, 2180, 2182, 2183, 2184, 2188, 2189, 2191, 2192, 2194, 2196, 2197, 2198, 2725, 2819, 2822, 2825, 2844, 2848, 2851, 2852, 2853, 2854, 2856, 2858, 2863, 2865, 2866, 2867, 2870, 2871, 2872, 2873, 2874, 2875, 2876, 2879, 2880, 2882, 2887, 2888, 2889, 2890, 2891, 2892, 2893, 2894, 2895, 2896, 2898, 2916, 3152, 3558, 3559, 3694, 3695, 3696, 3697, 3698, 3699, 3700, 3701, 3702, 3703, 3704, 3705, 3706, 3707, 3708, 3709, 3710, 3711, 3712, 3713, 3714, 3715, 3716, 3717, 3718, 3719, 3720, 3721, 3722, 3723, 3724, 3725, 3726, 3727, 3728, 3729, 3730, 3731, 3732, 3733, 3734, 3735, 3736, 3737, 3738, 3739, 3741, 3743, 3745, 3747, 3748, 3749, 3750, 3751, 3752, 3753, 3754, 3755, 3756, 3757, 3758, 3772, 3775, 3777, 4224, 4225, 4226, 4227, 4228, 4231, 4233, 4237, 4384, 4504, 4518, 4520, 4522, 4524, 4526, 4527, 4528, 4529, 4530, 4531, 4532, 4533, 4535, 4541, 4544, 4545, 4546, 4547, 4548, 4549, 4551, 4552, 4553, 4554, 4555, 4556, 4557, 4558, 4559, 4560, 4562, 4568, 4573, 4577, 4593, 4595, 4596, 4597, 4598, 5039, 5040, 5041, 5043, 5044, 5045, 5046, 5047, 5048, 5049, 5050, 5051, 5052, 5053, 5054, 5055, 5056, 5057, 5058, 5059, 5060, 5061, 5062, 5063, 5064, 5065, 5066, 5067, 5068, 5069, 5070, 5071, 5072, 5073, 5074, 5075, 5076, 5077, 5078, 5079, 5080, 5099, 5100, 5101, 5103, 5255, 5256, 5473, 5474, 5475, 5476, 5477, 5478, 5479, 5480, 5481, 5482, 5507, 5508, 5509, 5510, 5511, 5524, 5525, 5526, 5527, 5528, 5529, 5530, 5531, 5532, 5533, 5534, 5535, 5536, 5538, 5539, 5540, 5541, 5542, 5543, 5544, 5545, 5546, 5547, 5548, 5549, 5550, 5551, 5552, 5553, 6167, 6170, 6171, 6172, 6173, 6174, 6175, 6176, 6177, 6178, 6179, 6180, 6181, 6182, 6183, 6184, 6185, 6186, 6187, 6188, 6189, 6190, 6191, 6192, 6193, 6194, 6195, 6196, 6197, 6198, 6813, 6815, 7050, 7052, 7075, 7078, 7097, 7098, 7099, 7100, 7101, 7103, 7104, 7118, 7119, 7120, 7121, 7122, 7123, 7124, 7125, 7126, 7127, 7128, 7143, 7144, 7146, 7147, 7148, 7149, 7151, 7152]</t>
+        </is>
+      </c>
+      <c r="BV2" t="n">
+        <v>0.3092105263157894</v>
+      </c>
+      <c r="BW2" t="inlineStr">
+        <is>
+          <t>{'initial_window': 1335, 'window_size': 200, 'num_trees': 15, 'max_depth': 10}</t>
+        </is>
+      </c>
+      <c r="BX2" t="n">
+        <v>1.949806470998737</v>
+      </c>
+      <c r="BY2" t="inlineStr">
         <is>
           <t>[849, 2047, 2115, 2116, 5952, 6109, 6201, 6208, 6945, 7185]</t>
         </is>
       </c>
-      <c r="BR2" t="n">
+      <c r="BZ2" t="n">
         <v>0.3749999999999999</v>
       </c>
-      <c r="BS2" t="inlineStr">
+      <c r="CA2" t="inlineStr">
         <is>
           <t>{'AR_window_size': 69, 'differencing-order': 0}</t>
         </is>
       </c>
-      <c r="BT2" t="n">
+      <c r="CB2" t="n">
         <v>147.1378787180874</v>
       </c>
-      <c r="BU2" t="inlineStr">
+      <c r="CC2" t="inlineStr">
         <is>
           <t xml:space="preserve">[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86, 87, 88, 89, 90, 91, 92, 93, 94, 95, 96, 97, 98, 99, 100, 101, 102, 103, 104, 105, 106, 107, 108, 109, 110, 111, 112, 113, 114, 115, 116, 117, 118, 119, 120, 121, 122, 123, 124, 125, 126, 127, 128, 129, 130, 131, 132, 133, 134, 135, 136, 137, 138, 139, 140, 141, 142, 143, 144, 145, 146, 147, 148, 149, 150, 151, 152, 153, 154, 155, 156, 157, 158, 159, 160, 161, 162, 163, 164, 165, 166, 167, 168, 169, 170, 171, 172, 173, 174, 175, 176, 177, 178, 179, 180, 181, 182, 183, 184, 185, 186, 187, 188, 189, 190, 191, 192, 193, 194, 195, 196, 197, 198, 199, 200, 201, 202, 203, 204, 205, 206, 207, 208, 209, 210, 211, 212, 213, 214, 215, 216, 217, 218, 219, 220, 221, 222, 223, 224, 225, 226, 227, 228, 229, 230, 231, 232, 233, 234, 235, 236, 237, 238, 239, 240, 241, 242, 243, 244, 245, 246, 247, 248, 249, 250, 251, 252, 253, 254, 255, 256, 257, 258, 259, 260, 261, 262, 263, 264, 265, 266, 267, 268, 269, 270, 271, 272, 273, 274, 275, 276, 277, 278, 279, 280, 281, 282, 283, 284, 285, 286, 287, 288, 289, 290, 291, 292, 293, 294, 295, 296, 297, 298, 299, 300, 301, 302, 303, 304, 305, 306, 307, 308, 309, 310, 311, 312, 313, 314, 315, 316, 317, 318, 319, 320, 321, 322, 323, 324, 325, 326, 327, 328, 329, 330, 331, 332, 333, 334, 335, 336, 337, 338, 339, 340, 341, 342, 343, 344, 345, 346, 347, 348, 349, 350, 351, 352, 353, 354, 355, 356, 357, 358, 359, 360, 361, 362, 363, 364, 365, 366, 367, 368, 369, 370, 371, 372, 373, 374, 375, 376, 377, 378, 379, 380, 381, 382, 383, 384, 385, 386, 387, 388, 389, 390, 391, 392, 393, 394, 395, 396, 397, 398, 399, 400, 401, 402, 403, 404, 405, 406, 407, 408, 409, 410, 411, 412, 413, 414, 415, 416, 417, 418, 419, 420, 421, 422, 423, 424, 425, 426, 427, 428, 429, 430, 431, 432, 433, 434, 435, 436, 437, 438, 439, 440, 441, 442, 443, 444, 445, 446, 447, 448, 449, 450, 451, 452, 453, 454, 455, 456, 457, 458, 459, 460, 461, 462, 463, 464, 465, 466, 467, 468, 469, 470, 471, 472, 473, 474, 475, 476, 477, 478, 479, 480, 481, 482, 483, 484, 485, 486, 487, 488, 489, 490, 491, 492, 493, 494, 495, 496, 497, 498, 499, 500, 501, 502, 503, 504, 505, 506, 507, 508, 509, 510, 511, 512, 513, 514, 515, 516, 517, 518, 519, 520, 521, 522, 523, 524, 525, 526, 527, 528, 529, 530, 531, 532, 533, 534, 535, 536, 537, 538, 539, 540, 541, 542, 543, 544, 545, 546, 547, 548, 549, 550, 551, 552, 553, 554, 555, 556, 557, 558, 559, 560, 561, 562, 563, 564, 565, 566, 567, 568, 569, 570, 571, 572, 573, 574, 575, 576, 577, 578, 579, 580, 581, 582, 583, 584, 585, 586, 587, 588, 589, 590, 591, 592, 593, 594, 595, 596, 597, 598, 599, 600, 601, 602, 603, 604, 605, 606, 607, 608, 609, 610, 611, 612, 613, 614, 615, 616, 617, 618, 619, 620, 621, 622, 623, 624, 625, 626, 627, 628, 629, 630, 631, 632, 633, 634, 635, 636, 637, 638, 639, 640, 641, 642, 643, 644, 645, 646, 647, 648, 649, 650, 651, 652, 653, 654, 655, 656, 657, 658, 659, 660, 661, 662, 663, 664, 665, 666, 667, 668, 669, 670, 671, 672, 673, 674, 675, 676, 677, 678, 679, 680, 681, 682, 683, 684, 685, 686, 687, 688, 689, 690, 691, 692, 693, 694, 695, 696, 697, 698, 699, 700, 701, 702, 703, 704, 705, 706, 707, 708, 709, 710, 711, 712, 713, 714, 715, 716, 717, 718, 719, 720, 721, 722, 723, 724, 725, 726, 727, 728, 729, 730, 731, 732, 733, 734, 735, 736, 737, 738, 739, 740, 741, 742, 743, 744, 745, 746, 747, 748, 749, 750, 751, 752, 753, 754, 755, 756, 757, 758, 759, 760, 761, 762, 763, 764, 765, 766, 767, 768, 769, 770, 771, 772, 773, 774, 775, 776, 777, 778, 779, 780, 781, 782, 783, 784, 785, 786, 787, 788, 789, 790, 791, 792, 793, 794, 795, 796, 797, 798, 799, 800, 801, 802, 803, 804, 805, 806, 807, 808, 809, 810, 811, 812, 813, 814, 815, 816, 817, 818, 819, 820, 821, 822, 823, 824, 825, 826, 827, 828, 829, 830, 831, 832, 833, 834, 835, 836, 837, 838, 839, 840, 841, 842, 843, 844, 845, 846, 847, 848, 849, 850, 851, 852, 853, 854, 855, 856, 857, 858, 859, 860, 861, 862, 863, 864, 865, 866, 867, 868, 869, 870, 871, 872, 873, 874, 875, 876, 877, 878, 879, 880, 881, 882, 883, 884, 885, 886, 887, 888, 889, 890, 891, 892, 893, 894, 895, 896, 897, 898, 899, 900, 901, 902, 903, 904, 905, 906, 907, 908, 909, 910, 911, 912, 913, 914, 915, 916, 917, 918, 919, 920, 921, 922, 923, 924, 925, 926, 927, 928, 929, 930, 931, 932, 933, 934, 935, 936, 937, 938, 939, 940, 941, 942, 943, 944, 945, 946, 947, 948, 949, 950, 951, 952, 953, 954, 955, 956, 957, 958, 959, 960, 961, 962, 963, 964, 965, 966, 967, 968, 969, 970, 971, 972, 973, 974, 975, 976, 977, 978, 979, 980, 981, 982, 983, 984, 985, 986, 987, 988, 989, 990, 991, 992, 993, 994, 995, 996, 997, 998, 999, 1000, 1001, 1002, 1003, 1004, 1005, 1006, 1007, 1008, 1009, 1010, 1011, 1012, 1013, 1014, 1015, 1016, 1017, 1018, 1019, 1020, 1021, 1022, 1023, 1024, 1025, 1026, 1027, 1028, 1029, 1030, 1031, 1032, 1033, 1034, 1035, 1036, 1037, 1038, 1039, 1040, 1041, 1042, 1043, 1044, 1045, 1046, 1047, 1048, 1049, 1050, 1051, 1052, 1053, 1054, 1055, 1056, 1057, 1058, 1059, 1060, 1061, 1062, 1063, 1064, 1065, 1066, 1067, 1068, 1069, 1070, 1071, 1072, 1073, 1074, 1075, 1076, 1077, 1078, 1079, 1080, 1081, 1082, 1083, 1084, 1085, 1086, 1087, 1088, 1089, 1090, 1091, 1092, 1093, 1094, 1095, 1096, 1097, 1098, 1099, 1100, 1101, 1102, 1103, 1104, 1105, 1106, 1107, 1108, 1109, 1110, 1111, 1112, 1113, 1114, 1115, 1116, 1117, 1118, 1119, 1120, 1121, 1122, 1123, 1124, 1125, 1126, 1127, 1128, 1129, 1130, 1131, 1132, 1133, 1134, 1135, 1136, 1137, 1138, 1139, 1140, 1141, 1142, 1143, 1144, 1145, 1146, 1147, 1148, 1149, 1150, 1151, 1152, 1153, 1154, 1155, 1156, 1157, 1158, 1159, 1160, 1161, 1162, 1163, 1164, 1165, 1166, 1167, 1168, 1169, 1170, 1171, 1172, 1173, 1174, 1175, 1176, 1177, 1178, 1179, 1180, 1181, 1182, 1183, 1184, 1185, 1186, 1187, 1188, 1189, 1190, 1191, 1192, 1193, 1194, 1195, 1196, 1197, 1198, 1199, 1200, 1201, 1202, 1203, 1204, 1205, 1206, 1207, 1208, 1209, 1210, 1211, 1212, 1213, 1214, 1215, 1216, 1217, 1218, 1219, 1220, 1221, 1222, 1223, 1224, 1225, 1226, 1227, 1228, 1229, 1230, 1231, 1232, 1233, 1234, 1235, 1236, 1237, 1238, 1239, 1240, 1241, 1242, 1243, 1244, 1245, 1246, 1247, 1248, 1249, 1250, 1251, 1252, 1253, 1254, 1255, 1256, 1257, 1258, 1259, 1260, 1261, 1262, 1263, 1264, 1265, 1266, 1267, 1268, 1269, 1270, 1271, 1272, 1273, 1274, 1275, 1276, 1277, 1278, 1279, 1280, 1281, 1282, 1283, 1284, 1285, 1286, 1287, 1288, 1289, 1290, 1291, 1292, 1293, 1294, 1295, 1296, 1297, 1298, 1299, 1300, 1301, 1302, 1303, 1304, 1305, 1306, 1307, 1308, 1309, 1310, 1311, 1312, 1313, 1314, 1315, 1316, 1317, 1318, 1319, 1320, 1321, 1322, 1323, 1324, 1325, 1326, 1327, 1328, 1329, 1330, 1331, 1332, 1333, 1334, 1335, 1336, 1337, 1338, 1339, 1340, 1341, 1342, 1343, 1344, 1345, 1346, 1347, 1348, 1349, 1350, 1351, 1352, 1353, 1354, 1355, 1356, 1357, 1358, 1359, 1360, 1361, 1362, 1363, 1364, 1365, 1366, 1367, 1368, 1369, 1370, 1371, 1372, 1373, 1374, 1375, 1376, 1377, 1378, 1379, 1380, 1381, 1382, 1383, 1384, 1385, 1386, 1387, 1388, 1389, 1390, 1391, 1392, 1393, 1394, 1395, 1396, 1397, 1398, 1399, 1400, 1401, 1402, 1403, 1404, 1405, 1406, 1407, 1408, 1409, 1410, 1411, 1412, 1413, 1414, 1415, 1416, 1417, 1418, 1419, 1420, 1421, 1422, 1423, 1424, 1425, 1426, 1427, 1428, 1429, 1430, 1431, 1432, 1433, 1434, 1435, 1436, 1437, 1438, 1439, 1440, 1441, 1442, 1443, 1444, 1445, 1446, 1447, 1448, 1449, 1450, 1451, 1452, 1453, 1454, 1455, 1456, 1457, 1458, 1459, 1460, 1461, 1462, 1463, 1464, 1465, 1466, 1467, 1468, 1469, 1470, 1471, 1472, 1473, 1474, 1475, 1476, 1477, 1478, 1479, 1480, 1481, 1482, 1483, 1484, 1485, 1486, 1487, 1488, 1489, 1490, 1491, 1492, 1493, 1494, 1495, 1496, 1497, 1498, 1499, 1500, 1501, 1502, 1503, 1504, 1505, 1506, 1507, 1508, 1509, 1510, 1511, 1512, 1513, 1514, 1515, 1516, 1517, 1518, 1519, 1520, 1521, 1522, 1523, 1524, 1525, 1526, 1527, 1528, 1529, 1530, 1531, 1532, 1533, 1534, 1535, 1536, 1537, 1538, 1539, 1540, 1542, 1543, 1544, 1545, 1546, 1547, 1548, 1549, 1550, 1551, 1552, 1553, 1554, 1555, 1556, 1557, 1558, 1559, 1560, 1561, 1562, 1563, 1564, 1565, 1566, 1567, 1568, 1569, 1570, 1571, 1572, 1573, 1574, 1575, 1576, 1577, 1578, 1579, 1580, 1581, 1582, 1583, 1584, 1585, 1586, 1587, 1588, 1589, 1590, 1591, 1592, 1593, 1594, 1595, 1596, 1597, 1598, 1599, 1600, 1601, 1602, 1603, 1604, 1605, 1606, 1607, 1608, 1609, 1610, 1611, 1612, 1613, 1614, 1615, 1616, 1617, 1618, 1619, 1620, 1621, 1622, 1623, 1624, 1625, 1626, 1627, 1628, 1629, 1630, 1631, 1632, 1633, 1634, 1635, 1636, 1637, 1638, 1639, 1640, 1641, 1642, 1643, 1644, 1645, 1646, 1647, 1648, 1649, 1650, 1651, 1652, 1653, 1654, 1655, 1656, 1657, 1658, 1659, 1660, 1661, 1662, 1663, 1664, 1665, 1666, 1667, 1668, 1669, 1670, 1671, 1672, 1673, 1674, 1675, 1676, 1677, 1678, 1679, 1680, 1681, 1682, 1683, 1684, 1685, 1686, 1687, 1688, 1689, 1690, 1691, 1692, 1693, 1694, 1695, 1696, 1697, 1698, 1699, 1700, 1701, 1702, 1703, 1704, 1705, 1706, 1707, 1708, 1709, 1710, 1711, 1712, 1713, 1714, 1715, 1716, 1717, 1718, 1719, 1720, 1721, 1722, 1723, 1724, 1725, 1726, 1727, 1728, 1729, 1730, 1731, 1732, 1733, 1734, 1735, 1736, 1737, 1738, 1739, 1740, 1741, 1742, 1743, 1744, 1745, 1746, 1747, 1748, 1749, 1750, 1751, 1752, 1753, 1754, 1755, 1756, 1757, 1758, 1759, 1760, 1761, 1762, 1763, 1764, 1765, 1766, 1767, 1768, 1769, 1770, 1771, 1772, 1773, 1774, 1775, 1776, 1777, 1778, 1779, 1780, 1781, 1782, 1783, 1784, 1785, 1786, 1787, 1788, 1789, 1790, 1791, 1792, 1793, 1794, 1795, 1796, 1797, 1798, 1799, 1800, 1801, 1802, 1803, 1804, 1805, 1806, 1807, 1808, 1809, 1810, 1811, 1812, 1813, 1814, 1815, 1816, 1817, 1818, 1819, 1820, 1821, 1822, 1823, 1824, 1825, 1826, 1827, 1828, 1829, 1830, 1831, 1832, 1833, 1834, 1835, 1836, 1837, 1838, 1839, 1840, 1841, 1842, 1843, 1844, 1845, 1846, 1847, 1848, 1849, 1850, 1851, 1852, 1853, 1854, 1855, 1856, 1857, 1858, 1859, 1860, 1861, 1862, 1863, 1864, 1865, 1866, 1867, 1868, 1869, 1870, 1871, 1872, 1873, 1874, 1875, 1876, 1877, 1878, 1879, 1880, 1881, 1882, 1883, 1884, 1885, 1886, 1887, 1888, 1889, 1890, 1891, 1892, 1893, 1894, 1895, 1896, 1897, 1898, 1899, 1900, 1901, 1902, 1903, 1904, 1905, 1906, 1907, 1908, 1909, 1910, 1911, 1912, 1913, 1914, 1915, 1916, 1917, 1918, 1919, 1920, 1921, 1922, 1923, 1924, 1925, 1926, 1927, 1928, 1929, 1930, 1931, 1932, 1933, 1934, 1935, 1936, 1937, 1938, 1939, 1940, 1941, 1942, 1943, 1944, 1945, 1946, 1947, 1948, 1949, 1950, 1951, 1952, 1953, 1954, 1955, 1956, 1957, 1958, 1959, 1960, 1961, 1962, 1963, 1964, 1965, 1966, 1967, 1968, 1969, 1970, 1971, 1972, 1973, 1974, 1975, 1976, 1977, 1978, 1979, 1980, 1981, 1982, 1983, 1984, 1985, 1986, 1987, 1988, 1989, 1991, 1992, 1993, 1994, 1995, 1996, 1997, 1998, 1999, 2000, 2001, 2002, 2003, 2004, 2005, 2006, 2007, 2008, 2009, 2010, 2011, 2012, 2013, 2014, 2015, 2016, 2017, 2018, 2019, 2020, 2021, 2022, 2023, 2024, 2025, 2026, 2027, 2028, 2029, 2030, 2031, 2032, 2033, 2034, 2035, 2036, 2037, 2038, 2039, 2040, 2041, 2042, 2043, 2044, 2045, 2046, 2047, 2048, 2049, 2050, 2051, 2052, 2053, 2054, 2055, 2056, 2057, 2058, 2059, 2060, 2061, 2062, 2063, 2064, 2065, 2066, 2067, 2068, 2069, 2070, 2071, 2072, 2073, 2074, 2075, 2076, 2077, 2078, 2079, 2080, 2081, 2082, 2083, 2084, 2085, 2086, 2087, 2088, 2089, 2090, 2091, 2092, 2093, 2094, 2095, 2096, 2097, 2098, 2099, 2100, 2101, 2102, 2103, 2104, 2105, 2106, 2107, 2108, 2109, 2110, 2111, 2112, 2113, 2114, 2115, 2116, 2117, 2118, 2119, 2120, 2121, 2122, 2123, 2124, 2125, 2126, 2127, 2128, 2129, 2130, 2131, 2132, 2133, 2134, 2135, 2136, 2137, 2138, 2139, 2140, 2141, 2142, 2143, 2144, 2145, 2146, 2147, 2148, 2149, 2150, 2151, 2152, 2153, 2154, 2155, 2156, 2157, 2158, 2159, 2160, 2161, 2162, 2163, 2164, 2165, 2166, 2167, 2168, 2169, 2170, 2171, 2172, 2173, 2174, 2175, 2176, 2177, 2178, 2179, 2180, 2181, 2182, 2183, 2184, 2185, 2186, 2187, 2188, 2189, 2190, 2191, 2192, 2193, 2194, 2195, 2196, 2197, 2198, 2199, 2200, 2201, 2202, 2203, 2204, 2205, 2206, 2207, 2208, 2209, 2210, 2211, 2212, 2213, 2214, 2215, 2216, 2217, 2218, 2219, 2220, 2221, 2222, 2223, 2224, 2225, 2226, 2227, 2228, 2229, 2230, 2231, 2232, 2233, 2234, 2235, 2236, 2237, 2238, 2239, 2240, 2241, 2242, 2243, 2244, 2245, 2246, 2247, 2248, 2249, 2250, 2251, 2252, 2253, 2254, 2255, 2256, 2257, 2258, 2259, 2260, 2261, 2262, 2263, 2264, 2265, 2266, 2267, 2268, 2269, 2270, 2271, 2272, 2273, 2274, 2275, 2276, 2277, 2278, 2279, 2280, 2281, 2282, 2283, 2284, 2285, 2286, 2287, 2288, 2289, 2290, 2291, 2292, 2293, 2294, 2295, 2296, 2297, 2298, 2299, 2300, 2301, 2302, 2303, 2304, 2305, 2306, 2307, 2309, 2310, 2311, 2312, 2313, 2314, 2315, 2316, 2317, 2318, 2319, 2320, 2321, 2322, 2323, 2324, 2325, 2326, 2327, 2328, 2329, 2330, 2331, 2332, 2333, 2334, 2335, 2336, 2337, 2338, 2339, 2340, 2341, 2342, 2343, 2344, 2345, 2346, 2347, 2348, 2349, 2350, 2351, 2352, 2353, 2354, 2355, 2356, 2357, 2358, 2359, 2360, 2361, 2362, 2363, 2364, 2365, 2366, 2367, 2368, 2369, 2370, 2371, 2372, 2373, 2374, 2375, 2376, 2377, 2378, 2379, 2380, 2381, 2382, 2383, 2384, 2385, 2386, 2387, 2388, 2389, 2390, 2391, 2392, 2393, 2394, 2395, 2396, 2397, 2398, 2399, 2400, 2401, 2402, 2403, 2404, 2405, 2406, 2407, 2408, 2409, 2410, 2411, 2412, 2413, 2414, 2415, 2416, 2417, 2418, 2419, 2420, 2421, 2422, 2423, 2424, 2425, 2426, 2427, 2428, 2429, 2430, 2431, 2432, 2433, 2434, 2435, 2436, 2437, 2438, 2439, 2440, 2441, 2442, 2443, 2444, 2445, 2446, 2447, 2448, 2449, 2450, 2451, 2452, 2453, 2454, 2455, 2456, 2457, 2458, 2459, 2460, 2461, 2462, 2463, 2464, 2465, 2466, 2467, 2468, 2469, 2470, 2471, 2472, 2473, 2474, 2475, 2476, 2477, 2478, 2479, 2480, 2481, 2482, 2483, 2484, 2485, 2486, 2487, 2488, 2489, 2490, 2491, 2492, 2493, 2494, 2495, 2496, 2497, 2498, 2499, 2500, 2501, 2502, 2503, 2504, 2505, 2506, 2507, 2508, 2509, 2510, 2511, 2512, 2513, 2514, 2515, 2516, 2517, 2518, 2519, 2521, 2522, 2523, 2524, 2525, 2526, 2527, 2528, 2529, 2530, 2531, 2532, 2533, 2534, 2535, 2536, 2537, 2538, 2539, 2540, 2541, 2542, 2543, 2544, 2545, 2546, 2547, 2548, 2549, 2550, 2551, 2552, 2553, 2554, 2555, 2556, 2557, 2558, 2559, 2560, 2561, 2562, 2563, 2564, 2565, 2566, 2567, 2568, 2569, 2570, 2571, 2572, 2573, 2574, 2575, 2576, 2577, 2578, 2580, 2581, 2582, 2583, 2584, 2585, 2587, 2588, 2589, 2590, 2591, 2592, 2593, 2594, 2595, 2596, 2597, 2598, 2599, 2600, 2601, 2602, 2603, 2604, 2605, 2606, 2607, 2608, 2609, 2610, 2611, 2612, 2613, 2614, 2615, 2616, 2617, 2618, 2619, 2620, 2621, 2622, 2623, 2624, 2625, 2626, 2627, 2628, 2629, 2630, 2631, 2632, 2633, 2634, 2635, 2636, 2637, 2638, 2639, 2640, 2641, 2642, 2643, 2644, 2645, 2646, 2647, 2648, 2649, 2650, 2651, 2652, 2653, 2654, 2655, 2656, 2657, 2658, 2659, 2660, 2661, 2662, 2663, 2664, 2665, 2666, 2667, 2668, 2669, 2670, 2671, 2672, 2673, 2674, 2675, 2676, 2677, 2678, 2679, 2680, 2681, 2682, 2683, 2684, 2685, 2686, 2687, 2688, 2689, 2690, 2691, 2692, 2693, 2694, 2695, 2696, 2697, 2698, 2699, 2700, 2701, 2702, 2703, 2704, 2705, 2706, 2707, 2708, 2709, 2710, 2711, 2712, 2713, 2714, 2715, 2716, 2717, 2718, 2719, 2720, 2721, 2722, 2723, 2724, 2725, 2726, 2727, 2728, 2729, 2730, 2731, 2732, 2733, 2734, 2735, 2736, 2737, 2738, 2739, 2740, 2741, 2742, 2743, 2744, 2745, 2746, 2747, 2748, 2749, 2750, 2751, 2752, 2753, 2754, 2755, 2756, 2757, 2758, 2759, 2760, 2761, 2762, 2763, 2764, 2765, 2766, 2767, 2768, 2769, 2770, 2771, 2772, 2773, 2774, 2775, 2776, 2777, 2778, 2779, 2780, 2781, 2782, 2783, 2784, 2785, 2786, 2787, 2788, 2789, 2790, 2791, 2792, 2793, 2794, 2795, 2796, 2797, 2798, 2799, 2800, 2801, 2802, 2803, 2804, 2805, 2806, 2807, 2808, 2809, 2810, 2811, 2812, 2813, 2814, 2815, 2816, 2817, 2818, 2819, 2820, 2821, 2822, 2823, 2824, 2825, 2826, 2827, 2828, 2829, 2830, 2831, 2832, 2833, 2834, 2835, 2836, 2837, 2838, 2839, 2840, 2841, 2842, 2843, 2844, 2845, 2846, 2847, 2848, 2849, 2850, 2851, 2852, 2853, 2854, 2855, 2856, 2857, 2858, 2859, 2860, 2861, 2862, 2863, 2864, 2865, 2866, 2867, 2868, 2869, 2870, 2871, 2872, 2873, 2874, 2875, 2876, 2877, 2878, 2879, 2880, 2881, 2882, 2883, 2884, 2885, 2886, 2887, 2888, 2889, 2890, 2891, 2892, 2893, 2894, 2895, 2896, 2897, 2898, 2899, 2900, 2901, 2902, 2903, 2904, 2905, 2906, 2907, 2908, 2909, 2910, 2911, 2912, 2913, 2914, 2915, 2916, 2917, 2918, 2919, 2920, 2921, 2922, 2923, 2924, 2925, 2926, 2927, 2928, 2929, 2930, 2931, 2932, 2933, 2934, 2935, 2936, 2937, 2938, 2939, 2940, 2941, 2942, 2943, 2944, 2945, 2946, 2947, 2948, 2949, 2950, 2951, 2952, 2953, 2954, 2955, 2956, 2957, 2958, 2959, 2960, 2961, 2962, 2963, 2964, 2965, 2966, 2967, 2968, 2969, 2970, 2971, 2972, 2973, 2974, 2975, 2976, 2977, 2978, 2979, 2980, 2981, 2982, 2983, 2985, 2986, 2987, 2988, 2989, 2990, 2991, 2992, 2993, 2994, 2995, 2996, 2997, 2998, 2999, 3000, 3001, 3002, 3003, 3004, 3005, 3006, 3007, 3008, 3009, 3010, 3011, 3012, 3013, 3014, 3015, 3016, 3017, 3018, 3019, 3020, 3021, 3022, 3023, 3024, 3025, 3026, 3027, 3028, 3029, 3030, 3031, 3032, 3033, 3034, 3035, 3036, 3037, 3038, 3039, 3040, 3041, 3042, 3043, 3044, 3045, 3046, 3047, 3048, 3049, 3050, 3051, 3052, 3053, 3054, 3055, 3056, 3057, 3058, 3059, 3060, 3061, 3062, 3063, 3064, 3065, 3066, 3067, 3068, 3069, 3070, 3071, 3072, 3073, 3074, 3075, 3076, 3077, 3078, 3079, 3080, 3081, 3082, 3083, 3084, 3085, 3086, 3087, 3088, 3089, 3090, 3091, 3092, 3093, 3094, 3095, 3096, 3097, 3098, 3099, 3100, 3101, 3102, 3103, 3104, 3105, 3106, 3107, 3108, 3109, 3110, 3111, 3112, 3113, 3114, 3115, 3116, 3117, 3118, 3119, 3120, 3121, 3122, 3123, 3124, 3125, 3126, 3127, 3128, 3129, 3130, 3131, 3132, 3133, 3134, 3135, 3136, 3137, 3138, 3139, 3140, 3141, 3142, 3143, 3144, 3145, 3146, 3147, 3148, 3149, 3150, 3151, 3152, 3153, 3154, 3155, 3156, 3157, 3158, 3159, 3160, 3161, 3162, 3163, 3164, 3165, 3166, 3167, 3168, 3169, 3170, 3171, 3172, 3173, 3174, 3175, 3176, 3177, 3178, 3179, 3180, 3181, 3182, 3183, 3184, 3185, 3186, 3187, 3188, 3189, 3190, 3191, 3192, 3193, 3194, 3195, 3196, 3197, 3198, 3199, 3200, 3201, 3202, 3203, 3204, 3205, 3206, 3207, 3208, 3209, 3210, 3211, 3212, 3213, 3214, 3215, 3216, 3217, 3218, 3219, 3220, 3221, 3222, 3223, 3224, 3225, 3226, 3227, 3228, 3229, 3230, 3231, 3232, 3233, 3234, 3235, 3236, 3237, 3238, 3239, 3240, 3241, 3242, 3243, 3244, 3245, 3246, 3247, 3248, 3249, 3250, 3251, 3252, 3253, 3254, 3255, 3256, 3257, 3258, 3259, 3260, 3261, 3262, 3263, 3264, 3265, 3266, 3267, 3268, 3269, 3270, 3271, 3272, 3273, 3274, 3275, 3276, 3277, 3278, 3279, 3280, 3281, 3282, 3283, 3284, 3285, 3286, 3287, 3288, 3289, 3290, 3291, 3292, 3293, 3294, 3295, 3296, 3297, 3298, 3299, 3300, 3301, 3302, 3303, 3304, 3305, 3306, 3307, 3308, 3309, 3310, 3311, 3312, 3313, 3314, 3315, 3316, 3317, 3318, 3319, 3320, 3321, 3322, 3323, 3324, 3325, 3326, 3327, 3328, 3329, 3330, 3331, 3332, 3333, 3334, 3335, 3336, 3337, 3338, 3339, 3340, 3341, 3342, 3343, 3344, 3345, 3346, 3347, 3348, 3349, 3350, 3351, 3352, 3353, 3354, 3355, 3356, 3357, 3358, 3359, 3360, 3361, 3362, 3363, 3364, 3365, 3366, 3367, 3368, 3369, 3370, 3371, 3372, 3373, 3374, 3375, 3376, 3377, 3378, 3379, 3380, 3381, 3382, 3383, 3384, 3385, 3386, 3387, 3388, 3389, 3390, 3391, 3392, 3393, 3394, 3395, 3396, 3397, 3398, 3399, 3400, 3401, 3402, 3403, 3404, 3405, 3406, 3407, 3408, 3409, 3410, 3411, 3412, 3413, 3414, 3415, 3416, 3417, 3418, 3419, 3420, 3421, 3422, 3423, 3424, 3425, 3426, 3427, 3428, 3429, 3430, 3431, 3432, 3433, 3434, 3435, 3436, 3437, 3438, 3439, 3440, 3441, 3442, 3443, 3444, 3445, 3446, 3447, 3448, 3449, 3450, 3451, 3452, 3453, 3454, 3455, 3456, 3457, 3458, 3459, 3460, 3461, 3462, 3463, 3464, 3465, 3466, 3467, 3468, 3469, 3470, 3471, 3472, 3473, 3474, 3475, 3476, 3477, 3478, 3479, 3480, 3481, 3482, 3483, 3484, 3485, 3486, 3487, 3488, 3489, 3490, 3491, 3492, 3493, 3494, 3495, 3496, 3497, 3498, 3499, 3500, 3501, 3502, 3503, 3504, 3505, 3506, 3507, 3508, 3509, 3510, 3511, 3512, 3513, 3514, 3515, 3516, 3517, 3518, 3519, 3520, 3521, 3522, 3523, 3524, 3525, 3526, 3527, 3528, 3529, 3530, 3531, 3532, 3533, 3534, 3535, 3536, 3537, 3538, 3539, 3540, 3541, 3542, 3543, 3544, 3545, 3546, 3547, 3548, 3549, 3550, 3551, 3552, 3553, 3554, 3555, 3556, 3557, 3558, 3559, 3560, 3561, 3562, 3563, 3564, 3565, 3566, 3567, 3568, 3569, 3570, 3571, 3572, 3573, 3574, 3575, 3576, 3577, 3578, 3579, 3580, 3581, 3582, 3583, 3584, 3585, 3586, 3587, 3588, 3589, 3590, 3591, 3592, 3593, 3594, 3595, 3596, 3597, 3598, 3599, 3600, 3601, 3602, 3603, 3604, 3605, 3606, 3607, 3608, 3609, 3610, 3611, 3612, 3613, 3614, 3615, 3616, 3617, 3618, 3619, 3620, 3621, 3622, 3623, 3624, 3625, 3626, 3627, 3628, 3629, 3630, 3631, 3632, 3633, 3634, 3635, 3636, 3637, 3638, 3639, 3640, 3641, 3642, 3643, 3644, 3645, 3646, 3647, 3648, 3649, 3650, 3651, 3652, 3653, 3654, 3655, 3656, 3657, 3658, 3659, 3660, 3661, 3662, 3663, 3664, 3665, 3666, 3667, 3668, 3669, 3670, 3671, 3672, 3673, 3674, 3675, 3676, 3677, 3678, 3679, 3680, 3681, 3682, 3683, 3684, 3685, 3686, 3687, 3688, 3689, 3690, 3691, 3692, 3693, 3694, 3695, 3696, 3697, 3698, 3699, 3700, 3701, 3702, 3703, 3704, 3705, 3706, 3707, 3708, 3709, 3710, 3711, 3712, 3713, 3714, 3715, 3716, 3717, 3718, 3719, 3720, 3721, 3722, 3723, 3724, 3725, 3726, 3727, 3728, 3729, 3730, 3731, 3732, 3733, 3734, 3735, 3736, 3737, 3738, 3739, 3740, 3741, 3742, 3743, 3744, 3745, 3746, 3747, 3748, 3749, 3750, 3751, 3752, 3753, 3754, 3755, 3756, 3757, 3758, 3759, 3760, 3761, 3762, 3763, 3764, 3765, 3766, 3767, 3768, 3769, 3770, 3771, 3772, 3773, 3774, 3775, 3776, 3777, 3778, 3779, 3780, 3781, 3782, 3783, 3784, 3785, 3786, 3787, 3788, 3789, 3790, 3791, 3792, 3793, 3794, 3795, 3796, 3797, 3798, 3799, 3800, 3801, 3802, 3803, 3804, 3805, 3806, 3807, 3808, 3809, 3810, 3811, 3812, 3813, 3814, 3815, 3816, 3817, 3818, 3819, 3820, 3821, 3822, 3823, 3824, 3825, 3826, 3827, 3828, 3829, 3830, 3831, 3832, 3833, 3834, 3835, 3836, 3837, 3838, 3839, 3840, 3841, 3842, 3843, 3844, 3845, 3846, 3847, 3848, 3849, 3850, 3851, 3852, 3853, 3854, 3855, 3856, 3857, 3858, 3859, 3860, 3861, 3862, 3863, 3864, 3865, 3866, 3867, 3868, 3869, 3870, 3871, 3872, 3873, 3874, 3875, 3876, 3877, 3878, 3879, 3880, 3881, 3882, 3883, 3884, 3885, 3886, 3887, 3888, 3889, 3890, 3891, 3892, 3893, 3894, 3895, 3896, 3897, 3898, 3899, 3900, 3901, 3902, 3903, 3904, 3905, 3906, 3907, 3908, 3909, 3910, 3911, 3912, 3913, 3914, 3915, 3916, 3917, 3918, 3919, 3920, 3921, 3922, 3923, 3924, 3925, 3926, 3927, 3928, 3929, 3930, 3931, 3932, 3933, 3934, 3935, 3936, 3937, 3938, 3939, 3940, 3941, 3942, 3943, 3944, 3945, 3946, 3947, 3948, 3949, 3950, 3951, 3952, 3953, 3954, 3955, 3956, 3957, 3958, 3959, 3960, 3961, 3962, 3963, 3964, 3965, 3966, 3967, 3968, 3969, 3970, 3971, 3972, 3973, 3974, 3975, 3976, 3977, 3978, 3979, 3980, 3981, 3982, 3983, 3984, 3985, 3986, 3987, 3988, 3989, 3990, 3991, 3992, 3993, 3994, 3995, 3996, 3997, 3998, 3999, 4000, 4001, 4002, 4003, 4004, 4005, 4006, 4007, 4008, 4009, 4010, 4011, 4012, 4013, 4014, 4015, 4016, 4017, 4018, 4019, 4020, 4021, 4022, 4023, 4024, 4025, 4026, 4027, 4028, 4029, 4030, 4031, 4032, 4033, 4034, 4035, 4036, 4037, 4038, 4039, 4040, 4041, 4042, 4043, 4044, 4045, 4046, 4047, 4048, 4049, 4050, 4051, 4052, 4053, 4054, 4055, 4056, 4057, 4059, 4060, 4061, 4062, 4063, 4064, 4065, 4066, 4067, 4068, 4069, 4070, 4071, 4072, 4073, 4075, 4076, 4077, 4078, 4079, 4080, 4081, 4082, 4083, 4084, 4085, 4086, 4087, 4088, 4089, 4090, 4091, 4092, 4093, 4094, 4095, 4096, 4097, 4098, 4099, 4100, 4101, 4102, 4103, 4104, 4105, 4106, 4107, 4108, 4109, 4110, 4111, 4112, 4113, 4114, 4115, 4116, 4117, 4118, 4119, 4120, 4121, 4122, 4123, 4124, 4125, 4126, 4127, 4128, 4129, 4130, 4131, 4132, 4133, 4134, 4135, 4136, 4137, 4138, 4139, 4140, 4141, 4142, 4143, 4144, 4145, 4146, 4147, 4148, 4149, 4150, 4151, 4152, 4153, 4154, 4155, 4156, 4157, 4158, 4159, 4160, 4161, 4162, 4163, 4164, 4165, 4166, 4167, 4168, 4169, 4170, 4172, 4173, 4174, 4175, 4176, 4177, 4178, 4179, 4180, 4181, 4182, 4183, 4184, 4185, 4186, 4187, 4188, 4189, 4190, 4191, 4192, 4193, 4194, 4195, 4196, 4197, 4198, 4199, 4200, 4201, 4202, 4203, 4204, 4205, 4206, 4207, 4208, 4209, 4210, 4211, 4212, 4213, 4214, 4215, 4216, 4218, 4219, 4220, 4221, 4222, 4223, 4224, 4225, 4226, 4227, 4228, 4229, 4230, 4231, 4232, 4233, 4234, 4235, 4236, 4237, 4238, 4239, 4240, 4241, 4242, 4243, 4244, 4245, 4246, 4247, 4248, 4249, 4250, 4251, 4252, 4253, 4254, 4255, 4256, 4257, 4258, 4259, 4260, 4261, 4262, 4263, 4264, 4265, 4266, 4267, 4268, 4269, 4270, 4271, 4272, 4273, 4274, 4275, 4276, 4277, 4278, 4279, 4280, 4281, 4282, 4283, 4284, 4285, 4286, 4287, 4288, 4289, 4290, 4291, 4292, 4293, 4294, 4295, 4296, 4297, 4298, 4299, 4300, 4301, 4302, 4303, 4304, 4305, 4306, 4307, 4308, 4309, 4310, 4311, 4312, 4313, 4314, 4315, 4316, 4317, 4318, 4319, 4320, 4321, 4322, 4323, 4324, 4325, 4326, 4327, 4328, 4329, 4330, 4331, 4332, 4333, 4334, 4335, 4336, 4337, 4338, 4339, 4340, 4341, 4342, 4343, 4344, 4345, 4346, 4347, 4348, 4349, 4350, 4351, 4352, 4353, 4354, 4355, 4356, 4357, 4358, 4359, 4360, 4361, 4362, 4363, 4364, 4365, 4366, 4367, 4368, 4369, 4370, 4371, 4372, 4373, 4374, 4375, 4376, 4377, 4378, 4379, 4380, 4381, 4382, 4383, 4384, 4385, 4386, 4387, 4388, 4389, 4390, 4391, 4392, 4393, 4394, 4395, 4396, 4397, 4398, 4399, 4400, 4401, 4402, 4403, 4404, 4405, 4406, 4407, 4408, 4409, 4410, 4411, 4412, 4413, 4414, 4415, 4416, 4417, 4418, 4419, 4420, 4421, 4422, 4423, 4424, 4425, 4426, 4427, 4428, 4429, 4430, 4431, 4432, 4433, 4434, 4435, 4436, 4437, 4438, 4439, 4440, 4441, 4442, 4443, 4444, 4445, 4446, 4447, 4448, 4449, 4450, 4451, 4452, 4453, 4454, 4455, 4456, 4457, 4458, 4459, 4460, 4461, 4462, 4463, 4464, 4465, 4466, 4467, 4468, 4469, 4470, 4471, 4472, 4473, 4474, 4475, 4476, 4477, 4478, 4479, 4480, 4481, 4482, 4483, 4484, 4486, 4487, 4488, 4489, 4490, 4491, 4492, 4493, 4494, 4495, 4496, 4497, 4498, 4499, 4500, 4501, 4502, 4503, 4504, 4505, 4506, 4507, 4508, 4509, 4510, 4511, 4512, 4513, 4514, 4515, 4516, 4517, 4518, 4519, 4520, 4521, 4522, 4523, 4524, 4525, 4526, 4527, 4528, 4529, 4530, 4531, 4532, 4533, 4534, 4535, 4536, 4537, 4538, 4539, 4540, 4541, 4542, 4543, 4544, 4545, 4546, 4547, 4548, 4549, 4550, 4551, 4552, 4553, 4554, 4555, 4556, 4557, 4558, 4559, 4560, 4561, 4562, 4563, 4564, 4565, 4566, 4567, 4568, 4569, 4570, 4571, 4572, 4573, 4574, 4575, 4576, 4577, 4578, 4579, 4580, 4581, 4582, 4583, 4584, 4585, 4586, 4587, 4588, 4589, 4590, 4591, 4592, 4593, 4594, 4595, 4596, 4597, 4598, 4599, 4600, 4601, 4602, 4603, 4604, 4605, 4606, 4607, 4608, 4609, 4610, 4611, 4612, 4613, 4614, 4615, 4616, 4617, 4618, 4619, 4620, 4621, 4622, 4623, 4624, 4625, 4626, 4627, 4628, 4629, 4630, 4631, 4632, 4633, 4634, 4635, 4636, 4637, 4638, 4639, 4640, 4641, 4642, 4643, 4644, 4645, 4646, 4647, 4648, 4649, 4650, 4651, 4652, 4653, 4654, 4655, 4656, 4657, 4658, 4659, 4660, 4661, 4662, 4663, 4664, 4665, 4666, 4667, 4668, 4669, 4670, 4671, 4672, 4673, 4674, 4675, 4676, 4677, 4678, 4679, 4680, 4681, 4682, 4683, 4684, 4685, 4686, 4687, 4688, 4689, 4690, 4691, 4692, 4693, 4694, 4695, 4696, 4697, 4698, 4699, 4700, 4701, 4702, 4703, 4704, 4705, 4706, 4707, 4708, 4709, 4710, 4711, 4712, 4713, 4714, 4715, 4716, 4717, 4718, 4719, 4720, 4721, 4722, 4723, 4724, 4725, 4726, 4727, 4728, 4729, 4730, 4731, 4732, 4733, 4734, 4735, 4736, 4737, 4738, 4739, 4740, 4741, 4742, 4743, 4744, 4745, 4746, 4747, 4748, 4749, 4750, 4751, 4752, 4753, 4754, 4755, 4756, 4757, 4758, 4759, 4760, 4761, 4762, 4763, 4764, 4765, 4766, 4767, 4768, 4769, 4770, 4771, 4772, 4773, 4774, 4775, 4776, 4777, 4778, 4779, 4780, 4781, 4782, 4783, 4784, 4785, 4786, 4787, 4788, 4789, 4790, 4791, 4792, 4793, 4794, 4795, 4796, 4797, 4798, 4799, 4800, 4801, 4802, 4803, 4804, 4805, 4806, 4807, 4808, 4809, 4810, 4811, 4812, 4813, 4814, 4815, 4816, 4817, 4818, 4819, 4820, 4821, 4822, 4823, 4824, 4825, 4826, 4827, 4828, 4829, 4830, 4831, 4832, 4833, 4834, 4835, 4836, 4837, 4838, 4839, 4840, 4841, 4842, 4843, 4844, 4845, 4846, 4847, 4848, 4849, 4850, 4851, 4852, 4853, 4854, 4855, 4856, 4857, 4858, 4859, 4860, 4861, 4862, 4863, 4864, 4865, 4866, 4867, 4868, 4869, 4870, 4871, 4872, 4873, 4874, 4875, 4876, 4877, 4878, 4879, 4880, 4881, 4882, 4883, 4884, 4885, 4886, 4887, 4888, 4889, 4890, 4891, 4892, 4893, 4894, 4895, 4896, 4897, 4898, 4899, 4900, 4901, 4902, 4903, 4904, 4905, 4906, 4907, 4908, 4909, 4910, 4911, 4912, 4913, 4914, 4915, 4916, 4917, 4918, 4919, 4920, 4921, 4922, 4923, 4924, 4925, 4926, 4927, 4928, 4929, 4930, 4931, 4932, 4933, 4934, 4935, 4936, 4937, 4938, 4939, 4940, 4941, 4942, 4943, 4944, 4945, 4946, 4947, 4948, 4949, 4950, 4951, 4952, 4953, 4954, 4955, 4956, 4957, 4958, 4959, 4960, 4961, 4962, 4963, 4964, 4965, 4966, 4967, 4968, 4969, 4970, 4971, 4972, 4973, 4974, 4975, 4976, 4977, 4978, 4979, 4980, 4981, 4982, 4983, 4984, 4985, 4986, 4987, 4988, 4989, 4990, 4991, 4992, 4993, 4994, 4995, 4996, 4997, 4998, 4999, 5000, 5001, 5002, 5003, 5004, 5005, 5006, 5007, 5008, 5009, 5010, 5011, 5012, 5013, 5014, 5015, 5016, 5017, 5018, 5019, 5020, 5021, 5022, 5023, 5024, 5025, 5026, 5027, 5028, 5029, 5030, 5031, 5032, 5033, 5034, 5035, 5036, 5037, 5038, 5039, 5040, 5041, 5042, 5043, 5044, 5045, 5046, 5047, 5048, 5049, 5050, 5051, 5052, 5053, 5054, 5055, 5056, 5057, 5058, 5059, 5060, 5061, 5062, 5063, 5064, 5065, 5066, 5067, 5068, 5069, 5070, 5071, 5072, 5073, 5074, 5075, 5076, 5077, 5078, 5079, 5080, 5081, 5082, 5083, 5084, 5085, 5086, 5087, 5088, 5089, 5090, 5091, 5092, 5093, 5094, 5095, 5096, 5097, 5098, 5099, 5100, 5101, 5102, 5103, 5104, 5105, 5106, 5107, 5108, 5109, 5110, 5111, 5112, 5113, 5114, 5115, 5116, 5117, 5118, 5119, 5120, 5121, 5122, 5123, 5124, 5125, 5126, 5127, 5128, 5129, 5130, 5131, 5132, 5133, 5134, 5135, 5136, 5137, 5138, 5139, 5140, 5141, 5142, 5143, 5144, 5145, 5146, 5147, 5148, 5149, 5150, 5151, 5152, 5153, 5154, 5155, 5156, 5157, 5158, 5159, 5160, 5161, 5162, 5163, 5164, 5165, 5166, 5167, 5168, 5169, 5170, 5171, 5172, 5173, 5174, 5175, 5176, 5177, 5178, 5179, 5180, 5181, 5182, 5183, 5184, 5185, 5186, 5187, 5188, 5189, 5190, 5191, 5192, 5193, 5194, 5195, 5196, 5197, 5198, 5199, 5200, 5201, 5202, 5203, 5204, 5205, 5206, 5207, 5208, 5209, 5210, 5211, 5212, 5213, 5214, 5215, 5217, 5218, 5219, 5220, 5221, 5222, 5223, 5224, 5225, 5226, 5227, 5228, 5229, 5230, 5231, 5232, 5233, 5234, 5235, 5236, 5237, 5238, 5239, 5240, 5241, 5242, 5243, 5244, 5245, 5246, 5247, 5248, 5249, 5250, 5251, 5252, 5253, 5254, 5255, 5256, 5257, 5258, 5259, 5260, 5261, 5262, 5263, 5264, 5265, 5266, 5267, 5268, 5269, 5270, 5271, 5272, 5273, 5274, 5275, 5276, 5277, 5278, 5279, 5280, 5281, 5282, 5283, 5284, 5285, 5286, 5287, 5288, 5289, 5290, 5291, 5292, 5293, 5294, 5295, 5296, 5297, 5298, 5299, 5300, 5301, 5302, 5303, 5304, 5305, 5306, 5307, 5308, 5309, 5310, 5311, 5312, 5313, 5314, 5315, 5316, 5317, 5318, 5319, 5320, 5321, 5322, 5323, 5324, 5325, 5326, 5328, 5329, 5330, 5331, 5332, 5333, 5334, 5335, 5336, 5337, 5338, 5339, 5340, 5341, 5342, 5343, 5344, 5345, 5346, 5347, 5348, 5349, 5350, 5351, 5352, 5353, 5354, 5355, 5356, 5357, 5358, 5359, 5360, 5361, 5362, 5363, 5364, 5365, 5366, 5367, 5368, 5369, 5370, 5371, 5372, 5373, 5374, 5375, 5376, 5377, 5378, 5379, 5380, 5381, 5382, 5383, 5384, 5385, 5386, 5387, 5388, 5389, 5390, 5391, 5392, 5393, 5394, 5395, 5396, 5397, 5398, 5399, 5400, 5401, 5402, 5403, 5404, 5405, 5406, 5407, 5408, 5409, 5410, 5411, 5412, 5413, 5414, 5415, 5416, 5417, 5418, 5419, 5420, 5421, 5422, 5423, 5424, 5425, 5426, 5427, 5428, 5429, 5430, 5431, 5432, 5433, 5434, 5435, 5436, 5437, 5438, 5439, 5440, 5441, 5442, 5443, 5444, 5445, 5446, 5447, 5448, 5449, 5450, 5451, 5452, 5453, 5454, 5456, 5457, 5458, 5459, 5460, 5461, 5462, 5463, 5464, 5465, 5466, 5467, 5468, 5469, 5470, 5471, 5472, 5473, 5474, 5475, 5476, 5477, 5478, 5479, 5480, 5481, 5482, 5483, 5484, 5485, 5486, 5487, 5488, 5489, 5490, 5491, 5492, 5493, 5494, 5495, 5496, 5497, 5498, 5499, 5500, 5501, 5502, 5503, 5504, 5505, 5506, 5507, 5508, 5509, 5510, 5511, 5512, 5513, 5514, 5515, 5516, 5517, 5518, 5519, 5520, 5521, 5522, 5523, 5524, 5525, 5526, 5527, 5528, 5529, 5530, 5531, 5532, 5533, 5534, 5535, 5536, 5537, 5538, 5539, 5540, 5541, 5542, 5543, 5544, 5545, 5546, 5547, 5548, 5549, 5550, 5551, 5552, 5553, 5554, 5555, 5556, 5557, 5558, 5559, 5560, 5561, 5562, 5563, 5564, 5565, 5566, 5567, 5568, 5569, 5570, 5571, 5572, 5573, 5574, 5575, 5576, 5577, 5578, 5579, 5580, 5581, 5582, 5583, 5584, 5585, 5586, 5587, 5588, 5589, 5590, 5591, 5592, 5593, 5594, 5595, 5596, 5597, 5598, 5599, 5600, 5601, 5602, 5603, 5604, 5605, 5606, 5607, 5608, 5609, 5610, 5611, 5612, 5613, 5614, 5615, 5616, 5617, 5618, 5619, 5620, 5621, 5622, 5623, 5624, 5625, 5626, 5627, 5628, 5629, 5630, 5631, 5632, 5633, 5634, 5635, 5636, 5637, 5638, 5639, 5640, 5641, 5642, 5643, 5644, 5645, 5646, 5647, 5648, 5649, 5650, 5651, 5652, 5653, 5654, 5655, 5656, 5657, 5658, 5660, 5661, </t>
         </is>
       </c>
-      <c r="BV2" t="n">
+      <c r="CD2" t="n">
         <v>0.07643312101910829</v>
       </c>
-      <c r="BW2" t="inlineStr">
+      <c r="CE2" t="inlineStr">
         <is>
           <t>{'Numk': 31, 'KPar': 8, 'Bucket_index': 1000}</t>
         </is>
       </c>
-      <c r="BX2" t="n">
+      <c r="CF2" t="n">
         <v>193.3085851250216</v>
       </c>
-      <c r="BY2" t="inlineStr">
+      <c r="CG2" t="inlineStr">
         <is>
           <t>no</t>
         </is>
       </c>
-      <c r="BZ2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CA2" t="inlineStr">
+      <c r="CH2" t="n">
+        <v>0</v>
+      </c>
+      <c r="CI2" t="inlineStr">
         <is>
           <t>params</t>
         </is>
       </c>
-      <c r="CB2" t="n">
+      <c r="CJ2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1264,93 +1328,117 @@
       <c r="BE3" t="n">
         <v>1</v>
       </c>
-      <c r="BF3" t="inlineStr"/>
-      <c r="BG3" t="inlineStr">
+      <c r="BF3" t="n">
+        <v>1</v>
+      </c>
+      <c r="BG3" t="n">
+        <v>1</v>
+      </c>
+      <c r="BH3" t="n">
+        <v>1</v>
+      </c>
+      <c r="BI3" t="n">
+        <v>1</v>
+      </c>
+      <c r="BJ3" t="n">
+        <v>1</v>
+      </c>
+      <c r="BK3" t="n">
+        <v>1</v>
+      </c>
+      <c r="BL3" t="n">
+        <v>1</v>
+      </c>
+      <c r="BM3" t="n">
+        <v>1</v>
+      </c>
+      <c r="BN3" t="inlineStr"/>
+      <c r="BO3" t="inlineStr">
         <is>
           <t>nab-data/realKnownCause/cpu_utilization_asg_misconfiguration.csv</t>
         </is>
       </c>
-      <c r="BH3" t="n">
+      <c r="BP3" t="n">
         <v>18050</v>
       </c>
-      <c r="BI3" t="inlineStr">
+      <c r="BQ3" t="inlineStr">
         <is>
           <t>NAB</t>
         </is>
       </c>
-      <c r="BJ3" t="n">
-        <v>1</v>
-      </c>
-      <c r="BK3" t="inlineStr">
+      <c r="BR3" t="n">
+        <v>1</v>
+      </c>
+      <c r="BS3" t="inlineStr">
         <is>
           <t>16551</t>
         </is>
       </c>
-      <c r="BL3" t="n">
+      <c r="BT3" t="n">
         <v>1498</v>
       </c>
-      <c r="BM3" t="inlineStr">
+      <c r="BU3" t="inlineStr">
         <is>
           <t>[1, 3, 34, 240, 551, 587, 623, 659, 779, 803, 815, 839, 851, 863, 875, 887, 899, 935, 947, 959, 1007, 1019, 1031, 1043, 1091, 1103, 1127, 1151, 1163, 1175, 1199, 1211, 1223, 1247, 1259, 1271, 1295, 1307, 1319, 1331, 1355, 1367, 1379, 1403, 1463, 1475, 1487, 1511, 1559, 1571, 1583, 1595, 1607, 1619, 1643, 1655, 1667, 1703, 2412, 2459, 2472, 2532, 2544, 2580, 2616, 2664, 2736, 2748, 2760, 2772, 2808, 2820, 2832, 2833, 2917, 3431, 3479, 3527, 3575, 3599, 3611, 3659, 3683, 3695, 3707, 3719, 3731, 3755, 3779, 3803, 3815, 3827, 3851, 3863, 3875, 3887, 3899, 3911, 3947, 3959, 3971, 3983, 3995, 4019, 4031, 4043, 4054, 4067, 4079, 4091, 4103, 4115, 4127, 4139, 4151, 4163, 4175, 4187, 4199, 4211, 4235, 4247, 4271, 4283, 4295, 4307, 4319, 4367, 4379, 4415, 4427, 4439, 4451, 4463, 4475, 4487, 4499, 4511, 4523, 4535, 4547, 4559, 4571, 4583, 4593, 4596, 4597, 4599, 4607, 4619, 4655, 4667, 4679, 4691, 4703, 4715, 4727, 4739, 4751, 4763, 4775, 4787, 4799, 4811, 4823, 4835, 4847, 4859, 4871, 4883, 4895, 4907, 4919, 4931, 4943, 4955, 4967, 4979, 4991, 4992, 5003, 5015, 5027, 5039, 5051, 5063, 5075, 5087, 5099, 5111, 5123, 5135, 5147, 5159, 5171, 5183, 5195, 5207, 5219, 5230, 5231, 5243, 5267, 5279, 5303, 5315, 5327, 5339, 5351, 5363, 5375, 5387, 5399, 5411, 5422, 5423, 5435, 5459, 5471, 5495, 5519, 5531, 5543, 5555, 5567, 5579, 5591, 5615, 5639, 5651, 5652, 5662, 5663, 5675, 5699, 5700, 5711, 5712, 5723, 5735, 5736, 5747, 5748, 5759, 5760, 5771, 5772, 5783, 5795, 5807, 5819, 5831, 5832, 5843, 5844, 5855, 5867, 5868, 5879, 5880, 5891, 5892, 5903, 5904, 5915, 5916, 5927, 5939, 5940, 5952, 6107, 6234, 6251, 6275, 6299, 6311, 6335, 6359, 6383, 6479, 6503, 6539, 6575, 6599, 6635, 6647, 6731, 6743, 6779, 6791, 6803, 6815, 6827, 6839, 6851, 6863, 6875, 6887, 6899, 6911, 6923, 6935, 6947, 6959, 6971, 6983, 7019, 7031, 7055, 7091, 7103, 7115, 7127, 7139, 7151, 7163, 7187, 7199, 7211, 7223, 7247, 7271, 7283, 7295, 7307, 7331, 7367, 7391, 7403, 7415, 7427, 7439, 7451, 7463, 7475, 7487, 7499, 7511, 7523, 7535, 7559, 7571, 7583, 7595, 7607, 7619, 7631, 7655, 7824, 7908, 7920, 7932, 7944, 7956, 7968, 7980, 8004, 8007, 8013, 8014, 8016, 8208, 8227, 8230, 8231, 8243, 8255, 8256, 8259, 8260, 8261, 8262, 8267, 8279, 8291, 8292, 8303, 8307, 8308, 8309, 8311, 8312, 8327, 8339, 8363, 8379, 8399, 8411, 8435, 8471, 8495, 8507, 8543, 8567, 8568, 8580, 8615, 8628, 8651, 8652, 8663, 8675, 8699, 8711, 8723, 8735, 8736, 8747, 8771, 8783, 8795, 8796, 8807, 8820, 8831, 8832, 8843, 8855, 8867, 8879, 8903, 8915, 8949, 8951, 8952, 8953, 8954, 8958, 8963, 8964, 8975, 8987, 8999, 9011, 9012, 9023, 9035, 9036, 9047, 9048, 9059, 9071, 9083, 9095, 9096, 9107, 9119, 9120, 9131, 9132, 9143, 9144, 9154, 9155, 9157, 9158, 9161, 9163, 9164, 9165, 9635, 9659, 9695, 9707, 9719, 9731, 9743, 9755, 9767, 9779, 9791, 9803, 9815, 9827, 9839, 9863, 9875, 9887, 9899, 9911, 9923, 9935, 9947, 9971, 9983, 9995, 10007, 10019, 10031, 10055, 10067, 10079, 10091, 10103, 10134, 10137, 10139, 10175, 10199, 10211, 10271, 10307, 10367, 10391, 10463, 10475, 10523, 10535, 10583, 10595, 10607, 10691, 10715, 10739, 10763, 10775, 10787, 10799, 10847, 10859, 10877, 10907, 10955, 11039, 11063, 11075, 11171, 11231, 11256, 11315, 11447, 11531, 11544, 11579, 11712, 11733, 11736, 11769, 11770, 11783, 11843, 11867, 11879, 11927, 11975, 12023, 12083, 12095, 12119, 12131, 12143, 12191, 12203, 12239, 12275, 12323, 12347, 12383, 12395, 12407, 12431, 12467, 12479, 12491, 12503, 12515, 12527, 12551, 12563, 12575, 12582, 12587, 12611, 12623, 12635, 12647, 12659, 12671, 12683, 12719, 12731, 12743, 12755, 12767, 12791, 12803, 12815, 12827, 12839, 12851, 12863, 12875, 12887, 12899, 12911, 12923, 12947, 12971, 12983, 13007, 13055, 13067, 13091, 13103, 13127, 13139, 13151, 13163, 13175, 13187, 13199, 13211, 13223, 13247, 13259, 13271, 13272, 13283, 13307, 13319, 13331, 13343, 13355, 13367, 13379, 13403, 13415, 13427, 13439, 13451, 13463, 13475, 13487, 13499, 13511, 13523, 13535, 13547, 13559, 13571, 13572, 13583, 13595, 13607, 13619, 13631, 13643, 13655, 13667, 13691, 13715, 13799, 14022, 14052, 14112, 14123, 14160, 14172, 14196, 14208, 14232, 14243, 14256, 14268, 14280, 14292, 14303, 14316, 14328, 14340, 14352, 14364, 14375, 14388, 14399, 14412, 14424, 14436, 14484, 14496, 14508, 14520, 14532, 14544, 14555, 14568, 14580, 14592, 14603, 14616, 14628, 14652, 14711, 14724, 14736, 14748, 14760, 14796, 14820, 14832, 14868, 14880, 14892, 14904, 14916, 14928, 14940, 14952, 14964, 14976, 14987, 15000, 15024, 15048, 15060, 15072, 15084, 15096, 15108, 15120, 15132, 15156, 15168, 15180, 15204, 15228, 15240, 15251, 15264, 15288, 15300, 15324, 15336, 15360, 15372, 15384, 15396, 15420, 15444, 15455, 15468, 15492, 15516, 15528, 15563, 15576, 15588, 15600, 15612, 15623, 15636, 15660, 15672, 15684, 15696, 15744, 15780, 15840, 15888, 15900, 15912, 15924, 15936, 15948, 15984, 15996, 16031, 16056, 16091, 16104, 16116, 16152, 16156, 16188, 16212, 16236, 16248, 16260, 16272, 16307, 16368, 16392, 16416, 16440, 16476, 16500, 16524, 16584, 16608, 16644, 16655, 16668, 16680, 16734, 16752, 16776, 16824, 16836, 16860, 16872, 16884, 16896, 16907, 16908, 16920, 16926, 16931, 16955, 16956, 16968, 16980, 16992, 16993, 16994, 16995, 16997, 16998, 16999, 17000, 17001, 17003, 17004, 17005, 17006, 17007, 17008, 17009, 17010, 17011, 17013, 17015, 17016, 17017, 17018, 17019, 17020, 17021, 17022, 17023, 17024, 17025, 17026, 17027, 17031, 17032, 17033, 17035, 17036, 17038, 17039, 17041, 17044, 17048, 17049, 17050, 17052, 17055, 17056, 17057, 17058, 17061, 17062, 17063, 17064, 17065, 17068, 17069, 17070, 17071, 17073, 17075, 17076, 17078, 17079, 17081, 17082, 17083, 17084, 17085, 17087, 17089, 17090, 17091, 17093, 17095, 17096, 17097, 17098, 17100, 17101, 17102, 17103, 17104, 17105, 17106, 17109, 17110, 17111, 17115, 17118, 17120, 17121, 17122, 17123, 17125, 17126, 17127, 17128, 17129, 17132, 17133, 17134, 17135, 17136, 17137, 17139, 17141, 17142, 17143, 17145, 17146, 17147, 17148, 17150, 17151, 17153, 17154, 17155, 17156, 17157, 17159, 17160, 17161, 17162, 17165, 17167, 17168, 17169, 17170, 17172, 17173, 17175, 17176, 17178, 17180, 17181, 17184, 17187, 17189, 17190, 17191, 17193, 17195, 17196, 17197, 17199, 17200, 17201, 17206, 17207, 17208, 17211, 17213, 17214, 17215, 17217, 17220, 17222, 17223, 17225, 17226, 17227, 17229, 17230, 17231, 17232, 17233, 17235, 17236, 17237, 17238, 17239, 17240, 17241, 17242, 17243, 17244, 17245, 17247, 17248, 17250, 17252, 17253, 17254, 17255, 17256, 17259, 17260, 17261, 17262, 17263, 17268, 17270, 17273, 17275, 17276, 17277, 17278, 17279, 17280, 17281, 17285, 17286, 17287, 17288, 17289, 17291, 17292, 17293, 17295, 17297, 17301, 17302, 17304, 17305, 17307, 17309, 17312, 17313, 17315, 17316, 17317, 17318, 17320, 17321, 17322, 17323, 17325, 17326, 17328, 17331, 17332, 17335, 17337, 17338, 17339, 17340, 17343, 17344, 17345, 17346, 17349, 17350, 17351, 17352, 17353, 17355, 17356, 17357, 17359, 17360, 17361, 17362, 17363, 17367, 17368, 17369, 17370, 17371, 17373, 17375, 17376, 17378, 17379, 17381, 17382, 17387, 17388, 17389, 17390, 17393, 17395, 17398, 17399, 17401, 17402, 17403, 17404, 17407, 17409, 17410, 17411, 17412, 17415, 17416, 17418, 17421, 17422, 17423, 17424, 17425, 17426, 17427, 17428, 17429, 17430, 17431, 17433, 17434, 17435, 17436, 17438, 17439, 17441, 17442, 17443, 17444, 17445, 17446, 17448, 17449, 17452, 17458, 17459, 17461, 17462, 17465, 17466, 17467, 17468, 17469, 17470, 17471, 17472, 17473, 17474, 17479, 17480, 17481, 17482, 17484, 17485, 17486, 17487, 17488, 17489, 17491, 17493, 17494, 17495, 17496, 17497, 17498, 17499, 17501, 17502, 17503, 17505, 17507, 17508, 17509, 17510, 17511, 17512, 17513, 17514, 17515, 17516, 17521, 17522, 17523, 17524, 17525, 17527, 17528, 17529, 17530, 17531, 17532, 17533, 17534, 17538, 17539, 17540, 17542, 17543, 17544, 17545, 17546, 17547, 17548, 17549, 17550, 17551, 17552, 17553, 17554, 17555, 17556, 17557, 17558, 17559, 17561, 17563, 17564, 17565, 17566, 17567, 17568, 17569, 17570, 17572, 17573, 17575, 17576, 17578, 17579, 17581, 17582, 17584, 17586, 17587, 17588, 17590, 17591, 17592, 17593, 17595, 17596, 17597, 17599, 17600, 17601, 17602, 17603, 17604, 17607, 17608, 17610, 17612, 17613, 17614, 17616, 17617, 17618, 17620, 17621, 17622, 17625, 17631, 17632, 17633, 17634, 17635, 17636, 17640, 17641, 17642, 17643, 17645, 17646, 17647, 17648, 17651, 17652, 17653, 17654, 17655, 17657, 17658, 17659, 17660, 17663, 17664, 17665, 17666, 17667, 17668, 17669, 17670, 17673, 17675, 17676, 17678, 17679, 17681, 17682, 17686, 17687, 17688, 17690, 17693, 17694, 17695, 17696, 17698, 17699, 17700, 17701, 17702, 17703, 17704, 17707, 17708, 17709, 17710, 17711, 17712, 17713, 17714, 17716, 17718, 17719, 17721, 17722, 17723, 17724, 17725, 17726, 17727, 17728, 17729, 17730, 17731, 17732, 17733, 17734, 17735, 17736, 17738, 17739, 17740, 17741, 17744, 17745, 17746, 17748, 17749, 17750, 17751, 17752, 17753, 17754, 17755, 17756, 17758, 17759, 17760, 17761, 17762, 17763, 17764, 17765, 17767, 17768, 17770, 17771, 17772, 17773, 17774, 17775, 17776, 17777, 17778, 17780, 17781, 17783, 17784, 17785, 17786, 17787, 17792, 17793, 17794, 17795, 17796, 17797, 17798, 17799, 17800, 17801, 17802, 17804, 17805, 17807, 17809, 17810, 17811, 17812, 17813, 17814, 17815, 17816, 17817, 17818, 17819, 17820, 17821, 17822, 17823, 17824, 17825, 17826, 17827, 17828, 17829, 17830, 17831, 17832, 17833, 17834, 17835, 17836, 17837, 17838, 17839, 17840, 17841, 17842, 17843, 17844, 17845, 17846, 17847, 17848, 17849, 17850, 17851, 17852, 17853, 17854, 17855, 17856, 17857, 17858, 17859, 17860, 17861, 17862, 17863, 17864, 17865, 17866, 17867, 17868, 17869, 17870, 17871, 17872, 17873, 17874, 17875, 17876, 17877, 17878, 17880, 17881, 17882, 17883, 17884, 17885, 17886, 17887, 17888, 17889, 17890, 17891, 17892, 17893, 17894, 17895, 17896, 17897, 17898, 17899, 17900, 17901, 17902, 17903, 17904, 17905, 17906, 17907, 17908, 17909, 17910, 17911, 17912, 17913, 17914, 17915, 17916, 17917, 17918, 17919, 17920, 17921, 17922, 17923, 17924, 17925, 17926, 17927, 17928, 17929, 17930, 17931, 17932, 17933, 17934, 17935, 17936, 17937, 17938, 17939, 17940, 17941, 17942, 17943, 17944, 17945, 17946, 17947, 17948, 17949, 17950, 17951, 17952, 17953, 17954, 17955, 17956, 17957, 17958, 17959, 17960, 17961, 17962, 17963, 17964, 17965, 17966, 17967, 17968, 17969, 17970, 17971, 17972, 17973, 17974, 17975, 17976, 17977, 17978, 17979, 17980, 17981, 17982, 17983, 17984, 17985, 17986, 17987, 17988, 17989, 17990, 17991, 17992, 17993, 17994, 17995, 17996, 17997, 17998, 17999, 18000, 18001, 18002, 18003, 18004, 18005, 18006, 18007, 18008, 18009, 18010, 18011, 18012, 18013, 18014, 18015, 18016, 18017, 18018, 18019, 18020, 18021, 18022, 18023, 18024, 18025, 18026, 18027, 18028, 18029, 18030, 18031, 18032, 18033, 18034, 18035, 18036, 18037, 18038, 18039, 18040, 18041, 18042, 18043, 18044, 18045, 18046, 18048, 18049]</t>
         </is>
       </c>
-      <c r="BN3" t="n">
+      <c r="BV3" t="n">
         <v>0.4466762314681971</v>
       </c>
-      <c r="BO3" t="inlineStr">
+      <c r="BW3" t="inlineStr">
         <is>
           <t>{'initial_window': 339, 'window_size': 3855, 'num_trees': 19, 'max_depth': 11}</t>
         </is>
       </c>
-      <c r="BP3" t="n">
+      <c r="BX3" t="n">
         <v>10.22733592498116</v>
       </c>
-      <c r="BQ3" t="inlineStr">
+      <c r="BY3" t="inlineStr">
         <is>
           <t>[16926, 16998, 17644]</t>
         </is>
       </c>
-      <c r="BR3" t="n">
-        <v>1</v>
-      </c>
-      <c r="BS3" t="inlineStr">
+      <c r="BZ3" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA3" t="inlineStr">
         <is>
           <t>{'AR_window_size': 29, 'differencing-order': 0}</t>
         </is>
       </c>
-      <c r="BT3" t="n">
+      <c r="CB3" t="n">
         <v>129.9010999479797</v>
       </c>
-      <c r="BU3" t="inlineStr">
+      <c r="CC3" t="inlineStr">
         <is>
           <t xml:space="preserve">[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86, 87, 88, 89, 90, 91, 92, 93, 94, 95, 96, 97, 98, 99, 100, 101, 102, 103, 104, 105, 106, 107, 108, 109, 110, 111, 112, 113, 114, 115, 116, 117, 118, 119, 120, 121, 122, 123, 124, 125, 126, 127, 128, 129, 130, 131, 132, 133, 134, 135, 136, 137, 138, 139, 140, 141, 142, 143, 144, 145, 146, 147, 148, 149, 150, 151, 152, 153, 154, 155, 156, 157, 158, 159, 160, 161, 162, 163, 164, 165, 166, 167, 168, 169, 170, 171, 172, 173, 174, 175, 176, 177, 178, 179, 180, 181, 182, 183, 184, 185, 186, 187, 188, 189, 190, 191, 192, 193, 194, 195, 196, 197, 198, 199, 200, 201, 202, 203, 204, 205, 206, 207, 208, 209, 210, 211, 212, 213, 214, 215, 216, 217, 218, 219, 220, 221, 222, 223, 224, 225, 226, 227, 228, 229, 230, 231, 232, 233, 234, 235, 236, 237, 238, 239, 240, 241, 242, 243, 244, 245, 246, 247, 248, 249, 250, 251, 252, 253, 254, 255, 256, 257, 258, 259, 260, 261, 262, 263, 264, 265, 266, 267, 268, 269, 270, 271, 272, 273, 274, 275, 276, 277, 278, 279, 280, 281, 282, 283, 284, 285, 286, 287, 288, 289, 290, 291, 292, 293, 294, 295, 296, 297, 298, 299, 300, 301, 302, 303, 304, 305, 306, 307, 308, 309, 310, 311, 312, 313, 314, 315, 316, 317, 318, 319, 320, 321, 322, 323, 324, 325, 326, 327, 328, 329, 330, 331, 332, 333, 334, 335, 336, 337, 338, 339, 340, 341, 342, 343, 344, 345, 346, 347, 348, 349, 350, 351, 352, 353, 354, 355, 356, 357, 358, 359, 360, 361, 362, 363, 364, 365, 366, 367, 368, 369, 370, 371, 372, 373, 374, 375, 376, 377, 378, 379, 380, 381, 382, 383, 384, 385, 386, 387, 388, 389, 390, 391, 392, 393, 394, 395, 396, 397, 398, 399, 400, 401, 402, 403, 404, 405, 406, 407, 408, 409, 410, 411, 412, 413, 414, 415, 416, 417, 418, 419, 420, 421, 422, 423, 424, 425, 426, 427, 428, 429, 430, 431, 432, 433, 434, 435, 436, 437, 438, 439, 440, 441, 442, 443, 444, 445, 446, 447, 448, 449, 450, 451, 452, 453, 454, 455, 456, 457, 458, 459, 460, 461, 462, 463, 464, 465, 466, 467, 468, 469, 470, 471, 472, 473, 474, 475, 476, 477, 478, 479, 480, 481, 482, 483, 484, 485, 486, 487, 488, 489, 490, 491, 492, 493, 494, 495, 496, 497, 498, 499, 500, 501, 502, 503, 504, 505, 506, 507, 508, 509, 510, 511, 512, 513, 514, 515, 516, 517, 518, 519, 520, 521, 522, 523, 524, 525, 526, 527, 528, 529, 530, 531, 532, 533, 534, 535, 536, 537, 538, 539, 540, 541, 542, 543, 544, 545, 546, 547, 548, 549, 550, 551, 552, 553, 554, 555, 556, 557, 558, 559, 560, 561, 562, 563, 564, 565, 566, 567, 568, 569, 570, 571, 572, 573, 574, 575, 576, 577, 578, 579, 580, 581, 582, 583, 584, 585, 586, 587, 588, 589, 590, 591, 592, 593, 594, 595, 596, 597, 598, 599, 600, 601, 602, 603, 604, 605, 606, 607, 608, 609, 610, 611, 612, 613, 614, 615, 616, 617, 618, 619, 620, 621, 622, 623, 624, 625, 626, 627, 628, 629, 630, 631, 632, 633, 634, 635, 636, 637, 638, 639, 640, 641, 642, 643, 644, 645, 646, 647, 648, 649, 650, 651, 652, 653, 654, 655, 656, 657, 658, 659, 660, 661, 662, 663, 664, 665, 666, 667, 668, 669, 670, 671, 672, 673, 674, 675, 676, 677, 678, 679, 680, 681, 682, 683, 684, 685, 686, 687, 688, 689, 690, 691, 692, 693, 694, 695, 696, 697, 698, 699, 700, 701, 702, 703, 704, 705, 706, 707, 708, 709, 710, 711, 712, 713, 714, 715, 716, 717, 718, 719, 720, 721, 722, 723, 724, 725, 726, 727, 728, 729, 730, 731, 732, 733, 734, 735, 736, 737, 738, 739, 740, 741, 742, 743, 744, 745, 746, 747, 748, 749, 750, 751, 752, 753, 754, 755, 756, 757, 758, 759, 760, 761, 762, 763, 764, 765, 766, 767, 768, 769, 770, 771, 772, 773, 774, 775, 776, 777, 778, 779, 780, 781, 782, 783, 784, 785, 786, 787, 788, 789, 790, 791, 792, 793, 794, 795, 796, 797, 798, 799, 800, 801, 802, 803, 804, 805, 806, 807, 808, 809, 810, 811, 812, 813, 814, 815, 816, 817, 818, 819, 820, 821, 822, 823, 824, 825, 826, 827, 828, 829, 830, 831, 832, 833, 834, 835, 836, 837, 838, 839, 840, 841, 842, 843, 844, 845, 846, 847, 848, 849, 850, 851, 852, 853, 854, 855, 856, 857, 858, 859, 860, 861, 862, 863, 864, 865, 866, 867, 868, 869, 870, 871, 872, 873, 874, 875, 876, 877, 878, 879, 880, 881, 882, 883, 884, 885, 886, 887, 888, 889, 890, 891, 892, 893, 894, 895, 896, 897, 898, 899, 900, 901, 902, 903, 904, 905, 906, 907, 908, 909, 910, 911, 912, 913, 914, 915, 916, 917, 918, 919, 920, 921, 922, 923, 924, 925, 926, 927, 928, 929, 930, 931, 932, 933, 934, 935, 936, 937, 938, 939, 940, 941, 942, 943, 944, 945, 946, 947, 948, 949, 950, 951, 952, 953, 954, 955, 956, 957, 958, 959, 960, 961, 962, 963, 964, 965, 966, 967, 968, 969, 970, 971, 972, 973, 974, 975, 976, 977, 978, 979, 980, 981, 982, 983, 984, 985, 986, 987, 988, 989, 990, 991, 992, 993, 994, 995, 996, 997, 998, 999, 1000, 1001, 1002, 1003, 1004, 1005, 1006, 1007, 1008, 1009, 1010, 1011, 1012, 1013, 1014, 1015, 1016, 1017, 1018, 1019, 1020, 1021, 1022, 1023, 1024, 1025, 1026, 1027, 1028, 1029, 1030, 1031, 1032, 1033, 1034, 1035, 1036, 1037, 1038, 1039, 1040, 1041, 1042, 1043, 1044, 1045, 1046, 1047, 1048, 1049, 1050, 1051, 1052, 1053, 1054, 1055, 1056, 1057, 1058, 1059, 1060, 1061, 1062, 1063, 1064, 1065, 1066, 1067, 1068, 1069, 1070, 1071, 1072, 1073, 1074, 1075, 1076, 1077, 1078, 1079, 1080, 1081, 1082, 1083, 1084, 1085, 1086, 1087, 1088, 1089, 1090, 1091, 1092, 1093, 1094, 1095, 1096, 1097, 1098, 1099, 1100, 1101, 1102, 1103, 1104, 1105, 1106, 1107, 1108, 1109, 1110, 1111, 1112, 1113, 1114, 1115, 1116, 1117, 1118, 1119, 1120, 1121, 1122, 1123, 1124, 1125, 1126, 1127, 1128, 1129, 1130, 1131, 1132, 1133, 1134, 1135, 1136, 1137, 1138, 1139, 1140, 1141, 1142, 1143, 1144, 1145, 1146, 1147, 1148, 1149, 1150, 1151, 1152, 1153, 1154, 1155, 1156, 1157, 1158, 1159, 1160, 1161, 1162, 1163, 1164, 1165, 1166, 1167, 1168, 1169, 1170, 1171, 1172, 1173, 1174, 1175, 1176, 1177, 1178, 1179, 1180, 1181, 1182, 1183, 1184, 1185, 1186, 1187, 1188, 1189, 1190, 1191, 1192, 1193, 1194, 1195, 1196, 1197, 1198, 1199, 1200, 1201, 1202, 1203, 1204, 1205, 1206, 1207, 1208, 1209, 1210, 1211, 1212, 1213, 1214, 1215, 1216, 1217, 1218, 1219, 1220, 1221, 1222, 1223, 1224, 1225, 1226, 1227, 1228, 1229, 1230, 1231, 1232, 1233, 1234, 1235, 1236, 1237, 1238, 1239, 1240, 1241, 1242, 1243, 1244, 1245, 1246, 1247, 1248, 1249, 1250, 1251, 1252, 1253, 1254, 1255, 1256, 1257, 1258, 1259, 1260, 1261, 1262, 1263, 1264, 1265, 1266, 1267, 1268, 1269, 1270, 1271, 1272, 1273, 1274, 1275, 1276, 1277, 1278, 1279, 1280, 1281, 1282, 1283, 1284, 1285, 1286, 1287, 1288, 1289, 1290, 1291, 1292, 1293, 1294, 1295, 1296, 1297, 1298, 1299, 1300, 1301, 1302, 1303, 1304, 1305, 1306, 1307, 1308, 1309, 1310, 1311, 1312, 1313, 1314, 1315, 1316, 1317, 1318, 1319, 1320, 1321, 1322, 1323, 1324, 1325, 1326, 1327, 1328, 1329, 1330, 1331, 1332, 1333, 1334, 1335, 1336, 1337, 1338, 1339, 1340, 1341, 1342, 1343, 1344, 1345, 1346, 1347, 1348, 1349, 1350, 1351, 1352, 1353, 1354, 1355, 1356, 1357, 1358, 1359, 1360, 1361, 1362, 1363, 1364, 1365, 1366, 1367, 1368, 1369, 1370, 1371, 1372, 1373, 1374, 1375, 1376, 1377, 1378, 1379, 1380, 1381, 1382, 1383, 1384, 1385, 1386, 1387, 1388, 1389, 1390, 1391, 1392, 1393, 1394, 1395, 1396, 1397, 1398, 1399, 1400, 1401, 1402, 1403, 1404, 1405, 1406, 1407, 1408, 1409, 1410, 1411, 1412, 1413, 1414, 1415, 1416, 1417, 1418, 1419, 1420, 1421, 1422, 1423, 1424, 1425, 1426, 1427, 1428, 1429, 1430, 1431, 1432, 1433, 1434, 1435, 1436, 1437, 1438, 1439, 1440, 1441, 1442, 1443, 1444, 1445, 1446, 1447, 1448, 1449, 1450, 1451, 1452, 1453, 1454, 1455, 1456, 1457, 1458, 1459, 1460, 1461, 1462, 1463, 1464, 1465, 1466, 1467, 1468, 1469, 1470, 1471, 1472, 1473, 1474, 1475, 1476, 1477, 1478, 1479, 1480, 1481, 1482, 1483, 1484, 1485, 1486, 1487, 1488, 1489, 1490, 1491, 1492, 1493, 1494, 1495, 1496, 1497, 1498, 1499, 1500, 1501, 1502, 1503, 1504, 1505, 1506, 1507, 1508, 1509, 1510, 1511, 1512, 1513, 1514, 1515, 1516, 1517, 1518, 1519, 1520, 1521, 1522, 1523, 1524, 1525, 1526, 1527, 1528, 1529, 1530, 1531, 1532, 1533, 1534, 1535, 1536, 1537, 1538, 1539, 1540, 1541, 1542, 1543, 1544, 1545, 1546, 1547, 1548, 1549, 1550, 1551, 1552, 1553, 1554, 1555, 1556, 1557, 1558, 1559, 1560, 1561, 1562, 1563, 1564, 1565, 1566, 1567, 1568, 1569, 1570, 1571, 1572, 1573, 1574, 1575, 1576, 1577, 1578, 1579, 1580, 1581, 1582, 1583, 1584, 1585, 1586, 1587, 1588, 1589, 1590, 1591, 1592, 1593, 1594, 1595, 1596, 1597, 1598, 1599, 1600, 1601, 1602, 1603, 1604, 1605, 1606, 1607, 1608, 1609, 1610, 1611, 1612, 1613, 1614, 1615, 1616, 1617, 1618, 1619, 1620, 1621, 1622, 1623, 1624, 1625, 1626, 1627, 1628, 1629, 1630, 1631, 1632, 1633, 1634, 1635, 1636, 1637, 1638, 1639, 1640, 1641, 1642, 1643, 1644, 1645, 1646, 1647, 1648, 1649, 1650, 1651, 1652, 1653, 1654, 1655, 1656, 1657, 1658, 1659, 1660, 1661, 1662, 1663, 1664, 1665, 1666, 1667, 1668, 1669, 1670, 1671, 1672, 1673, 1674, 1675, 1676, 1677, 1678, 1679, 1680, 1681, 1682, 1683, 1684, 1685, 1686, 1687, 1688, 1689, 1690, 1691, 1692, 1693, 1694, 1695, 1696, 1697, 1698, 1699, 1700, 1701, 1702, 1703, 1704, 1705, 1706, 1707, 1708, 1709, 1710, 1711, 1712, 1713, 1714, 1715, 1716, 1717, 1718, 1719, 1720, 1721, 1722, 1723, 1724, 1725, 1726, 1727, 1728, 1729, 1730, 1731, 1732, 1733, 1734, 1735, 1736, 1737, 1738, 1739, 1740, 1741, 1742, 1743, 1744, 1745, 1746, 1747, 1748, 1749, 1750, 1751, 1752, 1753, 1754, 1755, 1756, 1757, 1758, 1759, 1760, 1761, 1762, 1763, 1764, 1765, 1766, 1767, 1768, 1769, 1770, 1771, 1772, 1773, 1774, 1775, 1776, 1777, 1778, 1779, 1780, 1781, 1782, 1783, 1784, 1785, 1786, 1787, 1788, 1789, 1790, 1791, 1792, 1793, 1794, 1795, 1796, 1797, 1798, 1799, 1800, 1801, 1802, 1803, 1804, 1805, 1806, 1807, 1808, 1809, 1810, 1811, 1812, 1813, 1814, 1815, 1816, 1817, 1818, 1819, 1820, 1821, 1822, 1823, 1824, 1825, 1826, 1827, 1828, 1829, 1830, 1831, 1832, 1833, 1834, 1835, 1836, 1837, 1838, 1839, 1840, 1841, 1842, 1843, 1844, 1845, 1846, 1847, 1848, 1849, 1850, 1851, 1852, 1853, 1854, 1855, 1856, 1857, 1858, 1859, 1860, 1861, 1862, 1863, 1864, 1865, 1866, 1867, 1868, 1869, 1870, 1871, 1872, 1873, 1874, 1875, 1876, 1877, 1878, 1879, 1880, 1881, 1882, 1883, 1884, 1885, 1886, 1887, 1888, 1889, 1890, 1891, 1892, 1893, 1894, 1895, 1896, 1897, 1898, 1899, 1900, 1901, 1902, 1903, 1904, 1905, 1906, 1907, 1908, 1909, 1910, 1911, 1912, 1913, 1914, 1915, 1916, 1917, 1918, 1919, 1920, 1921, 1922, 1923, 1924, 1925, 1926, 1927, 1928, 1929, 1930, 1931, 1932, 1933, 1934, 1935, 1936, 1937, 1938, 1939, 1940, 1941, 1942, 1943, 1944, 1945, 1946, 1947, 1948, 1949, 1950, 1951, 1952, 1953, 1954, 1955, 1956, 1957, 1958, 1959, 1960, 1961, 1962, 1963, 1964, 1965, 1966, 1967, 1968, 1969, 1970, 1971, 1972, 1973, 1974, 1975, 1976, 1977, 1978, 1979, 1980, 1981, 1982, 1983, 1984, 1985, 1986, 1987, 1988, 1989, 1990, 1991, 1992, 1993, 1994, 1995, 1996, 1997, 1998, 1999, 2000, 2001, 2002, 2003, 2004, 2005, 2006, 2007, 2008, 2009, 2010, 2011, 2012, 2013, 2014, 2015, 2016, 2017, 2018, 2019, 2020, 2021, 2022, 2023, 2024, 2025, 2026, 2027, 2028, 2029, 2030, 2031, 2032, 2033, 2034, 2035, 2036, 2037, 2038, 2039, 2040, 2041, 2042, 2043, 2044, 2045, 2046, 2047, 2048, 2049, 2050, 2051, 2052, 2053, 2054, 2055, 2056, 2057, 2058, 2059, 2060, 2061, 2062, 2063, 2064, 2065, 2066, 2067, 2068, 2069, 2070, 2071, 2072, 2073, 2074, 2075, 2076, 2077, 2078, 2079, 2080, 2081, 2082, 2083, 2084, 2085, 2086, 2087, 2088, 2089, 2090, 2091, 2092, 2093, 2094, 2095, 2096, 2097, 2098, 2099, 2100, 2101, 2102, 2103, 2104, 2105, 2106, 2107, 2108, 2109, 2110, 2111, 2112, 2113, 2114, 2115, 2116, 2117, 2118, 2119, 2120, 2121, 2122, 2123, 2124, 2125, 2126, 2127, 2128, 2129, 2130, 2131, 2132, 2133, 2134, 2135, 2136, 2137, 2138, 2139, 2140, 2141, 2142, 2143, 2144, 2145, 2146, 2147, 2148, 2149, 2150, 2151, 2152, 2153, 2154, 2155, 2156, 2157, 2158, 2159, 2160, 2161, 2162, 2163, 2164, 2165, 2166, 2167, 2168, 2169, 2170, 2171, 2172, 2173, 2174, 2175, 2176, 2177, 2178, 2179, 2180, 2181, 2182, 2183, 2184, 2185, 2186, 2187, 2188, 2189, 2190, 2191, 2192, 2193, 2194, 2195, 2196, 2197, 2198, 2199, 2200, 2201, 2202, 2203, 2204, 2205, 2206, 2207, 2208, 2209, 2210, 2211, 2212, 2213, 2214, 2215, 2216, 2217, 2218, 2219, 2220, 2221, 2222, 2223, 2224, 2225, 2226, 2227, 2228, 2229, 2230, 2231, 2232, 2233, 2234, 2235, 2236, 2237, 2238, 2239, 2240, 2241, 2242, 2243, 2244, 2245, 2246, 2247, 2248, 2249, 2250, 2251, 2252, 2253, 2254, 2255, 2256, 2257, 2258, 2259, 2260, 2261, 2262, 2263, 2264, 2265, 2266, 2267, 2268, 2269, 2270, 2271, 2272, 2273, 2274, 2275, 2276, 2277, 2278, 2279, 2280, 2281, 2282, 2283, 2284, 2285, 2286, 2287, 2288, 2289, 2290, 2291, 2292, 2293, 2294, 2295, 2296, 2297, 2298, 2299, 2300, 2301, 2302, 2303, 2304, 2305, 2306, 2307, 2308, 2309, 2310, 2311, 2312, 2313, 2314, 2315, 2316, 2317, 2318, 2319, 2320, 2321, 2322, 2323, 2324, 2325, 2326, 2327, 2328, 2329, 2330, 2331, 2332, 2333, 2334, 2335, 2336, 2337, 2338, 2339, 2340, 2341, 2342, 2343, 2344, 2345, 2346, 2347, 2348, 2349, 2350, 2351, 2352, 2353, 2354, 2355, 2356, 2357, 2358, 2359, 2360, 2361, 2362, 2363, 2364, 2365, 2366, 2367, 2368, 2369, 2370, 2371, 2372, 2373, 2374, 2375, 2376, 2377, 2378, 2379, 2380, 2381, 2382, 2383, 2384, 2385, 2386, 2387, 2388, 2389, 2390, 2391, 2392, 2393, 2394, 2395, 2396, 2397, 2398, 2399, 2400, 2401, 2402, 2403, 2404, 2405, 2406, 2407, 2408, 2409, 2410, 2411, 2412, 2413, 2414, 2415, 2416, 2417, 2418, 2419, 2420, 2421, 2422, 2423, 2424, 2425, 2426, 2427, 2428, 2429, 2430, 2431, 2432, 2433, 2434, 2435, 2436, 2437, 2438, 2439, 2440, 2441, 2442, 2443, 2444, 2445, 2446, 2447, 2448, 2449, 2450, 2451, 2452, 2453, 2454, 2455, 2456, 2457, 2458, 2459, 2460, 2461, 2462, 2463, 2464, 2465, 2466, 2467, 2468, 2469, 2470, 2471, 2472, 2473, 2474, 2475, 2476, 2477, 2478, 2479, 2480, 2481, 2482, 2483, 2484, 2485, 2486, 2487, 2488, 2489, 2490, 2491, 2492, 2493, 2494, 2495, 2496, 2497, 2498, 2499, 2500, 2501, 2502, 2503, 2504, 2505, 2506, 2507, 2508, 2509, 2510, 2511, 2512, 2513, 2514, 2515, 2516, 2517, 2518, 2519, 2520, 2521, 2522, 2523, 2524, 2525, 2526, 2527, 2528, 2529, 2530, 2531, 2532, 2533, 2534, 2535, 2536, 2537, 2538, 2539, 2540, 2541, 2542, 2543, 2544, 2545, 2546, 2547, 2548, 2549, 2550, 2551, 2552, 2553, 2554, 2555, 2556, 2557, 2558, 2559, 2560, 2561, 2562, 2563, 2564, 2565, 2566, 2567, 2568, 2569, 2570, 2571, 2572, 2573, 2574, 2575, 2576, 2577, 2578, 2579, 2580, 2581, 2582, 2583, 2584, 2585, 2586, 2587, 2588, 2589, 2590, 2591, 2592, 2593, 2594, 2595, 2596, 2597, 2598, 2599, 2600, 2601, 2602, 2603, 2604, 2605, 2606, 2607, 2608, 2609, 2610, 2611, 2612, 2613, 2614, 2615, 2616, 2617, 2618, 2619, 2620, 2621, 2622, 2623, 2624, 2625, 2626, 2627, 2628, 2629, 2630, 2631, 2632, 2633, 2634, 2635, 2636, 2637, 2638, 2639, 2640, 2641, 2642, 2643, 2644, 2645, 2646, 2647, 2648, 2649, 2650, 2651, 2652, 2653, 2654, 2655, 2656, 2657, 2658, 2659, 2660, 2661, 2662, 2663, 2664, 2665, 2666, 2667, 2668, 2669, 2670, 2671, 2672, 2673, 2674, 2675, 2676, 2677, 2678, 2679, 2680, 2681, 2682, 2683, 2684, 2685, 2686, 2687, 2688, 2689, 2690, 2691, 2692, 2693, 2694, 2695, 2696, 2697, 2698, 2699, 2700, 2701, 2702, 2703, 2704, 2705, 2706, 2707, 2708, 2709, 2710, 2711, 2712, 2713, 2714, 2715, 2716, 2717, 2718, 2719, 2720, 2721, 2722, 2723, 2724, 2725, 2726, 2727, 2728, 2729, 2730, 2731, 2732, 2733, 2734, 2735, 2736, 2737, 2738, 2739, 2740, 2741, 2742, 2743, 2744, 2745, 2746, 2747, 2748, 2749, 2750, 2751, 2752, 2753, 2754, 2755, 2756, 2757, 2758, 2759, 2760, 2761, 2762, 2763, 2764, 2765, 2766, 2767, 2768, 2769, 2770, 2771, 2772, 2773, 2774, 2775, 2776, 2777, 2778, 2779, 2780, 2781, 2782, 2783, 2784, 2785, 2786, 2787, 2788, 2789, 2790, 2791, 2792, 2793, 2794, 2795, 2796, 2797, 2798, 2799, 2800, 2801, 2802, 2803, 2804, 2805, 2806, 2807, 2808, 2809, 2810, 2811, 2812, 2813, 2814, 2815, 2816, 2817, 2818, 2819, 2820, 2821, 2822, 2823, 2824, 2825, 2826, 2827, 2828, 2829, 2830, 2831, 2832, 2833, 2834, 2835, 2836, 2837, 2838, 2839, 2840, 2841, 2842, 2843, 2844, 2845, 2846, 2847, 2848, 2849, 2850, 2851, 2852, 2853, 2854, 2855, 2856, 2857, 2858, 2859, 2860, 2861, 2862, 2863, 2864, 2865, 2866, 2867, 2868, 2869, 2870, 2871, 2872, 2873, 2874, 2875, 2876, 2877, 2878, 2879, 2880, 2881, 2882, 2883, 2884, 2885, 2886, 2887, 2888, 2889, 2890, 2891, 2892, 2893, 2894, 2895, 2896, 2897, 2898, 2899, 2900, 2901, 2902, 2903, 2904, 2905, 2906, 2907, 2908, 2909, 2910, 2911, 2912, 2913, 2914, 2915, 2916, 2917, 2918, 2919, 2920, 2921, 2922, 2923, 2924, 2925, 2926, 2927, 2928, 2929, 2930, 2931, 2932, 2933, 2934, 2935, 2936, 2937, 2938, 2939, 2940, 2941, 2942, 2943, 2944, 2945, 2946, 2947, 2948, 2949, 2950, 2951, 2952, 2953, 2954, 2955, 2956, 2957, 2958, 2959, 2960, 2961, 2962, 2963, 2964, 2965, 2966, 2967, 2968, 2969, 2970, 2971, 2972, 2973, 2974, 2975, 2976, 2977, 2978, 2979, 2980, 2981, 2982, 2983, 2984, 2985, 2986, 2987, 2988, 2989, 2990, 2991, 2992, 2993, 2994, 2995, 2996, 2997, 2998, 2999, 3000, 3001, 3002, 3003, 3004, 3005, 3006, 3007, 3008, 3009, 3010, 3011, 3012, 3013, 3014, 3015, 3016, 3017, 3018, 3019, 3020, 3021, 3022, 3023, 3024, 3025, 3026, 3027, 3028, 3029, 3030, 3031, 3032, 3033, 3034, 3035, 3036, 3037, 3038, 3039, 3040, 3041, 3042, 3043, 3044, 3045, 3046, 3047, 3048, 3049, 3050, 3051, 3052, 3053, 3054, 3055, 3056, 3057, 3058, 3059, 3060, 3061, 3062, 3063, 3064, 3065, 3066, 3067, 3068, 3069, 3070, 3071, 3072, 3073, 3074, 3075, 3076, 3077, 3078, 3079, 3080, 3081, 3082, 3083, 3084, 3085, 3086, 3087, 3088, 3089, 3090, 3091, 3092, 3093, 3094, 3095, 3096, 3097, 3098, 3099, 3100, 3101, 3102, 3103, 3104, 3105, 3106, 3107, 3108, 3109, 3110, 3111, 3112, 3113, 3114, 3115, 3116, 3117, 3118, 3119, 3120, 3121, 3122, 3123, 3124, 3125, 3126, 3127, 3128, 3129, 3130, 3131, 3132, 3133, 3134, 3135, 3136, 3137, 3138, 3139, 3140, 3141, 3142, 3143, 3144, 3145, 3146, 3147, 3148, 3149, 3150, 3151, 3152, 3153, 3154, 3155, 3156, 3157, 3158, 3159, 3160, 3161, 3162, 3163, 3164, 3165, 3166, 3167, 3168, 3169, 3170, 3171, 3172, 3173, 3174, 3175, 3176, 3177, 3178, 3179, 3180, 3181, 3182, 3183, 3184, 3185, 3186, 3187, 3188, 3189, 3190, 3191, 3192, 3193, 3194, 3195, 3196, 3197, 3198, 3199, 3200, 3201, 3202, 3203, 3204, 3205, 3206, 3207, 3208, 3209, 3210, 3211, 3212, 3213, 3214, 3215, 3216, 3217, 3218, 3219, 3220, 3221, 3222, 3223, 3224, 3225, 3226, 3227, 3228, 3229, 3230, 3231, 3232, 3233, 3234, 3235, 3236, 3237, 3238, 3239, 3240, 3241, 3242, 3243, 3244, 3245, 3246, 3247, 3248, 3249, 3250, 3251, 3252, 3253, 3254, 3255, 3256, 3257, 3258, 3259, 3260, 3261, 3262, 3263, 3264, 3265, 3266, 3267, 3268, 3269, 3270, 3271, 3272, 3273, 3274, 3275, 3276, 3277, 3278, 3279, 3280, 3281, 3282, 3283, 3284, 3285, 3286, 3287, 3288, 3289, 3290, 3291, 3292, 3293, 3294, 3295, 3296, 3297, 3298, 3299, 3300, 3301, 3302, 3303, 3304, 3305, 3306, 3307, 3308, 3309, 3310, 3311, 3312, 3313, 3314, 3315, 3316, 3317, 3318, 3319, 3320, 3321, 3322, 3323, 3324, 3325, 3326, 3327, 3328, 3329, 3330, 3331, 3332, 3333, 3334, 3335, 3336, 3337, 3338, 3339, 3340, 3341, 3342, 3343, 3344, 3345, 3346, 3347, 3348, 3349, 3350, 3351, 3352, 3353, 3354, 3355, 3356, 3357, 3358, 3359, 3360, 3361, 3362, 3363, 3364, 3365, 3366, 3367, 3368, 3369, 3370, 3371, 3372, 3373, 3374, 3375, 3376, 3377, 3378, 3379, 3380, 3381, 3382, 3383, 3384, 3385, 3386, 3387, 3388, 3389, 3390, 3391, 3392, 3393, 3394, 3395, 3396, 3397, 3398, 3399, 3400, 3401, 3402, 3403, 3404, 3405, 3406, 3407, 3408, 3409, 3410, 3411, 3412, 3413, 3414, 3415, 3416, 3417, 3418, 3419, 3420, 3421, 3422, 3423, 3424, 3425, 3426, 3427, 3428, 3429, 3430, 3431, 3432, 3433, 3434, 3435, 3436, 3437, 3438, 3439, 3440, 3441, 3442, 3443, 3444, 3445, 3446, 3447, 3448, 3449, 3450, 3451, 3452, 3453, 3454, 3455, 3456, 3457, 3458, 3459, 3460, 3461, 3462, 3463, 3464, 3465, 3466, 3467, 3468, 3469, 3470, 3471, 3472, 3473, 3474, 3475, 3476, 3477, 3478, 3479, 3480, 3481, 3482, 3483, 3484, 3485, 3486, 3487, 3488, 3489, 3490, 3491, 3492, 3493, 3494, 3495, 3496, 3497, 3498, 3499, 3500, 3501, 3502, 3503, 3504, 3505, 3506, 3507, 3508, 3509, 3510, 3511, 3512, 3513, 3514, 3515, 3516, 3517, 3518, 3519, 3520, 3521, 3522, 3523, 3524, 3525, 3526, 3527, 3528, 3529, 3530, 3531, 3532, 3533, 3534, 3535, 3536, 3537, 3538, 3539, 3540, 3541, 3542, 3543, 3544, 3545, 3546, 3547, 3548, 3549, 3550, 3551, 3552, 3553, 3554, 3555, 3556, 3557, 3558, 3559, 3560, 3561, 3562, 3563, 3564, 3565, 3566, 3567, 3568, 3569, 3570, 3571, 3572, 3573, 3574, 3575, 3576, 3577, 3578, 3579, 3580, 3581, 3582, 3583, 3584, 3585, 3586, 3587, 3588, 3589, 3590, 3591, 3592, 3593, 3594, 3595, 3596, 3597, 3598, 3599, 3600, 3601, 3602, 3603, 3604, 3605, 3606, 3607, 3608, 3609, 3610, 3611, 3612, 3613, 3614, 3615, 3616, 3617, 3618, 3619, 3620, 3621, 3622, 3623, 3624, 3625, 3626, 3627, 3628, 3629, 3630, 3631, 3632, 3633, 3634, 3635, 3636, 3637, 3638, 3639, 3640, 3641, 3642, 3643, 3644, 3645, 3646, 3647, 3648, 3649, 3650, 3651, 3652, 3653, 3654, 3655, 3656, 3657, 3658, 3659, 3660, 3661, 3662, 3663, 3664, 3665, 3666, 3667, 3668, 3669, 3670, 3671, 3672, 3673, 3674, 3675, 3676, 3677, 3678, 3679, 3680, 3681, 3682, 3683, 3684, 3685, 3686, 3687, 3688, 3689, 3690, 3691, 3692, 3693, 3694, 3695, 3696, 3697, 3698, 3699, 3700, 3701, 3702, 3703, 3704, 3705, 3706, 3707, 3708, 3709, 3710, 3711, 3712, 3713, 3714, 3715, 3716, 3717, 3718, 3719, 3720, 3721, 3722, 3723, 3724, 3725, 3726, 3727, 3728, 3729, 3730, 3731, 3732, 3733, 3734, 3735, 3736, 3737, 3738, 3739, 3740, 3741, 3742, 3743, 3744, 3745, 3746, 3747, 3748, 3749, 3750, 3751, 3752, 3753, 3754, 3755, 3756, 3757, 3758, 3759, 3760, 3761, 3762, 3763, 3764, 3765, 3766, 3767, 3768, 3769, 3770, 3771, 3772, 3773, 3774, 3775, 3776, 3777, 3778, 3779, 3780, 3781, 3782, 3783, 3784, 3785, 3786, 3787, 3788, 3789, 3790, 3791, 3792, 3793, 3794, 3795, 3796, 3797, 3798, 3799, 3800, 3801, 3802, 3803, 3804, 3805, 3806, 3807, 3808, 3809, 3810, 3811, 3812, 3813, 3814, 3815, 3816, 3817, 3818, 3819, 3820, 3821, 3822, 3823, 3824, 3825, 3826, 3827, 3828, 3829, 3830, 3831, 3832, 3833, 3834, 3835, 3836, 3837, 3838, 3839, 3840, 3841, 3842, 3843, 3844, 3845, 3846, 3847, 3848, 3849, 3850, 3851, 3852, 3853, 3854, 3855, 3856, 3857, 3858, 3859, 3860, 3861, 3862, 3863, 3864, 3865, 3866, 3867, 3868, 3869, 3870, 3871, 3872, 3873, 3874, 3875, 3876, 3877, 3878, 3879, 3880, 3881, 3882, 3883, 3884, 3885, 3886, 3887, 3888, 3889, 3890, 3891, 3892, 3893, 3894, 3895, 3896, 3897, 3898, 3899, 3900, 3901, 3902, 3903, 3904, 3905, 3906, 3907, 3908, 3909, 3910, 3911, 3912, 3913, 3914, 3915, 3916, 3917, 3918, 3919, 3920, 3921, 3922, 3923, 3924, 3925, 3926, 3927, 3928, 3929, 3930, 3931, 3932, 3933, 3934, 3935, 3936, 3937, 3938, 3939, 3940, 3941, 3942, 3943, 3944, 3945, 3946, 3947, 3948, 3949, 3950, 3951, 3952, 3953, 3954, 3955, 3956, 3957, 3958, 3959, 3960, 3961, 3962, 3963, 3964, 3965, 3966, 3967, 3968, 3969, 3970, 3971, 3972, 3973, 3974, 3975, 3976, 3977, 3978, 3979, 3980, 3981, 3982, 3983, 3984, 3985, 3986, 3987, 3988, 3989, 3990, 3991, 3992, 3993, 3994, 3995, 3996, 3997, 3998, 3999, 4000, 4001, 4002, 4003, 4004, 4005, 4006, 4007, 4008, 4009, 4010, 4011, 4012, 4013, 4014, 4015, 4016, 4017, 4018, 4019, 4020, 4021, 4022, 4023, 4024, 4025, 4026, 4027, 4028, 4029, 4030, 4031, 4032, 4033, 4034, 4035, 4036, 4037, 4038, 4039, 4040, 4041, 4042, 4043, 4044, 4045, 4046, 4047, 4048, 4049, 4050, 4051, 4052, 4053, 4054, 4055, 4056, 4057, 4058, 4059, 4060, 4061, 4062, 4063, 4064, 4065, 4066, 4067, 4068, 4069, 4070, 4071, 4072, 4073, 4074, 4075, 4076, 4077, 4078, 4079, 4080, 4081, 4082, 4083, 4084, 4085, 4086, 4087, 4088, 4089, 4090, 4091, 4092, 4093, 4094, 4095, 4096, 4097, 4098, 4099, 4100, 4101, 4102, 4103, 4104, 4105, 4106, 4107, 4108, 4109, 4110, 4111, 4112, 4113, 4114, 4115, 4116, 4117, 4118, 4119, 4120, 4121, 4122, 4123, 4124, 4125, 4126, 4127, 4128, 4129, 4130, 4131, 4132, 4133, 4134, 4135, 4136, 4137, 4138, 4139, 4140, 4141, 4142, 4143, 4144, 4145, 4146, 4147, 4148, 4149, 4150, 4151, 4152, 4153, 4154, 4155, 4156, 4157, 4158, 4159, 4160, 4161, 4162, 4163, 4164, 4165, 4166, 4167, 4168, 4169, 4170, 4171, 4172, 4173, 4174, 4175, 4176, 4177, 4178, 4179, 4180, 4181, 4182, 4183, 4184, 4185, 4186, 4187, 4188, 4189, 4190, 4191, 4192, 4193, 4194, 4195, 4196, 4197, 4198, 4199, 4200, 4201, 4202, 4203, 4204, 4205, 4206, 4207, 4208, 4209, 4210, 4211, 4212, 4213, 4214, 4215, 4216, 4217, 4218, 4219, 4220, 4221, 4222, 4223, 4224, 4225, 4226, 4227, 4228, 4229, 4230, 4231, 4232, 4233, 4234, 4235, 4236, 4237, 4238, 4239, 4240, 4241, 4242, 4243, 4244, 4245, 4246, 4247, 4248, 4249, 4250, 4251, 4252, 4253, 4254, 4255, 4256, 4257, 4258, 4259, 4260, 4261, 4262, 4263, 4264, 4265, 4266, 4267, 4268, 4269, 4270, 4271, 4272, 4273, 4274, 4275, 4276, 4277, 4278, 4279, 4280, 4281, 4282, 4283, 4284, 4285, 4286, 4287, 4288, 4289, 4290, 4291, 4292, 4293, 4294, 4295, 4296, 4297, 4298, 4299, 4300, 4301, 4302, 4303, 4304, 4305, 4306, 4307, 4308, 4309, 4310, 4311, 4312, 4313, 4314, 4315, 4316, 4317, 4318, 4319, 4320, 4321, 4322, 4323, 4324, 4325, 4326, 4327, 4328, 4329, 4330, 4331, 4332, 4333, 4334, 4335, 4336, 4337, 4338, 4339, 4340, 4341, 4342, 4343, 4344, 4345, 4346, 4347, 4348, 4349, 4350, 4351, 4352, 4353, 4354, 4355, 4356, 4357, 4358, 4359, 4360, 4361, 4362, 4363, 4364, 4365, 4366, 4367, 4368, 4369, 4370, 4371, 4372, 4373, 4374, 4375, 4376, 4377, 4378, 4379, 4380, 4381, 4382, 4383, 4384, 4385, 4386, 4387, 4388, 4389, 4390, 4391, 4392, 4393, 4394, 4395, 4396, 4397, 4398, 4399, 4400, 4401, 4402, 4403, 4404, 4405, 4406, 4407, 4408, 4409, 4410, 4411, 4412, 4413, 4414, 4415, 4416, 4417, 4418, 4419, 4420, 4421, 4422, 4423, 4424, 4425, 4426, 4427, 4428, 4429, 4430, 4431, 4432, 4433, 4434, 4435, 4436, 4437, 4438, 4439, 4440, 4441, 4442, 4443, 4444, 4445, 4446, 4447, 4448, 4449, 4450, 4451, 4452, 4453, 4454, 4455, 4456, 4457, 4458, 4459, 4460, 4461, 4462, 4463, 4464, 4465, 4466, 4467, 4468, 4469, 4470, 4471, 4472, 4473, 4474, 4475, 4476, 4477, 4478, 4479, 4480, 4481, 4482, 4483, 4484, 4485, 4486, 4487, 4488, 4489, 4490, 4491, 4492, 4493, 4494, 4495, 4496, 4497, 4498, 4499, 4500, 4501, 4502, 4503, 4504, 4505, 4506, 4507, 4508, 4509, 4510, 4511, 4512, 4513, 4514, 4515, 4516, 4517, 4518, 4519, 4520, 4521, 4522, 4523, 4524, 4525, 4526, 4527, 4528, 4529, 4530, 4531, 4532, 4533, 4534, 4535, 4536, 4537, 4538, 4539, 4540, 4541, 4542, 4543, 4544, 4545, 4546, 4547, 4548, 4549, 4550, 4551, 4552, 4553, 4554, 4555, 4556, 4557, 4558, 4559, 4560, 4561, 4562, 4563, 4564, 4565, 4566, 4567, 4568, 4569, 4570, 4571, 4572, 4573, 4574, 4575, 4576, 4577, 4578, 4579, 4580, 4581, 4582, 4583, 4584, 4585, 4586, 4587, 4588, 4589, 4590, 4591, 4592, 4593, 4594, 4595, 4596, 4597, 4598, 4599, 4600, 4601, 4602, 4603, 4604, 4605, 4606, 4607, 4608, 4609, 4610, 4611, 4612, 4613, 4614, 4615, 4616, 4617, 4618, 4619, 4620, 4621, 4622, 4623, 4624, 4625, 4626, 4627, 4628, 4629, 4630, 4631, 4632, 4633, 4634, 4635, 4636, 4637, 4638, 4639, 4640, 4641, 4642, 4643, 4644, 4645, 4646, 4647, 4648, 4649, 4650, 4651, 4652, 4653, 4654, 4655, 4656, 4657, 4658, 4659, 4660, 4661, 4662, 4663, 4664, 4665, 4666, 4667, 4668, 4669, 4670, 4671, 4672, 4673, 4674, 4675, 4676, 4677, 4678, 4679, 4680, 4681, 4682, 4683, 4684, 4685, 4686, 4687, 4688, 4689, 4690, 4691, 4692, 4693, 4694, 4695, 4696, 4697, 4698, 4699, 4700, 4701, 4702, 4703, 4704, 4705, 4706, 4707, 4708, 4709, 4710, 4711, 4712, 4713, 4714, 4715, 4716, 4717, 4718, 4719, 4720, 4721, 4722, 4723, 4724, 4725, 4726, 4727, 4728, 4729, 4730, 4731, 4732, 4733, 4734, 4735, 4736, 4737, 4738, 4739, 4740, 4741, 4742, 4743, 4744, 4745, 4746, 4747, 4748, 4749, 4750, 4751, 4752, 4753, 4754, 4755, 4756, 4757, 4758, 4759, 4760, 4761, 4762, 4763, 4764, 4765, 4766, 4767, 4768, 4769, 4770, 4771, 4772, 4773, 4774, 4775, 4776, 4777, 4778, 4779, 4780, 4781, 4782, 4783, 4784, 4785, 4786, 4787, 4788, 4789, 4790, 4791, 4792, 4793, 4794, 4795, 4796, 4797, 4798, 4799, 4800, 4801, 4802, 4803, 4804, 4805, 4806, 4807, 4808, 4809, 4810, 4811, 4812, 4813, 4814, 4815, 4816, 4817, 4818, 4819, 4820, 4821, 4822, 4823, 4824, 4825, 4826, 4827, 4828, 4829, 4830, 4831, 4832, 4833, 4834, 4835, 4836, 4837, 4838, 4839, 4840, 4841, 4842, 4843, 4844, 4845, 4846, 4847, 4848, 4849, 4850, 4851, 4852, 4853, 4854, 4855, 4856, 4857, 4858, 4859, 4860, 4861, 4862, 4863, 4864, 4865, 4866, 4867, 4868, 4869, 4870, 4871, 4872, 4873, 4874, 4875, 4876, 4877, 4878, 4879, 4880, 4881, 4882, 4883, 4884, 4885, 4886, 4887, 4888, 4889, 4890, 4891, 4892, 4893, 4894, 4895, 4896, 4897, 4898, 4899, 4900, 4901, 4902, 4903, 4904, 4905, 4906, 4907, 4908, 4909, 4910, 4911, 4912, 4913, 4914, 4915, 4916, 4917, 4918, 4919, 4920, 4921, 4922, 4923, 4924, 4925, 4926, 4927, 4928, 4929, 4930, 4931, 4932, 4933, 4934, 4935, 4936, 4937, 4938, 4939, 4940, 4941, 4942, 4943, 4944, 4945, 4946, 4947, 4948, 4949, 4950, 4951, 4952, 4953, 4954, 4955, 4956, 4957, 4958, 4959, 4960, 4961, 4962, 4963, 4964, 4965, 4966, 4967, 4968, 4969, 4970, 4971, 4972, 4973, 4974, 4975, 4976, 4977, 4978, 4979, 4980, 4981, 4983, 4984, 4985, 4986, 4987, 4988, 4989, 4990, 4991, 4992, 4993, 4994, 4995, 4996, 4997, 4998, 4999, 5000, 5001, 5002, 5003, 5004, 5005, 5006, 5007, 5008, 5009, 5010, 5011, 5012, 5013, 5014, 5015, 5016, 5017, 5018, 5019, 5020, 5021, 5022, 5023, 5024, 5025, 5026, 5027, 5028, 5029, 5030, 5031, 5032, 5033, 5034, 5035, 5036, 5037, 5038, 5039, 5040, 5041, 5042, 5043, 5044, 5045, 5046, 5047, 5048, 5049, 5050, 5051, 5052, 5053, 5054, 5055, 5056, 5057, 5058, 5059, 5060, 5061, 5062, 5063, 5064, 5065, 5066, 5067, 5068, 5069, 5070, 5071, 5072, 5073, 5074, 5075, 5076, 5077, 5078, 5079, 5080, 5081, 5082, 5083, 5084, 5085, 5086, 5087, 5088, 5089, 5090, 5091, 5092, 5093, 5094, 5095, 5096, 5097, 5098, 5099, 5100, 5101, 5102, 5103, 5104, 5105, 5106, 5107, 5108, 5109, 5110, 5111, 5112, 5113, 5114, 5115, 5116, 5117, 5118, 5119, 5120, 5121, 5122, 5123, 5124, 5125, 5126, 5127, 5128, 5129, 5130, 5131, 5132, 5133, 5134, 5135, 5136, 5137, 5138, 5139, 5140, 5141, 5142, 5143, 5144, 5145, 5146, 5147, 5148, 5149, 5150, 5151, 5152, 5153, 5154, 5155, 5156, 5157, 5158, 5159, 5160, 5161, 5162, 5163, 5164, 5165, 5166, 5167, 5168, 5169, 5170, 5171, 5172, 5173, 5174, 5175, 5176, 5177, 5178, 5179, 5180, 5181, 5182, 5183, 5184, 5185, 5186, 5187, 5188, 5189, 5190, 5191, 5192, 5193, 5194, 5195, 5196, 5197, 5198, 5199, 5200, 5201, 5202, 5203, 5204, 5205, 5206, 5207, 5208, 5209, 5210, 5211, 5212, 5213, 5214, 5215, 5216, 5217, 5218, 5219, 5220, 5221, 5222, 5223, 5224, 5225, 5226, 5227, 5228, 5229, 5230, 5231, 5232, 5233, 5234, 5235, 5236, 5237, 5238, 5239, 5240, 5241, 5242, 5243, 5244, 5245, 5246, 5247, 5248, 5249, 5250, 5251, 5252, 5253, 5254, 5255, 5256, 5257, 5258, 5259, 5260, 5261, 5262, 5263, 5264, 5265, 5266, 5267, 5268, 5269, 5270, 5271, 5272, 5273, 5274, 5275, 5276, 5277, 5278, 5279, 5280, 5281, 5282, 5283, 5284, 5285, 5286, 5287, 5288, 5289, 5290, 5291, 5292, 5293, 5294, 5295, 5296, 5297, 5298, 5299, 5300, 5301, 5302, 5303, 5304, 5305, 5306, 5307, 5308, 5309, 5310, 5311, 5312, 5313, 5314, 5315, 5316, 5317, 5318, 5319, 5320, 5321, 5322, 5323, 5324, 5325, 5326, 5327, 5328, 5329, 5330, 5331, 5332, 5333, 5334, 5335, 5336, 5337, 5338, 5339, 5340, 5341, 5342, 5343, 5344, 5345, 5346, 5347, 5348, 5349, 5350, 5351, 5352, 5353, 5354, 5355, 5356, 5357, 5358, 5359, 5360, 5361, 5362, 5363, 5364, 5365, 5366, 5367, 5368, 5369, 5370, 5371, 5372, 5373, 5374, 5375, 5376, 5377, 5378, 5379, 5380, 5381, 5382, 5383, 5384, 5385, 5386, 5387, 5388, 5389, 5390, 5391, 5392, 5393, 5394, 5395, 5396, 5397, 5398, 5399, 5400, 5401, 5402, 5403, 5404, 5405, 5406, 5407, 5408, 5409, 5410, 5411, 5412, 5413, 5414, 5415, 5416, 5417, 5418, 5419, 5420, 5421, 5422, 5423, 5424, 5425, 5426, 5427, 5428, 5429, 5430, 5431, 5432, 5433, 5434, 5435, 5436, 5437, 5438, 5439, 5440, 5441, 5442, 5443, 5444, 5445, 5446, 5447, 5448, 5449, 5450, 5451, 5452, 5453, 5454, 5455, 5456, 5457, 5458, 5459, 5460, 5461, 5462, 5463, 5464, 5465, 5466, 5467, 5468, 5469, 5470, 5471, 5472, 5473, 5474, 5475, 5476, 5477, 5478, 5479, 5480, 5481, 5482, 5483, 5484, 5485, 5486, 5487, 5488, 5489, 5490, 5491, 5492, 5493, 5494, 5495, 5496, 5497, 5498, 5499, 5500, 5501, 5502, 5503, 5504, 5505, 5506, 5507, 5508, 5509, 5510, 5511, 5512, 5513, 5514, 5515, 5516, 5517, 5518, 5519, 5520, 5521, 5522, 5523, 5524, 5525, 5526, 5527, 5528, 5529, 5530, 5531, 5532, 5533, 5534, 5535, 5536, 5537, 5538, 5539, 5540, 5541, 5542, 5543, 5544, 5545, 5546, 5547, 5548, 5549, 5550, 5551, 5552, 5553, 5554, 5555, 5556, 5557, 5558, 5559, 5560, 5561, 5562, 5563, 5564, 5565, 5566, 5567, 5568, 5569, 5570, 5571, 5572, 5573, 5574, 5575, 5576, 5577, 5578, 5579, 5580, 5581, 5582, 5583, 5584, 5585, 5586, 5587, 5588, 5589, 5590, 5591, 5592, 5593, 5594, 5595, 5596, 5597, 5598, 5599, 5600, 5601, 5602, 5603, 5604, 5605, 5606, 5607, 5608, 5609, 5610, 5611, 5612, 5613, 5614, 5615, 5616, 5617, 5618, 5619, 5620, 5621, 5622, 5623, 5624, 5625, 5626, 5627, 5628, 5629, 5630, 5631, 5632, 5633, 5634, 5635, 5636, 5637, 5638, 5639, 5640, 5641, 5642, 5643, 5644, 5645, 5646, </t>
         </is>
       </c>
-      <c r="BV3" t="n">
+      <c r="CD3" t="n">
         <v>0.07673860911270983</v>
       </c>
-      <c r="BW3" t="inlineStr">
+      <c r="CE3" t="inlineStr">
         <is>
           <t>{'Numk': 16, 'KPar': 10, 'Bucket_index': 1000}</t>
         </is>
       </c>
-      <c r="BX3" t="n">
+      <c r="CF3" t="n">
         <v>413.5598660029937</v>
       </c>
-      <c r="BY3" t="inlineStr">
+      <c r="CG3" t="inlineStr">
         <is>
           <t>no</t>
         </is>
       </c>
-      <c r="BZ3" t="n">
-        <v>0</v>
-      </c>
-      <c r="CA3" t="inlineStr">
+      <c r="CH3" t="n">
+        <v>0</v>
+      </c>
+      <c r="CI3" t="inlineStr">
         <is>
           <t>params</t>
         </is>
       </c>
-      <c r="CB3" t="n">
+      <c r="CJ3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1526,93 +1614,117 @@
       <c r="BE4" t="n">
         <v>2</v>
       </c>
-      <c r="BF4" t="inlineStr"/>
-      <c r="BG4" t="inlineStr">
+      <c r="BF4" t="n">
+        <v>2</v>
+      </c>
+      <c r="BG4" t="n">
+        <v>2</v>
+      </c>
+      <c r="BH4" t="n">
+        <v>2</v>
+      </c>
+      <c r="BI4" t="n">
+        <v>2</v>
+      </c>
+      <c r="BJ4" t="n">
+        <v>2</v>
+      </c>
+      <c r="BK4" t="n">
+        <v>2</v>
+      </c>
+      <c r="BL4" t="n">
+        <v>2</v>
+      </c>
+      <c r="BM4" t="n">
+        <v>2</v>
+      </c>
+      <c r="BN4" t="inlineStr"/>
+      <c r="BO4" t="inlineStr">
         <is>
           <t>nab-data/realKnownCause/ec2_request_latency_system_failure.csv</t>
         </is>
       </c>
-      <c r="BH4" t="n">
+      <c r="BP4" t="n">
         <v>4032</v>
       </c>
-      <c r="BI4" t="inlineStr">
+      <c r="BQ4" t="inlineStr">
         <is>
           <t>NAB</t>
         </is>
       </c>
-      <c r="BJ4" t="n">
-        <v>3</v>
-      </c>
-      <c r="BK4" t="inlineStr">
+      <c r="BR4" t="n">
+        <v>3</v>
+      </c>
+      <c r="BS4" t="inlineStr">
         <is>
           <t>2014; 3328; 3956</t>
         </is>
       </c>
-      <c r="BL4" t="n">
+      <c r="BT4" t="n">
         <v>134</v>
       </c>
-      <c r="BM4" t="inlineStr">
-        <is>
-          <t>[2081, 3394, 3395, 4023, 4025, 4027, 4029, 4030, 4031]</t>
-        </is>
-      </c>
-      <c r="BN4" t="n">
-        <v>1</v>
-      </c>
-      <c r="BO4" t="inlineStr">
-        <is>
-          <t>{'initial_window': 303, 'window_size': 487, 'num_trees': 24, 'max_depth': 13}</t>
-        </is>
-      </c>
-      <c r="BP4" t="n">
-        <v>10.23753639101051</v>
-      </c>
-      <c r="BQ4" t="inlineStr">
+      <c r="BU4" t="inlineStr">
+        <is>
+          <t>[1337, 2081, 3394, 3395, 4023, 4025, 4027, 4029, 4030, 4031]</t>
+        </is>
+      </c>
+      <c r="BV4" t="n">
+        <v>0.9473684210526316</v>
+      </c>
+      <c r="BW4" t="inlineStr">
+        <is>
+          <t>{'initial_window': 659, 'window_size': 200, 'num_trees': 15, 'max_depth': 10}</t>
+        </is>
+      </c>
+      <c r="BX4" t="n">
+        <v>2.076758354000049</v>
+      </c>
+      <c r="BY4" t="inlineStr">
         <is>
           <t>[2102, 3413, 3415]</t>
         </is>
       </c>
-      <c r="BR4" t="n">
+      <c r="BZ4" t="n">
         <v>0.8</v>
       </c>
-      <c r="BS4" t="inlineStr">
+      <c r="CA4" t="inlineStr">
         <is>
           <t>{'AR_window_size': 20, 'differencing-order': 1}</t>
         </is>
       </c>
-      <c r="BT4" t="n">
+      <c r="CB4" t="n">
         <v>32.07578844204545</v>
       </c>
-      <c r="BU4" t="inlineStr">
+      <c r="CC4" t="inlineStr">
         <is>
           <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86, 87, 88, 89, 90, 91, 92, 93, 94, 95, 96, 97, 98, 99, 100, 101, 102, 103, 104, 105, 106, 107, 108, 109, 110, 111, 112, 113, 114, 115, 116, 117, 118, 119, 120, 121, 122, 123, 124, 125, 126, 127, 128, 129, 130, 131, 132, 133, 134, 135, 136, 137, 138, 139, 140, 141, 142, 143, 144, 145, 146, 147, 148, 149, 150, 151, 152, 153, 154, 155, 156, 157, 158, 159, 160, 161, 162, 163, 164, 165, 166, 167, 168, 169, 170, 171, 172, 173, 174, 175, 176, 177, 178, 179, 180, 181, 182, 183, 184, 185, 186, 187, 188, 189, 190, 191, 192, 193, 194, 195, 196, 197, 198, 199, 200, 201, 202, 203, 204, 205, 206, 207, 208, 209, 210, 211, 212, 213, 214, 215, 216, 217, 218, 219, 220, 221, 222, 223, 224, 225, 226, 227, 228, 229, 230, 231, 232, 233, 234, 235, 236, 237, 238, 239, 240, 241, 242, 243, 244, 245, 246, 247, 248, 249, 250, 251, 252, 253, 254, 255, 256, 257, 258, 259, 260, 261, 262, 263, 264, 265, 266, 267, 268, 269, 270, 271, 272, 273, 274, 275, 276, 277, 278, 279, 280, 281, 282, 283, 284, 285, 286, 287, 288, 289, 290, 291, 292, 293, 294, 295, 296, 297, 298, 299, 300, 301, 302, 303, 304, 305, 306, 307, 308, 309, 310, 311, 312, 313, 314, 315, 316, 317, 318, 319, 320, 321, 322, 323, 324, 325, 326, 327, 328, 329, 330, 331, 332, 333, 334, 335, 336, 337, 338, 339, 340, 341, 342, 343, 344, 345, 346, 347, 348, 349, 350, 351, 352, 353, 354, 355, 356, 357, 358, 359, 360, 361, 362, 363, 364, 365, 366, 367, 368, 369, 370, 371, 372, 373, 374, 375, 376, 377, 378, 379, 380, 381, 382, 383, 384, 385, 386, 387, 388, 389, 390, 391, 392, 393, 394, 395, 396, 397, 398, 399, 400, 401, 402, 403, 404, 405, 406, 407, 408, 409, 410, 411, 412, 413, 414, 415, 416, 417, 418, 419, 420, 421, 422, 423, 424, 425, 426, 427, 428, 429, 430, 431, 432, 433, 434, 435, 436, 437, 438, 439, 440, 441, 442, 443, 444, 445, 446, 447, 448, 449, 450, 451, 452, 453, 454, 455, 456, 457, 458, 459, 460, 461, 462, 463, 464, 465, 466, 467, 468, 469, 470, 471, 472, 473, 474, 475, 476, 477, 478, 479, 480, 481, 482, 483, 484, 485, 486, 487, 488, 489, 490, 491, 492, 493, 494, 495, 496, 497, 498, 499, 500, 501, 502, 503, 504, 505, 506, 507, 508, 509, 510, 511, 512, 513, 514, 515, 516, 517, 518, 519, 520, 521, 522, 523, 524, 525, 526, 527, 528, 529, 530, 531, 532, 533, 534, 535, 536, 537, 538, 539, 540, 541, 542, 543, 544, 545, 546, 547, 548, 549, 550, 551, 552, 553, 554, 555, 556, 557, 558, 559, 560, 561, 562, 563, 564, 565, 566, 567, 568, 569, 570, 571, 572, 573, 574, 575, 576, 577, 578, 579, 580, 581, 582, 583, 584, 585, 586, 587, 588, 589, 590, 591, 592, 593, 594, 595, 596, 597, 598, 599, 600, 601, 602, 603, 604, 605, 606, 607, 608, 609, 610, 611, 612, 613, 614, 615, 616, 617, 618, 619, 620, 621, 622, 623, 624, 625, 626, 627, 628, 629, 630, 631, 632, 633, 634, 635, 636, 637, 638, 639, 640, 641, 642, 643, 644, 645, 646, 647, 648, 649, 650, 651, 652, 653, 654, 655, 656, 657, 658, 659, 660, 661, 662, 663, 664, 665, 666, 667, 668, 669, 670, 671, 672, 673, 674, 675, 676, 677, 678, 679, 680, 681, 682, 683, 684, 685, 686, 687, 688, 689, 690, 691, 692, 693, 694, 695, 696, 697, 698, 699, 700, 701, 702, 703, 704, 705, 706, 707, 708, 709, 710, 711, 712, 713, 714, 715, 716, 717, 718, 719, 720, 721, 722, 723, 724, 725, 726, 727, 728, 729, 730, 731, 732, 733, 734, 735, 736, 737, 738, 739, 740, 741, 742, 743, 744, 745, 746, 747, 748, 749, 750, 751, 752, 753, 754, 755, 756, 757, 758, 759, 760, 761, 762, 763, 764, 765, 766, 767, 768, 769, 770, 771, 772, 773, 774, 775, 776, 777, 778, 779, 780, 781, 782, 783, 784, 785, 786, 787, 788, 789, 790, 791, 792, 793, 794, 795, 796, 797, 798, 799, 800, 801, 802, 803, 804, 805, 806, 807, 808, 809, 810, 811, 812, 813, 814, 815, 816, 817, 818, 819, 820, 821, 822, 823, 824, 825, 826, 827, 828, 829, 830, 831, 832, 833, 834, 835, 836, 837, 838, 839, 840, 841, 842, 843, 844, 845, 846, 847, 848, 849, 850, 851, 852, 853, 854, 855, 856, 857, 858, 859, 860, 861, 862, 863, 864, 865, 866, 867, 868, 869, 870, 871, 872, 873, 874, 875, 876, 877, 878, 879, 880, 881, 882, 883, 884, 885, 886, 887, 888, 889, 890, 891, 892, 893, 894, 895, 896, 897, 898, 899, 900, 901, 902, 903, 904, 905, 906, 907, 908, 909, 910, 911, 912, 913, 914, 915, 916, 917, 918, 919, 920, 921, 922, 923, 924, 925, 926, 927, 928, 929, 930, 931, 932, 933, 934, 935, 936, 937, 938, 939, 940, 941, 942, 943, 944, 945, 946, 947, 948, 949, 950, 951, 952, 953, 954, 955, 956, 957, 958, 959, 960, 961, 962, 963, 964, 965, 966, 967, 968, 969, 970, 971, 972, 973, 974, 975, 976, 977, 978, 979, 980, 981, 982, 983, 984, 985, 986, 987, 988, 989, 990, 991, 992, 993, 994, 995, 996, 997, 998, 999, 1000, 1001, 1002, 1003, 1004, 1005, 1006, 1007, 1008, 1009, 1010, 1011, 1012, 1013, 1014, 1015, 1016, 1017, 1018, 1019, 1020, 1021, 1022, 1023, 1024, 1025, 1026, 1027, 1028, 1029, 1030, 1031, 1032, 1033, 1034, 1035, 1036, 1037, 1038, 1039, 1040, 1041, 1042, 1043, 1044, 1045, 1046, 1047, 1048, 1049, 1050, 1051, 1052, 1053, 1054, 1055, 1056, 1057, 1058, 1059, 1060, 1061, 1062, 1063, 1064, 1065, 1066, 1067, 1068, 1069, 1070, 1071, 1072, 1073, 1074, 1075, 1076, 1077, 1078, 1079, 1080, 1081, 1082, 1083, 1084, 1085, 1086, 1087, 1088, 1089, 1090, 1091, 1092, 1093, 1094, 1095, 1096, 1097, 1098, 1099, 1100, 1101, 1102, 1103, 1104, 1105, 1106, 1107, 1108, 1109, 1110, 1111, 1112, 1113, 1114, 1115, 1116, 1117, 1118, 1119, 1120, 1121, 1122, 1123, 1124, 1125, 1126, 1127, 1128, 1129, 1130, 1131, 1132, 1133, 1134, 1135, 1136, 1137, 1138, 1139, 1140, 1141, 1142, 1143, 1144, 1145, 1146, 1147, 1148, 1149, 1150, 1151, 1152, 1153, 1154, 1155, 1156, 1157, 1158, 1159, 1160, 1161, 1162, 1163, 1164, 1165, 1166, 1167, 1168, 1169, 1170, 1171, 1172, 1173, 1174, 1175, 1176, 1177, 1178, 1179, 1180, 1181, 1182, 1183, 1184, 1185, 1186, 1187, 1188, 1189, 1190, 1191, 1192, 1193, 1194, 1195, 1196, 1197, 1198, 1199, 1200, 1201, 1202, 1203, 1204, 1205, 1206, 1207, 1208, 1209, 1210, 1211, 1212, 1213, 1214, 1215, 1216, 1217, 1218, 1219, 1220, 1221, 1222, 1223, 1224, 1225, 1226, 1227, 1228, 1229, 1230, 1231, 1232, 1233, 1234, 1235, 1236, 1237, 1238, 1239, 1240, 1241, 1242, 1243, 1244, 1245, 1246, 1247, 1248, 1249, 1250, 1251, 1252, 1253, 1254, 1255, 1256, 1257, 1258, 1259, 1260, 1261, 1262, 1263, 1264, 1265, 1266, 1267, 1268, 1269, 1270, 1271, 1272, 1273, 1274, 1275, 1276, 1277, 1278, 1279, 1280, 1281, 1282, 1283, 1284, 1285, 1286, 1287, 1288, 1289, 1290, 1291, 1292, 1293, 1294, 1295, 1296, 1297, 1298, 1299, 1300, 1301, 1302, 1303, 1304, 1305, 1306, 1307, 1308, 1309, 1310, 1311, 1312, 1313, 1314, 1315, 1316, 1317, 1318, 1319, 1320, 1321, 1322, 1323, 1324, 1325, 1326, 1327, 1328, 1329, 1330, 1331, 1332, 1333, 1334, 1335, 1336, 1337, 1338, 1339, 1340, 1341, 1342, 1343, 1344, 1345, 1346, 1347, 1348, 1349, 1350, 1351, 1352, 1353, 1354, 1355, 1356, 1357, 1358, 1359, 1360, 1361, 1362, 1363, 1364, 1365, 1366, 1367, 1368, 1369, 1370, 1371, 1372, 1373, 1374, 1375, 1376, 1377, 1378, 1379, 1380, 1381, 1382, 1383, 1384, 1385, 1386, 1387, 1388, 1389, 1390, 1391, 1392, 1393, 1394, 1395, 1396, 1397, 1398, 1399, 1400, 1401, 1402, 1403, 1404, 1405, 1406, 1407, 1408, 1409, 1410, 1411, 1412, 1413, 1414, 1415, 1416, 1417, 1418, 1419, 1420, 1421, 1422, 1423, 1424, 1425, 1426, 1427, 1428, 1429, 1430, 1431, 1432, 1433, 1434, 1435, 1436, 1437, 1438, 1439, 1440, 1441, 1442, 1443, 1444, 1445, 1446, 1447, 1448, 1449, 1450, 1451, 1452, 1453, 1454, 1455, 1456, 1457, 1458, 1459, 1460, 1461, 1462, 1463, 1464, 1465, 1466, 1467, 1468, 1469, 1470, 1471, 1472, 1473, 1474, 1475, 1476, 1477, 1478, 1479, 1480, 1481, 1482, 1483, 1484, 1485, 1486, 1487, 1488, 1489, 1490, 1491, 1492, 1493, 1494, 1495, 1496, 1497, 1498, 1499, 1500, 1501, 1502, 1503, 1504, 1505, 1506, 1507, 1508, 1509, 1510, 1511, 1512, 1513, 1514, 1515, 1516, 1517, 1518, 1519, 1520, 1521, 1522, 1523, 1524, 1525, 1526, 1527, 1528, 1529, 1530, 1531, 1532, 1533, 1534, 1535, 1536, 1537, 1538, 1539, 1540, 1541, 1542, 1543, 1544, 1545, 1546, 1547, 1548, 1549, 1550, 1551, 1552, 1553, 1554, 1555, 1556, 1557, 1558, 1559, 1560, 1561, 1562, 1563, 1564, 1565, 1566, 1567, 1568, 1569, 1570, 1571, 1572, 1573, 1574, 1575, 1576, 1577, 1578, 1579, 1580, 1581, 1582, 1583, 1584, 1585, 1586, 1587, 1588, 1589, 1590, 1591, 1592, 1593, 1594, 1595, 1596, 1597, 1598, 1599, 1600, 1601, 1602, 1603, 1604, 1605, 1606, 1607, 1608, 1609, 1610, 1611, 1612, 1613, 1614, 1615, 1616, 1617, 1618, 1619, 1620, 1621, 1622, 1623, 1624, 1625, 1626, 1627, 1628, 1629, 1630, 1631, 1632, 1633, 1634, 1635, 1636, 1637, 1638, 1639, 1640, 1641, 1642, 1643, 1644, 1645, 1646, 1647, 1648, 1649, 1650, 1651, 1652, 1653, 1654, 1655, 1656, 1657, 1658, 1659, 1660, 1661, 1662, 1663, 1664, 1665, 1666, 1667, 1668, 1669, 1670, 1671, 1672, 1673, 1674, 1675, 1676, 1677, 1678, 1679, 1680, 1681, 1682, 1683, 1684, 1685, 1686, 1687, 1688, 1689, 1690, 1691, 1692, 1693, 1694, 1695, 1696, 1697, 1698, 1699, 1700, 1701, 1702, 1703, 1704, 1705, 1706, 1707, 1708, 1709, 1710, 1711, 1712, 1713, 1714, 1715, 1716, 1717, 1718, 1719, 1720, 1721, 1722, 1723, 1724, 1725, 1726, 1727, 1728, 1729, 1730, 1731, 1732, 1733, 1734, 1735, 1736, 1737, 1738, 1739, 1740, 1741, 1742, 1743, 1744, 1745, 1746, 1747, 1748, 1749, 1750, 1751, 1752, 1753, 1754, 1755, 1756, 1757, 1758, 1759, 1760, 1761, 1762, 1763, 1764, 1765, 1766, 1767, 1768, 1769, 1770, 1771, 1772, 1773, 1774, 1775, 1776, 1777, 1778, 1779, 1780, 1781, 1782, 1783, 1784, 1785, 1786, 1787, 1788, 1789, 1790, 1791, 1792, 1793, 1794, 1795, 1796, 1797, 1798, 1799, 1800, 1801, 1802, 1803, 1804, 1805, 1806, 1807, 1808, 1809, 1810, 1811, 1812, 1813, 1814, 1815, 1816, 1817, 1818, 1819, 1820, 1821, 1822, 1823, 1824, 1825, 1826, 1827, 1828, 1829, 1830, 1831, 1832, 1833, 1834, 1835, 1836, 1837, 1838, 1839, 1840, 1841, 1842, 1843, 1844, 1845, 1846, 1847, 1848, 1849, 1850, 1851, 1852, 1853, 1854, 1855, 1856, 1857, 1858, 1859, 1860, 1861, 1862, 1863, 1864, 1865, 1866, 1867, 1868, 1869, 1870, 1871, 1872, 1873, 1874, 1875, 1876, 1877, 1878, 1879, 1880, 1881, 1882, 1883, 1884, 1885, 1886, 1887, 1888, 1889, 1890, 1891, 1892, 1893, 1894, 1895, 1896, 1897, 1898, 1899, 1900, 1901, 1902, 1903, 1904, 1905, 1906, 1907, 1908, 1909, 1910, 1911, 1912, 1913, 1914, 1915, 1916, 1917, 1918, 1919, 1920, 1921, 1922, 1923, 1924, 1925, 1926, 1927, 1928, 1929, 1930, 1931, 1932, 1933, 1934, 1935, 1936, 1937, 1938, 1939, 1940, 1941, 1942, 1943, 1944, 1945, 1946, 1947, 1948, 1949, 1950, 1951, 1952, 1953, 1954, 1955, 1956, 1957, 1958, 1959, 1960, 1961, 1962, 1963, 1964, 1965, 1966, 1967, 1968, 1969, 1970, 1971, 1972, 1973, 1974, 1975, 1976, 1977, 1978, 1979, 1980, 1981, 1982, 1983, 1984, 1985, 1986, 1987, 1988, 1989, 1990, 1991, 1992, 1993, 1994, 1995, 1996, 1997, 1998, 1999, 2000, 2001, 2002, 2003, 2004, 2005, 2006, 2007, 2008, 2009, 2010, 2011, 2012, 2013, 2014, 2015, 2016, 2017, 2018, 2019, 2020, 2021, 2022, 2023, 2024, 2025, 2026, 2027, 2028, 2029, 2030, 2031, 2032, 2033, 2034, 2035, 2036, 2037, 2038, 2039, 2040, 2041, 2042, 2043, 2044, 2045, 2046, 2047, 2048, 2049, 2050, 2051, 2052, 2053, 2054, 2055, 2056, 2057, 2058, 2059, 2060, 2061, 2062, 2063, 2064, 2065, 2066, 2067, 2068, 2069, 2070, 2071, 2072, 2073, 2074, 2075, 2076, 2077, 2078, 2079, 2080, 2081, 2082, 2083, 2084, 2085, 2086, 2087, 2088, 2089, 2090, 2091, 2092, 2093, 2094, 2095, 2096, 2097, 2098, 2099, 2100, 2101, 2102, 2103, 2104, 2105, 2106, 2107, 2108, 2109, 2110, 2111, 2112, 2113, 2114, 2115, 2116, 2117, 2118, 2119, 2120, 2121, 2122, 2123, 2124, 2125, 2126, 2127, 2128, 2129, 2130, 2131, 2132, 2133, 2134, 2135, 2136, 2137, 2138, 2139, 2140, 2141, 2142, 2143, 2144, 2145, 2146, 2147, 2148, 2149, 2150, 2151, 2152, 2153, 2154, 2155, 2156, 2157, 2158, 2159, 2160, 2161, 2162, 2163, 2164, 2165, 2166, 2167, 2168, 2169, 2170, 2171, 2172, 2173, 2174, 2175, 2176, 2177, 2178, 2179, 2180, 2181, 2182, 2183, 2184, 2185, 2186, 2187, 2188, 2189, 2190, 2191, 2192, 2193, 2194, 2195, 2196, 2197, 2198, 2199, 2200, 2201, 2202, 2203, 2204, 2205, 2206, 2207, 2208, 2209, 2210, 2211, 2212, 2213, 2214, 2215, 2216, 2217, 2218, 2219, 2220, 2221, 2222, 2223, 2224, 2225, 2226, 2227, 2228, 2229, 2230, 2231, 2232, 2233, 2234, 2235, 2236, 2237, 2238, 2239, 2240, 2241, 2242, 2243, 2244, 2245, 2246, 2247, 2248, 2249, 2250, 2251, 2252, 2253, 2254, 2255, 2256, 2257, 2258, 2259, 2260, 2261, 2262, 2263, 2264, 2265, 2266, 2267, 2268, 2269, 2270, 2271, 2272, 2273, 2274, 2275, 2276, 2277, 2278, 2279, 2280, 2281, 2282, 2283, 2284, 2285, 2286, 2287, 2288, 2289, 2290, 2291, 2292, 2293, 2294, 2295, 2296, 2297, 2298, 2299, 2300, 2301, 2302, 2303, 2304, 2305, 2306, 2307, 2308, 2309, 2310, 2311, 2312, 2313, 2314, 2315, 2316, 2317, 2318, 2319, 2320, 2321, 2322, 2323, 2324, 2325, 2326, 2327, 2328, 2329, 2330, 2331, 2332, 2333, 2334, 2335, 2336, 2337, 2338, 2339, 2340, 2341, 2342, 2343, 2344, 2345, 2346, 2347, 2348, 2349, 2350, 2351, 2352, 2353, 2354, 2355, 2356, 2357, 2358, 2359, 2360, 2361, 2362, 2363, 2364, 2365, 2366, 2367, 2368, 2369, 2370, 2371, 2372, 2373, 2374, 2375, 2376, 2377, 2378, 2379, 2380, 2381, 2382, 2383, 2384, 2385, 2386, 2387, 2388, 2389, 2390, 2391, 2392, 2393, 2394, 2395, 2396, 2397, 2398, 2399, 2400, 2401, 2402, 2403, 2404, 2405, 2406, 2407, 2408, 2409, 2410, 2411, 2412, 2413, 2414, 2415, 2416, 2417, 2418, 2419, 2420, 2421, 2422, 2423, 2424, 2425, 2426, 2427, 2428, 2429, 2430, 2431, 2432, 2433, 2434, 2435, 2436, 2437, 2438, 2439, 2440, 2441, 2442, 2443, 2444, 2445, 2446, 2447, 2448, 2449, 2450, 2451, 2452, 2453, 2454, 2455, 2456, 2457, 2458, 2459, 2460, 2461, 2462, 2463, 2464, 2465, 2466, 2467, 2468, 2469, 2470, 2471, 2472, 2473, 2474, 2475, 2476, 2477, 2478, 2479, 2480, 2481, 2482, 2483, 2484, 2485, 2486, 2487, 2488, 2489, 2490, 2491, 2492, 2493, 2494, 2495, 2496, 2497, 2498, 2499, 2500, 2501, 2502, 2503, 2504, 2505, 2506, 2507, 2508, 2509, 2510, 2511, 2512, 2513, 2514, 2515, 2516, 2517, 2518, 2519, 2520, 2521, 2522, 2523, 2524, 2525, 2526, 2527, 2528, 2529, 2530, 2531, 2532, 2533, 2534, 2535, 2536, 2537, 2538, 2539, 2540, 2541, 2542, 2543, 2544, 2545, 2546, 2547, 2548, 2549, 2550, 2551, 2552, 2553, 2554, 2555, 2556, 2557, 2558, 2559, 2560, 2561, 2562, 2563, 2564, 2565, 2566, 2567, 2568, 2569, 2570, 2571, 2572, 2573, 2574, 2575, 2576, 2577, 2578, 2579, 2580, 2581, 2582, 2583, 2584, 2585, 2586, 2587, 2588, 2589, 2590, 2591, 2592, 2593, 2594, 2595, 2596, 2597, 2598, 2599, 2600, 2601, 2602, 2603, 2604, 2605, 2606, 2607, 2608, 2609, 2610, 2611, 2612, 2613, 2614, 2615, 2616, 2617, 2618, 2619, 2620, 2621, 2622, 2623, 2624, 2625, 2626, 2627, 2628, 2629, 2630, 2631, 2632, 2633, 2634, 2635, 2636, 2637, 2638, 2639, 2640, 2641, 2642, 2643, 2644, 2645, 2646, 2647, 2648, 2649, 2650, 2651, 2652, 2653, 2654, 2655, 2656, 2657, 2658, 2659, 2660, 2661, 2662, 2663, 2664, 2665, 2666, 2667, 2668, 2669, 2670, 2671, 2672, 2673, 2674, 2675, 2676, 2677, 2678, 2679, 2680, 2681, 2682, 2683, 2684, 2685, 2686, 2687, 2688, 2689, 2690, 2691, 2692, 2693, 2694, 2695, 2696, 2697, 2698, 2699, 2700, 2701, 2702, 2703, 2704, 2705, 2706, 2707, 2708, 2709, 2710, 2711, 2712, 2713, 2714, 2715, 2716, 2717, 2718, 2719, 2720, 2721, 2722, 2723, 2724, 2725, 2726, 2727, 2728, 2729, 2730, 2731, 2732, 2733, 2734, 2735, 2736, 2737, 2738, 2739, 2740, 2741, 2742, 2743, 2744, 2745, 2746, 2747, 2748, 2749, 2750, 2751, 2752, 2753, 2754, 2755, 2756, 2757, 2758, 2759, 2760, 2761, 2762, 2763, 2764, 2765, 2766, 2767, 2768, 2769, 2770, 2771, 2772, 2773, 2774, 2775, 2776, 2777, 2778, 2779, 2780, 2781, 2782, 2783, 2784, 2785, 2786, 2787, 2788, 2789, 2790, 2791, 2792, 2793, 2794, 2795, 2796, 2797, 2798, 2799, 2800, 2801, 2802, 2803, 2804, 2805, 2806, 2807, 2808, 2809, 2810, 2811, 2812, 2813, 2814, 2815, 2816, 2817, 2818, 2819, 2820, 2821, 2822, 2823, 2824, 2825, 2826, 2827, 2828, 2829, 2830, 2831, 2832, 2833, 2834, 2835, 2836, 2837, 2838, 2839, 2840, 2841, 2842, 2843, 2844, 2845, 2846, 2847, 2848, 2849, 2850, 2851, 2852, 2853, 2854, 2855, 2856, 2857, 2858, 2859, 2860, 2861, 2862, 2863, 2864, 2865, 2866, 2867, 2868, 2869, 2870, 2871, 2872, 2873, 2874, 2875, 2876, 2877, 2878, 2879, 2880, 2881, 2882, 2883, 2884, 2885, 2886, 2887, 2888, 2889, 2890, 2891, 2892, 2893, 2894, 2895, 2896, 2897, 2898, 2899, 2900, 2901, 2902, 2903, 2904, 2905, 2906, 2907, 2908, 2909, 2910, 2911, 2912, 2913, 2914, 2915, 2916, 2917, 2918, 2919, 2920, 2921, 2922, 2923, 2924, 2925, 2926, 2927, 2928, 2929, 2930, 2931, 2932, 2933, 2934, 2935, 2936, 2937, 2938, 2939, 2940, 2941, 2942, 2943, 2944, 2945, 2946, 2947, 2948, 2949, 2950, 2951, 2952, 2953, 2954, 2955, 2956, 2957, 2958, 2959, 2960, 2961, 2962, 2963, 2964, 2965, 2966, 2967, 2968, 2969, 2970, 2971, 2972, 2973, 2974, 2975, 2976, 2977, 2978, 2979, 2980, 2981, 2982, 2983, 2984, 2985, 2986, 2987, 2988, 2989, 2990, 2991, 2992, 2993, 2994, 2995, 2996, 2997, 2998, 2999, 3000, 3001, 3002, 3003, 3004, 3005, 3006, 3007, 3008, 3009, 3010, 3011, 3012, 3013, 3014, 3015, 3016, 3017, 3018, 3019, 3020, 3021, 3022, 3023, 3024, 3025, 3026, 3027, 3028, 3029, 3030, 3031, 3032, 3033, 3034, 3035, 3036, 3037, 3038, 3039, 3040, 3041, 3042, 3043, 3044, 3045, 3046, 3047, 3048, 3049, 3050, 3051, 3052, 3053, 3054, 3055, 3056, 3057, 3058, 3059, 3060, 3061, 3062, 3063, 3064, 3065, 3066, 3067, 3068, 3069, 3070, 3071, 3072, 3073, 3074, 3075, 3076, 3077, 3078, 3079, 3080, 3081, 3082, 3083, 3084, 3085, 3086, 3087, 3088, 3089, 3090, 3091, 3092, 3093, 3094, 3095, 3096, 3097, 3098, 3099, 3100, 3101, 3102, 3103, 3104, 3105, 3106, 3107, 3108, 3109, 3110, 3111, 3112, 3113, 3114, 3115, 3116, 3117, 3118, 3119, 3120, 3121, 3122, 3123, 3124, 3125, 3126, 3127, 3128, 3129, 3130, 3131, 3132, 3133, 3134, 3135, 3136, 3137, 3138, 3139, 3140, 3141, 3142, 3143, 3144, 3145, 3146, 3147, 3148, 3149, 3150, 3151, 3152, 3153, 3154, 3155, 3156, 3157, 3158, 3159, 3160, 3161, 3162, 3163, 3164, 3165, 3166, 3167, 3168, 3169, 3170, 3171, 3172, 3173, 3174, 3175, 3176, 3177, 3178, 3179, 3180, 3181, 3182, 3183, 3184, 3185, 3186, 3187, 3188, 3189, 3190, 3191, 3192, 3193, 3194, 3195, 3196, 3197, 3198, 3199, 3200, 3201, 3202, 3203, 3204, 3205, 3206, 3207, 3208, 3209, 3210, 3211, 3212, 3213, 3214, 3215, 3216, 3217, 3218, 3219, 3220, 3221, 3222, 3223, 3224, 3225, 3226, 3227, 3228, 3229, 3230, 3231, 3232, 3233, 3234, 3235, 3236, 3237, 3238, 3239, 3240, 3241, 3242, 3243, 3244, 3245, 3246, 3247, 3248, 3249, 3250, 3251, 3252, 3253, 3254, 3255, 3256, 3257, 3258, 3259, 3260, 3261, 3262, 3263, 3264, 3265, 3266, 3267, 3268, 3269, 3270, 3271, 3272, 3273, 3274, 3275, 3276, 3277, 3278, 3279, 3280, 3281, 3282, 3283, 3284, 3285, 3286, 3287, 3288, 3289, 3290, 3291, 3292, 3293, 3294, 3295, 3296, 3297, 3298, 3299, 3300, 3301, 3302, 3303, 3304, 3305, 3306, 3307, 3308, 3309, 3310, 3311, 3312, 3313, 3314, 3315, 3316, 3317, 3318, 3319, 3320, 3321, 3322, 3323, 3324, 3325, 3326, 3327, 3328, 3329, 3330, 3331, 3332, 3333, 3334, 3335, 3336, 3337, 3338, 3339, 3340, 3341, 3342, 3343, 3344, 3345, 3346, 3347, 3348, 3349, 3350, 3351, 3352, 3353, 3354, 3355, 3356, 3357, 3358, 3359, 3360, 3361, 3362, 3363, 3364, 3365, 3366, 3367, 3368, 3369, 3370, 3371, 3372, 3373, 3374, 3375, 3376, 3377, 3378, 3379, 3380, 3381, 3382, 3383, 3384, 3385, 3386, 3387, 3388, 3389, 3390, 3391, 3392, 3393, 3394, 3395, 3396, 3397, 3398, 3399, 3400, 3401, 3402, 3403, 3404, 3405, 3406, 3407, 3408, 3409, 3410, 3411, 3412, 3413, 3414, 3415, 3416, 3417, 3418, 3419, 3420, 3421, 3422, 3423, 3424, 3425, 3426, 3427, 3428, 3429, 3430, 3431, 3432, 3433, 3434, 3435, 3436, 3437, 3438, 3439, 3440, 3441, 3442, 3443, 3444, 3445, 3446, 3447, 3448, 3449, 3450, 3451, 3452, 3453, 3454, 3455, 3456, 3457, 3458, 3459, 3460, 3461, 3462, 3463, 3464, 3465, 3466, 3467, 3468, 3469, 3470, 3471, 3472, 3473, 3474, 3475, 3476, 3477, 3478, 3479, 3480, 3481, 3482, 3483, 3484, 3485, 3486, 3487, 3488, 3489, 3490, 3491, 3492, 3493, 3494, 3495, 3496, 3497, 3498, 3499, 3500, 3501, 3502, 3503, 3504, 3505, 3506, 3507, 3508, 3509, 3510, 3511, 3512, 3513, 3514, 3515, 3516, 3517, 3518, 3519, 3520, 3521, 3522, 3523, 3524, 3525, 3526, 3527, 3528, 3529, 3530, 3531, 3532, 3533, 3534, 3535, 3536, 3537, 3538, 3539, 3540, 3541, 3542, 3543, 3544, 3545, 3546, 3547, 3548, 3549, 3550, 3551, 3552, 3553, 3554, 3555, 3556, 3557, 3558, 3559, 3560, 3561, 3562, 3563, 3564, 3565, 3566, 3567, 3568, 3569, 3570, 3571, 3572, 3573, 3574, 3575, 3576, 3577, 3578, 3579, 3580, 3581, 3582, 3583, 3584, 3585, 3586, 3587, 3588, 3589, 3590, 3591, 3592, 3593, 3594, 3595, 3596, 3597, 3598, 3599, 3600, 3601, 3602, 3603, 3604, 3605, 3606, 3607, 3608, 3609, 3610, 3611, 3612, 3613, 3614, 3615, 3616, 3617, 3618, 3619, 3620, 3621, 3622, 3623, 3624, 3625, 3626, 3627, 3628, 3629, 3630, 3631, 3632, 3633, 3634, 3635, 3636, 3637, 3638, 3639, 3640, 3641, 3642, 3643, 3644, 3645, 3646, 3647, 3648, 3649, 3650, 3651, 3652, 3653, 3654, 3655, 3656, 3657, 3658, 3659, 3660, 3661, 3662, 3663, 3664, 3665, 3666, 3667, 3668, 3669, 3670, 3671, 3672, 3673, 3674, 3675, 3676, 3677, 3678, 3679, 3680, 3681, 3682, 3683, 3684, 3685, 3686, 3687, 3688, 3689, 3690, 3691, 3692, 3693, 3694, 3695, 3696, 3697, 3698, 3699, 3700, 3701, 3702, 3703, 3704, 3705, 3706, 3707, 3708, 3709, 3710, 3711, 3712, 3713, 3714, 3715, 3716, 3717, 3718, 3719, 3720, 3721, 3722, 3723, 3724, 3725, 3726, 3727, 3728, 3729, 3730, 3731, 3732, 3733, 3734, 3735, 3736, 3737, 3738, 3739, 3740, 3741, 3742, 3743, 3744, 3745, 3746, 3747, 3748, 3749, 3750, 3751, 3752, 3753, 3754, 3755, 3756, 3757, 3758, 3759, 3760, 3761, 3762, 3763, 3764, 3765, 3766, 3767, 3768, 3769, 3770, 3771, 3772, 3773, 3774, 3775, 3776, 3777, 3778, 3779, 3780, 3781, 3782, 3783, 3784, 3785, 3786, 3787, 3788, 3789, 3790, 3791, 3792, 3793, 3794, 3795, 3796, 3797, 3798, 3799, 3800, 3801, 3802, 3803, 3804, 3805, 3806, 3807, 3808, 3809, 3810, 3811, 3812, 3813, 3814, 3815, 3816, 3817, 3818, 3819, 3820, 3821, 3822, 3823, 3824, 3825, 3826, 3827, 3828, 3829, 3830, 3831, 3832, 3833, 3834, 3835, 3836, 3837, 3838, 3839, 3840, 3841, 3842, 3843, 3844, 3845, 3846, 3847, 3848, 3849, 3850, 3851, 3852, 3853, 3854, 3855, 3856, 3857, 3858, 3859, 3860, 3861, 3862, 3863, 3864, 3865, 3866, 3867, 3868, 3869, 3870, 3871, 3872, 3873, 3874, 3875, 3876, 3877, 3878, 3879, 3880, 3881, 3882, 3883, 3884, 3885, 3886, 3887, 3888, 3889, 3890, 3891, 3892, 3893, 3894, 3895, 3896, 3897, 3898, 3899, 3900, 3901, 3902, 3903, 3904, 3905, 3906, 3907, 3908, 3909, 3910, 3911, 3912, 3913, 3914, 3915, 3916, 3917, 3918, 3919, 3920, 3921, 3922, 3923, 3924, 3925, 3926, 3927, 3928, 3929, 3930, 3931, 3932, 3933, 3934, 3935, 3936, 3937, 3938, 3939, 3940, 3941, 3942, 3943, 3944, 3945, 3946, 3947, 3948, 3949, 3950, 3951, 3952, 3953, 3954, 3955, 3956, 3957, 3958, 3959, 3960, 3961, 3962, 3963, 3964, 3965, 3966, 3967, 3968, 3969, 3970, 3971, 3972, 3973, 3974, 3975, 3976, 3977, 3978, 3979, 3980, 3981, 3982, 3983, 3984, 3985, 3986, 3987, 3988, 3989, 3990, 3991, 3992, 3993, 3994, 3995, 3996, 3997, 3998, 3999, 4000, 4001, 4002, 4003, 4004, 4005, 4006, 4007, 4008, 4009, 4010, 4011, 4012, 4013, 4014, 4015, 4016, 4017, 4018, 4019, 4020, 4021, 4022, 4023, 4024, 4025, 4026, 4027, 4028, 4029, 4030, 4031]</t>
         </is>
       </c>
-      <c r="BV4" t="n">
+      <c r="CD4" t="n">
         <v>0.0985616599858524</v>
       </c>
-      <c r="BW4" t="inlineStr">
+      <c r="CE4" t="inlineStr">
         <is>
           <t>{'Numk': 20, 'KPar': 17, 'Bucket_index': 1000}</t>
         </is>
       </c>
-      <c r="BX4" t="n">
+      <c r="CF4" t="n">
         <v>30.30766875389963</v>
       </c>
-      <c r="BY4" t="inlineStr">
+      <c r="CG4" t="inlineStr">
         <is>
           <t>no</t>
         </is>
       </c>
-      <c r="BZ4" t="n">
-        <v>0</v>
-      </c>
-      <c r="CA4" t="inlineStr">
+      <c r="CH4" t="n">
+        <v>0</v>
+      </c>
+      <c r="CI4" t="inlineStr">
         <is>
           <t>params</t>
         </is>
       </c>
-      <c r="CB4" t="n">
+      <c r="CJ4" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1788,93 +1900,117 @@
       <c r="BE5" t="n">
         <v>3</v>
       </c>
-      <c r="BF5" t="inlineStr"/>
-      <c r="BG5" t="inlineStr">
+      <c r="BF5" t="n">
+        <v>3</v>
+      </c>
+      <c r="BG5" t="n">
+        <v>3</v>
+      </c>
+      <c r="BH5" t="n">
+        <v>3</v>
+      </c>
+      <c r="BI5" t="n">
+        <v>3</v>
+      </c>
+      <c r="BJ5" t="n">
+        <v>3</v>
+      </c>
+      <c r="BK5" t="n">
+        <v>3</v>
+      </c>
+      <c r="BL5" t="n">
+        <v>3</v>
+      </c>
+      <c r="BM5" t="n">
+        <v>3</v>
+      </c>
+      <c r="BN5" t="inlineStr"/>
+      <c r="BO5" t="inlineStr">
         <is>
           <t>nab-data/realKnownCause/machine_temperature_system_failure.csv</t>
         </is>
       </c>
-      <c r="BH5" t="n">
+      <c r="BP5" t="n">
         <v>22695</v>
       </c>
-      <c r="BI5" t="inlineStr">
+      <c r="BQ5" t="inlineStr">
         <is>
           <t>NAB</t>
         </is>
       </c>
-      <c r="BJ5" t="n">
-        <v>4</v>
-      </c>
-      <c r="BK5" t="inlineStr">
+      <c r="BR5" t="n">
+        <v>4</v>
+      </c>
+      <c r="BS5" t="inlineStr">
         <is>
           <t>2126; 3703; 16057; 19232</t>
         </is>
       </c>
-      <c r="BL5" t="n">
+      <c r="BT5" t="n">
         <v>566</v>
       </c>
-      <c r="BM5" t="inlineStr">
+      <c r="BU5" t="inlineStr">
         <is>
           <t>[840, 842, 843, 845, 846, 847, 848, 849, 850, 851, 852, 853, 854, 2126, 2127, 2128, 2129, 2130, 2131, 2132, 2133, 2134, 2135, 2136, 2137, 2138, 2139, 2140, 2141, 2142, 2143, 2144, 2145, 2146, 2147, 2148, 2149, 2150, 2151, 2152, 2153, 2154, 2155, 2156, 2157, 2158, 2159, 2160, 2161, 2162, 2163, 2164, 2165, 2166, 2167, 2168, 2169, 2170, 2171, 2172, 2173, 2174, 2175, 2176, 2177, 2178, 2179, 2180, 2181, 2182, 2183, 2184, 2185, 2186, 2187, 2188, 2189, 2190, 2191, 2192, 2193, 2194, 2195, 2196, 2197, 2198, 2199, 2200, 2201, 2202, 2203, 2204, 2205, 2206, 2207, 2208, 2209, 2210, 2211, 2212, 2213, 2214, 2215, 2216, 2217, 2218, 2219, 2220, 2221, 2222, 2223, 2224, 2225, 2226, 2227, 2228, 2229, 2230, 2231, 2232, 2233, 2234, 2235, 2236, 2237, 2238, 2239, 2240, 2241, 2242, 2243, 2244, 2245, 2246, 2247, 2248, 2249, 2250, 2251, 2252, 2253, 2254, 2255, 2256, 2257, 2258, 2259, 2260, 2261, 2262, 2263, 2264, 2265, 2266, 2267, 2269, 2270, 2271, 2272, 2273, 2274, 2276, 2278, 2279, 2280, 2281, 2282, 2283, 2285, 2286, 2287, 2289, 2290, 2291, 2292, 2294, 2298, 2301, 3837, 3839, 3840, 3842, 3844, 3846, 3847, 3848, 3849, 3850, 3851, 3852, 3853, 3854, 3855, 3856, 3857, 3858, 3859, 3860, 3861, 3862, 3863, 3864, 3865, 3866, 3867, 3868, 3869, 3870, 3871, 3872, 3873, 3874, 3875, 3876, 3877, 3878, 3879, 3880, 3881, 3882, 3883, 3884, 3885, 3886, 9721, 9723, 9726, 9727, 9728, 9729, 9730, 9731, 9732, 9733, 9734, 9735, 9736, 9737, 9738, 9739, 9740, 9741, 9742, 9743, 9744, 9745, 9746, 9747, 9748, 15158, 15161, 15162, 15163, 15164, 15165, 15166, 15167, 15168, 15169, 15170, 15171, 15172, 15173, 16332, 16333, 16334, 16335, 16336, 16337, 16338, 16339, 16340, 16341, 16342, 16343, 16344, 16345, 16346, 16347, 16348, 16349, 16350, 16351, 16352, 16353, 16354, 16355, 16356, 16357, 16358, 16359, 16360, 16361, 16362, 16363, 16364, 16365, 16366, 16367, 16368, 16369, 16370, 16371, 16372, 16373, 16374, 16375, 16376, 16377, 16378, 16379, 16380, 16381, 16382, 16384, 16385, 17959, 17963, 17965, 17968, 17969, 17970, 17971, 17972, 17973, 17974, 17975, 17976, 17977, 17978, 17979, 17980, 19245, 19249, 19251, 19254, 19255, 19256, 19257, 19259, 19262, 19263, 19264, 19265, 19266, 19267, 19268, 19269, 19270, 19271, 19272, 19273, 19274, 19275, 19276, 19277, 19278, 19279, 19280, 19281, 19282, 19283, 19284, 19285, 19286, 19287, 19288, 19289, 19290, 19291, 19292, 19293, 19294, 19295, 19296, 19297, 19298, 19299, 19300, 19301, 19302, 19303, 19304, 19305, 19306, 19307, 19308, 19309, 19310, 19311, 19312, 19313, 19314, 19315, 19316, 19317, 19318, 19319, 19320, 19321, 19322, 19323, 19324, 19325, 19326, 19327, 19328, 19329, 19330, 19331, 19332, 19333, 19334, 19335, 19336, 19337, 19338, 19339, 19340, 19341, 19342, 19343, 19344, 19345, 19346, 19347, 19348, 19349, 19350, 19351, 19352, 19353, 19354, 19355, 19356, 19357, 19358, 19359, 19360, 19361, 19362, 19363, 19364, 19365, 19366, 19367, 19368, 19369, 19370, 19371, 19372, 19373, 19374, 19375, 19376, 19377, 19378, 19379, 19380, 19381, 19382, 19383, 19384, 19385, 19386, 19387, 19388, 19389, 19390, 19391, 19392, 19393, 19394, 19395, 19396, 19397, 19398, 19399, 19400, 19401, 19402, 19403, 19404, 19405, 19406, 19407, 19408, 19409, 19410, 19411, 19412, 19413, 19414, 19415, 19416, 19417, 19418, 19419, 19420, 19421, 19422, 19423, 19424, 19425, 19426, 19427, 19428, 19429, 19430, 19431, 19432, 19433, 19434, 19435, 19436, 19437, 19438]</t>
         </is>
       </c>
-      <c r="BN5" t="n">
+      <c r="BV5" t="n">
         <v>0.7578947368421053</v>
       </c>
-      <c r="BO5" t="inlineStr">
+      <c r="BW5" t="inlineStr">
         <is>
           <t>{'initial_window': 892, 'window_size': 486, 'num_trees': 17, 'max_depth': 12}</t>
         </is>
       </c>
-      <c r="BP5" t="n">
+      <c r="BX5" t="n">
         <v>8.018043743912131</v>
       </c>
-      <c r="BQ5" t="inlineStr">
+      <c r="BY5" t="inlineStr">
         <is>
           <t>no</t>
         </is>
       </c>
-      <c r="BR5" t="n">
-        <v>0</v>
-      </c>
-      <c r="BS5" t="inlineStr">
+      <c r="BZ5" t="n">
+        <v>0</v>
+      </c>
+      <c r="CA5" t="inlineStr">
         <is>
           <t>params</t>
         </is>
       </c>
-      <c r="BT5" t="n">
-        <v>0</v>
-      </c>
-      <c r="BU5" t="inlineStr">
+      <c r="CB5" t="n">
+        <v>0</v>
+      </c>
+      <c r="CC5" t="inlineStr">
         <is>
           <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86, 87, 88, 89, 90, 91, 92, 93, 94, 95, 96, 97, 98, 99, 100, 101, 102, 103, 104, 105, 106, 107, 108, 109, 110, 111, 112, 113, 114, 115, 116, 117, 118, 119, 120, 121, 122, 123, 124, 125, 126, 127, 128, 129, 130, 131, 132, 133, 134, 135, 136, 137, 138, 139, 140, 141, 142, 143, 144, 145, 146, 147, 148, 149, 150, 151, 152, 153, 154, 155, 156, 157, 158, 159, 160, 161, 162, 163, 164, 165, 166, 167, 168, 169, 170, 171, 172, 173, 174, 175, 176, 177, 178, 179, 180, 181, 182, 183, 184, 185, 186, 187, 188, 189, 190, 191, 192, 193, 194, 195, 196, 197, 198, 199, 200, 201, 202, 203, 204, 205, 206, 207, 208, 209, 210, 211, 212, 213, 214, 215, 216, 217, 218, 219, 220, 221, 222, 223, 224, 225, 226, 227, 228, 229, 230, 231, 232, 233, 234, 235, 236, 237, 238, 239, 240, 241, 242, 243, 244, 245, 246, 247, 248, 249, 250, 251, 252, 253, 254, 255, 256, 257, 258, 259, 260, 261, 262, 263, 264, 265, 266, 267, 268, 269, 270, 271, 272, 273, 274, 275, 276, 277, 278, 279, 280, 281, 282, 283, 284, 285, 286, 287, 288, 289, 290, 291, 292, 293, 294, 295, 296, 297, 298, 299, 300, 301, 302, 303, 304, 305, 306, 307, 308, 309, 310, 311, 312, 313, 314, 315, 316, 317, 318, 319, 320, 321, 322, 323, 324, 325, 326, 327, 328, 329, 330, 331, 332, 333, 334, 335, 336, 337, 338, 339, 340, 341, 342, 343, 344, 345, 346, 347, 348, 349, 350, 351, 352, 353, 354, 355, 356, 357, 358, 359, 360, 361, 362, 363, 364, 365, 366, 367, 368, 369, 370, 371, 372, 373, 374, 375, 376, 377, 378, 379, 380, 381, 382, 383, 384, 385, 386, 387, 388, 389, 390, 391, 392, 393, 394, 395, 396, 397, 398, 399, 400, 401, 402, 403, 404, 405, 406, 407, 408, 409, 410, 411, 412, 413, 414, 415, 416, 417, 418, 419, 420, 421, 422, 423, 424, 425, 426, 427, 428, 429, 430, 431, 432, 433, 434, 435, 436, 437, 438, 439, 440, 441, 442, 443, 444, 445, 446, 447, 448, 449, 450, 451, 452, 453, 454, 455, 456, 457, 458, 459, 460, 461, 462, 463, 464, 465, 466, 467, 468, 469, 470, 471, 472, 473, 474, 475, 476, 477, 478, 479, 480, 481, 482, 483, 484, 485, 486, 487, 488, 489, 490, 491, 492, 493, 494, 495, 496, 497, 498, 499, 500, 501, 502, 503, 504, 505, 506, 507, 508, 509, 510, 511, 512, 513, 514, 515, 516, 517, 518, 519, 520, 521, 522, 523, 524, 525, 526, 527, 528, 529, 530, 531, 532, 533, 534, 535, 536, 537, 538, 539, 540, 541, 542, 543, 544, 545, 546, 547, 548, 549, 550, 551, 552, 553, 554, 555, 556, 557, 558, 559, 560, 561, 562, 563, 564, 565, 566, 567, 568, 569, 570, 571, 572, 573, 574, 575, 576, 577, 578, 579, 580, 581, 582, 583, 584, 585, 586, 587, 588, 589, 590, 591, 592, 593, 594, 595, 596, 597, 598, 599, 600, 601, 602, 603, 604, 605, 606, 607, 608, 609, 610, 611, 612, 613, 614, 615, 616, 617, 618, 619, 620, 621, 622, 623, 624, 625, 626, 627, 628, 629, 630, 631, 632, 633, 634, 635, 636, 637, 638, 639, 640, 641, 642, 643, 644, 645, 646, 647, 648, 649, 650, 651, 652, 653, 654, 655, 656, 657, 658, 659, 660, 661, 662, 663, 664, 665, 666, 667, 668, 669, 670, 671, 672, 673, 674, 675, 676, 677, 678, 679, 680, 681, 682, 683, 684, 685, 686, 687, 688, 689, 690, 691, 692, 693, 694, 695, 696, 697, 698, 699, 700, 701, 702, 703, 704, 705, 706, 707, 708, 709, 710, 711, 712, 713, 714, 715, 716, 717, 718, 719, 720, 721, 722, 723, 724, 725, 727, 728, 729, 730, 731, 732, 733, 734, 735, 736, 737, 738, 739, 740, 741, 742, 743, 744, 745, 746, 747, 748, 749, 750, 751, 752, 753, 754, 755, 756, 757, 758, 759, 760, 761, 762, 763, 764, 765, 766, 767, 768, 769, 770, 771, 772, 773, 774, 775, 776, 777, 778, 779, 780, 781, 782, 783, 784, 785, 786, 787, 788, 789, 790, 791, 792, 793, 794, 795, 796, 797, 798, 799, 800, 801, 802, 803, 804, 805, 806, 807, 808, 809, 810, 811, 812, 813, 814, 815, 816, 817, 818, 819, 820, 821, 822, 823, 824, 825, 826, 827, 828, 829, 830, 831, 832, 833, 834, 835, 836, 837, 838, 839, 840, 841, 842, 843, 844, 845, 846, 847, 848, 849, 850, 851, 852, 853, 854, 855, 856, 857, 858, 859, 860, 861, 862, 863, 864, 865, 866, 867, 868, 869, 870, 871, 872, 873, 874, 875, 876, 877, 878, 879, 880, 881, 882, 883, 884, 885, 886, 887, 888, 889, 890, 891, 892, 893, 894, 895, 896, 897, 898, 899, 900, 901, 902, 903, 904, 905, 906, 907, 908, 909, 910, 911, 912, 913, 914, 915, 916, 917, 918, 919, 920, 921, 922, 923, 924, 925, 926, 927, 928, 929, 930, 931, 932, 933, 934, 935, 936, 937, 938, 939, 940, 941, 942, 943, 944, 945, 946, 947, 948, 949, 950, 951, 952, 953, 954, 955, 956, 957, 958, 959, 960, 961, 962, 963, 964, 965, 966, 967, 968, 969, 970, 971, 972, 973, 974, 975, 976, 977, 978, 979, 980, 981, 982, 983, 984, 985, 986, 987, 988, 989, 990, 991, 992, 993, 994, 995, 996, 997, 998, 999, 1000, 1001, 1002, 1003, 1004, 1005, 1006, 1007, 1008, 1009, 1010, 1011, 1012, 1013, 1014, 1015, 1016, 1017, 1018, 1019, 1020, 1021, 1022, 1023, 1024, 1025, 1026, 1027, 1028, 1029, 1030, 1031, 1032, 1033, 1034, 1035, 1036, 1037, 1038, 1039, 1040, 1041, 1042, 1043, 1044, 1045, 1046, 1047, 1048, 1049, 1050, 1051, 1052, 1053, 1054, 1055, 1056, 1057, 1058, 1059, 1060, 1061, 1062, 1063, 1064, 1065, 1066, 1067, 1068, 1069, 1070, 1071, 1072, 1073, 1074, 1075, 1076, 1077, 1078, 1079, 1080, 1081, 1082, 1083, 1084, 1085, 1086, 1087, 1088, 1089, 1090, 1091, 1092, 1093, 1094, 1095, 1096, 1097, 1098, 1099, 1100, 1101, 1102, 1103, 1104, 1105, 1106, 1107, 1108, 1109, 1110, 1111, 1112, 1113, 1114, 1115, 1116, 1117, 1118, 1119, 1120, 1121, 1122, 1123, 1124, 1125, 1126, 1127, 1128, 1129, 1130, 1131, 1132, 1133, 1134, 1135, 1136, 1137, 1138, 1139, 1140, 1141, 1142, 1143, 1144, 1145, 1146, 1147, 1148, 1149, 1150, 1151, 1152, 1153, 1154, 1155, 1156, 1157, 1158, 1159, 1160, 1161, 1162, 1163, 1164, 1165, 1166, 1167, 1168, 1169, 1170, 1171, 1172, 1173, 1174, 1175, 1176, 1177, 1178, 1179, 1180, 1181, 1182, 1183, 1184, 1185, 1186, 1187, 1188, 1189, 1190, 1191, 1192, 1193, 1194, 1195, 1196, 1197, 1198, 1199, 1200, 1201, 1202, 1203, 1204, 1205, 1206, 1207, 1208, 1209, 1210, 1211, 1212, 1213, 1214, 1215, 1216, 1217, 1218, 1219, 1220, 1221, 1222, 1223, 1224, 1225, 1226, 1227, 1228, 1229, 1230, 1231, 1232, 1233, 1234, 1235, 1236, 1237, 1238, 1239, 1240, 1241, 1242, 1243, 1244, 1245, 1246, 1247, 1248, 1249, 1250, 1251, 1252, 1253, 1254, 1255, 1256, 1257, 1258, 1259, 1260, 1261, 1262, 1263, 1264, 1265, 1266, 1267, 1268, 1269, 1270, 1271, 1272, 1273, 1274, 1275, 1276, 1277, 1278, 1279, 1280, 1281, 1282, 1283, 1284, 1285, 1286, 1287, 1288, 1289, 1290, 1291, 1292, 1293, 1294, 1295, 1296, 1297, 1298, 1299, 1300, 1301, 1302, 1303, 1304, 1305, 1306, 1307, 1308, 1309, 1310, 1311, 1312, 1313, 1314, 1315, 1316, 1317, 1318, 1319, 1320, 1321, 1322, 1323, 1324, 1325, 1326, 1327, 1328, 1329, 1330, 1331, 1332, 1333, 1334, 1335, 1336, 1337, 1338, 1339, 1340, 1341, 1342, 1343, 1344, 1345, 1346, 1347, 1348, 1349, 1350, 1351, 1352, 1353, 1354, 1355, 1356, 1357, 1358, 1359, 1360, 1361, 1362, 1363, 1364, 1365, 1366, 1367, 1368, 1369, 1370, 1371, 1372, 1373, 1374, 1375, 1376, 1377, 1378, 1379, 1380, 1381, 1382, 1383, 1384, 1385, 1386, 1387, 1388, 1389, 1390, 1391, 1392, 1393, 1394, 1395, 1396, 1397, 1398, 1399, 1400, 1401, 1402, 1403, 1404, 1405, 1406, 1407, 1408, 1409, 1410, 1411, 1412, 1413, 1414, 1415, 1416, 1417, 1418, 1419, 1420, 1421, 1422, 1423, 1424, 1425, 1426, 1427, 1428, 1429, 1430, 1431, 1432, 1433, 1434, 1435, 1436, 1437, 1438, 1439, 1440, 1441, 1442, 1443, 1444, 1445, 1446, 1447, 1448, 1449, 1450, 1451, 1452, 1453, 1454, 1455, 1456, 1457, 1458, 1459, 1460, 1461, 1462, 1463, 1464, 1465, 1466, 1467, 1468, 1469, 1470, 1471, 1472, 1473, 1474, 1475, 1476, 1477, 1478, 1479, 1480, 1481, 1482, 1483, 1484, 1485, 1486, 1487, 1488, 1489, 1490, 1491, 1492, 1493, 1494, 1495, 1496, 1497, 1498, 1499, 1500, 1501, 1502, 1503, 1504, 1505, 1506, 1507, 1508, 1509, 1510, 1511, 1512, 1513, 1514, 1515, 1516, 1517, 1518, 1519, 1520, 1521, 1522, 1523, 1524, 1525, 1526, 1527, 1528, 1529, 1530, 1531, 1532, 1533, 1534, 1535, 1536, 1537, 1538, 1539, 1540, 1541, 1542, 1543, 1544, 1545, 1546, 1547, 1548, 1549, 1550, 1551, 1552, 1553, 1554, 1555, 1556, 1557, 1558, 1559, 1560, 1561, 1562, 1563, 1564, 1565, 1566, 1567, 1568, 1569, 1570, 1571, 1572, 1573, 1574, 1575, 1576, 1577, 1578, 1579, 1580, 1581, 1582, 1583, 1584, 1585, 1586, 1587, 1588, 1589, 1590, 1591, 1592, 1593, 1594, 1595, 1596, 1597, 1598, 1599, 1600, 1601, 1602, 1603, 1604, 1605, 1606, 1607, 1608, 1609, 1610, 1612, 1613, 1614, 1615, 1616, 1617, 1618, 1619, 1620, 1621, 1622, 1623, 1624, 1625, 1626, 1627, 1628, 1629, 1630, 1631, 1632, 1633, 1634, 1635, 1636, 1637, 1638, 1639, 1640, 1641, 1642, 1643, 1644, 1645, 1646, 1647, 1648, 1649, 1650, 1651, 1652, 1653, 1654, 1655, 1656, 1657, 1658, 1659, 1660, 1661, 1662, 1663, 1664, 1665, 1666, 1667, 1668, 1669, 1670, 1671, 1672, 1674, 1675, 1676, 1677, 1678, 1679, 1680, 1681, 1682, 1683, 1684, 1685, 1686, 1687, 1688, 1689, 1690, 1691, 1692, 1693, 1694, 1695, 1696, 1697, 1698, 1699, 1700, 1701, 1702, 1703, 1704, 1705, 1706, 1707, 1708, 1709, 1710, 1711, 1712, 1713, 1714, 1715, 1716, 1717, 1718, 1719, 1720, 1721, 1722, 1723, 1724, 1725, 1726, 1727, 1728, 1729, 1730, 1731, 1732, 1733, 1734, 1735, 1736, 1737, 1738, 1739, 1740, 1741, 1742, 1743, 1744, 1745, 1746, 1747, 1748, 1749, 1750, 1751, 1752, 1753, 1754, 1755, 1756, 1757, 1758, 1759, 1760, 1761, 1762, 1763, 1764, 1765, 1766, 1767, 1768, 1769, 1770, 1771, 1772, 1773, 1774, 1775, 1776, 1777, 1778, 1779, 1780, 1781, 1782, 1783, 1784, 1785, 1786, 1787, 1788, 1789, 1790, 1791, 1792, 1793, 1794, 1795, 1796, 1797, 1798, 1799, 1800, 1801, 1802, 1803, 1804, 1805, 1806, 1807, 1808, 1809, 1810, 1811, 1812, 1813, 1814, 1815, 1816, 1817, 1818, 1819, 1820, 1821, 1822, 1823, 1824, 1825, 1826, 1827, 1828, 1829, 1830, 1831, 1832, 1833, 1834, 1835, 1836, 1837, 1838, 1839, 1840, 1841, 1842, 1843, 1844, 1845, 1846, 1847, 1848, 1849, 1850, 1851, 1852, 1853, 1854, 1855, 1856, 1857, 1858, 1859, 1860, 1861, 1862, 1863, 1864, 1865, 1866, 1867, 1868, 1869, 1870, 1871, 1872, 1874, 1875, 1876, 1877, 1878, 1879, 1880, 1881, 1882, 1883, 1884, 1885, 1886, 1887, 1888, 1889, 1890, 1891, 1892, 1893, 1894, 1895, 1896, 1897, 1898, 1899, 1900, 1901, 1902, 1903, 1904, 1905, 1906, 1907, 1908, 1909, 1910, 1911, 1912, 1913, 1914, 1915, 1916, 1917, 1918, 1919, 1920, 1921, 1922, 1923, 1924, 1925, 1926, 1927, 1928, 1929, 1930, 1931, 1932, 1933, 1934, 1935, 1936, 1937, 1938, 1939, 1940, 1941, 1942, 1943, 1944, 1945, 1946, 1947, 1948, 1949, 1950, 1951, 1952, 1953, 1954, 1955, 1956, 1957, 1958, 1959, 1960, 1961, 1962, 1963, 1964, 1965, 1966, 1967, 1968, 1969, 1970, 1971, 1972, 1973, 1974, 1975, 1976, 1977, 1978, 1979, 1980, 1981, 1982, 1983, 1984, 1985, 1986, 1987, 1988, 1989, 1990, 1991, 1992, 1993, 1994, 1995, 1996, 1997, 1998, 1999, 2000, 2001, 2002, 2003, 2004, 2005, 2006, 2007, 2008, 2009, 2010, 2011, 2012, 2013, 2014, 2015, 2016, 2017, 2018, 2019, 2020, 2021, 2022, 2023, 2024, 2025, 2026, 2027, 2028, 2029, 2030, 2031, 2032, 2033, 2034, 2035, 2036, 2037, 2038, 2039, 2040, 2041, 2042, 2043, 2044, 2045, 2046, 2047, 2048, 2049, 2050, 2051, 2052, 2053, 2054, 2055, 2056, 2057, 2058, 2059, 2060, 2061, 2062, 2063, 2064, 2065, 2066, 2067, 2068, 2069, 2070, 2071, 2072, 2073, 2074, 2075, 2076, 2077, 2078, 2079, 2080, 2081, 2082, 2083, 2084, 2085, 2086, 2087, 2088, 2089, 2090, 2091, 2092, 2093, 2094, 2095, 2096, 2097, 2098, 2099, 2100, 2101, 2102, 2103, 2104, 2105, 2106, 2107, 2108, 2109, 2110, 2111, 2112, 2113, 2114, 2115, 2116, 2117, 2118, 2119, 2120, 2121, 2122, 2123, 2124, 2125, 2126, 2127, 2128, 2129, 2130, 2131, 2132, 2133, 2134, 2135, 2136, 2137, 2138, 2139, 2140, 2141, 2142, 2143, 2144, 2145, 2146, 2147, 2148, 2149, 2150, 2151, 2152, 2153, 2154, 2155, 2156, 2157, 2158, 2159, 2160, 2161, 2162, 2163, 2164, 2165, 2166, 2167, 2168, 2169, 2170, 2171, 2172, 2173, 2174, 2175, 2176, 2177, 2178, 2179, 2180, 2181, 2182, 2183, 2184, 2185, 2186, 2187, 2188, 2189, 2190, 2191, 2192, 2193, 2194, 2195, 2196, 2197, 2198, 2199, 2200, 2201, 2202, 2203, 2204, 2205, 2206, 2207, 2208, 2209, 2210, 2211, 2212, 2213, 2214, 2215, 2216, 2217, 2218, 2219, 2220, 2221, 2222, 2223, 2224, 2225, 2226, 2227, 2228, 2229, 2230, 2231, 2232, 2233, 2234, 2235, 2236, 2237, 2238, 2239, 2240, 2241, 2242, 2243, 2244, 2245, 2246, 2247, 2248, 2249, 2250, 2251, 2252, 2253, 2254, 2255, 2256, 2257, 2258, 2259, 2260, 2261, 2262, 2263, 2264, 2265, 2266, 2267, 2268, 2269, 2270, 2271, 2272, 2273, 2274, 2275, 2276, 2277, 2278, 2279, 2280, 2281, 2282, 2283, 2284, 2285, 2286, 2287, 2288, 2289, 2290, 2291, 2292, 2293, 2294, 2295, 2296, 2297, 2298, 2299, 2300, 2301, 2302, 2303, 2304, 2305, 2306, 2307, 2308, 2309, 2310, 2311, 2312, 2313, 2314, 2315, 2316, 2317, 2318, 2319, 2320, 2321, 2322, 2323, 2324, 2325, 2326, 2327, 2328, 2329, 2330, 2331, 2332, 2333, 2334, 2335, 2336, 2337, 2338, 2339, 2340, 2341, 2342, 2343, 2344, 2345, 2346, 2347, 2348, 2349, 2350, 2351, 2352, 2353, 2354, 2355, 2356, 2357, 2358, 2359, 2360, 2361, 2362, 2363, 2364, 2365, 2366, 2367, 2368, 2369, 2370, 2371, 2372, 2373, 2374, 2375, 2376, 2377, 2378, 2379, 2380, 2381, 2382, 2383, 2384, 2385, 2386, 2387, 2388, 2389, 2390, 2391, 2392, 2393, 2394, 2395, 2396, 2397, 2398, 2399, 2400, 2401, 2402, 2403, 2404, 2405, 2406, 2407, 2408, 2409, 2410, 2411, 2412, 2413, 2414, 2415, 2416, 2417, 2418, 2419, 2420, 2421, 2422, 2423, 2424, 2425, 2426, 2427, 2428, 2429, 2430, 2431, 2432, 2433, 2434, 2435, 2436, 2437, 2438, 2439, 2440, 2441, 2442, 2443, 2444, 2445, 2446, 2447, 2448, 2449, 2450, 2451, 2452, 2453, 2454, 2455, 2456, 2457, 2458, 2459, 2460, 2461, 2462, 2463, 2464, 2465, 2466, 2467, 2468, 2469, 2470, 2471, 2472, 2473, 2474, 2475, 2476, 2477, 2478, 2479, 2480, 2481, 2482, 2483, 2484, 2485, 2486, 2487, 2488, 2489, 2490, 2491, 2492, 2493, 2494, 2495, 2496, 2497, 2498, 2499, 2500, 2501, 2502, 2503, 2504, 2505, 2506, 2507, 2508, 2509, 2510, 2511, 2512, 2513, 2514, 2515, 2516, 2517, 2518, 2519, 2520, 2521, 2522, 2523, 2524, 2525, 2526, 2527, 2528, 2529, 2530, 2531, 2532, 2533, 2534, 2535, 2536, 2537, 2538, 2539, 2540, 2541, 2542, 2543, 2544, 2545, 2546, 2547, 2548, 2549, 2550, 2551, 2552, 2553, 2554, 2555, 2556, 2557, 2558, 2559, 2560, 2561, 2562, 2563, 2564, 2565, 2566, 2567, 2568, 2569, 2570, 2571, 2572, 2573, 2574, 2575, 2576, 2577, 2578, 2579, 2580, 2581, 2582, 2583, 2584, 2585, 2586, 2587, 2588, 2589, 2590, 2591, 2592, 2593, 2594, 2595, 2596, 2597, 2598, 2599, 2600, 2601, 2602, 2603, 2604, 2605, 2606, 2607, 2608, 2609, 2610, 2611, 2612, 2613, 2614, 2615, 2616, 2617, 2618, 2619, 2620, 2621, 2622, 2623, 2624, 2625, 2626, 2627, 2628, 2629, 2630, 2631, 2632, 2633, 2634, 2635, 2636, 2637, 2638, 2639, 2640, 2641, 2642, 2643, 2644, 2645, 2646, 2647, 2648, 2649, 2650, 2651, 2652, 2653, 2654, 2655, 2656, 2657, 2658, 2659, 2660, 2661, 2662, 2663, 2664, 2665, 2666, 2667, 2668, 2669, 2670, 2671, 2672, 2673, 2674, 2675, 2676, 2677, 2678, 2679, 2680, 2681, 2682, 2683, 2684, 2685, 2686, 2687, 2688, 2689, 2690, 2691, 2692, 2693, 2694, 2695, 2696, 2697, 2698, 2699, 2700, 2701, 2702, 2703, 2704, 2705, 2706, 2707, 2708, 2709, 2710, 2711, 2712, 2713, 2714, 2715, 2716, 2717, 2718, 2719, 2720, 2721, 2722, 2723, 2724, 2725, 2726, 2727, 2728, 2729, 2730, 2731, 2732, 2733, 2734, 2735, 2736, 2737, 2738, 2739, 2740, 2741, 2742, 2743, 2744, 2745, 2746, 2747, 2748, 2749, 2750, 2751, 2752, 2753, 2754, 2755, 2756, 2757, 2758, 2759, 2760, 2761, 2762, 2763, 2764, 2765, 2766, 2767, 2768, 2769, 2770, 2771, 2772, 2773, 2774, 2775, 2776, 2777, 2778, 2779, 2780, 2781, 2782, 2783, 2784, 2785, 2786, 2787, 2788, 2789, 2790, 2791, 2792, 2793, 2794, 2795, 2796, 2797, 2798, 2799, 2800, 2801, 2802, 2803, 2804, 2805, 2806, 2807, 2808, 2809, 2810, 2811, 2812, 2813, 2814, 2815, 2816, 2817, 2818, 2819, 2820, 2821, 2822, 2823, 2824, 2825, 2826, 2827, 2828, 2829, 2830, 2831, 2832, 2833, 2834, 2835, 2836, 2837, 2838, 2839, 2840, 2841, 2842, 2843, 2844, 2845, 2846, 2847, 2848, 2849, 2850, 2851, 2852, 2853, 2854, 2855, 2856, 2857, 2858, 2859, 2860, 2861, 2862, 2863, 2864, 2865, 2866, 2867, 2868, 2869, 2870, 2871, 2872, 2873, 2874, 2875, 2876, 2877, 2878, 2879, 2880, 2881, 2882, 2883, 2884, 2885, 2886, 2887, 2888, 2889, 2890, 2891, 2892, 2893, 2894, 2895, 2896, 2897, 2898, 2899, 2900, 2901, 2902, 2903, 2904, 2905, 2906, 2907, 2908, 2909, 2910, 2911, 2912, 2913, 2914, 2915, 2916, 2917, 2918, 2919, 2920, 2921, 2922, 2923, 2924, 2925, 2926, 2927, 2928, 2929, 2930, 2931, 2932, 2933, 2934, 2935, 2936, 2937, 2938, 2939, 2940, 2941, 2942, 2943, 2944, 2945, 2946, 2947, 2948, 2949, 2950, 2951, 2952, 2953, 2954, 2955, 2956, 2957, 2958, 2959, 2960, 2961, 2962, 2963, 2964, 2965, 2967, 2968, 2969, 2970, 2971, 2972, 2973, 2974, 2975, 2976, 2977, 2978, 2979, 2980, 2981, 2982, 2983, 2984, 2985, 2986, 2987, 2988, 2989, 2990, 2991, 2992, 2993, 2994, 2995, 2996, 2997, 2998, 2999, 3000, 3001, 3002, 3003, 3004, 3005, 3006, 3007, 3008, 3009, 3010, 3011, 3012, 3013, 3014, 3015, 3016, 3017, 3018, 3019, 3020, 3021, 3022, 3023, 3024, 3025, 3026, 3027, 3028, 3029, 3030, 3031, 3032, 3033, 3034, 3035, 3036, 3037, 3038, 3039, 3040, 3041, 3042, 3043, 3044, 3045, 3046, 3047, 3048, 3049, 3050, 3051, 3052, 3053, 3054, 3055, 3056, 3057, 3058, 3059, 3060, 3061, 3062, 3063, 3064, 3065, 3066, 3067, 3068, 3069, 3070, 3071, 3072, 3073, 3074, 3075, 3076, 3077, 3078, 3079, 3080, 3081, 3082, 3083, 3084, 3085, 3086, 3087, 3088, 3089, 3090, 3091, 3092, 3093, 3094, 3095, 3096, 3097, 3098, 3099, 3100, 3101, 3102, 3103, 3104, 3105, 3106, 3107, 3108, 3109, 3110, 3111, 3112, 3113, 3114, 3115, 3116, 3117, 3118, 3119, 3120, 3121, 3122, 3123, 3124, 3125, 3126, 3127, 3128, 3129, 3130, 3131, 3132, 3133, 3134, 3135, 3136, 3137, 3138, 3139, 3140, 3141, 3142, 3143, 3144, 3145, 3146, 3147, 3148, 3149, 3150, 3151, 3152, 3153, 3154, 3155, 3156, 3157, 3158, 3159, 3160, 3161, 3162, 3163, 3164, 3165, 3166, 3167, 3168, 3169, 3170, 3171, 3172, 3173, 3174, 3175, 3176, 3177, 3178, 3179, 3180, 3181, 3182, 3183, 3184, 3185, 3186, 3187, 3188, 3189, 3190, 3191, 3192, 3193, 3194, 3195, 3196, 3197, 3198, 3199, 3200, 3201, 3202, 3203, 3204, 3205, 3206, 3207, 3208, 3209, 3210, 3211, 3212, 3213, 3214, 3215, 3216, 3217, 3218, 3219, 3220, 3221, 3222, 3223, 3224, 3225, 3226, 3227, 3228, 3229, 3230, 3231, 3232, 3233, 3234, 3235, 3236, 3237, 3238, 3239, 3240, 3241, 3242, 3243, 3244, 3245, 3246, 3247, 3248, 3249, 3250, 3251, 3252, 3253, 3254, 3255, 3256, 3257, 3258, 3259, 3260, 3261, 3262, 3263, 3264, 3265, 3266, 3267, 3268, 3269, 3270, 3271, 3272, 3273, 3274, 3275, 3276, 3277, 3278, 3279, 3280, 3281, 3282, 3283, 3284, 3285, 3286, 3287, 3288, 3289, 3290, 3291, 3292, 3293, 3294, 3295, 3296, 3297, 3298, 3299, 3300, 3301, 3302, 3303, 3304, 3305, 3306, 3307, 3308, 3309, 3310, 3311, 3312, 3313, 3314, 3315, 3316, 3317, 3318, 3319, 3320, 3321, 3322, 3323, 3324, 3325, 3326, 3327, 3328, 3329, 3330, 3331, 3332, 3333, 3334, 3335, 3336, 3337, 3338, 3339, 3340, 3341, 3342, 3343, 3344, 3345, 3346, 3347, 3348, 3349, 3350, 3351, 3352, 3353, 3354, 3355, 3356, 3357, 3358, 3359, 3360, 3361, 3362, 3363, 3364, 3365, 3366, 3367, 3368, 3369, 3370, 3371, 3372, 3373, 3374, 3375, 3376, 3377, 3378, 3379, 3380, 3381, 3382, 3383, 3384, 3385, 3386, 3387, 3388, 3389, 3390, 3391, 3392, 3393, 3394, 3395, 3396, 3397, 3398, 3399, 3400, 3401, 3402, 3403, 3404, 3405, 3406, 3407, 3408, 3409, 3410, 3411, 3412, 3413, 3414, 3415, 3416, 3417, 3418, 3419, 3420, 3421, 3422, 3423, 3424, 3425, 3426, 3427, 3428, 3429, 3430, 3431, 3432, 3433, 3434, 3435, 3436, 3437, 3438, 3439, 3440, 3441, 3442, 3443, 3444, 3445, 3446, 3447, 3448, 3449, 3450, 3451, 3452, 3453, 3454, 3455, 3456, 3457, 3458, 3459, 3460, 3461, 3462, 3463, 3464, 3465, 3466, 3467, 3468, 3469, 3470, 3471, 3472, 3473, 3474, 3475, 3476, 3477, 3478, 3479, 3480, 3481, 3482, 3483, 3484, 3485, 3486, 3487, 3488, 3489, 3490, 3491, 3492, 3493, 3494, 3495, 3496, 3497, 3498, 3499, 3500, 3501, 3502, 3503, 3504, 3505, 3506, 3507, 3508, 3509, 3510, 3511, 3512, 3513, 3514, 3515, 3516, 3517, 3518, 3519, 3520, 3521, 3522, 3523, 3524, 3525, 3526, 3527, 3528, 3529, 3530, 3531, 3532, 3533, 3534, 3535, 3536, 3537, 3538, 3539, 3540, 3541, 3542, 3543, 3544, 3545, 3546, 3547, 3548, 3549, 3550, 3551, 3552, 3553, 3554, 3555, 3556, 3557, 3558, 3559, 3560, 3561, 3562, 3563, 3564, 3565, 3566, 3567, 3568, 3569, 3570, 3571, 3572, 3573, 3574, 3575, 3576, 3577, 3578, 3579, 3580, 3581, 3582, 3583, 3584, 3585, 3586, 3587, 3588, 3589, 3590, 3591, 3592, 3593, 3594, 3595, 3596, 3597, 3598, 3599, 3600, 3601, 3602, 3603, 3604, 3605, 3606, 3607, 3608, 3609, 3610, 3611, 3612, 3613, 3614, 3615, 3616, 3617, 3618, 3619, 3620, 3621, 3622, 3623, 3624, 3625, 3626, 3627, 3628, 3629, 3630, 3631, 3632, 3633, 3634, 3635, 3636, 3637, 3638, 3639, 3640, 3641, 3642, 3643, 3644, 3645, 3646, 3647, 3648, 3649, 3650, 3651, 3652, 3653, 3654, 3655, 3656, 3657, 3658, 3659, 3660, 3661, 3662, 3663, 3664, 3665, 3666, 3667, 3668, 3669, 3670, 3671, 3672, 3673, 3674, 3675, 3676, 3677, 3678, 3679, 3680, 3681, 3682, 3683, 3684, 3685, 3686, 3687, 3688, 3689, 3690, 3691, 3692, 3693, 3694, 3695, 3696, 3697, 3698, 3699, 3700, 3701, 3702, 3703, 3704, 3705, 3706, 3707, 3708, 3709, 3710, 3711, 3712, 3713, 3714, 3715, 3716, 3717, 3718, 3719, 3720, 3721, 3722, 3723, 3724, 3725, 3726, 3727, 3728, 3729, 3730, 3731, 3732, 3733, 3734, 3735, 3736, 3737, 3738, 3739, 3740, 3741, 3742, 3743, 3744, 3745, 3746, 3747, 3748, 3749, 3750, 3751, 3752, 3753, 3754, 3755, 3756, 3757, 3758, 3759, 3760, 3761, 3762, 3763, 3764, 3765, 3766, 3767, 3768, 3769, 3770, 3771, 3772, 3773, 3774, 3775, 3776, 3777, 3778, 3779, 3780, 3781, 3782, 3783, 3784, 3785, 3786, 3787, 3788, 3789, 3790, 3791, 3792, 3793, 3794, 3795, 3796, 3797, 3798, 3799, 3800, 3801, 3802, 3803, 3804, 3805, 3806, 3807, 3808, 3809, 3810, 3811, 3812, 3813, 3814, 3815, 3816, 3817, 3818, 3819, 3820, 3821, 3822, 3823, 3824, 3825, 3826, 3827, 3828, 3829, 3830, 3831, 3832, 3833, 3834, 3835, 3836, 3837, 3838, 3839, 3840, 3841, 3842, 3843, 3844, 3845, 3846, 3847, 3848, 3849, 3850, 3851, 3852, 3853, 3854, 3855, 3856, 3857, 3858, 3859, 3860, 3861, 3862, 3863, 3864, 3865, 3866, 3867, 3868, 3869, 3870, 3871, 3872, 3873, 3874, 3875, 3876, 3877, 3878, 3879, 3880, 3881, 3882, 3883, 3884, 3885, 3886, 3887, 3888, 3889, 3890, 3891, 3892, 3893, 3894, 3895, 3896, 3897, 3898, 3899, 3900, 3901, 3902, 3903, 3904, 3905, 3906, 3907, 3908, 3909, 3910, 3911, 3912, 3913, 3914, 3915, 3916, 3917, 3918, 3919, 3920, 3921, 3922, 3923, 3924, 3925, 3926, 3927, 3928, 3929, 3930, 3931, 3932, 3933, 3934, 3935, 3936, 3937, 3938, 3939, 3940, 3941, 3942, 3943, 3944, 3945, 3946, 3947, 3948, 3949, 3950, 3951, 3952, 3953, 3954, 3955, 3956, 3957, 3958, 3959, 3960, 3961, 3962, 3963, 3964, 3965, 3966, 3967, 3968, 3969, 3970, 3971, 3972, 3973, 3974, 3975, 3976, 3977, 3978, 3979, 3980, 3981, 3982, 3983, 3984, 3985, 3986, 3987, 3988, 3989, 3990, 3991, 3992, 3993, 3994, 3995, 3996, 3997, 3998, 3999, 4000, 4001, 4002, 4003, 4004, 4005, 4006, 4007, 4008, 4009, 4010, 4011, 4012, 4013, 4014, 4015, 4016, 4017, 4018, 4019, 4020, 4021, 4022, 4023, 4024, 4025, 4026, 4027, 4028, 4029, 4030, 4031, 4032, 4033, 4034, 4035, 4036, 4037, 4038, 4039, 4040, 4041, 4042, 4043, 4044, 4045, 4046, 4047, 4048, 4049, 4050, 4051, 4052, 4053, 4054, 4055, 4056, 4057, 4058, 4059, 4060, 4061, 4062, 4063, 4064, 4065, 4066, 4067, 4068, 4069, 4070, 4071, 4072, 4073, 4074, 4075, 4076, 4077, 4078, 4079, 4080, 4081, 4082, 4083, 4084, 4085, 4086, 4087, 4088, 4089, 4090, 4091, 4092, 4093, 4094, 4095, 4096, 4097, 4098, 4099, 4100, 4101, 4102, 4103, 4104, 4105, 4106, 4107, 4108, 4109, 4110, 4111, 4112, 4113, 4114, 4115, 4116, 4117, 4118, 4119, 4120, 4121, 4122, 4123, 4124, 4125, 4126, 4127, 4128, 4129, 4130, 4131, 4132, 4133, 4134, 4135, 4136, 4137, 4138, 4139, 4140, 4141, 4142, 4143, 4144, 4145, 4146, 4147, 4148, 4149, 4150, 4151, 4152, 4153, 4154, 4155, 4156, 4157, 4158, 4159, 4160, 4161, 4162, 4163, 4164, 4165, 4166, 4167, 4168, 4169, 4170, 4171, 4172, 4173, 4174, 4175, 4176, 4177, 4178, 4179, 4180, 4181, 4182, 4183, 4184, 4185, 4186, 4187, 4188, 4189, 4190, 4191, 4192, 4193, 4194, 4195, 4196, 4197, 4198, 4199, 4200, 4201, 4202, 4203, 4204, 4205, 4206, 4207, 4208, 4209, 4210, 4211, 4212, 4213, 4214, 4215, 4216, 4217, 4218, 4219, 4220, 4221, 4222, 4223, 4224, 4225, 4226, 4227, 4228, 4229, 4230, 4231, 4232, 4233, 4234, 4235, 4236, 4237, 4238, 4239, 4240, 4241, 4242, 4243, 4244, 4245, 4246, 4247, 4248, 4249, 4250, 4251, 4252, 4253, 4254, 4255, 4256, 4257, 4258, 4259, 4260, 4261, 4262, 4263, 4264, 4265, 4266, 4267, 4268, 4269, 4270, 4271, 4272, 4273, 4274, 4275, 4276, 4277, 4278, 4279, 4280, 4281, 4282, 4283, 4284, 4285, 4286, 4287, 4288, 4289, 4290, 4291, 4292, 4293, 4294, 4295, 4296, 4297, 4298, 4299, 4300, 4301, 4302, 4303, 4304, 4305, 4306, 4307, 4308, 4309, 4310, 4311, 4312, 4313, 4314, 4315, 4316, 4317, 4318, 4319, 4320, 4321, 4322, 4323, 4324, 4325, 4326, 4327, 4328, 4329, 4330, 4331, 4332, 4333, 4334, 4335, 4336, 4337, 4338, 4339, 4340, 4341, 4342, 4343, 4344, 4345, 4346, 4347, 4348, 4349, 4350, 4351, 4352, 4353, 4354, 4355, 4356, 4357, 4358, 4359, 4360, 4361, 4362, 4363, 4364, 4365, 4366, 4367, 4368, 4369, 4370, 4371, 4372, 4373, 4374, 4375, 4376, 4377, 4378, 4379, 4380, 4381, 4382, 4383, 4384, 4385, 4386, 4387, 4388, 4389, 4390, 4391, 4392, 4393, 4394, 4395, 4396, 4397, 4398, 4399, 4400, 4401, 4402, 4403, 4404, 4405, 4406, 4407, 4408, 4409, 4410, 4411, 4412, 4413, 4414, 4415, 4416, 4417, 4418, 4419, 4420, 4421, 4422, 4423, 4424, 4425, 4426, 4427, 4428, 4429, 4430, 4431, 4432, 4433, 4434, 4435, 4436, 4437, 4438, 4439, 4440, 4441, 4442, 4443, 4444, 4445, 4446, 4447, 4448, 4449, 4450, 4451, 4452, 4453, 4454, 4455, 4456, 4457, 4458, 4459, 4460, 4461, 4462, 4463, 4464, 4465, 4466, 4467, 4468, 4469, 4470, 4471, 4472, 4473, 4474, 4475, 4476, 4477, 4478, 4479, 4480, 4481, 4482, 4483, 4484, 4485, 4486, 4487, 4488, 4489, 4490, 4491, 4492, 4493, 4494, 4495, 4496, 4497, 4498, 4499, 4500, 4501, 4502, 4503, 4504, 4505, 4506, 4507, 4508, 4509, 4510, 4511, 4512, 4513, 4514, 4515, 4516, 4517, 4518, 4519, 4520, 4521, 4522, 4523, 4524, 4525, 4526, 4527, 4528, 4529, 4530, 4531, 4532, 4533, 4534, 4535, 4536, 4537, 4538, 4539, 4540, 4541, 4542, 4543, 4544, 4545, 4546, 4547, 4548, 4549, 4550, 4551, 4552, 4553, 4554, 4555, 4556, 4557, 4558, 4559, 4560, 4561, 4562, 4563, 4564, 4565, 4566, 4567, 4568, 4569, 4570, 4571, 4572, 4573, 4574, 4575, 4576, 4577, 4578, 4579, 4580, 4581, 4582, 4583, 4584, 4585, 4586, 4587, 4588, 4589, 4590, 4591, 4592, 4593, 4594, 4595, 4596, 4597, 4598, 4599, 4600, 4601, 4602, 4603, 4604, 4605, 4606, 4607, 4608, 4609, 4610, 4611, 4612, 4613, 4614, 4615, 4616, 4617, 4618, 4619, 4620, 4621, 4622, 4623, 4624, 4625, 4626, 4627, 4628, 4629, 4630, 4631, 4632, 4633, 4634, 4635, 4636, 4637, 4638, 4639, 4640, 4641, 4642, 4643, 4644, 4645, 4646, 4647, 4648, 4649, 4650, 4651, 4652, 4653, 4654, 4655, 4656, 4657, 4658, 4659, 4660, 4661, 4662, 4663, 4664, 4665, 4666, 4667, 4668, 4669, 4670, 4671, 4672, 4673, 4674, 4675, 4676, 4677, 4678, 4679, 4680, 4681, 4682, 4683, 4684, 4685, 4686, 4687, 4688, 4689, 4690, 4691, 4692, 4693, 4694, 4695, 4696, 4697, 4698, 4699, 4700, 4701, 4702, 4703, 4704, 4705, 4706, 4707, 4708, 4709, 4710, 4711, 4712, 4713, 4714, 4715, 4716, 4717, 4718, 4719, 4720, 4721, 4722, 4723, 4724, 4725, 4726, 4727, 4728, 4729, 4730, 4731, 4732, 4733, 4734, 4735, 4736, 4737, 4738, 4739, 4740, 4741, 4742, 4743, 4744, 4745, 4746, 4747, 4748, 4749, 4750, 4751, 4752, 4753, 4754, 4755, 4756, 4757, 4758, 4759, 4760, 4761, 4762, 4763, 4764, 4765, 4766, 4767, 4768, 4769, 4770, 4771, 4772, 4773, 4774, 4775, 4776, 4777, 4778, 4779, 4780, 4781, 4782, 4783, 4784, 4785, 4786, 4787, 4788, 4789, 4790, 4791, 4792, 4793, 4794, 4795, 4796, 4797, 4798, 4799, 4800, 4801, 4802, 4803, 4804, 4805, 4806, 4807, 4808, 4809, 4810, 4811, 4812, 4813, 4814, 4815, 4816, 4817, 4818, 4819, 4820, 4821, 4822, 4823, 4824, 4825, 4826, 4827, 4828, 4829, 4830, 4831, 4832, 4833, 4834, 4835, 4836, 4837, 4838, 4839, 4840, 4841, 4842, 4843, 4844, 4845, 4846, 4847, 4848, 4849, 4850, 4851, 4852, 4853, 4854, 4855, 4856, 4857, 4858, 4859, 4860, 4861, 4862, 4863, 4864, 4865, 4866, 4867, 4868, 4869, 4870, 4871, 4872, 4873, 4874, 4875, 4876, 4877, 4878, 4879, 4880, 4881, 4882, 4883, 4884, 4885, 4886, 4887, 4888, 4889, 4890, 4891, 4892, 4893, 4894, 4895, 4896, 4897, 4898, 4899, 4900, 4901, 4902, 4903, 4904, 4905, 4906, 4907, 4908, 4909, 4910, 4911, 4912, 4913, 4914, 4915, 4916, 4917, 4918, 4919, 4920, 4921, 4922, 4923, 4924, 4925, 4926, 4927, 4928, 4929, 4930, 4931, 4932, 4933, 4934, 4935, 4936, 4937, 4938, 4939, 4940, 4941, 4942, 4943, 4944, 4945, 4946, 4947, 4948, 4949, 4950, 4951, 4952, 4953, 4954, 4955, 4956, 4957, 4958, 4959, 4960, 4961, 4962, 4963, 4964, 4965, 4966, 4967, 4968, 4969, 4970, 4971, 4972, 4973, 4974, 4975, 4976, 4977, 4978, 4979, 4980, 4981, 4982, 4983, 4984, 4985, 4986, 4987, 4988, 4989, 4990, 4991, 4992, 4993, 4994, 4995, 4996, 4997, 4998, 4999, 5000, 5001, 5002, 5003, 5004, 5005, 5006, 5007, 5008, 5009, 5010, 5011, 5012, 5013, 5014, 5015, 5016, 5017, 5018, 5019, 5020, 5021, 5022, 5023, 5024, 5025, 5026, 5027, 5028, 5029, 5030, 5031, 5032, 5033, 5034, 5035, 5036, 5037, 5038, 5039, 5040, 5041, 5042, 5043, 5044, 5045, 5046, 5047, 5048, 5049, 5050, 5051, 5052, 5053, 5054, 5055, 5056, 5057, 5058, 5059, 5060, 5061, 5062, 5063, 5064, 5065, 5066, 5067, 5068, 5069, 5070, 5071, 5072, 5073, 5074, 5075, 5076, 5077, 5078, 5079, 5080, 5081, 5082, 5083, 5084, 5085, 5086, 5087, 5088, 5089, 5090, 5091, 5092, 5093, 5094, 5095, 5096, 5097, 5098, 5099, 5100, 5101, 5102, 5103, 5104, 5105, 5106, 5107, 5108, 5109, 5110, 5111, 5112, 5113, 5114, 5115, 5116, 5117, 5118, 5119, 5120, 5121, 5122, 5123, 5124, 5125, 5126, 5127, 5128, 5129, 5130, 5131, 5132, 5133, 5134, 5135, 5136, 5137, 5138, 5139, 5140, 5141, 5142, 5143, 5144, 5145, 5146, 5147, 5148, 5149, 5150, 5151, 5152, 5153, 5154, 5155, 5156, 5157, 5158, 5159, 5160, 5161, 5162, 5163, 5164, 5165, 5166, 5167, 5168, 5169, 5170, 5171, 5172, 5173, 5174, 5175, 5176, 5177, 5178, 5179, 5180, 5181, 5182, 5183, 5184, 5185, 5186, 5187, 5188, 5189, 5190, 5191, 5192, 5193, 5194, 5195, 5196, 5197, 5198, 5199, 5200, 5201, 5202, 5203, 5204, 5205, 5206, 5207, 5208, 5209, 5210, 5211, 5212, 5213, 5214, 5215, 5216, 5217, 5218, 5219, 5220, 5221, 5222, 5223, 5224, 5225, 5226, 5227, 5228, 5229, 5230, 5231, 5232, 5233, 5234, 5235, 5236, 5237, 5238, 5239, 5240, 5241, 5242, 5243, 5244, 5245, 5246, 5247, 5248, 5249, 5250, 5251, 5252, 5253, 5254, 5255, 5256, 5257, 5258, 5259, 5260, 5261, 5262, 5263, 5264, 5265, 5266, 5267, 5268, 5269, 5270, 5271, 5272, 5273, 5274, 5275, 5276, 5277, 5278, 5279, 5280, 5281, 5282, 5283, 5284, 5285, 5286, 5287, 5288, 5289, 5290, 5291, 5292, 5293, 5294, 5295, 5296, 5297, 5298, 5299, 5300, 5301, 5302, 5303, 5304, 5305, 5306, 5307, 5308, 5309, 5310, 5311, 5312, 5313, 5314, 5315, 5316, 5317, 5318, 5319, 5320, 5321, 5322, 5323, 5324, 5325, 5326, 5327, 5328, 5329, 5330, 5331, 5332, 5333, 5334, 5335, 5336, 5337, 5338, 5339, 5340, 5341, 5342, 5343, 5344, 5345, 5346, 5347, 5348, 5349, 5350, 5351, 5352, 5353, 5354, 5355, 5356, 5357, 5358, 5359, 5360, 5361, 5362, 5363, 5364, 5365, 5366, 5367, 5368, 5369, 5370, 5371, 5372, 5373, 5374, 5375, 5376, 5377, 5378, 5379, 5380, 5381, 5382, 5383, 5384, 5385, 5386, 5387, 5388, 5389, 5390, 5391, 5392, 5393, 5394, 5395, 5396, 5397, 5398, 5399, 5400, 5401, 5402, 5403, 5404, 5405, 5406, 5407, 5408, 5409, 5410, 5411, 5412, 5413, 5414, 5415, 5416, 5417, 5418, 5419, 5420, 5421, 5422, 5423, 5424, 5425, 5426, 5427, 5428, 5429, 5430, 5431, 5432, 5433, 5434, 5435, 5436, 5437, 5438, 5439, 5440, 5441, 5442, 5443, 5444, 5445, 5446, 5447, 5448, 5449, 5450, 5451, 5452, 5453, 5454, 5455, 5456, 5457, 5458, 5459, 5460, 5461, 5462, 5463, 5464, 5465, 5466, 5467, 5468, 5469, 5470, 5471, 5472, 5473, 5474, 5475, 5476, 5477, 5478, 5479, 5480, 5481, 5482, 5483, 5484, 5485, 5486, 5487, 5488, 5489, 5490, 5491, 5492, 5493, 5494, 5495, 5496, 5497, 5498, 5499, 5500, 5501, 5502, 5503, 5504, 5505, 5506, 5507, 5508, 5509, 5510, 5511, 5512, 5513, 5514, 5515, 5516, 5517, 5518, 5519, 5520, 5521, 5522, 5523, 5524, 5525, 5526, 5527, 5528, 5529, 5530, 5531, 5532, 5533, 5534, 5535, 5536, 5537, 5538, 5539, 5540, 5541, 5542, 5543, 5544, 5545, 5546, 5547, 5548, 5549, 5550, 5551, 5552, 5553, 5554, 5555, 5556, 5557, 5558, 5559, 5560, 5561, 5562, 5563, 5564, 5565, 5566, 5567, 5568, 5569, 5570, 5571, 5572, 5573, 5574, 5575, 5576, 5577, 5578, 5579, 5580, 5581, 5582, 5583, 5584, 5585, 5586, 5587, 5588, 5589, 5590, 5591, 5592, 5593, 5594, 5595, 5596, 5597, 5598, 5599, 5600, 5601, 5602, 5603, 5604, 5605, 5606, 5607, 5608, 5609, 5610, 5611, 5612, 5613, 5614, 5615, 5616, 5617, 5618, 5619, 5620, 5621, 5622, 5623, 5624, 5625, 5626, 5627, 5628, 5629, 5630, 5631, 5632, 5633, 5634, 5635, 5636, 5637, 5638, 5639, 5640, 5641, 5642, 5643, 5644, 5645, 5646, 5647, 5648, 5649, 5650,</t>
         </is>
       </c>
-      <c r="BV5" t="n">
+      <c r="CD5" t="n">
         <v>0.1476882862277406</v>
       </c>
-      <c r="BW5" t="inlineStr">
+      <c r="CE5" t="inlineStr">
         <is>
           <t>{'Numk': 15, 'KPar': 5, 'Bucket_index': 1000}</t>
         </is>
       </c>
-      <c r="BX5" t="n">
+      <c r="CF5" t="n">
         <v>1603.097915115068</v>
       </c>
-      <c r="BY5" t="inlineStr">
+      <c r="CG5" t="inlineStr">
         <is>
           <t>[519, 521, 840, 842, 843, 845, 846, 847, 848, 849, 850, 851, 852, 853, 854, 2126, 2127, 2128, 2131, 2132, 2133, 2134, 2136, 2137, 2138, 2139, 2140, 2141, 2142, 2143, 2144, 2145, 2146, 2147, 2148, 2149, 2150, 2151, 2152, 2153, 2154, 2155, 2156, 2157, 2158, 2159, 2160, 2161, 2162, 2163, 2164, 2165, 2166, 2167, 2168, 2169, 2170, 2171, 2172, 2173, 2174, 2175, 2176, 2177, 2178, 2179, 2180, 2181, 2182, 2183, 2184, 2185, 2186, 2187, 2188, 2189, 2190, 2191, 2192, 2193, 2194, 2195, 2196, 2197, 2198, 2199, 2200, 2201, 2202, 2203, 2204, 2205, 2206, 2207, 2208, 2209, 2210, 2211, 2212, 2213, 2214, 2215, 2216, 2217, 2218, 2219, 2220, 2221, 2222, 2223, 2224, 2225, 2226, 2227, 2228, 2229, 2230, 2231, 2232, 2233, 2234, 2235, 2236, 2237, 2238, 2239, 2240, 2241, 2242, 2243, 2244, 2245, 2246, 2247, 2248, 2249, 2250, 2251, 2252, 2253, 2254, 2256, 2257, 2258, 2259, 2260, 2261, 2263, 2265, 2267, 2269, 2270, 2273, 2276, 2280, 2287, 2289, 2290, 2292, 3846, 3847, 3848, 3849, 3853, 3854, 3855, 3856, 3857, 3858, 3859, 3860, 3861, 3862, 3863, 3864, 3865, 3866, 3867, 3868, 3869, 3870, 3871, 3872, 3873, 3874, 3875, 3876, 3877, 3878, 3879, 3880, 3881, 3882, 3883, 3884, 3885, 3886, 3887, 3888, 3889, 3890, 3891, 3892, 3893, 3894, 3895, 3896, 3897, 3898, 3899, 3900, 3901, 3902, 3903, 3904, 3905, 3906, 3907, 3908, 3909, 3910, 3911, 3912, 3913, 9694, 9696, 9697, 9698, 9699, 9700, 9701, 9702, 9703, 9704, 9705, 9706, 9707, 9708, 9709, 9710, 9711, 9712, 9713, 9714, 9715, 9716, 9717, 9718, 9719, 9720, 9721, 9722, 9723, 9724, 9725, 9726, 9727, 9728, 9729, 9730, 9731, 9732, 9733, 9734, 9735, 9736, 9737, 9738, 9739, 9740, 9741, 9742, 9743, 9744, 9745, 9746, 9747, 9748, 9749, 16153, 16154, 16156, 16158, 16178, 16179, 16184, 16185, 16186, 16187, 16188, 16189, 16190, 16191, 16192, 16193, 16194, 16195, 16196, 16197, 16198, 16199, 16200, 16201, 16202, 16241, 16242, 16243, 16244, 16245, 16246, 16247, 16248, 16249, 16250, 16251, 16252, 16253, 16254, 16255, 16256, 16257, 16258, 16259, 16260, 16261, 16262, 16263, 16264, 16265, 16266, 16267, 16268, 16269, 16270, 16271, 16272, 16273, 16275, 16277, 16278, 16279, 16280, 16281, 16282, 16284, 16285, 16286, 16288, 16304, 16305, 16307, 16308, 16309, 16310, 16311, 16312, 16313, 16314, 16316, 16319, 16320, 16321, 16322, 16323, 16324, 16325, 16326, 16327, 16328, 16329, 16330, 16331, 16332, 16333, 16334, 16335, 16336, 16337, 16338, 16339, 16340, 16341, 16342, 16343, 16344, 16345, 16346, 16347, 16348, 16349, 16350, 16351, 16352, 16353, 16354, 16355, 16356, 16357, 16358, 16359, 16360, 16361, 16362, 16363, 16364, 16365, 16366, 16367, 16368, 16369, 16370, 16371, 16372, 16373, 16374, 16375, 16376, 16377, 16378, 16379, 16380, 16381, 16382, 16383, 16384, 16385, 16386, 16387, 16388, 16389, 16390, 16391, 16392, 16393, 16394, 16395, 16396, 16397, 16398, 16399, 16400, 16401, 16402, 16403, 16404, 16405, 16419, 16420, 16421, 16422, 16423, 16424, 16425, 16426, 16427, 16428, 16429, 16430, 16431, 16432, 16433, 16434, 16435, 16608, 16609, 16610, 16611, 16612, 16613, 16614, 16615, 16616, 16617, 16618, 16619, 16620, 16621, 16622, 16623, 16624, 16625, 16626, 16627, 16628, 16629, 16630, 16631, 16632, 16633, 16634, 16635, 16636, 16637, 16638, 16639, 16640, 16641, 16642, 16643, 16644, 16645, 16646, 16647, 16648, 16649, 16650, 16651, 16652, 16653, 16654, 16655, 16656, 16657, 16658, 16659, 16660, 16661, 16662, 16663, 16664, 16665, 16666, 16667, 16668, 16669, 16670, 16671, 16672, 16673, 16674, 16675, 16676, 16677, 16678, 16679, 16680, 16681, 16682, 16917, 16918, 16919, 16920, 16921, 16922, 16923, 16924, 16925, 16926, 16927, 16928, 16929, 16930, 16931, 16932, 16933, 16934, 16935, 16936, 16937, 16938, 16939, 16940, 16941, 16942, 16943, 16944, 16945, 16946, 16947, 16948, 16949, 16950, 16951, 16952, 16953, 16954, 16955, 16956, 16957, 16958, 16959, 16960, 16961, 16962, 16963, 16964, 16965, 16966, 16967, 16968, 16969, 16970, 16971, 16972, 16973, 16974, 16975, 16976, 16977, 16978, 16979, 16980, 16981, 16982, 16983, 16984, 16985, 16986, 16987, 16988, 16989, 16990, 16991, 16992, 16993, 16994, 16995, 16996, 16997, 16998, 16999, 17000, 17001, 17002, 17003, 17004, 17005, 17006, 17007, 17008, 17009, 17010, 17011, 17012, 17013, 17014, 17015, 17016, 17017, 17018, 17019, 17020, 17021, 17022, 17023, 17024, 17025, 17026, 17027, 17028, 17029, 17030, 17031, 17174, 17175, 17176, 17177, 17178, 17179, 17180, 17181, 17182, 17183, 17184, 17185, 17186, 17187, 17188, 17189, 17190, 17191, 17192, 18022, 18023, 18024, 18026, 18028, 18029, 18030, 18031, 18032, 18033, 18034, 18035, 18036, 18037, 18038, 18039, 18040, 18041, 18042, 19317, 19320, 19321, 19323, 19325, 19326, 19328, 19329, 19330, 19331, 19332, 19333, 19334, 19335, 19336, 19337, 19338, 19339, 19340, 19341, 19342, 19343, 19344, 19345, 19346, 19347, 19348, 19349, 19350, 19351, 19352, 19353, 19354, 19355, 19356, 19357, 19358, 19359, 19360, 19361, 19362, 19363, 19364, 19365, 19366, 19367, 19368, 19369, 19370, 19371, 19372, 19373, 19374, 19375, 19376, 19377, 19378, 19379, 19380, 19381, 19382, 19383, 19384, 19385, 19386, 19387, 19388, 19389, 19390, 19391, 19392, 19393, 19394, 19395, 19396, 19397, 19398, 19399, 19400, 19401, 19402, 19403, 19404, 19405, 19406, 19407, 19408, 19409, 19410, 19411, 19412, 19413, 19414, 19415, 19416, 19417, 19418, 19419, 19420, 19421, 19422, 19423, 19424, 19425, 19426, 19427, 19428, 19429, 19430, 19431, 19432, 19433, 19434, 19435, 19436, 19437, 19438, 19439, 19440, 19441, 19442, 19443, 19444, 19445, 19446, 19447, 19448, 19449, 19450, 19451, 19452, 19453, 19454, 19455, 19456, 19457, 19458, 19459, 19460, 19461, 19462, 19463, 19464, 19465, 19466, 19467, 19468, 19469, 19470, 19471, 19472, 19473, 19474, 19475, 19476, 19477, 19478, 19479, 19480, 19481, 19482, 19483, 19484, 19485, 19486, 19487, 19488, 19489, 19490, 19491, 19492, 19493, 19494, 19495, 19496, 19497, 19498, 19499, 19500, 19501, 19502, 19503, 19504, 19505, 19506, 19507, 19508, 19509, 19510, 19511, 19512, 19513, 19514, 19515, 19516, 19517, 19518, 19519, 19520, 19521, 19522, 19523, 19524, 19525, 19526, 19527, 19528, 19529, 19530, 19531, 19532, 19533, 19534, 19535, 19536, 19537, 19538, 19539, 19540, 19541, 19542, 19543, 19544, 19545, 19546, 19547, 19548, 19549, 19550, 19551, 19552, 19553, 19554, 19555, 19556, 19557, 19558, 19559, 19560, 19561, 19562, 19563, 19564, 19565, 19566, 19567, 19568, 19569]</t>
         </is>
       </c>
-      <c r="BZ5" t="n">
+      <c r="CH5" t="n">
         <v>0.6078576723498887</v>
       </c>
-      <c r="CA5" t="inlineStr">
+      <c r="CI5" t="inlineStr">
         <is>
           <t>{'max_features': 1, 'window_size': 1957, 'n_estimator': 23}</t>
         </is>
       </c>
-      <c r="CB5" t="n">
+      <c r="CJ5" t="n">
         <v>580.5829102229327</v>
       </c>
     </row>
@@ -2050,93 +2186,117 @@
       <c r="BE6" t="n">
         <v>4</v>
       </c>
-      <c r="BF6" t="inlineStr"/>
-      <c r="BG6" t="inlineStr">
+      <c r="BF6" t="n">
+        <v>4</v>
+      </c>
+      <c r="BG6" t="n">
+        <v>4</v>
+      </c>
+      <c r="BH6" t="n">
+        <v>4</v>
+      </c>
+      <c r="BI6" t="n">
+        <v>4</v>
+      </c>
+      <c r="BJ6" t="n">
+        <v>4</v>
+      </c>
+      <c r="BK6" t="n">
+        <v>4</v>
+      </c>
+      <c r="BL6" t="n">
+        <v>4</v>
+      </c>
+      <c r="BM6" t="n">
+        <v>4</v>
+      </c>
+      <c r="BN6" t="inlineStr"/>
+      <c r="BO6" t="inlineStr">
         <is>
           <t>nab-data/realKnownCause/nyc_taxi.csv</t>
         </is>
       </c>
-      <c r="BH6" t="n">
+      <c r="BP6" t="n">
         <v>10320</v>
       </c>
-      <c r="BI6" t="inlineStr">
+      <c r="BQ6" t="inlineStr">
         <is>
           <t>NAB</t>
         </is>
       </c>
-      <c r="BJ6" t="n">
-        <v>5</v>
-      </c>
-      <c r="BK6" t="inlineStr">
+      <c r="BR6" t="n">
+        <v>5</v>
+      </c>
+      <c r="BS6" t="inlineStr">
         <is>
           <t>5839; 7080; 8423; 8731; 9977</t>
         </is>
       </c>
-      <c r="BL6" t="n">
+      <c r="BT6" t="n">
         <v>206</v>
       </c>
-      <c r="BM6" t="inlineStr">
+      <c r="BU6" t="inlineStr">
         <is>
           <t>[3261, 3262, 5954, 5955, 8833, 8834]</t>
         </is>
       </c>
-      <c r="BN6" t="n">
+      <c r="BV6" t="n">
         <v>0.5</v>
       </c>
-      <c r="BO6" t="inlineStr">
+      <c r="BW6" t="inlineStr">
         <is>
           <t>{'initial_window': 1121, 'window_size': 1899, 'num_trees': 17, 'max_depth': 19}</t>
         </is>
       </c>
-      <c r="BP6" t="n">
+      <c r="BX6" t="n">
         <v>383.268750739051</v>
       </c>
-      <c r="BQ6" t="inlineStr">
+      <c r="BY6" t="inlineStr">
         <is>
           <t>[170, 753, 1274, 3660, 6042, 6043, 6045, 6348, 7130, 8282, 8474, 8922, 9393, 10044]</t>
         </is>
       </c>
-      <c r="BR6" t="n">
+      <c r="BZ6" t="n">
         <v>0.6</v>
       </c>
-      <c r="BS6" t="inlineStr">
+      <c r="CA6" t="inlineStr">
         <is>
           <t>{'AR_window_size': 89, 'differencing-order': 1}</t>
         </is>
       </c>
-      <c r="BT6" t="n">
+      <c r="CB6" t="n">
         <v>390.7265384758357</v>
       </c>
-      <c r="BU6" t="inlineStr">
+      <c r="CC6" t="inlineStr">
         <is>
           <t xml:space="preserve">[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86, 87, 88, 89, 90, 91, 92, 93, 94, 95, 96, 97, 98, 99, 100, 101, 102, 103, 104, 105, 106, 107, 108, 109, 110, 111, 112, 113, 114, 115, 116, 117, 118, 119, 120, 121, 122, 123, 124, 125, 126, 127, 128, 129, 130, 131, 132, 133, 134, 135, 136, 137, 138, 139, 140, 141, 142, 143, 144, 145, 146, 147, 148, 149, 150, 151, 152, 153, 154, 155, 156, 157, 158, 159, 160, 161, 162, 163, 164, 165, 166, 167, 168, 169, 170, 171, 172, 173, 174, 175, 176, 177, 178, 179, 180, 181, 182, 183, 184, 185, 186, 187, 188, 189, 190, 191, 192, 193, 194, 195, 196, 197, 198, 199, 200, 201, 202, 203, 204, 205, 206, 207, 208, 209, 210, 211, 212, 213, 214, 215, 216, 217, 218, 219, 220, 221, 222, 223, 224, 225, 226, 227, 228, 229, 230, 231, 232, 233, 234, 235, 236, 237, 238, 239, 240, 241, 242, 243, 244, 245, 246, 247, 248, 249, 250, 251, 252, 253, 254, 255, 256, 257, 258, 259, 260, 261, 262, 263, 264, 265, 266, 267, 268, 269, 270, 271, 272, 273, 274, 275, 276, 277, 278, 279, 280, 281, 282, 283, 284, 285, 286, 287, 288, 289, 290, 291, 292, 293, 294, 295, 296, 297, 298, 299, 300, 301, 302, 303, 304, 305, 306, 307, 308, 309, 310, 311, 312, 313, 314, 315, 316, 317, 318, 319, 320, 321, 322, 323, 324, 325, 326, 327, 328, 329, 330, 331, 332, 333, 334, 335, 336, 337, 338, 339, 340, 341, 342, 343, 344, 345, 346, 347, 348, 349, 350, 351, 352, 353, 354, 355, 356, 357, 358, 359, 360, 361, 362, 363, 364, 365, 366, 367, 368, 369, 370, 371, 372, 373, 374, 375, 376, 377, 378, 379, 380, 381, 382, 383, 384, 385, 386, 387, 388, 389, 390, 391, 392, 393, 394, 395, 396, 397, 398, 399, 400, 401, 402, 403, 404, 405, 406, 407, 408, 409, 410, 411, 412, 413, 414, 415, 416, 417, 418, 419, 420, 421, 422, 423, 424, 425, 426, 427, 428, 429, 430, 431, 432, 433, 434, 435, 436, 437, 438, 439, 440, 441, 442, 443, 444, 445, 446, 447, 448, 449, 450, 451, 452, 453, 454, 455, 456, 457, 458, 459, 460, 461, 462, 463, 464, 465, 466, 467, 468, 469, 470, 471, 472, 473, 474, 475, 476, 477, 478, 479, 480, 481, 482, 483, 484, 485, 486, 487, 488, 489, 490, 491, 492, 493, 494, 495, 496, 497, 498, 499, 500, 501, 502, 503, 504, 505, 506, 507, 508, 509, 510, 511, 512, 513, 514, 515, 516, 517, 518, 519, 520, 521, 522, 523, 524, 525, 526, 527, 528, 529, 530, 531, 532, 533, 534, 535, 536, 537, 538, 539, 540, 541, 542, 543, 544, 545, 546, 547, 548, 549, 550, 551, 552, 553, 554, 555, 556, 557, 558, 559, 560, 561, 562, 563, 564, 565, 566, 567, 568, 569, 570, 571, 572, 573, 574, 575, 576, 577, 578, 579, 580, 581, 582, 583, 584, 585, 586, 587, 588, 589, 590, 591, 592, 593, 594, 595, 596, 597, 598, 599, 600, 601, 602, 603, 604, 605, 606, 607, 608, 609, 610, 611, 612, 613, 614, 615, 616, 617, 618, 619, 620, 621, 622, 623, 624, 625, 626, 627, 628, 629, 630, 631, 632, 633, 634, 635, 636, 637, 638, 639, 640, 641, 642, 643, 644, 645, 646, 647, 648, 649, 650, 651, 652, 653, 654, 655, 656, 657, 658, 659, 660, 661, 662, 663, 664, 665, 666, 667, 668, 669, 670, 671, 672, 673, 674, 675, 676, 677, 678, 679, 680, 681, 682, 683, 684, 685, 686, 687, 688, 689, 690, 691, 692, 693, 694, 695, 696, 697, 698, 699, 700, 701, 702, 703, 704, 705, 706, 707, 708, 709, 710, 711, 712, 713, 714, 715, 716, 717, 718, 719, 720, 721, 722, 723, 724, 725, 726, 727, 728, 729, 730, 731, 732, 733, 734, 735, 736, 737, 738, 739, 740, 741, 742, 743, 744, 745, 746, 747, 748, 749, 750, 751, 752, 753, 754, 755, 756, 757, 758, 759, 760, 761, 762, 763, 764, 765, 766, 767, 768, 769, 770, 771, 772, 773, 774, 775, 776, 777, 778, 779, 780, 781, 782, 783, 784, 785, 786, 787, 788, 789, 790, 791, 792, 793, 794, 795, 796, 797, 798, 799, 800, 801, 802, 803, 804, 805, 806, 807, 808, 809, 810, 811, 812, 813, 814, 815, 816, 817, 818, 819, 820, 821, 822, 823, 824, 825, 826, 827, 828, 829, 830, 831, 832, 833, 834, 835, 836, 837, 838, 839, 840, 841, 842, 843, 844, 845, 846, 847, 848, 849, 850, 851, 852, 853, 854, 855, 856, 857, 858, 859, 860, 861, 862, 863, 864, 865, 866, 867, 868, 869, 870, 871, 872, 873, 874, 875, 876, 877, 878, 879, 880, 881, 882, 883, 884, 885, 886, 887, 888, 889, 890, 891, 892, 893, 894, 895, 896, 897, 898, 899, 900, 901, 902, 903, 904, 905, 906, 907, 908, 909, 910, 911, 912, 913, 914, 915, 916, 917, 918, 919, 920, 921, 922, 923, 924, 925, 926, 927, 928, 929, 930, 931, 932, 933, 934, 935, 936, 937, 938, 939, 940, 941, 942, 943, 944, 945, 946, 947, 948, 949, 950, 951, 952, 953, 954, 955, 956, 957, 958, 959, 960, 961, 962, 963, 964, 965, 966, 967, 968, 969, 970, 971, 972, 973, 974, 975, 976, 977, 978, 979, 980, 981, 982, 983, 984, 985, 986, 987, 988, 989, 990, 991, 992, 993, 994, 995, 996, 997, 998, 999, 1000, 1001, 1002, 1003, 1004, 1005, 1006, 1007, 1008, 1009, 1010, 1011, 1012, 1013, 1014, 1015, 1016, 1017, 1018, 1019, 1020, 1021, 1022, 1023, 1024, 1025, 1026, 1027, 1028, 1029, 1030, 1031, 1032, 1033, 1034, 1035, 1036, 1037, 1038, 1039, 1040, 1041, 1042, 1043, 1044, 1045, 1046, 1047, 1048, 1049, 1050, 1051, 1052, 1053, 1054, 1055, 1056, 1057, 1058, 1059, 1060, 1061, 1062, 1063, 1064, 1065, 1066, 1067, 1068, 1069, 1070, 1071, 1072, 1073, 1074, 1075, 1076, 1077, 1078, 1079, 1080, 1081, 1082, 1083, 1084, 1085, 1086, 1087, 1088, 1089, 1090, 1091, 1092, 1093, 1094, 1095, 1096, 1097, 1098, 1099, 1100, 1101, 1102, 1103, 1104, 1105, 1106, 1107, 1108, 1109, 1110, 1111, 1112, 1113, 1114, 1115, 1116, 1117, 1118, 1119, 1120, 1121, 1122, 1123, 1124, 1125, 1126, 1127, 1128, 1129, 1130, 1131, 1132, 1133, 1134, 1135, 1136, 1137, 1138, 1139, 1140, 1141, 1142, 1143, 1144, 1145, 1146, 1147, 1148, 1149, 1150, 1151, 1152, 1153, 1154, 1155, 1156, 1157, 1158, 1159, 1160, 1161, 1162, 1163, 1164, 1165, 1166, 1167, 1168, 1169, 1170, 1171, 1172, 1173, 1174, 1175, 1176, 1177, 1178, 1179, 1180, 1181, 1182, 1183, 1184, 1185, 1186, 1187, 1188, 1189, 1190, 1191, 1192, 1193, 1194, 1195, 1196, 1197, 1198, 1199, 1200, 1201, 1202, 1203, 1204, 1205, 1206, 1207, 1208, 1209, 1210, 1211, 1212, 1213, 1214, 1215, 1216, 1217, 1218, 1219, 1220, 1221, 1222, 1223, 1224, 1225, 1226, 1227, 1228, 1229, 1230, 1231, 1232, 1233, 1234, 1235, 1236, 1237, 1238, 1239, 1240, 1241, 1242, 1243, 1244, 1245, 1246, 1247, 1248, 1249, 1250, 1251, 1252, 1253, 1254, 1255, 1256, 1257, 1258, 1259, 1260, 1261, 1262, 1263, 1264, 1265, 1266, 1267, 1268, 1269, 1270, 1271, 1272, 1273, 1274, 1275, 1276, 1277, 1278, 1279, 1280, 1281, 1282, 1283, 1284, 1285, 1286, 1287, 1288, 1289, 1290, 1291, 1292, 1293, 1294, 1295, 1296, 1297, 1298, 1299, 1300, 1301, 1302, 1303, 1304, 1305, 1306, 1307, 1308, 1309, 1310, 1311, 1312, 1313, 1314, 1315, 1316, 1317, 1318, 1319, 1320, 1321, 1322, 1323, 1324, 1325, 1326, 1327, 1328, 1329, 1330, 1331, 1332, 1333, 1334, 1335, 1336, 1337, 1338, 1339, 1340, 1341, 1342, 1343, 1344, 1345, 1346, 1347, 1348, 1349, 1350, 1351, 1352, 1353, 1354, 1355, 1356, 1357, 1358, 1359, 1360, 1361, 1362, 1363, 1364, 1365, 1366, 1367, 1368, 1369, 1370, 1371, 1372, 1373, 1374, 1375, 1376, 1377, 1378, 1379, 1380, 1381, 1382, 1383, 1384, 1385, 1386, 1387, 1388, 1389, 1390, 1391, 1392, 1393, 1394, 1395, 1396, 1397, 1398, 1399, 1400, 1401, 1402, 1403, 1404, 1405, 1406, 1407, 1408, 1409, 1410, 1411, 1412, 1413, 1414, 1415, 1416, 1417, 1418, 1419, 1420, 1421, 1422, 1423, 1424, 1425, 1426, 1427, 1428, 1429, 1430, 1431, 1432, 1433, 1434, 1435, 1436, 1437, 1438, 1439, 1440, 1441, 1442, 1443, 1444, 1445, 1446, 1447, 1448, 1449, 1450, 1451, 1452, 1453, 1454, 1455, 1456, 1457, 1458, 1459, 1460, 1461, 1462, 1463, 1464, 1465, 1466, 1467, 1468, 1469, 1470, 1471, 1472, 1473, 1474, 1475, 1476, 1477, 1478, 1479, 1480, 1481, 1482, 1483, 1484, 1485, 1486, 1487, 1488, 1489, 1490, 1491, 1492, 1493, 1494, 1495, 1496, 1497, 1498, 1499, 1500, 1501, 1502, 1503, 1504, 1505, 1506, 1507, 1508, 1509, 1510, 1511, 1512, 1513, 1514, 1515, 1516, 1517, 1518, 1519, 1520, 1521, 1522, 1523, 1524, 1525, 1526, 1527, 1528, 1529, 1530, 1531, 1532, 1533, 1534, 1535, 1536, 1537, 1538, 1539, 1540, 1541, 1542, 1543, 1544, 1545, 1546, 1547, 1548, 1549, 1550, 1551, 1552, 1553, 1554, 1555, 1556, 1557, 1558, 1559, 1560, 1561, 1562, 1563, 1564, 1565, 1566, 1567, 1568, 1569, 1570, 1571, 1572, 1573, 1574, 1575, 1576, 1577, 1578, 1579, 1580, 1581, 1582, 1583, 1584, 1585, 1586, 1587, 1588, 1589, 1590, 1591, 1592, 1593, 1594, 1595, 1596, 1597, 1598, 1599, 1600, 1601, 1602, 1603, 1604, 1605, 1606, 1607, 1608, 1609, 1610, 1611, 1612, 1613, 1614, 1615, 1616, 1617, 1618, 1619, 1620, 1621, 1622, 1623, 1624, 1625, 1626, 1627, 1628, 1629, 1630, 1631, 1632, 1633, 1634, 1635, 1636, 1637, 1638, 1639, 1640, 1641, 1642, 1643, 1644, 1645, 1646, 1647, 1648, 1649, 1650, 1651, 1652, 1653, 1654, 1655, 1656, 1657, 1658, 1659, 1660, 1661, 1662, 1663, 1664, 1665, 1666, 1667, 1668, 1669, 1670, 1671, 1672, 1673, 1674, 1675, 1676, 1677, 1678, 1679, 1680, 1681, 1682, 1683, 1684, 1685, 1686, 1687, 1688, 1689, 1690, 1691, 1692, 1693, 1694, 1695, 1696, 1697, 1698, 1699, 1700, 1701, 1702, 1703, 1704, 1705, 1706, 1707, 1708, 1709, 1710, 1711, 1712, 1713, 1714, 1715, 1716, 1717, 1718, 1719, 1720, 1721, 1722, 1723, 1724, 1725, 1726, 1727, 1728, 1729, 1730, 1731, 1732, 1733, 1734, 1735, 1736, 1737, 1738, 1739, 1740, 1741, 1742, 1743, 1744, 1745, 1746, 1747, 1748, 1749, 1750, 1751, 1752, 1753, 1754, 1755, 1756, 1757, 1758, 1759, 1760, 1761, 1762, 1763, 1764, 1765, 1766, 1767, 1768, 1769, 1770, 1771, 1772, 1773, 1774, 1775, 1776, 1777, 1778, 1779, 1780, 1781, 1782, 1783, 1784, 1785, 1786, 1787, 1788, 1789, 1790, 1791, 1792, 1793, 1794, 1795, 1796, 1797, 1798, 1799, 1800, 1801, 1802, 1803, 1804, 1805, 1806, 1807, 1808, 1809, 1810, 1811, 1812, 1813, 1814, 1815, 1816, 1817, 1818, 1819, 1820, 1821, 1822, 1823, 1824, 1825, 1826, 1827, 1828, 1829, 1830, 1831, 1832, 1833, 1834, 1835, 1836, 1837, 1838, 1839, 1840, 1841, 1842, 1843, 1844, 1845, 1846, 1847, 1848, 1849, 1850, 1851, 1852, 1853, 1854, 1855, 1856, 1857, 1858, 1859, 1860, 1861, 1862, 1863, 1864, 1865, 1866, 1867, 1868, 1869, 1870, 1871, 1872, 1873, 1874, 1875, 1876, 1877, 1878, 1879, 1880, 1881, 1882, 1883, 1884, 1885, 1886, 1887, 1888, 1889, 1890, 1891, 1892, 1893, 1894, 1895, 1896, 1897, 1898, 1899, 1900, 1901, 1902, 1903, 1904, 1905, 1906, 1907, 1908, 1909, 1910, 1911, 1912, 1913, 1914, 1915, 1916, 1917, 1918, 1919, 1920, 1921, 1922, 1923, 1924, 1925, 1926, 1927, 1928, 1929, 1930, 1931, 1932, 1933, 1934, 1935, 1936, 1937, 1938, 1939, 1940, 1941, 1942, 1943, 1944, 1945, 1946, 1947, 1948, 1949, 1950, 1951, 1952, 1953, 1954, 1955, 1956, 1957, 1958, 1959, 1960, 1961, 1962, 1963, 1964, 1965, 1966, 1967, 1968, 1969, 1970, 1971, 1972, 1973, 1974, 1975, 1976, 1977, 1978, 1979, 1980, 1981, 1982, 1983, 1984, 1985, 1986, 1987, 1988, 1989, 1990, 1991, 1992, 1993, 1994, 1995, 1996, 1997, 1998, 1999, 2000, 2001, 2002, 2003, 2004, 2005, 2006, 2007, 2008, 2009, 2010, 2011, 2012, 2013, 2014, 2015, 2016, 2017, 2018, 2019, 2020, 2021, 2022, 2023, 2024, 2025, 2026, 2027, 2028, 2029, 2030, 2031, 2032, 2033, 2034, 2035, 2036, 2037, 2038, 2039, 2040, 2041, 2042, 2043, 2044, 2045, 2046, 2047, 2048, 2049, 2050, 2051, 2052, 2053, 2054, 2055, 2056, 2057, 2058, 2059, 2060, 2061, 2062, 2063, 2064, 2065, 2066, 2067, 2068, 2069, 2070, 2071, 2072, 2073, 2074, 2075, 2076, 2077, 2078, 2079, 2080, 2081, 2082, 2083, 2084, 2085, 2086, 2087, 2088, 2089, 2090, 2091, 2092, 2093, 2094, 2095, 2096, 2097, 2098, 2099, 2100, 2101, 2102, 2103, 2104, 2105, 2106, 2107, 2108, 2109, 2110, 2111, 2112, 2113, 2114, 2115, 2116, 2117, 2118, 2119, 2120, 2121, 2122, 2123, 2124, 2125, 2126, 2127, 2128, 2129, 2130, 2131, 2132, 2133, 2134, 2135, 2136, 2137, 2138, 2139, 2140, 2141, 2142, 2143, 2144, 2145, 2146, 2147, 2148, 2149, 2150, 2151, 2152, 2153, 2154, 2155, 2156, 2157, 2158, 2159, 2160, 2161, 2162, 2163, 2164, 2165, 2166, 2167, 2168, 2169, 2170, 2171, 2172, 2173, 2174, 2175, 2176, 2177, 2178, 2179, 2180, 2181, 2182, 2183, 2184, 2185, 2186, 2187, 2188, 2189, 2190, 2191, 2192, 2193, 2194, 2195, 2196, 2197, 2198, 2199, 2200, 2201, 2202, 2203, 2204, 2205, 2206, 2207, 2208, 2209, 2210, 2211, 2212, 2213, 2214, 2215, 2216, 2217, 2218, 2219, 2220, 2221, 2222, 2223, 2224, 2225, 2226, 2227, 2228, 2229, 2230, 2231, 2232, 2233, 2234, 2235, 2236, 2237, 2238, 2239, 2240, 2241, 2242, 2243, 2244, 2245, 2246, 2247, 2248, 2249, 2250, 2251, 2252, 2253, 2254, 2255, 2256, 2257, 2258, 2259, 2260, 2261, 2262, 2263, 2264, 2265, 2266, 2267, 2268, 2269, 2270, 2271, 2272, 2273, 2274, 2275, 2276, 2277, 2278, 2279, 2280, 2281, 2282, 2283, 2284, 2285, 2286, 2287, 2288, 2289, 2290, 2291, 2292, 2293, 2294, 2295, 2296, 2297, 2298, 2299, 2300, 2301, 2302, 2303, 2304, 2305, 2306, 2307, 2308, 2309, 2310, 2311, 2312, 2313, 2314, 2315, 2316, 2317, 2318, 2319, 2320, 2321, 2322, 2323, 2324, 2325, 2326, 2327, 2328, 2329, 2330, 2331, 2332, 2333, 2334, 2335, 2336, 2337, 2338, 2339, 2340, 2341, 2342, 2343, 2344, 2345, 2346, 2347, 2348, 2349, 2350, 2351, 2352, 2353, 2354, 2355, 2356, 2357, 2358, 2359, 2360, 2361, 2362, 2363, 2364, 2365, 2366, 2367, 2368, 2369, 2370, 2371, 2372, 2373, 2374, 2375, 2376, 2377, 2378, 2379, 2380, 2381, 2382, 2383, 2384, 2385, 2386, 2387, 2388, 2389, 2390, 2391, 2392, 2393, 2394, 2395, 2396, 2397, 2398, 2399, 2400, 2401, 2402, 2403, 2404, 2405, 2406, 2407, 2408, 2409, 2410, 2411, 2412, 2413, 2414, 2415, 2416, 2417, 2418, 2419, 2420, 2421, 2422, 2423, 2424, 2425, 2426, 2427, 2428, 2429, 2430, 2431, 2432, 2433, 2434, 2435, 2436, 2437, 2438, 2439, 2440, 2441, 2442, 2443, 2444, 2445, 2446, 2447, 2448, 2449, 2450, 2451, 2452, 2453, 2454, 2455, 2456, 2457, 2458, 2459, 2460, 2461, 2462, 2463, 2464, 2465, 2466, 2467, 2468, 2469, 2470, 2471, 2472, 2473, 2474, 2475, 2476, 2477, 2478, 2479, 2480, 2481, 2482, 2483, 2484, 2485, 2486, 2487, 2488, 2489, 2490, 2491, 2492, 2493, 2494, 2495, 2496, 2497, 2498, 2499, 2500, 2501, 2502, 2503, 2504, 2505, 2506, 2507, 2508, 2509, 2510, 2511, 2512, 2513, 2514, 2515, 2516, 2517, 2518, 2519, 2520, 2521, 2522, 2523, 2524, 2525, 2526, 2527, 2528, 2529, 2530, 2531, 2532, 2533, 2534, 2535, 2536, 2537, 2538, 2539, 2540, 2541, 2542, 2543, 2544, 2545, 2546, 2547, 2548, 2549, 2550, 2551, 2552, 2553, 2554, 2555, 2556, 2557, 2558, 2559, 2560, 2561, 2562, 2563, 2564, 2565, 2566, 2567, 2568, 2569, 2570, 2571, 2572, 2573, 2574, 2575, 2576, 2577, 2578, 2579, 2580, 2581, 2582, 2583, 2584, 2585, 2586, 2587, 2588, 2589, 2590, 2591, 2592, 2593, 2594, 2595, 2596, 2597, 2598, 2599, 2600, 2601, 2602, 2603, 2604, 2605, 2606, 2607, 2608, 2609, 2610, 2611, 2612, 2613, 2614, 2615, 2616, 2617, 2618, 2619, 2620, 2621, 2622, 2623, 2624, 2625, 2626, 2627, 2628, 2629, 2630, 2631, 2632, 2633, 2634, 2635, 2636, 2637, 2638, 2639, 2640, 2641, 2642, 2643, 2644, 2645, 2646, 2647, 2648, 2649, 2650, 2651, 2652, 2653, 2654, 2655, 2656, 2657, 2658, 2659, 2660, 2661, 2662, 2663, 2664, 2665, 2666, 2667, 2668, 2669, 2670, 2671, 2672, 2673, 2674, 2675, 2676, 2677, 2678, 2679, 2680, 2681, 2682, 2683, 2684, 2685, 2686, 2687, 2688, 2689, 2690, 2691, 2692, 2693, 2694, 2695, 2696, 2697, 2698, 2699, 2700, 2701, 2702, 2703, 2704, 2705, 2706, 2707, 2708, 2709, 2710, 2711, 2712, 2713, 2714, 2715, 2716, 2717, 2718, 2719, 2720, 2721, 2722, 2723, 2724, 2725, 2726, 2727, 2728, 2729, 2730, 2731, 2732, 2733, 2734, 2735, 2736, 2737, 2738, 2739, 2740, 2741, 2742, 2743, 2744, 2745, 2746, 2747, 2748, 2749, 2750, 2751, 2752, 2753, 2754, 2755, 2756, 2757, 2758, 2759, 2760, 2761, 2762, 2763, 2764, 2765, 2766, 2767, 2768, 2769, 2770, 2771, 2772, 2773, 2774, 2775, 2776, 2777, 2778, 2779, 2780, 2781, 2782, 2783, 2784, 2785, 2786, 2787, 2788, 2789, 2790, 2791, 2792, 2793, 2794, 2795, 2796, 2797, 2798, 2799, 2800, 2801, 2802, 2803, 2804, 2805, 2806, 2807, 2808, 2809, 2810, 2811, 2812, 2813, 2814, 2815, 2816, 2817, 2818, 2819, 2820, 2821, 2822, 2823, 2824, 2825, 2826, 2827, 2828, 2829, 2830, 2831, 2832, 2833, 2834, 2835, 2836, 2837, 2838, 2839, 2840, 2841, 2842, 2843, 2844, 2845, 2846, 2847, 2848, 2849, 2850, 2851, 2852, 2853, 2854, 2855, 2856, 2857, 2858, 2859, 2860, 2861, 2862, 2863, 2864, 2865, 2866, 2867, 2868, 2869, 2870, 2871, 2872, 2873, 2874, 2875, 2876, 2877, 2878, 2879, 2880, 2881, 2882, 2883, 2884, 2885, 2886, 2887, 2888, 2889, 2890, 2891, 2892, 2893, 2894, 2895, 2896, 2897, 2898, 2899, 2900, 2901, 2902, 2903, 2904, 2905, 2906, 2907, 2908, 2909, 2910, 2911, 2912, 2913, 2914, 2915, 2916, 2917, 2918, 2919, 2920, 2921, 2922, 2923, 2924, 2925, 2926, 2927, 2928, 2929, 2930, 2931, 2932, 2933, 2934, 2935, 2936, 2937, 2938, 2939, 2940, 2941, 2942, 2943, 2944, 2945, 2946, 2947, 2948, 2949, 2950, 2951, 2952, 2953, 2954, 2955, 2956, 2957, 2958, 2959, 2960, 2961, 2962, 2963, 2964, 2965, 2966, 2967, 2968, 2969, 2970, 2971, 2972, 2973, 2974, 2975, 2976, 2977, 2978, 2979, 2980, 2981, 2982, 2983, 2984, 2985, 2986, 2987, 2988, 2989, 2990, 2991, 2992, 2993, 2994, 2995, 2996, 2997, 2998, 2999, 3000, 3001, 3002, 3003, 3004, 3005, 3006, 3007, 3008, 3009, 3010, 3011, 3012, 3013, 3014, 3015, 3016, 3017, 3018, 3019, 3020, 3021, 3022, 3023, 3024, 3025, 3026, 3027, 3028, 3029, 3030, 3031, 3032, 3033, 3034, 3035, 3036, 3037, 3038, 3039, 3040, 3041, 3042, 3043, 3044, 3045, 3046, 3047, 3048, 3049, 3050, 3051, 3052, 3053, 3054, 3055, 3056, 3057, 3058, 3059, 3060, 3061, 3062, 3063, 3064, 3065, 3066, 3067, 3068, 3069, 3070, 3071, 3072, 3073, 3074, 3075, 3076, 3077, 3078, 3079, 3080, 3081, 3082, 3083, 3084, 3085, 3086, 3087, 3088, 3089, 3090, 3091, 3092, 3093, 3094, 3095, 3096, 3097, 3098, 3099, 3100, 3101, 3102, 3103, 3104, 3105, 3106, 3107, 3108, 3109, 3110, 3111, 3112, 3113, 3114, 3115, 3116, 3117, 3118, 3119, 3120, 3121, 3122, 3123, 3124, 3125, 3126, 3127, 3128, 3129, 3130, 3131, 3132, 3133, 3134, 3135, 3136, 3137, 3138, 3139, 3140, 3141, 3142, 3143, 3144, 3145, 3146, 3147, 3148, 3149, 3150, 3151, 3152, 3153, 3154, 3155, 3156, 3157, 3158, 3159, 3160, 3161, 3162, 3163, 3164, 3165, 3166, 3167, 3168, 3169, 3170, 3171, 3172, 3173, 3174, 3175, 3176, 3177, 3178, 3179, 3180, 3181, 3182, 3183, 3184, 3185, 3186, 3187, 3188, 3189, 3190, 3191, 3192, 3193, 3194, 3195, 3196, 3197, 3198, 3199, 3200, 3201, 3202, 3203, 3204, 3205, 3206, 3207, 3208, 3209, 3210, 3211, 3212, 3213, 3214, 3215, 3216, 3217, 3218, 3219, 3220, 3221, 3222, 3223, 3224, 3225, 3226, 3227, 3228, 3229, 3230, 3231, 3232, 3233, 3234, 3235, 3236, 3237, 3238, 3239, 3240, 3241, 3242, 3243, 3244, 3245, 3246, 3247, 3248, 3249, 3250, 3251, 3252, 3253, 3254, 3255, 3256, 3257, 3258, 3259, 3260, 3261, 3262, 3263, 3264, 3265, 3266, 3267, 3268, 3269, 3270, 3271, 3272, 3273, 3274, 3275, 3276, 3277, 3278, 3279, 3280, 3281, 3282, 3283, 3284, 3285, 3286, 3287, 3288, 3289, 3290, 3291, 3292, 3293, 3294, 3295, 3296, 3297, 3298, 3299, 3300, 3301, 3302, 3303, 3304, 3305, 3306, 3307, 3308, 3309, 3310, 3311, 3312, 3313, 3314, 3315, 3316, 3317, 3318, 3319, 3320, 3321, 3322, 3323, 3324, 3325, 3326, 3327, 3328, 3329, 3330, 3331, 3332, 3333, 3334, 3335, 3336, 3337, 3338, 3339, 3340, 3341, 3342, 3343, 3344, 3345, 3346, 3347, 3348, 3349, 3350, 3351, 3352, 3353, 3354, 3355, 3356, 3357, 3358, 3359, 3360, 3361, 3362, 3363, 3364, 3365, 3366, 3367, 3368, 3369, 3370, 3371, 3372, 3373, 3374, 3375, 3376, 3377, 3378, 3379, 3380, 3381, 3382, 3383, 3384, 3385, 3386, 3387, 3388, 3389, 3390, 3391, 3392, 3393, 3394, 3395, 3396, 3397, 3398, 3399, 3400, 3401, 3402, 3403, 3404, 3405, 3406, 3407, 3408, 3409, 3410, 3411, 3412, 3413, 3414, 3415, 3416, 3417, 3418, 3419, 3420, 3421, 3422, 3423, 3424, 3425, 3426, 3427, 3428, 3429, 3430, 3431, 3432, 3433, 3434, 3435, 3436, 3437, 3438, 3439, 3440, 3441, 3442, 3443, 3444, 3445, 3446, 3447, 3448, 3449, 3450, 3451, 3452, 3453, 3454, 3455, 3456, 3457, 3458, 3459, 3460, 3461, 3462, 3463, 3464, 3465, 3466, 3467, 3468, 3469, 3470, 3471, 3472, 3473, 3474, 3475, 3476, 3477, 3478, 3479, 3480, 3481, 3482, 3483, 3484, 3485, 3486, 3487, 3488, 3489, 3490, 3491, 3492, 3493, 3494, 3495, 3496, 3497, 3498, 3499, 3500, 3501, 3502, 3503, 3504, 3505, 3506, 3507, 3508, 3509, 3510, 3511, 3512, 3513, 3514, 3515, 3516, 3517, 3518, 3519, 3520, 3521, 3522, 3523, 3524, 3525, 3526, 3527, 3528, 3529, 3530, 3531, 3532, 3533, 3534, 3535, 3536, 3537, 3538, 3539, 3540, 3541, 3542, 3543, 3544, 3545, 3546, 3547, 3548, 3549, 3550, 3551, 3552, 3553, 3554, 3555, 3556, 3557, 3558, 3559, 3560, 3561, 3562, 3563, 3564, 3565, 3566, 3567, 3568, 3569, 3570, 3571, 3572, 3573, 3574, 3575, 3576, 3577, 3578, 3579, 3580, 3581, 3582, 3583, 3584, 3585, 3586, 3587, 3588, 3589, 3590, 3591, 3592, 3593, 3594, 3595, 3596, 3597, 3598, 3599, 3600, 3601, 3602, 3603, 3604, 3605, 3606, 3607, 3608, 3609, 3610, 3611, 3612, 3613, 3614, 3615, 3616, 3617, 3618, 3619, 3620, 3621, 3622, 3623, 3624, 3625, 3626, 3627, 3628, 3629, 3630, 3631, 3632, 3633, 3634, 3635, 3636, 3637, 3638, 3639, 3640, 3641, 3642, 3643, 3644, 3645, 3646, 3647, 3648, 3649, 3650, 3651, 3652, 3653, 3654, 3655, 3656, 3657, 3658, 3659, 3660, 3661, 3662, 3663, 3664, 3665, 3666, 3667, 3668, 3669, 3670, 3671, 3672, 3673, 3674, 3675, 3676, 3677, 3678, 3679, 3680, 3681, 3682, 3683, 3684, 3685, 3686, 3687, 3688, 3689, 3690, 3691, 3692, 3693, 3694, 3695, 3696, 3697, 3698, 3699, 3700, 3701, 3702, 3703, 3704, 3705, 3706, 3707, 3708, 3709, 3710, 3711, 3712, 3713, 3714, 3715, 3716, 3717, 3718, 3719, 3720, 3721, 3722, 3723, 3724, 3725, 3726, 3727, 3728, 3729, 3730, 3731, 3732, 3733, 3734, 3735, 3736, 3737, 3738, 3739, 3740, 3741, 3742, 3743, 3744, 3745, 3746, 3747, 3748, 3749, 3750, 3751, 3752, 3753, 3754, 3755, 3756, 3757, 3758, 3759, 3760, 3761, 3762, 3763, 3764, 3765, 3766, 3767, 3768, 3769, 3770, 3771, 3772, 3773, 3774, 3775, 3776, 3777, 3778, 3779, 3780, 3781, 3782, 3783, 3784, 3785, 3786, 3787, 3788, 3789, 3790, 3791, 3792, 3793, 3794, 3795, 3796, 3797, 3798, 3799, 3800, 3801, 3802, 3803, 3804, 3805, 3806, 3807, 3808, 3809, 3810, 3811, 3812, 3813, 3814, 3815, 3816, 3817, 3818, 3819, 3820, 3821, 3822, 3823, 3824, 3825, 3826, 3827, 3828, 3829, 3830, 3831, 3832, 3833, 3834, 3835, 3836, 3837, 3838, 3839, 3840, 3841, 3842, 3843, 3844, 3845, 3846, 3847, 3848, 3849, 3850, 3851, 3852, 3853, 3854, 3855, 3856, 3857, 3858, 3859, 3860, 3861, 3862, 3863, 3864, 3865, 3866, 3867, 3868, 3869, 3870, 3871, 3872, 3873, 3874, 3875, 3876, 3877, 3878, 3879, 3880, 3881, 3882, 3883, 3884, 3885, 3886, 3887, 3888, 3889, 3890, 3891, 3892, 3893, 3894, 3895, 3896, 3897, 3898, 3899, 3900, 3901, 3902, 3903, 3904, 3905, 3906, 3907, 3908, 3909, 3910, 3911, 3912, 3913, 3914, 3915, 3916, 3917, 3918, 3919, 3920, 3921, 3922, 3923, 3924, 3925, 3926, 3927, 3928, 3929, 3930, 3931, 3932, 3933, 3934, 3935, 3936, 3937, 3938, 3939, 3940, 3941, 3942, 3943, 3944, 3945, 3946, 3947, 3948, 3949, 3950, 3951, 3952, 3953, 3954, 3955, 3956, 3957, 3958, 3959, 3960, 3961, 3962, 3963, 3964, 3965, 3966, 3967, 3968, 3969, 3970, 3971, 3972, 3973, 3974, 3975, 3976, 3977, 3978, 3979, 3980, 3981, 3982, 3983, 3984, 3985, 3986, 3987, 3988, 3989, 3990, 3991, 3992, 3993, 3994, 3995, 3996, 3997, 3998, 3999, 4000, 4001, 4002, 4003, 4004, 4005, 4006, 4007, 4008, 4009, 4010, 4011, 4012, 4013, 4014, 4015, 4016, 4017, 4018, 4019, 4020, 4021, 4022, 4023, 4024, 4025, 4026, 4027, 4028, 4029, 4030, 4031, 4032, 4033, 4034, 4035, 4036, 4037, 4038, 4039, 4040, 4041, 4042, 4043, 4044, 4045, 4046, 4047, 4048, 4049, 4050, 4051, 4052, 4053, 4054, 4055, 4056, 4057, 4058, 4059, 4060, 4061, 4062, 4063, 4064, 4065, 4066, 4067, 4068, 4069, 4070, 4071, 4072, 4073, 4074, 4075, 4076, 4077, 4078, 4079, 4080, 4081, 4082, 4083, 4084, 4085, 4086, 4087, 4088, 4089, 4090, 4091, 4092, 4093, 4094, 4095, 4096, 4097, 4098, 4099, 4100, 4101, 4102, 4103, 4104, 4105, 4106, 4107, 4108, 4109, 4110, 4111, 4112, 4113, 4114, 4115, 4116, 4117, 4118, 4119, 4120, 4121, 4122, 4123, 4124, 4125, 4126, 4127, 4128, 4129, 4130, 4131, 4132, 4133, 4134, 4135, 4136, 4137, 4138, 4139, 4140, 4141, 4142, 4143, 4144, 4145, 4146, 4147, 4148, 4149, 4150, 4151, 4152, 4153, 4154, 4155, 4156, 4157, 4158, 4159, 4160, 4161, 4162, 4163, 4164, 4165, 4166, 4167, 4168, 4169, 4170, 4171, 4172, 4173, 4174, 4175, 4176, 4177, 4178, 4179, 4180, 4181, 4182, 4183, 4184, 4185, 4186, 4187, 4188, 4189, 4190, 4191, 4192, 4193, 4194, 4195, 4196, 4197, 4198, 4199, 4200, 4201, 4202, 4203, 4204, 4205, 4206, 4207, 4208, 4209, 4210, 4211, 4212, 4213, 4214, 4215, 4216, 4217, 4218, 4219, 4220, 4221, 4222, 4223, 4224, 4225, 4226, 4227, 4228, 4229, 4230, 4231, 4232, 4233, 4234, 4235, 4236, 4237, 4238, 4239, 4240, 4241, 4242, 4243, 4244, 4245, 4246, 4247, 4248, 4249, 4250, 4251, 4252, 4253, 4254, 4255, 4256, 4257, 4258, 4259, 4260, 4261, 4262, 4263, 4264, 4265, 4266, 4267, 4268, 4269, 4270, 4271, 4272, 4273, 4274, 4275, 4276, 4277, 4278, 4279, 4280, 4281, 4282, 4283, 4284, 4285, 4286, 4287, 4288, 4289, 4290, 4291, 4292, 4293, 4294, 4295, 4296, 4297, 4298, 4299, 4300, 4301, 4302, 4303, 4304, 4305, 4306, 4307, 4308, 4309, 4310, 4311, 4312, 4313, 4314, 4315, 4316, 4317, 4318, 4319, 4320, 4321, 4322, 4323, 4324, 4325, 4326, 4327, 4328, 4329, 4330, 4331, 4332, 4333, 4334, 4335, 4336, 4337, 4338, 4339, 4340, 4341, 4342, 4343, 4344, 4345, 4346, 4347, 4348, 4349, 4350, 4351, 4352, 4353, 4354, 4355, 4356, 4357, 4358, 4359, 4360, 4361, 4362, 4363, 4364, 4365, 4366, 4367, 4368, 4369, 4370, 4371, 4372, 4373, 4374, 4375, 4376, 4377, 4378, 4379, 4380, 4381, 4382, 4383, 4384, 4385, 4386, 4387, 4388, 4389, 4390, 4391, 4392, 4393, 4394, 4395, 4396, 4397, 4398, 4399, 4400, 4401, 4402, 4403, 4404, 4405, 4406, 4407, 4408, 4409, 4410, 4411, 4412, 4413, 4414, 4415, 4416, 4417, 4418, 4419, 4420, 4421, 4422, 4423, 4424, 4425, 4426, 4427, 4428, 4429, 4430, 4431, 4432, 4433, 4434, 4435, 4436, 4437, 4438, 4439, 4440, 4441, 4442, 4443, 4444, 4445, 4446, 4447, 4448, 4449, 4450, 4451, 4452, 4453, 4454, 4455, 4456, 4457, 4458, 4459, 4460, 4461, 4462, 4463, 4464, 4465, 4466, 4467, 4468, 4469, 4470, 4471, 4472, 4473, 4474, 4475, 4476, 4477, 4478, 4479, 4480, 4481, 4482, 4483, 4484, 4485, 4486, 4487, 4488, 4489, 4490, 4491, 4492, 4493, 4494, 4495, 4496, 4497, 4498, 4499, 4500, 4501, 4502, 4503, 4504, 4505, 4506, 4507, 4508, 4509, 4510, 4511, 4512, 4513, 4514, 4515, 4516, 4517, 4518, 4519, 4520, 4521, 4522, 4523, 4524, 4525, 4526, 4527, 4528, 4529, 4530, 4531, 4532, 4533, 4534, 4535, 4536, 4537, 4538, 4539, 4540, 4541, 4542, 4543, 4544, 4545, 4546, 4547, 4548, 4549, 4550, 4551, 4552, 4553, 4554, 4555, 4556, 4557, 4558, 4559, 4560, 4561, 4562, 4563, 4564, 4565, 4566, 4567, 4568, 4569, 4570, 4571, 4572, 4573, 4574, 4575, 4576, 4577, 4578, 4579, 4580, 4581, 4582, 4583, 4584, 4585, 4586, 4587, 4588, 4589, 4590, 4591, 4592, 4593, 4594, 4595, 4596, 4597, 4598, 4599, 4600, 4601, 4602, 4603, 4604, 4605, 4606, 4607, 4608, 4609, 4610, 4611, 4612, 4613, 4614, 4615, 4616, 4617, 4618, 4619, 4620, 4621, 4622, 4623, 4624, 4625, 4626, 4627, 4628, 4629, 4630, 4631, 4632, 4633, 4634, 4635, 4636, 4637, 4638, 4639, 4640, 4641, 4642, 4643, 4644, 4645, 4646, 4647, 4648, 4649, 4650, 4651, 4652, 4653, 4654, 4655, 4656, 4657, 4658, 4659, 4660, 4661, 4662, 4663, 4664, 4665, 4666, 4667, 4668, 4669, 4670, 4671, 4672, 4673, 4674, 4675, 4676, 4677, 4678, 4679, 4680, 4681, 4682, 4683, 4684, 4685, 4686, 4687, 4688, 4689, 4690, 4691, 4692, 4693, 4694, 4695, 4696, 4697, 4698, 4699, 4700, 4701, 4702, 4703, 4704, 4705, 4706, 4707, 4708, 4709, 4710, 4711, 4712, 4713, 4714, 4715, 4716, 4717, 4718, 4719, 4720, 4721, 4722, 4723, 4724, 4725, 4726, 4727, 4728, 4729, 4730, 4731, 4732, 4733, 4734, 4735, 4736, 4737, 4738, 4739, 4740, 4741, 4742, 4743, 4744, 4745, 4746, 4747, 4748, 4749, 4750, 4751, 4752, 4753, 4754, 4755, 4756, 4757, 4758, 4759, 4760, 4761, 4762, 4763, 4764, 4765, 4766, 4767, 4768, 4769, 4770, 4771, 4772, 4773, 4774, 4775, 4776, 4777, 4778, 4779, 4780, 4781, 4782, 4783, 4784, 4785, 4786, 4787, 4788, 4789, 4790, 4791, 4792, 4793, 4794, 4795, 4796, 4797, 4798, 4799, 4800, 4801, 4802, 4803, 4804, 4805, 4806, 4807, 4808, 4809, 4810, 4811, 4812, 4813, 4814, 4815, 4816, 4817, 4818, 4819, 4820, 4821, 4822, 4823, 4824, 4825, 4826, 4827, 4828, 4829, 4830, 4831, 4832, 4833, 4834, 4835, 4836, 4837, 4838, 4839, 4840, 4841, 4842, 4843, 4844, 4845, 4846, 4847, 4848, 4849, 4850, 4851, 4852, 4853, 4854, 4855, 4856, 4857, 4858, 4859, 4860, 4861, 4862, 4863, 4864, 4865, 4866, 4867, 4868, 4869, 4870, 4871, 4872, 4873, 4874, 4875, 4876, 4877, 4878, 4879, 4880, 4881, 4882, 4883, 4884, 4885, 4886, 4887, 4888, 4889, 4890, 4891, 4892, 4893, 4894, 4895, 4896, 4897, 4898, 4899, 4900, 4901, 4902, 4903, 4904, 4905, 4906, 4907, 4908, 4909, 4910, 4911, 4912, 4913, 4914, 4915, 4916, 4917, 4918, 4919, 4920, 4921, 4922, 4923, 4924, 4925, 4926, 4927, 4928, 4929, 4930, 4931, 4932, 4933, 4934, 4935, 4936, 4937, 4938, 4939, 4940, 4941, 4942, 4943, 4944, 4945, 4946, 4947, 4948, 4949, 4950, 4951, 4952, 4953, 4954, 4955, 4956, 4957, 4958, 4959, 4960, 4961, 4962, 4963, 4964, 4965, 4966, 4967, 4968, 4969, 4970, 4971, 4972, 4973, 4974, 4975, 4976, 4977, 4978, 4979, 4980, 4981, 4982, 4983, 4984, 4985, 4986, 4987, 4988, 4989, 4990, 4991, 4992, 4993, 4994, 4995, 4996, 4997, 4998, 4999, 5000, 5001, 5002, 5003, 5004, 5005, 5006, 5007, 5008, 5009, 5010, 5011, 5012, 5013, 5014, 5015, 5016, 5017, 5018, 5019, 5020, 5021, 5022, 5023, 5024, 5025, 5026, 5027, 5028, 5029, 5030, 5031, 5032, 5033, 5034, 5035, 5036, 5037, 5038, 5039, 5040, 5041, 5042, 5043, 5044, 5045, 5046, 5047, 5048, 5049, 5050, 5051, 5052, 5053, 5054, 5055, 5056, 5057, 5058, 5059, 5060, 5061, 5062, 5063, 5064, 5065, 5066, 5067, 5068, 5069, 5070, 5071, 5072, 5073, 5074, 5075, 5076, 5077, 5078, 5079, 5080, 5081, 5082, 5083, 5084, 5085, 5086, 5087, 5088, 5089, 5090, 5091, 5092, 5093, 5094, 5095, 5096, 5097, 5098, 5099, 5100, 5101, 5102, 5103, 5104, 5105, 5106, 5107, 5108, 5109, 5110, 5111, 5112, 5113, 5114, 5115, 5116, 5117, 5118, 5119, 5120, 5121, 5122, 5123, 5124, 5125, 5126, 5127, 5128, 5129, 5130, 5131, 5132, 5133, 5134, 5135, 5136, 5137, 5138, 5139, 5140, 5141, 5142, 5143, 5144, 5145, 5146, 5147, 5148, 5149, 5150, 5151, 5152, 5153, 5154, 5155, 5156, 5157, 5158, 5159, 5160, 5161, 5162, 5163, 5164, 5165, 5166, 5167, 5168, 5169, 5170, 5171, 5172, 5173, 5174, 5175, 5176, 5177, 5178, 5179, 5180, 5181, 5182, 5183, 5184, 5185, 5186, 5187, 5188, 5189, 5190, 5191, 5192, 5193, 5194, 5195, 5196, 5197, 5198, 5199, 5200, 5201, 5202, 5203, 5204, 5205, 5206, 5207, 5208, 5209, 5210, 5211, 5212, 5213, 5214, 5215, 5216, 5217, 5218, 5219, 5220, 5221, 5222, 5223, 5224, 5225, 5226, 5227, 5228, 5229, 5230, 5231, 5232, 5233, 5234, 5235, 5236, 5237, 5238, 5239, 5240, 5241, 5242, 5243, 5244, 5245, 5246, 5247, 5248, 5249, 5250, 5251, 5252, 5253, 5254, 5255, 5256, 5257, 5258, 5259, 5260, 5261, 5262, 5263, 5264, 5265, 5266, 5267, 5268, 5269, 5270, 5271, 5272, 5273, 5274, 5275, 5276, 5277, 5278, 5279, 5280, 5281, 5282, 5283, 5284, 5285, 5286, 5287, 5288, 5289, 5290, 5291, 5292, 5293, 5294, 5295, 5296, 5297, 5298, 5299, 5300, 5301, 5302, 5303, 5304, 5305, 5306, 5307, 5308, 5309, 5310, 5311, 5312, 5313, 5314, 5315, 5316, 5317, 5318, 5319, 5320, 5321, 5322, 5323, 5324, 5325, 5326, 5327, 5328, 5329, 5330, 5331, 5332, 5333, 5334, 5335, 5336, 5337, 5338, 5339, 5340, 5341, 5342, 5343, 5344, 5345, 5346, 5347, 5348, 5349, 5350, 5351, 5352, 5353, 5354, 5355, 5356, 5357, 5358, 5359, 5360, 5361, 5362, 5363, 5364, 5365, 5366, 5367, 5368, 5369, 5370, 5371, 5372, 5373, 5374, 5375, 5376, 5377, 5378, 5379, 5380, 5381, 5382, 5383, 5384, 5385, 5386, 5387, 5388, 5389, 5390, 5391, 5392, 5393, 5394, 5395, 5396, 5397, 5398, 5399, 5400, 5401, 5402, 5403, 5404, 5405, 5406, 5407, 5408, 5409, 5410, 5411, 5412, 5413, 5414, 5415, 5416, 5417, 5418, 5419, 5420, 5421, 5422, 5423, 5424, 5425, 5426, 5427, 5428, 5429, 5430, 5431, 5432, 5433, 5434, 5435, 5436, 5437, 5438, 5439, 5440, 5441, 5442, 5443, 5444, 5445, 5446, 5447, 5448, 5449, 5450, 5451, 5452, 5453, 5454, 5455, 5456, 5457, 5458, 5459, 5460, 5461, 5462, 5463, 5464, 5465, 5466, 5467, 5468, 5469, 5470, 5471, 5472, 5473, 5474, 5475, 5476, 5477, 5478, 5479, 5480, 5481, 5482, 5483, 5484, 5485, 5486, 5487, 5488, 5489, 5490, 5491, 5492, 5493, 5494, 5495, 5496, 5497, 5498, 5499, 5500, 5501, 5502, 5503, 5504, 5505, 5506, 5507, 5508, 5509, 5510, 5511, 5512, 5513, 5514, 5515, 5516, 5517, 5518, 5519, 5520, 5521, 5522, 5523, 5524, 5525, 5526, 5527, 5528, 5529, 5530, 5531, 5532, 5533, 5534, 5535, 5536, 5537, 5538, 5539, 5540, 5541, 5542, 5543, 5544, 5545, 5546, 5547, 5548, 5549, 5550, 5551, 5552, 5553, 5554, 5555, 5556, 5557, 5558, 5559, 5560, 5561, 5562, 5563, 5564, 5565, 5566, 5567, 5568, 5569, 5570, 5571, 5572, 5573, 5574, 5575, 5576, 5577, 5578, 5579, 5580, 5581, 5582, 5583, 5584, 5585, 5586, 5587, 5588, 5589, 5590, 5591, 5592, 5593, 5594, 5595, 5596, 5597, 5598, 5599, 5600, 5601, 5602, 5603, 5604, 5605, 5606, 5607, 5608, 5609, 5610, 5611, 5612, 5613, 5614, 5615, 5616, 5617, 5618, 5619, 5620, 5621, 5622, 5623, 5624, 5625, 5626, 5627, 5628, 5629, 5630, 5631, 5632, 5633, 5634, 5635, 5636, 5637, 5638, 5639, 5640, 5641, 5642, 5643, 5644, 5645, </t>
         </is>
       </c>
-      <c r="BV6" t="n">
+      <c r="CD6" t="n">
         <v>0.1814977973568282</v>
       </c>
-      <c r="BW6" t="inlineStr">
+      <c r="CE6" t="inlineStr">
         <is>
           <t>{'Numk': 35, 'KPar': 28, 'Bucket_index': 1000}</t>
         </is>
       </c>
-      <c r="BX6" t="n">
+      <c r="CF6" t="n">
         <v>376.6167106030043</v>
       </c>
-      <c r="BY6" t="inlineStr">
+      <c r="CG6" t="inlineStr">
         <is>
           <t>no</t>
         </is>
       </c>
-      <c r="BZ6" t="n">
-        <v>0</v>
-      </c>
-      <c r="CA6" t="inlineStr">
+      <c r="CH6" t="n">
+        <v>0</v>
+      </c>
+      <c r="CI6" t="inlineStr">
         <is>
           <t>params</t>
         </is>
       </c>
-      <c r="CB6" t="n">
+      <c r="CJ6" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2312,93 +2472,117 @@
       <c r="BE7" t="n">
         <v>5</v>
       </c>
-      <c r="BF7" t="inlineStr"/>
-      <c r="BG7" t="inlineStr">
+      <c r="BF7" t="n">
+        <v>5</v>
+      </c>
+      <c r="BG7" t="n">
+        <v>5</v>
+      </c>
+      <c r="BH7" t="n">
+        <v>5</v>
+      </c>
+      <c r="BI7" t="n">
+        <v>5</v>
+      </c>
+      <c r="BJ7" t="n">
+        <v>5</v>
+      </c>
+      <c r="BK7" t="n">
+        <v>5</v>
+      </c>
+      <c r="BL7" t="n">
+        <v>5</v>
+      </c>
+      <c r="BM7" t="n">
+        <v>5</v>
+      </c>
+      <c r="BN7" t="inlineStr"/>
+      <c r="BO7" t="inlineStr">
         <is>
           <t>nab-data/realKnownCause/rogue_agent_key_hold.csv</t>
         </is>
       </c>
-      <c r="BH7" t="n">
+      <c r="BP7" t="n">
         <v>1882</v>
       </c>
-      <c r="BI7" t="inlineStr">
+      <c r="BQ7" t="inlineStr">
         <is>
           <t>NAB</t>
         </is>
       </c>
-      <c r="BJ7" t="n">
-        <v>2</v>
-      </c>
-      <c r="BK7" t="inlineStr">
+      <c r="BR7" t="n">
+        <v>2</v>
+      </c>
+      <c r="BS7" t="inlineStr">
         <is>
           <t>669; 1240</t>
         </is>
       </c>
-      <c r="BL7" t="n">
+      <c r="BT7" t="n">
         <v>94</v>
       </c>
-      <c r="BM7" t="inlineStr">
-        <is>
-          <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86, 87, 88, 89, 90, 91, 92, 93, 94, 95, 96, 97, 98, 99, 100, 101, 102, 103, 104, 105, 106, 107, 108, 109, 110, 111, 112, 113, 114, 115, 116, 117, 118, 119, 120, 121, 122, 123, 124, 125, 126, 127, 128, 129, 130, 131, 132, 133, 134, 135, 136, 137, 138, 139, 140, 141, 142, 143, 144, 145, 146, 147, 148, 149, 150, 151, 152, 153, 154, 155, 156, 157, 158, 159, 160, 161, 162, 163, 164, 165, 166, 167, 168, 169, 170, 171, 172, 173, 174, 175, 176, 177, 178, 179, 180, 181, 182, 183, 184, 185, 186, 187, 188, 189, 190, 191, 192, 193, 194, 195, 196, 197, 198, 199, 200, 201, 202, 203, 204, 205, 206, 207, 208, 209, 210, 211, 212, 213, 214, 215, 216, 217, 218, 219, 220, 221, 222, 223, 224, 225, 226, 227, 228, 229, 230, 231, 232, 233, 234, 235, 236, 237, 238, 239, 240, 241, 242, 243, 244, 245, 246, 247, 248, 249, 250, 251, 252, 253, 254, 255, 256, 257, 258, 259, 260, 261, 262, 263, 264, 265, 266, 267, 268, 269, 270, 271, 272, 273, 274, 275, 276, 277, 278, 279, 280, 281, 282, 283, 284, 285, 286, 287, 288, 289, 290, 291, 292, 293, 294, 295, 296, 297, 298, 299, 300, 301, 302, 303, 304, 305, 306, 307, 308, 309, 310, 311, 312, 313, 314, 315, 316, 317, 318, 319, 320, 321, 322, 323, 324, 325, 326, 327, 328, 329, 330, 331, 332, 333, 334, 335, 336, 337, 338, 339, 340, 341, 342, 343, 344, 345, 346, 347, 348, 349, 350, 351, 352, 353, 354, 355, 356, 357, 358, 359, 360, 361, 362, 363, 364, 365, 366, 367, 368, 369, 370, 371, 372, 373, 374, 375, 376, 377, 378, 379, 380, 381, 382, 383, 384, 385, 386, 387, 388, 389, 390, 391, 392, 393, 394, 395, 396, 397, 398, 399, 400, 401, 402, 403, 404, 405, 406, 407, 408, 409, 410, 411, 412, 413, 414, 415, 416, 417, 418, 419, 420, 421, 422, 423, 424, 425, 426, 427, 428, 429, 430, 431, 432, 433, 434, 435, 436, 437, 438, 439, 440, 441, 442, 443, 444, 445, 446, 447, 448, 449, 450, 451, 452, 453, 454, 455, 456, 457, 458, 459, 460, 461, 462, 463, 464, 465, 466, 467, 468, 469, 470, 471, 472, 473, 474, 475, 476, 477, 478, 479, 480, 481, 482, 483, 484, 485, 486, 487, 488, 489, 490, 491, 492, 493, 494, 495, 496, 497, 498, 499, 500, 501, 502, 503, 504, 505, 506, 507, 508, 509, 510, 511, 512, 513, 514, 515, 516, 517, 518, 519, 520, 521, 522, 523, 524, 525, 526, 527, 528, 529, 530, 531, 532, 533, 534, 535, 536, 537, 538, 539, 540, 541, 542, 543, 544, 545, 546, 547, 548, 549, 550, 551, 552, 553, 554, 555, 556, 557, 558, 559, 560, 561, 562, 563, 564, 565, 566, 567, 568, 569, 570, 571, 572, 573, 574, 575, 576, 577, 578, 579, 580, 581, 582, 583, 584, 585, 586, 587, 588, 589, 590, 591, 592, 593, 594, 595, 596, 597, 598, 599, 600, 601, 602, 603, 604, 605, 606, 607, 608, 609, 610, 611, 612, 613, 614, 615, 616, 617, 618, 619, 620, 621, 622, 623, 624, 625, 626, 627, 628, 629, 630, 631, 632, 633, 634, 635, 636, 637, 638, 639, 640, 641, 642, 643, 644, 645, 646, 647, 648, 649, 650, 651, 652, 653, 654, 655, 656, 657, 658, 659, 660, 661, 662, 663, 664, 665, 666, 667, 668, 669, 670, 671, 672, 673, 674, 675, 676, 677, 678, 679, 680, 681, 682, 683, 684, 685, 686, 687, 688, 689, 690, 691, 692, 693, 694, 695, 696, 697, 698, 699, 700, 701, 702, 703, 704, 705, 706, 707, 708, 709, 710, 711, 712, 713, 714, 715, 716, 717, 718, 719, 720, 721, 722, 723, 724, 725, 726, 727, 728, 729, 730, 731, 732, 733, 734, 735, 736, 737, 738, 739, 740, 741, 742, 743, 744, 745, 746, 747, 748, 749, 750, 751, 752, 753, 754, 755, 756, 757, 758, 759, 760, 761, 762, 763, 764, 765, 766, 767, 768, 769, 770, 771, 772, 773, 774, 775, 776, 777, 778, 779, 780, 781, 782, 783, 784, 785, 786, 787, 788, 789, 790, 791, 792, 793, 794, 795, 796, 797, 798, 799, 800, 801, 802, 803, 804, 805, 806, 807, 808, 809, 810, 811, 812, 813, 814, 815, 816, 817, 818, 819, 820, 821, 822, 823, 824, 825, 826, 827, 828, 829, 830, 831, 832, 833, 834, 835, 836, 837, 838, 839, 840, 841, 842, 843, 844, 845, 846, 847, 848, 849, 850, 851, 852, 853, 854, 855, 856, 857, 858, 859, 860, 861, 862, 863, 864, 865, 866, 867, 868, 869, 870, 871, 872, 873, 874, 875, 876, 877, 878, 879, 880, 881, 882, 883, 884, 885, 886, 887, 888, 889, 890, 891, 892, 893, 894, 895, 896, 897, 898, 899, 900, 901, 902, 903, 904, 905, 906, 907, 908, 909, 910, 911, 912, 913, 914, 915, 916, 917, 918, 919, 920, 921, 922, 923, 924, 925, 926, 927, 928, 929, 930, 931, 932, 933, 934, 935, 936, 937, 938, 939, 940, 941, 942, 943, 944, 945, 946, 947, 948, 949, 950, 951, 952, 953, 954, 955, 956, 957, 958, 959, 960, 961, 962, 963, 964, 965, 966, 967, 968, 969, 970, 971, 972, 973, 974, 975, 976, 977, 978, 979, 980, 981, 982, 983, 984, 985, 986, 987, 988, 989, 990, 991, 992, 993, 994, 995, 996, 997, 998, 999, 1000, 1001, 1002, 1003, 1004, 1005, 1006, 1007, 1008, 1009, 1010, 1011, 1012, 1013, 1014, 1015, 1016, 1017, 1018, 1019, 1020, 1021, 1022, 1023, 1024, 1025, 1026, 1027, 1028, 1029, 1030, 1031, 1032, 1033, 1034, 1035, 1036, 1037, 1038, 1039, 1040, 1041, 1042, 1043, 1044, 1045, 1046, 1047, 1048, 1049, 1050, 1051, 1052, 1053, 1054, 1055, 1056, 1057, 1058, 1059, 1060, 1061, 1062, 1063, 1064, 1065, 1066, 1067, 1068, 1069, 1070, 1071, 1072, 1073, 1074, 1075, 1076, 1077, 1078, 1079, 1080, 1081, 1082, 1083, 1084, 1085, 1086, 1087, 1088, 1089, 1090, 1091, 1092, 1093, 1094, 1095, 1096, 1097, 1098, 1099, 1100, 1101, 1102, 1103, 1104, 1105, 1106, 1107, 1108, 1109, 1110, 1111, 1112, 1113, 1114, 1115, 1116, 1117, 1118, 1119, 1120, 1121, 1122, 1123, 1124, 1125, 1126, 1127, 1128, 1129, 1130, 1131, 1132, 1133, 1134, 1135, 1136, 1137, 1138, 1139, 1140, 1141, 1142, 1143, 1144, 1145, 1146, 1147, 1148, 1149, 1150, 1151, 1152, 1153, 1154, 1155, 1156, 1157, 1158, 1159, 1160, 1161, 1162, 1163, 1164, 1165, 1166, 1167, 1168, 1169, 1170, 1171, 1172, 1173, 1174, 1175, 1176, 1177, 1178, 1179, 1180, 1181, 1182, 1183, 1184, 1185, 1186, 1187, 1188, 1189, 1190, 1191, 1192, 1193, 1194, 1195, 1196, 1197, 1198, 1199, 1200, 1201, 1202, 1203, 1204, 1205, 1206, 1207, 1208, 1209, 1210, 1211, 1212, 1213, 1214, 1215, 1216, 1217, 1218, 1219, 1220, 1221, 1222, 1223, 1224, 1225, 1226, 1227, 1228, 1229, 1230, 1231, 1232, 1233, 1234, 1235, 1236, 1237, 1238, 1239, 1240, 1241, 1242, 1243, 1244, 1245, 1246, 1247, 1248, 1249, 1250, 1251, 1252, 1253, 1254, 1255, 1256, 1257, 1258, 1259, 1260, 1261, 1262, 1263, 1264, 1265, 1266, 1267, 1268, 1269, 1270, 1271, 1272, 1273, 1274, 1275, 1276, 1277, 1278, 1279, 1280, 1281, 1282, 1283, 1284, 1285, 1286, 1287, 1288, 1289, 1290, 1291, 1292, 1293, 1294, 1295, 1296, 1297, 1298, 1299, 1300, 1303, 1313, 1314, 1317, 1318, 1319, 1320, 1321, 1322, 1323, 1324, 1325, 1326, 1327, 1328, 1329, 1330, 1336, 1337, 1343, 1344, 1345, 1386, 1387, 1388, 1389, 1390, 1391, 1392, 1393, 1394, 1395, 1396, 1397, 1398, 1399, 1400, 1401, 1402, 1403, 1404, 1405, 1406, 1407, 1408, 1409, 1410, 1411, 1412, 1413, 1414, 1415, 1416, 1417, 1418, 1419, 1420, 1421, 1422, 1423, 1424, 1425, 1426, 1427, 1428, 1429, 1430, 1432, 1433, 1434, 1435, 1436, 1440, 1441, 1444, 1449, 1450, 1451, 1452, 1453, 1454, 1455, 1456, 1457, 1459, 1460, 1461, 1463, 1464, 1465, 1466, 1467, 1468, 1469, 1470, 1471, 1472, 1473, 1474, 1475, 1476, 1477, 1478, 1481, 1482, 1483, 1484, 1485, 1486, 1487, 1488, 1489, 1490, 1491, 1492, 1493, 1494, 1495, 1496, 1497, 1498, 1499, 1500, 1501, 1502, 1503, 1504, 1505, 1506, 1507, 1508, 1509, 1510, 1511, 1512, 1513, 1514, 1517, 1518, 1519, 1520, 1521, 1522, 1523, 1524, 1525, 1526, 1527, 1528, 1529, 1530, 1531, 1532, 1533, 1534, 1535, 1536, 1541, 1542, 1543, 1550, 1551, 1553, 1554, 1555, 1556, 1557, 1558, 1559, 1560, 1561, 1562, 1563, 1564, 1565, 1566, 1567, 1568, 1569, 1570, 1572, 1573, 1574, 1575, 1576, 1577, 1578, 1579, 1580, 1581, 1582, 1583, 1584, 1585, 1586, 1587, 1588, 1589, 1590, 1591, 1592, 1602, 1603, 1605, 1606, 1607, 1608, 1609, 1610, 1611, 1612, 1613, 1614, 1615, 1616, 1617, 1618, 1619, 1620, 1621, 1622, 1623, 1624, 1625, 1626, 1627, 1628, 1629, 1630, 1631, 1632, 1633, 1634, 1635, 1636, 1637, 1638, 1639, 1640, 1641, 1642, 1643, 1645, 1646, 1647, 1648, 1649, 1650, 1651, 1652, 1653, 1654, 1655, 1656, 1657, 1658, 1660, 1661, 1662, 1663, 1664, 1665, 1666, 1667, 1668, 1669, 1670, 1671, 1672, 1673, 1674, 1675, 1676, 1677, 1678, 1679, 1680, 1681, 1682, 1685, 1686, 1687, 1688, 1689, 1690, 1691, 1693, 1695, 1696, 1698, 1702, 1703, 1708, 1709, 1710, 1711, 1713, 1714, 1715, 1716, 1717, 1718, 1719, 1720, 1723, 1724, 1735, 1736, 1737, 1738, 1739, 1740, 1741, 1742, 1743, 1744, 1745, 1746, 1747, 1748, 1749, 1750, 1751, 1752, 1753, 1754, 1755, 1756, 1757, 1758, 1759, 1760, 1761, 1762, 1763, 1764, 1765, 1766, 1767, 1768, 1769, 1770, 1771, 1772, 1773, 1774, 1775, 1776, 1777, 1778, 1779, 1780, 1781, 1782, 1783, 1784, 1785, 1786, 1787, 1788, 1789, 1790, 1791, 1792, 1793, 1794, 1795, 1796, 1797, 1798, 1799, 1800, 1801, 1802, 1803, 1804, 1805, 1806, 1807, 1808, 1809, 1810, 1811, 1812, 1813, 1814, 1815, 1816, 1817, 1818, 1819, 1820, 1821, 1822, 1823, 1824, 1825, 1826, 1827, 1828, 1829, 1830, 1831, 1832, 1833, 1834, 1835, 1836, 1837, 1838, 1839, 1840, 1841, 1842, 1843, 1844, 1845, 1846, 1847, 1848, 1849, 1850, 1851, 1852, 1853, 1854, 1855, 1856, 1857, 1858, 1859, 1860, 1861, 1862, 1863, 1864, 1865, 1866, 1867, 1868, 1869, 1870, 1871, 1872, 1873, 1874, 1875, 1876, 1877, 1878, 1879, 1880, 1881]</t>
-        </is>
-      </c>
-      <c r="BN7" t="n">
-        <v>0.07569939659901262</v>
-      </c>
-      <c r="BO7" t="inlineStr">
-        <is>
-          <t>{'initial_window': 276, 'window_size': 434, 'num_trees': 19, 'max_depth': 14}</t>
-        </is>
-      </c>
-      <c r="BP7" t="n">
-        <v>10.44551553297788</v>
-      </c>
-      <c r="BQ7" t="inlineStr">
+      <c r="BU7" t="inlineStr">
+        <is>
+          <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86, 87, 88, 89, 90, 91, 92, 93, 94, 95, 96, 97, 98, 99, 100, 101, 102, 103, 104, 105, 106, 107, 108, 109, 110, 111, 112, 113, 114, 115, 116, 117, 118, 119, 120, 121, 122, 123, 124, 125, 126, 127, 128, 129, 130, 131, 132, 133, 134, 135, 136, 137, 138, 139, 140, 141, 142, 143, 144, 145, 146, 147, 148, 149, 150, 151, 152, 153, 154, 155, 156, 157, 158, 159, 160, 161, 162, 163, 164, 165, 166, 167, 168, 169, 170, 171, 172, 173, 174, 175, 176, 177, 178, 179, 180, 181, 182, 183, 184, 185, 186, 187, 188, 189, 190, 191, 192, 193, 194, 195, 196, 197, 198, 199, 200, 201, 202, 203, 204, 205, 206, 207, 208, 209, 210, 211, 212, 213, 214, 215, 216, 217, 218, 219, 220, 221, 222, 223, 224, 225, 226, 227, 228, 229, 230, 231, 232, 233, 234, 235, 236, 237, 238, 239, 240, 241, 242, 243, 244, 245, 246, 247, 248, 249, 250, 251, 252, 253, 254, 255, 256, 257, 258, 259, 260, 261, 262, 263, 264, 265, 266, 267, 268, 269, 270, 271, 272, 273, 274, 275, 276, 277, 278, 279, 280, 281, 282, 283, 284, 285, 286, 287, 288, 289, 290, 291, 292, 293, 294, 295, 296, 297, 298, 299, 300, 301, 302, 303, 304, 305, 306, 307, 308, 309, 310, 311, 312, 313, 314, 315, 316, 317, 318, 319, 320, 321, 322, 323, 324, 325, 326, 327, 328, 329, 330, 331, 332, 333, 334, 335, 336, 337, 338, 339, 340, 341, 342, 343, 344, 345, 346, 347, 348, 349, 350, 351, 352, 353, 354, 355, 356, 357, 358, 359, 360, 361, 362, 363, 364, 365, 366, 367, 368, 369, 370, 371, 372, 373, 374, 375, 376, 377, 378, 379, 380, 381, 382, 383, 384, 385, 386, 387, 388, 389, 390, 391, 392, 393, 394, 395, 396, 397, 398, 399, 400, 401, 402, 403, 404, 405, 406, 407, 408, 409, 410, 411, 412, 413, 414, 415, 416, 417, 418, 419, 420, 421, 422, 423, 424, 425, 426, 427, 428, 429, 430, 431, 432, 433, 434, 435, 436, 437, 438, 439, 440, 441, 442, 443, 444, 445, 446, 447, 448, 449, 450, 451, 452, 453, 454, 455, 456, 457, 458, 459, 460, 461, 462, 463, 464, 465, 466, 467, 468, 469, 470, 471, 472, 473, 474, 475, 476, 477, 478, 479, 480, 481, 482, 483, 484, 485, 486, 487, 488, 489, 490, 491, 492, 493, 494, 495, 496, 497, 498, 499, 500, 501, 502, 503, 504, 505, 506, 507, 508, 509, 510, 511, 512, 513, 514, 515, 516, 517, 518, 519, 520, 521, 522, 523, 524, 525, 526, 527, 528, 529, 530, 531, 532, 533, 534, 535, 536, 537, 538, 539, 540, 541, 542, 543, 544, 545, 546, 547, 548, 549, 550, 551, 552, 553, 554, 555, 556, 557, 558, 559, 560, 561, 562, 563, 564, 565, 566, 567, 568, 569, 570, 571, 572, 573, 574, 575, 576, 577, 578, 579, 580, 581, 582, 583, 584, 585, 586, 587, 588, 589, 590, 591, 592, 593, 594, 595, 596, 597, 598, 599, 600, 601, 602, 603, 604, 605, 606, 607, 608, 609, 610, 611, 612, 613, 614, 615, 616, 617, 618, 619, 620, 621, 622, 623, 624, 625, 626, 627, 628, 629, 630, 631, 632, 633, 634, 635, 636, 637, 638, 639, 640, 641, 642, 643, 644, 645, 646, 647, 648, 649, 650, 651, 652, 653, 654, 655, 656, 657, 658, 659, 660, 661, 662, 663, 664, 665, 666, 667, 668, 669, 670, 671, 672, 673, 674, 675, 676, 677, 678, 679, 680, 681, 682, 683, 684, 685, 686, 687, 688, 689, 690, 691, 692, 693, 694, 695, 696, 697, 698, 699, 700, 701, 702, 703, 704, 705, 706, 707, 708, 709, 710, 711, 712, 713, 714, 715, 716, 717, 718, 719, 720, 721, 722, 723, 724, 725, 726, 727, 728, 729, 730, 731, 732, 733, 734, 735, 736, 737, 738, 739, 740, 741, 742, 743, 744, 745, 746, 747, 748, 749, 750, 751, 752, 753, 754, 755, 756, 757, 758, 759, 760, 761, 762, 763, 764, 765, 766, 767, 768, 769, 770, 771, 772, 773, 774, 775, 776, 777, 778, 779, 780, 781, 782, 783, 784, 785, 786, 787, 788, 789, 790, 791, 792, 793, 794, 795, 796, 797, 798, 799, 800, 801, 802, 803, 804, 805, 806, 807, 808, 809, 810, 811, 812, 813, 814, 815, 816, 817, 818, 819, 820, 821, 822, 823, 824, 825, 826, 827, 828, 829, 830, 831, 832, 833, 834, 835, 836, 837, 838, 839, 840, 841, 842, 843, 844, 845, 846, 847, 848, 849, 850, 851, 852, 853, 854, 855, 856, 857, 858, 859, 860, 861, 862, 863, 864, 865, 866, 867, 868, 869, 870, 871, 872, 873, 874, 875, 876, 877, 878, 879, 880, 881, 882, 883, 884, 885, 886, 887, 888, 889, 890, 891, 892, 893, 894, 895, 896, 897, 898, 899, 900, 901, 902, 903, 904, 905, 906, 907, 908, 909, 910, 911, 912, 913, 914, 915, 916, 917, 918, 919, 920, 921, 922, 923, 924, 925, 926, 927, 928, 929, 930, 931, 932, 933, 934, 935, 936, 937, 938, 939, 940, 941, 942, 943, 944, 945, 946, 947, 948, 949, 950, 951, 952, 953, 954, 955, 956, 957, 958, 959, 960, 961, 962, 963, 964, 965, 966, 967, 968, 969, 970, 971, 972, 973, 974, 975, 976, 977, 978, 979, 980, 981, 982, 983, 984, 985, 986, 987, 988, 989, 990, 991, 992, 993, 994, 995, 996, 997, 998, 999, 1000, 1001, 1002, 1003, 1004, 1005, 1006, 1007, 1008, 1009, 1010, 1011, 1012, 1013, 1014, 1015, 1016, 1017, 1018, 1019, 1020, 1021, 1022, 1023, 1024, 1025, 1026, 1027, 1028, 1029, 1030, 1031, 1032, 1033, 1034, 1035, 1036, 1037, 1038, 1039, 1040, 1041, 1042, 1043, 1044, 1045, 1046, 1047, 1048, 1049, 1050, 1051, 1052, 1053, 1054, 1055, 1056, 1057, 1058, 1059, 1060, 1061, 1062, 1063, 1064, 1065, 1066, 1067, 1068, 1069, 1070, 1071, 1072, 1073, 1074, 1075, 1076, 1077, 1078, 1079, 1080, 1081, 1082, 1083, 1084, 1085, 1086, 1087, 1088, 1089, 1090, 1091, 1092, 1093, 1094, 1095, 1096, 1097, 1098, 1099, 1100, 1101, 1102, 1103, 1104, 1105, 1106, 1107, 1108, 1109, 1110, 1111, 1112, 1113, 1114, 1115, 1116, 1117, 1118, 1119, 1120, 1121, 1122, 1123, 1124, 1125, 1126, 1127, 1128, 1129, 1130, 1131, 1132, 1133, 1134, 1135, 1136, 1137, 1138, 1139, 1140, 1141, 1142, 1143, 1144, 1145, 1146, 1147, 1148, 1149, 1150, 1151, 1152, 1153, 1154, 1155, 1156, 1157, 1158, 1159, 1160, 1161, 1162, 1163, 1164, 1165, 1166, 1167, 1168, 1169, 1170, 1171, 1172, 1173, 1174, 1175, 1176, 1177, 1178, 1179, 1180, 1181, 1182, 1183, 1184, 1185, 1186, 1187, 1188, 1189, 1190, 1191, 1192, 1193, 1194, 1195, 1196, 1197, 1198, 1199, 1200, 1201, 1202, 1203, 1204, 1205, 1206, 1207, 1208, 1209, 1210, 1211, 1212, 1213, 1214, 1215, 1216, 1217, 1218, 1219, 1220, 1221, 1222, 1223, 1224, 1225, 1226, 1227, 1228, 1229, 1230, 1231, 1232, 1233, 1234, 1235, 1236, 1237, 1238, 1239, 1240, 1241, 1242, 1243, 1244, 1245, 1246, 1247, 1248, 1249, 1250, 1251, 1252, 1253, 1254, 1255, 1256, 1257, 1258, 1259, 1260, 1261, 1262, 1263, 1264, 1265, 1266, 1267, 1268, 1269, 1270, 1271, 1272, 1273, 1274, 1275, 1276, 1277, 1278, 1279, 1280, 1281, 1282, 1283, 1284, 1285, 1286, 1287, 1288, 1289, 1290, 1291, 1292, 1293, 1294, 1295, 1296, 1297, 1298, 1299, 1300, 1301, 1302, 1303, 1304, 1305, 1306, 1307, 1308, 1309, 1310, 1311, 1312, 1313, 1314, 1315, 1316, 1317, 1318, 1319, 1320, 1321, 1322, 1323, 1324, 1325, 1326, 1327, 1328, 1329, 1330, 1331, 1332, 1333, 1334, 1335, 1336, 1337, 1338, 1339, 1340, 1341, 1342, 1343, 1344, 1345, 1346, 1347, 1348, 1349, 1350, 1351, 1352, 1353, 1354, 1355, 1356, 1357, 1358, 1359, 1360, 1361, 1362, 1363, 1364, 1365, 1366, 1367, 1368, 1369, 1370, 1371, 1372, 1373, 1374, 1375, 1376, 1377, 1378, 1379, 1380, 1381, 1382, 1383, 1384, 1385, 1386, 1387, 1388, 1389, 1390, 1391, 1392, 1393, 1394, 1395, 1396, 1397, 1398, 1399, 1400, 1401, 1402, 1403, 1404, 1405, 1406, 1407, 1408, 1409, 1410, 1411, 1412, 1413, 1414, 1415, 1416, 1417, 1418, 1419, 1420, 1421, 1422, 1423, 1424, 1425, 1426, 1427, 1428, 1429, 1430, 1431, 1432, 1433, 1434, 1435, 1436, 1437, 1438, 1439, 1440, 1441, 1442, 1443, 1444, 1445, 1446, 1447, 1448, 1449, 1450, 1451, 1452, 1453, 1454, 1455, 1456, 1457, 1458, 1459, 1460, 1461, 1462, 1463, 1464, 1465, 1466, 1467, 1468, 1469, 1470, 1471, 1472, 1473, 1474, 1475, 1476, 1477, 1478, 1479, 1480, 1481, 1482, 1483, 1484, 1485, 1486, 1487, 1488, 1489, 1490, 1491, 1492, 1493, 1494, 1495, 1496, 1497, 1498, 1499, 1500, 1501, 1502, 1503, 1504, 1505, 1506, 1507, 1508, 1509, 1510, 1511, 1512, 1513, 1514, 1515, 1516, 1517, 1518, 1519, 1520, 1521, 1522, 1523, 1524, 1525, 1526, 1527, 1528, 1529, 1530, 1531, 1532, 1533, 1534, 1535, 1536, 1537, 1538, 1539, 1540, 1541, 1542, 1543, 1544, 1545, 1546, 1547, 1548, 1549, 1550, 1551, 1552, 1553, 1554, 1555, 1556, 1557, 1558, 1559, 1560, 1561, 1562, 1563, 1564, 1565, 1566, 1567, 1568, 1569, 1570, 1571, 1572, 1573, 1574, 1575, 1576, 1577, 1578, 1579, 1580, 1581, 1582, 1583, 1584, 1585, 1586, 1587, 1588, 1589, 1590, 1591, 1592, 1593, 1594, 1595, 1596, 1597, 1598, 1599, 1600, 1601, 1602, 1603, 1604, 1605, 1606, 1607, 1608, 1609, 1610, 1611, 1612, 1613, 1614, 1615, 1616, 1617, 1618, 1619, 1620, 1621, 1622, 1623, 1624, 1625, 1626, 1627, 1628, 1629, 1630, 1631, 1632, 1633, 1634, 1635, 1636, 1637, 1638, 1639, 1640, 1641, 1642, 1643, 1644, 1645, 1646, 1647, 1648, 1649, 1650, 1651, 1652, 1653, 1654, 1655, 1656, 1657, 1658, 1659, 1660, 1661, 1662, 1663, 1664, 1665, 1666, 1667, 1668, 1669, 1670, 1671, 1672, 1673, 1674, 1675, 1676, 1677, 1678, 1679, 1680, 1681, 1682, 1683, 1684, 1685, 1686, 1687, 1688, 1689, 1690, 1691, 1692, 1693, 1694, 1695, 1696, 1697, 1698, 1699, 1700, 1701, 1702, 1703, 1704, 1705, 1706, 1707, 1708, 1709, 1710, 1711, 1712, 1713, 1714, 1715, 1716, 1717, 1718, 1719, 1720, 1721, 1722, 1723, 1724, 1725, 1726, 1727, 1728, 1729, 1730, 1731, 1732, 1733, 1734, 1735, 1736, 1737, 1738, 1739, 1740, 1741, 1742, 1743, 1744, 1745, 1746, 1747, 1748, 1749, 1750, 1751, 1752, 1753, 1754, 1755, 1756, 1757, 1758, 1759, 1760, 1761, 1762, 1763, 1764, 1765, 1766, 1767, 1768, 1769, 1770, 1771, 1772, 1773, 1774, 1775, 1776, 1777, 1778, 1779, 1780, 1781, 1782, 1783, 1784, 1785, 1786, 1787, 1788, 1789, 1790, 1791, 1792, 1793, 1794, 1795, 1796, 1797, 1798, 1799, 1800, 1801, 1802, 1803, 1804, 1805, 1806, 1807, 1808, 1809, 1810, 1811, 1812, 1813, 1814, 1815, 1816, 1817, 1818, 1819, 1820, 1821, 1822, 1823, 1824, 1825, 1826, 1827, 1828, 1829, 1830, 1831, 1832, 1833, 1834, 1835, 1836, 1837, 1838, 1839, 1840, 1841, 1842, 1843, 1844, 1845, 1846, 1847, 1848, 1849, 1850, 1851, 1852, 1853, 1854, 1855, 1856, 1857, 1858, 1859, 1860, 1861, 1862, 1863, 1864, 1865, 1866, 1867, 1868, 1869, 1870, 1871, 1872, 1873, 1874, 1875, 1876, 1877, 1878, 1879, 1880, 1881]</t>
+        </is>
+      </c>
+      <c r="BV7" t="n">
+        <v>0.07369498464687819</v>
+      </c>
+      <c r="BW7" t="inlineStr">
+        <is>
+          <t>{'initial_window': 139, 'window_size': 200, 'num_trees': 15, 'max_depth': 10}</t>
+        </is>
+      </c>
+      <c r="BX7" t="n">
+        <v>1.330645655001717</v>
+      </c>
+      <c r="BY7" t="inlineStr">
         <is>
           <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 60, 61, 64, 65, 66, 67, 68, 69, 70, 71, 79, 80, 84, 85, 86, 89, 90, 91, 92, 93, 94, 97, 98, 99, 100, 101, 102, 108, 112, 113, 114, 115, 116, 123, 124, 125, 126, 130, 133, 138, 139, 140, 141, 142, 149, 150, 151, 152, 154, 155, 157, 158, 159, 162, 163, 167, 168, 170, 171, 174, 175, 185, 186, 187, 189, 190, 191, 195, 196, 199, 200, 201, 202, 203, 206, 210, 211, 212, 215, 216, 220, 221, 222, 223, 224, 226, 227, 228, 229, 232, 233, 234, 235, 247, 248, 249, 252, 253, 254, 255, 256, 257, 259, 262, 266, 267, 268, 269, 282, 283, 284, 285, 287, 288, 294, 295, 296, 298, 299, 304, 312, 314, 319, 325, 329, 330, 332, 333, 334, 341, 342, 347, 348, 353, 354, 355, 357, 358, 359, 360, 361, 362, 363, 364, 365, 366, 367, 368, 369, 370, 371, 372, 373, 374, 375, 376, 377, 382, 384, 385, 386, 387, 388, 389, 390, 391, 392, 393, 394, 395, 396, 397, 398, 399, 400, 401, 402, 403, 404, 405, 406, 407, 408, 409, 410, 411, 412, 413, 414, 415, 416, 417, 418, 419, 420, 421, 422, 423, 424, 425, 426, 427, 428, 429, 430, 431, 432, 433, 434, 435, 436, 437, 438, 439, 440, 441, 442, 443, 444, 445, 446, 447, 448, 449, 450, 451, 452, 453, 454, 455, 456, 457, 458, 459, 460, 461, 462, 463, 464, 465, 466, 467, 468, 469, 470, 471, 472, 479, 482, 487, 488, 489, 490, 492, 496, 502, 503, 504, 505, 507, 508, 509, 510, 511, 512, 513, 514, 515, 516, 520, 521, 527, 528, 529, 530, 531, 532, 536, 537, 538, 539, 542, 543, 544, 545, 547, 548, 551, 553, 554, 555, 560, 561, 562, 563, 564, 569, 570, 571, 573, 574, 575, 576, 577, 578, 579, 580, 581, 582, 587, 588, 589, 593, 594, 597, 601, 602, 603, 604, 605, 606, 607, 608, 609, 610, 611, 612, 614, 615, 616, 617, 623, 627, 628, 629, 633, 634, 635, 636, 637, 638, 639, 640, 641, 642, 643, 644, 645, 646, 647, 648, 649, 650, 651, 652, 653, 654, 655, 656, 657, 658, 659, 660, 661, 662, 663, 667, 668, 669, 670, 673, 675, 676, 677, 678, 679, 680, 681, 682, 683, 684, 685, 686, 687, 688, 689, 690, 691, 692, 693, 694, 695, 696, 697, 698, 699, 700, 701, 702, 703, 704, 705, 706, 707, 708, 709, 710, 711, 712, 713, 714, 715, 716, 717, 718, 719, 720, 721, 722, 723, 724, 725, 726, 727, 728, 729, 730, 731, 732, 733, 734, 735, 736, 737, 738, 739, 740, 741, 742, 743, 744, 745, 746, 747, 748, 749, 750, 751, 752, 753, 754, 755, 756, 757, 758, 759, 760, 761, 762, 763, 764, 765, 766, 767, 768, 769, 770, 771, 772, 773, 774, 775, 776, 777, 778, 779, 780, 781, 782, 790, 791, 792, 793, 796, 797, 798, 799, 801, 802, 806, 807, 808, 809, 810, 811, 813, 814, 816, 819, 822, 828, 829, 830, 835, 836, 837, 840, 842, 843, 844, 845, 849, 850, 851, 852, 853, 854, 855, 856, 857, 861, 865, 866, 867, 868, 871, 872, 875, 879, 880, 881, 884, 885, 886, 887, 888, 889, 892, 893, 894, 895, 896, 897, 898, 899, 900, 901, 902, 903, 904, 905, 906, 907, 908, 909, 910, 911, 912, 913, 914, 915, 916, 917, 918, 919, 920, 921, 922, 923, 924, 925, 926, 927, 928, 929, 930, 935, 936, 937, 938, 939, 940, 941, 942, 943, 944, 945, 946, 947, 948, 949, 950, 951, 952, 953, 954, 955, 956, 957, 958, 959, 960, 961, 962, 963, 964, 965, 966, 967, 968, 969, 970, 971, 972, 973, 974, 975, 976, 977, 978, 979, 980, 981, 982, 983, 984, 985, 986, 987, 988, 989, 990, 991, 992, 993, 994, 995, 996, 997, 998, 999, 1000, 1001, 1002, 1003, 1004, 1005, 1006, 1007, 1008, 1009, 1010, 1011, 1012, 1013, 1014, 1015, 1016, 1017, 1018, 1019, 1020, 1021, 1022, 1023, 1024, 1025, 1026, 1027, 1028, 1029, 1030, 1031, 1032, 1033, 1034, 1035, 1036, 1037, 1038, 1039, 1040, 1041, 1042, 1043, 1044, 1045, 1046, 1047, 1048, 1049, 1050, 1051, 1052, 1053, 1054, 1055, 1056, 1057, 1058, 1059, 1060, 1065, 1066, 1067, 1068, 1069, 1070, 1071, 1072, 1073, 1074, 1075, 1076, 1077, 1078, 1079, 1080, 1081, 1082, 1083, 1084, 1085, 1086, 1087, 1088, 1089, 1090, 1091, 1092, 1093, 1094, 1095, 1096, 1097, 1098, 1099, 1100, 1101, 1102, 1103, 1104, 1105, 1106, 1107, 1108, 1109, 1110, 1111, 1112, 1113, 1114, 1115, 1116, 1117, 1118, 1119, 1120, 1121, 1122, 1123, 1124, 1125, 1126, 1127, 1128, 1129, 1130, 1131, 1132, 1133, 1134, 1135, 1136, 1137, 1138, 1139, 1140, 1141, 1142, 1143, 1144, 1145, 1146, 1147, 1148, 1149, 1150, 1151, 1152, 1153, 1154, 1155, 1156, 1157, 1158, 1159, 1160, 1168, 1169, 1170, 1171, 1172, 1173, 1174, 1175, 1176, 1177, 1178, 1179, 1180, 1181, 1182, 1183, 1184, 1185, 1186, 1187, 1188, 1189, 1190, 1191, 1192, 1193, 1194, 1195, 1196, 1197, 1198, 1199, 1200, 1201, 1202, 1203, 1204, 1205, 1206, 1207, 1208, 1209, 1210, 1211, 1212, 1213, 1214, 1215, 1216, 1217, 1218, 1219, 1220, 1221, 1222, 1223, 1224, 1225, 1226, 1227, 1228, 1229, 1230, 1231, 1232, 1233, 1234, 1235, 1236, 1237, 1238, 1239, 1240, 1241, 1242, 1243, 1244, 1245, 1246, 1247, 1248, 1249, 1250, 1251, 1252, 1253, 1254, 1255, 1256, 1257, 1258, 1259, 1260, 1261, 1262, 1263, 1264, 1265, 1266, 1267, 1268, 1269, 1270, 1271, 1272, 1273, 1274, 1275, 1276, 1277, 1278, 1279, 1280, 1281, 1282, 1283, 1284, 1285, 1286, 1287, 1288, 1289, 1290, 1291, 1292, 1293, 1294, 1295, 1296, 1297, 1298, 1299, 1300, 1301, 1302, 1303, 1304, 1305, 1306, 1307, 1308, 1309, 1310, 1311, 1312, 1313, 1314, 1315, 1316, 1317, 1318, 1319, 1320, 1321, 1322, 1323, 1324, 1325, 1326, 1328, 1329, 1330, 1331, 1332, 1333, 1334, 1335, 1336, 1337, 1338, 1339, 1340, 1341, 1342, 1343, 1344, 1345, 1346, 1347, 1348, 1349, 1350, 1351, 1355, 1356, 1357, 1358, 1359, 1360, 1361, 1362, 1363, 1364, 1367, 1370, 1376, 1380, 1382, 1383, 1384, 1385, 1392, 1393, 1394, 1400, 1401, 1402, 1403, 1404, 1405, 1406, 1407, 1408, 1409, 1410, 1411, 1412, 1413, 1414, 1415, 1416, 1417, 1418, 1419, 1420, 1421, 1422, 1423, 1424, 1425, 1426, 1427, 1428, 1429, 1430, 1431, 1432, 1433, 1434, 1435, 1436, 1437, 1438, 1440, 1441, 1442, 1443, 1444, 1445, 1446, 1447, 1458, 1461, 1467, 1468, 1469, 1470, 1471, 1472, 1476, 1477, 1478, 1479, 1480, 1485, 1488, 1489, 1492, 1493, 1494, 1502, 1503, 1504, 1505, 1506, 1507, 1508, 1509, 1510, 1514, 1515, 1516, 1518, 1519, 1520, 1521, 1527, 1528, 1537, 1538, 1539, 1540, 1541, 1543, 1549, 1550, 1552, 1553, 1554, 1556, 1557, 1561, 1568, 1572, 1573, 1581, 1584, 1585, 1589, 1593, 1597, 1598, 1599, 1600, 1602, 1603, 1607, 1608, 1612, 1613, 1614, 1622, 1624, 1625, 1626, 1627, 1628, 1629, 1630, 1631, 1632, 1634, 1635, 1639, 1640, 1647, 1648, 1649, 1650, 1651, 1652, 1654, 1655, 1656, 1658, 1661, 1662, 1663, 1664, 1665, 1668, 1671, 1672, 1673, 1677, 1678, 1679, 1680, 1684, 1685, 1687, 1688, 1689, 1690, 1691, 1701, 1704, 1706, 1707, 1708, 1709, 1710, 1712, 1714, 1715, 1716, 1717, 1718, 1719, 1721, 1724, 1725, 1726, 1727, 1731, 1732, 1738, 1739, 1740, 1741, 1742, 1743, 1752, 1753, 1758, 1759, 1760, 1761, 1766, 1767, 1773, 1775, 1779, 1780, 1781, 1782, 1783, 1784, 1785, 1786, 1787, 1790, 1791, 1800, 1801, 1802, 1803, 1807, 1808, 1812, 1813, 1815, 1816, 1817, 1820, 1822, 1824, 1825, 1826, 1827, 1828, 1832, 1833, 1834, 1835, 1836, 1837, 1840, 1841, 1842, 1843, 1846, 1850, 1851, 1852, 1854, 1855, 1862, 1864, 1865, 1866, 1867, 1869, 1870, 1876, 1877, 1878, 1879, 1880, 1881]</t>
         </is>
       </c>
-      <c r="BR7" t="n">
+      <c r="BZ7" t="n">
         <v>0.1036717062634989</v>
       </c>
-      <c r="BS7" t="inlineStr">
+      <c r="CA7" t="inlineStr">
         <is>
           <t>{'AR_window_size': 53, 'differencing-order': 4}</t>
         </is>
       </c>
-      <c r="BT7" t="n">
+      <c r="CB7" t="n">
         <v>36.00591896218248</v>
       </c>
-      <c r="BU7" t="inlineStr">
+      <c r="CC7" t="inlineStr">
         <is>
           <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86, 87, 88, 89, 90, 91, 92, 93, 94, 95, 96, 97, 98, 99, 100, 101, 102, 103, 104, 105, 106, 107, 108, 109, 110, 111, 112, 113, 114, 115, 116, 117, 118, 119, 120, 121, 122, 123, 124, 125, 126, 127, 128, 129, 130, 131, 132, 133, 134, 135, 136, 137, 138, 139, 140, 141, 142, 143, 144, 145, 146, 147, 148, 149, 150, 151, 153, 154, 155, 156, 157, 158, 159, 160, 161, 162, 163, 164, 165, 166, 167, 168, 169, 170, 171, 172, 173, 174, 175, 176, 177, 178, 179, 180, 181, 182, 183, 184, 185, 186, 187, 188, 189, 190, 191, 192, 193, 194, 195, 196, 197, 198, 199, 200, 201, 202, 203, 204, 205, 206, 207, 208, 209, 210, 211, 212, 213, 214, 215, 216, 217, 218, 219, 220, 221, 222, 223, 224, 225, 226, 227, 228, 229, 230, 231, 232, 233, 234, 235, 236, 237, 238, 239, 240, 241, 242, 243, 244, 246, 247, 248, 249, 250, 251, 252, 253, 254, 255, 256, 257, 258, 259, 260, 261, 262, 263, 264, 265, 267, 268, 269, 270, 271, 272, 273, 274, 275, 276, 277, 278, 279, 280, 281, 282, 283, 284, 285, 286, 287, 288, 289, 290, 291, 292, 293, 294, 295, 296, 297, 298, 299, 300, 301, 302, 303, 304, 305, 306, 307, 308, 309, 310, 311, 312, 313, 314, 315, 316, 317, 318, 319, 320, 321, 322, 323, 324, 325, 326, 327, 328, 329, 330, 331, 332, 333, 334, 335, 336, 337, 338, 339, 340, 341, 342, 343, 344, 345, 346, 347, 348, 349, 350, 351, 352, 353, 354, 355, 356, 357, 358, 359, 360, 361, 362, 363, 364, 365, 366, 367, 368, 369, 370, 371, 372, 373, 374, 375, 376, 377, 378, 379, 380, 381, 382, 383, 384, 385, 386, 387, 388, 389, 390, 391, 392, 393, 394, 395, 396, 397, 398, 399, 400, 401, 402, 403, 404, 405, 406, 407, 408, 409, 410, 411, 412, 413, 414, 415, 416, 417, 418, 419, 420, 421, 422, 423, 424, 425, 426, 427, 428, 429, 430, 431, 433, 434, 435, 436, 437, 438, 439, 440, 441, 442, 443, 444, 445, 446, 447, 448, 449, 450, 451, 452, 453, 454, 455, 456, 457, 458, 459, 460, 461, 462, 463, 464, 465, 466, 467, 468, 469, 470, 471, 472, 473, 474, 475, 476, 477, 478, 479, 480, 481, 482, 483, 484, 485, 486, 487, 488, 489, 490, 491, 492, 493, 494, 495, 496, 497, 498, 499, 500, 501, 502, 503, 504, 505, 506, 507, 508, 509, 510, 511, 512, 513, 514, 515, 516, 517, 518, 519, 520, 521, 522, 523, 524, 525, 526, 527, 528, 529, 530, 531, 532, 533, 534, 535, 536, 537, 538, 539, 540, 541, 542, 543, 544, 545, 546, 547, 548, 549, 550, 551, 552, 553, 554, 555, 556, 557, 558, 559, 560, 561, 562, 563, 564, 565, 566, 567, 568, 569, 570, 571, 572, 573, 574, 575, 576, 577, 578, 579, 580, 581, 582, 583, 584, 585, 586, 587, 588, 589, 590, 591, 592, 593, 594, 595, 596, 597, 598, 599, 600, 601, 602, 603, 604, 605, 606, 607, 608, 609, 610, 611, 612, 613, 614, 615, 616, 617, 618, 619, 620, 621, 622, 623, 624, 625, 626, 627, 628, 629, 630, 631, 632, 633, 634, 635, 636, 637, 638, 639, 640, 641, 642, 643, 644, 645, 646, 647, 648, 649, 650, 651, 652, 653, 654, 655, 656, 657, 658, 659, 660, 661, 662, 663, 664, 665, 666, 667, 668, 669, 670, 671, 672, 673, 674, 675, 676, 677, 678, 679, 680, 681, 682, 683, 684, 685, 686, 687, 688, 689, 690, 691, 692, 693, 694, 695, 696, 697, 698, 699, 700, 701, 702, 703, 704, 705, 706, 707, 708, 709, 710, 711, 712, 713, 714, 715, 716, 717, 718, 719, 720, 721, 722, 723, 724, 725, 726, 727, 728, 729, 730, 731, 732, 733, 734, 735, 736, 737, 738, 739, 740, 741, 742, 743, 744, 745, 746, 747, 748, 749, 750, 751, 752, 753, 754, 755, 756, 757, 758, 759, 760, 761, 762, 763, 764, 765, 766, 767, 768, 769, 770, 771, 772, 773, 774, 775, 776, 777, 778, 779, 780, 781, 782, 783, 784, 785, 786, 787, 788, 789, 790, 791, 792, 793, 794, 795, 796, 797, 798, 799, 800, 801, 802, 803, 804, 805, 806, 807, 808, 809, 810, 811, 812, 813, 814, 815, 816, 817, 818, 819, 820, 821, 822, 823, 824, 825, 826, 827, 828, 829, 830, 831, 832, 833, 834, 835, 836, 837, 838, 839, 840, 841, 842, 843, 844, 845, 846, 847, 848, 849, 850, 851, 852, 853, 854, 855, 856, 857, 858, 859, 860, 861, 862, 863, 864, 865, 866, 867, 868, 869, 870, 871, 872, 873, 874, 875, 876, 877, 878, 879, 880, 881, 882, 883, 884, 885, 886, 887, 888, 889, 890, 891, 892, 893, 894, 895, 896, 897, 898, 899, 900, 901, 902, 903, 904, 905, 906, 907, 908, 909, 910, 911, 912, 913, 914, 915, 916, 917, 918, 919, 920, 921, 922, 923, 924, 925, 926, 927, 928, 929, 930, 931, 932, 933, 934, 935, 936, 937, 938, 939, 940, 941, 942, 943, 944, 945, 946, 947, 948, 949, 950, 951, 952, 953, 954, 955, 956, 957, 958, 959, 960, 961, 962, 963, 964, 965, 966, 967, 968, 969, 970, 971, 972, 973, 974, 975, 976, 977, 978, 979, 980, 981, 982, 983, 984, 985, 986, 987, 988, 989, 990, 991, 992, 993, 994, 995, 996, 997, 998, 999, 1000, 1001, 1002, 1003, 1004, 1005, 1006, 1007, 1008, 1009, 1010, 1011, 1012, 1013, 1014, 1015, 1016, 1017, 1018, 1019, 1020, 1021, 1022, 1023, 1024, 1025, 1026, 1027, 1028, 1029, 1030, 1031, 1032, 1033, 1034, 1035, 1036, 1037, 1038, 1039, 1040, 1041, 1042, 1043, 1044, 1045, 1046, 1047, 1048, 1049, 1050, 1051, 1052, 1053, 1054, 1055, 1056, 1057, 1058, 1059, 1060, 1061, 1062, 1063, 1064, 1065, 1066, 1067, 1068, 1069, 1070, 1071, 1072, 1073, 1074, 1075, 1076, 1077, 1078, 1079, 1080, 1081, 1082, 1083, 1084, 1085, 1086, 1087, 1088, 1089, 1090, 1091, 1092, 1093, 1094, 1095, 1096, 1097, 1098, 1099, 1100, 1101, 1102, 1103, 1104, 1105, 1106, 1107, 1108, 1109, 1110, 1111, 1112, 1113, 1114, 1115, 1116, 1117, 1118, 1119, 1120, 1121, 1122, 1123, 1124, 1125, 1126, 1127, 1128, 1129, 1130, 1131, 1132, 1133, 1134, 1135, 1136, 1137, 1138, 1139, 1140, 1141, 1142, 1143, 1144, 1145, 1146, 1147, 1148, 1149, 1150, 1151, 1152, 1153, 1154, 1155, 1156, 1157, 1158, 1159, 1160, 1161, 1162, 1163, 1164, 1165, 1166, 1167, 1168, 1169, 1170, 1171, 1172, 1173, 1174, 1175, 1176, 1177, 1178, 1179, 1180, 1181, 1182, 1183, 1184, 1185, 1186, 1187, 1188, 1189, 1190, 1191, 1192, 1193, 1194, 1195, 1196, 1197, 1198, 1199, 1200, 1201, 1202, 1203, 1204, 1205, 1206, 1207, 1208, 1209, 1210, 1211, 1212, 1213, 1214, 1215, 1216, 1217, 1218, 1219, 1220, 1221, 1222, 1223, 1224, 1225, 1226, 1227, 1228, 1229, 1230, 1231, 1232, 1233, 1234, 1235, 1236, 1237, 1238, 1239, 1240, 1241, 1242, 1243, 1244, 1245, 1246, 1247, 1248, 1249, 1250, 1251, 1252, 1253, 1254, 1255, 1256, 1257, 1258, 1259, 1260, 1261, 1262, 1263, 1264, 1265, 1266, 1267, 1268, 1269, 1270, 1271, 1272, 1273, 1274, 1275, 1276, 1277, 1278, 1279, 1280, 1281, 1282, 1283, 1284, 1285, 1286, 1287, 1288, 1289, 1290, 1291, 1292, 1293, 1294, 1295, 1296, 1297, 1298, 1299, 1300, 1301, 1302, 1303, 1304, 1305, 1306, 1307, 1308, 1309, 1310, 1311, 1312, 1313, 1314, 1315, 1316, 1317, 1318, 1319, 1321, 1322, 1323, 1331, 1332, 1333, 1334, 1335, 1336, 1337, 1338, 1339, 1340, 1341, 1342, 1343, 1344, 1345, 1346, 1347, 1348, 1349, 1350, 1351, 1352, 1353, 1354, 1355, 1356, 1357, 1358, 1359, 1360, 1361, 1362, 1363, 1364, 1365, 1366, 1367, 1368, 1369, 1370, 1371, 1372, 1373, 1374, 1375, 1376, 1377, 1378, 1379, 1380, 1381, 1382, 1383, 1384, 1385, 1386, 1387, 1388, 1389, 1390, 1391, 1392, 1393, 1394, 1395, 1396, 1397, 1398, 1399, 1400, 1401, 1402, 1403, 1404, 1405, 1406, 1407, 1408, 1409, 1410, 1411, 1412, 1413, 1414, 1415, 1416, 1417, 1418, 1419, 1420, 1421, 1422, 1423, 1424, 1425, 1426, 1427, 1428, 1429, 1430, 1431, 1432, 1433, 1434, 1435, 1436, 1437, 1438, 1439, 1440, 1441, 1442, 1443, 1444, 1445, 1446, 1447, 1448, 1449, 1450, 1451, 1452, 1453, 1454, 1455, 1456, 1457, 1458, 1459, 1460, 1461, 1462, 1463, 1464, 1465, 1466, 1467, 1468, 1469, 1470, 1471, 1472, 1473, 1474, 1475, 1476, 1477, 1478, 1479, 1480, 1481, 1482, 1483, 1484, 1485, 1486, 1487, 1488, 1489, 1490, 1491, 1492, 1493, 1494, 1495, 1496, 1497, 1498, 1499, 1500, 1501, 1502, 1503, 1504, 1505, 1506, 1507, 1508, 1509, 1510, 1511, 1512, 1513, 1514, 1515, 1516, 1517, 1518, 1519, 1520, 1521, 1522, 1523, 1524, 1525, 1526, 1527, 1528, 1529, 1530, 1531, 1532, 1533, 1534, 1535, 1536, 1537, 1538, 1539, 1540, 1541, 1542, 1543, 1544, 1545, 1546, 1547, 1548, 1549, 1550, 1551, 1552, 1553, 1554, 1555, 1556, 1557, 1558, 1559, 1560, 1561, 1562, 1563, 1564, 1565, 1566, 1567, 1568, 1570, 1571, 1572, 1573, 1574, 1575, 1576, 1577, 1578, 1579, 1580, 1581, 1582, 1583, 1584, 1585, 1586, 1587, 1588, 1589, 1590, 1591, 1592, 1593, 1594, 1595, 1596, 1597, 1598, 1599, 1600, 1601, 1602, 1603, 1604, 1605, 1606, 1607, 1608, 1609, 1610, 1611, 1612, 1613, 1614, 1615, 1616, 1617, 1618, 1619, 1620, 1621, 1623, 1624, 1625, 1626, 1627, 1628, 1629, 1630, 1631, 1632, 1633, 1634, 1635, 1636, 1637, 1638, 1639, 1640, 1641, 1642, 1643, 1644, 1645, 1646, 1648, 1649, 1650, 1651, 1652, 1653, 1654, 1655, 1656, 1658, 1659, 1660, 1661, 1662, 1663, 1664, 1665, 1666, 1667, 1668, 1669, 1670, 1671, 1672, 1673, 1674, 1675, 1676, 1677, 1678, 1679, 1680, 1681, 1682, 1683, 1684, 1685, 1686, 1687, 1688, 1689, 1690, 1691, 1692, 1693, 1694, 1695, 1696, 1697, 1698, 1699, 1700, 1701, 1702, 1703, 1704, 1705, 1706, 1707, 1708, 1709, 1710, 1711, 1712, 1713, 1714, 1715, 1716, 1717, 1718, 1719, 1720, 1721, 1722, 1723, 1724, 1725, 1726, 1727, 1728, 1729, 1730, 1731, 1732, 1733, 1734, 1735, 1736, 1737, 1738, 1739, 1740, 1741, 1742, 1743, 1744, 1745, 1746, 1747, 1748, 1749, 1750, 1751, 1752, 1753, 1754, 1755, 1756, 1757, 1758, 1759, 1760, 1761, 1762, 1763, 1764, 1765, 1766, 1767, 1768, 1769, 1770, 1771, 1772, 1773, 1774, 1775, 1776, 1777, 1778, 1779, 1780, 1782, 1783, 1784, 1785, 1786, 1787, 1788, 1789, 1790, 1791, 1792, 1793, 1794, 1795, 1796, 1797, 1798, 1799, 1800, 1801, 1802, 1803, 1804, 1805, 1806, 1807, 1808, 1809, 1810, 1811, 1812, 1813, 1814, 1815, 1816, 1817, 1818, 1819, 1820, 1821, 1822, 1823, 1824, 1825, 1826, 1827, 1828, 1829, 1830, 1831, 1832, 1833, 1834, 1835, 1836, 1837, 1838, 1839, 1840, 1841, 1842, 1843, 1844, 1845, 1846, 1847, 1848, 1849, 1850, 1851, 1852, 1853, 1855, 1856, 1857, 1858, 1859, 1860, 1861, 1862, 1863, 1864, 1865, 1866, 1867, 1868, 1869, 1870, 1871, 1872, 1873, 1874, 1875, 1876, 1877, 1878, 1879, 1880, 1881]</t>
         </is>
       </c>
-      <c r="BV7" t="n">
+      <c r="CD7" t="n">
         <v>0.07441860465116279</v>
       </c>
-      <c r="BW7" t="inlineStr">
+      <c r="CE7" t="inlineStr">
         <is>
           <t>{'Numk': 31, 'KPar': 27, 'Bucket_index': 906}</t>
         </is>
       </c>
-      <c r="BX7" t="n">
+      <c r="CF7" t="n">
         <v>28.91637435695156</v>
       </c>
-      <c r="BY7" t="inlineStr">
+      <c r="CG7" t="inlineStr">
         <is>
           <t>no</t>
         </is>
       </c>
-      <c r="BZ7" t="n">
-        <v>0</v>
-      </c>
-      <c r="CA7" t="inlineStr">
+      <c r="CH7" t="n">
+        <v>0</v>
+      </c>
+      <c r="CI7" t="inlineStr">
         <is>
           <t>params</t>
         </is>
       </c>
-      <c r="CB7" t="n">
+      <c r="CJ7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2574,93 +2758,117 @@
       <c r="BE8" t="n">
         <v>6</v>
       </c>
-      <c r="BF8" t="inlineStr"/>
-      <c r="BG8" t="inlineStr">
+      <c r="BF8" t="n">
+        <v>6</v>
+      </c>
+      <c r="BG8" t="n">
+        <v>6</v>
+      </c>
+      <c r="BH8" t="n">
+        <v>6</v>
+      </c>
+      <c r="BI8" t="n">
+        <v>6</v>
+      </c>
+      <c r="BJ8" t="n">
+        <v>6</v>
+      </c>
+      <c r="BK8" t="n">
+        <v>6</v>
+      </c>
+      <c r="BL8" t="n">
+        <v>6</v>
+      </c>
+      <c r="BM8" t="n">
+        <v>6</v>
+      </c>
+      <c r="BN8" t="inlineStr"/>
+      <c r="BO8" t="inlineStr">
         <is>
           <t>nab-data/realKnownCause/rogue_agent_key_updown.csv</t>
         </is>
       </c>
-      <c r="BH8" t="n">
+      <c r="BP8" t="n">
         <v>5315</v>
       </c>
-      <c r="BI8" t="inlineStr">
+      <c r="BQ8" t="inlineStr">
         <is>
           <t>NAB</t>
         </is>
       </c>
-      <c r="BJ8" t="n">
-        <v>2</v>
-      </c>
-      <c r="BK8" t="inlineStr">
+      <c r="BR8" t="n">
+        <v>2</v>
+      </c>
+      <c r="BS8" t="inlineStr">
         <is>
           <t>2243; 2877</t>
         </is>
       </c>
-      <c r="BL8" t="n">
+      <c r="BT8" t="n">
         <v>264</v>
       </c>
-      <c r="BM8" t="inlineStr">
-        <is>
-          <t>[0, 1, 2, 3, 8, 240, 244, 245, 246, 247, 248, 254, 258, 259, 262, 263, 264, 265, 266, 267, 268, 270, 271, 272, 288, 289, 292, 293, 294, 295, 296, 297, 298, 299, 300, 301, 302, 303, 304, 305, 306, 307, 309, 310, 311, 312, 315, 317, 319, 320, 321, 322, 323, 324, 325, 326, 331, 332, 334, 335, 337, 338, 342, 343, 344, 345, 347, 348, 349, 350, 351, 352, 528, 529, 530, 532, 533, 540, 542, 546, 547, 548, 549, 550, 551, 552, 553, 554, 556, 559, 561, 566, 567, 568, 569, 570, 571, 575, 582, 584, 585, 593, 596, 597, 599, 603, 605, 610, 612, 615, 813, 814, 815, 817, 819, 820, 824, 827, 828, 830, 834, 835, 837, 838, 840, 841, 842, 843, 852, 853, 856, 857, 862, 866, 868, 869, 875, 876, 877, 885, 886, 1142, 1143, 1145, 1146, 1148, 1149, 1153, 1154, 1157, 1159, 1160, 1162, 1164, 1166, 1169, 1170, 1172, 1174, 1175, 1176, 1178, 1180, 1181, 1182, 1184, 1185, 1186, 1187, 1194, 1373, 1378, 1379, 1380, 1384, 1393, 1394, 1399, 1401, 1402, 1404, 1406, 1409, 1419, 1421, 1422, 1424, 1426, 1428, 1429, 1430, 1431, 1432, 1433, 1434, 1435, 1436, 1438, 1439, 1440, 1443, 1444, 1447, 1449, 1457, 1458, 1459, 1460, 1461, 1464, 1465, 1466, 1467, 1468, 1470, 1471, 1472, 1473, 1474, 1477, 1478, 1479, 1480, 1481, 1553, 1554, 1555, 1556, 1557, 1558, 1559, 1560, 1561, 1562, 1563, 1564, 1565, 1566, 1567, 1568, 1569, 1570, 1571, 1572, 1573, 1574, 1575, 1576, 1577, 1578, 1579, 1580, 1581, 1582, 1583, 1584, 1585, 1586, 1587, 1588, 1589, 1590, 1591, 1592, 1593, 1594, 1595, 1596, 1597, 1598, 1599, 1600, 1601, 1602, 1603, 1604, 1605, 1606, 1607, 1608, 1609, 1610, 1611, 1612, 1613, 1614, 1615, 1616, 1617, 1618, 1619, 1620, 1621, 1622, 1623, 1624, 1625, 1626, 1627, 1628, 1629, 1630, 1631, 1632, 1633, 1634, 1635, 1636, 1637, 1638, 1639, 1640, 1641, 1642, 1643, 1644, 1645, 1646, 1647, 1648, 1649, 1650, 1651, 1652, 1653, 1654, 1655, 1656, 1657, 1658, 1659, 1660, 1661, 1662, 1663, 1664, 1665, 1666, 1667, 1668, 1669, 1670, 1671, 1672, 1673, 1674, 1675, 1676, 1677, 1678, 1679, 1680, 1681, 1682, 1683, 1684, 1685, 1686, 1687, 1688, 1689, 1690, 1691, 1692, 1693, 1694, 1695, 1696, 1697, 1698, 1699, 1700, 1701, 1702, 1703, 1704, 1705, 1706, 1707, 1708, 1709, 1710, 1711, 1712, 1713, 1714, 1715, 1716, 1717, 1718, 1719, 1720, 1721, 1722, 1723, 1724, 1725, 1726, 1727, 1728, 1729, 1730, 1731, 1732, 1733, 1734, 1735, 1736, 1737, 1738, 1739, 1740, 1741, 1742, 1743, 1744, 1745, 1746, 1747, 1748, 1749, 1750, 1751, 1752, 1753, 1754, 1755, 1756, 1757, 1758, 1759, 1760, 1761, 1762, 1763, 1764, 1765, 1766, 1767, 1768, 1769, 1770, 1771, 1772, 1773, 1774, 1775, 1776, 1777, 1778, 1779, 1780, 1781, 1782, 1783, 1784, 1785, 1786, 1787, 1788, 1789, 1790, 1791, 1792, 1793, 1794, 1795, 1796, 1797, 1798, 1799, 1800, 1801, 1802, 1803, 1804, 1805, 1806, 1807, 1808, 1809, 1810, 1811, 1812, 1813, 1814, 1815, 1816, 1817, 1818, 1819, 1820, 1821, 1822, 1823, 1824, 1825, 1826, 1827, 1828, 1829, 1830, 1831, 1832, 1833, 1834, 1835, 1836, 1837, 1838, 1839, 1840, 1841, 1842, 1843, 1844, 1845, 1846, 1847, 1848, 1849, 1850, 1851, 1852, 1853, 1854, 1855, 1856, 1857, 1858, 1859, 1860, 1861, 1862, 1863, 1864, 1865, 1866, 1867, 1868, 1869, 1870, 1871, 1872, 1873, 1874, 1875, 1876, 1877, 1878, 1879, 1880, 1881, 1882, 1883, 1884, 1885, 1886, 1887, 1888, 1889, 1890, 1891, 1892, 1893, 1894, 1895, 1896, 1897, 1898, 1899, 1900, 1901, 1902, 1903, 1904, 1905, 1906, 1907, 1908, 1909, 1910, 1911, 1912, 1913, 1914, 1915, 1916, 1917, 1918, 1919, 1920, 1921, 1922, 1923, 1924, 1925, 1926, 1927, 1928, 1929, 1930, 1931, 1932, 1933, 1934, 1935, 1936, 1937, 1938, 1939, 1940, 1941, 1942, 1943, 1944, 1945, 1946, 1947, 1948, 1949, 1950, 1951, 1952, 1953, 1954, 1955, 1956, 1957, 1958, 1959, 1960, 1961, 1962, 1963, 1964, 1965, 1966, 1967, 1968, 1969, 1970, 1971, 1972, 1973, 1974, 1975, 1976, 1977, 1978, 1979, 1980, 1981, 1982, 1983, 1984, 1985, 1986, 1987, 1988, 1989, 1990, 1991, 1992, 1993, 1994, 1995, 1996, 1997, 1998, 1999, 2000, 2001, 2002, 2003, 2004, 2005, 2006, 2007, 2008, 2009, 2010, 2011, 2012, 2013, 2014, 2015, 2016, 2017, 2018, 2019, 2020, 2021, 2022, 2023, 2024, 2025, 2026, 2027, 2028, 2029, 2030, 2031, 2032, 2033, 2034, 2035, 2036, 2037, 2038, 2039, 2040, 2041, 2042, 2043, 2044, 2045, 2046, 2047, 2048, 2049, 2050, 2051, 2052, 2053, 2054, 2055, 2056, 2057, 2058, 2059, 2060, 2061, 2062, 2063, 2064, 2065, 2066, 2067, 2068, 2069, 2070, 2071, 2072, 2073, 2074, 2075, 2076, 2077, 2078, 2079, 2080, 2081, 2082, 2083, 2084, 2085, 2086, 2087, 2088, 2089, 2090, 2091, 2092, 2093, 2094, 2095, 2096, 2097, 2098, 2099, 2100, 2101, 2102, 2103, 2104, 2105, 2106, 2107, 2108, 2109, 2110, 2111, 2112, 2113, 2114, 2115, 2116, 2117, 2118, 2119, 2120, 2121, 2122, 2123, 2124, 2125, 2126, 2127, 2128, 2129, 2130, 2131, 2132, 2133, 2134, 2135, 2136, 2137, 2138, 2139, 2140, 2141, 2142, 2143, 2144, 2145, 2146, 2147, 2148, 2149, 2150, 2151, 2152, 2153, 2154, 2155, 2156, 2157, 2158, 2159, 2160, 2161, 2162, 2163, 2164, 2165, 2166, 2167, 2168, 2169, 2170, 2171, 2172, 2173, 2174, 2175, 2176, 2177, 2178, 2179, 2180, 2181, 2182, 2183, 2184, 2185, 2186, 2187, 2188, 2189, 2190, 2191, 2192, 2193, 2194, 2195, 2196, 2197, 2198, 2199, 2200, 2201, 2202, 2203, 2204, 2205, 2206, 2207, 2208, 2209, 2210, 2211, 2212, 2213, 2214, 2215, 2216, 2217, 2218, 2219, 2220, 2221, 2222, 2223, 2224, 2225, 2226, 2227, 2228, 2229, 2230, 2231, 2232, 2233, 2234, 2235, 2236, 2237, 2238, 2239, 2240, 2241, 2242, 2243, 2244, 2245, 2246, 2247, 2248, 2249, 2250, 2251, 2252, 2253, 2254, 2255, 2256, 2257, 2258, 2259, 2260, 2261, 2262, 2263, 2264, 2265, 2266, 2267, 2268, 2269, 2270, 2271, 2272, 2273, 2274, 2275, 2276, 2277, 2278, 2279, 2280, 2281, 2282, 2283, 2284, 2285, 2286, 2287, 2288, 2289, 2290, 2291, 2292, 2293, 2294, 2295, 2296, 2297, 2298, 2299, 2300, 2301, 2302, 2303, 2304, 2305, 2306, 2307, 2308, 2309, 2310, 2311, 2312, 2313, 2314, 2315, 2316, 2317, 2318, 2319, 2320, 2321, 2322, 2323, 2324, 2325, 2326, 2327, 2328, 2329, 2448, 2455, 2456, 2457, 2458, 2463, 2464, 2465, 2466, 2470, 2471, 2476, 2481, 2484, 2487, 2491, 2493, 2500, 2503, 2508, 2509, 2510, 2511, 2512, 2513, 2514, 2515, 2516, 2517, 2518, 2519, 2520, 2521, 2522, 2523, 2524, 2525, 2526, 2539, 2546, 2548, 2550, 2551, 2552, 2553, 2555, 2556, 2557, 2558, 2559, 2560, 2568, 2842, 2844, 3053, 3054, 3057, 3101, 3274, 3294, 3295, 3834, 3835, 3836, 3837, 3838, 3839, 3841, 3842, 3843, 3846, 3847, 3848, 3851, 3852, 3853, 3854, 3855, 3856, 3857, 3858, 3859, 3860, 3861, 3862, 3863, 3866, 3870, 4191, 4195, 4196, 4197, 4198, 4215, 4367, 4368, 4370, 4372, 4373, 4374, 4381, 4383, 4384, 4386, 4387, 4388, 4389, 4390, 4391, 4398, 4399, 4400, 4401, 4407, 4410, 4411, 4414, 4415, 4416, 4417, 4420, 4421, 4422, 4423, 4425, 4428, 4429, 4431, 4432, 4433, 4434, 4435, 4436, 4437, 4442, 4444, 4446, 4447, 4448, 4449, 4450, 4453, 4458, 4461, 4467, 4479, 4480, 4481, 4482, 4483, 4486, 4487, 4488, 4489, 4491, 4492, 4493, 4719, 4722, 4723, 4724, 4726, 4727, 4729, 4730, 4731, 4732, 4733, 4734, 4735, 4736, 4737, 4740, 4741, 4753, 4754, 4758, 4760, 4761, 4762, 4764, 4767, 4768, 4769, 4770, 4771, 4772, 4773, 4775, 4777, 4779, 4780, 4781, 4782, 4783, 4784, 4786, 4787, 4788, 4791, 4792, 4797, 4799, 4800, 4801, 4802, 4803, 4804, 4805, 4806, 4807, 4809, 4811, 4812, 4813, 4814, 4815, 4816, 4818, 4833, 4834, 4835, 4836, 4837, 4838, 4839, 4844, 4845, 4846, 4850, 4853, 4990, 4991, 4992, 4993, 4996, 4997, 4998, 4999, 5000, 5002, 5037, 5038, 5039, 5040, 5041, 5043, 5044, 5045, 5048, 5051, 5053, 5054, 5055, 5056, 5057, 5062, 5063, 5064, 5067, 5068, 5069, 5070, 5071, 5072, 5074, 5076, 5077, 5079, 5080, 5081, 5083, 5084, 5085, 5086, 5088, 5089, 5090, 5092, 5094, 5097, 5098, 5099, 5101, 5104, 5105, 5109, 5146, 5147, 5152, 5153, 5154, 5155, 5260, 5262, 5263, 5264, 5265, 5266, 5267, 5268, 5269, 5271, 5272, 5273, 5274, 5276, 5277, 5278, 5279, 5280, 5281, 5283, 5284, 5286, 5287, 5288, 5289, 5290, 5292, 5304, 5305, 5306, 5307, 5308, 5309, 5310, 5312, 5313]</t>
-        </is>
-      </c>
-      <c r="BN8" t="n">
-        <v>0.1502086230876217</v>
-      </c>
-      <c r="BO8" t="inlineStr">
-        <is>
-          <t>{'initial_window': 279, 'window_size': 777, 'num_trees': 29, 'max_depth': 15}</t>
-        </is>
-      </c>
-      <c r="BP8" t="n">
-        <v>21.3299277019687</v>
-      </c>
-      <c r="BQ8" t="inlineStr">
+      <c r="BU8" t="inlineStr">
+        <is>
+          <t>[575, 593, 1148, 1170, 1172, 1380, 2466, 2508, 2515, 3053, 3101, 3274, 4197, 4198, 4400, 4425, 4807, 5146]</t>
+        </is>
+      </c>
+      <c r="BV8" t="n">
+        <v>0.09999999999999999</v>
+      </c>
+      <c r="BW8" t="inlineStr">
+        <is>
+          <t>{'initial_window': 599, 'window_size': 200, 'num_trees': 15, 'max_depth': 10}</t>
+        </is>
+      </c>
+      <c r="BX8" t="n">
+        <v>2.539222264000273</v>
+      </c>
+      <c r="BY8" t="inlineStr">
         <is>
           <t>[333, 334, 342, 348, 351, 382, 621, 633, 643, 647, 648, 652, 653, 659, 675, 676, 677, 687, 690, 1235, 1236, 1238, 1241, 1243, 1248, 1253, 1254, 1256, 1258, 1260, 1264, 1266, 1272, 1275, 1276, 1281, 1288, 1467, 1487, 1493, 1500, 1516, 1518, 1520, 1522, 1529, 1532, 1534, 1538, 1541, 1553, 1558, 1562, 1567, 1568, 1571, 1575, 1776, 2328, 2329, 2332, 2333, 2339, 2341, 2343, 2344, 2379, 2552, 2563, 2565, 2587, 2593, 2594, 2596, 2597, 2601, 2602, 2604, 2605, 2606, 2608, 2609, 2612, 2620, 2633, 2640, 2662, 2938, 3146, 3147, 3151, 3194, 3195, 3367, 3368, 3929, 3931, 3935, 3947, 4290, 4292, 4309, 4460, 4461, 4466, 4475, 4480, 4482, 4492, 4500, 4501, 4514, 4515, 4516, 4518, 4519, 4531, 4552, 4554, 4555, 4579, 4580, 4586, 4587, 4818, 4819, 4823, 4826, 4829, 4830, 4835, 4851, 4854, 4867, 4868, 4880, 4881, 4892, 4900, 4901, 4906, 4931, 4939, 4940, 4946, 4947, 5085, 5090, 5093, 5094, 5095, 5148, 5149, 5155, 5156, 5166, 5169, 5170, 5174, 5175, 5176, 5180, 5182, 5184, 5185, 5186, 5188, 5191, 5192, 5194, 5195, 5198, 5239, 5240, 5241]</t>
         </is>
       </c>
-      <c r="BR8" t="n">
+      <c r="BZ8" t="n">
         <v>0.09326424870466322</v>
       </c>
-      <c r="BS8" t="inlineStr">
+      <c r="CA8" t="inlineStr">
         <is>
           <t>{'AR_window_size': 93, 'differencing-order': 0}</t>
         </is>
       </c>
-      <c r="BT8" t="n">
+      <c r="CB8" t="n">
         <v>231.0503054440487</v>
       </c>
-      <c r="BU8" t="inlineStr">
+      <c r="CC8" t="inlineStr">
         <is>
           <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 78, 79, 80, 81, 82, 83, 84, 85, 86, 87, 88, 89, 90, 91, 92, 93, 94, 95, 96, 97, 98, 99, 100, 101, 102, 103, 104, 105, 106, 107, 108, 109, 110, 111, 112, 113, 114, 115, 116, 117, 118, 119, 120, 121, 122, 123, 124, 125, 126, 127, 128, 129, 130, 131, 132, 133, 134, 135, 136, 137, 138, 139, 140, 141, 142, 143, 144, 145, 146, 147, 148, 149, 150, 151, 152, 153, 154, 155, 156, 157, 158, 159, 160, 161, 162, 163, 164, 165, 166, 167, 168, 169, 170, 171, 172, 173, 174, 175, 176, 177, 178, 179, 180, 181, 182, 183, 184, 185, 186, 187, 188, 189, 190, 191, 192, 193, 194, 195, 196, 197, 198, 199, 200, 201, 202, 203, 204, 205, 206, 207, 208, 209, 210, 211, 212, 213, 214, 215, 216, 217, 218, 219, 220, 221, 222, 223, 224, 225, 226, 227, 228, 229, 230, 231, 232, 233, 234, 235, 236, 237, 238, 239, 240, 241, 242, 243, 244, 245, 246, 247, 248, 249, 250, 251, 252, 253, 254, 255, 256, 257, 258, 259, 260, 261, 262, 263, 264, 265, 266, 267, 268, 269, 270, 271, 272, 273, 274, 275, 276, 277, 278, 279, 280, 281, 282, 283, 284, 285, 286, 287, 288, 289, 290, 291, 292, 293, 294, 295, 296, 297, 298, 299, 300, 301, 302, 303, 304, 305, 306, 307, 308, 309, 310, 311, 312, 313, 314, 315, 316, 317, 318, 319, 320, 321, 322, 323, 324, 325, 326, 327, 328, 329, 330, 331, 332, 333, 334, 335, 336, 337, 338, 339, 340, 341, 342, 343, 344, 345, 346, 347, 348, 349, 350, 351, 352, 353, 354, 355, 356, 357, 358, 359, 360, 361, 362, 363, 364, 365, 366, 367, 368, 369, 370, 371, 372, 373, 374, 375, 376, 377, 378, 379, 380, 381, 382, 383, 384, 385, 386, 387, 388, 389, 390, 391, 392, 393, 394, 395, 396, 397, 398, 399, 400, 401, 402, 403, 404, 405, 406, 407, 408, 409, 410, 411, 412, 413, 414, 415, 416, 417, 418, 419, 420, 421, 422, 423, 424, 425, 426, 427, 428, 429, 430, 431, 432, 433, 434, 435, 436, 437, 438, 439, 440, 441, 442, 443, 444, 445, 446, 447, 448, 449, 450, 451, 452, 453, 454, 455, 456, 457, 458, 459, 460, 461, 462, 463, 464, 465, 466, 467, 468, 469, 470, 471, 472, 473, 474, 475, 476, 477, 478, 479, 480, 481, 482, 483, 484, 485, 486, 487, 488, 489, 490, 491, 492, 493, 494, 495, 496, 497, 498, 499, 500, 501, 502, 503, 504, 505, 506, 507, 508, 509, 510, 511, 512, 513, 514, 515, 516, 517, 518, 519, 520, 521, 522, 523, 524, 525, 526, 527, 528, 529, 530, 531, 532, 533, 534, 535, 536, 537, 538, 539, 540, 541, 542, 543, 544, 545, 546, 547, 548, 549, 550, 551, 552, 553, 554, 555, 556, 557, 558, 559, 560, 561, 562, 563, 564, 565, 566, 567, 568, 569, 570, 571, 572, 573, 574, 576, 577, 578, 579, 580, 581, 582, 583, 584, 585, 586, 587, 588, 589, 590, 591, 592, 594, 595, 596, 597, 598, 599, 600, 601, 602, 603, 604, 605, 606, 607, 608, 609, 610, 611, 612, 613, 614, 615, 616, 617, 618, 619, 620, 621, 622, 623, 624, 625, 626, 627, 628, 629, 630, 631, 632, 633, 634, 635, 636, 637, 638, 639, 640, 641, 642, 643, 644, 645, 646, 647, 648, 649, 650, 651, 652, 653, 654, 655, 656, 657, 658, 659, 660, 661, 662, 663, 664, 665, 666, 667, 668, 669, 670, 671, 672, 673, 674, 675, 676, 677, 678, 679, 680, 681, 682, 683, 684, 685, 686, 687, 688, 689, 690, 691, 692, 693, 694, 695, 696, 697, 698, 699, 700, 701, 702, 703, 704, 705, 706, 707, 708, 709, 710, 711, 712, 713, 714, 715, 716, 717, 718, 719, 720, 721, 722, 723, 724, 725, 726, 727, 728, 729, 730, 731, 732, 733, 734, 735, 736, 737, 738, 739, 740, 741, 742, 743, 744, 745, 746, 747, 748, 749, 750, 751, 752, 753, 754, 755, 756, 757, 758, 759, 760, 761, 762, 763, 764, 765, 766, 767, 768, 769, 770, 771, 772, 773, 774, 775, 776, 777, 778, 779, 780, 781, 782, 783, 784, 785, 786, 787, 788, 789, 790, 791, 792, 793, 794, 795, 796, 797, 798, 799, 800, 801, 802, 803, 804, 805, 806, 807, 808, 809, 810, 811, 812, 813, 814, 815, 816, 817, 818, 819, 820, 821, 822, 823, 824, 825, 826, 827, 828, 829, 830, 831, 832, 833, 834, 835, 836, 837, 838, 839, 840, 841, 842, 843, 844, 845, 846, 847, 848, 849, 850, 851, 852, 853, 854, 855, 856, 857, 858, 859, 860, 861, 862, 863, 864, 865, 866, 867, 868, 869, 870, 871, 872, 873, 874, 875, 876, 877, 878, 879, 880, 881, 882, 883, 884, 885, 886, 887, 888, 889, 890, 891, 892, 893, 894, 895, 896, 897, 898, 899, 900, 901, 902, 903, 904, 905, 906, 907, 908, 909, 910, 911, 912, 913, 914, 915, 916, 917, 918, 919, 920, 921, 922, 923, 924, 925, 926, 927, 928, 929, 930, 931, 932, 933, 934, 935, 936, 937, 938, 939, 940, 941, 942, 943, 944, 945, 946, 947, 948, 949, 950, 951, 952, 953, 954, 955, 956, 957, 958, 959, 960, 961, 962, 963, 964, 965, 966, 967, 968, 969, 970, 971, 972, 973, 974, 975, 976, 977, 978, 979, 980, 981, 982, 983, 984, 985, 986, 987, 988, 989, 990, 991, 992, 993, 994, 995, 996, 997, 998, 999, 1000, 1001, 1002, 1003, 1004, 1005, 1006, 1007, 1008, 1009, 1010, 1011, 1012, 1013, 1014, 1015, 1016, 1017, 1018, 1019, 1020, 1021, 1022, 1023, 1024, 1025, 1026, 1027, 1028, 1029, 1030, 1031, 1032, 1033, 1034, 1035, 1036, 1037, 1038, 1039, 1040, 1041, 1042, 1043, 1044, 1045, 1046, 1047, 1048, 1049, 1050, 1051, 1052, 1053, 1054, 1055, 1056, 1057, 1058, 1059, 1060, 1061, 1062, 1063, 1064, 1065, 1066, 1067, 1068, 1069, 1070, 1071, 1072, 1073, 1074, 1075, 1076, 1077, 1078, 1079, 1080, 1081, 1082, 1083, 1084, 1085, 1086, 1087, 1088, 1089, 1090, 1091, 1092, 1093, 1094, 1095, 1096, 1097, 1098, 1099, 1100, 1101, 1102, 1103, 1104, 1105, 1106, 1107, 1108, 1109, 1110, 1111, 1112, 1113, 1114, 1115, 1116, 1117, 1118, 1119, 1120, 1121, 1122, 1123, 1124, 1125, 1126, 1127, 1128, 1129, 1130, 1131, 1132, 1133, 1134, 1135, 1136, 1137, 1138, 1139, 1140, 1141, 1142, 1143, 1144, 1145, 1146, 1147, 1149, 1150, 1151, 1152, 1153, 1154, 1155, 1156, 1157, 1158, 1159, 1160, 1161, 1162, 1163, 1164, 1165, 1166, 1167, 1168, 1169, 1171, 1173, 1174, 1175, 1176, 1177, 1178, 1179, 1180, 1181, 1182, 1183, 1184, 1185, 1186, 1187, 1188, 1189, 1190, 1191, 1192, 1193, 1194, 1195, 1196, 1197, 1198, 1199, 1200, 1201, 1202, 1203, 1204, 1205, 1206, 1207, 1208, 1209, 1210, 1211, 1212, 1213, 1214, 1215, 1216, 1217, 1218, 1219, 1220, 1221, 1222, 1223, 1224, 1225, 1226, 1227, 1228, 1229, 1230, 1231, 1232, 1233, 1234, 1235, 1236, 1237, 1238, 1239, 1240, 1241, 1242, 1243, 1244, 1245, 1246, 1247, 1248, 1249, 1250, 1251, 1252, 1253, 1254, 1255, 1256, 1257, 1258, 1259, 1260, 1261, 1262, 1263, 1264, 1265, 1266, 1267, 1268, 1269, 1270, 1271, 1272, 1273, 1274, 1275, 1276, 1277, 1278, 1279, 1280, 1281, 1282, 1283, 1284, 1285, 1286, 1287, 1288, 1289, 1290, 1291, 1292, 1293, 1294, 1295, 1296, 1297, 1298, 1299, 1300, 1301, 1302, 1303, 1304, 1305, 1306, 1307, 1308, 1309, 1310, 1311, 1312, 1313, 1314, 1315, 1316, 1317, 1318, 1319, 1320, 1321, 1322, 1323, 1324, 1325, 1326, 1327, 1328, 1329, 1330, 1331, 1332, 1333, 1334, 1335, 1336, 1337, 1338, 1339, 1340, 1341, 1342, 1343, 1344, 1345, 1346, 1347, 1348, 1349, 1350, 1351, 1352, 1353, 1354, 1355, 1356, 1357, 1358, 1359, 1360, 1361, 1362, 1363, 1364, 1365, 1366, 1367, 1368, 1369, 1370, 1371, 1372, 1373, 1374, 1375, 1376, 1377, 1378, 1379, 1381, 1382, 1383, 1384, 1385, 1386, 1387, 1388, 1389, 1390, 1391, 1392, 1393, 1394, 1395, 1396, 1397, 1398, 1399, 1400, 1401, 1402, 1403, 1404, 1405, 1406, 1407, 1408, 1409, 1410, 1411, 1412, 1413, 1414, 1415, 1416, 1417, 1418, 1419, 1420, 1421, 1422, 1423, 1424, 1425, 1426, 1427, 1428, 1429, 1430, 1431, 1432, 1433, 1434, 1435, 1436, 1437, 1438, 1439, 1440, 1441, 1442, 1443, 1444, 1445, 1446, 1447, 1448, 1449, 1450, 1451, 1452, 1453, 1454, 1455, 1456, 1457, 1458, 1459, 1460, 1461, 1462, 1463, 1464, 1465, 1466, 1467, 1468, 1469, 1470, 1471, 1472, 1473, 1474, 1475, 1476, 1477, 1478, 1479, 1480, 1481, 1482, 1483, 1484, 1485, 1486, 1487, 1488, 1489, 1490, 1491, 1492, 1493, 1494, 1495, 1496, 1497, 1498, 1499, 1500, 1501, 1502, 1503, 1504, 1505, 1506, 1507, 1508, 1509, 1510, 1511, 1512, 1513, 1514, 1515, 1516, 1517, 1518, 1519, 1520, 1521, 1522, 1523, 1524, 1525, 1526, 1527, 1528, 1529, 1530, 1531, 1532, 1533, 1534, 1535, 1536, 1537, 1538, 1539, 1540, 1541, 1542, 1543, 1544, 1545, 1546, 1547, 1548, 1549, 1550, 1551, 1552, 1553, 1554, 1555, 1556, 1557, 1558, 1559, 1560, 1561, 1562, 1563, 1564, 1565, 1566, 1567, 1568, 1569, 1570, 1571, 1572, 1573, 1574, 1575, 1576, 1577, 1578, 1579, 1580, 1581, 1582, 1583, 1584, 1585, 1586, 1587, 1588, 1589, 1590, 1591, 1592, 1593, 1594, 1595, 1596, 1597, 1598, 1599, 1600, 1601, 1602, 1603, 1604, 1605, 1606, 1607, 1608, 1609, 1610, 1611, 1612, 1613, 1614, 1615, 1616, 1617, 1618, 1619, 1620, 1621, 1622, 1623, 1624, 1625, 1626, 1627, 1628, 1629, 1630, 1631, 1632, 1633, 1634, 1635, 1636, 1637, 1638, 1639, 1640, 1641, 1642, 1643, 1644, 1645, 1646, 1647, 1648, 1649, 1650, 1651, 1652, 1653, 1654, 1655, 1656, 1657, 1658, 1659, 1660, 1661, 1662, 1663, 1664, 1665, 1666, 1667, 1668, 1669, 1670, 1671, 1672, 1673, 1674, 1675, 1676, 1677, 1678, 1679, 1680, 1681, 1682, 1683, 1684, 1685, 1686, 1687, 1688, 1689, 1690, 1691, 1692, 1693, 1694, 1695, 1696, 1697, 1698, 1699, 1700, 1701, 1702, 1703, 1704, 1705, 1706, 1707, 1708, 1709, 1710, 1711, 1712, 1713, 1714, 1715, 1716, 1717, 1718, 1719, 1720, 1721, 1722, 1723, 1724, 1725, 1726, 1727, 1728, 1729, 1730, 1731, 1732, 1733, 1734, 1735, 1736, 1737, 1738, 1739, 1740, 1741, 1742, 1743, 1744, 1745, 1746, 1747, 1748, 1749, 1750, 1751, 1752, 1753, 1754, 1755, 1756, 1757, 1758, 1759, 1760, 1761, 1762, 1763, 1764, 1765, 1766, 1767, 1768, 1769, 1770, 1771, 1772, 1773, 1774, 1775, 1776, 1777, 1778, 1779, 1780, 1781, 1782, 1783, 1784, 1785, 1786, 1787, 1788, 1789, 1790, 1791, 1792, 1793, 1794, 1795, 1796, 1797, 1798, 1799, 1800, 1801, 1802, 1803, 1804, 1805, 1806, 1807, 1808, 1809, 1810, 1811, 1812, 1813, 1814, 1815, 1816, 1817, 1818, 1819, 1820, 1821, 1822, 1823, 1824, 1825, 1826, 1827, 1828, 1829, 1830, 1831, 1832, 1833, 1834, 1835, 1836, 1837, 1838, 1839, 1840, 1841, 1842, 1843, 1844, 1845, 1846, 1847, 1848, 1849, 1850, 1851, 1852, 1853, 1854, 1855, 1856, 1857, 1858, 1859, 1860, 1861, 1862, 1863, 1864, 1865, 1866, 1867, 1868, 1869, 1870, 1871, 1872, 1873, 1874, 1875, 1876, 1877, 1878, 1879, 1880, 1881, 1882, 1883, 1884, 1885, 1886, 1887, 1888, 1889, 1890, 1891, 1892, 1893, 1894, 1895, 1896, 1897, 1898, 1899, 1900, 1901, 1902, 1903, 1904, 1905, 1906, 1907, 1908, 1909, 1910, 1911, 1912, 1913, 1914, 1915, 1916, 1917, 1918, 1919, 1920, 1921, 1922, 1923, 1924, 1925, 1926, 1927, 1928, 1929, 1930, 1931, 1932, 1933, 1934, 1935, 1936, 1937, 1938, 1939, 1940, 1941, 1942, 1943, 1944, 1945, 1946, 1947, 1948, 1949, 1950, 1951, 1952, 1953, 1954, 1955, 1956, 1957, 1958, 1959, 1960, 1961, 1962, 1963, 1964, 1965, 1966, 1967, 1968, 1969, 1970, 1971, 1972, 1973, 1974, 1975, 1976, 1977, 1978, 1979, 1980, 1981, 1982, 1983, 1984, 1985, 1986, 1987, 1988, 1989, 1990, 1991, 1992, 1993, 1994, 1995, 1996, 1997, 1998, 1999, 2000, 2001, 2002, 2003, 2004, 2005, 2006, 2007, 2008, 2009, 2010, 2011, 2012, 2013, 2014, 2015, 2016, 2017, 2018, 2019, 2020, 2021, 2022, 2023, 2024, 2025, 2026, 2027, 2028, 2029, 2030, 2031, 2032, 2033, 2034, 2035, 2036, 2037, 2038, 2039, 2040, 2041, 2042, 2043, 2044, 2045, 2046, 2047, 2048, 2049, 2050, 2051, 2052, 2053, 2054, 2055, 2056, 2057, 2058, 2059, 2060, 2061, 2062, 2063, 2064, 2065, 2066, 2067, 2068, 2069, 2070, 2071, 2072, 2073, 2074, 2075, 2076, 2077, 2078, 2079, 2080, 2081, 2082, 2083, 2084, 2085, 2086, 2087, 2088, 2089, 2090, 2091, 2092, 2093, 2094, 2095, 2096, 2097, 2098, 2099, 2100, 2101, 2102, 2103, 2104, 2105, 2106, 2107, 2108, 2109, 2110, 2111, 2112, 2113, 2114, 2115, 2116, 2117, 2118, 2119, 2120, 2121, 2122, 2123, 2124, 2125, 2126, 2127, 2128, 2129, 2130, 2131, 2132, 2133, 2134, 2135, 2136, 2137, 2138, 2139, 2140, 2141, 2142, 2143, 2144, 2145, 2146, 2147, 2148, 2149, 2150, 2151, 2152, 2153, 2154, 2155, 2156, 2157, 2158, 2159, 2160, 2161, 2162, 2163, 2164, 2165, 2166, 2167, 2168, 2169, 2170, 2171, 2172, 2173, 2174, 2175, 2176, 2177, 2178, 2179, 2180, 2181, 2182, 2183, 2184, 2185, 2186, 2187, 2188, 2189, 2190, 2191, 2192, 2193, 2194, 2195, 2196, 2197, 2198, 2199, 2200, 2201, 2202, 2203, 2204, 2205, 2206, 2207, 2208, 2209, 2210, 2211, 2212, 2213, 2214, 2215, 2216, 2217, 2218, 2219, 2220, 2221, 2222, 2223, 2224, 2225, 2226, 2227, 2228, 2229, 2230, 2231, 2232, 2233, 2234, 2235, 2236, 2237, 2238, 2239, 2240, 2241, 2242, 2243, 2244, 2245, 2246, 2247, 2248, 2249, 2250, 2251, 2252, 2253, 2254, 2255, 2256, 2257, 2258, 2259, 2260, 2261, 2262, 2263, 2264, 2265, 2266, 2267, 2268, 2269, 2270, 2271, 2272, 2273, 2274, 2275, 2276, 2277, 2278, 2279, 2280, 2281, 2282, 2283, 2284, 2285, 2286, 2287, 2288, 2289, 2290, 2291, 2292, 2293, 2294, 2295, 2296, 2297, 2298, 2299, 2300, 2301, 2302, 2303, 2304, 2305, 2306, 2307, 2308, 2309, 2310, 2311, 2312, 2313, 2314, 2315, 2316, 2317, 2318, 2319, 2320, 2321, 2322, 2323, 2324, 2325, 2326, 2327, 2328, 2329, 2330, 2331, 2332, 2333, 2334, 2335, 2336, 2337, 2338, 2339, 2340, 2341, 2342, 2343, 2344, 2345, 2346, 2347, 2348, 2349, 2350, 2351, 2352, 2353, 2354, 2355, 2356, 2357, 2358, 2359, 2360, 2361, 2362, 2363, 2364, 2365, 2366, 2367, 2368, 2369, 2370, 2371, 2372, 2373, 2374, 2375, 2376, 2377, 2378, 2379, 2380, 2381, 2382, 2383, 2384, 2385, 2386, 2387, 2388, 2389, 2390, 2391, 2392, 2393, 2394, 2395, 2396, 2397, 2398, 2399, 2400, 2401, 2402, 2403, 2404, 2405, 2406, 2407, 2408, 2409, 2410, 2411, 2412, 2413, 2414, 2415, 2416, 2417, 2418, 2419, 2420, 2421, 2422, 2423, 2424, 2425, 2426, 2427, 2428, 2429, 2430, 2431, 2432, 2433, 2434, 2435, 2436, 2437, 2438, 2439, 2440, 2441, 2442, 2443, 2444, 2445, 2446, 2447, 2448, 2449, 2450, 2451, 2452, 2453, 2454, 2455, 2456, 2457, 2458, 2459, 2460, 2461, 2462, 2463, 2464, 2465, 2467, 2468, 2469, 2470, 2471, 2472, 2473, 2474, 2475, 2476, 2477, 2478, 2479, 2480, 2481, 2482, 2483, 2484, 2485, 2486, 2487, 2488, 2489, 2490, 2491, 2492, 2493, 2494, 2495, 2496, 2497, 2498, 2499, 2500, 2501, 2502, 2503, 2504, 2505, 2506, 2507, 2509, 2510, 2511, 2512, 2513, 2514, 2516, 2517, 2518, 2519, 2520, 2521, 2522, 2523, 2524, 2525, 2526, 2527, 2528, 2529, 2530, 2531, 2532, 2533, 2534, 2535, 2536, 2537, 2538, 2539, 2540, 2541, 2542, 2543, 2544, 2545, 2546, 2547, 2548, 2549, 2550, 2551, 2552, 2553, 2554, 2555, 2556, 2557, 2558, 2559, 2560, 2561, 2562, 2563, 2564, 2565, 2566, 2567, 2568, 2569, 2570, 2571, 2572, 2573, 2574, 2575, 2576, 2577, 2578, 2579, 2580, 2581, 2582, 2583, 2584, 2585, 2586, 2587, 2588, 2589, 2590, 2591, 2592, 2593, 2594, 2595, 2596, 2597, 2598, 2599, 2600, 2601, 2602, 2603, 2604, 2605, 2606, 2607, 2608, 2609, 2610, 2611, 2612, 2613, 2614, 2615, 2616, 2617, 2618, 2619, 2620, 2621, 2622, 2623, 2624, 2625, 2626, 2627, 2628, 2629, 2630, 2631, 2632, 2633, 2634, 2635, 2636, 2637, 2638, 2639, 2640, 2641, 2642, 2643, 2644, 2645, 2646, 2647, 2648, 2649, 2650, 2651, 2652, 2653, 2654, 2655, 2656, 2657, 2658, 2659, 2660, 2661, 2662, 2663, 2664, 2665, 2666, 2667, 2668, 2669, 2670, 2671, 2672, 2673, 2674, 2675, 2676, 2677, 2678, 2679, 2680, 2681, 2682, 2683, 2684, 2685, 2686, 2687, 2688, 2689, 2690, 2691, 2692, 2693, 2694, 2695, 2696, 2697, 2698, 2699, 2700, 2701, 2702, 2703, 2704, 2705, 2706, 2707, 2708, 2709, 2710, 2711, 2712, 2713, 2714, 2715, 2716, 2717, 2718, 2719, 2720, 2721, 2722, 2723, 2724, 2725, 2726, 2727, 2728, 2729, 2730, 2731, 2732, 2733, 2734, 2735, 2736, 2737, 2738, 2739, 2740, 2741, 2742, 2743, 2744, 2745, 2746, 2747, 2748, 2749, 2750, 2751, 2752, 2753, 2754, 2755, 2756, 2757, 2758, 2759, 2760, 2761, 2762, 2763, 2764, 2765, 2766, 2767, 2768, 2769, 2770, 2771, 2772, 2773, 2774, 2775, 2776, 2777, 2778, 2779, 2780, 2781, 2782, 2783, 2784, 2785, 2786, 2787, 2788, 2789, 2790, 2791, 2792, 2793, 2794, 2795, 2796, 2797, 2798, 2799, 2800, 2801, 2802, 2803, 2804, 2805, 2806, 2807, 2808, 2809, 2810, 2811, 2812, 2813, 2814, 2815, 2816, 2817, 2818, 2819, 2820, 2821, 2822, 2823, 2824, 2825, 2826, 2827, 2828, 2829, 2830, 2831, 2832, 2833, 2834, 2835, 2836, 2837, 2838, 2839, 2840, 2841, 2842, 2843, 2844, 2845, 2846, 2847, 2848, 2849, 2850, 2851, 2852, 2853, 2854, 2855, 2856, 2857, 2858, 2859, 2860, 2861, 2862, 2863, 2864, 2865, 2866, 2867, 2868, 2869, 2870, 2871, 2872, 2873, 2874, 2875, 2876, 2877, 2878, 2879, 2880, 2881, 2882, 2883, 2884, 2885, 2886, 2887, 2888, 2889, 2890, 2891, 2892, 2893, 2894, 2895, 2896, 2897, 2898, 2899, 2900, 2901, 2902, 2903, 2904, 2905, 2906, 2907, 2908, 2909, 2910, 2911, 2912, 2913, 2914, 2915, 2916, 2917, 2918, 2919, 2920, 2921, 2922, 2923, 2924, 2925, 2926, 2927, 2928, 2929, 2930, 2931, 2932, 2933, 2934, 2935, 2936, 2937, 2938, 2939, 2940, 2941, 2942, 2943, 2944, 2945, 2946, 2947, 2948, 2949, 2950, 2951, 2952, 2953, 2954, 2955, 2956, 2957, 2958, 2959, 2960, 2961, 2962, 2963, 2964, 2965, 2966, 2967, 2968, 2969, 2970, 2971, 2972, 2973, 2974, 2975, 2976, 2977, 2978, 2979, 2980, 2981, 2982, 2983, 2984, 2985, 2986, 2987, 2988, 2989, 2990, 2991, 2992, 2993, 2994, 2995, 2996, 2997, 2998, 2999, 3000, 3001, 3002, 3003, 3004, 3005, 3006, 3007, 3008, 3009, 3010, 3011, 3012, 3013, 3014, 3015, 3016, 3017, 3018, 3019, 3020, 3021, 3022, 3023, 3024, 3025, 3026, 3027, 3028, 3029, 3030, 3031, 3032, 3033, 3034, 3035, 3036, 3037, 3038, 3039, 3040, 3041, 3042, 3043, 3044, 3045, 3046, 3047, 3048, 3049, 3050, 3051, 3052, 3053, 3054, 3055, 3056, 3057, 3058, 3059, 3060, 3061, 3062, 3063, 3064, 3065, 3066, 3067, 3068, 3069, 3070, 3071, 3072, 3073, 3074, 3075, 3076, 3077, 3078, 3079, 3080, 3081, 3082, 3083, 3084, 3085, 3086, 3087, 3088, 3089, 3090, 3091, 3092, 3093, 3094, 3095, 3096, 3097, 3098, 3099, 3100, 3102, 3103, 3104, 3105, 3106, 3107, 3108, 3109, 3110, 3111, 3112, 3113, 3114, 3115, 3116, 3117, 3118, 3119, 3120, 3121, 3122, 3123, 3124, 3125, 3126, 3127, 3128, 3129, 3130, 3131, 3132, 3133, 3134, 3135, 3136, 3137, 3138, 3139, 3140, 3141, 3142, 3143, 3144, 3145, 3146, 3147, 3148, 3149, 3150, 3151, 3152, 3153, 3154, 3155, 3156, 3157, 3158, 3159, 3160, 3161, 3162, 3163, 3164, 3165, 3166, 3167, 3168, 3169, 3170, 3171, 3172, 3173, 3174, 3175, 3176, 3177, 3178, 3179, 3180, 3181, 3182, 3183, 3184, 3185, 3186, 3187, 3188, 3189, 3190, 3191, 3192, 3193, 3194, 3195, 3196, 3197, 3198, 3199, 3200, 3201, 3202, 3203, 3204, 3205, 3206, 3207, 3208, 3209, 3210, 3211, 3212, 3213, 3214, 3215, 3216, 3217, 3218, 3219, 3220, 3221, 3222, 3223, 3224, 3225, 3226, 3227, 3228, 3229, 3230, 3231, 3232, 3233, 3234, 3235, 3236, 3237, 3238, 3239, 3240, 3241, 3242, 3243, 3244, 3245, 3246, 3247, 3248, 3249, 3250, 3251, 3252, 3253, 3254, 3255, 3256, 3257, 3258, 3259, 3260, 3261, 3262, 3263, 3264, 3265, 3266, 3267, 3268, 3269, 3270, 3271, 3272, 3273, 3275, 3276, 3277, 3278, 3279, 3280, 3281, 3282, 3283, 3284, 3285, 3286, 3287, 3288, 3289, 3290, 3291, 3292, 3293, 3294, 3295, 3296, 3297, 3298, 3299, 3300, 3301, 3302, 3303, 3304, 3305, 3306, 3307, 3308, 3309, 3310, 3311, 3312, 3313, 3314, 3315, 3316, 3317, 3318, 3319, 3320, 3321, 3322, 3323, 3324, 3325, 3326, 3327, 3328, 3329, 3330, 3331, 3332, 3333, 3334, 3335, 3336, 3337, 3338, 3339, 3340, 3341, 3342, 3343, 3344, 3345, 3346, 3347, 3348, 3349, 3350, 3351, 3352, 3353, 3354, 3355, 3356, 3357, 3358, 3359, 3360, 3361, 3362, 3363, 3364, 3365, 3366, 3367, 3368, 3369, 3370, 3371, 3372, 3373, 3374, 3375, 3376, 3377, 3378, 3379, 3380, 3381, 3382, 3383, 3384, 3385, 3386, 3387, 3388, 3389, 3390, 3391, 3392, 3393, 3394, 3395, 3396, 3397, 3398, 3399, 3400, 3401, 3402, 3403, 3404, 3405, 3406, 3407, 3408, 3409, 3410, 3411, 3412, 3413, 3414, 3415, 3416, 3417, 3418, 3419, 3420, 3421, 3422, 3423, 3424, 3425, 3426, 3427, 3428, 3429, 3430, 3431, 3432, 3433, 3434, 3435, 3436, 3437, 3438, 3439, 3440, 3441, 3442, 3443, 3444, 3445, 3446, 3447, 3448, 3449, 3450, 3451, 3452, 3453, 3454, 3455, 3456, 3457, 3458, 3459, 3460, 3461, 3462, 3463, 3464, 3465, 3466, 3467, 3468, 3469, 3470, 3471, 3472, 3473, 3474, 3475, 3476, 3477, 3478, 3479, 3480, 3481, 3482, 3483, 3484, 3485, 3486, 3487, 3488, 3489, 3490, 3491, 3492, 3493, 3494, 3495, 3496, 3497, 3498, 3499, 3500, 3501, 3502, 3503, 3504, 3505, 3506, 3507, 3508, 3509, 3510, 3511, 3512, 3513, 3514, 3515, 3516, 3517, 3518, 3519, 3520, 3521, 3522, 3523, 3524, 3525, 3526, 3527, 3528, 3529, 3530, 3531, 3532, 3533, 3534, 3535, 3536, 3537, 3538, 3539, 3540, 3541, 3542, 3543, 3544, 3545, 3546, 3547, 3548, 3549, 3550, 3551, 3552, 3553, 3554, 3555, 3556, 3557, 3558, 3559, 3560, 3561, 3562, 3563, 3564, 3565, 3566, 3567, 3568, 3569, 3570, 3571, 3572, 3573, 3574, 3575, 3576, 3577, 3578, 3579, 3580, 3581, 3582, 3583, 3584, 3585, 3586, 3587, 3588, 3589, 3590, 3591, 3592, 3593, 3594, 3595, 3596, 3597, 3598, 3599, 3600, 3601, 3602, 3603, 3604, 3605, 3606, 3607, 3608, 3609, 3610, 3611, 3612, 3613, 3614, 3615, 3616, 3617, 3618, 3619, 3620, 3621, 3622, 3623, 3624, 3625, 3626, 3627, 3628, 3629, 3630, 3631, 3632, 3633, 3634, 3635, 3636, 3637, 3638, 3639, 3640, 3641, 3642, 3643, 3644, 3645, 3646, 3647, 3648, 3649, 3650, 3651, 3652, 3653, 3654, 3655, 3656, 3657, 3658, 3659, 3660, 3661, 3662, 3663, 3664, 3665, 3666, 3667, 3668, 3669, 3670, 3671, 3672, 3673, 3674, 3675, 3676, 3677, 3678, 3679, 3680, 3681, 3682, 3683, 3684, 3685, 3686, 3687, 3688, 3689, 3690, 3691, 3692, 3693, 3694, 3695, 3696, 3697, 3698, 3699, 3700, 3701, 3702, 3703, 3704, 3705, 3706, 3707, 3708, 3709, 3710, 3711, 3712, 3713, 3714, 3715, 3716, 3717, 3718, 3719, 3720, 3721, 3722, 3723, 3724, 3725, 3726, 3727, 3728, 3729, 3730, 3731, 3732, 3733, 3734, 3735, 3736, 3737, 3738, 3739, 3740, 3741, 3742, 3743, 3744, 3745, 3746, 3747, 3748, 3749, 3750, 3751, 3752, 3753, 3754, 3755, 3756, 3757, 3758, 3759, 3760, 3761, 3762, 3763, 3764, 3765, 3766, 3767, 3768, 3769, 3770, 3771, 3772, 3773, 3774, 3775, 3776, 3777, 3778, 3779, 3780, 3781, 3782, 3783, 3784, 3785, 3786, 3787, 3788, 3789, 3790, 3791, 3792, 3793, 3794, 3795, 3796, 3797, 3798, 3799, 3800, 3801, 3802, 3803, 3804, 3805, 3806, 3807, 3808, 3809, 3810, 3811, 3812, 3813, 3814, 3815, 3816, 3817, 3818, 3819, 3820, 3821, 3822, 3823, 3824, 3825, 3826, 3827, 3828, 3829, 3830, 3831, 3832, 3833, 3834, 3835, 3836, 3837, 3838, 3839, 3840, 3841, 3842, 3843, 3844, 3845, 3846, 3847, 3848, 3849, 3850, 3851, 3852, 3853, 3854, 3855, 3856, 3857, 3858, 3859, 3860, 3861, 3862, 3863, 3864, 3865, 3866, 3867, 3868, 3869, 3870, 3871, 3872, 3873, 3874, 3875, 3876, 3877, 3878, 3879, 3880, 3881, 3882, 3883, 3884, 3885, 3886, 3887, 3888, 3889, 3890, 3891, 3892, 3893, 3894, 3895, 3896, 3897, 3898, 3899, 3900, 3901, 3902, 3903, 3904, 3905, 3906, 3907, 3908, 3909, 3910, 3911, 3912, 3913, 3914, 3915, 3916, 3917, 3918, 3919, 3920, 3921, 3922, 3923, 3924, 3925, 3926, 3927, 3928, 3929, 3930, 3931, 3932, 3933, 3934, 3935, 3936, 3937, 3938, 3939, 3940, 3941, 3942, 3943, 3944, 3945, 3946, 3947, 3948, 3949, 3950, 3951, 3952, 3953, 3954, 3955, 3956, 3957, 3958, 3959, 3960, 3961, 3962, 3963, 3964, 3965, 3966, 3967, 3968, 3969, 3970, 3971, 3972, 3973, 3974, 3975, 3976, 3977, 3978, 3979, 3980, 3981, 3982, 3983, 3984, 3985, 3986, 3987, 3988, 3989, 3990, 3991, 3992, 3993, 3994, 3995, 3996, 3997, 3998, 3999, 4000, 4001, 4002, 4003, 4004, 4005, 4006, 4007, 4008, 4009, 4010, 4011, 4012, 4013, 4014, 4015, 4016, 4017, 4018, 4019, 4020, 4021, 4022, 4023, 4024, 4025, 4026, 4027, 4028, 4029, 4030, 4031, 4032, 4033, 4034, 4035, 4036, 4037, 4038, 4039, 4040, 4041, 4042, 4043, 4044, 4045, 4046, 4047, 4048, 4049, 4050, 4051, 4052, 4053, 4054, 4055, 4056, 4057, 4058, 4059, 4060, 4061, 4062, 4063, 4064, 4065, 4066, 4067, 4068, 4069, 4070, 4071, 4072, 4073, 4074, 4075, 4076, 4077, 4078, 4079, 4080, 4081, 4082, 4083, 4084, 4085, 4086, 4087, 4088, 4089, 4090, 4091, 4092, 4093, 4094, 4095, 4096, 4097, 4098, 4099, 4100, 4101, 4102, 4103, 4104, 4105, 4106, 4107, 4108, 4109, 4110, 4111, 4112, 4113, 4114, 4115, 4116, 4117, 4118, 4119, 4120, 4121, 4122, 4123, 4124, 4125, 4126, 4127, 4128, 4129, 4130, 4131, 4132, 4133, 4134, 4135, 4136, 4137, 4138, 4139, 4140, 4141, 4142, 4143, 4144, 4145, 4146, 4147, 4148, 4149, 4150, 4151, 4152, 4153, 4154, 4155, 4156, 4157, 4158, 4159, 4160, 4161, 4162, 4163, 4164, 4165, 4166, 4167, 4168, 4169, 4170, 4171, 4172, 4173, 4174, 4175, 4176, 4177, 4178, 4179, 4180, 4181, 4182, 4183, 4184, 4185, 4186, 4187, 4188, 4189, 4190, 4191, 4192, 4193, 4194, 4195, 4196, 4198, 4199, 4200, 4201, 4202, 4203, 4204, 4205, 4206, 4207, 4208, 4209, 4210, 4211, 4212, 4213, 4214, 4215, 4216, 4217, 4218, 4219, 4220, 4221, 4222, 4223, 4224, 4225, 4226, 4227, 4228, 4229, 4230, 4231, 4232, 4233, 4234, 4235, 4236, 4237, 4238, 4239, 4240, 4241, 4242, 4243, 4244, 4245, 4246, 4247, 4248, 4249, 4250, 4251, 4252, 4253, 4254, 4255, 4256, 4257, 4258, 4259, 4260, 4261, 4262, 4263, 4264, 4265, 4266, 4267, 4268, 4269, 4270, 4271, 4272, 4273, 4274, 4275, 4276, 4277, 4278, 4279, 4280, 4281, 4282, 4283, 4284, 4285, 4286, 4287, 4288, 4289, 4290, 4291, 4292, 4293, 4294, 4295, 4296, 4297, 4298, 4299, 4300, 4301, 4302, 4303, 4304, 4305, 4306, 4307, 4308, 4309, 4310, 4311, 4312, 4313, 4314, 4315, 4316, 4317, 4318, 4319, 4320, 4321, 4322, 4323, 4324, 4325, 4326, 4327, 4328, 4329, 4330, 4331, 4332, 4333, 4334, 4335, 4336, 4337, 4338, 4339, 4340, 4341, 4342, 4343, 4344, 4345, 4346, 4347, 4348, 4349, 4350, 4351, 4352, 4353, 4354, 4355, 4356, 4357, 4358, 4359, 4360, 4361, 4362, 4363, 4364, 4365, 4366, 4367, 4368, 4369, 4370, 4371, 4372, 4373, 4374, 4375, 4376, 4377, 4378, 4379, 4380, 4381, 4382, 4383, 4384, 4385, 4386, 4387, 4389, 4390, 4391, 4392, 4393, 4394, 4395, 4396, 4397, 4398, 4399, 4402, 4403, 4404, 4405, 4406, 4407, 4408, 4409, 4410, 4411, 4412, 4413, 4414, 4415, 4416, 4417, 4418, 4419, 4420, 4421, 4422, 4423, 4424, 4426, 4427, 4428, 4429, 4430, 4431, 4432, 4433, 4434, 4435, 4436, 4437, 4438, 4439, 4440, 4441, 4442, 4443, 4444, 4445, 4446, 4447, 4448, 4449, 4450, 4451, 4452, 4453, 4454, 4455, 4456, 4457, 4458, 4459, 4460, 4461, 4462, 4463, 4464, 4465, 4466, 4467, 4468, 4469, 4470, 4471, 4472, 4473, 4474, 4475, 4476, 4477, 4478, 4479, 4480, 4481, 4482, 4483, 4484, 4485, 4486, 4487, 4488, 4489, 4490, 4491, 4492, 4493, 4494, 4495, 4496, 4497, 4498, 4499, 4500, 4501, 4502, 4503, 4504, 4505, 4506, 4507, 4508, 4509, 4510, 4511, 4512, 4513, 4514, 4515, 4516, 4517, 4518, 4519, 4520, 4521, 4522, 4523, 4524, 4525, 4526, 4527, 4528, 4529, 4530, 4531, 4532, 4533, 4534, 4535, 4536, 4537, 4538, 4539, 4540, 4541, 4542, 4543, 4544, 4545, 4546, 4547, 4548, 4549, 4550, 4551, 4552, 4553, 4554, 4555, 4556, 4557, 4558, 4559, 4560, 4561, 4562, 4563, 4564, 4565, 4566, 4567, 4568, 4569, 4570, 4571, 4572, 4573, 4574, 4575, 4576, 4577, 4578, 4579, 4580, 4581, 4582, 4583, 4584, 4585, 4586, 4587, 4588, 4589, 4590, 4591, 4592, 4593, 4594, 4595, 4596, 4597, 4598, 4599, 4600, 4601, 4602, 4603, 4604, 4605, 4606, 4607, 4608, 4609, 4610, 4611, 4612, 4613, 4614, 4615, 4616, 4617, 4618, 4619, 4620, 4621, 4622, 4623, 4624, 4625, 4626, 4627, 4628, 4629, 4630, 4631, 4632, 4633, 4634, 4635, 4636, 4637, 4638, 4639, 4640, 4641, 4642, 4643, 4644, 4645, 4646, 4647, 4648, 4649, 4650, 4651, 4652, 4653, 4654, 4655, 4656, 4657, 4658, 4659, 4660, 4661, 4662, 4663, 4664, 4665, 4666, 4667, 4668, 4669, 4670, 4671, 4672, 4673, 4674, 4675, 4676, 4677, 4678, 4679, 4680, 4681, 4682, 4683, 4684, 4685, 4686, 4687, 4688, 4689, 4690, 4691, 4692, 4693, 4694, 4695, 4696, 4697, 4698, 4699, 4700, 4701, 4702, 4703, 4704, 4705, 4706, 4707, 4708, 4709, 4710, 4711, 4712, 4713, 4714, 4715, 4716, 4717, 4718, 4719, 4720, 4721, 4722, 4723, 4724, 4725, 4726, 4727, 4728, 4729, 4730, 4731, 4732, 4733, 4734, 4735, 4736, 4737, 4738, 4739, 4740, 4741, 4742, 4743, 4744, 4745, 4746, 4747, 4748, 4749, 4750, 4751, 4752, 4753, 4754, 4755, 4756, 4757, 4758, 4759, 4760, 4761, 4762, 4763, 4764, 4765, 4766, 4767, 4768, 4769, 4770, 4771, 4772, 4773, 4774, 4775, 4776, 4777, 4778, 4779, 4780, 4781, 4782, 4783, 4784, 4785, 4786, 4787, 4788, 4789, 4790, 4791, 4792, 4793, 4794, 4795, 4796, 4797, 4798, 4799, 4800, 4801, 4802, 4803, 4804, 4805, 4806, 4808, 4809, 4810, 4811, 4812, 4813, 4814, 4815, 4816, 4817, 4818, 4819, 4820, 4821, 4822, 4823, 4824, 4825, 4826, 4827, 4828, 4829, 4830, 4831, 4832, 4833, 4834, 4835, 4836, 4837, 4838, 4839, 4840, 4841, 4842, 4843, 4844, 4845, 4846, 4847, 4848, 4849, 4850, 4851, 4852, 4853, 4854, 4855, 4856, 4857, 4858, 4859, 4860, 4861, 4862, 4863, 4864, 4865, 4866, 4867, 4868, 4869, 4870, 4871, 4872, 4873, 4874, 4875, 4876, 4877, 4878, 4879, 4880, 4881, 4882, 4883, 4884, 4885, 4886, 4887, 4888, 4889, 4890, 4891, 4892, 4893, 4894, 4895, 4896, 4897, 4898, 4899, 4900, 4901, 4902, 4903, 4904, 4905, 4906, 4907, 4908, 4909, 4910, 4911, 4912, 4913, 4914, 4915, 4916, 4917, 4918, 4919, 4920, 4921, 4922, 4923, 4924, 4925, 4926, 4927, 4928, 4929, 4930, 4931, 4932, 4933, 4934, 4935, 4936, 4937, 4938, 4939, 4940, 4941, 4942, 4943, 4944, 4945, 4946, 4947, 4948, 4949, 4950, 4951, 4952, 4953, 4954, 4955, 4956, 4957, 4958, 4959, 4960, 4961, 4962, 4963, 4964, 4965, 4966, 4967, 4968, 4969, 4970, 4971, 4972, 4973, 4974, 4975, 4976, 4977, 4978, 4979, 4980, 4981, 4982, 4983, 4984, 4985, 4986, 4987, 4988, 4989, 4990, 4991, 4992, 4993, 4994, 4995, 4996, 4997, 4998, 4999, 5000, 5001, 5002, 5003, 5004, 5005, 5006, 5007, 5008, 5009, 5010, 5011, 5012, 5013, 5014, 5015, 5016, 5017, 5018, 5019, 5020, 5021, 5022, 5023, 5024, 5025, 5026, 5027, 5028, 5029, 5030, 5031, 5032, 5033, 5034, 5035, 5036, 5037, 5038, 5039, 5040, 5041, 5042, 5043, 5044, 5045, 5046, 5047, 5048, 5049, 5050, 5051, 5052, 5053, 5054, 5055, 5056, 5057, 5058, 5059, 5060, 5061, 5062, 5063, 5064, 5065, 5066, 5067, 5068, 5069, 5070, 5071, 5072, 5073, 5074, 5075, 5076, 5077, 5078, 5079, 5080, 5081, 5082, 5083, 5084, 5085, 5086, 5087, 5088, 5090, 5091, 5092, 5093, 5094, 5095, 5096, 5097, 5098, 5099, 5100, 5101, 5102, 5103, 5104, 5105, 5106, 5107, 5108, 5109, 5110, 5111, 5112, 5113, 5114, 5115, 5116, 5117, 5118, 5119, 5120, 5121, 5122, 5123, 5124, 5125, 5126, 5127, 5128, 5129, 5130, 5131, 5132, 5133, 5134, 5135, 5136, 5137, 5138, 5139, 5140, 5141, 5142, 5143, 5144, 5145, 5147, 5148, 5149, 5150, 5151, 5152, 5153, 5154, 5155, 5156, 5157, 5158, 5159, 5160, 5161, 5162, 5163, 5164, 5165, 5166, 5167, 5168, 5169, 5170, 5171, 5172, 5173, 5174, 5175, 5176, 5177, 5178, 5179, 5180, 5181, 5182, 5183, 5184, 5185, 5186, 5187, 5188, 5189, 5190, 5191, 5192, 5193, 5194, 5195, 5196, 5197, 5198, 5199, 5200, 5201, 5202, 5203, 5204, 5205, 5206, 5207, 5208, 5209, 5210, 5211, 5212, 5213, 5214, 5215, 5216, 5217, 5218, 5219, 5220, 5221, 5222, 5223, 5224, 5225, 5226, 5227, 5228, 5229, 5230, 5231, 5232, 5233, 5234, 5235, 5236, 5237, 5238, 5239, 5240, 5241, 5242, 5243, 5244, 5245, 5246, 5247, 5248, 5249, 5250, 5251, 5252, 5253, 5254, 5255, 5256, 5257, 5258, 5259, 5260, 5261, 5262, 5263, 5264, 5265, 5266, 5267, 5268, 5269, 5270, 5271, 5272, 5273, 5274, 5275, 5276, 5277, 5278, 5279, 5280, 5281, 5282, 5283, 5284, 5285, 5286, 5287, 5288, 5289, 5290, 5291, 5292, 5293, 5294, 5295, 5296, 5297, 5298, 5299, 5300, 5301, 5302, 5303, 5304, 5305, 5306, 5307, 5308, 5309, 5310, 5311, 5312, 5313, 5314]</t>
         </is>
       </c>
-      <c r="BV8" t="n">
+      <c r="CD8" t="n">
         <v>0.07697893972403776</v>
       </c>
-      <c r="BW8" t="inlineStr">
+      <c r="CE8" t="inlineStr">
         <is>
           <t>{'Numk': 48, 'KPar': 20, 'Bucket_index': 569}</t>
         </is>
       </c>
-      <c r="BX8" t="n">
+      <c r="CF8" t="n">
         <v>12.06913982983679</v>
       </c>
-      <c r="BY8" t="inlineStr">
+      <c r="CG8" t="inlineStr">
         <is>
           <t>no</t>
         </is>
       </c>
-      <c r="BZ8" t="n">
-        <v>0</v>
-      </c>
-      <c r="CA8" t="inlineStr">
+      <c r="CH8" t="n">
+        <v>0</v>
+      </c>
+      <c r="CI8" t="inlineStr">
         <is>
           <t>params</t>
         </is>
       </c>
-      <c r="CB8" t="n">
+      <c r="CJ8" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>